<commit_message>
Various LLM outputs and mew Prompts
</commit_message>
<xml_diff>
--- a/exports/06_analysis/Sleep/all_correct_Sleep_Documents_att_True.xlsx
+++ b/exports/06_analysis/Sleep/all_correct_Sleep_Documents_att_True.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AC19"/>
+  <dimension ref="A1:Z19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -456,142 +456,129 @@
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
+          <t>Lemma</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
           <t>LLM_Events_all_evidence_Doc</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>Event_Name_LLM_Events_all_evidence_Doc</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>Attribute_LLM_Events_all_evidence_Doc</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
-        <is>
-          <t>Text_Quotes_LLM_Events_all_evidence_Doc</t>
-        </is>
-      </c>
       <c r="I1" s="1" t="inlineStr">
         <is>
+          <t>Text_Quote_LLM_Events_all_evidence_Doc</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>Order_LLM_Events_all_evidence_Doc</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
           <t>LLM_Events_keyword_evidence_Doc</t>
         </is>
       </c>
-      <c r="J1" s="1" t="inlineStr">
+      <c r="L1" s="1" t="inlineStr">
         <is>
           <t>Event_Name_LLM_Events_keyword_evidence_Doc</t>
         </is>
       </c>
-      <c r="K1" s="1" t="inlineStr">
+      <c r="M1" s="1" t="inlineStr">
         <is>
           <t>Attribute_LLM_Events_keyword_evidence_Doc</t>
         </is>
       </c>
-      <c r="L1" s="1" t="inlineStr">
-        <is>
-          <t>Text_Quotes_LLM_Events_keyword_evidence_Doc</t>
-        </is>
-      </c>
-      <c r="M1" s="1" t="inlineStr">
-        <is>
-          <t>LLM_Events_example_evidence_Doc</t>
-        </is>
-      </c>
       <c r="N1" s="1" t="inlineStr">
         <is>
-          <t>Event_Name_LLM_Events_example_evidence_Doc</t>
+          <t>Text_Quote_LLM_Events_keyword_evidence_Doc</t>
         </is>
       </c>
       <c r="O1" s="1" t="inlineStr">
         <is>
-          <t>Attribute_LLM_Events_example_evidence_Doc</t>
+          <t>Order_LLM_Events_keyword_evidence_Doc</t>
         </is>
       </c>
       <c r="P1" s="1" t="inlineStr">
         <is>
-          <t>Text_Quotes_LLM_Events_example_evidence_Doc</t>
+          <t>Sleep_time</t>
         </is>
       </c>
       <c r="Q1" s="1" t="inlineStr">
         <is>
-          <t>Sleep_time</t>
+          <t>focus_event</t>
         </is>
       </c>
       <c r="R1" s="1" t="inlineStr">
         <is>
-          <t>focus_event</t>
+          <t>negation</t>
         </is>
       </c>
       <c r="S1" s="1" t="inlineStr">
         <is>
-          <t>negation</t>
+          <t>Doc_gt_Sleep</t>
         </is>
       </c>
       <c r="T1" s="1" t="inlineStr">
         <is>
-          <t>Doc_gt_Sleep</t>
+          <t>is_keyword_present</t>
         </is>
       </c>
       <c r="U1" s="1" t="inlineStr">
         <is>
-          <t>is_keyword_present</t>
+          <t>dict_Lemma</t>
         </is>
       </c>
       <c r="V1" s="1" t="inlineStr">
         <is>
-          <t>dict_Lemma</t>
+          <t>LLM_Events_all_evidence_Doc_Sleep_time</t>
         </is>
       </c>
       <c r="W1" s="1" t="inlineStr">
         <is>
-          <t>LLM_Events_all_evidence_Doc_Sleep_time</t>
+          <t>LLM_Events_keyword_evidence_Doc_Sleep_time</t>
         </is>
       </c>
       <c r="X1" s="1" t="inlineStr">
         <is>
-          <t>LLM_Events_keyword_evidence_Doc_Sleep_time</t>
+          <t>Event_Name_Sleep</t>
         </is>
       </c>
       <c r="Y1" s="1" t="inlineStr">
         <is>
-          <t>LLM_Events_example_evidence_Doc_Sleep_time</t>
+          <t>Event_Name_LLM_Events_all_evidence_Doc_Sleep</t>
         </is>
       </c>
       <c r="Z1" s="1" t="inlineStr">
         <is>
-          <t>Event_Name_Sleep</t>
-        </is>
-      </c>
-      <c r="AA1" s="1" t="inlineStr">
-        <is>
-          <t>Event_Name_LLM_Events_all_evidence_Doc_Sleep</t>
-        </is>
-      </c>
-      <c r="AB1" s="1" t="inlineStr">
-        <is>
           <t>Event_Name_LLM_Events_keyword_evidence_Doc_Sleep</t>
-        </is>
-      </c>
-      <c r="AC1" s="1" t="inlineStr">
-        <is>
-          <t>Event_Name_LLM_Events_example_evidence_Doc_Sleep</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="n">
-        <v>1310477</v>
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>1310477</t>
+        </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>['Pain', 'Family', 'Unknown']</t>
+          <t>('Pain', 'Family', 'Unknown')</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>['son', 'pain']</t>
+          <t>('pain', 'son')</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -614,120 +601,111 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>{'text': 'ccu nursing admit note 0615\ns:  i stopped taking my blood pressure medicine.  i was supposed to see my doctor today.\n\no:  patient stopped taking lopressor 1 month ago as above (? confused it with "back pain" med), and presented to osh with c/o back pain and chills with bp up to 187/104 heart rate 104.\n\npmh includes afib, ascending aortic resection [**7-26**], htn.\npatient is allergic sulfa and pcn.\n\nsocially - patient lives with wife and son.  wife is legally [**month/year (2) 5720**] and patient is her primary care giver.  patient very anxious as wife is home alone at this point.\n\ncv - heart rate 130\'s 2:1 block, bp down to 104/70 on nipride .5mcg/kg/min and labetolol .73mg/min.  [**month/year (2) **] placed l radial in er.\n\nresp - o2 on 3ln/p with oxygen saturation 95-97% with decreased bs at bases\n\ngi - abd is soft with +bs.  patient\'s last stool [**3-9**]\n\ngu - urinating in urinal, but patient has spilled on himself, so i/o is inaccurate\n\nlabs - pnd\n\na:  84yom with history aortic aneurism now presents with htn as he self dc/d his lopressor\n\np:  monitor heart rate with goal 60 and bp with goal 100/.  titrate meds accordingly,  check pnd labs, monitor u/o and place foley cath, check pnd labs, social service to assist with home situation (son lives with parents and patient\'s wife is legally [**month/year (2) 5720**]).\n', 'event': ['Pain', 'Family', 'Excretion', 'Excretion', 'Pain', 'Family'], 'phrase': '', 'raw_output': '{\n  "events": [\n    {\n      "event_type": "Pain",\n      "text_quote": "c/o back pain and chills",\n      "attributes": {\n        "severity": "Unknown",\n        "location": "back",\n        "duration": "Unknown",\n        "time": "Unknown",\n        "caused_by": "Unknown"\n      }\n    },\n    {\n      "event_type": "Family",\n      "text_quote": "patient lives with wife and son.  wife is legally [**month/year (2) 5720**] and patient is her primary care giver.",\n      "attributes": {\n        "interaction": "Unknown",\n        "relation": "wife and son",\n        "time": "Unknown",\n        "caused_by": "Unknown"\n      }\n    },\n    {\n      "event_type": "Excretion",\n      "text_quote": "urinating in urinal, but patient has spilled on himself, so i/o is inaccurate",\n      "attributes": {\n        "type": "urine",\n        "frequency": "Unknown",\n        "quality": "Unknown",\n        "time": "Unknown",\n        "caused_by": "Unknown"\n      }\n    },\n    {\n      "event_type": "Excretion",\n      "text_quote": "patient\'s last stool [**3-9**]",\n      "attributes": {\n        "type": "stool",\n        "frequency": "[**3-9**]",\n        "quality": "Unknown",\n        "time": "Unknown",\n        "caused_by": "Unknown"\n      }\n    },\n    {\n      "event_type": "Pain",\n      "text_quote": "back pain",\n      "attributes": {\n        "severity": "Unknown",\n        "location": "back",\n        "duration": "Unknown",\n        "time": "Unknown",\n        "caused_by": "Unknown"\n      }\n    },\n    {\n      "event_type": "Family",\n      "text_quote": "patient very anxious as wife is home alone at this point.",\n      "attributes": {\n        "interaction": "Unknown",\n        "relation": "wife",\n        "time": "Unknown",\n        "caused_by": "Unknown"\n      }\n    }\n  ]\n}', 'attributes': [{'Pain': {'severity': 'Unknown', 'location': 'back', 'duration': 'Unknown', 'time': 'Unknown', 'caused_by': 'Unknown'}}, {'Family': {'interaction': 'Unknown', 'relation': 'wife and son', 'time': 'Unknown', 'caused_by': 'Unknown'}}, {'Excretion': {'type': 'urine', 'frequency': 'Unknown', 'quality': 'Unknown', 'time': 'Unknown', 'caused_by': 'Unknown'}}, {'Excretion': {'type': 'stool', 'frequency': '[**3-9**]', 'quality': 'Unknown', 'time': 'Unknown', 'caused_by': 'Unknown'}}, {'Pain': {'severity': 'Unknown', 'location': 'back', 'duration': 'Unknown', 'time': 'Unknown', 'caused_by': 'Unknown'}}, {'Family': {'interaction': 'Unknown', 'relation': 'wife', 'time': 'Unknown', 'caused_by': 'Unknown'}}], 'text_quotes': ['c/o back pain and chills', 'patient lives with wife and son.  wife is legally [**month/year (2) 5720**] and patient is her primary care giver.', 'urinating in urinal, but patient has spilled on himself, so i/o is inaccurate', "patient's last stool [**3-9**]", 'back pain', 'patient very anxious as wife is home alone at this point.'], 'event_name_prompt': 'Given the text: ccu nursing admit note 0615\ns:  i stopped taking my blood pressure medicine.  i was supposed to see my doctor today.\n\no:  patient stopped taking lopressor 1 month ago as above (? confused it with "back pain" med), and presented to osh with c/o back pain and chills with bp up to 187/104 heart rate 104.\n\npmh includes afib, ascending aortic resection [**7-26**], htn.\npatient is allergic sulfa and pcn.\n\nsocially - patient lives with wife and son.  wife is legally [**month/year (2) 5720**] and patient is her primary care giver.  patient very anxious as wife is home alone at this point.\n\ncv - heart rate 130\'s 2:1 block, bp down to 104/70 on nipride .5mcg/kg/min and labetolol .73mg/min.  [**month/year (2) **] placed l radial in er.\n\nresp - o2 on 3ln/p with oxygen saturation 95-97% with decreased bs at bases\n\ngi - abd is soft with +bs.  patient\'s last stool [**3-9**]\n\ngu - urinating in urinal, but patient has spilled on himself, so i/o is inaccurate\n\nlabs - pnd\n\na:  84yom with history aortic aneurism now presents with htn as he self dc/d his lopressor\n\np:  monitor heart rate with goal 60 and bp with goal 100/.  titrate meds accordingly,  check pnd labs, monitor u/o and place foley cath, check pnd labs, social service to assist with home situation (son lives with parents and patient\'s wife is legally [**month/year (2) 5720**]).\n, \n                        and the following event types with their definitions: Eating : The patient takes food into their body by mouth.\nExcretion : The patient discharges waste matter from their body.\nFamily : The patient has a visit, call, or communication with a family member.\nPain : The patient reports or shows signs of pain.\nSleep : The patient sleeps or the sleep’s quality or quantity is described.\nUnknown : choose "Unknown" if none of the other event type are applicable. \n                        ---\n                        Your task:\n                        0. Identify ALL events in the text (zero, one, or more).\n1. For each event, assign an event_type from the list above.\n2. If multiple event of same type is mentioned, assign the event_type multiple times\n3. Extract attributes for each event using ONLY the allowed attributes listed below.\n4. Use keyword evidence (Ki) ONLY if it is consistent with the text context.\n5. Output strictly valid JSON following the schema below.\n                        ---\n                        Classification Rules:\n                        - A text may contain multiple events of the same or different types.\n- Create a separate event object for each event mention.\n- If the text is explicitly a NEGATION (e.g., "denies pain"), do not extract that event.\n- If the text describes a FUTURE or HYPOTHETICAL event (e.g., "will eat tomorrow"), ignore it.\n- A valid event should have occurred in the recent past or is occurring during the time of writing of the text.\n- If no events are found or if unsure, return {"events": []}\n                        \n                        ---\n                                    Attributes allowed:\n                                    {\'Eating\': {\'food\': \'&lt;string&gt; # e.g., pancakes, porridge, etc.\', \'amount\': \'&lt;string&gt; # e.g., 1, 2 bowls, etc.\', \'method\': \'&lt;string&gt;  # e.g., oral, tube, etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, after shower, etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}, \'Excretion\': {\'type\': \'&lt;string&gt; # e.g., urine, stool, etc.\', \'frequency\': \'&lt;string&gt; # e.g., 2x, once, etc.\', \'quality\': \'&lt;string&gt; # e.g., loose, hard, etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, after shower, etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}, \'Family\': {\'interaction\': \'&lt;string&gt; # e.g., visit, call, communication, etc.\', \'relation\': \'&lt;string&gt; # e.g., mother, son, etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, after shower, etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}, \'Pain\': {\'severity\': \'&lt;string&gt; # e.g., mild, moderate, severe, numeric scale if present, etc.\', \'location\': \'&lt;string&gt; # e.g., right knee, head, etc.\', \'duration\': \'&lt;string&gt; # e.g., all night, 3 hours, etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, after shower, etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}, \'Sleep\': {\'quality\': \'&lt;string&gt; # e.g., good, poor, restless, etc.\', \'duration\': \'&lt;string&gt; # e.g., 6 hours, phrases like "all night", etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, after shower, etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}}\n                                    If no relevant attribute exists for an event, return an empty object {}.\n                                    \n                        \n                        ---\n                                    Keyword evidence (Ki):\n                                    Additional facts: A keyword matching algorithm without context detected keyword(s) [\'son\', \'pain\'].\n                                    Use this only as a pointer. If context contradicts, ignore.\n                        ---\n                        Output Schema (strict):\n                        {\n                                    "events": [\n                                        {\n                                        "event_type": "&lt;Pain | Sleep | Excretion | Eating | Family&gt;",\n                                        "text_quote": "&lt;fragement from the text indicating &gt;",\n                "attributes": {\n                    "&lt;attribute_name&gt;": "&lt;attribute_value&gt;"\n                }\n                                        }\n                                    ]\n                                    }\n                        \n                            Rules:\n                                - Ensure the output is valid JSON (parseable).\n                                - "eventS" must always be an array (can be empty).\n                                - Multiple instances of the same event type appear as individual elements in the event array.\n                                - Events appear in the array in the same order in which they appear in the text.\n                                - Do not include extra keys, comments, or text.\n                                - Each object in "events" must contain "event_type", "text_quote", and "attributes".\n                                -If an event attribute type has no value mentioned, return "attributes": {"&lt; attribute name &gt;:Unknown"} for each attribute type defined for the event type \n                        \n                        \n                        \n                ---\n                Examples:\n                \n                text: "Patient ate breakfast this morning. He seems less anxious."\n                output: {\n                "events": [\n                    {\n                    "event_type": "Eating",\n                    "text_quote":"Patient ate breakfast this morning",\n                    "attributes": {"food": "breakfast", \n                                   "amount": "Unknown",\n                                   "method": "Unknown",\n                                   "time":"morning",\n                                   "caused_by":"Unknown"}\n                    }\n                ]\n                }\n                \n                text: "Patient reported severe abdominal pain."\n                output: {\n                "events": [\n                    {\n                    "event_type": "Pain",\n                    "text_quote": "severe abdominal Pain",\n                    "attributes": {"severity": "severe", \n                                   "location": "abdominal",\n                                   "duration": "Unknown",\n                                   "time":"Unknown",\n                                   "caused_by":"Unknown"}\n                    }\n                ]\n                }\n                \n                text: "Patient called his son around 3 pm."\n                output: {\n                "events": [\n                    {\n                    "event_type": "Family",\n                    "text_quote": "called his son around 3 pm",\n                    "attributes": {"interaction": "call", \n                                    "relation": "son",\n                                    "time":"3 pm",\n                                    "caused_by":"Unknown"}\n                    }\n                ]\n                }\n                \n                text: "Patient had a loose stool overnight."\n                output: {\n                "events": [\n                    {\n                    "event_type": "Excretion",\n                    "text_quote": "loose stool overnight",\n                    "attributes": {"type": "stool", \n                                   "quality": "loose", \n                                   "frequency":"overnight", \n                                   "time":"night",\n                                   "caused_by":"Unknown"}\n                    }\n                ]\n                }\n                \n                text: "Patient was able to sleep well last night."\n                output: {\n                "events": [\n                    {\n                    "event_type": "Sleep",\n                    "text_quote": "sleep well last night",\n                    "attributes": {"quality": "well",\n                                    "duration": "Unknown", \n                                    "time":"night",\n                                    "caused_by":"Unknown"}\n                    }\n                ]\n                }\n                \n                text: "The patient couldn\'t sleep due to severe pain."\n                output: {\n                "events": [\n                    {\n                    "event_type": "Sleep",\n                    "text_quote": "couldn\'t sleep",\n                    "attributes": {"quality": "poor", \n                                    "duration": "Unknown",\n                                   "time":"Unknown",\n                                   "caused_by":"Pain"}\n                    },\n                    {\n                    "event_type": "Pain",\n                    "text_quote": "severe pain",\n                    "attributes": {"severity": "severe", \n                                    "location": "Unknown", \n                                    "duration": "Unknown", \n                                   "time":"before Sleep",\n                                   "caused_by":"Unknown"}\n                    }\n                ]\n                }\n                \n                text: "The patient complained of severe back pain, was given Tylenol, but the pain persisted and he was then prescribed stronger morphine."\n                output: {\n                "events": [\n                    {\n                    "event_type": "Pain",\n                    "text_quote": "complained of severe back pain",\n                    "attributes": {"severity": "severe", \n                                    "location": "back",\n                                    "duration": "Unknown", \n                                    "time":"Unknown",\n                                    "caused_by":"Unknown"}\n                    },\n                    {\n                    "event_type": "Pain",\n                    "text_quote": "pain persisted",\n                    "attributes": {"severity": "severe", \n                                   "location": "back",\n                                   "duration": "persistent", \n                                   "time":"after Tylenol",\n                                   "caused_by":"Unknown"}\n                    }\n                ]\n                }\n                \n                        ', 'event_detection_time': 16.225309804998687}</t>
+          <t>['pain', 'son']</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>['Pain', 'Family', 'Excretion', 'Excretion', 'Pain', 'Family']</t>
+          <t>{'text': 'ccu nursing admit note 0615\ns:  i stopped taking my blood pressure medicine.  i was supposed to see my doctor today.\n\no:  patient stopped taking lopressor 1 month ago as above (? confused it with "back pain" med), and presented to osh with c/o back pain and chills with bp up to 187/104 heart rate 104.\n\npmh includes afib, ascending aortic resection [**7-26**], htn.\npatient is allergic sulfa and pcn.\n\nsocially - patient lives with wife and son.  wife is legally [**month/year (2) 5720**] and patient is her primary care giver.  patient very anxious as wife is home alone at this point.\n\ncv - heart rate 130\'s 2:1 block, bp down to 104/70 on nipride .5mcg/kg/min and labetolol .73mg/min.  [**month/year (2) **] placed l radial in er.\n\nresp - o2 on 3ln/p with oxygen saturation 95-97% with decreased bs at bases\n\ngi - abd is soft with +bs.  patient\'s last stool [**3-9**]\n\ngu - urinating in urinal, but patient has spilled on himself, so i/o is inaccurate\n\nlabs - pnd\n\na:  84yom with history aortic aneurism now presents with htn as he self dc/d his lopressor\n\np:  monitor heart rate with goal 60 and bp with goal 100/.  titrate meds accordingly,  check pnd labs, monitor u/o and place foley cath, check pnd labs, social service to assist with home situation (son lives with parents and patient\'s wife is legally [**month/year (2) 5720**]).\n', 'event': ['Pain', 'Excretion', 'Family', 'Family', 'Excretion'], 'event_id': ['e1', 'e2', 'e3', 'e4', 'e5'], 'phrase': '', 'raw_output': '{\n  "events": [\n    {\n      "event_id": "e1",\n      "event_type": "Pain",\n      "text_quote": "back pain and chills",\n      "attributes": {\n        "severity": "Unknown",\n        "location": "back",\n        "duration": "Unknown",\n        "negation": "false",\n        "time": "Unknown",\n        "caused_by": "Unknown"\n      }\n    },\n    {\n      "event_id": "e2",\n      "event_type": "Excretion",\n      "text_quote": "urinating in urinal, but patient has spilled on himself",\n      "attributes": {\n        "type": "urine",\n        "frequency": "Unknown",\n        "quality": "Unknown",\n        "negation": "false",\n        "time": "Unknown",\n        "caused_by": "Unknown"\n      }\n    },\n    {\n      "event_id": "e3",\n      "event_type": "Family",\n      "text_quote": "patient very anxious as wife is home alone at this point",\n      "attributes": {\n        "interaction": "Unknown",\n        "relation": "wife",\n        "negation": "false",\n        "time": "Unknown",\n        "caused_by": "Unknown"\n      }\n    },\n    {\n      "event_id": "e4",\n      "event_type": "Family",\n      "text_quote": "patient lives with wife and son",\n      "attributes": {\n        "interaction": "Unknown",\n        "relation": "wife and son",\n        "negation": "false",\n        "time": "Unknown",\n        "caused_by": "Unknown"\n      }\n    },\n    {\n      "event_id": "e5",\n      "event_type": "Excretion",\n      "text_quote": "patient\'s last stool [3-9]",\n      "attributes": {\n        "type": "stool",\n        "frequency": "Unknown",\n        "quality": "Unknown",\n        "negation": "false",\n        "time": "[3-9]",\n        "caused_by": "Unknown"\n      }\n    }\n  ],\n  "order": []\n}', 'attributes': [{'Pain': {'severity': 'Unknown', 'location': 'back', 'duration': 'Unknown', 'negation': 'false', 'time': 'Unknown', 'caused_by': 'Unknown'}}, {'Excretion': {'type': 'urine', 'frequency': 'Unknown', 'quality': 'Unknown', 'negation': 'false', 'time': 'Unknown', 'caused_by': 'Unknown'}}, {'Family': {'interaction': 'Unknown', 'relation': 'wife', 'negation': 'false', 'time': 'Unknown', 'caused_by': 'Unknown'}}, {'Family': {'interaction': 'Unknown', 'relation': 'wife and son', 'negation': 'false', 'time': 'Unknown', 'caused_by': 'Unknown'}}, {'Excretion': {'type': 'stool', 'frequency': 'Unknown', 'quality': 'Unknown', 'negation': 'false', 'time': '[3-9]', 'caused_by': 'Unknown'}}], 'orders': [[]], 'text_quotes': ['back pain and chills', 'urinating in urinal, but patient has spilled on himself', 'patient very anxious as wife is home alone at this point', 'patient lives with wife and son', "patient's last stool [3-9]"], 'event_name_prompt': 'Given the text: ccu nursing admit note 0615\ns:  i stopped taking my blood pressure medicine.  i was supposed to see my doctor today.\n\no:  patient stopped taking lopressor 1 month ago as above (? confused it with "back pain" med), and presented to osh with c/o back pain and chills with bp up to 187/104 heart rate 104.\n\npmh includes afib, ascending aortic resection [**7-26**], htn.\npatient is allergic sulfa and pcn.\n\nsocially - patient lives with wife and son.  wife is legally [**month/year (2) 5720**] and patient is her primary care giver.  patient very anxious as wife is home alone at this point.\n\ncv - heart rate 130\'s 2:1 block, bp down to 104/70 on nipride .5mcg/kg/min and labetolol .73mg/min.  [**month/year (2) **] placed l radial in er.\n\nresp - o2 on 3ln/p with oxygen saturation 95-97% with decreased bs at bases\n\ngi - abd is soft with +bs.  patient\'s last stool [**3-9**]\n\ngu - urinating in urinal, but patient has spilled on himself, so i/o is inaccurate\n\nlabs - pnd\n\na:  84yom with history aortic aneurism now presents with htn as he self dc/d his lopressor\n\np:  monitor heart rate with goal 60 and bp with goal 100/.  titrate meds accordingly,  check pnd labs, monitor u/o and place foley cath, check pnd labs, social service to assist with home situation (son lives with parents and patient\'s wife is legally [**month/year (2) 5720**]).\n, \n                        and the following event types with their definitions: Eating : The patient takes food into their body by mouth.\nExcretion : The patient discharges waste matter from their body.\nFamily : The patient has a visit, call, or communication with a family member.\nPain : The patient reports or shows signs of pain.\nSleep : The patient sleeps or the sleep’s quality or quantity is described.\nUnknown : choose "Unknown" if none of the other event type are applicable. \n                        ---\n                        Your task:\n                        0. Identify ALL events in the text (zero, one, or more).\n1. For each event, assign an event_type from the list above.\n2. If multiple event of same type is mentioned, assign the event_type multiple times\n3. Extract attributes for each event using ONLY the allowed attributes listed below.\n4. Use keyword evidence (Ki) ONLY if it is consistent with the text context.\n5. Output strictly valid JSON following the schema below.\n                        ---\n                        Classification Rules:\n                        - A text may contain multiple events of the same or different types.\n- Create a separate event object for each event mention.\n- If the text is explicitly a NEGATION (e.g., "denies pain"), do not extract that event.\n- If the text describes a FUTURE or HYPOTHETICAL event (e.g., "will eat tomorrow"), ignore it.\n- A valid event should have occurred in the recent past or is occurring during the time of writing of the text.\n- If no events are found or if unsure, return {"events": []}\n                        \n                        ---\n                                    Attributes allowed:\n                                    {\'Eating\': {\'food\': \'&lt;string&gt; # e.g., pancakes, porridge, etc.\', \'amount\': \'&lt;string&gt; # e.g., 1, 2 bowls, etc.\', \'method\': \'&lt;string&gt;  # e.g., oral, tube, etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, evening etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}, \'Excretion\': {\'type\': \'&lt;string&gt; # e.g., urine, stool, etc.\', \'frequency\': \'&lt;string&gt; # e.g., 2x, once, etc.\', \'quality\': \'&lt;string&gt; # e.g., loose, hard, etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, evening etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}, \'Family\': {\'interaction\': \'&lt;string&gt; # e.g., visit, call, communication, etc.\', \'relation\': \'&lt;string&gt; # e.g., mother, son, etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, evening etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}, \'Pain\': {\'severity\': \'&lt;string&gt; # e.g., mild, moderate, severe, numeric scale if present, etc.\', \'location\': \'&lt;string&gt; # e.g., right knee, head, etc.\', \'duration\': \'&lt;string&gt; # e.g., all night, 3 hours, etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, evening etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}, \'Sleep\': {\'quality\': \'&lt;string&gt; # e.g., good, poor, restless, etc.\', \'duration\': \'&lt;string&gt; # e.g., 6 hours, phrases like "all night", etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, evening etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}}\n                                    If no relevant attribute exists for an event, return an empty object {}.\n                                    \n                        \n                        ---\n                                    Keyword evidence (Ki):\n                                    Additional facts: A keyword matching algorithm without context detected keyword(s) (\'pain\', \'son\').\n                                    Use this only as a pointer. If context contradicts, ignore.\n                        ---\n                        Output Schema (strict):\n                        {\n                                    "events": [\n                                        {\n                                        "event_id": "&lt; A unique id eg.: e1 | e2 |...&gt;"\n                                        "event_type": "&lt;Pain | Sleep | Excretion | Eating | Family&gt;",\n                                        "text_quote": "&lt;fragement from the text indicating the event_type&gt;",\n                "attributes": {\n                    "&lt;attribute_name&gt;": "&lt;attribute_value&gt;"\n                }\n                                        }\n                                    ],\n                                    "order": [\n                                        ["e1", "before" | "after" | "simultaneous", "e2" ]\n                                    ]\n                                    }\n                        \n                            Rules:\n                                - Ensure the output is valid JSON (parseable).\n                                - "eventS" must always be an array (can be empty).\n                                - Multiple instances of the same event type appear with different ids.\n                                - Events appear in the array in the same order in which they appear in the text.\n                                - Their partial orders can be expressed using the "order" section.\n                                - Do not include extra keys, comments, or text.\n                                - Each object in "events" must contain "event_type", "text_quote", and "attributes".\n                                - If an event attribute type has no value mentioned, return "attributes": {"&lt; attribute name &gt;:Unknown"} for each attribute type defined for the event type \n                        \n                        \n                        \n                ---\n                Examples:\n                \n                text: "Patient ate breakfast this morning. He seems less anxious."\n                output: {\n                "events": [\n                    {"event_id": "e1",\n                    "event_type": "Eating",\n                    "text_quote":"Patient ate breakfast this morning",\n                    "attributes": {"food": "breakfast", \n                                   "amount": "Unknown",\n                                   "method": "Unknown",\n                                   "negation": "false",\n                                   "time":"morning",\n                                   "caused_by":"Unknown"}\n                    }\n                ],\n                "order":[]\n                }\n                \n                text: "Patient reported severe abdominal pain."\n                output: {\n                "events": [\n                    {"event_id": "e1",\n                    "event_type": "Pain",\n                    "text_quote": "severe abdominal Pain",\n                    "attributes": {"severity": "severe", \n                                   "location": "abdominal",\n                                   "duration": "Unknown",\n                                   "negation": "false",\n                                   "time":"Unknown",\n                                   "caused_by":"Unknown"}\n                    }\n                ],\n                "order":[]\n                }\n                \n                text: "Patient called his son around 3 pm."\n                output: {\n                "events": [\n                    {"event_id": "e1",\n                    "event_type": "Family",\n                    "text_quote": "called his son around 3 pm",\n                    "attributes": {"interaction": "call", \n                                    "relation": "son",\n                                    "negation": "false",\n                                    "time":"3 pm",\n                                    "caused_by":"Unknown"}\n                    }\n                ],\n                "order":[]\n                }\n                \n                text: "Patient had a loose stool overnight."\n                output: {\n                "events": [\n                    {"event_id": "e1",\n                    "event_type": "Excretion",\n                    "text_quote": "loose stool overnight",\n                    "attributes": {"type": "stool", \n                                   "quality": "loose", \n                                   "frequency":"overnight", \n                                   "negation": "false",\n                                   "time":"night",\n                                   "caused_by":"Unknown"}\n                    }\n                ],\n                "order":[]\n                }\n                \n                text: "Patient was able to sleep well last night."\n                output: {\n                "events": [\n                    {"event_id": "e1",\n                    "event_type": "Sleep",\n                    "text_quote": "sleep well last night",\n                    "attributes": {"quality": "well",\n                                    "duration": "Unknown", \n                                    "negation": "false",\n                                    "time":"night",\n                                    "caused_by":"Unknown"}\n                    }\n                ],\n                "order":[]\n                }\n                \n                text: "The patient couldn\'t sleep due to severe pain."\n                output: {\n                "events": [\n                    {"event_id": "e1",\n                    "event_type": "Sleep",\n                    "text_quote": "couldn\'t sleep",\n                    "attributes": {"quality": "poor", \n                                    "duration": "Unknown",\n                                    "negation": "true",\n                                    "time":"Unknown",\n                                    "caused_by":"Pain"}\n                    },\n                    {"event_id": "e2",\n                    "event_type": "Pain",\n                    "text_quote": "severe pain",\n                    "attributes": {"severity": "severe", \n                                    "location": "Unknown", \n                                    "duration": "Unknown", \n                                    "time":"Unknown",\n                                    "caused_by":"Unknown"}\n                    }\n                ],\n                "order":["e1", "after", "e2"]\n                }\n                \n                text: "The patient complained of severe back pain, was given Tylenol, but the pain persisted and he was then prescribed stronger morphine."\n                output: {\n                "events": [\n                    {"event_id": "e1",\n                    "event_type": "Pain",\n                    "text_quote": "complained of severe back pain",\n                    "attributes": {"severity": "severe", \n                                    "location": "back",\n                                    "duration": "Unknown", \n                                    "time":"Unknown",\n                                    "caused_by":"Unknown"}\n                    },\n                    {"event_id": "e2",\n                    "event_type": "Pain",\n                    "text_quote": "pain persisted",\n                    "attributes": {"severity": "severe", \n                                   "location": "back",\n                                   "duration": "persistent", \n                                   "time":"after Tylenol",\n                                   "caused_by":"Unknown"}\n                    }\n                ],\n                "order":[["e1", "before", "e2"]]\n                }\n                \n                        ', 'event_detection_time': 16.14568631898146}</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>[{'Pain': {'severity': 'Unknown', 'location': 'back', 'duration': 'Unknown', 'time': 'Unknown', 'caused_by': 'Unknown'}}, {'Family': {'interaction': 'Unknown', 'relation': 'wife and son', 'time': 'Unknown', 'caused_by': 'Unknown'}}, {'Excretion': {'type': 'urine', 'frequency': 'Unknown', 'quality': 'Unknown', 'time': 'Unknown', 'caused_by': 'Unknown'}}, {'Excretion': {'type': 'stool', 'frequency': '[**3-9**]', 'quality': 'Unknown', 'time': 'Unknown', 'caused_by': 'Unknown'}}, {'Pain': {'severity': 'Unknown', 'location': 'back', 'duration': 'Unknown', 'time': 'Unknown', 'caused_by': 'Unknown'}}, {'Family': {'interaction': 'Unknown', 'relation': 'wife', 'time': 'Unknown', 'caused_by': 'Unknown'}}]</t>
+          <t>['Pain', 'Excretion', 'Family', 'Family', 'Excretion']</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>['c/o back pain and chills', 'patient lives with wife and son.  wife is legally [**month/year (2) 5720**] and patient is her primary care giver.', 'urinating in urinal, but patient has spilled on himself, so i/o is inaccurate', "patient's last stool [**3-9**]", 'back pain', 'patient very anxious as wife is home alone at this point.']</t>
+          <t>[{'Pain': {'severity': 'Unknown', 'location': 'back', 'duration': 'Unknown', 'negation': 'false', 'time': 'Unknown', 'caused_by': 'Unknown'}}, {'Excretion': {'type': 'urine', 'frequency': 'Unknown', 'quality': 'Unknown', 'negation': 'false', 'time': 'Unknown', 'caused_by': 'Unknown'}}, {'Family': {'interaction': 'Unknown', 'relation': 'wife', 'negation': 'false', 'time': 'Unknown', 'caused_by': 'Unknown'}}, {'Family': {'interaction': 'Unknown', 'relation': 'wife and son', 'negation': 'false', 'time': 'Unknown', 'caused_by': 'Unknown'}}, {'Excretion': {'type': 'stool', 'frequency': 'Unknown', 'quality': 'Unknown', 'negation': 'false', 'time': '[3-9]', 'caused_by': 'Unknown'}}]</t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>{'text': 'ccu nursing admit note 0615\ns:  i stopped taking my blood pressure medicine.  i was supposed to see my doctor today.\n\no:  patient stopped taking lopressor 1 month ago as above (? confused it with "back pain" med), and presented to osh with c/o back pain and chills with bp up to 187/104 heart rate 104.\n\npmh includes afib, ascending aortic resection [**7-26**], htn.\npatient is allergic sulfa and pcn.\n\nsocially - patient lives with wife and son.  wife is legally [**month/year (2) 5720**] and patient is her primary care giver.  patient very anxious as wife is home alone at this point.\n\ncv - heart rate 130\'s 2:1 block, bp down to 104/70 on nipride .5mcg/kg/min and labetolol .73mg/min.  [**month/year (2) **] placed l radial in er.\n\nresp - o2 on 3ln/p with oxygen saturation 95-97% with decreased bs at bases\n\ngi - abd is soft with +bs.  patient\'s last stool [**3-9**]\n\ngu - urinating in urinal, but patient has spilled on himself, so i/o is inaccurate\n\nlabs - pnd\n\na:  84yom with history aortic aneurism now presents with htn as he self dc/d his lopressor\n\np:  monitor heart rate with goal 60 and bp with goal 100/.  titrate meds accordingly,  check pnd labs, monitor u/o and place foley cath, check pnd labs, social service to assist with home situation (son lives with parents and patient\'s wife is legally [**month/year (2) 5720**]).\n', 'event': ['Family', 'Pain', 'Excretion', 'Excretion', 'Family', 'Family'], 'phrase': '', 'raw_output': '{\n  "events": [\n    {\n      "event_type": "Family",\n      "text_quote": "patient lives with wife and son.  wife is legally [**month/year (2) 5720**] and patient is her primary care giver.",\n      "attributes": {\n        "interaction": "Unknown",\n        "relation": "son, wife",\n        "negation": false,\n        "time": "Unknown",\n        "caused_by": "Unknown"\n      }\n    },\n    {\n      "event_type": "Pain",\n      "text_quote": "patient stopped taking lopressor 1 month ago as above (? confused it with \\"back pain\\" med), and presented to osh with c/o back pain and chills with bp up to 187/104 heart rate 104.",\n      "attributes": {\n        "severity": "Unknown",\n        "location": "back",\n        "duration": "Unknown",\n        "negation": false,\n        "time": "1 month ago",\n        "caused_by": "medication"\n      }\n    },\n    {\n      "event_type": "Excretion",\n      "text_quote": "gu - urinating in urinal, but patient has spilled on himself, so i/o is inaccurate",\n      "attributes": {\n        "type": "urine",\n        "frequency": "Unknown",\n        "quality": "Unknown",\n        "negation": false,\n        "time": "Unknown",\n        "caused_by": "Unknown"\n      }\n    },\n    {\n      "event_type": "Excretion",\n      "text_quote": "gi - abd is soft with +bs.  patient\'s last stool [**3-9**]",\n      "attributes": {\n        "type": "stool",\n        "frequency": "Unknown",\n        "quality": "+bs",\n        "negation": false,\n        "time": "[**3-9**]",\n        "caused_by": "Unknown"\n      }\n    },\n    {\n      "event_type": "Family",\n      "text_quote": "patient very anxious as wife is home alone at this point.",\n      "attributes": {\n        "interaction": "Unknown",\n        "relation": "wife",\n        "negation": false,\n        "time": "Unknown",\n        "caused_by": "Unknown"\n      }\n    },\n    {\n      "event_type": "Family",\n      "text_quote": "social service to assist with home situation (son lives with parents and patient\'s wife is legally [**month/year (2) 5720**])",\n      "attributes": {\n        "interaction": "Unknown",\n        "relation": "son, wife",\n        "negation": false,\n        "time": "Unknown",\n        "caused_by": "Unknown"\n      }\n    }\n  ]\n}', 'attributes': [{'Family': {'interaction': 'Unknown', 'relation': 'son, wife', 'negation': False, 'time': 'Unknown', 'caused_by': 'Unknown'}}, {'Pain': {'severity': 'Unknown', 'location': 'back', 'duration': 'Unknown', 'negation': False, 'time': '1 month ago', 'caused_by': 'medication'}}, {'Excretion': {'type': 'urine', 'frequency': 'Unknown', 'quality': 'Unknown', 'negation': False, 'time': 'Unknown', 'caused_by': 'Unknown'}}, {'Excretion': {'type': 'stool', 'frequency': 'Unknown', 'quality': '+bs', 'negation': False, 'time': '[**3-9**]', 'caused_by': 'Unknown'}}, {'Family': {'interaction': 'Unknown', 'relation': 'wife', 'negation': False, 'time': 'Unknown', 'caused_by': 'Unknown'}}, {'Family': {'interaction': 'Unknown', 'relation': 'son, wife', 'negation': False, 'time': 'Unknown', 'caused_by': 'Unknown'}}], 'text_quotes': ['patient lives with wife and son.  wife is legally [**month/year (2) 5720**] and patient is her primary care giver.', 'patient stopped taking lopressor 1 month ago as above (? confused it with "back pain" med), and presented to osh with c/o back pain and chills with bp up to 187/104 heart rate 104.', 'gu - urinating in urinal, but patient has spilled on himself, so i/o is inaccurate', "gi - abd is soft with +bs.  patient's last stool [**3-9**]", 'patient very anxious as wife is home alone at this point.', "social service to assist with home situation (son lives with parents and patient's wife is legally [**month/year (2) 5720**])"], 'event_name_prompt': 'Given the text: ccu nursing admit note 0615\ns:  i stopped taking my blood pressure medicine.  i was supposed to see my doctor today.\n\no:  patient stopped taking lopressor 1 month ago as above (? confused it with "back pain" med), and presented to osh with c/o back pain and chills with bp up to 187/104 heart rate 104.\n\npmh includes afib, ascending aortic resection [**7-26**], htn.\npatient is allergic sulfa and pcn.\n\nsocially - patient lives with wife and son.  wife is legally [**month/year (2) 5720**] and patient is her primary care giver.  patient very anxious as wife is home alone at this point.\n\ncv - heart rate 130\'s 2:1 block, bp down to 104/70 on nipride .5mcg/kg/min and labetolol .73mg/min.  [**month/year (2) **] placed l radial in er.\n\nresp - o2 on 3ln/p with oxygen saturation 95-97% with decreased bs at bases\n\ngi - abd is soft with +bs.  patient\'s last stool [**3-9**]\n\ngu - urinating in urinal, but patient has spilled on himself, so i/o is inaccurate\n\nlabs - pnd\n\na:  84yom with history aortic aneurism now presents with htn as he self dc/d his lopressor\n\np:  monitor heart rate with goal 60 and bp with goal 100/.  titrate meds accordingly,  check pnd labs, monitor u/o and place foley cath, check pnd labs, social service to assist with home situation (son lives with parents and patient\'s wife is legally [**month/year (2) 5720**]).\n, \n                        and the following event types with their definitions: Eating : The patient takes food into their body by mouth.\nExcretion : The patient discharges waste matter from their body.\nFamily : The patient has a visit, call, or communication with a family member.\nPain : The patient reports or shows signs of pain.\nSleep : The patient sleeps or the sleep’s quality or quantity is described.\nUnknown : choose "Unknown" if none of the other event type are applicable. \n                        ---\n                        Your task:\n                        0. Identify ALL events in the text (zero, one, or more).\n1. For each event, assign an event_type from the list above.\n2. If multiple event of same type is mentioned, assign the event_type multiple times\n3. Extract attributes for each event using ONLY the allowed attributes listed below.\n4. Use keyword evidence (Ki) ONLY if it is consistent with the text context.\n5. Output strictly valid JSON following the schema below.\n                        ---\n                        Classification Rules:\n                        - A text may contain multiple events of the same or different types.\n- Create a separate event object for each event mention.\n- If the text is explicitly a NEGATION (e.g., "denies pain"), do not extract that event.\n- If the text describes a FUTURE or HYPOTHETICAL event (e.g., "will eat tomorrow"), ignore it.\n- A valid event should have occurred in the recent past or is occurring during the time of writing of the text.\n- If no events are found or if unsure, return {"events": []}\n                        \n                        ---\n                                    Attributes allowed:\n                                    {\'Eating\': {\'food\': \'&lt;string&gt; # e.g., pancakes, porridge, etc.\', \'amount\': \'&lt;string&gt; # e.g., 1, 2 bowls, etc.\', \'method\': \'&lt;string&gt;  # e.g., oral, tube, etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, after shower, etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}, \'Excretion\': {\'type\': \'&lt;string&gt; # e.g., urine, stool, etc.\', \'frequency\': \'&lt;string&gt; # e.g., 2x, once, etc.\', \'quality\': \'&lt;string&gt; # e.g., loose, hard, etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, after shower, etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}, \'Family\': {\'interaction\': \'&lt;string&gt; # e.g., visit, call, communication, etc.\', \'relation\': \'&lt;string&gt; # e.g., mother, son, etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, after shower, etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}, \'Pain\': {\'severity\': \'&lt;string&gt; # e.g., mild, moderate, severe, numeric scale if present, etc.\', \'location\': \'&lt;string&gt; # e.g., right knee, head, etc.\', \'duration\': \'&lt;string&gt; # e.g., all night, 3 hours, etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, after shower, etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}, \'Sleep\': {\'quality\': \'&lt;string&gt; # e.g., good, poor, restless, etc.\', \'duration\': \'&lt;string&gt; # e.g., 6 hours, phrases like "all night", etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, after shower, etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}}\n                                    If no relevant attribute exists for an event, return an empty object {}.\n                                    \n                        \n                        ---\n                                    Keyword evidence (Ki):\n                                    Additional facts: A keyword matching algorithm without context detected keyword(s) [\'son\', \'pain\'].\n                                    Use this only as a pointer. If context contradicts, ignore.\n                        ---\n                        Output Schema (strict):\n                        {\n                                    "events": [\n                                        {\n                                        "event_type": "&lt;Pain | Sleep | Excretion | Eating | Family&gt;",\n                                        "text_quote": "&lt;fragement from the text indicating &gt;",\n                "attributes": {\n                    "&lt;attribute_name&gt;": "&lt;attribute_value&gt;"\n                }\n                                        }\n                                    ]\n                                    }\n                        \n                            Rules:\n                                - Ensure the output is valid JSON (parseable).\n                                - "eventS" must always be an array (can be empty).\n                                - Multiple instances of the same event type appear as individual elements in the event array.\n                                - Events appear in the array in the same order in which they appear in the text.\n                                - Do not include extra keys, comments, or text.\n                                - Each object in "events" must contain "event_type", "text_quote", and "attributes".\n                                -If an event attribute type has no value mentioned, return "attributes": {"&lt; attribute name &gt;:Unknown"} for each attribute type defined for the event type \n                        \n                        \n                        \n                        ', 'event_detection_time': 18.850996223991388}</t>
+          <t>['back pain and chills', 'urinating in urinal, but patient has spilled on himself', 'patient very anxious as wife is home alone at this point', 'patient lives with wife and son', "patient's last stool [3-9]"]</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>['Family', 'Pain', 'Excretion', 'Excretion', 'Family', 'Family']</t>
+          <t>[[]]</t>
         </is>
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>[{'Family': {'interaction': 'Unknown', 'relation': 'son, wife', 'negation': False, 'time': 'Unknown', 'caused_by': 'Unknown'}}, {'Pain': {'severity': 'Unknown', 'location': 'back', 'duration': 'Unknown', 'negation': False, 'time': '1 month ago', 'caused_by': 'medication'}}, {'Excretion': {'type': 'urine', 'frequency': 'Unknown', 'quality': 'Unknown', 'negation': False, 'time': 'Unknown', 'caused_by': 'Unknown'}}, {'Excretion': {'type': 'stool', 'frequency': 'Unknown', 'quality': '+bs', 'negation': False, 'time': '[**3-9**]', 'caused_by': 'Unknown'}}, {'Family': {'interaction': 'Unknown', 'relation': 'wife', 'negation': False, 'time': 'Unknown', 'caused_by': 'Unknown'}}, {'Family': {'interaction': 'Unknown', 'relation': 'son, wife', 'negation': False, 'time': 'Unknown', 'caused_by': 'Unknown'}}]</t>
+          <t>{'text': 'ccu nursing admit note 0615\ns:  i stopped taking my blood pressure medicine.  i was supposed to see my doctor today.\n\no:  patient stopped taking lopressor 1 month ago as above (? confused it with "back pain" med), and presented to osh with c/o back pain and chills with bp up to 187/104 heart rate 104.\n\npmh includes afib, ascending aortic resection [**7-26**], htn.\npatient is allergic sulfa and pcn.\n\nsocially - patient lives with wife and son.  wife is legally [**month/year (2) 5720**] and patient is her primary care giver.  patient very anxious as wife is home alone at this point.\n\ncv - heart rate 130\'s 2:1 block, bp down to 104/70 on nipride .5mcg/kg/min and labetolol .73mg/min.  [**month/year (2) **] placed l radial in er.\n\nresp - o2 on 3ln/p with oxygen saturation 95-97% with decreased bs at bases\n\ngi - abd is soft with +bs.  patient\'s last stool [**3-9**]\n\ngu - urinating in urinal, but patient has spilled on himself, so i/o is inaccurate\n\nlabs - pnd\n\na:  84yom with history aortic aneurism now presents with htn as he self dc/d his lopressor\n\np:  monitor heart rate with goal 60 and bp with goal 100/.  titrate meds accordingly,  check pnd labs, monitor u/o and place foley cath, check pnd labs, social service to assist with home situation (son lives with parents and patient\'s wife is legally [**month/year (2) 5720**]).\n', 'event': ['Pain', 'Excretion', 'Excretion', 'Family', 'Pain'], 'event_id': ['e1', 'e2', 'e3', 'e4', 'e5'], 'phrase': '', 'raw_output': '{\n  "events": [\n    {\n      "event_id": "e1",\n      "event_type": "Pain",\n      "text_quote": "c/o back pain and chills with bp up to 187/104 heart rate 104.",\n      "attributes": {\n        "severity": "Unknown",\n        "location": "back",\n        "duration": "Unknown",\n        "negation": false,\n        "time": "Unknown",\n        "caused_by": "Unknown"\n      }\n    },\n    {\n      "event_id": "e2",\n      "event_type": "Excretion",\n      "text_quote": "patient\'s last stool [**3-9**]",\n      "attributes": {\n        "type": "stool",\n        "frequency": "Unknown",\n        "quality": "Unknown",\n        "negation": false,\n        "time": "[**3-9**]",\n        "caused_by": "Unknown"\n      }\n    },\n    {\n      "event_id": "e3",\n      "event_type": "Excretion",\n      "text_quote": "urinating in urinal, but patient has spilled on himself, so i/o is inaccurate",\n      "attributes": {\n        "type": "urine",\n        "frequency": "Unknown",\n        "quality": "Unknown",\n        "negation": false,\n        "time": "Unknown",\n        "caused_by": "Unknown"\n      }\n    },\n    {\n      "event_id": "e4",\n      "event_type": "Family",\n      "text_quote": "patient lives with wife and son.  wife is legally [**month/year (2) 5720**] and patient is her primary care giver.",\n      "attributes": {\n        "interaction": "Unknown",\n        "relation": "wife, son",\n        "negation": false,\n        "time": "Unknown",\n        "caused_by": "Unknown"\n      }\n    },\n    {\n      "event_id": "e5",\n      "event_type": "Pain",\n      "text_quote": "back pain",\n      "attributes": {\n        "severity": "Unknown",\n        "location": "back",\n        "duration": "Unknown",\n        "negation": false,\n        "time": "Unknown",\n        "caused_by": "Unknown"\n      }\n    }\n  ],\n  "order": [\n    ["e1", "before", "e2"],\n    ["e2", "before", "e3"],\n    ["e3", "before", "e4"],\n    ["e4", "before", "e5"]\n  ]\n}', 'attributes': [{'Pain': {'severity': 'Unknown', 'location': 'back', 'duration': 'Unknown', 'negation': False, 'time': 'Unknown', 'caused_by': 'Unknown'}}, {'Excretion': {'type': 'stool', 'frequency': 'Unknown', 'quality': 'Unknown', 'negation': False, 'time': '[**3-9**]', 'caused_by': 'Unknown'}}, {'Excretion': {'type': 'urine', 'frequency': 'Unknown', 'quality': 'Unknown', 'negation': False, 'time': 'Unknown', 'caused_by': 'Unknown'}}, {'Family': {'interaction': 'Unknown', 'relation': 'wife, son', 'negation': False, 'time': 'Unknown', 'caused_by': 'Unknown'}}, {'Pain': {'severity': 'Unknown', 'location': 'back', 'duration': 'Unknown', 'negation': False, 'time': 'Unknown', 'caused_by': 'Unknown'}}], 'orders': [[['e1', 'before', 'e2'], ['e2', 'before', 'e3'], ['e3', 'before', 'e4'], ['e4', 'before', 'e5']]], 'text_quotes': ['c/o back pain and chills with bp up to 187/104 heart rate 104.', "patient's last stool [**3-9**]", 'urinating in urinal, but patient has spilled on himself, so i/o is inaccurate', 'patient lives with wife and son.  wife is legally [**month/year (2) 5720**] and patient is her primary care giver.', 'back pain'], 'event_name_prompt': 'Given the text: ccu nursing admit note 0615\ns:  i stopped taking my blood pressure medicine.  i was supposed to see my doctor today.\n\no:  patient stopped taking lopressor 1 month ago as above (? confused it with "back pain" med), and presented to osh with c/o back pain and chills with bp up to 187/104 heart rate 104.\n\npmh includes afib, ascending aortic resection [**7-26**], htn.\npatient is allergic sulfa and pcn.\n\nsocially - patient lives with wife and son.  wife is legally [**month/year (2) 5720**] and patient is her primary care giver.  patient very anxious as wife is home alone at this point.\n\ncv - heart rate 130\'s 2:1 block, bp down to 104/70 on nipride .5mcg/kg/min and labetolol .73mg/min.  [**month/year (2) **] placed l radial in er.\n\nresp - o2 on 3ln/p with oxygen saturation 95-97% with decreased bs at bases\n\ngi - abd is soft with +bs.  patient\'s last stool [**3-9**]\n\ngu - urinating in urinal, but patient has spilled on himself, so i/o is inaccurate\n\nlabs - pnd\n\na:  84yom with history aortic aneurism now presents with htn as he self dc/d his lopressor\n\np:  monitor heart rate with goal 60 and bp with goal 100/.  titrate meds accordingly,  check pnd labs, monitor u/o and place foley cath, check pnd labs, social service to assist with home situation (son lives with parents and patient\'s wife is legally [**month/year (2) 5720**]).\n, \n                        and the following event types with their definitions: Eating : The patient takes food into their body by mouth.\nExcretion : The patient discharges waste matter from their body.\nFamily : The patient has a visit, call, or communication with a family member.\nPain : The patient reports or shows signs of pain.\nSleep : The patient sleeps or the sleep’s quality or quantity is described.\nUnknown : choose "Unknown" if none of the other event type are applicable. \n                        ---\n                        Your task:\n                        0. Identify ALL events in the text (zero, one, or more).\n1. For each event, assign an event_type from the list above.\n2. If multiple event of same type is mentioned, assign the event_type multiple times\n3. Extract attributes for each event using ONLY the allowed attributes listed below.\n4. Use keyword evidence (Ki) ONLY if it is consistent with the text context.\n5. Output strictly valid JSON following the schema below.\n                        ---\n                        Classification Rules:\n                        - A text may contain multiple events of the same or different types.\n- Create a separate event object for each event mention.\n- If the text is explicitly a NEGATION (e.g., "denies pain"), do not extract that event.\n- If the text describes a FUTURE or HYPOTHETICAL event (e.g., "will eat tomorrow"), ignore it.\n- A valid event should have occurred in the recent past or is occurring during the time of writing of the text.\n- If no events are found or if unsure, return {"events": []}\n                        \n                        ---\n                                    Attributes allowed:\n                                    {\'Eating\': {\'food\': \'&lt;string&gt; # e.g., pancakes, porridge, etc.\', \'amount\': \'&lt;string&gt; # e.g., 1, 2 bowls, etc.\', \'method\': \'&lt;string&gt;  # e.g., oral, tube, etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, evening etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}, \'Excretion\': {\'type\': \'&lt;string&gt; # e.g., urine, stool, etc.\', \'frequency\': \'&lt;string&gt; # e.g., 2x, once, etc.\', \'quality\': \'&lt;string&gt; # e.g., loose, hard, etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, evening etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}, \'Family\': {\'interaction\': \'&lt;string&gt; # e.g., visit, call, communication, etc.\', \'relation\': \'&lt;string&gt; # e.g., mother, son, etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, evening etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}, \'Pain\': {\'severity\': \'&lt;string&gt; # e.g., mild, moderate, severe, numeric scale if present, etc.\', \'location\': \'&lt;string&gt; # e.g., right knee, head, etc.\', \'duration\': \'&lt;string&gt; # e.g., all night, 3 hours, etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, evening etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}, \'Sleep\': {\'quality\': \'&lt;string&gt; # e.g., good, poor, restless, etc.\', \'duration\': \'&lt;string&gt; # e.g., 6 hours, phrases like "all night", etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, evening etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}}\n                                    If no relevant attribute exists for an event, return an empty object {}.\n                                    \n                        \n                        ---\n                                    Keyword evidence (Ki):\n                                    Additional facts: A keyword matching algorithm without context detected keyword(s) (\'pain\', \'son\').\n                                    Use this only as a pointer. If context contradicts, ignore.\n                        ---\n                        Output Schema (strict):\n                        {\n                                    "events": [\n                                        {\n                                        "event_id": "&lt; A unique id eg.: e1 | e2 |...&gt;"\n                                        "event_type": "&lt;Pain | Sleep | Excretion | Eating | Family&gt;",\n                                        "text_quote": "&lt;fragement from the text indicating the event_type&gt;",\n                "attributes": {\n                    "&lt;attribute_name&gt;": "&lt;attribute_value&gt;"\n                }\n                                        }\n                                    ],\n                                    "order": [\n                                        ["e1", "before" | "after" | "simultaneous", "e2" ]\n                                    ]\n                                    }\n                        \n                            Rules:\n                                - Ensure the output is valid JSON (parseable).\n                                - "eventS" must always be an array (can be empty).\n                                - Multiple instances of the same event type appear with different ids.\n                                - Events appear in the array in the same order in which they appear in the text.\n                                - Their partial orders can be expressed using the "order" section.\n                                - Do not include extra keys, comments, or text.\n                                - Each object in "events" must contain "event_type", "text_quote", and "attributes".\n                                - If an event attribute type has no value mentioned, return "attributes": {"&lt; attribute name &gt;:Unknown"} for each attribute type defined for the event type \n                        \n                        \n                        \n                        ', 'event_detection_time': 17.742714701977093}</t>
         </is>
       </c>
       <c r="L2" t="inlineStr">
         <is>
-          <t>['patient lives with wife and son.  wife is legally [**month/year (2) 5720**] and patient is her primary care giver.', 'patient stopped taking lopressor 1 month ago as above (? confused it with "back pain" med), and presented to osh with c/o back pain and chills with bp up to 187/104 heart rate 104.', 'gu - urinating in urinal, but patient has spilled on himself, so i/o is inaccurate', "gi - abd is soft with +bs.  patient's last stool [**3-9**]", 'patient very anxious as wife is home alone at this point.', "social service to assist with home situation (son lives with parents and patient's wife is legally [**month/year (2) 5720**])"]</t>
+          <t>['Pain', 'Excretion', 'Excretion', 'Family', 'Pain']</t>
         </is>
       </c>
       <c r="M2" t="inlineStr">
         <is>
-          <t>{'text': 'ccu nursing admit note 0615\ns:  i stopped taking my blood pressure medicine.  i was supposed to see my doctor today.\n\no:  patient stopped taking lopressor 1 month ago as above (? confused it with "back pain" med), and presented to osh with c/o back pain and chills with bp up to 187/104 heart rate 104.\n\npmh includes afib, ascending aortic resection [**7-26**], htn.\npatient is allergic sulfa and pcn.\n\nsocially - patient lives with wife and son.  wife is legally [**month/year (2) 5720**] and patient is her primary care giver.  patient very anxious as wife is home alone at this point.\n\ncv - heart rate 130\'s 2:1 block, bp down to 104/70 on nipride .5mcg/kg/min and labetolol .73mg/min.  [**month/year (2) **] placed l radial in er.\n\nresp - o2 on 3ln/p with oxygen saturation 95-97% with decreased bs at bases\n\ngi - abd is soft with +bs.  patient\'s last stool [**3-9**]\n\ngu - urinating in urinal, but patient has spilled on himself, so i/o is inaccurate\n\nlabs - pnd\n\na:  84yom with history aortic aneurism now presents with htn as he self dc/d his lopressor\n\np:  monitor heart rate with goal 60 and bp with goal 100/.  titrate meds accordingly,  check pnd labs, monitor u/o and place foley cath, check pnd labs, social service to assist with home situation (son lives with parents and patient\'s wife is legally [**month/year (2) 5720**]).\n', 'event': ['Pain', 'Excretion', 'Excretion', 'Family', 'Family'], 'phrase': '', 'raw_output': '{\n  "events": [\n    {\n      "event_type": "Pain",\n      "text_quote": "c/o back pain and chills",\n      "attributes": {\n        "severity": "Unknown",\n        "location": "back",\n        "duration": "Unknown",\n        "time": "Unknown",\n        "caused_by": "Unknown"\n      }\n    },\n    {\n      "event_type": "Excretion",\n      "text_quote": "urinating in urinal, but patient has spilled on himself",\n      "attributes": {\n        "type": "urine",\n        "frequency": "Unknown",\n        "quality": "Unknown",\n        "negation": "false",\n        "time": "Unknown",\n        "caused_by": "Unknown"\n      }\n    },\n    {\n      "event_type": "Excretion",\n      "text_quote": "patient\'s last stool [3-9]",\n      "attributes": {\n        "type": "stool",\n        "frequency": "[3-9]",\n        "quality": "Unknown",\n        "negation": "false",\n        "time": "Unknown",\n        "caused_by": "Unknown"\n      }\n    },\n    {\n      "event_type": "Family",\n      "text_quote": "patient lives with wife and son.  wife is legally [month/year (2) 5720] and patient is her primary care giver.",\n      "attributes": {\n        "interaction": "Unknown",\n        "relation": "wife and son",\n        "negation": "false",\n        "time": "Unknown",\n        "caused_by": "Unknown"\n      }\n    },\n    {\n      "event_type": "Family",\n      "text_quote": "patient very anxious as wife is home alone at this point.",\n      "attributes": {\n        "interaction": "Unknown",\n        "relation": "wife",\n        "negation": "false",\n        "time": "Unknown",\n        "caused_by": "Unknown"\n      }\n    }\n  ]\n}', 'attributes': [{'Pain': {'severity': 'Unknown', 'location': 'back', 'duration': 'Unknown', 'time': 'Unknown', 'caused_by': 'Unknown'}}, {'Excretion': {'type': 'urine', 'frequency': 'Unknown', 'quality': 'Unknown', 'negation': 'false', 'time': 'Unknown', 'caused_by': 'Unknown'}}, {'Excretion': {'type': 'stool', 'frequency': '[3-9]', 'quality': 'Unknown', 'negation': 'false', 'time': 'Unknown', 'caused_by': 'Unknown'}}, {'Family': {'interaction': 'Unknown', 'relation': 'wife and son', 'negation': 'false', 'time': 'Unknown', 'caused_by': 'Unknown'}}, {'Family': {'interaction': 'Unknown', 'relation': 'wife', 'negation': 'false', 'time': 'Unknown', 'caused_by': 'Unknown'}}], 'text_quotes': ['c/o back pain and chills', 'urinating in urinal, but patient has spilled on himself', "patient's last stool [3-9]", 'patient lives with wife and son.  wife is legally [month/year (2) 5720] and patient is her primary care giver.', 'patient very anxious as wife is home alone at this point.'], 'event_name_prompt': 'Given the text: ccu nursing admit note 0615\ns:  i stopped taking my blood pressure medicine.  i was supposed to see my doctor today.\n\no:  patient stopped taking lopressor 1 month ago as above (? confused it with "back pain" med), and presented to osh with c/o back pain and chills with bp up to 187/104 heart rate 104.\n\npmh includes afib, ascending aortic resection [**7-26**], htn.\npatient is allergic sulfa and pcn.\n\nsocially - patient lives with wife and son.  wife is legally [**month/year (2) 5720**] and patient is her primary care giver.  patient very anxious as wife is home alone at this point.\n\ncv - heart rate 130\'s 2:1 block, bp down to 104/70 on nipride .5mcg/kg/min and labetolol .73mg/min.  [**month/year (2) **] placed l radial in er.\n\nresp - o2 on 3ln/p with oxygen saturation 95-97% with decreased bs at bases\n\ngi - abd is soft with +bs.  patient\'s last stool [**3-9**]\n\ngu - urinating in urinal, but patient has spilled on himself, so i/o is inaccurate\n\nlabs - pnd\n\na:  84yom with history aortic aneurism now presents with htn as he self dc/d his lopressor\n\np:  monitor heart rate with goal 60 and bp with goal 100/.  titrate meds accordingly,  check pnd labs, monitor u/o and place foley cath, check pnd labs, social service to assist with home situation (son lives with parents and patient\'s wife is legally [**month/year (2) 5720**]).\n, \n                        and the following event types with their definitions: Eating : The patient takes food into their body by mouth.\nExcretion : The patient discharges waste matter from their body.\nFamily : The patient has a visit, call, or communication with a family member.\nPain : The patient reports or shows signs of pain.\nSleep : The patient sleeps or the sleep’s quality or quantity is described.\nUnknown : choose "Unknown" if none of the other event type are applicable. \n                        ---\n                        Your task:\n                        0. Identify ALL events in the text (zero, one, or more).\n1. For each event, assign an event_type from the list above.\n2. If multiple event of same type is mentioned, assign the event_type multiple times\n3. Extract attributes for each event using ONLY the allowed attributes listed below.\n4. Output strictly valid JSON following the schema below.\n                        ---\n                        Classification Rules:\n                        - A text may contain multiple events of the same or different types.\n- Create a separate event object for each event mention.\n- If the text is explicitly a NEGATION (e.g., "denies pain"), do not extract that event.\n- If the text describes a FUTURE or HYPOTHETICAL event (e.g., "will eat tomorrow"), ignore it.\n- A valid event should have occurred in the recent past or is occurring during the time of writing of the text.\n- If no events are found or if unsure, return {"events": []}\n                        \n                        ---\n                                    Attributes allowed:\n                                    {\'Eating\': {\'food\': \'&lt;string&gt; # e.g., pancakes, porridge, etc.\', \'amount\': \'&lt;string&gt; # e.g., 1, 2 bowls, etc.\', \'method\': \'&lt;string&gt;  # e.g., oral, tube, etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, after shower, etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}, \'Excretion\': {\'type\': \'&lt;string&gt; # e.g., urine, stool, etc.\', \'frequency\': \'&lt;string&gt; # e.g., 2x, once, etc.\', \'quality\': \'&lt;string&gt; # e.g., loose, hard, etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, after shower, etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}, \'Family\': {\'interaction\': \'&lt;string&gt; # e.g., visit, call, communication, etc.\', \'relation\': \'&lt;string&gt; # e.g., mother, son, etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, after shower, etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}, \'Pain\': {\'severity\': \'&lt;string&gt; # e.g., mild, moderate, severe, numeric scale if present, etc.\', \'location\': \'&lt;string&gt; # e.g., right knee, head, etc.\', \'duration\': \'&lt;string&gt; # e.g., all night, 3 hours, etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, after shower, etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}, \'Sleep\': {\'quality\': \'&lt;string&gt; # e.g., good, poor, restless, etc.\', \'duration\': \'&lt;string&gt; # e.g., 6 hours, phrases like "all night", etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, after shower, etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}}\n                                    If no relevant attribute exists for an event, return an empty object {}.\n                                    \n                        \n                        \n                        ---\n                        Output Schema (strict):\n                        {\n                                    "events": [\n                                        {\n                                        "event_type": "&lt;Pain | Sleep | Excretion | Eating | Family&gt;",\n                                        "text_quote": "&lt;fragement from the text indicating &gt;",\n                "attributes": {\n                    "&lt;attribute_name&gt;": "&lt;attribute_value&gt;"\n                }\n                                        }\n                                    ]\n                                    }\n                        \n                            Rules:\n                                - Ensure the output is valid JSON (parseable).\n                                - "eventS" must always be an array (can be empty).\n                                - Multiple instances of the same event type appear as individual elements in the event array.\n                                - Events appear in the array in the same order in which they appear in the text.\n                                - Do not include extra keys, comments, or text.\n                                - Each object in "events" must contain "event_type", "text_quote", and "attributes".\n                                -If an event attribute type has no value mentioned, return "attributes": {"&lt; attribute name &gt;:Unknown"} for each attribute type defined for the event type \n                        \n                        \n                        \n                ---\n                Examples:\n                \n                text: "Patient ate breakfast this morning. He seems less anxious."\n                output: {\n                "events": [\n                    {\n                    "event_type": "Eating",\n                    "text_quote":"Patient ate breakfast this morning",\n                    "attributes": {"food": "breakfast", \n                                   "amount": "Unknown",\n                                   "method": "Unknown",\n                                   "time":"morning",\n                                   "caused_by":"Unknown"}\n                    }\n                ]\n                }\n                \n                text: "Patient reported severe abdominal pain."\n                output: {\n                "events": [\n                    {\n                    "event_type": "Pain",\n                    "text_quote": "severe abdominal Pain",\n                    "attributes": {"severity": "severe", \n                                   "location": "abdominal",\n                                   "duration": "Unknown",\n                                   "time":"Unknown",\n                                   "caused_by":"Unknown"}\n                    }\n                ]\n                }\n                \n                text: "Patient called his son around 3 pm."\n                output: {\n                "events": [\n                    {\n                    "event_type": "Family",\n                    "text_quote": "called his son around 3 pm",\n                    "attributes": {"interaction": "call", \n                                    "relation": "son",\n                                    "time":"3 pm",\n                                    "caused_by":"Unknown"}\n                    }\n                ]\n                }\n                \n                text: "Patient had a loose stool overnight."\n                output: {\n                "events": [\n                    {\n                    "event_type": "Excretion",\n                    "text_quote": "loose stool overnight",\n                    "attributes": {"type": "stool", \n                                   "quality": "loose", \n                                   "frequency":"overnight", \n                                   "time":"night",\n                                   "caused_by":"Unknown"}\n                    }\n                ]\n                }\n                \n                text: "Patient was able to sleep well last night."\n                output: {\n                "events": [\n                    {\n                    "event_type": "Sleep",\n                    "text_quote": "sleep well last night",\n                    "attributes": {"quality": "well",\n                                    "duration": "Unknown", \n                                    "time":"night",\n                                    "caused_by":"Unknown"}\n                    }\n                ]\n                }\n                \n                text: "The patient couldn\'t sleep due to severe pain."\n                output: {\n                "events": [\n                    {\n                    "event_type": "Sleep",\n                    "text_quote": "couldn\'t sleep",\n                    "attributes": {"quality": "poor", \n                                    "duration": "Unknown",\n                                   "time":"Unknown",\n                                   "caused_by":"Pain"}\n                    },\n                    {\n                    "event_type": "Pain",\n                    "text_quote": "severe pain",\n                    "attributes": {"severity": "severe", \n                                    "location": "Unknown", \n                                    "duration": "Unknown", \n                                   "time":"before Sleep",\n                                   "caused_by":"Unknown"}\n                    }\n                ]\n                }\n                \n                text: "The patient complained of severe back pain, was given Tylenol, but the pain persisted and he was then prescribed stronger morphine."\n                output: {\n                "events": [\n                    {\n                    "event_type": "Pain",\n                    "text_quote": "complained of severe back pain",\n                    "attributes": {"severity": "severe", \n                                    "location": "back",\n                                    "duration": "Unknown", \n                                    "time":"Unknown",\n                                    "caused_by":"Unknown"}\n                    },\n                    {\n                    "event_type": "Pain",\n                    "text_quote": "pain persisted",\n                    "attributes": {"severity": "severe", \n                                   "location": "back",\n                                   "duration": "persistent", \n                                   "time":"after Tylenol",\n                                   "caused_by":"Unknown"}\n                    }\n                ]\n                }\n                \n                        ', 'event_detection_time': 14.698525070998585}</t>
+          <t>[{'Pain': {'severity': 'Unknown', 'location': 'back', 'duration': 'Unknown', 'negation': False, 'time': 'Unknown', 'caused_by': 'Unknown'}}, {'Excretion': {'type': 'stool', 'frequency': 'Unknown', 'quality': 'Unknown', 'negation': False, 'time': '[**3-9**]', 'caused_by': 'Unknown'}}, {'Excretion': {'type': 'urine', 'frequency': 'Unknown', 'quality': 'Unknown', 'negation': False, 'time': 'Unknown', 'caused_by': 'Unknown'}}, {'Family': {'interaction': 'Unknown', 'relation': 'wife, son', 'negation': False, 'time': 'Unknown', 'caused_by': 'Unknown'}}, {'Pain': {'severity': 'Unknown', 'location': 'back', 'duration': 'Unknown', 'negation': False, 'time': 'Unknown', 'caused_by': 'Unknown'}}]</t>
         </is>
       </c>
       <c r="N2" t="inlineStr">
         <is>
-          <t>['Pain', 'Excretion', 'Excretion', 'Family', 'Family']</t>
+          <t>['c/o back pain and chills with bp up to 187/104 heart rate 104.', "patient's last stool [**3-9**]", 'urinating in urinal, but patient has spilled on himself, so i/o is inaccurate', 'patient lives with wife and son.  wife is legally [**month/year (2) 5720**] and patient is her primary care giver.', 'back pain']</t>
         </is>
       </c>
       <c r="O2" t="inlineStr">
         <is>
-          <t>[{'Pain': {'severity': 'Unknown', 'location': 'back', 'duration': 'Unknown', 'time': 'Unknown', 'caused_by': 'Unknown'}}, {'Excretion': {'type': 'urine', 'frequency': 'Unknown', 'quality': 'Unknown', 'negation': 'false', 'time': 'Unknown', 'caused_by': 'Unknown'}}, {'Excretion': {'type': 'stool', 'frequency': '[3-9]', 'quality': 'Unknown', 'negation': 'false', 'time': 'Unknown', 'caused_by': 'Unknown'}}, {'Family': {'interaction': 'Unknown', 'relation': 'wife and son', 'negation': 'false', 'time': 'Unknown', 'caused_by': 'Unknown'}}, {'Family': {'interaction': 'Unknown', 'relation': 'wife', 'negation': 'false', 'time': 'Unknown', 'caused_by': 'Unknown'}}]</t>
-        </is>
-      </c>
-      <c r="P2" t="inlineStr">
-        <is>
-          <t>['c/o back pain and chills', 'urinating in urinal, but patient has spilled on himself', "patient's last stool [3-9]", 'patient lives with wife and son.  wife is legally [month/year (2) 5720] and patient is her primary care giver.', 'patient very anxious as wife is home alone at this point.']</t>
-        </is>
-      </c>
-      <c r="Q2" t="n">
-        <v>0.003099834999375162</v>
-      </c>
-      <c r="R2" t="inlineStr">
+          <t>[[['e1', 'before', 'e2'], ['e2', 'before', 'e3'], ['e3', 'before', 'e4'], ['e4', 'before', 'e5']]]</t>
+        </is>
+      </c>
+      <c r="P2" t="n">
+        <v>0.00252554200051236</v>
+      </c>
+      <c r="Q2" t="inlineStr">
         <is>
           <t>Sleep</t>
         </is>
       </c>
-      <c r="S2" t="b">
+      <c r="R2" t="b">
+        <v>0</v>
+      </c>
+      <c r="S2" t="n">
         <v>0</v>
       </c>
       <c r="T2" t="n">
         <v>0</v>
       </c>
-      <c r="U2" t="n">
-        <v>0</v>
-      </c>
-      <c r="V2" t="inlineStr">
+      <c r="U2" t="inlineStr">
         <is>
           <t>('pain', 'son')</t>
         </is>
       </c>
+      <c r="V2" t="n">
+        <v>16.14568631898146</v>
+      </c>
       <c r="W2" t="n">
-        <v>16.22530980499869</v>
+        <v>17.74271470197709</v>
       </c>
       <c r="X2" t="n">
-        <v>18.85099622399139</v>
+        <v>0</v>
       </c>
       <c r="Y2" t="n">
-        <v>14.69852507099858</v>
+        <v>0</v>
       </c>
       <c r="Z2" t="n">
-        <v>0</v>
-      </c>
-      <c r="AA2" t="n">
-        <v>0</v>
-      </c>
-      <c r="AB2" t="n">
-        <v>0</v>
-      </c>
-      <c r="AC2" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="n">
-        <v>1310479</v>
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>1310479</t>
+        </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>['Pain', 'Sleep', 'Family', 'Unknown']</t>
+          <t>('Pain', 'Sleep', 'Family', 'Unknown')</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>['daughter', 'son', 'pain', 'sleeping', 'asleep', 'distress']</t>
+          <t>('asleep', 'daughter', 'son', 'pain', 'distress', 'sleeping')</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
@@ -762,118 +740,111 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>{'text': 'ccu nsg progress note 7p-7a/ aortic dissection\n\n\ns- "i have a little pain..not much..."\n\no-\n\n[**name (ni) 231**] patient initially on neo 0.86 mcg to keep maps &gt; 60. heart rate- 70\'s sr, no vea- bp- 86/40-120/58- rt ij inserted on eves- initial filling pressures wnl- high normal- pa- 40/18, pcw-18-22, cvp-16-18.\nco/ci/svr- 3.3/1.79/1624--started 0.375 mcg milrinone after 50mcg bolus. improved co/ci/svr- 5.7/3.1/730 but unable to wean neo much less than 0.7 mcg neo currently. while asleep- bp /pa # dropping , but improving once awake.\n\nresp- 6l np- some apnea, mouth breathing- oxygen saturation- 99-100%- down to 90-92% when mouth breathing/apnea periods occasionally.\nno distress/comfortable- no further diuresis nor ivf bolus for i/o (-)500cc as of 12am.\n\nid- afebrile\n\ngu- poor uo since mid afternoon hypotension and post diuresis.\neve creatinine- 1.7- am levels pending.\nnot much change in uo even after change in co/ci.\n\ngi- npo - taking small sips to wet mouth- took pm dose amiodorone and immediately felt nauseas, vomited- 100cc- felt ok afterwards- same nausea as with previous dose and emesis- but no hemodynamic changes this time- no vagal or hypotension.\nremains on protonix qd.\n\n[**name (ni) 324**] patient sedate, but easily [**name (ni) 8718**] son present all eve while pa line inserted- both aware of plan of care and reason for new invasive line.\npatient sleeping all of shift but for when woken up for questions.\nlast sedation given friday morning with tee/cdv- fent/versed/propofol.\n\na/[**name (ni) **] patient with hypotensive events requiring pressor initiation currently doing well on milrinone drops\nremains with poor uo/need for neo to maintain maps.\n\ncontinue to wean off neo today as tolerated once less sedate and not sleeping.\ncheck with team before attempting 3rd dose of amiodorone as has not tolerated past 2 doses.\nwatch for any further hypotension or tachyarrythnias.\ndiscuss with team ? more fluid today- await am creatine level as well as other lytes.\nserial hct/continue to assess for back pain/ type/location/level of pain. repeat diagnostics- ct/mri as needed if pain worsens or changes in nature.\nkeep patient and son/daughter aware of plan of care.\nnpo.\n\n', 'event': ['Pain'], 'phrase': '', 'raw_output': '{\n  "events": [\n    {\n      "event_type": "Pain",\n      "text_quote": "" \n      },\n      "attributes" \n        ]\n      }', 'attributes': [{'Pain': {}}], 'text_quotes': [''], 'event_name_prompt': 'Given the text: ccu nsg progress note 7p-7a/ aortic dissection\n\n\ns- "i have a little pain..not much..."\n\no-\n\n[**name (ni) 231**] patient initially on neo 0.86 mcg to keep maps &gt; 60. heart rate- 70\'s sr, no vea- bp- 86/40-120/58- rt ij inserted on eves- initial filling pressures wnl- high normal- pa- 40/18, pcw-18-22, cvp-16-18.\nco/ci/svr- 3.3/1.79/1624--started 0.375 mcg milrinone after 50mcg bolus. improved co/ci/svr- 5.7/3.1/730 but unable to wean neo much less than 0.7 mcg neo currently. while asleep- bp /pa # dropping , but improving once awake.\n\nresp- 6l np- some apnea, mouth breathing- oxygen saturation- 99-100%- down to 90-92% when mouth breathing/apnea periods occasionally.\nno distress/comfortable- no further diuresis nor ivf bolus for i/o (-)500cc as of 12am.\n\nid- afebrile\n\ngu- poor uo since mid afternoon hypotension and post diuresis.\neve creatinine- 1.7- am levels pending.\nnot much change in uo even after change in co/ci.\n\ngi- npo - taking small sips to wet mouth- took pm dose amiodorone and immediately felt nauseas, vomited- 100cc- felt ok afterwards- same nausea as with previous dose and emesis- but no hemodynamic changes this time- no vagal or hypotension.\nremains on protonix qd.\n\n[**name (ni) 324**] patient sedate, but easily [**name (ni) 8718**] son present all eve while pa line inserted- both aware of plan of care and reason for new invasive line.\npatient sleeping all of shift but for when woken up for questions.\nlast sedation given friday morning with tee/cdv- fent/versed/propofol.\n\na/[**name (ni) **] patient with hypotensive events requiring pressor initiation currently doing well on milrinone drops\nremains with poor uo/need for neo to maintain maps.\n\ncontinue to wean off neo today as tolerated once less sedate and not sleeping.\ncheck with team before attempting 3rd dose of amiodorone as has not tolerated past 2 doses.\nwatch for any further hypotension or tachyarrythnias.\ndiscuss with team ? more fluid today- await am creatine level as well as other lytes.\nserial hct/continue to assess for back pain/ type/location/level of pain. repeat diagnostics- ct/mri as needed if pain worsens or changes in nature.\nkeep patient and son/daughter aware of plan of care.\nnpo.\n\n, \n                        and the following event types with their definitions: Eating : The patient takes food into their body by mouth.\nExcretion : The patient discharges waste matter from their body.\nFamily : The patient has a visit, call, or communication with a family member.\nPain : The patient reports or shows signs of pain.\nSleep : The patient sleeps or the sleep’s quality or quantity is described.\nUnknown : choose "Unknown" if none of the other event type are applicable. \n                        ---\n                        Your task:\n                        0. Identify ALL events in the text (zero, one, or more).\n1. For each event, assign an event_type from the list above.\n2. If multiple event of same type is mentioned, assign the event_type multiple times\n3. Extract attributes for each event using ONLY the allowed attributes listed below.\n4. Use keyword evidence (Ki) ONLY if it is consistent with the text context.\n5. Output strictly valid JSON following the schema below.\n                        ---\n                        Classification Rules:\n                        - A text may contain multiple events of the same or different types.\n- Create a separate event object for each event mention.\n- If the text is explicitly a NEGATION (e.g., "denies pain"), do not extract that event.\n- If the text describes a FUTURE or HYPOTHETICAL event (e.g., "will eat tomorrow"), ignore it.\n- A valid event should have occurred in the recent past or is occurring during the time of writing of the text.\n- If no events are found or if unsure, return {"events": []}\n                        \n                        ---\n                                    Attributes allowed:\n                                    {\'Eating\': {\'food\': \'&lt;string&gt; # e.g., pancakes, porridge, etc.\', \'amount\': \'&lt;string&gt; # e.g., 1, 2 bowls, etc.\', \'method\': \'&lt;string&gt;  # e.g., oral, tube, etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, after shower, etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}, \'Excretion\': {\'type\': \'&lt;string&gt; # e.g., urine, stool, etc.\', \'frequency\': \'&lt;string&gt; # e.g., 2x, once, etc.\', \'quality\': \'&lt;string&gt; # e.g., loose, hard, etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, after shower, etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}, \'Family\': {\'interaction\': \'&lt;string&gt; # e.g., visit, call, communication, etc.\', \'relation\': \'&lt;string&gt; # e.g., mother, son, etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, after shower, etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}, \'Pain\': {\'severity\': \'&lt;string&gt; # e.g., mild, moderate, severe, numeric scale if present, etc.\', \'location\': \'&lt;string&gt; # e.g., right knee, head, etc.\', \'duration\': \'&lt;string&gt; # e.g., all night, 3 hours, etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, after shower, etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}, \'Sleep\': {\'quality\': \'&lt;string&gt; # e.g., good, poor, restless, etc.\', \'duration\': \'&lt;string&gt; # e.g., 6 hours, phrases like "all night", etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, after shower, etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}}\n                                    If no relevant attribute exists for an event, return an empty object {}.\n                                    \n                        \n                        ---\n                                    Keyword evidence (Ki):\n                                    Additional facts: A keyword matching algorithm without context detected keyword(s) [\'daughter\', \'son\', \'pain\', \'sleeping\', \'asleep\', \'distress\'].\n                                    Use this only as a pointer. If context contradicts, ignore.\n                        ---\n                        Output Schema (strict):\n                        {\n                                    "events": [\n                                        {\n                                        "event_type": "&lt;Pain | Sleep | Excretion | Eating | Family&gt;",\n                                        "text_quote": "&lt;fragement from the text indicating &gt;",\n                "attributes": {\n                    "&lt;attribute_name&gt;": "&lt;attribute_value&gt;"\n                }\n                                        }\n                                    ]\n                                    }\n                        \n                            Rules:\n                                - Ensure the output is valid JSON (parseable).\n                                - "eventS" must always be an array (can be empty).\n                                - Multiple instances of the same event type appear as individual elements in the event array.\n                                - Events appear in the array in the same order in which they appear in the text.\n                                - Do not include extra keys, comments, or text.\n                                - Each object in "events" must contain "event_type", "text_quote", and "attributes".\n                                -If an event attribute type has no value mentioned, return "attributes": {"&lt; attribute name &gt;:Unknown"} for each attribute type defined for the event type \n                        \n                        \n                        \n                ---\n                Examples:\n                \n                text: "Patient ate breakfast this morning. He seems less anxious."\n                output: {\n                "events": [\n                    {\n                    "event_type": "Eating",\n                    "text_quote":"Patient ate breakfast this morning",\n                    "attributes": {"food": "breakfast", \n                                   "amount": "Unknown",\n                                   "method": "Unknown",\n                                   "time":"morning",\n                                   "caused_by":"Unknown"}\n                    }\n                ]\n                }\n                \n                text: "Patient reported severe abdominal pain."\n                output: {\n                "events": [\n                    {\n                    "event_type": "Pain",\n                    "text_quote": "severe abdominal Pain",\n                    "attributes": {"severity": "severe", \n                                   "location": "abdominal",\n                                   "duration": "Unknown",\n                                   "time":"Unknown",\n                                   "caused_by":"Unknown"}\n                    }\n                ]\n                }\n                \n                text: "Patient called his son around 3 pm."\n                output: {\n                "events": [\n                    {\n                    "event_type": "Family",\n                    "text_quote": "called his son around 3 pm",\n                    "attributes": {"interaction": "call", \n                                    "relation": "son",\n                                    "time":"3 pm",\n                                    "caused_by":"Unknown"}\n                    }\n                ]\n                }\n                \n                text: "Patient had a loose stool overnight."\n                output: {\n                "events": [\n                    {\n                    "event_type": "Excretion",\n                    "text_quote": "loose stool overnight",\n                    "attributes": {"type": "stool", \n                                   "quality": "loose", \n                                   "frequency":"overnight", \n                                   "time":"night",\n                                   "caused_by":"Unknown"}\n                    }\n                ]\n                }\n                \n                text: "Patient was able to sleep well last night."\n                output: {\n                "events": [\n                    {\n                    "event_type": "Sleep",\n                    "text_quote": "sleep well last night",\n                    "attributes": {"quality": "well",\n                                    "duration": "Unknown", \n                                    "time":"night",\n                                    "caused_by":"Unknown"}\n                    }\n                ]\n                }\n                \n                text: "The patient couldn\'t sleep due to severe pain."\n                output: {\n                "events": [\n                    {\n                    "event_type": "Sleep",\n                    "text_quote": "couldn\'t sleep",\n                    "attributes": {"quality": "poor", \n                                    "duration": "Unknown",\n                                   "time":"Unknown",\n                                   "caused_by":"Pain"}\n                    },\n                    {\n                    "event_type": "Pain",\n                    "text_quote": "severe pain",\n                    "attributes": {"severity": "severe", \n                                    "location": "Unknown", \n                                    "duration": "Unknown", \n                                   "time":"before Sleep",\n                                   "caused_by":"Unknown"}\n                    }\n                ]\n                }\n                \n                text: "The patient complained of severe back pain, was given Tylenol, but the pain persisted and he was then prescribed stronger morphine."\n                output: {\n                "events": [\n                    {\n                    "event_type": "Pain",\n                    "text_quote": "complained of severe back pain",\n                    "attributes": {"severity": "severe", \n                                    "location": "back",\n                                    "duration": "Unknown", \n                                    "time":"Unknown",\n                                    "caused_by":"Unknown"}\n                    },\n                    {\n                    "event_type": "Pain",\n                    "text_quote": "pain persisted",\n                    "attributes": {"severity": "severe", \n                                   "location": "back",\n                                   "duration": "persistent", \n                                   "time":"after Tylenol",\n                                   "caused_by":"Unknown"}\n                    }\n                ]\n                }\n                \n                        ', 'event_detection_time': 3.828834353989805}</t>
+          <t>['asleep', 'daughter', 'son', 'pain', 'distress', 'sleeping']</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
+          <t>{'text': 'ccu nsg progress note 7p-7a/ aortic dissection\n\n\ns- "i have a little pain..not much..."\n\no-\n\n[**name (ni) 231**] patient initially on neo 0.86 mcg to keep maps &gt; 60. heart rate- 70\'s sr, no vea- bp- 86/40-120/58- rt ij inserted on eves- initial filling pressures wnl- high normal- pa- 40/18, pcw-18-22, cvp-16-18.\nco/ci/svr- 3.3/1.79/1624--started 0.375 mcg milrinone after 50mcg bolus. improved co/ci/svr- 5.7/3.1/730 but unable to wean neo much less than 0.7 mcg neo currently. while asleep- bp /pa # dropping , but improving once awake.\n\nresp- 6l np- some apnea, mouth breathing- oxygen saturation- 99-100%- down to 90-92% when mouth breathing/apnea periods occasionally.\nno distress/comfortable- no further diuresis nor ivf bolus for i/o (-)500cc as of 12am.\n\nid- afebrile\n\ngu- poor uo since mid afternoon hypotension and post diuresis.\neve creatinine- 1.7- am levels pending.\nnot much change in uo even after change in co/ci.\n\ngi- npo - taking small sips to wet mouth- took pm dose amiodorone and immediately felt nauseas, vomited- 100cc- felt ok afterwards- same nausea as with previous dose and emesis- but no hemodynamic changes this time- no vagal or hypotension.\nremains on protonix qd.\n\n[**name (ni) 324**] patient sedate, but easily [**name (ni) 8718**] son present all eve while pa line inserted- both aware of plan of care and reason for new invasive line.\npatient sleeping all of shift but for when woken up for questions.\nlast sedation given friday morning with tee/cdv- fent/versed/propofol.\n\na/[**name (ni) **] patient with hypotensive events requiring pressor initiation currently doing well on milrinone drops\nremains with poor uo/need for neo to maintain maps.\n\ncontinue to wean off neo today as tolerated once less sedate and not sleeping.\ncheck with team before attempting 3rd dose of amiodorone as has not tolerated past 2 doses.\nwatch for any further hypotension or tachyarrythnias.\ndiscuss with team ? more fluid today- await am creatine level as well as other lytes.\nserial hct/continue to assess for back pain/ type/location/level of pain. repeat diagnostics- ct/mri as needed if pain worsens or changes in nature.\nkeep patient and son/daughter aware of plan of care.\nnpo.\n\n', 'event': ['Pain'], 'event_id': ['e1'], 'phrase': '', 'raw_output': '{\n  "events": [\n    {\n      "event_id": "e1",\n      "event_type": "Pain",\n      "text_quote": "" \n      },\n      "attributes" \n        ]\n      }', 'attributes': [{'Pain': {}}], 'orders': [], 'text_quotes': [''], 'event_name_prompt': 'Given the text: ccu nsg progress note 7p-7a/ aortic dissection\n\n\ns- "i have a little pain..not much..."\n\no-\n\n[**name (ni) 231**] patient initially on neo 0.86 mcg to keep maps &gt; 60. heart rate- 70\'s sr, no vea- bp- 86/40-120/58- rt ij inserted on eves- initial filling pressures wnl- high normal- pa- 40/18, pcw-18-22, cvp-16-18.\nco/ci/svr- 3.3/1.79/1624--started 0.375 mcg milrinone after 50mcg bolus. improved co/ci/svr- 5.7/3.1/730 but unable to wean neo much less than 0.7 mcg neo currently. while asleep- bp /pa # dropping , but improving once awake.\n\nresp- 6l np- some apnea, mouth breathing- oxygen saturation- 99-100%- down to 90-92% when mouth breathing/apnea periods occasionally.\nno distress/comfortable- no further diuresis nor ivf bolus for i/o (-)500cc as of 12am.\n\nid- afebrile\n\ngu- poor uo since mid afternoon hypotension and post diuresis.\neve creatinine- 1.7- am levels pending.\nnot much change in uo even after change in co/ci.\n\ngi- npo - taking small sips to wet mouth- took pm dose amiodorone and immediately felt nauseas, vomited- 100cc- felt ok afterwards- same nausea as with previous dose and emesis- but no hemodynamic changes this time- no vagal or hypotension.\nremains on protonix qd.\n\n[**name (ni) 324**] patient sedate, but easily [**name (ni) 8718**] son present all eve while pa line inserted- both aware of plan of care and reason for new invasive line.\npatient sleeping all of shift but for when woken up for questions.\nlast sedation given friday morning with tee/cdv- fent/versed/propofol.\n\na/[**name (ni) **] patient with hypotensive events requiring pressor initiation currently doing well on milrinone drops\nremains with poor uo/need for neo to maintain maps.\n\ncontinue to wean off neo today as tolerated once less sedate and not sleeping.\ncheck with team before attempting 3rd dose of amiodorone as has not tolerated past 2 doses.\nwatch for any further hypotension or tachyarrythnias.\ndiscuss with team ? more fluid today- await am creatine level as well as other lytes.\nserial hct/continue to assess for back pain/ type/location/level of pain. repeat diagnostics- ct/mri as needed if pain worsens or changes in nature.\nkeep patient and son/daughter aware of plan of care.\nnpo.\n\n, \n                        and the following event types with their definitions: Eating : The patient takes food into their body by mouth.\nExcretion : The patient discharges waste matter from their body.\nFamily : The patient has a visit, call, or communication with a family member.\nPain : The patient reports or shows signs of pain.\nSleep : The patient sleeps or the sleep’s quality or quantity is described.\nUnknown : choose "Unknown" if none of the other event type are applicable. \n                        ---\n                        Your task:\n                        0. Identify ALL events in the text (zero, one, or more).\n1. For each event, assign an event_type from the list above.\n2. If multiple event of same type is mentioned, assign the event_type multiple times\n3. Extract attributes for each event using ONLY the allowed attributes listed below.\n4. Use keyword evidence (Ki) ONLY if it is consistent with the text context.\n5. Output strictly valid JSON following the schema below.\n                        ---\n                        Classification Rules:\n                        - A text may contain multiple events of the same or different types.\n- Create a separate event object for each event mention.\n- If the text is explicitly a NEGATION (e.g., "denies pain"), do not extract that event.\n- If the text describes a FUTURE or HYPOTHETICAL event (e.g., "will eat tomorrow"), ignore it.\n- A valid event should have occurred in the recent past or is occurring during the time of writing of the text.\n- If no events are found or if unsure, return {"events": []}\n                        \n                        ---\n                                    Attributes allowed:\n                                    {\'Eating\': {\'food\': \'&lt;string&gt; # e.g., pancakes, porridge, etc.\', \'amount\': \'&lt;string&gt; # e.g., 1, 2 bowls, etc.\', \'method\': \'&lt;string&gt;  # e.g., oral, tube, etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, evening etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}, \'Excretion\': {\'type\': \'&lt;string&gt; # e.g., urine, stool, etc.\', \'frequency\': \'&lt;string&gt; # e.g., 2x, once, etc.\', \'quality\': \'&lt;string&gt; # e.g., loose, hard, etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, evening etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}, \'Family\': {\'interaction\': \'&lt;string&gt; # e.g., visit, call, communication, etc.\', \'relation\': \'&lt;string&gt; # e.g., mother, son, etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, evening etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}, \'Pain\': {\'severity\': \'&lt;string&gt; # e.g., mild, moderate, severe, numeric scale if present, etc.\', \'location\': \'&lt;string&gt; # e.g., right knee, head, etc.\', \'duration\': \'&lt;string&gt; # e.g., all night, 3 hours, etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, evening etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}, \'Sleep\': {\'quality\': \'&lt;string&gt; # e.g., good, poor, restless, etc.\', \'duration\': \'&lt;string&gt; # e.g., 6 hours, phrases like "all night", etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, evening etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}}\n                                    If no relevant attribute exists for an event, return an empty object {}.\n                                    \n                        \n                        ---\n                                    Keyword evidence (Ki):\n                                    Additional facts: A keyword matching algorithm without context detected keyword(s) (\'asleep\', \'daughter\', \'son\', \'pain\', \'distress\', \'sleeping\').\n                                    Use this only as a pointer. If context contradicts, ignore.\n                        ---\n                        Output Schema (strict):\n                        {\n                                    "events": [\n                                        {\n                                        "event_id": "&lt; A unique id eg.: e1 | e2 |...&gt;"\n                                        "event_type": "&lt;Pain | Sleep | Excretion | Eating | Family&gt;",\n                                        "text_quote": "&lt;fragement from the text indicating the event_type&gt;",\n                "attributes": {\n                    "&lt;attribute_name&gt;": "&lt;attribute_value&gt;"\n                }\n                                        }\n                                    ],\n                                    "order": [\n                                        ["e1", "before" | "after" | "simultaneous", "e2" ]\n                                    ]\n                                    }\n                        \n                            Rules:\n                                - Ensure the output is valid JSON (parseable).\n                                - "eventS" must always be an array (can be empty).\n                                - Multiple instances of the same event type appear with different ids.\n                                - Events appear in the array in the same order in which they appear in the text.\n                                - Their partial orders can be expressed using the "order" section.\n                                - Do not include extra keys, comments, or text.\n                                - Each object in "events" must contain "event_type", "text_quote", and "attributes".\n                                - If an event attribute type has no value mentioned, return "attributes": {"&lt; attribute name &gt;:Unknown"} for each attribute type defined for the event type \n                        \n                        \n                        \n                ---\n                Examples:\n                \n                text: "Patient ate breakfast this morning. He seems less anxious."\n                output: {\n                "events": [\n                    {"event_id": "e1",\n                    "event_type": "Eating",\n                    "text_quote":"Patient ate breakfast this morning",\n                    "attributes": {"food": "breakfast", \n                                   "amount": "Unknown",\n                                   "method": "Unknown",\n                                   "negation": "false",\n                                   "time":"morning",\n                                   "caused_by":"Unknown"}\n                    }\n                ],\n                "order":[]\n                }\n                \n                text: "Patient reported severe abdominal pain."\n                output: {\n                "events": [\n                    {"event_id": "e1",\n                    "event_type": "Pain",\n                    "text_quote": "severe abdominal Pain",\n                    "attributes": {"severity": "severe", \n                                   "location": "abdominal",\n                                   "duration": "Unknown",\n                                   "negation": "false",\n                                   "time":"Unknown",\n                                   "caused_by":"Unknown"}\n                    }\n                ],\n                "order":[]\n                }\n                \n                text: "Patient called his son around 3 pm."\n                output: {\n                "events": [\n                    {"event_id": "e1",\n                    "event_type": "Family",\n                    "text_quote": "called his son around 3 pm",\n                    "attributes": {"interaction": "call", \n                                    "relation": "son",\n                                    "negation": "false",\n                                    "time":"3 pm",\n                                    "caused_by":"Unknown"}\n                    }\n                ],\n                "order":[]\n                }\n                \n                text: "Patient had a loose stool overnight."\n                output: {\n                "events": [\n                    {"event_id": "e1",\n                    "event_type": "Excretion",\n                    "text_quote": "loose stool overnight",\n                    "attributes": {"type": "stool", \n                                   "quality": "loose", \n                                   "frequency":"overnight", \n                                   "negation": "false",\n                                   "time":"night",\n                                   "caused_by":"Unknown"}\n                    }\n                ],\n                "order":[]\n                }\n                \n                text: "Patient was able to sleep well last night."\n                output: {\n                "events": [\n                    {"event_id": "e1",\n                    "event_type": "Sleep",\n                    "text_quote": "sleep well last night",\n                    "attributes": {"quality": "well",\n                                    "duration": "Unknown", \n                                    "negation": "false",\n                                    "time":"night",\n                                    "caused_by":"Unknown"}\n                    }\n                ],\n                "order":[]\n                }\n                \n                text: "The patient couldn\'t sleep due to severe pain."\n                output: {\n                "events": [\n                    {"event_id": "e1",\n                    "event_type": "Sleep",\n                    "text_quote": "couldn\'t sleep",\n                    "attributes": {"quality": "poor", \n                                    "duration": "Unknown",\n                                    "negation": "true",\n                                    "time":"Unknown",\n                                    "caused_by":"Pain"}\n                    },\n                    {"event_id": "e2",\n                    "event_type": "Pain",\n                    "text_quote": "severe pain",\n                    "attributes": {"severity": "severe", \n                                    "location": "Unknown", \n                                    "duration": "Unknown", \n                                    "time":"Unknown",\n                                    "caused_by":"Unknown"}\n                    }\n                ],\n                "order":["e1", "after", "e2"]\n                }\n                \n                text: "The patient complained of severe back pain, was given Tylenol, but the pain persisted and he was then prescribed stronger morphine."\n                output: {\n                "events": [\n                    {"event_id": "e1",\n                    "event_type": "Pain",\n                    "text_quote": "complained of severe back pain",\n                    "attributes": {"severity": "severe", \n                                    "location": "back",\n                                    "duration": "Unknown", \n                                    "time":"Unknown",\n                                    "caused_by":"Unknown"}\n                    },\n                    {"event_id": "e2",\n                    "event_type": "Pain",\n                    "text_quote": "pain persisted",\n                    "attributes": {"severity": "severe", \n                                   "location": "back",\n                                   "duration": "persistent", \n                                   "time":"after Tylenol",\n                                   "caused_by":"Unknown"}\n                    }\n                ],\n                "order":[["e1", "before", "e2"]]\n                }\n                \n                        ', 'event_detection_time': 4.333308640983887}</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
           <t>['Pain']</t>
         </is>
       </c>
-      <c r="G3" t="inlineStr">
+      <c r="H3" t="inlineStr">
         <is>
           <t>[{'Pain': {}}]</t>
         </is>
       </c>
-      <c r="H3" t="inlineStr">
+      <c r="I3" t="inlineStr">
         <is>
           <t>['']</t>
         </is>
       </c>
-      <c r="I3" t="inlineStr">
-        <is>
-          <t>{'text': 'ccu nsg progress note 7p-7a/ aortic dissection\n\n\ns- "i have a little pain..not much..."\n\no-\n\n[**name (ni) 231**] patient initially on neo 0.86 mcg to keep maps &gt; 60. heart rate- 70\'s sr, no vea- bp- 86/40-120/58- rt ij inserted on eves- initial filling pressures wnl- high normal- pa- 40/18, pcw-18-22, cvp-16-18.\nco/ci/svr- 3.3/1.79/1624--started 0.375 mcg milrinone after 50mcg bolus. improved co/ci/svr- 5.7/3.1/730 but unable to wean neo much less than 0.7 mcg neo currently. while asleep- bp /pa # dropping , but improving once awake.\n\nresp- 6l np- some apnea, mouth breathing- oxygen saturation- 99-100%- down to 90-92% when mouth breathing/apnea periods occasionally.\nno distress/comfortable- no further diuresis nor ivf bolus for i/o (-)500cc as of 12am.\n\nid- afebrile\n\ngu- poor uo since mid afternoon hypotension and post diuresis.\neve creatinine- 1.7- am levels pending.\nnot much change in uo even after change in co/ci.\n\ngi- npo - taking small sips to wet mouth- took pm dose amiodorone and immediately felt nauseas, vomited- 100cc- felt ok afterwards- same nausea as with previous dose and emesis- but no hemodynamic changes this time- no vagal or hypotension.\nremains on protonix qd.\n\n[**name (ni) 324**] patient sedate, but easily [**name (ni) 8718**] son present all eve while pa line inserted- both aware of plan of care and reason for new invasive line.\npatient sleeping all of shift but for when woken up for questions.\nlast sedation given friday morning with tee/cdv- fent/versed/propofol.\n\na/[**name (ni) **] patient with hypotensive events requiring pressor initiation currently doing well on milrinone drops\nremains with poor uo/need for neo to maintain maps.\n\ncontinue to wean off neo today as tolerated once less sedate and not sleeping.\ncheck with team before attempting 3rd dose of amiodorone as has not tolerated past 2 doses.\nwatch for any further hypotension or tachyarrythnias.\ndiscuss with team ? more fluid today- await am creatine level as well as other lytes.\nserial hct/continue to assess for back pain/ type/location/level of pain. repeat diagnostics- ct/mri as needed if pain worsens or changes in nature.\nkeep patient and son/daughter aware of plan of care.\nnpo.\n\n', 'event': ['Pain'], 'phrase': '', 'raw_output': '{\n  "events": [\n    {\n      "event_type": "Pain",\n      "text_quote": "" \n      },\n      "attributes" \n        ]\n    }', 'attributes': [{'Pain': {}}], 'text_quotes': [''], 'event_name_prompt': 'Given the text: ccu nsg progress note 7p-7a/ aortic dissection\n\n\ns- "i have a little pain..not much..."\n\no-\n\n[**name (ni) 231**] patient initially on neo 0.86 mcg to keep maps &gt; 60. heart rate- 70\'s sr, no vea- bp- 86/40-120/58- rt ij inserted on eves- initial filling pressures wnl- high normal- pa- 40/18, pcw-18-22, cvp-16-18.\nco/ci/svr- 3.3/1.79/1624--started 0.375 mcg milrinone after 50mcg bolus. improved co/ci/svr- 5.7/3.1/730 but unable to wean neo much less than 0.7 mcg neo currently. while asleep- bp /pa # dropping , but improving once awake.\n\nresp- 6l np- some apnea, mouth breathing- oxygen saturation- 99-100%- down to 90-92% when mouth breathing/apnea periods occasionally.\nno distress/comfortable- no further diuresis nor ivf bolus for i/o (-)500cc as of 12am.\n\nid- afebrile\n\ngu- poor uo since mid afternoon hypotension and post diuresis.\neve creatinine- 1.7- am levels pending.\nnot much change in uo even after change in co/ci.\n\ngi- npo - taking small sips to wet mouth- took pm dose amiodorone and immediately felt nauseas, vomited- 100cc- felt ok afterwards- same nausea as with previous dose and emesis- but no hemodynamic changes this time- no vagal or hypotension.\nremains on protonix qd.\n\n[**name (ni) 324**] patient sedate, but easily [**name (ni) 8718**] son present all eve while pa line inserted- both aware of plan of care and reason for new invasive line.\npatient sleeping all of shift but for when woken up for questions.\nlast sedation given friday morning with tee/cdv- fent/versed/propofol.\n\na/[**name (ni) **] patient with hypotensive events requiring pressor initiation currently doing well on milrinone drops\nremains with poor uo/need for neo to maintain maps.\n\ncontinue to wean off neo today as tolerated once less sedate and not sleeping.\ncheck with team before attempting 3rd dose of amiodorone as has not tolerated past 2 doses.\nwatch for any further hypotension or tachyarrythnias.\ndiscuss with team ? more fluid today- await am creatine level as well as other lytes.\nserial hct/continue to assess for back pain/ type/location/level of pain. repeat diagnostics- ct/mri as needed if pain worsens or changes in nature.\nkeep patient and son/daughter aware of plan of care.\nnpo.\n\n, \n                        and the following event types with their definitions: Eating : The patient takes food into their body by mouth.\nExcretion : The patient discharges waste matter from their body.\nFamily : The patient has a visit, call, or communication with a family member.\nPain : The patient reports or shows signs of pain.\nSleep : The patient sleeps or the sleep’s quality or quantity is described.\nUnknown : choose "Unknown" if none of the other event type are applicable. \n                        ---\n                        Your task:\n                        0. Identify ALL events in the text (zero, one, or more).\n1. For each event, assign an event_type from the list above.\n2. If multiple event of same type is mentioned, assign the event_type multiple times\n3. Extract attributes for each event using ONLY the allowed attributes listed below.\n4. Use keyword evidence (Ki) ONLY if it is consistent with the text context.\n5. Output strictly valid JSON following the schema below.\n                        ---\n                        Classification Rules:\n                        - A text may contain multiple events of the same or different types.\n- Create a separate event object for each event mention.\n- If the text is explicitly a NEGATION (e.g., "denies pain"), do not extract that event.\n- If the text describes a FUTURE or HYPOTHETICAL event (e.g., "will eat tomorrow"), ignore it.\n- A valid event should have occurred in the recent past or is occurring during the time of writing of the text.\n- If no events are found or if unsure, return {"events": []}\n                        \n                        ---\n                                    Attributes allowed:\n                                    {\'Eating\': {\'food\': \'&lt;string&gt; # e.g., pancakes, porridge, etc.\', \'amount\': \'&lt;string&gt; # e.g., 1, 2 bowls, etc.\', \'method\': \'&lt;string&gt;  # e.g., oral, tube, etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, after shower, etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}, \'Excretion\': {\'type\': \'&lt;string&gt; # e.g., urine, stool, etc.\', \'frequency\': \'&lt;string&gt; # e.g., 2x, once, etc.\', \'quality\': \'&lt;string&gt; # e.g., loose, hard, etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, after shower, etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}, \'Family\': {\'interaction\': \'&lt;string&gt; # e.g., visit, call, communication, etc.\', \'relation\': \'&lt;string&gt; # e.g., mother, son, etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, after shower, etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}, \'Pain\': {\'severity\': \'&lt;string&gt; # e.g., mild, moderate, severe, numeric scale if present, etc.\', \'location\': \'&lt;string&gt; # e.g., right knee, head, etc.\', \'duration\': \'&lt;string&gt; # e.g., all night, 3 hours, etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, after shower, etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}, \'Sleep\': {\'quality\': \'&lt;string&gt; # e.g., good, poor, restless, etc.\', \'duration\': \'&lt;string&gt; # e.g., 6 hours, phrases like "all night", etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, after shower, etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}}\n                                    If no relevant attribute exists for an event, return an empty object {}.\n                                    \n                        \n                        ---\n                                    Keyword evidence (Ki):\n                                    Additional facts: A keyword matching algorithm without context detected keyword(s) [\'daughter\', \'son\', \'pain\', \'sleeping\', \'asleep\', \'distress\'].\n                                    Use this only as a pointer. If context contradicts, ignore.\n                        ---\n                        Output Schema (strict):\n                        {\n                                    "events": [\n                                        {\n                                        "event_type": "&lt;Pain | Sleep | Excretion | Eating | Family&gt;",\n                                        "text_quote": "&lt;fragement from the text indicating &gt;",\n                "attributes": {\n                    "&lt;attribute_name&gt;": "&lt;attribute_value&gt;"\n                }\n                                        }\n                                    ]\n                                    }\n                        \n                            Rules:\n                                - Ensure the output is valid JSON (parseable).\n                                - "eventS" must always be an array (can be empty).\n                                - Multiple instances of the same event type appear as individual elements in the event array.\n                                - Events appear in the array in the same order in which they appear in the text.\n                                - Do not include extra keys, comments, or text.\n                                - Each object in "events" must contain "event_type", "text_quote", and "attributes".\n                                -If an event attribute type has no value mentioned, return "attributes": {"&lt; attribute name &gt;:Unknown"} for each attribute type defined for the event type \n                        \n                        \n                        \n                        ', 'event_detection_time': 3.0247997129918076}</t>
-        </is>
-      </c>
       <c r="J3" t="inlineStr">
         <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="K3" t="inlineStr">
+        <is>
+          <t>{'text': 'ccu nsg progress note 7p-7a/ aortic dissection\n\n\ns- "i have a little pain..not much..."\n\no-\n\n[**name (ni) 231**] patient initially on neo 0.86 mcg to keep maps &gt; 60. heart rate- 70\'s sr, no vea- bp- 86/40-120/58- rt ij inserted on eves- initial filling pressures wnl- high normal- pa- 40/18, pcw-18-22, cvp-16-18.\nco/ci/svr- 3.3/1.79/1624--started 0.375 mcg milrinone after 50mcg bolus. improved co/ci/svr- 5.7/3.1/730 but unable to wean neo much less than 0.7 mcg neo currently. while asleep- bp /pa # dropping , but improving once awake.\n\nresp- 6l np- some apnea, mouth breathing- oxygen saturation- 99-100%- down to 90-92% when mouth breathing/apnea periods occasionally.\nno distress/comfortable- no further diuresis nor ivf bolus for i/o (-)500cc as of 12am.\n\nid- afebrile\n\ngu- poor uo since mid afternoon hypotension and post diuresis.\neve creatinine- 1.7- am levels pending.\nnot much change in uo even after change in co/ci.\n\ngi- npo - taking small sips to wet mouth- took pm dose amiodorone and immediately felt nauseas, vomited- 100cc- felt ok afterwards- same nausea as with previous dose and emesis- but no hemodynamic changes this time- no vagal or hypotension.\nremains on protonix qd.\n\n[**name (ni) 324**] patient sedate, but easily [**name (ni) 8718**] son present all eve while pa line inserted- both aware of plan of care and reason for new invasive line.\npatient sleeping all of shift but for when woken up for questions.\nlast sedation given friday morning with tee/cdv- fent/versed/propofol.\n\na/[**name (ni) **] patient with hypotensive events requiring pressor initiation currently doing well on milrinone drops\nremains with poor uo/need for neo to maintain maps.\n\ncontinue to wean off neo today as tolerated once less sedate and not sleeping.\ncheck with team before attempting 3rd dose of amiodorone as has not tolerated past 2 doses.\nwatch for any further hypotension or tachyarrythnias.\ndiscuss with team ? more fluid today- await am creatine level as well as other lytes.\nserial hct/continue to assess for back pain/ type/location/level of pain. repeat diagnostics- ct/mri as needed if pain worsens or changes in nature.\nkeep patient and son/daughter aware of plan of care.\nnpo.\n\n', 'event': ['Pain'], 'event_id': ['e1'], 'phrase': '', 'raw_output': '{\n  "events": [\n    {\n      "event_id": "e1",\n      "event_type": "Pain",\n      "text_quote": "" \n      },\n      "attributes" \n        ]\n      }', 'attributes': [{'Pain': {}}], 'orders': [], 'text_quotes': [''], 'event_name_prompt': 'Given the text: ccu nsg progress note 7p-7a/ aortic dissection\n\n\ns- "i have a little pain..not much..."\n\no-\n\n[**name (ni) 231**] patient initially on neo 0.86 mcg to keep maps &gt; 60. heart rate- 70\'s sr, no vea- bp- 86/40-120/58- rt ij inserted on eves- initial filling pressures wnl- high normal- pa- 40/18, pcw-18-22, cvp-16-18.\nco/ci/svr- 3.3/1.79/1624--started 0.375 mcg milrinone after 50mcg bolus. improved co/ci/svr- 5.7/3.1/730 but unable to wean neo much less than 0.7 mcg neo currently. while asleep- bp /pa # dropping , but improving once awake.\n\nresp- 6l np- some apnea, mouth breathing- oxygen saturation- 99-100%- down to 90-92% when mouth breathing/apnea periods occasionally.\nno distress/comfortable- no further diuresis nor ivf bolus for i/o (-)500cc as of 12am.\n\nid- afebrile\n\ngu- poor uo since mid afternoon hypotension and post diuresis.\neve creatinine- 1.7- am levels pending.\nnot much change in uo even after change in co/ci.\n\ngi- npo - taking small sips to wet mouth- took pm dose amiodorone and immediately felt nauseas, vomited- 100cc- felt ok afterwards- same nausea as with previous dose and emesis- but no hemodynamic changes this time- no vagal or hypotension.\nremains on protonix qd.\n\n[**name (ni) 324**] patient sedate, but easily [**name (ni) 8718**] son present all eve while pa line inserted- both aware of plan of care and reason for new invasive line.\npatient sleeping all of shift but for when woken up for questions.\nlast sedation given friday morning with tee/cdv- fent/versed/propofol.\n\na/[**name (ni) **] patient with hypotensive events requiring pressor initiation currently doing well on milrinone drops\nremains with poor uo/need for neo to maintain maps.\n\ncontinue to wean off neo today as tolerated once less sedate and not sleeping.\ncheck with team before attempting 3rd dose of amiodorone as has not tolerated past 2 doses.\nwatch for any further hypotension or tachyarrythnias.\ndiscuss with team ? more fluid today- await am creatine level as well as other lytes.\nserial hct/continue to assess for back pain/ type/location/level of pain. repeat diagnostics- ct/mri as needed if pain worsens or changes in nature.\nkeep patient and son/daughter aware of plan of care.\nnpo.\n\n, \n                        and the following event types with their definitions: Eating : The patient takes food into their body by mouth.\nExcretion : The patient discharges waste matter from their body.\nFamily : The patient has a visit, call, or communication with a family member.\nPain : The patient reports or shows signs of pain.\nSleep : The patient sleeps or the sleep’s quality or quantity is described.\nUnknown : choose "Unknown" if none of the other event type are applicable. \n                        ---\n                        Your task:\n                        0. Identify ALL events in the text (zero, one, or more).\n1. For each event, assign an event_type from the list above.\n2. If multiple event of same type is mentioned, assign the event_type multiple times\n3. Extract attributes for each event using ONLY the allowed attributes listed below.\n4. Use keyword evidence (Ki) ONLY if it is consistent with the text context.\n5. Output strictly valid JSON following the schema below.\n                        ---\n                        Classification Rules:\n                        - A text may contain multiple events of the same or different types.\n- Create a separate event object for each event mention.\n- If the text is explicitly a NEGATION (e.g., "denies pain"), do not extract that event.\n- If the text describes a FUTURE or HYPOTHETICAL event (e.g., "will eat tomorrow"), ignore it.\n- A valid event should have occurred in the recent past or is occurring during the time of writing of the text.\n- If no events are found or if unsure, return {"events": []}\n                        \n                        ---\n                                    Attributes allowed:\n                                    {\'Eating\': {\'food\': \'&lt;string&gt; # e.g., pancakes, porridge, etc.\', \'amount\': \'&lt;string&gt; # e.g., 1, 2 bowls, etc.\', \'method\': \'&lt;string&gt;  # e.g., oral, tube, etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, evening etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}, \'Excretion\': {\'type\': \'&lt;string&gt; # e.g., urine, stool, etc.\', \'frequency\': \'&lt;string&gt; # e.g., 2x, once, etc.\', \'quality\': \'&lt;string&gt; # e.g., loose, hard, etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, evening etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}, \'Family\': {\'interaction\': \'&lt;string&gt; # e.g., visit, call, communication, etc.\', \'relation\': \'&lt;string&gt; # e.g., mother, son, etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, evening etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}, \'Pain\': {\'severity\': \'&lt;string&gt; # e.g., mild, moderate, severe, numeric scale if present, etc.\', \'location\': \'&lt;string&gt; # e.g., right knee, head, etc.\', \'duration\': \'&lt;string&gt; # e.g., all night, 3 hours, etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, evening etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}, \'Sleep\': {\'quality\': \'&lt;string&gt; # e.g., good, poor, restless, etc.\', \'duration\': \'&lt;string&gt; # e.g., 6 hours, phrases like "all night", etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, evening etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}}\n                                    If no relevant attribute exists for an event, return an empty object {}.\n                                    \n                        \n                        ---\n                                    Keyword evidence (Ki):\n                                    Additional facts: A keyword matching algorithm without context detected keyword(s) (\'asleep\', \'daughter\', \'son\', \'pain\', \'distress\', \'sleeping\').\n                                    Use this only as a pointer. If context contradicts, ignore.\n                        ---\n                        Output Schema (strict):\n                        {\n                                    "events": [\n                                        {\n                                        "event_id": "&lt; A unique id eg.: e1 | e2 |...&gt;"\n                                        "event_type": "&lt;Pain | Sleep | Excretion | Eating | Family&gt;",\n                                        "text_quote": "&lt;fragement from the text indicating the event_type&gt;",\n                "attributes": {\n                    "&lt;attribute_name&gt;": "&lt;attribute_value&gt;"\n                }\n                                        }\n                                    ],\n                                    "order": [\n                                        ["e1", "before" | "after" | "simultaneous", "e2" ]\n                                    ]\n                                    }\n                        \n                            Rules:\n                                - Ensure the output is valid JSON (parseable).\n                                - "eventS" must always be an array (can be empty).\n                                - Multiple instances of the same event type appear with different ids.\n                                - Events appear in the array in the same order in which they appear in the text.\n                                - Their partial orders can be expressed using the "order" section.\n                                - Do not include extra keys, comments, or text.\n                                - Each object in "events" must contain "event_type", "text_quote", and "attributes".\n                                - If an event attribute type has no value mentioned, return "attributes": {"&lt; attribute name &gt;:Unknown"} for each attribute type defined for the event type \n                        \n                        \n                        \n                        ', 'event_detection_time': 3.344547467015218}</t>
+        </is>
+      </c>
+      <c r="L3" t="inlineStr">
+        <is>
           <t>['Pain']</t>
         </is>
       </c>
-      <c r="K3" t="inlineStr">
+      <c r="M3" t="inlineStr">
         <is>
           <t>[{'Pain': {}}]</t>
         </is>
       </c>
-      <c r="L3" t="inlineStr">
+      <c r="N3" t="inlineStr">
         <is>
           <t>['']</t>
         </is>
       </c>
-      <c r="M3" t="inlineStr">
-        <is>
-          <t>{'text': 'ccu nsg progress note 7p-7a/ aortic dissection\n\n\ns- "i have a little pain..not much..."\n\no-\n\n[**name (ni) 231**] patient initially on neo 0.86 mcg to keep maps &gt; 60. heart rate- 70\'s sr, no vea- bp- 86/40-120/58- rt ij inserted on eves- initial filling pressures wnl- high normal- pa- 40/18, pcw-18-22, cvp-16-18.\nco/ci/svr- 3.3/1.79/1624--started 0.375 mcg milrinone after 50mcg bolus. improved co/ci/svr- 5.7/3.1/730 but unable to wean neo much less than 0.7 mcg neo currently. while asleep- bp /pa # dropping , but improving once awake.\n\nresp- 6l np- some apnea, mouth breathing- oxygen saturation- 99-100%- down to 90-92% when mouth breathing/apnea periods occasionally.\nno distress/comfortable- no further diuresis nor ivf bolus for i/o (-)500cc as of 12am.\n\nid- afebrile\n\ngu- poor uo since mid afternoon hypotension and post diuresis.\neve creatinine- 1.7- am levels pending.\nnot much change in uo even after change in co/ci.\n\ngi- npo - taking small sips to wet mouth- took pm dose amiodorone and immediately felt nauseas, vomited- 100cc- felt ok afterwards- same nausea as with previous dose and emesis- but no hemodynamic changes this time- no vagal or hypotension.\nremains on protonix qd.\n\n[**name (ni) 324**] patient sedate, but easily [**name (ni) 8718**] son present all eve while pa line inserted- both aware of plan of care and reason for new invasive line.\npatient sleeping all of shift but for when woken up for questions.\nlast sedation given friday morning with tee/cdv- fent/versed/propofol.\n\na/[**name (ni) **] patient with hypotensive events requiring pressor initiation currently doing well on milrinone drops\nremains with poor uo/need for neo to maintain maps.\n\ncontinue to wean off neo today as tolerated once less sedate and not sleeping.\ncheck with team before attempting 3rd dose of amiodorone as has not tolerated past 2 doses.\nwatch for any further hypotension or tachyarrythnias.\ndiscuss with team ? more fluid today- await am creatine level as well as other lytes.\nserial hct/continue to assess for back pain/ type/location/level of pain. repeat diagnostics- ct/mri as needed if pain worsens or changes in nature.\nkeep patient and son/daughter aware of plan of care.\nnpo.\n\n', 'event': ['Pain', 'Sleep', 'Family', 'Excretion', 'Eating', 'Excretion'], 'phrase': '', 'raw_output': '{\n  "events": [\n    {\n      "event_type": "Pain",\n      "text_quote": "i have a little pain..not much...",\n      "attributes": {\n        "severity": "little",\n        "location": "Unknown",\n        "duration": "Unknown",\n        "time": "Unknown",\n        "caused_by": "Unknown"\n      }\n    },\n    {\n      "event_type": "Sleep",\n      "text_quote": "patient sleeping all of shift but for when woken up for questions.",\n      "attributes": {\n        "quality": "Unknown",\n        "duration": "all of shift",\n        "time": "Unknown",\n        "caused_by": "Unknown"\n      }\n    },\n    {\n      "event_type": "Family",\n      "text_quote": "son present all eve while pa line inserted- both aware of plan of care and reason for new invasive line.",\n      "attributes": {\n        "interaction": "visit",\n        "relation": "son",\n        "time": "evening",\n        "caused_by": "Unknown"\n      }\n    },\n    {\n      "event_type": "Excretion",\n      "text_quote": "poor uo since mid afternoon hypotension and post diuresis.",\n      "attributes": {\n        "type": "urine",\n        "frequency": "poor",\n        "quality": "Unknown",\n        "time": "afternoon",\n        "caused_by": "hypotension and post diuresis"\n      }\n    },\n    {\n      "event_type": "Eating",\n      "text_quote": "taking small sips to wet mouth- took pm dose amiodorone and immediately felt nauseas, vomited- 100cc- felt ok afterwards",\n      "attributes": {\n        "food": "small sips",\n        "amount": "Unknown",\n        "method": "oral",\n        "time": "afternoon",\n        "caused_by": "amiodorone"\n      }\n    },\n    {\n      "event_type": "Excretion",\n      "text_quote": "vomited- 100cc",\n      "attributes": {\n        "type": "vomit",\n        "frequency": "once",\n        "quality": "Unknown",\n        "time": "afternoon",\n        "caused_by": "amiodorone"\n      }\n    }\n  ]\n}', 'attributes': [{'Pain': {'severity': 'little', 'location': 'Unknown', 'duration': 'Unknown', 'time': 'Unknown', 'caused_by': 'Unknown'}}, {'Sleep': {'quality': 'Unknown', 'duration': 'all of shift', 'time': 'Unknown', 'caused_by': 'Unknown'}}, {'Family': {'interaction': 'visit', 'relation': 'son', 'time': 'evening', 'caused_by': 'Unknown'}}, {'Excretion': {'type': 'urine', 'frequency': 'poor', 'quality': 'Unknown', 'time': 'afternoon', 'caused_by': 'hypotension and post diuresis'}}, {'Eating': {'food': 'small sips', 'amount': 'Unknown', 'method': 'oral', 'time': 'afternoon', 'caused_by': 'amiodorone'}}, {'Excretion': {'type': 'vomit', 'frequency': 'once', 'quality': 'Unknown', 'time': 'afternoon', 'caused_by': 'amiodorone'}}], 'text_quotes': ['i have a little pain..not much...', 'patient sleeping all of shift but for when woken up for questions.', 'son present all eve while pa line inserted- both aware of plan of care and reason for new invasive line.', 'poor uo since mid afternoon hypotension and post diuresis.', 'taking small sips to wet mouth- took pm dose amiodorone and immediately felt nauseas, vomited- 100cc- felt ok afterwards', 'vomited- 100cc'], 'event_name_prompt': 'Given the text: ccu nsg progress note 7p-7a/ aortic dissection\n\n\ns- "i have a little pain..not much..."\n\no-\n\n[**name (ni) 231**] patient initially on neo 0.86 mcg to keep maps &gt; 60. heart rate- 70\'s sr, no vea- bp- 86/40-120/58- rt ij inserted on eves- initial filling pressures wnl- high normal- pa- 40/18, pcw-18-22, cvp-16-18.\nco/ci/svr- 3.3/1.79/1624--started 0.375 mcg milrinone after 50mcg bolus. improved co/ci/svr- 5.7/3.1/730 but unable to wean neo much less than 0.7 mcg neo currently. while asleep- bp /pa # dropping , but improving once awake.\n\nresp- 6l np- some apnea, mouth breathing- oxygen saturation- 99-100%- down to 90-92% when mouth breathing/apnea periods occasionally.\nno distress/comfortable- no further diuresis nor ivf bolus for i/o (-)500cc as of 12am.\n\nid- afebrile\n\ngu- poor uo since mid afternoon hypotension and post diuresis.\neve creatinine- 1.7- am levels pending.\nnot much change in uo even after change in co/ci.\n\ngi- npo - taking small sips to wet mouth- took pm dose amiodorone and immediately felt nauseas, vomited- 100cc- felt ok afterwards- same nausea as with previous dose and emesis- but no hemodynamic changes this time- no vagal or hypotension.\nremains on protonix qd.\n\n[**name (ni) 324**] patient sedate, but easily [**name (ni) 8718**] son present all eve while pa line inserted- both aware of plan of care and reason for new invasive line.\npatient sleeping all of shift but for when woken up for questions.\nlast sedation given friday morning with tee/cdv- fent/versed/propofol.\n\na/[**name (ni) **] patient with hypotensive events requiring pressor initiation currently doing well on milrinone drops\nremains with poor uo/need for neo to maintain maps.\n\ncontinue to wean off neo today as tolerated once less sedate and not sleeping.\ncheck with team before attempting 3rd dose of amiodorone as has not tolerated past 2 doses.\nwatch for any further hypotension or tachyarrythnias.\ndiscuss with team ? more fluid today- await am creatine level as well as other lytes.\nserial hct/continue to assess for back pain/ type/location/level of pain. repeat diagnostics- ct/mri as needed if pain worsens or changes in nature.\nkeep patient and son/daughter aware of plan of care.\nnpo.\n\n, \n                        and the following event types with their definitions: Eating : The patient takes food into their body by mouth.\nExcretion : The patient discharges waste matter from their body.\nFamily : The patient has a visit, call, or communication with a family member.\nPain : The patient reports or shows signs of pain.\nSleep : The patient sleeps or the sleep’s quality or quantity is described.\nUnknown : choose "Unknown" if none of the other event type are applicable. \n                        ---\n                        Your task:\n                        0. Identify ALL events in the text (zero, one, or more).\n1. For each event, assign an event_type from the list above.\n2. If multiple event of same type is mentioned, assign the event_type multiple times\n3. Extract attributes for each event using ONLY the allowed attributes listed below.\n4. Output strictly valid JSON following the schema below.\n                        ---\n                        Classification Rules:\n                        - A text may contain multiple events of the same or different types.\n- Create a separate event object for each event mention.\n- If the text is explicitly a NEGATION (e.g., "denies pain"), do not extract that event.\n- If the text describes a FUTURE or HYPOTHETICAL event (e.g., "will eat tomorrow"), ignore it.\n- A valid event should have occurred in the recent past or is occurring during the time of writing of the text.\n- If no events are found or if unsure, return {"events": []}\n                        \n                        ---\n                                    Attributes allowed:\n                                    {\'Eating\': {\'food\': \'&lt;string&gt; # e.g., pancakes, porridge, etc.\', \'amount\': \'&lt;string&gt; # e.g., 1, 2 bowls, etc.\', \'method\': \'&lt;string&gt;  # e.g., oral, tube, etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, after shower, etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}, \'Excretion\': {\'type\': \'&lt;string&gt; # e.g., urine, stool, etc.\', \'frequency\': \'&lt;string&gt; # e.g., 2x, once, etc.\', \'quality\': \'&lt;string&gt; # e.g., loose, hard, etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, after shower, etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}, \'Family\': {\'interaction\': \'&lt;string&gt; # e.g., visit, call, communication, etc.\', \'relation\': \'&lt;string&gt; # e.g., mother, son, etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, after shower, etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}, \'Pain\': {\'severity\': \'&lt;string&gt; # e.g., mild, moderate, severe, numeric scale if present, etc.\', \'location\': \'&lt;string&gt; # e.g., right knee, head, etc.\', \'duration\': \'&lt;string&gt; # e.g., all night, 3 hours, etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, after shower, etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}, \'Sleep\': {\'quality\': \'&lt;string&gt; # e.g., good, poor, restless, etc.\', \'duration\': \'&lt;string&gt; # e.g., 6 hours, phrases like "all night", etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, after shower, etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}}\n                                    If no relevant attribute exists for an event, return an empty object {}.\n                                    \n                        \n                        \n                        ---\n                        Output Schema (strict):\n                        {\n                                    "events": [\n                                        {\n                                        "event_type": "&lt;Pain | Sleep | Excretion | Eating | Family&gt;",\n                                        "text_quote": "&lt;fragement from the text indicating &gt;",\n                "attributes": {\n                    "&lt;attribute_name&gt;": "&lt;attribute_value&gt;"\n                }\n                                        }\n                                    ]\n                                    }\n                        \n                            Rules:\n                                - Ensure the output is valid JSON (parseable).\n                                - "eventS" must always be an array (can be empty).\n                                - Multiple instances of the same event type appear as individual elements in the event array.\n                                - Events appear in the array in the same order in which they appear in the text.\n                                - Do not include extra keys, comments, or text.\n                                - Each object in "events" must contain "event_type", "text_quote", and "attributes".\n                                -If an event attribute type has no value mentioned, return "attributes": {"&lt; attribute name &gt;:Unknown"} for each attribute type defined for the event type \n                        \n                        \n                        \n                ---\n                Examples:\n                \n                text: "Patient ate breakfast this morning. He seems less anxious."\n                output: {\n                "events": [\n                    {\n                    "event_type": "Eating",\n                    "text_quote":"Patient ate breakfast this morning",\n                    "attributes": {"food": "breakfast", \n                                   "amount": "Unknown",\n                                   "method": "Unknown",\n                                   "time":"morning",\n                                   "caused_by":"Unknown"}\n                    }\n                ]\n                }\n                \n                text: "Patient reported severe abdominal pain."\n                output: {\n                "events": [\n                    {\n                    "event_type": "Pain",\n                    "text_quote": "severe abdominal Pain",\n                    "attributes": {"severity": "severe", \n                                   "location": "abdominal",\n                                   "duration": "Unknown",\n                                   "time":"Unknown",\n                                   "caused_by":"Unknown"}\n                    }\n                ]\n                }\n                \n                text: "Patient called his son around 3 pm."\n                output: {\n                "events": [\n                    {\n                    "event_type": "Family",\n                    "text_quote": "called his son around 3 pm",\n                    "attributes": {"interaction": "call", \n                                    "relation": "son",\n                                    "time":"3 pm",\n                                    "caused_by":"Unknown"}\n                    }\n                ]\n                }\n                \n                text: "Patient had a loose stool overnight."\n                output: {\n                "events": [\n                    {\n                    "event_type": "Excretion",\n                    "text_quote": "loose stool overnight",\n                    "attributes": {"type": "stool", \n                                   "quality": "loose", \n                                   "frequency":"overnight", \n                                   "time":"night",\n                                   "caused_by":"Unknown"}\n                    }\n                ]\n                }\n                \n                text: "Patient was able to sleep well last night."\n                output: {\n                "events": [\n                    {\n                    "event_type": "Sleep",\n                    "text_quote": "sleep well last night",\n                    "attributes": {"quality": "well",\n                                    "duration": "Unknown", \n                                    "time":"night",\n                                    "caused_by":"Unknown"}\n                    }\n                ]\n                }\n                \n                text: "The patient couldn\'t sleep due to severe pain."\n                output: {\n                "events": [\n                    {\n                    "event_type": "Sleep",\n                    "text_quote": "couldn\'t sleep",\n                    "attributes": {"quality": "poor", \n                                    "duration": "Unknown",\n                                   "time":"Unknown",\n                                   "caused_by":"Pain"}\n                    },\n                    {\n                    "event_type": "Pain",\n                    "text_quote": "severe pain",\n                    "attributes": {"severity": "severe", \n                                    "location": "Unknown", \n                                    "duration": "Unknown", \n                                   "time":"before Sleep",\n                                   "caused_by":"Unknown"}\n                    }\n                ]\n                }\n                \n                text: "The patient complained of severe back pain, was given Tylenol, but the pain persisted and he was then prescribed stronger morphine."\n                output: {\n                "events": [\n                    {\n                    "event_type": "Pain",\n                    "text_quote": "complained of severe back pain",\n                    "attributes": {"severity": "severe", \n                                    "location": "back",\n                                    "duration": "Unknown", \n                                    "time":"Unknown",\n                                    "caused_by":"Unknown"}\n                    },\n                    {\n                    "event_type": "Pain",\n                    "text_quote": "pain persisted",\n                    "attributes": {"severity": "severe", \n                                   "location": "back",\n                                   "duration": "persistent", \n                                   "time":"after Tylenol",\n                                   "caused_by":"Unknown"}\n                    }\n                ]\n                }\n                \n                        ', 'event_detection_time': 17.334568329999456}</t>
-        </is>
-      </c>
-      <c r="N3" t="inlineStr">
-        <is>
-          <t>['Pain', 'Sleep', 'Family', 'Excretion', 'Eating', 'Excretion']</t>
-        </is>
-      </c>
       <c r="O3" t="inlineStr">
         <is>
-          <t>[{'Pain': {'severity': 'little', 'location': 'Unknown', 'duration': 'Unknown', 'time': 'Unknown', 'caused_by': 'Unknown'}}, {'Sleep': {'quality': 'Unknown', 'duration': 'all of shift', 'time': 'Unknown', 'caused_by': 'Unknown'}}, {'Family': {'interaction': 'visit', 'relation': 'son', 'time': 'evening', 'caused_by': 'Unknown'}}, {'Excretion': {'type': 'urine', 'frequency': 'poor', 'quality': 'Unknown', 'time': 'afternoon', 'caused_by': 'hypotension and post diuresis'}}, {'Eating': {'food': 'small sips', 'amount': 'Unknown', 'method': 'oral', 'time': 'afternoon', 'caused_by': 'amiodorone'}}, {'Excretion': {'type': 'vomit', 'frequency': 'once', 'quality': 'Unknown', 'time': 'afternoon', 'caused_by': 'amiodorone'}}]</t>
-        </is>
-      </c>
-      <c r="P3" t="inlineStr">
-        <is>
-          <t>['i have a little pain..not much...', 'patient sleeping all of shift but for when woken up for questions.', 'son present all eve while pa line inserted- both aware of plan of care and reason for new invasive line.', 'poor uo since mid afternoon hypotension and post diuresis.', 'taking small sips to wet mouth- took pm dose amiodorone and immediately felt nauseas, vomited- 100cc- felt ok afterwards', 'vomited- 100cc']</t>
-        </is>
-      </c>
-      <c r="Q3" t="inlineStr"/>
-      <c r="R3" t="inlineStr">
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="P3" t="n">
+        <v>2.335000317543745e-06</v>
+      </c>
+      <c r="Q3" t="inlineStr">
         <is>
           <t>Sleep</t>
         </is>
       </c>
-      <c r="S3" t="b">
-        <v>0</v>
+      <c r="R3" t="b">
+        <v>0</v>
+      </c>
+      <c r="S3" t="n">
+        <v>1</v>
       </c>
       <c r="T3" t="n">
         <v>1</v>
       </c>
-      <c r="U3" t="n">
-        <v>1</v>
-      </c>
-      <c r="V3" t="inlineStr">
+      <c r="U3" t="inlineStr">
         <is>
           <t>('asleep', 'daughter', 'son', 'pain', 'distress', 'sleeping')</t>
         </is>
       </c>
+      <c r="V3" t="n">
+        <v>4.333308640983887</v>
+      </c>
       <c r="W3" t="n">
-        <v>3.828834353989805</v>
+        <v>3.344547467015218</v>
       </c>
       <c r="X3" t="n">
-        <v>3.024799712991808</v>
+        <v>1</v>
       </c>
       <c r="Y3" t="n">
-        <v>17.33456832999946</v>
+        <v>0</v>
       </c>
       <c r="Z3" t="n">
-        <v>1</v>
-      </c>
-      <c r="AA3" t="n">
-        <v>0</v>
-      </c>
-      <c r="AB3" t="n">
-        <v>0</v>
-      </c>
-      <c r="AC3" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="n">
-        <v>1310480</v>
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>1310480</t>
+        </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>['Pain', 'Sleep', 'Unknown']</t>
+          <t>('Pain', 'Sleep', 'Unknown')</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>['sleeping', 'pain']</t>
+          <t>('pain', 'sleeping')</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
@@ -891,120 +862,111 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>{'text': 'patient denies pain,nausea.sleeping all day but easily aroused ,alert and oreinted.\n\nsr no ect. .neo dc ci 2.99/svr 858.now weaning milrinone.pad 13 to 19.pa sat 73 .cvp 10 to 20 .map 75 to 87.good distal pulses,bp equal both arms .\n\n6l np 7.38/32/87/20/96\n\ntaking cl liquids ,abd soft, no stool\n\nhuo 15 to 20 ,lytes sent\n\nseen by sx ,[**month (only) 108**] need mra\n\nrecheck hemodynamics and wean milrinone as tol\nfollow hcts\n', 'event': ['Sleep', 'Eating', 'Excretion'], 'phrase': '', 'raw_output': '{\n  "events": [\n    {\n      "event_type": "Sleep",\n      "text_quote": "sleeping all day but easily aroused",\n      "attributes": {\n        "quality": "poor",\n        "duration": "all day",\n        "time": "day",\n        "caused_by": "Unknown"\n      }\n    },\n    {\n      "event_type": "Eating",\n      "text_quote": "taking cl liquids",\n      "attributes": {\n        "food": "cl liquids",\n        "amount": "Unknown",\n        "method": "oral",\n        "time": "Unknown",\n        "caused_by": "Unknown"\n      }\n    },\n    {\n      "event_type": "Excretion",\n      "text_quote": "no stool",\n      "attributes": {\n        "type": "stool",\n        "frequency": "none",\n        "quality": "Unknown",\n        "time": "Unknown",\n        "caused_by": "Unknown"\n      }\n    }\n  ]\n}', 'attributes': [{'Sleep': {'quality': 'poor', 'duration': 'all day', 'time': 'day', 'caused_by': 'Unknown'}}, {'Eating': {'food': 'cl liquids', 'amount': 'Unknown', 'method': 'oral', 'time': 'Unknown', 'caused_by': 'Unknown'}}, {'Excretion': {'type': 'stool', 'frequency': 'none', 'quality': 'Unknown', 'time': 'Unknown', 'caused_by': 'Unknown'}}], 'text_quotes': ['sleeping all day but easily aroused', 'taking cl liquids', 'no stool'], 'event_name_prompt': 'Given the text: patient denies pain,nausea.sleeping all day but easily aroused ,alert and oreinted.\n\nsr no ect. .neo dc ci 2.99/svr 858.now weaning milrinone.pad 13 to 19.pa sat 73 .cvp 10 to 20 .map 75 to 87.good distal pulses,bp equal both arms .\n\n6l np 7.38/32/87/20/96\n\ntaking cl liquids ,abd soft, no stool\n\nhuo 15 to 20 ,lytes sent\n\nseen by sx ,[**month (only) 108**] need mra\n\nrecheck hemodynamics and wean milrinone as tol\nfollow hcts\n, \n                        and the following event types with their definitions: Eating : The patient takes food into their body by mouth.\nExcretion : The patient discharges waste matter from their body.\nFamily : The patient has a visit, call, or communication with a family member.\nPain : The patient reports or shows signs of pain.\nSleep : The patient sleeps or the sleep’s quality or quantity is described.\nUnknown : choose "Unknown" if none of the other event type are applicable. \n                        ---\n                        Your task:\n                        0. Identify ALL events in the text (zero, one, or more).\n1. For each event, assign an event_type from the list above.\n2. If multiple event of same type is mentioned, assign the event_type multiple times\n3. Extract attributes for each event using ONLY the allowed attributes listed below.\n4. Use keyword evidence (Ki) ONLY if it is consistent with the text context.\n5. Output strictly valid JSON following the schema below.\n                        ---\n                        Classification Rules:\n                        - A text may contain multiple events of the same or different types.\n- Create a separate event object for each event mention.\n- If the text is explicitly a NEGATION (e.g., "denies pain"), do not extract that event.\n- If the text describes a FUTURE or HYPOTHETICAL event (e.g., "will eat tomorrow"), ignore it.\n- A valid event should have occurred in the recent past or is occurring during the time of writing of the text.\n- If no events are found or if unsure, return {"events": []}\n                        \n                        ---\n                                    Attributes allowed:\n                                    {\'Eating\': {\'food\': \'&lt;string&gt; # e.g., pancakes, porridge, etc.\', \'amount\': \'&lt;string&gt; # e.g., 1, 2 bowls, etc.\', \'method\': \'&lt;string&gt;  # e.g., oral, tube, etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, after shower, etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}, \'Excretion\': {\'type\': \'&lt;string&gt; # e.g., urine, stool, etc.\', \'frequency\': \'&lt;string&gt; # e.g., 2x, once, etc.\', \'quality\': \'&lt;string&gt; # e.g., loose, hard, etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, after shower, etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}, \'Family\': {\'interaction\': \'&lt;string&gt; # e.g., visit, call, communication, etc.\', \'relation\': \'&lt;string&gt; # e.g., mother, son, etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, after shower, etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}, \'Pain\': {\'severity\': \'&lt;string&gt; # e.g., mild, moderate, severe, numeric scale if present, etc.\', \'location\': \'&lt;string&gt; # e.g., right knee, head, etc.\', \'duration\': \'&lt;string&gt; # e.g., all night, 3 hours, etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, after shower, etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}, \'Sleep\': {\'quality\': \'&lt;string&gt; # e.g., good, poor, restless, etc.\', \'duration\': \'&lt;string&gt; # e.g., 6 hours, phrases like "all night", etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, after shower, etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}}\n                                    If no relevant attribute exists for an event, return an empty object {}.\n                                    \n                        \n                        ---\n                                    Keyword evidence (Ki):\n                                    Additional facts: A keyword matching algorithm without context detected keyword(s) [\'sleeping\', \'pain\'].\n                                    Use this only as a pointer. If context contradicts, ignore.\n                        ---\n                        Output Schema (strict):\n                        {\n                                    "events": [\n                                        {\n                                        "event_type": "&lt;Pain | Sleep | Excretion | Eating | Family&gt;",\n                                        "text_quote": "&lt;fragement from the text indicating &gt;",\n                "attributes": {\n                    "&lt;attribute_name&gt;": "&lt;attribute_value&gt;"\n                }\n                                        }\n                                    ]\n                                    }\n                        \n                            Rules:\n                                - Ensure the output is valid JSON (parseable).\n                                - "eventS" must always be an array (can be empty).\n                                - Multiple instances of the same event type appear as individual elements in the event array.\n                                - Events appear in the array in the same order in which they appear in the text.\n                                - Do not include extra keys, comments, or text.\n                                - Each object in "events" must contain "event_type", "text_quote", and "attributes".\n                                -If an event attribute type has no value mentioned, return "attributes": {"&lt; attribute name &gt;:Unknown"} for each attribute type defined for the event type \n                        \n                        \n                        \n                ---\n                Examples:\n                \n                text: "Patient ate breakfast this morning. He seems less anxious."\n                output: {\n                "events": [\n                    {\n                    "event_type": "Eating",\n                    "text_quote":"Patient ate breakfast this morning",\n                    "attributes": {"food": "breakfast", \n                                   "amount": "Unknown",\n                                   "method": "Unknown",\n                                   "time":"morning",\n                                   "caused_by":"Unknown"}\n                    }\n                ]\n                }\n                \n                text: "Patient reported severe abdominal pain."\n                output: {\n                "events": [\n                    {\n                    "event_type": "Pain",\n                    "text_quote": "severe abdominal Pain",\n                    "attributes": {"severity": "severe", \n                                   "location": "abdominal",\n                                   "duration": "Unknown",\n                                   "time":"Unknown",\n                                   "caused_by":"Unknown"}\n                    }\n                ]\n                }\n                \n                text: "Patient called his son around 3 pm."\n                output: {\n                "events": [\n                    {\n                    "event_type": "Family",\n                    "text_quote": "called his son around 3 pm",\n                    "attributes": {"interaction": "call", \n                                    "relation": "son",\n                                    "time":"3 pm",\n                                    "caused_by":"Unknown"}\n                    }\n                ]\n                }\n                \n                text: "Patient had a loose stool overnight."\n                output: {\n                "events": [\n                    {\n                    "event_type": "Excretion",\n                    "text_quote": "loose stool overnight",\n                    "attributes": {"type": "stool", \n                                   "quality": "loose", \n                                   "frequency":"overnight", \n                                   "time":"night",\n                                   "caused_by":"Unknown"}\n                    }\n                ]\n                }\n                \n                text: "Patient was able to sleep well last night."\n                output: {\n                "events": [\n                    {\n                    "event_type": "Sleep",\n                    "text_quote": "sleep well last night",\n                    "attributes": {"quality": "well",\n                                    "duration": "Unknown", \n                                    "time":"night",\n                                    "caused_by":"Unknown"}\n                    }\n                ]\n                }\n                \n                text: "The patient couldn\'t sleep due to severe pain."\n                output: {\n                "events": [\n                    {\n                    "event_type": "Sleep",\n                    "text_quote": "couldn\'t sleep",\n                    "attributes": {"quality": "poor", \n                                    "duration": "Unknown",\n                                   "time":"Unknown",\n                                   "caused_by":"Pain"}\n                    },\n                    {\n                    "event_type": "Pain",\n                    "text_quote": "severe pain",\n                    "attributes": {"severity": "severe", \n                                    "location": "Unknown", \n                                    "duration": "Unknown", \n                                   "time":"before Sleep",\n                                   "caused_by":"Unknown"}\n                    }\n                ]\n                }\n                \n                text: "The patient complained of severe back pain, was given Tylenol, but the pain persisted and he was then prescribed stronger morphine."\n                output: {\n                "events": [\n                    {\n                    "event_type": "Pain",\n                    "text_quote": "complained of severe back pain",\n                    "attributes": {"severity": "severe", \n                                    "location": "back",\n                                    "duration": "Unknown", \n                                    "time":"Unknown",\n                                    "caused_by":"Unknown"}\n                    },\n                    {\n                    "event_type": "Pain",\n                    "text_quote": "pain persisted",\n                    "attributes": {"severity": "severe", \n                                   "location": "back",\n                                   "duration": "persistent", \n                                   "time":"after Tylenol",\n                                   "caused_by":"Unknown"}\n                    }\n                ]\n                }\n                \n                        ', 'event_detection_time': 8.34106302598957}</t>
+          <t>['pain', 'sleeping']</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>['Sleep', 'Eating', 'Excretion']</t>
+          <t>{'text': 'patient denies pain,nausea.sleeping all day but easily aroused ,alert and oreinted.\n\nsr no ect. .neo dc ci 2.99/svr 858.now weaning milrinone.pad 13 to 19.pa sat 73 .cvp 10 to 20 .map 75 to 87.good distal pulses,bp equal both arms .\n\n6l np 7.38/32/87/20/96\n\ntaking cl liquids ,abd soft, no stool\n\nhuo 15 to 20 ,lytes sent\n\nseen by sx ,[**month (only) 108**] need mra\n\nrecheck hemodynamics and wean milrinone as tol\nfollow hcts\n', 'event': ['Sleep', 'Eating', 'Excretion', 'Pain'], 'event_id': ['e1', 'e2', 'e3', 'e4'], 'phrase': '', 'raw_output': '{\n  "events": [\n    {\n      "event_id": "e1",\n      "event_type": "Sleep",\n      "text_quote": "sleeping all day but easily aroused",\n      "attributes": {\n        "quality": "Unknown",\n        "duration": "all day",\n        "negation": "false",\n        "time": "day",\n        "caused_by": "Unknown"\n      }\n    },\n    {\n      "event_id": "e2",\n      "event_type": "Eating",\n      "text_quote": "taking cl liquids",\n      "attributes": {\n        "food": "cl liquids",\n        "amount": "Unknown",\n        "method": "oral",\n        "negation": "false",\n        "time": "Unknown",\n        "caused_by": "Unknown"\n      }\n    },\n    {\n      "event_id": "e3",\n      "event_type": "Excretion",\n      "text_quote": "no stool",\n      "attributes": {\n        "type": "stool",\n        "frequency": "none",\n        "quality": "Unknown",\n        "negation": "true",\n        "time": "Unknown",\n        "caused_by": "Unknown"\n      }\n    },\n    {\n      "event_id": "e4",\n      "event_type": "Pain",\n      "text_quote": "patient denies pain",\n      "attributes": {\n        "severity": "Unknown",\n        "location": "Unknown",\n        "duration": "Unknown",\n        "negation": "true",\n        "time": "Unknown",\n        "caused_by": "Unknown"\n      }\n    }\n  ],\n  "order": []\n}', 'attributes': [{'Sleep': {'quality': 'Unknown', 'duration': 'all day', 'negation': 'false', 'time': 'day', 'caused_by': 'Unknown'}}, {'Eating': {'food': 'cl liquids', 'amount': 'Unknown', 'method': 'oral', 'negation': 'false', 'time': 'Unknown', 'caused_by': 'Unknown'}}, {'Excretion': {'type': 'stool', 'frequency': 'none', 'quality': 'Unknown', 'negation': 'true', 'time': 'Unknown', 'caused_by': 'Unknown'}}, {'Pain': {'severity': 'Unknown', 'location': 'Unknown', 'duration': 'Unknown', 'negation': 'true', 'time': 'Unknown', 'caused_by': 'Unknown'}}], 'orders': [[]], 'text_quotes': ['sleeping all day but easily aroused', 'taking cl liquids', 'no stool', 'patient denies pain'], 'event_name_prompt': 'Given the text: patient denies pain,nausea.sleeping all day but easily aroused ,alert and oreinted.\n\nsr no ect. .neo dc ci 2.99/svr 858.now weaning milrinone.pad 13 to 19.pa sat 73 .cvp 10 to 20 .map 75 to 87.good distal pulses,bp equal both arms .\n\n6l np 7.38/32/87/20/96\n\ntaking cl liquids ,abd soft, no stool\n\nhuo 15 to 20 ,lytes sent\n\nseen by sx ,[**month (only) 108**] need mra\n\nrecheck hemodynamics and wean milrinone as tol\nfollow hcts\n, \n                        and the following event types with their definitions: Eating : The patient takes food into their body by mouth.\nExcretion : The patient discharges waste matter from their body.\nFamily : The patient has a visit, call, or communication with a family member.\nPain : The patient reports or shows signs of pain.\nSleep : The patient sleeps or the sleep’s quality or quantity is described.\nUnknown : choose "Unknown" if none of the other event type are applicable. \n                        ---\n                        Your task:\n                        0. Identify ALL events in the text (zero, one, or more).\n1. For each event, assign an event_type from the list above.\n2. If multiple event of same type is mentioned, assign the event_type multiple times\n3. Extract attributes for each event using ONLY the allowed attributes listed below.\n4. Use keyword evidence (Ki) ONLY if it is consistent with the text context.\n5. Output strictly valid JSON following the schema below.\n                        ---\n                        Classification Rules:\n                        - A text may contain multiple events of the same or different types.\n- Create a separate event object for each event mention.\n- If the text is explicitly a NEGATION (e.g., "denies pain"), do not extract that event.\n- If the text describes a FUTURE or HYPOTHETICAL event (e.g., "will eat tomorrow"), ignore it.\n- A valid event should have occurred in the recent past or is occurring during the time of writing of the text.\n- If no events are found or if unsure, return {"events": []}\n                        \n                        ---\n                                    Attributes allowed:\n                                    {\'Eating\': {\'food\': \'&lt;string&gt; # e.g., pancakes, porridge, etc.\', \'amount\': \'&lt;string&gt; # e.g., 1, 2 bowls, etc.\', \'method\': \'&lt;string&gt;  # e.g., oral, tube, etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, evening etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}, \'Excretion\': {\'type\': \'&lt;string&gt; # e.g., urine, stool, etc.\', \'frequency\': \'&lt;string&gt; # e.g., 2x, once, etc.\', \'quality\': \'&lt;string&gt; # e.g., loose, hard, etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, evening etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}, \'Family\': {\'interaction\': \'&lt;string&gt; # e.g., visit, call, communication, etc.\', \'relation\': \'&lt;string&gt; # e.g., mother, son, etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, evening etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}, \'Pain\': {\'severity\': \'&lt;string&gt; # e.g., mild, moderate, severe, numeric scale if present, etc.\', \'location\': \'&lt;string&gt; # e.g., right knee, head, etc.\', \'duration\': \'&lt;string&gt; # e.g., all night, 3 hours, etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, evening etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}, \'Sleep\': {\'quality\': \'&lt;string&gt; # e.g., good, poor, restless, etc.\', \'duration\': \'&lt;string&gt; # e.g., 6 hours, phrases like "all night", etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, evening etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}}\n                                    If no relevant attribute exists for an event, return an empty object {}.\n                                    \n                        \n                        ---\n                                    Keyword evidence (Ki):\n                                    Additional facts: A keyword matching algorithm without context detected keyword(s) (\'pain\', \'sleeping\').\n                                    Use this only as a pointer. If context contradicts, ignore.\n                        ---\n                        Output Schema (strict):\n                        {\n                                    "events": [\n                                        {\n                                        "event_id": "&lt; A unique id eg.: e1 | e2 |...&gt;"\n                                        "event_type": "&lt;Pain | Sleep | Excretion | Eating | Family&gt;",\n                                        "text_quote": "&lt;fragement from the text indicating the event_type&gt;",\n                "attributes": {\n                    "&lt;attribute_name&gt;": "&lt;attribute_value&gt;"\n                }\n                                        }\n                                    ],\n                                    "order": [\n                                        ["e1", "before" | "after" | "simultaneous", "e2" ]\n                                    ]\n                                    }\n                        \n                            Rules:\n                                - Ensure the output is valid JSON (parseable).\n                                - "eventS" must always be an array (can be empty).\n                                - Multiple instances of the same event type appear with different ids.\n                                - Events appear in the array in the same order in which they appear in the text.\n                                - Their partial orders can be expressed using the "order" section.\n                                - Do not include extra keys, comments, or text.\n                                - Each object in "events" must contain "event_type", "text_quote", and "attributes".\n                                - If an event attribute type has no value mentioned, return "attributes": {"&lt; attribute name &gt;:Unknown"} for each attribute type defined for the event type \n                        \n                        \n                        \n                ---\n                Examples:\n                \n                text: "Patient ate breakfast this morning. He seems less anxious."\n                output: {\n                "events": [\n                    {"event_id": "e1",\n                    "event_type": "Eating",\n                    "text_quote":"Patient ate breakfast this morning",\n                    "attributes": {"food": "breakfast", \n                                   "amount": "Unknown",\n                                   "method": "Unknown",\n                                   "negation": "false",\n                                   "time":"morning",\n                                   "caused_by":"Unknown"}\n                    }\n                ],\n                "order":[]\n                }\n                \n                text: "Patient reported severe abdominal pain."\n                output: {\n                "events": [\n                    {"event_id": "e1",\n                    "event_type": "Pain",\n                    "text_quote": "severe abdominal Pain",\n                    "attributes": {"severity": "severe", \n                                   "location": "abdominal",\n                                   "duration": "Unknown",\n                                   "negation": "false",\n                                   "time":"Unknown",\n                                   "caused_by":"Unknown"}\n                    }\n                ],\n                "order":[]\n                }\n                \n                text: "Patient called his son around 3 pm."\n                output: {\n                "events": [\n                    {"event_id": "e1",\n                    "event_type": "Family",\n                    "text_quote": "called his son around 3 pm",\n                    "attributes": {"interaction": "call", \n                                    "relation": "son",\n                                    "negation": "false",\n                                    "time":"3 pm",\n                                    "caused_by":"Unknown"}\n                    }\n                ],\n                "order":[]\n                }\n                \n                text: "Patient had a loose stool overnight."\n                output: {\n                "events": [\n                    {"event_id": "e1",\n                    "event_type": "Excretion",\n                    "text_quote": "loose stool overnight",\n                    "attributes": {"type": "stool", \n                                   "quality": "loose", \n                                   "frequency":"overnight", \n                                   "negation": "false",\n                                   "time":"night",\n                                   "caused_by":"Unknown"}\n                    }\n                ],\n                "order":[]\n                }\n                \n                text: "Patient was able to sleep well last night."\n                output: {\n                "events": [\n                    {"event_id": "e1",\n                    "event_type": "Sleep",\n                    "text_quote": "sleep well last night",\n                    "attributes": {"quality": "well",\n                                    "duration": "Unknown", \n                                    "negation": "false",\n                                    "time":"night",\n                                    "caused_by":"Unknown"}\n                    }\n                ],\n                "order":[]\n                }\n                \n                text: "The patient couldn\'t sleep due to severe pain."\n                output: {\n                "events": [\n                    {"event_id": "e1",\n                    "event_type": "Sleep",\n                    "text_quote": "couldn\'t sleep",\n                    "attributes": {"quality": "poor", \n                                    "duration": "Unknown",\n                                    "negation": "true",\n                                    "time":"Unknown",\n                                    "caused_by":"Pain"}\n                    },\n                    {"event_id": "e2",\n                    "event_type": "Pain",\n                    "text_quote": "severe pain",\n                    "attributes": {"severity": "severe", \n                                    "location": "Unknown", \n                                    "duration": "Unknown", \n                                    "time":"Unknown",\n                                    "caused_by":"Unknown"}\n                    }\n                ],\n                "order":["e1", "after", "e2"]\n                }\n                \n                text: "The patient complained of severe back pain, was given Tylenol, but the pain persisted and he was then prescribed stronger morphine."\n                output: {\n                "events": [\n                    {"event_id": "e1",\n                    "event_type": "Pain",\n                    "text_quote": "complained of severe back pain",\n                    "attributes": {"severity": "severe", \n                                    "location": "back",\n                                    "duration": "Unknown", \n                                    "time":"Unknown",\n                                    "caused_by":"Unknown"}\n                    },\n                    {"event_id": "e2",\n                    "event_type": "Pain",\n                    "text_quote": "pain persisted",\n                    "attributes": {"severity": "severe", \n                                   "location": "back",\n                                   "duration": "persistent", \n                                   "time":"after Tylenol",\n                                   "caused_by":"Unknown"}\n                    }\n                ],\n                "order":[["e1", "before", "e2"]]\n                }\n                \n                        ', 'event_detection_time': 12.703115155978594}</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>[{'Sleep': {'quality': 'poor', 'duration': 'all day', 'time': 'day', 'caused_by': 'Unknown'}}, {'Eating': {'food': 'cl liquids', 'amount': 'Unknown', 'method': 'oral', 'time': 'Unknown', 'caused_by': 'Unknown'}}, {'Excretion': {'type': 'stool', 'frequency': 'none', 'quality': 'Unknown', 'time': 'Unknown', 'caused_by': 'Unknown'}}]</t>
+          <t>['Sleep', 'Eating', 'Excretion', 'Pain']</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>['sleeping all day but easily aroused', 'taking cl liquids', 'no stool']</t>
+          <t>[{'Sleep': {'quality': 'Unknown', 'duration': 'all day', 'negation': 'false', 'time': 'day', 'caused_by': 'Unknown'}}, {'Eating': {'food': 'cl liquids', 'amount': 'Unknown', 'method': 'oral', 'negation': 'false', 'time': 'Unknown', 'caused_by': 'Unknown'}}, {'Excretion': {'type': 'stool', 'frequency': 'none', 'quality': 'Unknown', 'negation': 'true', 'time': 'Unknown', 'caused_by': 'Unknown'}}, {'Pain': {'severity': 'Unknown', 'location': 'Unknown', 'duration': 'Unknown', 'negation': 'true', 'time': 'Unknown', 'caused_by': 'Unknown'}}]</t>
         </is>
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>{'text': 'patient denies pain,nausea.sleeping all day but easily aroused ,alert and oreinted.\n\nsr no ect. .neo dc ci 2.99/svr 858.now weaning milrinone.pad 13 to 19.pa sat 73 .cvp 10 to 20 .map 75 to 87.good distal pulses,bp equal both arms .\n\n6l np 7.38/32/87/20/96\n\ntaking cl liquids ,abd soft, no stool\n\nhuo 15 to 20 ,lytes sent\n\nseen by sx ,[**month (only) 108**] need mra\n\nrecheck hemodynamics and wean milrinone as tol\nfollow hcts\n', 'event': ['Sleep', 'Pain', 'Eating', 'Excretion'], 'phrase': '', 'raw_output': '{\n  "events": [\n    {\n      "event_type": "Sleep",\n      "text_quote": "sleeping all day but easily aroused",\n      "attributes": {\n        "quality": "good",\n        "duration": "all day",\n        "negation": false,\n        "time": "day"\n      }\n    },\n    {\n      "event_type": "Pain",\n      "text_quote": "patient denies pain",\n      "attributes": {}\n    },\n    {\n      "event_type": "Eating",\n      "text_quote": "taking cl liquids",\n      "attributes": {\n        "food": "cl liquids",\n        "amount": "",\n        "method": "oral",\n        "negation": false,\n        "time": ""\n      }\n    },\n    {\n      "event_type": "Excretion",\n      "text_quote": "no stool",\n      "attributes": {\n        "type": "stool",\n        "frequency": "",\n        "quality": "",\n        "negation": true,\n        "time": ""\n      }\n    }\n  ]\n}', 'attributes': [{'Sleep': {'quality': 'good', 'duration': 'all day', 'negation': False, 'time': 'day'}}, {'Pain': {}}, {'Eating': {'food': 'cl liquids', 'amount': '', 'method': 'oral', 'negation': False, 'time': ''}}, {'Excretion': {'type': 'stool', 'frequency': '', 'quality': '', 'negation': True, 'time': ''}}], 'text_quotes': ['sleeping all day but easily aroused', 'patient denies pain', 'taking cl liquids', 'no stool'], 'event_name_prompt': 'Given the text: patient denies pain,nausea.sleeping all day but easily aroused ,alert and oreinted.\n\nsr no ect. .neo dc ci 2.99/svr 858.now weaning milrinone.pad 13 to 19.pa sat 73 .cvp 10 to 20 .map 75 to 87.good distal pulses,bp equal both arms .\n\n6l np 7.38/32/87/20/96\n\ntaking cl liquids ,abd soft, no stool\n\nhuo 15 to 20 ,lytes sent\n\nseen by sx ,[**month (only) 108**] need mra\n\nrecheck hemodynamics and wean milrinone as tol\nfollow hcts\n, \n                        and the following event types with their definitions: Eating : The patient takes food into their body by mouth.\nExcretion : The patient discharges waste matter from their body.\nFamily : The patient has a visit, call, or communication with a family member.\nPain : The patient reports or shows signs of pain.\nSleep : The patient sleeps or the sleep’s quality or quantity is described.\nUnknown : choose "Unknown" if none of the other event type are applicable. \n                        ---\n                        Your task:\n                        0. Identify ALL events in the text (zero, one, or more).\n1. For each event, assign an event_type from the list above.\n2. If multiple event of same type is mentioned, assign the event_type multiple times\n3. Extract attributes for each event using ONLY the allowed attributes listed below.\n4. Use keyword evidence (Ki) ONLY if it is consistent with the text context.\n5. Output strictly valid JSON following the schema below.\n                        ---\n                        Classification Rules:\n                        - A text may contain multiple events of the same or different types.\n- Create a separate event object for each event mention.\n- If the text is explicitly a NEGATION (e.g., "denies pain"), do not extract that event.\n- If the text describes a FUTURE or HYPOTHETICAL event (e.g., "will eat tomorrow"), ignore it.\n- A valid event should have occurred in the recent past or is occurring during the time of writing of the text.\n- If no events are found or if unsure, return {"events": []}\n                        \n                        ---\n                                    Attributes allowed:\n                                    {\'Eating\': {\'food\': \'&lt;string&gt; # e.g., pancakes, porridge, etc.\', \'amount\': \'&lt;string&gt; # e.g., 1, 2 bowls, etc.\', \'method\': \'&lt;string&gt;  # e.g., oral, tube, etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, after shower, etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}, \'Excretion\': {\'type\': \'&lt;string&gt; # e.g., urine, stool, etc.\', \'frequency\': \'&lt;string&gt; # e.g., 2x, once, etc.\', \'quality\': \'&lt;string&gt; # e.g., loose, hard, etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, after shower, etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}, \'Family\': {\'interaction\': \'&lt;string&gt; # e.g., visit, call, communication, etc.\', \'relation\': \'&lt;string&gt; # e.g., mother, son, etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, after shower, etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}, \'Pain\': {\'severity\': \'&lt;string&gt; # e.g., mild, moderate, severe, numeric scale if present, etc.\', \'location\': \'&lt;string&gt; # e.g., right knee, head, etc.\', \'duration\': \'&lt;string&gt; # e.g., all night, 3 hours, etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, after shower, etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}, \'Sleep\': {\'quality\': \'&lt;string&gt; # e.g., good, poor, restless, etc.\', \'duration\': \'&lt;string&gt; # e.g., 6 hours, phrases like "all night", etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, after shower, etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}}\n                                    If no relevant attribute exists for an event, return an empty object {}.\n                                    \n                        \n                        ---\n                                    Keyword evidence (Ki):\n                                    Additional facts: A keyword matching algorithm without context detected keyword(s) [\'sleeping\', \'pain\'].\n                                    Use this only as a pointer. If context contradicts, ignore.\n                        ---\n                        Output Schema (strict):\n                        {\n                                    "events": [\n                                        {\n                                        "event_type": "&lt;Pain | Sleep | Excretion | Eating | Family&gt;",\n                                        "text_quote": "&lt;fragement from the text indicating &gt;",\n                "attributes": {\n                    "&lt;attribute_name&gt;": "&lt;attribute_value&gt;"\n                }\n                                        }\n                                    ]\n                                    }\n                        \n                            Rules:\n                                - Ensure the output is valid JSON (parseable).\n                                - "eventS" must always be an array (can be empty).\n                                - Multiple instances of the same event type appear as individual elements in the event array.\n                                - Events appear in the array in the same order in which they appear in the text.\n                                - Do not include extra keys, comments, or text.\n                                - Each object in "events" must contain "event_type", "text_quote", and "attributes".\n                                -If an event attribute type has no value mentioned, return "attributes": {"&lt; attribute name &gt;:Unknown"} for each attribute type defined for the event type \n                        \n                        \n                        \n                        ', 'event_detection_time': 7.890463899995666}</t>
+          <t>['sleeping all day but easily aroused', 'taking cl liquids', 'no stool', 'patient denies pain']</t>
         </is>
       </c>
       <c r="J4" t="inlineStr">
         <is>
-          <t>['Sleep', 'Pain', 'Eating', 'Excretion']</t>
+          <t>[[]]</t>
         </is>
       </c>
       <c r="K4" t="inlineStr">
         <is>
-          <t>[{'Sleep': {'quality': 'good', 'duration': 'all day', 'negation': False, 'time': 'day'}}, {'Pain': {}}, {'Eating': {'food': 'cl liquids', 'amount': '', 'method': 'oral', 'negation': False, 'time': ''}}, {'Excretion': {'type': 'stool', 'frequency': '', 'quality': '', 'negation': True, 'time': ''}}]</t>
+          <t>{'text': 'patient denies pain,nausea.sleeping all day but easily aroused ,alert and oreinted.\n\nsr no ect. .neo dc ci 2.99/svr 858.now weaning milrinone.pad 13 to 19.pa sat 73 .cvp 10 to 20 .map 75 to 87.good distal pulses,bp equal both arms .\n\n6l np 7.38/32/87/20/96\n\ntaking cl liquids ,abd soft, no stool\n\nhuo 15 to 20 ,lytes sent\n\nseen by sx ,[**month (only) 108**] need mra\n\nrecheck hemodynamics and wean milrinone as tol\nfollow hcts\n', 'event': ['Sleep', 'Eating', 'Excretion', 'Pain'], 'event_id': ['e1', 'e2', 'e3', 'e4'], 'phrase': '', 'raw_output': '{\n  "events": [\n    {\n      "event_id": "e1",\n      "event_type": "Sleep",\n      "text_quote": "sleeping all day but easily aroused",\n      "attributes": {\n        "quality": "Unknown",\n        "duration": "all day",\n        "negation": false,\n        "time": "day",\n        "caused_by": "Unknown"\n      }\n    },\n    {\n      "event_id": "e2",\n      "event_type": "Eating",\n      "text_quote": "taking cl liquids",\n      "attributes": {\n        "food": "cl liquids",\n        "amount": "Unknown",\n        "method": "oral",\n        "negation": false,\n        "time": "Unknown",\n        "caused_by": "Unknown"\n      }\n    },\n    {\n      "event_id": "e3",\n      "event_type": "Excretion",\n      "text_quote": "no stool",\n      "attributes": {\n        "type": "stool",\n        "frequency": "Unknown",\n        "quality": "Unknown",\n        "negation": true,\n        "time": "Unknown",\n        "caused_by": "Unknown"\n      }\n    },\n    {\n      "event_id": "e4",\n      "event_type": "Pain",\n      "text_quote": "patient denies pain",\n      "attributes": {}\n    }\n  ],\n  "order": [\n    ["e1", "before", "e2"],\n    ["e2", "before", "e3"],\n    ["e3", "before", "e4"]\n  ]\n}', 'attributes': [{'Sleep': {'quality': 'Unknown', 'duration': 'all day', 'negation': False, 'time': 'day', 'caused_by': 'Unknown'}}, {'Eating': {'food': 'cl liquids', 'amount': 'Unknown', 'method': 'oral', 'negation': False, 'time': 'Unknown', 'caused_by': 'Unknown'}}, {'Excretion': {'type': 'stool', 'frequency': 'Unknown', 'quality': 'Unknown', 'negation': True, 'time': 'Unknown', 'caused_by': 'Unknown'}}, {'Pain': {}}], 'orders': [[['e1', 'before', 'e2'], ['e2', 'before', 'e3'], ['e3', 'before', 'e4']]], 'text_quotes': ['sleeping all day but easily aroused', 'taking cl liquids', 'no stool', 'patient denies pain'], 'event_name_prompt': 'Given the text: patient denies pain,nausea.sleeping all day but easily aroused ,alert and oreinted.\n\nsr no ect. .neo dc ci 2.99/svr 858.now weaning milrinone.pad 13 to 19.pa sat 73 .cvp 10 to 20 .map 75 to 87.good distal pulses,bp equal both arms .\n\n6l np 7.38/32/87/20/96\n\ntaking cl liquids ,abd soft, no stool\n\nhuo 15 to 20 ,lytes sent\n\nseen by sx ,[**month (only) 108**] need mra\n\nrecheck hemodynamics and wean milrinone as tol\nfollow hcts\n, \n                        and the following event types with their definitions: Eating : The patient takes food into their body by mouth.\nExcretion : The patient discharges waste matter from their body.\nFamily : The patient has a visit, call, or communication with a family member.\nPain : The patient reports or shows signs of pain.\nSleep : The patient sleeps or the sleep’s quality or quantity is described.\nUnknown : choose "Unknown" if none of the other event type are applicable. \n                        ---\n                        Your task:\n                        0. Identify ALL events in the text (zero, one, or more).\n1. For each event, assign an event_type from the list above.\n2. If multiple event of same type is mentioned, assign the event_type multiple times\n3. Extract attributes for each event using ONLY the allowed attributes listed below.\n4. Use keyword evidence (Ki) ONLY if it is consistent with the text context.\n5. Output strictly valid JSON following the schema below.\n                        ---\n                        Classification Rules:\n                        - A text may contain multiple events of the same or different types.\n- Create a separate event object for each event mention.\n- If the text is explicitly a NEGATION (e.g., "denies pain"), do not extract that event.\n- If the text describes a FUTURE or HYPOTHETICAL event (e.g., "will eat tomorrow"), ignore it.\n- A valid event should have occurred in the recent past or is occurring during the time of writing of the text.\n- If no events are found or if unsure, return {"events": []}\n                        \n                        ---\n                                    Attributes allowed:\n                                    {\'Eating\': {\'food\': \'&lt;string&gt; # e.g., pancakes, porridge, etc.\', \'amount\': \'&lt;string&gt; # e.g., 1, 2 bowls, etc.\', \'method\': \'&lt;string&gt;  # e.g., oral, tube, etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, evening etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}, \'Excretion\': {\'type\': \'&lt;string&gt; # e.g., urine, stool, etc.\', \'frequency\': \'&lt;string&gt; # e.g., 2x, once, etc.\', \'quality\': \'&lt;string&gt; # e.g., loose, hard, etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, evening etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}, \'Family\': {\'interaction\': \'&lt;string&gt; # e.g., visit, call, communication, etc.\', \'relation\': \'&lt;string&gt; # e.g., mother, son, etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, evening etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}, \'Pain\': {\'severity\': \'&lt;string&gt; # e.g., mild, moderate, severe, numeric scale if present, etc.\', \'location\': \'&lt;string&gt; # e.g., right knee, head, etc.\', \'duration\': \'&lt;string&gt; # e.g., all night, 3 hours, etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, evening etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}, \'Sleep\': {\'quality\': \'&lt;string&gt; # e.g., good, poor, restless, etc.\', \'duration\': \'&lt;string&gt; # e.g., 6 hours, phrases like "all night", etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, evening etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}}\n                                    If no relevant attribute exists for an event, return an empty object {}.\n                                    \n                        \n                        ---\n                                    Keyword evidence (Ki):\n                                    Additional facts: A keyword matching algorithm without context detected keyword(s) (\'pain\', \'sleeping\').\n                                    Use this only as a pointer. If context contradicts, ignore.\n                        ---\n                        Output Schema (strict):\n                        {\n                                    "events": [\n                                        {\n                                        "event_id": "&lt; A unique id eg.: e1 | e2 |...&gt;"\n                                        "event_type": "&lt;Pain | Sleep | Excretion | Eating | Family&gt;",\n                                        "text_quote": "&lt;fragement from the text indicating the event_type&gt;",\n                "attributes": {\n                    "&lt;attribute_name&gt;": "&lt;attribute_value&gt;"\n                }\n                                        }\n                                    ],\n                                    "order": [\n                                        ["e1", "before" | "after" | "simultaneous", "e2" ]\n                                    ]\n                                    }\n                        \n                            Rules:\n                                - Ensure the output is valid JSON (parseable).\n                                - "eventS" must always be an array (can be empty).\n                                - Multiple instances of the same event type appear with different ids.\n                                - Events appear in the array in the same order in which they appear in the text.\n                                - Their partial orders can be expressed using the "order" section.\n                                - Do not include extra keys, comments, or text.\n                                - Each object in "events" must contain "event_type", "text_quote", and "attributes".\n                                - If an event attribute type has no value mentioned, return "attributes": {"&lt; attribute name &gt;:Unknown"} for each attribute type defined for the event type \n                        \n                        \n                        \n                        ', 'event_detection_time': 11.330217683047522}</t>
         </is>
       </c>
       <c r="L4" t="inlineStr">
         <is>
-          <t>['sleeping all day but easily aroused', 'patient denies pain', 'taking cl liquids', 'no stool']</t>
+          <t>['Sleep', 'Eating', 'Excretion', 'Pain']</t>
         </is>
       </c>
       <c r="M4" t="inlineStr">
         <is>
-          <t>{'text': 'patient denies pain,nausea.sleeping all day but easily aroused ,alert and oreinted.\n\nsr no ect. .neo dc ci 2.99/svr 858.now weaning milrinone.pad 13 to 19.pa sat 73 .cvp 10 to 20 .map 75 to 87.good distal pulses,bp equal both arms .\n\n6l np 7.38/32/87/20/96\n\ntaking cl liquids ,abd soft, no stool\n\nhuo 15 to 20 ,lytes sent\n\nseen by sx ,[**month (only) 108**] need mra\n\nrecheck hemodynamics and wean milrinone as tol\nfollow hcts\n', 'event': ['Sleep', 'Eating', 'Excretion'], 'phrase': '', 'raw_output': '{\n  "events": [\n    {\n      "event_type": "Sleep",\n      "text_quote": "sleeping all day but easily aroused",\n      "attributes": {\n        "quality": "poor",\n        "duration": "all day",\n        "time": "day",\n        "caused_by": "Unknown"\n      }\n    },\n    {\n      "event_type": "Eating",\n      "text_quote": "taking cl liquids",\n      "attributes": {\n        "food": "cl liquids",\n        "amount": "Unknown",\n        "method": "oral",\n        "time": "Unknown",\n        "caused_by": "Unknown"\n      }\n    },\n    {\n      "event_type": "Excretion",\n      "text_quote": "no stool",\n      "attributes": {\n        "type": "stool",\n        "frequency": "none",\n        "quality": "Unknown",\n        "time": "Unknown",\n        "caused_by": "Unknown"\n      }\n    }\n  ]\n}', 'attributes': [{'Sleep': {'quality': 'poor', 'duration': 'all day', 'time': 'day', 'caused_by': 'Unknown'}}, {'Eating': {'food': 'cl liquids', 'amount': 'Unknown', 'method': 'oral', 'time': 'Unknown', 'caused_by': 'Unknown'}}, {'Excretion': {'type': 'stool', 'frequency': 'none', 'quality': 'Unknown', 'time': 'Unknown', 'caused_by': 'Unknown'}}], 'text_quotes': ['sleeping all day but easily aroused', 'taking cl liquids', 'no stool'], 'event_name_prompt': 'Given the text: patient denies pain,nausea.sleeping all day but easily aroused ,alert and oreinted.\n\nsr no ect. .neo dc ci 2.99/svr 858.now weaning milrinone.pad 13 to 19.pa sat 73 .cvp 10 to 20 .map 75 to 87.good distal pulses,bp equal both arms .\n\n6l np 7.38/32/87/20/96\n\ntaking cl liquids ,abd soft, no stool\n\nhuo 15 to 20 ,lytes sent\n\nseen by sx ,[**month (only) 108**] need mra\n\nrecheck hemodynamics and wean milrinone as tol\nfollow hcts\n, \n                        and the following event types with their definitions: Eating : The patient takes food into their body by mouth.\nExcretion : The patient discharges waste matter from their body.\nFamily : The patient has a visit, call, or communication with a family member.\nPain : The patient reports or shows signs of pain.\nSleep : The patient sleeps or the sleep’s quality or quantity is described.\nUnknown : choose "Unknown" if none of the other event type are applicable. \n                        ---\n                        Your task:\n                        0. Identify ALL events in the text (zero, one, or more).\n1. For each event, assign an event_type from the list above.\n2. If multiple event of same type is mentioned, assign the event_type multiple times\n3. Extract attributes for each event using ONLY the allowed attributes listed below.\n4. Output strictly valid JSON following the schema below.\n                        ---\n                        Classification Rules:\n                        - A text may contain multiple events of the same or different types.\n- Create a separate event object for each event mention.\n- If the text is explicitly a NEGATION (e.g., "denies pain"), do not extract that event.\n- If the text describes a FUTURE or HYPOTHETICAL event (e.g., "will eat tomorrow"), ignore it.\n- A valid event should have occurred in the recent past or is occurring during the time of writing of the text.\n- If no events are found or if unsure, return {"events": []}\n                        \n                        ---\n                                    Attributes allowed:\n                                    {\'Eating\': {\'food\': \'&lt;string&gt; # e.g., pancakes, porridge, etc.\', \'amount\': \'&lt;string&gt; # e.g., 1, 2 bowls, etc.\', \'method\': \'&lt;string&gt;  # e.g., oral, tube, etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, after shower, etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}, \'Excretion\': {\'type\': \'&lt;string&gt; # e.g., urine, stool, etc.\', \'frequency\': \'&lt;string&gt; # e.g., 2x, once, etc.\', \'quality\': \'&lt;string&gt; # e.g., loose, hard, etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, after shower, etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}, \'Family\': {\'interaction\': \'&lt;string&gt; # e.g., visit, call, communication, etc.\', \'relation\': \'&lt;string&gt; # e.g., mother, son, etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, after shower, etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}, \'Pain\': {\'severity\': \'&lt;string&gt; # e.g., mild, moderate, severe, numeric scale if present, etc.\', \'location\': \'&lt;string&gt; # e.g., right knee, head, etc.\', \'duration\': \'&lt;string&gt; # e.g., all night, 3 hours, etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, after shower, etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}, \'Sleep\': {\'quality\': \'&lt;string&gt; # e.g., good, poor, restless, etc.\', \'duration\': \'&lt;string&gt; # e.g., 6 hours, phrases like "all night", etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, after shower, etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}}\n                                    If no relevant attribute exists for an event, return an empty object {}.\n                                    \n                        \n                        \n                        ---\n                        Output Schema (strict):\n                        {\n                                    "events": [\n                                        {\n                                        "event_type": "&lt;Pain | Sleep | Excretion | Eating | Family&gt;",\n                                        "text_quote": "&lt;fragement from the text indicating &gt;",\n                "attributes": {\n                    "&lt;attribute_name&gt;": "&lt;attribute_value&gt;"\n                }\n                                        }\n                                    ]\n                                    }\n                        \n                            Rules:\n                                - Ensure the output is valid JSON (parseable).\n                                - "eventS" must always be an array (can be empty).\n                                - Multiple instances of the same event type appear as individual elements in the event array.\n                                - Events appear in the array in the same order in which they appear in the text.\n                                - Do not include extra keys, comments, or text.\n                                - Each object in "events" must contain "event_type", "text_quote", and "attributes".\n                                -If an event attribute type has no value mentioned, return "attributes": {"&lt; attribute name &gt;:Unknown"} for each attribute type defined for the event type \n                        \n                        \n                        \n                ---\n                Examples:\n                \n                text: "Patient ate breakfast this morning. He seems less anxious."\n                output: {\n                "events": [\n                    {\n                    "event_type": "Eating",\n                    "text_quote":"Patient ate breakfast this morning",\n                    "attributes": {"food": "breakfast", \n                                   "amount": "Unknown",\n                                   "method": "Unknown",\n                                   "time":"morning",\n                                   "caused_by":"Unknown"}\n                    }\n                ]\n                }\n                \n                text: "Patient reported severe abdominal pain."\n                output: {\n                "events": [\n                    {\n                    "event_type": "Pain",\n                    "text_quote": "severe abdominal Pain",\n                    "attributes": {"severity": "severe", \n                                   "location": "abdominal",\n                                   "duration": "Unknown",\n                                   "time":"Unknown",\n                                   "caused_by":"Unknown"}\n                    }\n                ]\n                }\n                \n                text: "Patient called his son around 3 pm."\n                output: {\n                "events": [\n                    {\n                    "event_type": "Family",\n                    "text_quote": "called his son around 3 pm",\n                    "attributes": {"interaction": "call", \n                                    "relation": "son",\n                                    "time":"3 pm",\n                                    "caused_by":"Unknown"}\n                    }\n                ]\n                }\n                \n                text: "Patient had a loose stool overnight."\n                output: {\n                "events": [\n                    {\n                    "event_type": "Excretion",\n                    "text_quote": "loose stool overnight",\n                    "attributes": {"type": "stool", \n                                   "quality": "loose", \n                                   "frequency":"overnight", \n                                   "time":"night",\n                                   "caused_by":"Unknown"}\n                    }\n                ]\n                }\n                \n                text: "Patient was able to sleep well last night."\n                output: {\n                "events": [\n                    {\n                    "event_type": "Sleep",\n                    "text_quote": "sleep well last night",\n                    "attributes": {"quality": "well",\n                                    "duration": "Unknown", \n                                    "time":"night",\n                                    "caused_by":"Unknown"}\n                    }\n                ]\n                }\n                \n                text: "The patient couldn\'t sleep due to severe pain."\n                output: {\n                "events": [\n                    {\n                    "event_type": "Sleep",\n                    "text_quote": "couldn\'t sleep",\n                    "attributes": {"quality": "poor", \n                                    "duration": "Unknown",\n                                   "time":"Unknown",\n                                   "caused_by":"Pain"}\n                    },\n                    {\n                    "event_type": "Pain",\n                    "text_quote": "severe pain",\n                    "attributes": {"severity": "severe", \n                                    "location": "Unknown", \n                                    "duration": "Unknown", \n                                   "time":"before Sleep",\n                                   "caused_by":"Unknown"}\n                    }\n                ]\n                }\n                \n                text: "The patient complained of severe back pain, was given Tylenol, but the pain persisted and he was then prescribed stronger morphine."\n                output: {\n                "events": [\n                    {\n                    "event_type": "Pain",\n                    "text_quote": "complained of severe back pain",\n                    "attributes": {"severity": "severe", \n                                    "location": "back",\n                                    "duration": "Unknown", \n                                    "time":"Unknown",\n                                    "caused_by":"Unknown"}\n                    },\n                    {\n                    "event_type": "Pain",\n                    "text_quote": "pain persisted",\n                    "attributes": {"severity": "severe", \n                                   "location": "back",\n                                   "duration": "persistent", \n                                   "time":"after Tylenol",\n                                   "caused_by":"Unknown"}\n                    }\n                ]\n                }\n                \n                        ', 'event_detection_time': 8.200177528007771}</t>
+          <t>[{'Sleep': {'quality': 'Unknown', 'duration': 'all day', 'negation': False, 'time': 'day', 'caused_by': 'Unknown'}}, {'Eating': {'food': 'cl liquids', 'amount': 'Unknown', 'method': 'oral', 'negation': False, 'time': 'Unknown', 'caused_by': 'Unknown'}}, {'Excretion': {'type': 'stool', 'frequency': 'Unknown', 'quality': 'Unknown', 'negation': True, 'time': 'Unknown', 'caused_by': 'Unknown'}}, {'Pain': {}}]</t>
         </is>
       </c>
       <c r="N4" t="inlineStr">
         <is>
-          <t>['Sleep', 'Eating', 'Excretion']</t>
+          <t>['sleeping all day but easily aroused', 'taking cl liquids', 'no stool', 'patient denies pain']</t>
         </is>
       </c>
       <c r="O4" t="inlineStr">
         <is>
-          <t>[{'Sleep': {'quality': 'poor', 'duration': 'all day', 'time': 'day', 'caused_by': 'Unknown'}}, {'Eating': {'food': 'cl liquids', 'amount': 'Unknown', 'method': 'oral', 'time': 'Unknown', 'caused_by': 'Unknown'}}, {'Excretion': {'type': 'stool', 'frequency': 'none', 'quality': 'Unknown', 'time': 'Unknown', 'caused_by': 'Unknown'}}]</t>
-        </is>
-      </c>
-      <c r="P4" t="inlineStr">
-        <is>
-          <t>['sleeping all day but easily aroused', 'taking cl liquids', 'no stool']</t>
-        </is>
-      </c>
-      <c r="Q4" t="n">
-        <v>0.003026361999218352</v>
-      </c>
-      <c r="R4" t="inlineStr">
+          <t>[[['e1', 'before', 'e2'], ['e2', 'before', 'e3'], ['e3', 'before', 'e4']]]</t>
+        </is>
+      </c>
+      <c r="P4" t="n">
+        <v>0.002323559998330893</v>
+      </c>
+      <c r="Q4" t="inlineStr">
         <is>
           <t>Sleep</t>
         </is>
       </c>
-      <c r="S4" t="b">
-        <v>0</v>
+      <c r="R4" t="b">
+        <v>0</v>
+      </c>
+      <c r="S4" t="n">
+        <v>1</v>
       </c>
       <c r="T4" t="n">
         <v>1</v>
       </c>
-      <c r="U4" t="n">
-        <v>1</v>
-      </c>
-      <c r="V4" t="inlineStr">
+      <c r="U4" t="inlineStr">
         <is>
           <t>('pain', 'sleeping')</t>
         </is>
       </c>
+      <c r="V4" t="n">
+        <v>12.70311515597859</v>
+      </c>
       <c r="W4" t="n">
-        <v>8.34106302598957</v>
+        <v>11.33021768304752</v>
       </c>
       <c r="X4" t="n">
-        <v>7.890463899995666</v>
+        <v>1</v>
       </c>
       <c r="Y4" t="n">
-        <v>8.200177528007771</v>
+        <v>1</v>
       </c>
       <c r="Z4" t="n">
-        <v>1</v>
-      </c>
-      <c r="AA4" t="n">
-        <v>1</v>
-      </c>
-      <c r="AB4" t="n">
-        <v>1</v>
-      </c>
-      <c r="AC4" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" t="n">
-        <v>1310481</v>
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>1310481</t>
+        </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>['Pain', 'Unknown']</t>
+          <t>('Pain', 'Unknown')</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>['pain']</t>
+          <t>('pain',)</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
@@ -1015,120 +977,111 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>{'text': '7 pm  bp to 80,ci &gt; 2 on less milrinone,wedge 16 .patient co of mild back pain .seen by ho.fluid bollus ordered.stat hct,chem 6 sent\n', 'event': ['Pain', 'Family'], 'phrase': '', 'raw_output': '{\n  "events": [\n    {\n      "event_type": "Pain",\n      "text_quote": "patient co of mild back pain",\n      "attributes": {\n        "severity": "mild",\n        "location": "back",\n        "duration": "Unknown",\n        "time": "Unknown",\n        "caused_by": "Unknown"\n      }\n    },\n    {\n      "event_type": "Family",\n      "text_quote": "seen by ho",\n      "attributes": {\n        "interaction": "visit",\n        "relation": "Unknown",\n        "time": "Unknown",\n        "caused_by": "Unknown"\n      }\n    }\n  ]\n}', 'attributes': [{'Pain': {'severity': 'mild', 'location': 'back', 'duration': 'Unknown', 'time': 'Unknown', 'caused_by': 'Unknown'}}, {'Family': {'interaction': 'visit', 'relation': 'Unknown', 'time': 'Unknown', 'caused_by': 'Unknown'}}], 'text_quotes': ['patient co of mild back pain', 'seen by ho'], 'event_name_prompt': 'Given the text: 7 pm  bp to 80,ci &gt; 2 on less milrinone,wedge 16 .patient co of mild back pain .seen by ho.fluid bollus ordered.stat hct,chem 6 sent\n, \n                        and the following event types with their definitions: Eating : The patient takes food into their body by mouth.\nExcretion : The patient discharges waste matter from their body.\nFamily : The patient has a visit, call, or communication with a family member.\nPain : The patient reports or shows signs of pain.\nSleep : The patient sleeps or the sleep’s quality or quantity is described.\nUnknown : choose "Unknown" if none of the other event type are applicable. \n                        ---\n                        Your task:\n                        0. Identify ALL events in the text (zero, one, or more).\n1. For each event, assign an event_type from the list above.\n2. If multiple event of same type is mentioned, assign the event_type multiple times\n3. Extract attributes for each event using ONLY the allowed attributes listed below.\n4. Use keyword evidence (Ki) ONLY if it is consistent with the text context.\n5. Output strictly valid JSON following the schema below.\n                        ---\n                        Classification Rules:\n                        - A text may contain multiple events of the same or different types.\n- Create a separate event object for each event mention.\n- If the text is explicitly a NEGATION (e.g., "denies pain"), do not extract that event.\n- If the text describes a FUTURE or HYPOTHETICAL event (e.g., "will eat tomorrow"), ignore it.\n- A valid event should have occurred in the recent past or is occurring during the time of writing of the text.\n- If no events are found or if unsure, return {"events": []}\n                        \n                        ---\n                                    Attributes allowed:\n                                    {\'Eating\': {\'food\': \'&lt;string&gt; # e.g., pancakes, porridge, etc.\', \'amount\': \'&lt;string&gt; # e.g., 1, 2 bowls, etc.\', \'method\': \'&lt;string&gt;  # e.g., oral, tube, etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, after shower, etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}, \'Excretion\': {\'type\': \'&lt;string&gt; # e.g., urine, stool, etc.\', \'frequency\': \'&lt;string&gt; # e.g., 2x, once, etc.\', \'quality\': \'&lt;string&gt; # e.g., loose, hard, etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, after shower, etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}, \'Family\': {\'interaction\': \'&lt;string&gt; # e.g., visit, call, communication, etc.\', \'relation\': \'&lt;string&gt; # e.g., mother, son, etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, after shower, etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}, \'Pain\': {\'severity\': \'&lt;string&gt; # e.g., mild, moderate, severe, numeric scale if present, etc.\', \'location\': \'&lt;string&gt; # e.g., right knee, head, etc.\', \'duration\': \'&lt;string&gt; # e.g., all night, 3 hours, etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, after shower, etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}, \'Sleep\': {\'quality\': \'&lt;string&gt; # e.g., good, poor, restless, etc.\', \'duration\': \'&lt;string&gt; # e.g., 6 hours, phrases like "all night", etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, after shower, etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}}\n                                    If no relevant attribute exists for an event, return an empty object {}.\n                                    \n                        \n                        ---\n                                    Keyword evidence (Ki):\n                                    Additional facts: A keyword matching algorithm without context detected keyword(s) [\'pain\'].\n                                    Use this only as a pointer. If context contradicts, ignore.\n                        ---\n                        Output Schema (strict):\n                        {\n                                    "events": [\n                                        {\n                                        "event_type": "&lt;Pain | Sleep | Excretion | Eating | Family&gt;",\n                                        "text_quote": "&lt;fragement from the text indicating &gt;",\n                "attributes": {\n                    "&lt;attribute_name&gt;": "&lt;attribute_value&gt;"\n                }\n                                        }\n                                    ]\n                                    }\n                        \n                            Rules:\n                                - Ensure the output is valid JSON (parseable).\n                                - "eventS" must always be an array (can be empty).\n                                - Multiple instances of the same event type appear as individual elements in the event array.\n                                - Events appear in the array in the same order in which they appear in the text.\n                                - Do not include extra keys, comments, or text.\n                                - Each object in "events" must contain "event_type", "text_quote", and "attributes".\n                                -If an event attribute type has no value mentioned, return "attributes": {"&lt; attribute name &gt;:Unknown"} for each attribute type defined for the event type \n                        \n                        \n                        \n                ---\n                Examples:\n                \n                text: "Patient ate breakfast this morning. He seems less anxious."\n                output: {\n                "events": [\n                    {\n                    "event_type": "Eating",\n                    "text_quote":"Patient ate breakfast this morning",\n                    "attributes": {"food": "breakfast", \n                                   "amount": "Unknown",\n                                   "method": "Unknown",\n                                   "time":"morning",\n                                   "caused_by":"Unknown"}\n                    }\n                ]\n                }\n                \n                text: "Patient reported severe abdominal pain."\n                output: {\n                "events": [\n                    {\n                    "event_type": "Pain",\n                    "text_quote": "severe abdominal Pain",\n                    "attributes": {"severity": "severe", \n                                   "location": "abdominal",\n                                   "duration": "Unknown",\n                                   "time":"Unknown",\n                                   "caused_by":"Unknown"}\n                    }\n                ]\n                }\n                \n                text: "Patient called his son around 3 pm."\n                output: {\n                "events": [\n                    {\n                    "event_type": "Family",\n                    "text_quote": "called his son around 3 pm",\n                    "attributes": {"interaction": "call", \n                                    "relation": "son",\n                                    "time":"3 pm",\n                                    "caused_by":"Unknown"}\n                    }\n                ]\n                }\n                \n                text: "Patient had a loose stool overnight."\n                output: {\n                "events": [\n                    {\n                    "event_type": "Excretion",\n                    "text_quote": "loose stool overnight",\n                    "attributes": {"type": "stool", \n                                   "quality": "loose", \n                                   "frequency":"overnight", \n                                   "time":"night",\n                                   "caused_by":"Unknown"}\n                    }\n                ]\n                }\n                \n                text: "Patient was able to sleep well last night."\n                output: {\n                "events": [\n                    {\n                    "event_type": "Sleep",\n                    "text_quote": "sleep well last night",\n                    "attributes": {"quality": "well",\n                                    "duration": "Unknown", \n                                    "time":"night",\n                                    "caused_by":"Unknown"}\n                    }\n                ]\n                }\n                \n                text: "The patient couldn\'t sleep due to severe pain."\n                output: {\n                "events": [\n                    {\n                    "event_type": "Sleep",\n                    "text_quote": "couldn\'t sleep",\n                    "attributes": {"quality": "poor", \n                                    "duration": "Unknown",\n                                   "time":"Unknown",\n                                   "caused_by":"Pain"}\n                    },\n                    {\n                    "event_type": "Pain",\n                    "text_quote": "severe pain",\n                    "attributes": {"severity": "severe", \n                                    "location": "Unknown", \n                                    "duration": "Unknown", \n                                   "time":"before Sleep",\n                                   "caused_by":"Unknown"}\n                    }\n                ]\n                }\n                \n                text: "The patient complained of severe back pain, was given Tylenol, but the pain persisted and he was then prescribed stronger morphine."\n                output: {\n                "events": [\n                    {\n                    "event_type": "Pain",\n                    "text_quote": "complained of severe back pain",\n                    "attributes": {"severity": "severe", \n                                    "location": "back",\n                                    "duration": "Unknown", \n                                    "time":"Unknown",\n                                    "caused_by":"Unknown"}\n                    },\n                    {\n                    "event_type": "Pain",\n                    "text_quote": "pain persisted",\n                    "attributes": {"severity": "severe", \n                                   "location": "back",\n                                   "duration": "persistent", \n                                   "time":"after Tylenol",\n                                   "caused_by":"Unknown"}\n                    }\n                ]\n                }\n                \n                        ', 'event_detection_time': 6.121830725009204}</t>
+          <t>['pain']</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
+          <t>{'text': '7 pm  bp to 80,ci &gt; 2 on less milrinone,wedge 16 .patient co of mild back pain .seen by ho.fluid bollus ordered.stat hct,chem 6 sent\n', 'event': ['Pain', 'Family'], 'event_id': ['e1', 'e2'], 'phrase': '', 'raw_output': '{\n  "events": [\n    {\n      "event_id": "e1",\n      "event_type": "Pain",\n      "text_quote": "patient co of mild back pain",\n      "attributes": {\n        "severity": "mild",\n        "location": "back",\n        "duration": "Unknown",\n        "negation": "false",\n        "time": "Unknown",\n        "caused_by": "Unknown"\n      }\n    },\n    {\n      "event_id": "e2",\n      "event_type": "Family",\n      "text_quote": "seen by ho",\n      "attributes": {\n        "interaction": "visit",\n        "relation": "Unknown",\n        "negation": "false",\n        "time": "Unknown",\n        "caused_by": "Unknown"\n      }\n    }\n  ],\n  "order": []\n}', 'attributes': [{'Pain': {'severity': 'mild', 'location': 'back', 'duration': 'Unknown', 'negation': 'false', 'time': 'Unknown', 'caused_by': 'Unknown'}}, {'Family': {'interaction': 'visit', 'relation': 'Unknown', 'negation': 'false', 'time': 'Unknown', 'caused_by': 'Unknown'}}], 'orders': [[]], 'text_quotes': ['patient co of mild back pain', 'seen by ho'], 'event_name_prompt': 'Given the text: 7 pm  bp to 80,ci &gt; 2 on less milrinone,wedge 16 .patient co of mild back pain .seen by ho.fluid bollus ordered.stat hct,chem 6 sent\n, \n                        and the following event types with their definitions: Eating : The patient takes food into their body by mouth.\nExcretion : The patient discharges waste matter from their body.\nFamily : The patient has a visit, call, or communication with a family member.\nPain : The patient reports or shows signs of pain.\nSleep : The patient sleeps or the sleep’s quality or quantity is described.\nUnknown : choose "Unknown" if none of the other event type are applicable. \n                        ---\n                        Your task:\n                        0. Identify ALL events in the text (zero, one, or more).\n1. For each event, assign an event_type from the list above.\n2. If multiple event of same type is mentioned, assign the event_type multiple times\n3. Extract attributes for each event using ONLY the allowed attributes listed below.\n4. Use keyword evidence (Ki) ONLY if it is consistent with the text context.\n5. Output strictly valid JSON following the schema below.\n                        ---\n                        Classification Rules:\n                        - A text may contain multiple events of the same or different types.\n- Create a separate event object for each event mention.\n- If the text is explicitly a NEGATION (e.g., "denies pain"), do not extract that event.\n- If the text describes a FUTURE or HYPOTHETICAL event (e.g., "will eat tomorrow"), ignore it.\n- A valid event should have occurred in the recent past or is occurring during the time of writing of the text.\n- If no events are found or if unsure, return {"events": []}\n                        \n                        ---\n                                    Attributes allowed:\n                                    {\'Eating\': {\'food\': \'&lt;string&gt; # e.g., pancakes, porridge, etc.\', \'amount\': \'&lt;string&gt; # e.g., 1, 2 bowls, etc.\', \'method\': \'&lt;string&gt;  # e.g., oral, tube, etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, evening etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}, \'Excretion\': {\'type\': \'&lt;string&gt; # e.g., urine, stool, etc.\', \'frequency\': \'&lt;string&gt; # e.g., 2x, once, etc.\', \'quality\': \'&lt;string&gt; # e.g., loose, hard, etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, evening etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}, \'Family\': {\'interaction\': \'&lt;string&gt; # e.g., visit, call, communication, etc.\', \'relation\': \'&lt;string&gt; # e.g., mother, son, etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, evening etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}, \'Pain\': {\'severity\': \'&lt;string&gt; # e.g., mild, moderate, severe, numeric scale if present, etc.\', \'location\': \'&lt;string&gt; # e.g., right knee, head, etc.\', \'duration\': \'&lt;string&gt; # e.g., all night, 3 hours, etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, evening etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}, \'Sleep\': {\'quality\': \'&lt;string&gt; # e.g., good, poor, restless, etc.\', \'duration\': \'&lt;string&gt; # e.g., 6 hours, phrases like "all night", etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, evening etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}}\n                                    If no relevant attribute exists for an event, return an empty object {}.\n                                    \n                        \n                        ---\n                                    Keyword evidence (Ki):\n                                    Additional facts: A keyword matching algorithm without context detected keyword(s) (\'pain\',).\n                                    Use this only as a pointer. If context contradicts, ignore.\n                        ---\n                        Output Schema (strict):\n                        {\n                                    "events": [\n                                        {\n                                        "event_id": "&lt; A unique id eg.: e1 | e2 |...&gt;"\n                                        "event_type": "&lt;Pain | Sleep | Excretion | Eating | Family&gt;",\n                                        "text_quote": "&lt;fragement from the text indicating the event_type&gt;",\n                "attributes": {\n                    "&lt;attribute_name&gt;": "&lt;attribute_value&gt;"\n                }\n                                        }\n                                    ],\n                                    "order": [\n                                        ["e1", "before" | "after" | "simultaneous", "e2" ]\n                                    ]\n                                    }\n                        \n                            Rules:\n                                - Ensure the output is valid JSON (parseable).\n                                - "eventS" must always be an array (can be empty).\n                                - Multiple instances of the same event type appear with different ids.\n                                - Events appear in the array in the same order in which they appear in the text.\n                                - Their partial orders can be expressed using the "order" section.\n                                - Do not include extra keys, comments, or text.\n                                - Each object in "events" must contain "event_type", "text_quote", and "attributes".\n                                - If an event attribute type has no value mentioned, return "attributes": {"&lt; attribute name &gt;:Unknown"} for each attribute type defined for the event type \n                        \n                        \n                        \n                ---\n                Examples:\n                \n                text: "Patient ate breakfast this morning. He seems less anxious."\n                output: {\n                "events": [\n                    {"event_id": "e1",\n                    "event_type": "Eating",\n                    "text_quote":"Patient ate breakfast this morning",\n                    "attributes": {"food": "breakfast", \n                                   "amount": "Unknown",\n                                   "method": "Unknown",\n                                   "negation": "false",\n                                   "time":"morning",\n                                   "caused_by":"Unknown"}\n                    }\n                ],\n                "order":[]\n                }\n                \n                text: "Patient reported severe abdominal pain."\n                output: {\n                "events": [\n                    {"event_id": "e1",\n                    "event_type": "Pain",\n                    "text_quote": "severe abdominal Pain",\n                    "attributes": {"severity": "severe", \n                                   "location": "abdominal",\n                                   "duration": "Unknown",\n                                   "negation": "false",\n                                   "time":"Unknown",\n                                   "caused_by":"Unknown"}\n                    }\n                ],\n                "order":[]\n                }\n                \n                text: "Patient called his son around 3 pm."\n                output: {\n                "events": [\n                    {"event_id": "e1",\n                    "event_type": "Family",\n                    "text_quote": "called his son around 3 pm",\n                    "attributes": {"interaction": "call", \n                                    "relation": "son",\n                                    "negation": "false",\n                                    "time":"3 pm",\n                                    "caused_by":"Unknown"}\n                    }\n                ],\n                "order":[]\n                }\n                \n                text: "Patient had a loose stool overnight."\n                output: {\n                "events": [\n                    {"event_id": "e1",\n                    "event_type": "Excretion",\n                    "text_quote": "loose stool overnight",\n                    "attributes": {"type": "stool", \n                                   "quality": "loose", \n                                   "frequency":"overnight", \n                                   "negation": "false",\n                                   "time":"night",\n                                   "caused_by":"Unknown"}\n                    }\n                ],\n                "order":[]\n                }\n                \n                text: "Patient was able to sleep well last night."\n                output: {\n                "events": [\n                    {"event_id": "e1",\n                    "event_type": "Sleep",\n                    "text_quote": "sleep well last night",\n                    "attributes": {"quality": "well",\n                                    "duration": "Unknown", \n                                    "negation": "false",\n                                    "time":"night",\n                                    "caused_by":"Unknown"}\n                    }\n                ],\n                "order":[]\n                }\n                \n                text: "The patient couldn\'t sleep due to severe pain."\n                output: {\n                "events": [\n                    {"event_id": "e1",\n                    "event_type": "Sleep",\n                    "text_quote": "couldn\'t sleep",\n                    "attributes": {"quality": "poor", \n                                    "duration": "Unknown",\n                                    "negation": "true",\n                                    "time":"Unknown",\n                                    "caused_by":"Pain"}\n                    },\n                    {"event_id": "e2",\n                    "event_type": "Pain",\n                    "text_quote": "severe pain",\n                    "attributes": {"severity": "severe", \n                                    "location": "Unknown", \n                                    "duration": "Unknown", \n                                    "time":"Unknown",\n                                    "caused_by":"Unknown"}\n                    }\n                ],\n                "order":["e1", "after", "e2"]\n                }\n                \n                text: "The patient complained of severe back pain, was given Tylenol, but the pain persisted and he was then prescribed stronger morphine."\n                output: {\n                "events": [\n                    {"event_id": "e1",\n                    "event_type": "Pain",\n                    "text_quote": "complained of severe back pain",\n                    "attributes": {"severity": "severe", \n                                    "location": "back",\n                                    "duration": "Unknown", \n                                    "time":"Unknown",\n                                    "caused_by":"Unknown"}\n                    },\n                    {"event_id": "e2",\n                    "event_type": "Pain",\n                    "text_quote": "pain persisted",\n                    "attributes": {"severity": "severe", \n                                   "location": "back",\n                                   "duration": "persistent", \n                                   "time":"after Tylenol",\n                                   "caused_by":"Unknown"}\n                    }\n                ],\n                "order":[["e1", "before", "e2"]]\n                }\n                \n                        ', 'event_detection_time': 7.570417581999209}</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
           <t>['Pain', 'Family']</t>
         </is>
       </c>
-      <c r="G5" t="inlineStr">
-        <is>
-          <t>[{'Pain': {'severity': 'mild', 'location': 'back', 'duration': 'Unknown', 'time': 'Unknown', 'caused_by': 'Unknown'}}, {'Family': {'interaction': 'visit', 'relation': 'Unknown', 'time': 'Unknown', 'caused_by': 'Unknown'}}]</t>
-        </is>
-      </c>
       <c r="H5" t="inlineStr">
         <is>
+          <t>[{'Pain': {'severity': 'mild', 'location': 'back', 'duration': 'Unknown', 'negation': 'false', 'time': 'Unknown', 'caused_by': 'Unknown'}}, {'Family': {'interaction': 'visit', 'relation': 'Unknown', 'negation': 'false', 'time': 'Unknown', 'caused_by': 'Unknown'}}]</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
           <t>['patient co of mild back pain', 'seen by ho']</t>
         </is>
       </c>
-      <c r="I5" t="inlineStr">
-        <is>
-          <t>{'text': '7 pm  bp to 80,ci &gt; 2 on less milrinone,wedge 16 .patient co of mild back pain .seen by ho.fluid bollus ordered.stat hct,chem 6 sent\n', 'event': ['Pain', 'Family'], 'phrase': '', 'raw_output': '{\n  "events": [\n    {\n      "event_type": "Pain",\n      "text_quote": "patient co of mild back pain",\n      "attributes": {\n        "severity": "mild",\n        "location": "back",\n        "duration": "Unknown",\n        "negation": false,\n        "time": "Unknown",\n        "caused_by": "Unknown"\n      }\n    },\n    {\n      "event_type": "Family",\n      "text_quote": "seen by ho",\n      "attributes": {\n        "interaction": "visit",\n        "relation": "Unknown",\n        "negation": false,\n        "time": "Unknown",\n        "caused_by": "Unknown"\n      }\n    }\n  ]\n}', 'attributes': [{'Pain': {'severity': 'mild', 'location': 'back', 'duration': 'Unknown', 'negation': False, 'time': 'Unknown', 'caused_by': 'Unknown'}}, {'Family': {'interaction': 'visit', 'relation': 'Unknown', 'negation': False, 'time': 'Unknown', 'caused_by': 'Unknown'}}], 'text_quotes': ['patient co of mild back pain', 'seen by ho'], 'event_name_prompt': 'Given the text: 7 pm  bp to 80,ci &gt; 2 on less milrinone,wedge 16 .patient co of mild back pain .seen by ho.fluid bollus ordered.stat hct,chem 6 sent\n, \n                        and the following event types with their definitions: Eating : The patient takes food into their body by mouth.\nExcretion : The patient discharges waste matter from their body.\nFamily : The patient has a visit, call, or communication with a family member.\nPain : The patient reports or shows signs of pain.\nSleep : The patient sleeps or the sleep’s quality or quantity is described.\nUnknown : choose "Unknown" if none of the other event type are applicable. \n                        ---\n                        Your task:\n                        0. Identify ALL events in the text (zero, one, or more).\n1. For each event, assign an event_type from the list above.\n2. If multiple event of same type is mentioned, assign the event_type multiple times\n3. Extract attributes for each event using ONLY the allowed attributes listed below.\n4. Use keyword evidence (Ki) ONLY if it is consistent with the text context.\n5. Output strictly valid JSON following the schema below.\n                        ---\n                        Classification Rules:\n                        - A text may contain multiple events of the same or different types.\n- Create a separate event object for each event mention.\n- If the text is explicitly a NEGATION (e.g., "denies pain"), do not extract that event.\n- If the text describes a FUTURE or HYPOTHETICAL event (e.g., "will eat tomorrow"), ignore it.\n- A valid event should have occurred in the recent past or is occurring during the time of writing of the text.\n- If no events are found or if unsure, return {"events": []}\n                        \n                        ---\n                                    Attributes allowed:\n                                    {\'Eating\': {\'food\': \'&lt;string&gt; # e.g., pancakes, porridge, etc.\', \'amount\': \'&lt;string&gt; # e.g., 1, 2 bowls, etc.\', \'method\': \'&lt;string&gt;  # e.g., oral, tube, etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, after shower, etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}, \'Excretion\': {\'type\': \'&lt;string&gt; # e.g., urine, stool, etc.\', \'frequency\': \'&lt;string&gt; # e.g., 2x, once, etc.\', \'quality\': \'&lt;string&gt; # e.g., loose, hard, etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, after shower, etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}, \'Family\': {\'interaction\': \'&lt;string&gt; # e.g., visit, call, communication, etc.\', \'relation\': \'&lt;string&gt; # e.g., mother, son, etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, after shower, etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}, \'Pain\': {\'severity\': \'&lt;string&gt; # e.g., mild, moderate, severe, numeric scale if present, etc.\', \'location\': \'&lt;string&gt; # e.g., right knee, head, etc.\', \'duration\': \'&lt;string&gt; # e.g., all night, 3 hours, etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, after shower, etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}, \'Sleep\': {\'quality\': \'&lt;string&gt; # e.g., good, poor, restless, etc.\', \'duration\': \'&lt;string&gt; # e.g., 6 hours, phrases like "all night", etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, after shower, etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}}\n                                    If no relevant attribute exists for an event, return an empty object {}.\n                                    \n                        \n                        ---\n                                    Keyword evidence (Ki):\n                                    Additional facts: A keyword matching algorithm without context detected keyword(s) [\'pain\'].\n                                    Use this only as a pointer. If context contradicts, ignore.\n                        ---\n                        Output Schema (strict):\n                        {\n                                    "events": [\n                                        {\n                                        "event_type": "&lt;Pain | Sleep | Excretion | Eating | Family&gt;",\n                                        "text_quote": "&lt;fragement from the text indicating &gt;",\n                "attributes": {\n                    "&lt;attribute_name&gt;": "&lt;attribute_value&gt;"\n                }\n                                        }\n                                    ]\n                                    }\n                        \n                            Rules:\n                                - Ensure the output is valid JSON (parseable).\n                                - "eventS" must always be an array (can be empty).\n                                - Multiple instances of the same event type appear as individual elements in the event array.\n                                - Events appear in the array in the same order in which they appear in the text.\n                                - Do not include extra keys, comments, or text.\n                                - Each object in "events" must contain "event_type", "text_quote", and "attributes".\n                                -If an event attribute type has no value mentioned, return "attributes": {"&lt; attribute name &gt;:Unknown"} for each attribute type defined for the event type \n                        \n                        \n                        \n                        ', 'event_detection_time': 5.772808704001363}</t>
-        </is>
-      </c>
       <c r="J5" t="inlineStr">
         <is>
+          <t>[[]]</t>
+        </is>
+      </c>
+      <c r="K5" t="inlineStr">
+        <is>
+          <t>{'text': '7 pm  bp to 80,ci &gt; 2 on less milrinone,wedge 16 .patient co of mild back pain .seen by ho.fluid bollus ordered.stat hct,chem 6 sent\n', 'event': ['Pain', 'Family'], 'event_id': ['e1', 'e2'], 'phrase': '', 'raw_output': '{\n  "events": [\n    {\n      "event_id": "e1",\n      "event_type": "Pain",\n      "text_quote": "patient co of mild back pain",\n      "attributes": {\n        "severity": "mild",\n        "location": "back",\n        "duration": "Unknown",\n        "negation": false,\n        "time": "Unknown",\n        "caused_by": "Unknown"\n      }\n    },\n    {\n      "event_id": "e2",\n      "event_type": "Family",\n      "text_quote": "seen by ho",\n      "attributes": {\n        "interaction": "visit",\n        "relation": "Unknown",\n        "negation": false,\n        "time": "Unknown",\n        "caused_by": "Unknown"\n      }\n    }\n  ],\n  "order": [\n    ["e1", "before", "e2"]\n  ]\n}', 'attributes': [{'Pain': {'severity': 'mild', 'location': 'back', 'duration': 'Unknown', 'negation': False, 'time': 'Unknown', 'caused_by': 'Unknown'}}, {'Family': {'interaction': 'visit', 'relation': 'Unknown', 'negation': False, 'time': 'Unknown', 'caused_by': 'Unknown'}}], 'orders': [[['e1', 'before', 'e2']]], 'text_quotes': ['patient co of mild back pain', 'seen by ho'], 'event_name_prompt': 'Given the text: 7 pm  bp to 80,ci &gt; 2 on less milrinone,wedge 16 .patient co of mild back pain .seen by ho.fluid bollus ordered.stat hct,chem 6 sent\n, \n                        and the following event types with their definitions: Eating : The patient takes food into their body by mouth.\nExcretion : The patient discharges waste matter from their body.\nFamily : The patient has a visit, call, or communication with a family member.\nPain : The patient reports or shows signs of pain.\nSleep : The patient sleeps or the sleep’s quality or quantity is described.\nUnknown : choose "Unknown" if none of the other event type are applicable. \n                        ---\n                        Your task:\n                        0. Identify ALL events in the text (zero, one, or more).\n1. For each event, assign an event_type from the list above.\n2. If multiple event of same type is mentioned, assign the event_type multiple times\n3. Extract attributes for each event using ONLY the allowed attributes listed below.\n4. Use keyword evidence (Ki) ONLY if it is consistent with the text context.\n5. Output strictly valid JSON following the schema below.\n                        ---\n                        Classification Rules:\n                        - A text may contain multiple events of the same or different types.\n- Create a separate event object for each event mention.\n- If the text is explicitly a NEGATION (e.g., "denies pain"), do not extract that event.\n- If the text describes a FUTURE or HYPOTHETICAL event (e.g., "will eat tomorrow"), ignore it.\n- A valid event should have occurred in the recent past or is occurring during the time of writing of the text.\n- If no events are found or if unsure, return {"events": []}\n                        \n                        ---\n                                    Attributes allowed:\n                                    {\'Eating\': {\'food\': \'&lt;string&gt; # e.g., pancakes, porridge, etc.\', \'amount\': \'&lt;string&gt; # e.g., 1, 2 bowls, etc.\', \'method\': \'&lt;string&gt;  # e.g., oral, tube, etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, evening etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}, \'Excretion\': {\'type\': \'&lt;string&gt; # e.g., urine, stool, etc.\', \'frequency\': \'&lt;string&gt; # e.g., 2x, once, etc.\', \'quality\': \'&lt;string&gt; # e.g., loose, hard, etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, evening etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}, \'Family\': {\'interaction\': \'&lt;string&gt; # e.g., visit, call, communication, etc.\', \'relation\': \'&lt;string&gt; # e.g., mother, son, etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, evening etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}, \'Pain\': {\'severity\': \'&lt;string&gt; # e.g., mild, moderate, severe, numeric scale if present, etc.\', \'location\': \'&lt;string&gt; # e.g., right knee, head, etc.\', \'duration\': \'&lt;string&gt; # e.g., all night, 3 hours, etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, evening etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}, \'Sleep\': {\'quality\': \'&lt;string&gt; # e.g., good, poor, restless, etc.\', \'duration\': \'&lt;string&gt; # e.g., 6 hours, phrases like "all night", etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, evening etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}}\n                                    If no relevant attribute exists for an event, return an empty object {}.\n                                    \n                        \n                        ---\n                                    Keyword evidence (Ki):\n                                    Additional facts: A keyword matching algorithm without context detected keyword(s) (\'pain\',).\n                                    Use this only as a pointer. If context contradicts, ignore.\n                        ---\n                        Output Schema (strict):\n                        {\n                                    "events": [\n                                        {\n                                        "event_id": "&lt; A unique id eg.: e1 | e2 |...&gt;"\n                                        "event_type": "&lt;Pain | Sleep | Excretion | Eating | Family&gt;",\n                                        "text_quote": "&lt;fragement from the text indicating the event_type&gt;",\n                "attributes": {\n                    "&lt;attribute_name&gt;": "&lt;attribute_value&gt;"\n                }\n                                        }\n                                    ],\n                                    "order": [\n                                        ["e1", "before" | "after" | "simultaneous", "e2" ]\n                                    ]\n                                    }\n                        \n                            Rules:\n                                - Ensure the output is valid JSON (parseable).\n                                - "eventS" must always be an array (can be empty).\n                                - Multiple instances of the same event type appear with different ids.\n                                - Events appear in the array in the same order in which they appear in the text.\n                                - Their partial orders can be expressed using the "order" section.\n                                - Do not include extra keys, comments, or text.\n                                - Each object in "events" must contain "event_type", "text_quote", and "attributes".\n                                - If an event attribute type has no value mentioned, return "attributes": {"&lt; attribute name &gt;:Unknown"} for each attribute type defined for the event type \n                        \n                        \n                        \n                        ', 'event_detection_time': 6.916339256975334}</t>
+        </is>
+      </c>
+      <c r="L5" t="inlineStr">
+        <is>
           <t>['Pain', 'Family']</t>
         </is>
       </c>
-      <c r="K5" t="inlineStr">
+      <c r="M5" t="inlineStr">
         <is>
           <t>[{'Pain': {'severity': 'mild', 'location': 'back', 'duration': 'Unknown', 'negation': False, 'time': 'Unknown', 'caused_by': 'Unknown'}}, {'Family': {'interaction': 'visit', 'relation': 'Unknown', 'negation': False, 'time': 'Unknown', 'caused_by': 'Unknown'}}]</t>
         </is>
       </c>
-      <c r="L5" t="inlineStr">
+      <c r="N5" t="inlineStr">
         <is>
           <t>['patient co of mild back pain', 'seen by ho']</t>
         </is>
       </c>
-      <c r="M5" t="inlineStr">
-        <is>
-          <t>{'text': '7 pm  bp to 80,ci &gt; 2 on less milrinone,wedge 16 .patient co of mild back pain .seen by ho.fluid bollus ordered.stat hct,chem 6 sent\n', 'event': ['Pain', 'Family'], 'phrase': '', 'raw_output': '{\n  "events": [\n    {\n      "event_type": "Pain",\n      "text_quote": "patient co of mild back pain",\n      "attributes": {\n        "severity": "mild",\n        "location": "back",\n        "duration": "Unknown",\n        "time": "Unknown",\n        "caused_by": "Unknown"\n      }\n    },\n    {\n      "event_type": "Family",\n      "text_quote": "seen by ho",\n      "attributes": {\n        "interaction": "visit",\n        "relation": "Unknown",\n        "negation": "false",\n        "time": "Unknown",\n        "caused_by": "Unknown"\n      }\n    }\n  ]\n}', 'attributes': [{'Pain': {'severity': 'mild', 'location': 'back', 'duration': 'Unknown', 'time': 'Unknown', 'caused_by': 'Unknown'}}, {'Family': {'interaction': 'visit', 'relation': 'Unknown', 'negation': 'false', 'time': 'Unknown', 'caused_by': 'Unknown'}}], 'text_quotes': ['patient co of mild back pain', 'seen by ho'], 'event_name_prompt': 'Given the text: 7 pm  bp to 80,ci &gt; 2 on less milrinone,wedge 16 .patient co of mild back pain .seen by ho.fluid bollus ordered.stat hct,chem 6 sent\n, \n                        and the following event types with their definitions: Eating : The patient takes food into their body by mouth.\nExcretion : The patient discharges waste matter from their body.\nFamily : The patient has a visit, call, or communication with a family member.\nPain : The patient reports or shows signs of pain.\nSleep : The patient sleeps or the sleep’s quality or quantity is described.\nUnknown : choose "Unknown" if none of the other event type are applicable. \n                        ---\n                        Your task:\n                        0. Identify ALL events in the text (zero, one, or more).\n1. For each event, assign an event_type from the list above.\n2. If multiple event of same type is mentioned, assign the event_type multiple times\n3. Extract attributes for each event using ONLY the allowed attributes listed below.\n4. Output strictly valid JSON following the schema below.\n                        ---\n                        Classification Rules:\n                        - A text may contain multiple events of the same or different types.\n- Create a separate event object for each event mention.\n- If the text is explicitly a NEGATION (e.g., "denies pain"), do not extract that event.\n- If the text describes a FUTURE or HYPOTHETICAL event (e.g., "will eat tomorrow"), ignore it.\n- A valid event should have occurred in the recent past or is occurring during the time of writing of the text.\n- If no events are found or if unsure, return {"events": []}\n                        \n                        ---\n                                    Attributes allowed:\n                                    {\'Eating\': {\'food\': \'&lt;string&gt; # e.g., pancakes, porridge, etc.\', \'amount\': \'&lt;string&gt; # e.g., 1, 2 bowls, etc.\', \'method\': \'&lt;string&gt;  # e.g., oral, tube, etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, after shower, etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}, \'Excretion\': {\'type\': \'&lt;string&gt; # e.g., urine, stool, etc.\', \'frequency\': \'&lt;string&gt; # e.g., 2x, once, etc.\', \'quality\': \'&lt;string&gt; # e.g., loose, hard, etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, after shower, etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}, \'Family\': {\'interaction\': \'&lt;string&gt; # e.g., visit, call, communication, etc.\', \'relation\': \'&lt;string&gt; # e.g., mother, son, etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, after shower, etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}, \'Pain\': {\'severity\': \'&lt;string&gt; # e.g., mild, moderate, severe, numeric scale if present, etc.\', \'location\': \'&lt;string&gt; # e.g., right knee, head, etc.\', \'duration\': \'&lt;string&gt; # e.g., all night, 3 hours, etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, after shower, etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}, \'Sleep\': {\'quality\': \'&lt;string&gt; # e.g., good, poor, restless, etc.\', \'duration\': \'&lt;string&gt; # e.g., 6 hours, phrases like "all night", etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, after shower, etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}}\n                                    If no relevant attribute exists for an event, return an empty object {}.\n                                    \n                        \n                        \n                        ---\n                        Output Schema (strict):\n                        {\n                                    "events": [\n                                        {\n                                        "event_type": "&lt;Pain | Sleep | Excretion | Eating | Family&gt;",\n                                        "text_quote": "&lt;fragement from the text indicating &gt;",\n                "attributes": {\n                    "&lt;attribute_name&gt;": "&lt;attribute_value&gt;"\n                }\n                                        }\n                                    ]\n                                    }\n                        \n                            Rules:\n                                - Ensure the output is valid JSON (parseable).\n                                - "eventS" must always be an array (can be empty).\n                                - Multiple instances of the same event type appear as individual elements in the event array.\n                                - Events appear in the array in the same order in which they appear in the text.\n                                - Do not include extra keys, comments, or text.\n                                - Each object in "events" must contain "event_type", "text_quote", and "attributes".\n                                -If an event attribute type has no value mentioned, return "attributes": {"&lt; attribute name &gt;:Unknown"} for each attribute type defined for the event type \n                        \n                        \n                        \n                ---\n                Examples:\n                \n                text: "Patient ate breakfast this morning. He seems less anxious."\n                output: {\n                "events": [\n                    {\n                    "event_type": "Eating",\n                    "text_quote":"Patient ate breakfast this morning",\n                    "attributes": {"food": "breakfast", \n                                   "amount": "Unknown",\n                                   "method": "Unknown",\n                                   "time":"morning",\n                                   "caused_by":"Unknown"}\n                    }\n                ]\n                }\n                \n                text: "Patient reported severe abdominal pain."\n                output: {\n                "events": [\n                    {\n                    "event_type": "Pain",\n                    "text_quote": "severe abdominal Pain",\n                    "attributes": {"severity": "severe", \n                                   "location": "abdominal",\n                                   "duration": "Unknown",\n                                   "time":"Unknown",\n                                   "caused_by":"Unknown"}\n                    }\n                ]\n                }\n                \n                text: "Patient called his son around 3 pm."\n                output: {\n                "events": [\n                    {\n                    "event_type": "Family",\n                    "text_quote": "called his son around 3 pm",\n                    "attributes": {"interaction": "call", \n                                    "relation": "son",\n                                    "time":"3 pm",\n                                    "caused_by":"Unknown"}\n                    }\n                ]\n                }\n                \n                text: "Patient had a loose stool overnight."\n                output: {\n                "events": [\n                    {\n                    "event_type": "Excretion",\n                    "text_quote": "loose stool overnight",\n                    "attributes": {"type": "stool", \n                                   "quality": "loose", \n                                   "frequency":"overnight", \n                                   "time":"night",\n                                   "caused_by":"Unknown"}\n                    }\n                ]\n                }\n                \n                text: "Patient was able to sleep well last night."\n                output: {\n                "events": [\n                    {\n                    "event_type": "Sleep",\n                    "text_quote": "sleep well last night",\n                    "attributes": {"quality": "well",\n                                    "duration": "Unknown", \n                                    "time":"night",\n                                    "caused_by":"Unknown"}\n                    }\n                ]\n                }\n                \n                text: "The patient couldn\'t sleep due to severe pain."\n                output: {\n                "events": [\n                    {\n                    "event_type": "Sleep",\n                    "text_quote": "couldn\'t sleep",\n                    "attributes": {"quality": "poor", \n                                    "duration": "Unknown",\n                                   "time":"Unknown",\n                                   "caused_by":"Pain"}\n                    },\n                    {\n                    "event_type": "Pain",\n                    "text_quote": "severe pain",\n                    "attributes": {"severity": "severe", \n                                    "location": "Unknown", \n                                    "duration": "Unknown", \n                                   "time":"before Sleep",\n                                   "caused_by":"Unknown"}\n                    }\n                ]\n                }\n                \n                text: "The patient complained of severe back pain, was given Tylenol, but the pain persisted and he was then prescribed stronger morphine."\n                output: {\n                "events": [\n                    {\n                    "event_type": "Pain",\n                    "text_quote": "complained of severe back pain",\n                    "attributes": {"severity": "severe", \n                                    "location": "back",\n                                    "duration": "Unknown", \n                                    "time":"Unknown",\n                                    "caused_by":"Unknown"}\n                    },\n                    {\n                    "event_type": "Pain",\n                    "text_quote": "pain persisted",\n                    "attributes": {"severity": "severe", \n                                   "location": "back",\n                                   "duration": "persistent", \n                                   "time":"after Tylenol",\n                                   "caused_by":"Unknown"}\n                    }\n                ]\n                }\n                \n                        ', 'event_detection_time': 6.2967024270037655}</t>
-        </is>
-      </c>
-      <c r="N5" t="inlineStr">
-        <is>
-          <t>['Pain', 'Family']</t>
-        </is>
-      </c>
       <c r="O5" t="inlineStr">
         <is>
-          <t>[{'Pain': {'severity': 'mild', 'location': 'back', 'duration': 'Unknown', 'time': 'Unknown', 'caused_by': 'Unknown'}}, {'Family': {'interaction': 'visit', 'relation': 'Unknown', 'negation': 'false', 'time': 'Unknown', 'caused_by': 'Unknown'}}]</t>
-        </is>
-      </c>
-      <c r="P5" t="inlineStr">
-        <is>
-          <t>['patient co of mild back pain', 'seen by ho']</t>
-        </is>
-      </c>
-      <c r="Q5" t="n">
-        <v>0.003013232000739663</v>
-      </c>
-      <c r="R5" t="inlineStr">
+          <t>[[['e1', 'before', 'e2']]]</t>
+        </is>
+      </c>
+      <c r="P5" t="n">
+        <v>0.002344322998396819</v>
+      </c>
+      <c r="Q5" t="inlineStr">
         <is>
           <t>Sleep</t>
         </is>
       </c>
-      <c r="S5" t="b">
+      <c r="R5" t="b">
+        <v>0</v>
+      </c>
+      <c r="S5" t="n">
         <v>0</v>
       </c>
       <c r="T5" t="n">
         <v>0</v>
       </c>
-      <c r="U5" t="n">
-        <v>0</v>
-      </c>
-      <c r="V5" t="inlineStr">
+      <c r="U5" t="inlineStr">
         <is>
           <t>('pain',)</t>
         </is>
       </c>
+      <c r="V5" t="n">
+        <v>7.570417581999209</v>
+      </c>
       <c r="W5" t="n">
-        <v>6.121830725009204</v>
+        <v>6.916339256975334</v>
       </c>
       <c r="X5" t="n">
-        <v>5.772808704001363</v>
+        <v>0</v>
       </c>
       <c r="Y5" t="n">
-        <v>6.296702427003765</v>
+        <v>0</v>
       </c>
       <c r="Z5" t="n">
-        <v>0</v>
-      </c>
-      <c r="AA5" t="n">
-        <v>0</v>
-      </c>
-      <c r="AB5" t="n">
-        <v>0</v>
-      </c>
-      <c r="AC5" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" t="n">
-        <v>1310482</v>
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>1310482</t>
+        </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>['Sleep', 'Pain', 'Family', 'Unknown']</t>
+          <t>('Pain', 'Sleep', 'Family', 'Unknown')</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>['asleep', 'distress', 'son', 'pain']</t>
+          <t>('pain', 'distress', 'son', 'asleep')</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
@@ -1164,120 +1117,111 @@
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>{'text': 'ccu nsg progress note 7p-7a/ status post aortic dissection\n\ns- " i don\'t remember doing that"?\n\no- see flowsheet for objective data\n\n[**name (ni) 231**] patient [**name (ni) 591**] hypotensive slightly - 90/40- dipping to low 80\'s asleep systolically- given 500cc ivf normal saline bolus, increased milrinone to 0.375 mcg and decreased per schedule amiodorone to 0.5mg. no significant improvement in bp and by 9:30- decided to add back small amount neo drops- 0.2 mcg/kg.\ndenies worse back pain, serial hct wnl, no evidence of worsening disection.\npa # wnl- pa- 33/17-18 ; cvp- 14-17, pcw- 16-18.\npatient found to have self d/c pa line and introducer from rt ij- bleeding small amount-\nheld pressure- no evidence of pneumo/ho called and came to examine.\nwith commotion of pa line d/c- bp up to 130/.\nd/c neo drops as of 2am and remains off drops.\n\n[**name (ni) 62**] patient on 6l np- resp rate- mid 20\'s, lungs clear- appears comfortable in no distress.\n\nid- temp flat- no fever\n\ngu-20cc/hour via foley catheter- am creat to be checked- atn\n\n[**name (ni) 232**] patient taking meds/lix without issue\n(+) bowel sounds, no stool.\n\n[**name (ni) 324**] patient alert and oriented- when awakened in middle of nite with pa line self d/[**name (ni) **] patient slightly disoriented , but easily reoriented to\ntime/place.\nson and wife in evening to visit.\nall aware of plan of care.\n\na/[**name (ni) **] patient status post aortic dissection- currently stable on milrinone drops 0.375\n- transiently requiring neo drops for low normal bp\n\ncontinue milrinone as ordered, am labs- replete lytes as needed.\nserial hct\'s check to make sure no sign of acute expansion in disection- assess back pain/level etc.\nkeep patient safe, and continue to closely assess mental status.\nif bp continues to stay above 120-130\'s, discuss with team ? addition again of some esmolol type [**doctor last name 528**] to control rate pressure product\nkeep patient aware of plan of care.\n', 'event': ['Sleep', 'Family', 'Excretion', 'Pain', 'Sleep'], 'phrase': '', 'raw_output': '{\n  "events": [\n    {\n      "event_type": "Sleep",\n      "text_quote": "asleep systolically-",\n      "attributes": {\n        "quality": "Unknown",\n        "duration": "Unknown",\n        "time": "night",\n        "caused_by": "Unknown"\n      }\n    },\n    {\n      "event_type": "Family",\n      "text_quote": "son and wife in evening to visit.",\n      "attributes": {\n        "interaction": "visit",\n        "relation": "son, wife",\n        "time": "evening",\n        "caused_by": "Unknown"\n      }\n    },\n    {\n      "event_type": "Excretion",\n      "text_quote": "gu-20cc/hour via foley catheter",\n      "attributes": {\n        "type": "urine",\n        "frequency": "20cc/hour",\n        "quality": "Unknown",\n        "time": "Unknown",\n        "caused_by": "Unknown"\n      }\n    },\n    {\n      "event_type": "Pain",\n      "text_quote": "denies worse back pain",\n      "attributes": {\n        "severity": "Unknown",\n        "location": "back",\n        "duration": "Unknown",\n        "time": "Unknown",\n        "caused_by": "Unknown"\n      }\n    },\n    {\n      "event_type": "Sleep",\n      "text_quote": "bp up to 130/.",\n      "attributes": {\n        "quality": "Unknown",\n        "duration": "Unknown",\n        "time": "night",\n        "caused_by": "Unknown"\n      }\n    }\n  ]\n}', 'attributes': [{'Sleep': {'quality': 'Unknown', 'duration': 'Unknown', 'time': 'night', 'caused_by': 'Unknown'}}, {'Family': {'interaction': 'visit', 'relation': 'son, wife', 'time': 'evening', 'caused_by': 'Unknown'}}, {'Excretion': {'type': 'urine', 'frequency': '20cc/hour', 'quality': 'Unknown', 'time': 'Unknown', 'caused_by': 'Unknown'}}, {'Pain': {'severity': 'Unknown', 'location': 'back', 'duration': 'Unknown', 'time': 'Unknown', 'caused_by': 'Unknown'}}, {'Sleep': {'quality': 'Unknown', 'duration': 'Unknown', 'time': 'night', 'caused_by': 'Unknown'}}], 'text_quotes': ['asleep systolically-', 'son and wife in evening to visit.', 'gu-20cc/hour via foley catheter', 'denies worse back pain', 'bp up to 130/.'], 'event_name_prompt': 'Given the text: ccu nsg progress note 7p-7a/ status post aortic dissection\n\ns- " i don\'t remember doing that"?\n\no- see flowsheet for objective data\n\n[**name (ni) 231**] patient [**name (ni) 591**] hypotensive slightly - 90/40- dipping to low 80\'s asleep systolically- given 500cc ivf normal saline bolus, increased milrinone to 0.375 mcg and decreased per schedule amiodorone to 0.5mg. no significant improvement in bp and by 9:30- decided to add back small amount neo drops- 0.2 mcg/kg.\ndenies worse back pain, serial hct wnl, no evidence of worsening disection.\npa # wnl- pa- 33/17-18 ; cvp- 14-17, pcw- 16-18.\npatient found to have self d/c pa line and introducer from rt ij- bleeding small amount-\nheld pressure- no evidence of pneumo/ho called and came to examine.\nwith commotion of pa line d/c- bp up to 130/.\nd/c neo drops as of 2am and remains off drops.\n\n[**name (ni) 62**] patient on 6l np- resp rate- mid 20\'s, lungs clear- appears comfortable in no distress.\n\nid- temp flat- no fever\n\ngu-20cc/hour via foley catheter- am creat to be checked- atn\n\n[**name (ni) 232**] patient taking meds/lix without issue\n(+) bowel sounds, no stool.\n\n[**name (ni) 324**] patient alert and oriented- when awakened in middle of nite with pa line self d/[**name (ni) **] patient slightly disoriented , but easily reoriented to\ntime/place.\nson and wife in evening to visit.\nall aware of plan of care.\n\na/[**name (ni) **] patient status post aortic dissection- currently stable on milrinone drops 0.375\n- transiently requiring neo drops for low normal bp\n\ncontinue milrinone as ordered, am labs- replete lytes as needed.\nserial hct\'s check to make sure no sign of acute expansion in disection- assess back pain/level etc.\nkeep patient safe, and continue to closely assess mental status.\nif bp continues to stay above 120-130\'s, discuss with team ? addition again of some esmolol type [**doctor last name 528**] to control rate pressure product\nkeep patient aware of plan of care.\n, \n                        and the following event types with their definitions: Eating : The patient takes food into their body by mouth.\nExcretion : The patient discharges waste matter from their body.\nFamily : The patient has a visit, call, or communication with a family member.\nPain : The patient reports or shows signs of pain.\nSleep : The patient sleeps or the sleep’s quality or quantity is described.\nUnknown : choose "Unknown" if none of the other event type are applicable. \n                        ---\n                        Your task:\n                        0. Identify ALL events in the text (zero, one, or more).\n1. For each event, assign an event_type from the list above.\n2. If multiple event of same type is mentioned, assign the event_type multiple times\n3. Extract attributes for each event using ONLY the allowed attributes listed below.\n4. Use keyword evidence (Ki) ONLY if it is consistent with the text context.\n5. Output strictly valid JSON following the schema below.\n                        ---\n                        Classification Rules:\n                        - A text may contain multiple events of the same or different types.\n- Create a separate event object for each event mention.\n- If the text is explicitly a NEGATION (e.g., "denies pain"), do not extract that event.\n- If the text describes a FUTURE or HYPOTHETICAL event (e.g., "will eat tomorrow"), ignore it.\n- A valid event should have occurred in the recent past or is occurring during the time of writing of the text.\n- If no events are found or if unsure, return {"events": []}\n                        \n                        ---\n                                    Attributes allowed:\n                                    {\'Eating\': {\'food\': \'&lt;string&gt; # e.g., pancakes, porridge, etc.\', \'amount\': \'&lt;string&gt; # e.g., 1, 2 bowls, etc.\', \'method\': \'&lt;string&gt;  # e.g., oral, tube, etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, after shower, etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}, \'Excretion\': {\'type\': \'&lt;string&gt; # e.g., urine, stool, etc.\', \'frequency\': \'&lt;string&gt; # e.g., 2x, once, etc.\', \'quality\': \'&lt;string&gt; # e.g., loose, hard, etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, after shower, etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}, \'Family\': {\'interaction\': \'&lt;string&gt; # e.g., visit, call, communication, etc.\', \'relation\': \'&lt;string&gt; # e.g., mother, son, etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, after shower, etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}, \'Pain\': {\'severity\': \'&lt;string&gt; # e.g., mild, moderate, severe, numeric scale if present, etc.\', \'location\': \'&lt;string&gt; # e.g., right knee, head, etc.\', \'duration\': \'&lt;string&gt; # e.g., all night, 3 hours, etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, after shower, etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}, \'Sleep\': {\'quality\': \'&lt;string&gt; # e.g., good, poor, restless, etc.\', \'duration\': \'&lt;string&gt; # e.g., 6 hours, phrases like "all night", etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, after shower, etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}}\n                                    If no relevant attribute exists for an event, return an empty object {}.\n                                    \n                        \n                        ---\n                                    Keyword evidence (Ki):\n                                    Additional facts: A keyword matching algorithm without context detected keyword(s) [\'asleep\', \'distress\', \'son\', \'pain\'].\n                                    Use this only as a pointer. If context contradicts, ignore.\n                        ---\n                        Output Schema (strict):\n                        {\n                                    "events": [\n                                        {\n                                        "event_type": "&lt;Pain | Sleep | Excretion | Eating | Family&gt;",\n                                        "text_quote": "&lt;fragement from the text indicating &gt;",\n                "attributes": {\n                    "&lt;attribute_name&gt;": "&lt;attribute_value&gt;"\n                }\n                                        }\n                                    ]\n                                    }\n                        \n                            Rules:\n                                - Ensure the output is valid JSON (parseable).\n                                - "eventS" must always be an array (can be empty).\n                                - Multiple instances of the same event type appear as individual elements in the event array.\n                                - Events appear in the array in the same order in which they appear in the text.\n                                - Do not include extra keys, comments, or text.\n                                - Each object in "events" must contain "event_type", "text_quote", and "attributes".\n                                -If an event attribute type has no value mentioned, return "attributes": {"&lt; attribute name &gt;:Unknown"} for each attribute type defined for the event type \n                        \n                        \n                        \n                ---\n                Examples:\n                \n                text: "Patient ate breakfast this morning. He seems less anxious."\n                output: {\n                "events": [\n                    {\n                    "event_type": "Eating",\n                    "text_quote":"Patient ate breakfast this morning",\n                    "attributes": {"food": "breakfast", \n                                   "amount": "Unknown",\n                                   "method": "Unknown",\n                                   "time":"morning",\n                                   "caused_by":"Unknown"}\n                    }\n                ]\n                }\n                \n                text: "Patient reported severe abdominal pain."\n                output: {\n                "events": [\n                    {\n                    "event_type": "Pain",\n                    "text_quote": "severe abdominal Pain",\n                    "attributes": {"severity": "severe", \n                                   "location": "abdominal",\n                                   "duration": "Unknown",\n                                   "time":"Unknown",\n                                   "caused_by":"Unknown"}\n                    }\n                ]\n                }\n                \n                text: "Patient called his son around 3 pm."\n                output: {\n                "events": [\n                    {\n                    "event_type": "Family",\n                    "text_quote": "called his son around 3 pm",\n                    "attributes": {"interaction": "call", \n                                    "relation": "son",\n                                    "time":"3 pm",\n                                    "caused_by":"Unknown"}\n                    }\n                ]\n                }\n                \n                text: "Patient had a loose stool overnight."\n                output: {\n                "events": [\n                    {\n                    "event_type": "Excretion",\n                    "text_quote": "loose stool overnight",\n                    "attributes": {"type": "stool", \n                                   "quality": "loose", \n                                   "frequency":"overnight", \n                                   "time":"night",\n                                   "caused_by":"Unknown"}\n                    }\n                ]\n                }\n                \n                text: "Patient was able to sleep well last night."\n                output: {\n                "events": [\n                    {\n                    "event_type": "Sleep",\n                    "text_quote": "sleep well last night",\n                    "attributes": {"quality": "well",\n                                    "duration": "Unknown", \n                                    "time":"night",\n                                    "caused_by":"Unknown"}\n                    }\n                ]\n                }\n                \n                text: "The patient couldn\'t sleep due to severe pain."\n                output: {\n                "events": [\n                    {\n                    "event_type": "Sleep",\n                    "text_quote": "couldn\'t sleep",\n                    "attributes": {"quality": "poor", \n                                    "duration": "Unknown",\n                                   "time":"Unknown",\n                                   "caused_by":"Pain"}\n                    },\n                    {\n                    "event_type": "Pain",\n                    "text_quote": "severe pain",\n                    "attributes": {"severity": "severe", \n                                    "location": "Unknown", \n                                    "duration": "Unknown", \n                                   "time":"before Sleep",\n                                   "caused_by":"Unknown"}\n                    }\n                ]\n                }\n                \n                text: "The patient complained of severe back pain, was given Tylenol, but the pain persisted and he was then prescribed stronger morphine."\n                output: {\n                "events": [\n                    {\n                    "event_type": "Pain",\n                    "text_quote": "complained of severe back pain",\n                    "attributes": {"severity": "severe", \n                                    "location": "back",\n                                    "duration": "Unknown", \n                                    "time":"Unknown",\n                                    "caused_by":"Unknown"}\n                    },\n                    {\n                    "event_type": "Pain",\n                    "text_quote": "pain persisted",\n                    "attributes": {"severity": "severe", \n                                   "location": "back",\n                                   "duration": "persistent", \n                                   "time":"after Tylenol",\n                                   "caused_by":"Unknown"}\n                    }\n                ]\n                }\n                \n                        ', 'event_detection_time': 12.947839500993723}</t>
+          <t>['pain', 'distress', 'son', 'asleep']</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>['Sleep', 'Family', 'Excretion', 'Pain', 'Sleep']</t>
+          <t>{'text': 'ccu nsg progress note 7p-7a/ status post aortic dissection\n\ns- " i don\'t remember doing that"?\n\no- see flowsheet for objective data\n\n[**name (ni) 231**] patient [**name (ni) 591**] hypotensive slightly - 90/40- dipping to low 80\'s asleep systolically- given 500cc ivf normal saline bolus, increased milrinone to 0.375 mcg and decreased per schedule amiodorone to 0.5mg. no significant improvement in bp and by 9:30- decided to add back small amount neo drops- 0.2 mcg/kg.\ndenies worse back pain, serial hct wnl, no evidence of worsening disection.\npa # wnl- pa- 33/17-18 ; cvp- 14-17, pcw- 16-18.\npatient found to have self d/c pa line and introducer from rt ij- bleeding small amount-\nheld pressure- no evidence of pneumo/ho called and came to examine.\nwith commotion of pa line d/c- bp up to 130/.\nd/c neo drops as of 2am and remains off drops.\n\n[**name (ni) 62**] patient on 6l np- resp rate- mid 20\'s, lungs clear- appears comfortable in no distress.\n\nid- temp flat- no fever\n\ngu-20cc/hour via foley catheter- am creat to be checked- atn\n\n[**name (ni) 232**] patient taking meds/lix without issue\n(+) bowel sounds, no stool.\n\n[**name (ni) 324**] patient alert and oriented- when awakened in middle of nite with pa line self d/[**name (ni) **] patient slightly disoriented , but easily reoriented to\ntime/place.\nson and wife in evening to visit.\nall aware of plan of care.\n\na/[**name (ni) **] patient status post aortic dissection- currently stable on milrinone drops 0.375\n- transiently requiring neo drops for low normal bp\n\ncontinue milrinone as ordered, am labs- replete lytes as needed.\nserial hct\'s check to make sure no sign of acute expansion in disection- assess back pain/level etc.\nkeep patient safe, and continue to closely assess mental status.\nif bp continues to stay above 120-130\'s, discuss with team ? addition again of some esmolol type [**doctor last name 528**] to control rate pressure product\nkeep patient aware of plan of care.\n', 'event': ['Sleep', 'Pain', 'Excretion', 'Family', 'Sleep'], 'event_id': ['e1', 'e2', 'e3', 'e4', 'e5'], 'phrase': '', 'raw_output': '{\n  "events": [\n    {\n      "event_id": "e1",\n      "event_type": "Sleep",\n      "text_quote": "asleep systolically-",\n      "attributes": {\n        "quality": "Unknown",\n        "duration": "Unknown",\n        "negation": "false",\n        "time": "night",\n        "caused_by": "Unknown"\n      }\n    },\n    {\n      "event_id": "e2",\n      "event_type": "Pain",\n      "text_quote": "denies worse back pain",\n      "attributes": {\n        "severity": "Unknown",\n        "location": "back",\n        "duration": "Unknown",\n        "negation": "true",\n        "time": "Unknown",\n        "caused_by": "Unknown"\n      }\n    },\n    {\n      "event_id": "e3",\n      "event_type": "Excretion",\n      "text_quote": "gu-20cc/hour via foley catheter",\n      "attributes": {\n        "type": "urine",\n        "frequency": "20cc/hour",\n        "quality": "Unknown",\n        "negation": "false",\n        "time": "Unknown",\n        "caused_by": "Unknown"\n      }\n    },\n    {\n      "event_id": "e4",\n      "event_type": "Family",\n      "text_quote": "son and wife in evening to visit",\n      "attributes": {\n        "interaction": "visit",\n        "relation": "son and wife",\n        "negation": "false",\n        "time": "evening",\n        "caused_by": "Unknown"\n      }\n    },\n    {\n      "event_id": "e5",\n      "event_type": "Sleep",\n      "text_quote": "patient slightly disoriented , but easily reoriented to time/place",\n      "attributes": {\n        "quality": "poor",\n        "duration": "Unknown",\n        "negation": "false",\n        "time": "night",\n        "caused_by": "Unknown"\n      }\n    }\n  ],\n  "order": []\n}', 'attributes': [{'Sleep': {'quality': 'Unknown', 'duration': 'Unknown', 'negation': 'false', 'time': 'night', 'caused_by': 'Unknown'}}, {'Pain': {'severity': 'Unknown', 'location': 'back', 'duration': 'Unknown', 'negation': 'true', 'time': 'Unknown', 'caused_by': 'Unknown'}}, {'Excretion': {'type': 'urine', 'frequency': '20cc/hour', 'quality': 'Unknown', 'negation': 'false', 'time': 'Unknown', 'caused_by': 'Unknown'}}, {'Family': {'interaction': 'visit', 'relation': 'son and wife', 'negation': 'false', 'time': 'evening', 'caused_by': 'Unknown'}}, {'Sleep': {'quality': 'poor', 'duration': 'Unknown', 'negation': 'false', 'time': 'night', 'caused_by': 'Unknown'}}], 'orders': [[]], 'text_quotes': ['asleep systolically-', 'denies worse back pain', 'gu-20cc/hour via foley catheter', 'son and wife in evening to visit', 'patient slightly disoriented , but easily reoriented to time/place'], 'event_name_prompt': 'Given the text: ccu nsg progress note 7p-7a/ status post aortic dissection\n\ns- " i don\'t remember doing that"?\n\no- see flowsheet for objective data\n\n[**name (ni) 231**] patient [**name (ni) 591**] hypotensive slightly - 90/40- dipping to low 80\'s asleep systolically- given 500cc ivf normal saline bolus, increased milrinone to 0.375 mcg and decreased per schedule amiodorone to 0.5mg. no significant improvement in bp and by 9:30- decided to add back small amount neo drops- 0.2 mcg/kg.\ndenies worse back pain, serial hct wnl, no evidence of worsening disection.\npa # wnl- pa- 33/17-18 ; cvp- 14-17, pcw- 16-18.\npatient found to have self d/c pa line and introducer from rt ij- bleeding small amount-\nheld pressure- no evidence of pneumo/ho called and came to examine.\nwith commotion of pa line d/c- bp up to 130/.\nd/c neo drops as of 2am and remains off drops.\n\n[**name (ni) 62**] patient on 6l np- resp rate- mid 20\'s, lungs clear- appears comfortable in no distress.\n\nid- temp flat- no fever\n\ngu-20cc/hour via foley catheter- am creat to be checked- atn\n\n[**name (ni) 232**] patient taking meds/lix without issue\n(+) bowel sounds, no stool.\n\n[**name (ni) 324**] patient alert and oriented- when awakened in middle of nite with pa line self d/[**name (ni) **] patient slightly disoriented , but easily reoriented to\ntime/place.\nson and wife in evening to visit.\nall aware of plan of care.\n\na/[**name (ni) **] patient status post aortic dissection- currently stable on milrinone drops 0.375\n- transiently requiring neo drops for low normal bp\n\ncontinue milrinone as ordered, am labs- replete lytes as needed.\nserial hct\'s check to make sure no sign of acute expansion in disection- assess back pain/level etc.\nkeep patient safe, and continue to closely assess mental status.\nif bp continues to stay above 120-130\'s, discuss with team ? addition again of some esmolol type [**doctor last name 528**] to control rate pressure product\nkeep patient aware of plan of care.\n, \n                        and the following event types with their definitions: Eating : The patient takes food into their body by mouth.\nExcretion : The patient discharges waste matter from their body.\nFamily : The patient has a visit, call, or communication with a family member.\nPain : The patient reports or shows signs of pain.\nSleep : The patient sleeps or the sleep’s quality or quantity is described.\nUnknown : choose "Unknown" if none of the other event type are applicable. \n                        ---\n                        Your task:\n                        0. Identify ALL events in the text (zero, one, or more).\n1. For each event, assign an event_type from the list above.\n2. If multiple event of same type is mentioned, assign the event_type multiple times\n3. Extract attributes for each event using ONLY the allowed attributes listed below.\n4. Use keyword evidence (Ki) ONLY if it is consistent with the text context.\n5. Output strictly valid JSON following the schema below.\n                        ---\n                        Classification Rules:\n                        - A text may contain multiple events of the same or different types.\n- Create a separate event object for each event mention.\n- If the text is explicitly a NEGATION (e.g., "denies pain"), do not extract that event.\n- If the text describes a FUTURE or HYPOTHETICAL event (e.g., "will eat tomorrow"), ignore it.\n- A valid event should have occurred in the recent past or is occurring during the time of writing of the text.\n- If no events are found or if unsure, return {"events": []}\n                        \n                        ---\n                                    Attributes allowed:\n                                    {\'Eating\': {\'food\': \'&lt;string&gt; # e.g., pancakes, porridge, etc.\', \'amount\': \'&lt;string&gt; # e.g., 1, 2 bowls, etc.\', \'method\': \'&lt;string&gt;  # e.g., oral, tube, etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, evening etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}, \'Excretion\': {\'type\': \'&lt;string&gt; # e.g., urine, stool, etc.\', \'frequency\': \'&lt;string&gt; # e.g., 2x, once, etc.\', \'quality\': \'&lt;string&gt; # e.g., loose, hard, etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, evening etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}, \'Family\': {\'interaction\': \'&lt;string&gt; # e.g., visit, call, communication, etc.\', \'relation\': \'&lt;string&gt; # e.g., mother, son, etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, evening etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}, \'Pain\': {\'severity\': \'&lt;string&gt; # e.g., mild, moderate, severe, numeric scale if present, etc.\', \'location\': \'&lt;string&gt; # e.g., right knee, head, etc.\', \'duration\': \'&lt;string&gt; # e.g., all night, 3 hours, etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, evening etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}, \'Sleep\': {\'quality\': \'&lt;string&gt; # e.g., good, poor, restless, etc.\', \'duration\': \'&lt;string&gt; # e.g., 6 hours, phrases like "all night", etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, evening etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}}\n                                    If no relevant attribute exists for an event, return an empty object {}.\n                                    \n                        \n                        ---\n                                    Keyword evidence (Ki):\n                                    Additional facts: A keyword matching algorithm without context detected keyword(s) (\'pain\', \'distress\', \'son\', \'asleep\').\n                                    Use this only as a pointer. If context contradicts, ignore.\n                        ---\n                        Output Schema (strict):\n                        {\n                                    "events": [\n                                        {\n                                        "event_id": "&lt; A unique id eg.: e1 | e2 |...&gt;"\n                                        "event_type": "&lt;Pain | Sleep | Excretion | Eating | Family&gt;",\n                                        "text_quote": "&lt;fragement from the text indicating the event_type&gt;",\n                "attributes": {\n                    "&lt;attribute_name&gt;": "&lt;attribute_value&gt;"\n                }\n                                        }\n                                    ],\n                                    "order": [\n                                        ["e1", "before" | "after" | "simultaneous", "e2" ]\n                                    ]\n                                    }\n                        \n                            Rules:\n                                - Ensure the output is valid JSON (parseable).\n                                - "eventS" must always be an array (can be empty).\n                                - Multiple instances of the same event type appear with different ids.\n                                - Events appear in the array in the same order in which they appear in the text.\n                                - Their partial orders can be expressed using the "order" section.\n                                - Do not include extra keys, comments, or text.\n                                - Each object in "events" must contain "event_type", "text_quote", and "attributes".\n                                - If an event attribute type has no value mentioned, return "attributes": {"&lt; attribute name &gt;:Unknown"} for each attribute type defined for the event type \n                        \n                        \n                        \n                ---\n                Examples:\n                \n                text: "Patient ate breakfast this morning. He seems less anxious."\n                output: {\n                "events": [\n                    {"event_id": "e1",\n                    "event_type": "Eating",\n                    "text_quote":"Patient ate breakfast this morning",\n                    "attributes": {"food": "breakfast", \n                                   "amount": "Unknown",\n                                   "method": "Unknown",\n                                   "negation": "false",\n                                   "time":"morning",\n                                   "caused_by":"Unknown"}\n                    }\n                ],\n                "order":[]\n                }\n                \n                text: "Patient reported severe abdominal pain."\n                output: {\n                "events": [\n                    {"event_id": "e1",\n                    "event_type": "Pain",\n                    "text_quote": "severe abdominal Pain",\n                    "attributes": {"severity": "severe", \n                                   "location": "abdominal",\n                                   "duration": "Unknown",\n                                   "negation": "false",\n                                   "time":"Unknown",\n                                   "caused_by":"Unknown"}\n                    }\n                ],\n                "order":[]\n                }\n                \n                text: "Patient called his son around 3 pm."\n                output: {\n                "events": [\n                    {"event_id": "e1",\n                    "event_type": "Family",\n                    "text_quote": "called his son around 3 pm",\n                    "attributes": {"interaction": "call", \n                                    "relation": "son",\n                                    "negation": "false",\n                                    "time":"3 pm",\n                                    "caused_by":"Unknown"}\n                    }\n                ],\n                "order":[]\n                }\n                \n                text: "Patient had a loose stool overnight."\n                output: {\n                "events": [\n                    {"event_id": "e1",\n                    "event_type": "Excretion",\n                    "text_quote": "loose stool overnight",\n                    "attributes": {"type": "stool", \n                                   "quality": "loose", \n                                   "frequency":"overnight", \n                                   "negation": "false",\n                                   "time":"night",\n                                   "caused_by":"Unknown"}\n                    }\n                ],\n                "order":[]\n                }\n                \n                text: "Patient was able to sleep well last night."\n                output: {\n                "events": [\n                    {"event_id": "e1",\n                    "event_type": "Sleep",\n                    "text_quote": "sleep well last night",\n                    "attributes": {"quality": "well",\n                                    "duration": "Unknown", \n                                    "negation": "false",\n                                    "time":"night",\n                                    "caused_by":"Unknown"}\n                    }\n                ],\n                "order":[]\n                }\n                \n                text: "The patient couldn\'t sleep due to severe pain."\n                output: {\n                "events": [\n                    {"event_id": "e1",\n                    "event_type": "Sleep",\n                    "text_quote": "couldn\'t sleep",\n                    "attributes": {"quality": "poor", \n                                    "duration": "Unknown",\n                                    "negation": "true",\n                                    "time":"Unknown",\n                                    "caused_by":"Pain"}\n                    },\n                    {"event_id": "e2",\n                    "event_type": "Pain",\n                    "text_quote": "severe pain",\n                    "attributes": {"severity": "severe", \n                                    "location": "Unknown", \n                                    "duration": "Unknown", \n                                    "time":"Unknown",\n                                    "caused_by":"Unknown"}\n                    }\n                ],\n                "order":["e1", "after", "e2"]\n                }\n                \n                text: "The patient complained of severe back pain, was given Tylenol, but the pain persisted and he was then prescribed stronger morphine."\n                output: {\n                "events": [\n                    {"event_id": "e1",\n                    "event_type": "Pain",\n                    "text_quote": "complained of severe back pain",\n                    "attributes": {"severity": "severe", \n                                    "location": "back",\n                                    "duration": "Unknown", \n                                    "time":"Unknown",\n                                    "caused_by":"Unknown"}\n                    },\n                    {"event_id": "e2",\n                    "event_type": "Pain",\n                    "text_quote": "pain persisted",\n                    "attributes": {"severity": "severe", \n                                   "location": "back",\n                                   "duration": "persistent", \n                                   "time":"after Tylenol",\n                                   "caused_by":"Unknown"}\n                    }\n                ],\n                "order":[["e1", "before", "e2"]]\n                }\n                \n                        ', 'event_detection_time': 16.169218705035746}</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>[{'Sleep': {'quality': 'Unknown', 'duration': 'Unknown', 'time': 'night', 'caused_by': 'Unknown'}}, {'Family': {'interaction': 'visit', 'relation': 'son, wife', 'time': 'evening', 'caused_by': 'Unknown'}}, {'Excretion': {'type': 'urine', 'frequency': '20cc/hour', 'quality': 'Unknown', 'time': 'Unknown', 'caused_by': 'Unknown'}}, {'Pain': {'severity': 'Unknown', 'location': 'back', 'duration': 'Unknown', 'time': 'Unknown', 'caused_by': 'Unknown'}}, {'Sleep': {'quality': 'Unknown', 'duration': 'Unknown', 'time': 'night', 'caused_by': 'Unknown'}}]</t>
+          <t>['Sleep', 'Pain', 'Excretion', 'Family', 'Sleep']</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>['asleep systolically-', 'son and wife in evening to visit.', 'gu-20cc/hour via foley catheter', 'denies worse back pain', 'bp up to 130/.']</t>
+          <t>[{'Sleep': {'quality': 'Unknown', 'duration': 'Unknown', 'negation': 'false', 'time': 'night', 'caused_by': 'Unknown'}}, {'Pain': {'severity': 'Unknown', 'location': 'back', 'duration': 'Unknown', 'negation': 'true', 'time': 'Unknown', 'caused_by': 'Unknown'}}, {'Excretion': {'type': 'urine', 'frequency': '20cc/hour', 'quality': 'Unknown', 'negation': 'false', 'time': 'Unknown', 'caused_by': 'Unknown'}}, {'Family': {'interaction': 'visit', 'relation': 'son and wife', 'negation': 'false', 'time': 'evening', 'caused_by': 'Unknown'}}, {'Sleep': {'quality': 'poor', 'duration': 'Unknown', 'negation': 'false', 'time': 'night', 'caused_by': 'Unknown'}}]</t>
         </is>
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>{'text': 'ccu nsg progress note 7p-7a/ status post aortic dissection\n\ns- " i don\'t remember doing that"?\n\no- see flowsheet for objective data\n\n[**name (ni) 231**] patient [**name (ni) 591**] hypotensive slightly - 90/40- dipping to low 80\'s asleep systolically- given 500cc ivf normal saline bolus, increased milrinone to 0.375 mcg and decreased per schedule amiodorone to 0.5mg. no significant improvement in bp and by 9:30- decided to add back small amount neo drops- 0.2 mcg/kg.\ndenies worse back pain, serial hct wnl, no evidence of worsening disection.\npa # wnl- pa- 33/17-18 ; cvp- 14-17, pcw- 16-18.\npatient found to have self d/c pa line and introducer from rt ij- bleeding small amount-\nheld pressure- no evidence of pneumo/ho called and came to examine.\nwith commotion of pa line d/c- bp up to 130/.\nd/c neo drops as of 2am and remains off drops.\n\n[**name (ni) 62**] patient on 6l np- resp rate- mid 20\'s, lungs clear- appears comfortable in no distress.\n\nid- temp flat- no fever\n\ngu-20cc/hour via foley catheter- am creat to be checked- atn\n\n[**name (ni) 232**] patient taking meds/lix without issue\n(+) bowel sounds, no stool.\n\n[**name (ni) 324**] patient alert and oriented- when awakened in middle of nite with pa line self d/[**name (ni) **] patient slightly disoriented , but easily reoriented to\ntime/place.\nson and wife in evening to visit.\nall aware of plan of care.\n\na/[**name (ni) **] patient status post aortic dissection- currently stable on milrinone drops 0.375\n- transiently requiring neo drops for low normal bp\n\ncontinue milrinone as ordered, am labs- replete lytes as needed.\nserial hct\'s check to make sure no sign of acute expansion in disection- assess back pain/level etc.\nkeep patient safe, and continue to closely assess mental status.\nif bp continues to stay above 120-130\'s, discuss with team ? addition again of some esmolol type [**doctor last name 528**] to control rate pressure product\nkeep patient aware of plan of care.\n', 'event': ['Sleep', 'Pain', 'Excretion', 'Family', 'Sleep', 'Sleep'], 'phrase': '', 'raw_output': '{\n  "events": [\n    {\n      "event_type": "Sleep",\n      "text_quote": "hypotensive slightly - 90/40- dipping to low 80\'s asleep systolically",\n      "attributes": {\n        "quality": "Unknown",\n        "duration": "Unknown",\n        "negation": false,\n        "time": "Unknown",\n        "caused_by": "Unknown"\n      }\n    },\n    {\n      "event_type": "Pain",\n      "text_quote": "denies worse back pain",\n      "attributes": {\n        "severity": "Unknown",\n        "location": "back",\n        "duration": "Unknown",\n        "negation": true,\n        "time": "Unknown",\n        "caused_by": "Unknown"\n      }\n    },\n    {\n      "event_type": "Excretion",\n      "text_quote": "gu-20cc/hour via foley catheter",\n      "attributes": {\n        "type": "urine",\n        "frequency": "Unknown",\n        "quality": "Unknown",\n        "negation": false,\n        "time": "Unknown",\n        "caused_by": "Unknown"\n      }\n    },\n    {\n      "event_type": "Family",\n      "text_quote": "son and wife in evening to visit",\n      "attributes": {\n        "interaction": "visit",\n        "relation": "son, wife",\n        "negation": false,\n        "time": "evening",\n        "caused_by": "Unknown"\n      }\n    },\n    {\n      "event_type": "Sleep",\n      "text_quote": "patient found to have self d/c pa line and introducer from rt ij- bleeding small amount- held pressure- no evidence of pneumo/ho called and came to examine. with commotion of pa line d/c- bp up to 130/",\n      "attributes": {\n        "quality": "Unknown",\n        "duration": "Unknown",\n        "negation": false,\n        "time": "Unknown",\n        "caused_by": "Unknown"\n      }\n    },\n    {\n      "event_type": "Sleep",\n      "text_quote": "patient slightly disoriented , but easily reoriented to time/place.",\n      "attributes": {\n        "quality": "Unknown",\n        "duration": "Unknown",\n        "negation": false,\n        "time": "Unknown",\n        "caused_by": "Unknown"\n      }\n    }\n  ]\n}', 'attributes': [{'Sleep': {'quality': 'Unknown', 'duration': 'Unknown', 'negation': False, 'time': 'Unknown', 'caused_by': 'Unknown'}}, {'Pain': {'severity': 'Unknown', 'location': 'back', 'duration': 'Unknown', 'negation': True, 'time': 'Unknown', 'caused_by': 'Unknown'}}, {'Excretion': {'type': 'urine', 'frequency': 'Unknown', 'quality': 'Unknown', 'negation': False, 'time': 'Unknown', 'caused_by': 'Unknown'}}, {'Family': {'interaction': 'visit', 'relation': 'son, wife', 'negation': False, 'time': 'evening', 'caused_by': 'Unknown'}}, {'Sleep': {'quality': 'Unknown', 'duration': 'Unknown', 'negation': False, 'time': 'Unknown', 'caused_by': 'Unknown'}}, {'Sleep': {'quality': 'Unknown', 'duration': 'Unknown', 'negation': False, 'time': 'Unknown', 'caused_by': 'Unknown'}}], 'text_quotes': ["hypotensive slightly - 90/40- dipping to low 80's asleep systolically", 'denies worse back pain', 'gu-20cc/hour via foley catheter', 'son and wife in evening to visit', 'patient found to have self d/c pa line and introducer from rt ij- bleeding small amount- held pressure- no evidence of pneumo/ho called and came to examine. with commotion of pa line d/c- bp up to 130/', 'patient slightly disoriented , but easily reoriented to time/place.'], 'event_name_prompt': 'Given the text: ccu nsg progress note 7p-7a/ status post aortic dissection\n\ns- " i don\'t remember doing that"?\n\no- see flowsheet for objective data\n\n[**name (ni) 231**] patient [**name (ni) 591**] hypotensive slightly - 90/40- dipping to low 80\'s asleep systolically- given 500cc ivf normal saline bolus, increased milrinone to 0.375 mcg and decreased per schedule amiodorone to 0.5mg. no significant improvement in bp and by 9:30- decided to add back small amount neo drops- 0.2 mcg/kg.\ndenies worse back pain, serial hct wnl, no evidence of worsening disection.\npa # wnl- pa- 33/17-18 ; cvp- 14-17, pcw- 16-18.\npatient found to have self d/c pa line and introducer from rt ij- bleeding small amount-\nheld pressure- no evidence of pneumo/ho called and came to examine.\nwith commotion of pa line d/c- bp up to 130/.\nd/c neo drops as of 2am and remains off drops.\n\n[**name (ni) 62**] patient on 6l np- resp rate- mid 20\'s, lungs clear- appears comfortable in no distress.\n\nid- temp flat- no fever\n\ngu-20cc/hour via foley catheter- am creat to be checked- atn\n\n[**name (ni) 232**] patient taking meds/lix without issue\n(+) bowel sounds, no stool.\n\n[**name (ni) 324**] patient alert and oriented- when awakened in middle of nite with pa line self d/[**name (ni) **] patient slightly disoriented , but easily reoriented to\ntime/place.\nson and wife in evening to visit.\nall aware of plan of care.\n\na/[**name (ni) **] patient status post aortic dissection- currently stable on milrinone drops 0.375\n- transiently requiring neo drops for low normal bp\n\ncontinue milrinone as ordered, am labs- replete lytes as needed.\nserial hct\'s check to make sure no sign of acute expansion in disection- assess back pain/level etc.\nkeep patient safe, and continue to closely assess mental status.\nif bp continues to stay above 120-130\'s, discuss with team ? addition again of some esmolol type [**doctor last name 528**] to control rate pressure product\nkeep patient aware of plan of care.\n, \n                        and the following event types with their definitions: Eating : The patient takes food into their body by mouth.\nExcretion : The patient discharges waste matter from their body.\nFamily : The patient has a visit, call, or communication with a family member.\nPain : The patient reports or shows signs of pain.\nSleep : The patient sleeps or the sleep’s quality or quantity is described.\nUnknown : choose "Unknown" if none of the other event type are applicable. \n                        ---\n                        Your task:\n                        0. Identify ALL events in the text (zero, one, or more).\n1. For each event, assign an event_type from the list above.\n2. If multiple event of same type is mentioned, assign the event_type multiple times\n3. Extract attributes for each event using ONLY the allowed attributes listed below.\n4. Use keyword evidence (Ki) ONLY if it is consistent with the text context.\n5. Output strictly valid JSON following the schema below.\n                        ---\n                        Classification Rules:\n                        - A text may contain multiple events of the same or different types.\n- Create a separate event object for each event mention.\n- If the text is explicitly a NEGATION (e.g., "denies pain"), do not extract that event.\n- If the text describes a FUTURE or HYPOTHETICAL event (e.g., "will eat tomorrow"), ignore it.\n- A valid event should have occurred in the recent past or is occurring during the time of writing of the text.\n- If no events are found or if unsure, return {"events": []}\n                        \n                        ---\n                                    Attributes allowed:\n                                    {\'Eating\': {\'food\': \'&lt;string&gt; # e.g., pancakes, porridge, etc.\', \'amount\': \'&lt;string&gt; # e.g., 1, 2 bowls, etc.\', \'method\': \'&lt;string&gt;  # e.g., oral, tube, etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, after shower, etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}, \'Excretion\': {\'type\': \'&lt;string&gt; # e.g., urine, stool, etc.\', \'frequency\': \'&lt;string&gt; # e.g., 2x, once, etc.\', \'quality\': \'&lt;string&gt; # e.g., loose, hard, etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, after shower, etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}, \'Family\': {\'interaction\': \'&lt;string&gt; # e.g., visit, call, communication, etc.\', \'relation\': \'&lt;string&gt; # e.g., mother, son, etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, after shower, etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}, \'Pain\': {\'severity\': \'&lt;string&gt; # e.g., mild, moderate, severe, numeric scale if present, etc.\', \'location\': \'&lt;string&gt; # e.g., right knee, head, etc.\', \'duration\': \'&lt;string&gt; # e.g., all night, 3 hours, etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, after shower, etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}, \'Sleep\': {\'quality\': \'&lt;string&gt; # e.g., good, poor, restless, etc.\', \'duration\': \'&lt;string&gt; # e.g., 6 hours, phrases like "all night", etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, after shower, etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}}\n                                    If no relevant attribute exists for an event, return an empty object {}.\n                                    \n                        \n                        ---\n                                    Keyword evidence (Ki):\n                                    Additional facts: A keyword matching algorithm without context detected keyword(s) [\'asleep\', \'distress\', \'son\', \'pain\'].\n                                    Use this only as a pointer. If context contradicts, ignore.\n                        ---\n                        Output Schema (strict):\n                        {\n                                    "events": [\n                                        {\n                                        "event_type": "&lt;Pain | Sleep | Excretion | Eating | Family&gt;",\n                                        "text_quote": "&lt;fragement from the text indicating &gt;",\n                "attributes": {\n                    "&lt;attribute_name&gt;": "&lt;attribute_value&gt;"\n                }\n                                        }\n                                    ]\n                                    }\n                        \n                            Rules:\n                                - Ensure the output is valid JSON (parseable).\n                                - "eventS" must always be an array (can be empty).\n                                - Multiple instances of the same event type appear as individual elements in the event array.\n                                - Events appear in the array in the same order in which they appear in the text.\n                                - Do not include extra keys, comments, or text.\n                                - Each object in "events" must contain "event_type", "text_quote", and "attributes".\n                                -If an event attribute type has no value mentioned, return "attributes": {"&lt; attribute name &gt;:Unknown"} for each attribute type defined for the event type \n                        \n                        \n                        \n                        ', 'event_detection_time': 16.87695832499594}</t>
+          <t>['asleep systolically-', 'denies worse back pain', 'gu-20cc/hour via foley catheter', 'son and wife in evening to visit', 'patient slightly disoriented , but easily reoriented to time/place']</t>
         </is>
       </c>
       <c r="J6" t="inlineStr">
         <is>
-          <t>['Sleep', 'Pain', 'Excretion', 'Family', 'Sleep', 'Sleep']</t>
+          <t>[[]]</t>
         </is>
       </c>
       <c r="K6" t="inlineStr">
         <is>
-          <t>[{'Sleep': {'quality': 'Unknown', 'duration': 'Unknown', 'negation': False, 'time': 'Unknown', 'caused_by': 'Unknown'}}, {'Pain': {'severity': 'Unknown', 'location': 'back', 'duration': 'Unknown', 'negation': True, 'time': 'Unknown', 'caused_by': 'Unknown'}}, {'Excretion': {'type': 'urine', 'frequency': 'Unknown', 'quality': 'Unknown', 'negation': False, 'time': 'Unknown', 'caused_by': 'Unknown'}}, {'Family': {'interaction': 'visit', 'relation': 'son, wife', 'negation': False, 'time': 'evening', 'caused_by': 'Unknown'}}, {'Sleep': {'quality': 'Unknown', 'duration': 'Unknown', 'negation': False, 'time': 'Unknown', 'caused_by': 'Unknown'}}, {'Sleep': {'quality': 'Unknown', 'duration': 'Unknown', 'negation': False, 'time': 'Unknown', 'caused_by': 'Unknown'}}]</t>
+          <t>{'text': 'ccu nsg progress note 7p-7a/ status post aortic dissection\n\ns- " i don\'t remember doing that"?\n\no- see flowsheet for objective data\n\n[**name (ni) 231**] patient [**name (ni) 591**] hypotensive slightly - 90/40- dipping to low 80\'s asleep systolically- given 500cc ivf normal saline bolus, increased milrinone to 0.375 mcg and decreased per schedule amiodorone to 0.5mg. no significant improvement in bp and by 9:30- decided to add back small amount neo drops- 0.2 mcg/kg.\ndenies worse back pain, serial hct wnl, no evidence of worsening disection.\npa # wnl- pa- 33/17-18 ; cvp- 14-17, pcw- 16-18.\npatient found to have self d/c pa line and introducer from rt ij- bleeding small amount-\nheld pressure- no evidence of pneumo/ho called and came to examine.\nwith commotion of pa line d/c- bp up to 130/.\nd/c neo drops as of 2am and remains off drops.\n\n[**name (ni) 62**] patient on 6l np- resp rate- mid 20\'s, lungs clear- appears comfortable in no distress.\n\nid- temp flat- no fever\n\ngu-20cc/hour via foley catheter- am creat to be checked- atn\n\n[**name (ni) 232**] patient taking meds/lix without issue\n(+) bowel sounds, no stool.\n\n[**name (ni) 324**] patient alert and oriented- when awakened in middle of nite with pa line self d/[**name (ni) **] patient slightly disoriented , but easily reoriented to\ntime/place.\nson and wife in evening to visit.\nall aware of plan of care.\n\na/[**name (ni) **] patient status post aortic dissection- currently stable on milrinone drops 0.375\n- transiently requiring neo drops for low normal bp\n\ncontinue milrinone as ordered, am labs- replete lytes as needed.\nserial hct\'s check to make sure no sign of acute expansion in disection- assess back pain/level etc.\nkeep patient safe, and continue to closely assess mental status.\nif bp continues to stay above 120-130\'s, discuss with team ? addition again of some esmolol type [**doctor last name 528**] to control rate pressure product\nkeep patient aware of plan of care.\n', 'event': ['Sleep', 'Excretion', 'Family', 'Pain', 'Sleep', 'Sleep'], 'event_id': ['e1', 'e2', 'e3', 'e4', 'e5', 'e6'], 'phrase': '', 'raw_output': '{\n  "events": [\n    {\n      "event_id": "e1",\n      "event_type": "Sleep",\n      "text_quote": "hypotensive slightly - 90/40- dipping to low 80\'s asleep systolically",\n      "attributes": {\n        "quality": "Unknown",\n        "duration": "Unknown",\n        "negation": false,\n        "time": "asleep"\n      }\n    },\n    {\n      "event_id": "e2",\n      "event_type": "Excretion",\n      "text_quote": "gu-20cc/hour via foley catheter",\n      "attributes": {\n        "type": "urine",\n        "frequency": "Unknown",\n        "quality": "Unknown",\n        "negation": false,\n        "time": "Unknown"\n      }\n    },\n    {\n      "event_id": "e3",\n      "event_type": "Family",\n      "text_quote": "son and wife in evening to visit",\n      "attributes": {\n        "interaction": "visit",\n        "relation": "son, wife",\n        "negation": false,\n        "time": "evening"\n      }\n    },\n    {\n      "event_id": "e4",\n      "event_type": "Pain",\n      "text_quote": "denies worse back pain",\n      "attributes": {\n        "severity": "Unknown",\n        "location": "back",\n        "duration": "Unknown",\n        "negation": true,\n        "time": "Unknown"\n      }\n    },\n    {\n      "event_id": "e5",\n      "event_type": "Sleep",\n      "text_quote": "patient found to have self d/c pa line and introducer from rt ij- bleeding small amount- held pressure- no evidence of pneumo/ho called and came to examine. with commotion of pa line d/c- bp up to 130/",\n      "attributes": {\n        "quality": "Unknown",\n        "duration": "Unknown",\n        "negation": false,\n        "time": "Unknown"\n      }\n    },\n    {\n      "event_id": "e6",\n      "event_type": "Sleep",\n      "text_quote": "patient alert and oriented- when awakened in middle of nite with pa line self d/[**name (ni) **] patient slightly disoriented , but easily reoriented to time/place.",\n      "attributes": {\n        "quality": "Unknown",\n        "duration": "Unknown",\n        "negation": false,\n        "time": "middle of night"\n      }\n    }\n  ],\n  "order": [\n    ["e1", "before", "e2"],\n    ["e2", "before", "e3"],\n    ["e3", "before", "e4"],\n    ["e4", "before", "e5"],\n    ["e5", "before", "e6"]\n  ]\n}', 'attributes': [{'Sleep': {'quality': 'Unknown', 'duration': 'Unknown', 'negation': False, 'time': 'asleep'}}, {'Excretion': {'type': 'urine', 'frequency': 'Unknown', 'quality': 'Unknown', 'negation': False, 'time': 'Unknown'}}, {'Family': {'interaction': 'visit', 'relation': 'son, wife', 'negation': False, 'time': 'evening'}}, {'Pain': {'severity': 'Unknown', 'location': 'back', 'duration': 'Unknown', 'negation': True, 'time': 'Unknown'}}, {'Sleep': {'quality': 'Unknown', 'duration': 'Unknown', 'negation': False, 'time': 'Unknown'}}, {'Sleep': {'quality': 'Unknown', 'duration': 'Unknown', 'negation': False, 'time': 'middle of night'}}], 'orders': [[['e1', 'before', 'e2'], ['e2', 'before', 'e3'], ['e3', 'before', 'e4'], ['e4', 'before', 'e5'], ['e5', 'before', 'e6']]], 'text_quotes': ["hypotensive slightly - 90/40- dipping to low 80's asleep systolically", 'gu-20cc/hour via foley catheter', 'son and wife in evening to visit', 'denies worse back pain', 'patient found to have self d/c pa line and introducer from rt ij- bleeding small amount- held pressure- no evidence of pneumo/ho called and came to examine. with commotion of pa line d/c- bp up to 130/', 'patient alert and oriented- when awakened in middle of nite with pa line self d/[**name (ni) **] patient slightly disoriented , but easily reoriented to time/place.'], 'event_name_prompt': 'Given the text: ccu nsg progress note 7p-7a/ status post aortic dissection\n\ns- " i don\'t remember doing that"?\n\no- see flowsheet for objective data\n\n[**name (ni) 231**] patient [**name (ni) 591**] hypotensive slightly - 90/40- dipping to low 80\'s asleep systolically- given 500cc ivf normal saline bolus, increased milrinone to 0.375 mcg and decreased per schedule amiodorone to 0.5mg. no significant improvement in bp and by 9:30- decided to add back small amount neo drops- 0.2 mcg/kg.\ndenies worse back pain, serial hct wnl, no evidence of worsening disection.\npa # wnl- pa- 33/17-18 ; cvp- 14-17, pcw- 16-18.\npatient found to have self d/c pa line and introducer from rt ij- bleeding small amount-\nheld pressure- no evidence of pneumo/ho called and came to examine.\nwith commotion of pa line d/c- bp up to 130/.\nd/c neo drops as of 2am and remains off drops.\n\n[**name (ni) 62**] patient on 6l np- resp rate- mid 20\'s, lungs clear- appears comfortable in no distress.\n\nid- temp flat- no fever\n\ngu-20cc/hour via foley catheter- am creat to be checked- atn\n\n[**name (ni) 232**] patient taking meds/lix without issue\n(+) bowel sounds, no stool.\n\n[**name (ni) 324**] patient alert and oriented- when awakened in middle of nite with pa line self d/[**name (ni) **] patient slightly disoriented , but easily reoriented to\ntime/place.\nson and wife in evening to visit.\nall aware of plan of care.\n\na/[**name (ni) **] patient status post aortic dissection- currently stable on milrinone drops 0.375\n- transiently requiring neo drops for low normal bp\n\ncontinue milrinone as ordered, am labs- replete lytes as needed.\nserial hct\'s check to make sure no sign of acute expansion in disection- assess back pain/level etc.\nkeep patient safe, and continue to closely assess mental status.\nif bp continues to stay above 120-130\'s, discuss with team ? addition again of some esmolol type [**doctor last name 528**] to control rate pressure product\nkeep patient aware of plan of care.\n, \n                        and the following event types with their definitions: Eating : The patient takes food into their body by mouth.\nExcretion : The patient discharges waste matter from their body.\nFamily : The patient has a visit, call, or communication with a family member.\nPain : The patient reports or shows signs of pain.\nSleep : The patient sleeps or the sleep’s quality or quantity is described.\nUnknown : choose "Unknown" if none of the other event type are applicable. \n                        ---\n                        Your task:\n                        0. Identify ALL events in the text (zero, one, or more).\n1. For each event, assign an event_type from the list above.\n2. If multiple event of same type is mentioned, assign the event_type multiple times\n3. Extract attributes for each event using ONLY the allowed attributes listed below.\n4. Use keyword evidence (Ki) ONLY if it is consistent with the text context.\n5. Output strictly valid JSON following the schema below.\n                        ---\n                        Classification Rules:\n                        - A text may contain multiple events of the same or different types.\n- Create a separate event object for each event mention.\n- If the text is explicitly a NEGATION (e.g., "denies pain"), do not extract that event.\n- If the text describes a FUTURE or HYPOTHETICAL event (e.g., "will eat tomorrow"), ignore it.\n- A valid event should have occurred in the recent past or is occurring during the time of writing of the text.\n- If no events are found or if unsure, return {"events": []}\n                        \n                        ---\n                                    Attributes allowed:\n                                    {\'Eating\': {\'food\': \'&lt;string&gt; # e.g., pancakes, porridge, etc.\', \'amount\': \'&lt;string&gt; # e.g., 1, 2 bowls, etc.\', \'method\': \'&lt;string&gt;  # e.g., oral, tube, etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, evening etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}, \'Excretion\': {\'type\': \'&lt;string&gt; # e.g., urine, stool, etc.\', \'frequency\': \'&lt;string&gt; # e.g., 2x, once, etc.\', \'quality\': \'&lt;string&gt; # e.g., loose, hard, etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, evening etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}, \'Family\': {\'interaction\': \'&lt;string&gt; # e.g., visit, call, communication, etc.\', \'relation\': \'&lt;string&gt; # e.g., mother, son, etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, evening etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}, \'Pain\': {\'severity\': \'&lt;string&gt; # e.g., mild, moderate, severe, numeric scale if present, etc.\', \'location\': \'&lt;string&gt; # e.g., right knee, head, etc.\', \'duration\': \'&lt;string&gt; # e.g., all night, 3 hours, etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, evening etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}, \'Sleep\': {\'quality\': \'&lt;string&gt; # e.g., good, poor, restless, etc.\', \'duration\': \'&lt;string&gt; # e.g., 6 hours, phrases like "all night", etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, evening etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}}\n                                    If no relevant attribute exists for an event, return an empty object {}.\n                                    \n                        \n                        ---\n                                    Keyword evidence (Ki):\n                                    Additional facts: A keyword matching algorithm without context detected keyword(s) (\'pain\', \'distress\', \'son\', \'asleep\').\n                                    Use this only as a pointer. If context contradicts, ignore.\n                        ---\n                        Output Schema (strict):\n                        {\n                                    "events": [\n                                        {\n                                        "event_id": "&lt; A unique id eg.: e1 | e2 |...&gt;"\n                                        "event_type": "&lt;Pain | Sleep | Excretion | Eating | Family&gt;",\n                                        "text_quote": "&lt;fragement from the text indicating the event_type&gt;",\n                "attributes": {\n                    "&lt;attribute_name&gt;": "&lt;attribute_value&gt;"\n                }\n                                        }\n                                    ],\n                                    "order": [\n                                        ["e1", "before" | "after" | "simultaneous", "e2" ]\n                                    ]\n                                    }\n                        \n                            Rules:\n                                - Ensure the output is valid JSON (parseable).\n                                - "eventS" must always be an array (can be empty).\n                                - Multiple instances of the same event type appear with different ids.\n                                - Events appear in the array in the same order in which they appear in the text.\n                                - Their partial orders can be expressed using the "order" section.\n                                - Do not include extra keys, comments, or text.\n                                - Each object in "events" must contain "event_type", "text_quote", and "attributes".\n                                - If an event attribute type has no value mentioned, return "attributes": {"&lt; attribute name &gt;:Unknown"} for each attribute type defined for the event type \n                        \n                        \n                        \n                        ', 'event_detection_time': 19.795291120943148}</t>
         </is>
       </c>
       <c r="L6" t="inlineStr">
         <is>
-          <t>["hypotensive slightly - 90/40- dipping to low 80's asleep systolically", 'denies worse back pain', 'gu-20cc/hour via foley catheter', 'son and wife in evening to visit', 'patient found to have self d/c pa line and introducer from rt ij- bleeding small amount- held pressure- no evidence of pneumo/ho called and came to examine. with commotion of pa line d/c- bp up to 130/', 'patient slightly disoriented , but easily reoriented to time/place.']</t>
+          <t>['Sleep', 'Excretion', 'Family', 'Pain', 'Sleep', 'Sleep']</t>
         </is>
       </c>
       <c r="M6" t="inlineStr">
         <is>
-          <t>{'text': 'ccu nsg progress note 7p-7a/ status post aortic dissection\n\ns- " i don\'t remember doing that"?\n\no- see flowsheet for objective data\n\n[**name (ni) 231**] patient [**name (ni) 591**] hypotensive slightly - 90/40- dipping to low 80\'s asleep systolically- given 500cc ivf normal saline bolus, increased milrinone to 0.375 mcg and decreased per schedule amiodorone to 0.5mg. no significant improvement in bp and by 9:30- decided to add back small amount neo drops- 0.2 mcg/kg.\ndenies worse back pain, serial hct wnl, no evidence of worsening disection.\npa # wnl- pa- 33/17-18 ; cvp- 14-17, pcw- 16-18.\npatient found to have self d/c pa line and introducer from rt ij- bleeding small amount-\nheld pressure- no evidence of pneumo/ho called and came to examine.\nwith commotion of pa line d/c- bp up to 130/.\nd/c neo drops as of 2am and remains off drops.\n\n[**name (ni) 62**] patient on 6l np- resp rate- mid 20\'s, lungs clear- appears comfortable in no distress.\n\nid- temp flat- no fever\n\ngu-20cc/hour via foley catheter- am creat to be checked- atn\n\n[**name (ni) 232**] patient taking meds/lix without issue\n(+) bowel sounds, no stool.\n\n[**name (ni) 324**] patient alert and oriented- when awakened in middle of nite with pa line self d/[**name (ni) **] patient slightly disoriented , but easily reoriented to\ntime/place.\nson and wife in evening to visit.\nall aware of plan of care.\n\na/[**name (ni) **] patient status post aortic dissection- currently stable on milrinone drops 0.375\n- transiently requiring neo drops for low normal bp\n\ncontinue milrinone as ordered, am labs- replete lytes as needed.\nserial hct\'s check to make sure no sign of acute expansion in disection- assess back pain/level etc.\nkeep patient safe, and continue to closely assess mental status.\nif bp continues to stay above 120-130\'s, discuss with team ? addition again of some esmolol type [**doctor last name 528**] to control rate pressure product\nkeep patient aware of plan of care.\n', 'event': ['Sleep', 'Excretion', 'Family', 'Pain', 'Sleep'], 'phrase': '', 'raw_output': '{\n  "events": [\n    {\n      "event_type": "Sleep",\n      "text_quote": "asleep systolically-",\n      "attributes": {\n        "quality": "Unknown",\n        "duration": "Unknown",\n        "time": "Unknown",\n        "caused_by": "Unknown"\n      }\n    },\n    {\n      "event_type": "Excretion",\n      "text_quote": "gu-20cc/hour via foley catheter",\n      "attributes": {\n        "type": "urine",\n        "frequency": "20cc/hour",\n        "quality": "Unknown",\n        "time": "Unknown",\n        "caused_by": "Unknown"\n      }\n    },\n    {\n      "event_type": "Family",\n      "text_quote": "son and wife in evening to visit.",\n      "attributes": {\n        "interaction": "visit",\n        "relation": "son, wife",\n        "time": "evening",\n        "caused_by": "Unknown"\n      }\n    },\n    {\n      "event_type": "Pain",\n      "text_quote": "denies worse back pain",\n      "attributes": {\n        "severity": "Unknown",\n        "location": "back",\n        "duration": "Unknown",\n        "time": "Unknown",\n        "caused_by": "Unknown"\n      }\n    },\n    {\n      "event_type": "Sleep",\n      "text_quote": "bp up to 130/.",\n      "attributes": {\n        "quality": "Unknown",\n        "duration": "Unknown",\n        "time": "Unknown",\n        "caused_by": "Unknown"\n      }\n    }\n  ]\n}', 'attributes': [{'Sleep': {'quality': 'Unknown', 'duration': 'Unknown', 'time': 'Unknown', 'caused_by': 'Unknown'}}, {'Excretion': {'type': 'urine', 'frequency': '20cc/hour', 'quality': 'Unknown', 'time': 'Unknown', 'caused_by': 'Unknown'}}, {'Family': {'interaction': 'visit', 'relation': 'son, wife', 'time': 'evening', 'caused_by': 'Unknown'}}, {'Pain': {'severity': 'Unknown', 'location': 'back', 'duration': 'Unknown', 'time': 'Unknown', 'caused_by': 'Unknown'}}, {'Sleep': {'quality': 'Unknown', 'duration': 'Unknown', 'time': 'Unknown', 'caused_by': 'Unknown'}}], 'text_quotes': ['asleep systolically-', 'gu-20cc/hour via foley catheter', 'son and wife in evening to visit.', 'denies worse back pain', 'bp up to 130/.'], 'event_name_prompt': 'Given the text: ccu nsg progress note 7p-7a/ status post aortic dissection\n\ns- " i don\'t remember doing that"?\n\no- see flowsheet for objective data\n\n[**name (ni) 231**] patient [**name (ni) 591**] hypotensive slightly - 90/40- dipping to low 80\'s asleep systolically- given 500cc ivf normal saline bolus, increased milrinone to 0.375 mcg and decreased per schedule amiodorone to 0.5mg. no significant improvement in bp and by 9:30- decided to add back small amount neo drops- 0.2 mcg/kg.\ndenies worse back pain, serial hct wnl, no evidence of worsening disection.\npa # wnl- pa- 33/17-18 ; cvp- 14-17, pcw- 16-18.\npatient found to have self d/c pa line and introducer from rt ij- bleeding small amount-\nheld pressure- no evidence of pneumo/ho called and came to examine.\nwith commotion of pa line d/c- bp up to 130/.\nd/c neo drops as of 2am and remains off drops.\n\n[**name (ni) 62**] patient on 6l np- resp rate- mid 20\'s, lungs clear- appears comfortable in no distress.\n\nid- temp flat- no fever\n\ngu-20cc/hour via foley catheter- am creat to be checked- atn\n\n[**name (ni) 232**] patient taking meds/lix without issue\n(+) bowel sounds, no stool.\n\n[**name (ni) 324**] patient alert and oriented- when awakened in middle of nite with pa line self d/[**name (ni) **] patient slightly disoriented , but easily reoriented to\ntime/place.\nson and wife in evening to visit.\nall aware of plan of care.\n\na/[**name (ni) **] patient status post aortic dissection- currently stable on milrinone drops 0.375\n- transiently requiring neo drops for low normal bp\n\ncontinue milrinone as ordered, am labs- replete lytes as needed.\nserial hct\'s check to make sure no sign of acute expansion in disection- assess back pain/level etc.\nkeep patient safe, and continue to closely assess mental status.\nif bp continues to stay above 120-130\'s, discuss with team ? addition again of some esmolol type [**doctor last name 528**] to control rate pressure product\nkeep patient aware of plan of care.\n, \n                        and the following event types with their definitions: Eating : The patient takes food into their body by mouth.\nExcretion : The patient discharges waste matter from their body.\nFamily : The patient has a visit, call, or communication with a family member.\nPain : The patient reports or shows signs of pain.\nSleep : The patient sleeps or the sleep’s quality or quantity is described.\nUnknown : choose "Unknown" if none of the other event type are applicable. \n                        ---\n                        Your task:\n                        0. Identify ALL events in the text (zero, one, or more).\n1. For each event, assign an event_type from the list above.\n2. If multiple event of same type is mentioned, assign the event_type multiple times\n3. Extract attributes for each event using ONLY the allowed attributes listed below.\n4. Output strictly valid JSON following the schema below.\n                        ---\n                        Classification Rules:\n                        - A text may contain multiple events of the same or different types.\n- Create a separate event object for each event mention.\n- If the text is explicitly a NEGATION (e.g., "denies pain"), do not extract that event.\n- If the text describes a FUTURE or HYPOTHETICAL event (e.g., "will eat tomorrow"), ignore it.\n- A valid event should have occurred in the recent past or is occurring during the time of writing of the text.\n- If no events are found or if unsure, return {"events": []}\n                        \n                        ---\n                                    Attributes allowed:\n                                    {\'Eating\': {\'food\': \'&lt;string&gt; # e.g., pancakes, porridge, etc.\', \'amount\': \'&lt;string&gt; # e.g., 1, 2 bowls, etc.\', \'method\': \'&lt;string&gt;  # e.g., oral, tube, etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, after shower, etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}, \'Excretion\': {\'type\': \'&lt;string&gt; # e.g., urine, stool, etc.\', \'frequency\': \'&lt;string&gt; # e.g., 2x, once, etc.\', \'quality\': \'&lt;string&gt; # e.g., loose, hard, etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, after shower, etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}, \'Family\': {\'interaction\': \'&lt;string&gt; # e.g., visit, call, communication, etc.\', \'relation\': \'&lt;string&gt; # e.g., mother, son, etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, after shower, etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}, \'Pain\': {\'severity\': \'&lt;string&gt; # e.g., mild, moderate, severe, numeric scale if present, etc.\', \'location\': \'&lt;string&gt; # e.g., right knee, head, etc.\', \'duration\': \'&lt;string&gt; # e.g., all night, 3 hours, etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, after shower, etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}, \'Sleep\': {\'quality\': \'&lt;string&gt; # e.g., good, poor, restless, etc.\', \'duration\': \'&lt;string&gt; # e.g., 6 hours, phrases like "all night", etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, after shower, etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}}\n                                    If no relevant attribute exists for an event, return an empty object {}.\n                                    \n                        \n                        \n                        ---\n                        Output Schema (strict):\n                        {\n                                    "events": [\n                                        {\n                                        "event_type": "&lt;Pain | Sleep | Excretion | Eating | Family&gt;",\n                                        "text_quote": "&lt;fragement from the text indicating &gt;",\n                "attributes": {\n                    "&lt;attribute_name&gt;": "&lt;attribute_value&gt;"\n                }\n                                        }\n                                    ]\n                                    }\n                        \n                            Rules:\n                                - Ensure the output is valid JSON (parseable).\n                                - "eventS" must always be an array (can be empty).\n                                - Multiple instances of the same event type appear as individual elements in the event array.\n                                - Events appear in the array in the same order in which they appear in the text.\n                                - Do not include extra keys, comments, or text.\n                                - Each object in "events" must contain "event_type", "text_quote", and "attributes".\n                                -If an event attribute type has no value mentioned, return "attributes": {"&lt; attribute name &gt;:Unknown"} for each attribute type defined for the event type \n                        \n                        \n                        \n                ---\n                Examples:\n                \n                text: "Patient ate breakfast this morning. He seems less anxious."\n                output: {\n                "events": [\n                    {\n                    "event_type": "Eating",\n                    "text_quote":"Patient ate breakfast this morning",\n                    "attributes": {"food": "breakfast", \n                                   "amount": "Unknown",\n                                   "method": "Unknown",\n                                   "time":"morning",\n                                   "caused_by":"Unknown"}\n                    }\n                ]\n                }\n                \n                text: "Patient reported severe abdominal pain."\n                output: {\n                "events": [\n                    {\n                    "event_type": "Pain",\n                    "text_quote": "severe abdominal Pain",\n                    "attributes": {"severity": "severe", \n                                   "location": "abdominal",\n                                   "duration": "Unknown",\n                                   "time":"Unknown",\n                                   "caused_by":"Unknown"}\n                    }\n                ]\n                }\n                \n                text: "Patient called his son around 3 pm."\n                output: {\n                "events": [\n                    {\n                    "event_type": "Family",\n                    "text_quote": "called his son around 3 pm",\n                    "attributes": {"interaction": "call", \n                                    "relation": "son",\n                                    "time":"3 pm",\n                                    "caused_by":"Unknown"}\n                    }\n                ]\n                }\n                \n                text: "Patient had a loose stool overnight."\n                output: {\n                "events": [\n                    {\n                    "event_type": "Excretion",\n                    "text_quote": "loose stool overnight",\n                    "attributes": {"type": "stool", \n                                   "quality": "loose", \n                                   "frequency":"overnight", \n                                   "time":"night",\n                                   "caused_by":"Unknown"}\n                    }\n                ]\n                }\n                \n                text: "Patient was able to sleep well last night."\n                output: {\n                "events": [\n                    {\n                    "event_type": "Sleep",\n                    "text_quote": "sleep well last night",\n                    "attributes": {"quality": "well",\n                                    "duration": "Unknown", \n                                    "time":"night",\n                                    "caused_by":"Unknown"}\n                    }\n                ]\n                }\n                \n                text: "The patient couldn\'t sleep due to severe pain."\n                output: {\n                "events": [\n                    {\n                    "event_type": "Sleep",\n                    "text_quote": "couldn\'t sleep",\n                    "attributes": {"quality": "poor", \n                                    "duration": "Unknown",\n                                   "time":"Unknown",\n                                   "caused_by":"Pain"}\n                    },\n                    {\n                    "event_type": "Pain",\n                    "text_quote": "severe pain",\n                    "attributes": {"severity": "severe", \n                                    "location": "Unknown", \n                                    "duration": "Unknown", \n                                   "time":"before Sleep",\n                                   "caused_by":"Unknown"}\n                    }\n                ]\n                }\n                \n                text: "The patient complained of severe back pain, was given Tylenol, but the pain persisted and he was then prescribed stronger morphine."\n                output: {\n                "events": [\n                    {\n                    "event_type": "Pain",\n                    "text_quote": "complained of severe back pain",\n                    "attributes": {"severity": "severe", \n                                    "location": "back",\n                                    "duration": "Unknown", \n                                    "time":"Unknown",\n                                    "caused_by":"Unknown"}\n                    },\n                    {\n                    "event_type": "Pain",\n                    "text_quote": "pain persisted",\n                    "attributes": {"severity": "severe", \n                                   "location": "back",\n                                   "duration": "persistent", \n                                   "time":"after Tylenol",\n                                   "caused_by":"Unknown"}\n                    }\n                ]\n                }\n                \n                        ', 'event_detection_time': 12.834220667005866}</t>
+          <t>[{'Sleep': {'quality': 'Unknown', 'duration': 'Unknown', 'negation': False, 'time': 'asleep'}}, {'Excretion': {'type': 'urine', 'frequency': 'Unknown', 'quality': 'Unknown', 'negation': False, 'time': 'Unknown'}}, {'Family': {'interaction': 'visit', 'relation': 'son, wife', 'negation': False, 'time': 'evening'}}, {'Pain': {'severity': 'Unknown', 'location': 'back', 'duration': 'Unknown', 'negation': True, 'time': 'Unknown'}}, {'Sleep': {'quality': 'Unknown', 'duration': 'Unknown', 'negation': False, 'time': 'Unknown'}}, {'Sleep': {'quality': 'Unknown', 'duration': 'Unknown', 'negation': False, 'time': 'middle of night'}}]</t>
         </is>
       </c>
       <c r="N6" t="inlineStr">
         <is>
-          <t>['Sleep', 'Excretion', 'Family', 'Pain', 'Sleep']</t>
+          <t>["hypotensive slightly - 90/40- dipping to low 80's asleep systolically", 'gu-20cc/hour via foley catheter', 'son and wife in evening to visit', 'denies worse back pain', 'patient found to have self d/c pa line and introducer from rt ij- bleeding small amount- held pressure- no evidence of pneumo/ho called and came to examine. with commotion of pa line d/c- bp up to 130/', 'patient alert and oriented- when awakened in middle of nite with pa line self d/[**name (ni) **] patient slightly disoriented , but easily reoriented to time/place.']</t>
         </is>
       </c>
       <c r="O6" t="inlineStr">
         <is>
-          <t>[{'Sleep': {'quality': 'Unknown', 'duration': 'Unknown', 'time': 'Unknown', 'caused_by': 'Unknown'}}, {'Excretion': {'type': 'urine', 'frequency': '20cc/hour', 'quality': 'Unknown', 'time': 'Unknown', 'caused_by': 'Unknown'}}, {'Family': {'interaction': 'visit', 'relation': 'son, wife', 'time': 'evening', 'caused_by': 'Unknown'}}, {'Pain': {'severity': 'Unknown', 'location': 'back', 'duration': 'Unknown', 'time': 'Unknown', 'caused_by': 'Unknown'}}, {'Sleep': {'quality': 'Unknown', 'duration': 'Unknown', 'time': 'Unknown', 'caused_by': 'Unknown'}}]</t>
-        </is>
-      </c>
-      <c r="P6" t="inlineStr">
-        <is>
-          <t>['asleep systolically-', 'gu-20cc/hour via foley catheter', 'son and wife in evening to visit.', 'denies worse back pain', 'bp up to 130/.']</t>
-        </is>
-      </c>
-      <c r="Q6" t="n">
-        <v>0.002996749000885757</v>
-      </c>
-      <c r="R6" t="inlineStr">
+          <t>[[['e1', 'before', 'e2'], ['e2', 'before', 'e3'], ['e3', 'before', 'e4'], ['e4', 'before', 'e5'], ['e5', 'before', 'e6']]]</t>
+        </is>
+      </c>
+      <c r="P6" t="n">
+        <v>0.002427657000225736</v>
+      </c>
+      <c r="Q6" t="inlineStr">
         <is>
           <t>Sleep</t>
         </is>
       </c>
-      <c r="S6" t="b">
-        <v>0</v>
+      <c r="R6" t="b">
+        <v>0</v>
+      </c>
+      <c r="S6" t="n">
+        <v>1</v>
       </c>
       <c r="T6" t="n">
         <v>1</v>
       </c>
-      <c r="U6" t="n">
-        <v>1</v>
-      </c>
-      <c r="V6" t="inlineStr">
+      <c r="U6" t="inlineStr">
         <is>
           <t>('pain', 'distress', 'son', 'asleep')</t>
         </is>
       </c>
+      <c r="V6" t="n">
+        <v>16.16921870503575</v>
+      </c>
       <c r="W6" t="n">
-        <v>12.94783950099372</v>
+        <v>19.79529112094315</v>
       </c>
       <c r="X6" t="n">
-        <v>16.87695832499594</v>
+        <v>1</v>
       </c>
       <c r="Y6" t="n">
-        <v>12.83422066700587</v>
+        <v>1</v>
       </c>
       <c r="Z6" t="n">
-        <v>1</v>
-      </c>
-      <c r="AA6" t="n">
-        <v>1</v>
-      </c>
-      <c r="AB6" t="n">
-        <v>1</v>
-      </c>
-      <c r="AC6" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" t="n">
-        <v>1310483</v>
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>1310483</t>
+        </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>['Pain', 'Unknown']</t>
+          <t>('Pain', 'Unknown')</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>['pain']</t>
+          <t>('pain',)</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
@@ -1298,120 +1242,111 @@
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>{'text': '84 yr old c dissecting aortic aneurysm .\n\nsr c blocked beats .bp labile ranging 160 to 77 systolic.labetolol drip for short time .to have mri this pm. k, mg repleted .milrinone continues on .375.amniodarone dc iv .patient feels nauseous when bp under 110\n\nbs diminished ,7.38/32/115/20 on 6lnp\n\ntaking cl liquids,pos bs ,no stool\n\nhuo 10 to 20,creat\n\npatient restless.co low back pain some releif c tylenol and sitting on side of bed .\n\nlabile bp unexplained ,need mri to check aneurysm\n\nfollow hct,lytes\naim bp 110 to 120\nmri this pm\n\naim bp 110 to 120 sys\n\n', 'event': ['Pain', 'Eating', 'Excretion', 'Sleep'], 'phrase': '', 'raw_output': '{\n  "events": [\n    {\n      "event_type": "Pain",\n      "text_quote": "low back pain some releif c tylenol and sitting on side of bed",\n      "attributes": {\n        "severity": "Unknown",\n        "location": "low back",\n        "duration": "some releif",\n        "time": "Unknown",\n        "caused_by": "Unknown"\n      }\n    },\n    {\n      "event_type": "Eating",\n      "text_quote": "taking cl liquids,pos bs ,no stool",\n      "attributes": {\n        "food": "cl liquids",\n        "amount": "Unknown",\n        "method": "oral",\n        "time": "Unknown",\n        "caused_by": "Unknown"\n      }\n    },\n    {\n      "event_type": "Excretion",\n      "text_quote": "taking cl liquids,pos bs ,no stool",\n      "attributes": {\n        "type": "stool",\n        "frequency": "none",\n        "quality": "Unknown",\n        "time": "Unknown",\n        "caused_by": "Unknown"\n      }\n    },\n    {\n      "event_type": "Sleep",\n      "text_quote": "patient restless",\n      "attributes": {\n        "quality": "restless",\n        "duration": "Unknown",\n        "time": "Unknown",\n        "caused_by": "Unknown"\n      }\n    }\n  ]\n}', 'attributes': [{'Pain': {'severity': 'Unknown', 'location': 'low back', 'duration': 'some releif', 'time': 'Unknown', 'caused_by': 'Unknown'}}, {'Eating': {'food': 'cl liquids', 'amount': 'Unknown', 'method': 'oral', 'time': 'Unknown', 'caused_by': 'Unknown'}}, {'Excretion': {'type': 'stool', 'frequency': 'none', 'quality': 'Unknown', 'time': 'Unknown', 'caused_by': 'Unknown'}}, {'Sleep': {'quality': 'restless', 'duration': 'Unknown', 'time': 'Unknown', 'caused_by': 'Unknown'}}], 'text_quotes': ['low back pain some releif c tylenol and sitting on side of bed', 'taking cl liquids,pos bs ,no stool', 'taking cl liquids,pos bs ,no stool', 'patient restless'], 'event_name_prompt': 'Given the text: 84 yr old c dissecting aortic aneurysm .\n\nsr c blocked beats .bp labile ranging 160 to 77 systolic.labetolol drip for short time .to have mri this pm. k, mg repleted .milrinone continues on .375.amniodarone dc iv .patient feels nauseous when bp under 110\n\nbs diminished ,7.38/32/115/20 on 6lnp\n\ntaking cl liquids,pos bs ,no stool\n\nhuo 10 to 20,creat\n\npatient restless.co low back pain some releif c tylenol and sitting on side of bed .\n\nlabile bp unexplained ,need mri to check aneurysm\n\nfollow hct,lytes\naim bp 110 to 120\nmri this pm\n\naim bp 110 to 120 sys\n\n, \n                        and the following event types with their definitions: Eating : The patient takes food into their body by mouth.\nExcretion : The patient discharges waste matter from their body.\nFamily : The patient has a visit, call, or communication with a family member.\nPain : The patient reports or shows signs of pain.\nSleep : The patient sleeps or the sleep’s quality or quantity is described.\nUnknown : choose "Unknown" if none of the other event type are applicable. \n                        ---\n                        Your task:\n                        0. Identify ALL events in the text (zero, one, or more).\n1. For each event, assign an event_type from the list above.\n2. If multiple event of same type is mentioned, assign the event_type multiple times\n3. Extract attributes for each event using ONLY the allowed attributes listed below.\n4. Use keyword evidence (Ki) ONLY if it is consistent with the text context.\n5. Output strictly valid JSON following the schema below.\n                        ---\n                        Classification Rules:\n                        - A text may contain multiple events of the same or different types.\n- Create a separate event object for each event mention.\n- If the text is explicitly a NEGATION (e.g., "denies pain"), do not extract that event.\n- If the text describes a FUTURE or HYPOTHETICAL event (e.g., "will eat tomorrow"), ignore it.\n- A valid event should have occurred in the recent past or is occurring during the time of writing of the text.\n- If no events are found or if unsure, return {"events": []}\n                        \n                        ---\n                                    Attributes allowed:\n                                    {\'Eating\': {\'food\': \'&lt;string&gt; # e.g., pancakes, porridge, etc.\', \'amount\': \'&lt;string&gt; # e.g., 1, 2 bowls, etc.\', \'method\': \'&lt;string&gt;  # e.g., oral, tube, etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, after shower, etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}, \'Excretion\': {\'type\': \'&lt;string&gt; # e.g., urine, stool, etc.\', \'frequency\': \'&lt;string&gt; # e.g., 2x, once, etc.\', \'quality\': \'&lt;string&gt; # e.g., loose, hard, etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, after shower, etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}, \'Family\': {\'interaction\': \'&lt;string&gt; # e.g., visit, call, communication, etc.\', \'relation\': \'&lt;string&gt; # e.g., mother, son, etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, after shower, etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}, \'Pain\': {\'severity\': \'&lt;string&gt; # e.g., mild, moderate, severe, numeric scale if present, etc.\', \'location\': \'&lt;string&gt; # e.g., right knee, head, etc.\', \'duration\': \'&lt;string&gt; # e.g., all night, 3 hours, etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, after shower, etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}, \'Sleep\': {\'quality\': \'&lt;string&gt; # e.g., good, poor, restless, etc.\', \'duration\': \'&lt;string&gt; # e.g., 6 hours, phrases like "all night", etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, after shower, etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}}\n                                    If no relevant attribute exists for an event, return an empty object {}.\n                                    \n                        \n                        ---\n                                    Keyword evidence (Ki):\n                                    Additional facts: A keyword matching algorithm without context detected keyword(s) [\'pain\'].\n                                    Use this only as a pointer. If context contradicts, ignore.\n                        ---\n                        Output Schema (strict):\n                        {\n                                    "events": [\n                                        {\n                                        "event_type": "&lt;Pain | Sleep | Excretion | Eating | Family&gt;",\n                                        "text_quote": "&lt;fragement from the text indicating &gt;",\n                "attributes": {\n                    "&lt;attribute_name&gt;": "&lt;attribute_value&gt;"\n                }\n                                        }\n                                    ]\n                                    }\n                        \n                            Rules:\n                                - Ensure the output is valid JSON (parseable).\n                                - "eventS" must always be an array (can be empty).\n                                - Multiple instances of the same event type appear as individual elements in the event array.\n                                - Events appear in the array in the same order in which they appear in the text.\n                                - Do not include extra keys, comments, or text.\n                                - Each object in "events" must contain "event_type", "text_quote", and "attributes".\n                                -If an event attribute type has no value mentioned, return "attributes": {"&lt; attribute name &gt;:Unknown"} for each attribute type defined for the event type \n                        \n                        \n                        \n                ---\n                Examples:\n                \n                text: "Patient ate breakfast this morning. He seems less anxious."\n                output: {\n                "events": [\n                    {\n                    "event_type": "Eating",\n                    "text_quote":"Patient ate breakfast this morning",\n                    "attributes": {"food": "breakfast", \n                                   "amount": "Unknown",\n                                   "method": "Unknown",\n                                   "time":"morning",\n                                   "caused_by":"Unknown"}\n                    }\n                ]\n                }\n                \n                text: "Patient reported severe abdominal pain."\n                output: {\n                "events": [\n                    {\n                    "event_type": "Pain",\n                    "text_quote": "severe abdominal Pain",\n                    "attributes": {"severity": "severe", \n                                   "location": "abdominal",\n                                   "duration": "Unknown",\n                                   "time":"Unknown",\n                                   "caused_by":"Unknown"}\n                    }\n                ]\n                }\n                \n                text: "Patient called his son around 3 pm."\n                output: {\n                "events": [\n                    {\n                    "event_type": "Family",\n                    "text_quote": "called his son around 3 pm",\n                    "attributes": {"interaction": "call", \n                                    "relation": "son",\n                                    "time":"3 pm",\n                                    "caused_by":"Unknown"}\n                    }\n                ]\n                }\n                \n                text: "Patient had a loose stool overnight."\n                output: {\n                "events": [\n                    {\n                    "event_type": "Excretion",\n                    "text_quote": "loose stool overnight",\n                    "attributes": {"type": "stool", \n                                   "quality": "loose", \n                                   "frequency":"overnight", \n                                   "time":"night",\n                                   "caused_by":"Unknown"}\n                    }\n                ]\n                }\n                \n                text: "Patient was able to sleep well last night."\n                output: {\n                "events": [\n                    {\n                    "event_type": "Sleep",\n                    "text_quote": "sleep well last night",\n                    "attributes": {"quality": "well",\n                                    "duration": "Unknown", \n                                    "time":"night",\n                                    "caused_by":"Unknown"}\n                    }\n                ]\n                }\n                \n                text: "The patient couldn\'t sleep due to severe pain."\n                output: {\n                "events": [\n                    {\n                    "event_type": "Sleep",\n                    "text_quote": "couldn\'t sleep",\n                    "attributes": {"quality": "poor", \n                                    "duration": "Unknown",\n                                   "time":"Unknown",\n                                   "caused_by":"Pain"}\n                    },\n                    {\n                    "event_type": "Pain",\n                    "text_quote": "severe pain",\n                    "attributes": {"severity": "severe", \n                                    "location": "Unknown", \n                                    "duration": "Unknown", \n                                   "time":"before Sleep",\n                                   "caused_by":"Unknown"}\n                    }\n                ]\n                }\n                \n                text: "The patient complained of severe back pain, was given Tylenol, but the pain persisted and he was then prescribed stronger morphine."\n                output: {\n                "events": [\n                    {\n                    "event_type": "Pain",\n                    "text_quote": "complained of severe back pain",\n                    "attributes": {"severity": "severe", \n                                    "location": "back",\n                                    "duration": "Unknown", \n                                    "time":"Unknown",\n                                    "caused_by":"Unknown"}\n                    },\n                    {\n                    "event_type": "Pain",\n                    "text_quote": "pain persisted",\n                    "attributes": {"severity": "severe", \n                                   "location": "back",\n                                   "duration": "persistent", \n                                   "time":"after Tylenol",\n                                   "caused_by":"Unknown"}\n                    }\n                ]\n                }\n                \n                        ', 'event_detection_time': 10.98690803500358}</t>
+          <t>['pain']</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
+          <t>{'text': '84 yr old c dissecting aortic aneurysm .\n\nsr c blocked beats .bp labile ranging 160 to 77 systolic.labetolol drip for short time .to have mri this pm. k, mg repleted .milrinone continues on .375.amniodarone dc iv .patient feels nauseous when bp under 110\n\nbs diminished ,7.38/32/115/20 on 6lnp\n\ntaking cl liquids,pos bs ,no stool\n\nhuo 10 to 20,creat\n\npatient restless.co low back pain some releif c tylenol and sitting on side of bed .\n\nlabile bp unexplained ,need mri to check aneurysm\n\nfollow hct,lytes\naim bp 110 to 120\nmri this pm\n\naim bp 110 to 120 sys\n\n', 'event': ['Pain', 'Eating', 'Excretion', 'Sleep'], 'event_id': ['e1', 'e2', 'e3', 'e4'], 'phrase': '', 'raw_output': '{\n  "events": [\n    {\n      "event_id": "e1",\n      "event_type": "Pain",\n      "text_quote": "low back pain some releif c tylenol and sitting on side of bed",\n      "attributes": {\n        "severity": "Unknown",\n        "location": "low back",\n        "duration": "Unknown",\n        "negation": "false",\n        "time": "Unknown",\n        "caused_by": "Unknown"\n      }\n    },\n    {\n      "event_id": "e2",\n      "event_type": "Eating",\n      "text_quote": "taking cl liquids,pos bs ,no stool",\n      "attributes": {\n        "food": "cl liquids",\n        "amount": "Unknown",\n        "method": "oral",\n        "negation": "false",\n        "time": "Unknown",\n        "caused_by": "Unknown"\n      }\n    },\n    {\n      "event_id": "e3",\n      "event_type": "Excretion",\n      "text_quote": "no stool",\n      "attributes": {\n        "type": "stool",\n        "frequency": "none",\n        "quality": "Unknown",\n        "negation": "true",\n        "time": "Unknown",\n        "caused_by": "Unknown"\n      }\n    },\n    {\n      "event_id": "e4",\n      "event_type": "Sleep",\n      "text_quote": "patient restless",\n      "attributes": {\n        "quality": "poor",\n        "duration": "Unknown",\n        "negation": "false",\n        "time": "Unknown",\n        "caused_by": "Unknown"\n      }\n    }\n  ],\n  "order": []\n}', 'attributes': [{'Pain': {'severity': 'Unknown', 'location': 'low back', 'duration': 'Unknown', 'negation': 'false', 'time': 'Unknown', 'caused_by': 'Unknown'}}, {'Eating': {'food': 'cl liquids', 'amount': 'Unknown', 'method': 'oral', 'negation': 'false', 'time': 'Unknown', 'caused_by': 'Unknown'}}, {'Excretion': {'type': 'stool', 'frequency': 'none', 'quality': 'Unknown', 'negation': 'true', 'time': 'Unknown', 'caused_by': 'Unknown'}}, {'Sleep': {'quality': 'poor', 'duration': 'Unknown', 'negation': 'false', 'time': 'Unknown', 'caused_by': 'Unknown'}}], 'orders': [[]], 'text_quotes': ['low back pain some releif c tylenol and sitting on side of bed', 'taking cl liquids,pos bs ,no stool', 'no stool', 'patient restless'], 'event_name_prompt': 'Given the text: 84 yr old c dissecting aortic aneurysm .\n\nsr c blocked beats .bp labile ranging 160 to 77 systolic.labetolol drip for short time .to have mri this pm. k, mg repleted .milrinone continues on .375.amniodarone dc iv .patient feels nauseous when bp under 110\n\nbs diminished ,7.38/32/115/20 on 6lnp\n\ntaking cl liquids,pos bs ,no stool\n\nhuo 10 to 20,creat\n\npatient restless.co low back pain some releif c tylenol and sitting on side of bed .\n\nlabile bp unexplained ,need mri to check aneurysm\n\nfollow hct,lytes\naim bp 110 to 120\nmri this pm\n\naim bp 110 to 120 sys\n\n, \n                        and the following event types with their definitions: Eating : The patient takes food into their body by mouth.\nExcretion : The patient discharges waste matter from their body.\nFamily : The patient has a visit, call, or communication with a family member.\nPain : The patient reports or shows signs of pain.\nSleep : The patient sleeps or the sleep’s quality or quantity is described.\nUnknown : choose "Unknown" if none of the other event type are applicable. \n                        ---\n                        Your task:\n                        0. Identify ALL events in the text (zero, one, or more).\n1. For each event, assign an event_type from the list above.\n2. If multiple event of same type is mentioned, assign the event_type multiple times\n3. Extract attributes for each event using ONLY the allowed attributes listed below.\n4. Use keyword evidence (Ki) ONLY if it is consistent with the text context.\n5. Output strictly valid JSON following the schema below.\n                        ---\n                        Classification Rules:\n                        - A text may contain multiple events of the same or different types.\n- Create a separate event object for each event mention.\n- If the text is explicitly a NEGATION (e.g., "denies pain"), do not extract that event.\n- If the text describes a FUTURE or HYPOTHETICAL event (e.g., "will eat tomorrow"), ignore it.\n- A valid event should have occurred in the recent past or is occurring during the time of writing of the text.\n- If no events are found or if unsure, return {"events": []}\n                        \n                        ---\n                                    Attributes allowed:\n                                    {\'Eating\': {\'food\': \'&lt;string&gt; # e.g., pancakes, porridge, etc.\', \'amount\': \'&lt;string&gt; # e.g., 1, 2 bowls, etc.\', \'method\': \'&lt;string&gt;  # e.g., oral, tube, etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, evening etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}, \'Excretion\': {\'type\': \'&lt;string&gt; # e.g., urine, stool, etc.\', \'frequency\': \'&lt;string&gt; # e.g., 2x, once, etc.\', \'quality\': \'&lt;string&gt; # e.g., loose, hard, etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, evening etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}, \'Family\': {\'interaction\': \'&lt;string&gt; # e.g., visit, call, communication, etc.\', \'relation\': \'&lt;string&gt; # e.g., mother, son, etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, evening etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}, \'Pain\': {\'severity\': \'&lt;string&gt; # e.g., mild, moderate, severe, numeric scale if present, etc.\', \'location\': \'&lt;string&gt; # e.g., right knee, head, etc.\', \'duration\': \'&lt;string&gt; # e.g., all night, 3 hours, etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, evening etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}, \'Sleep\': {\'quality\': \'&lt;string&gt; # e.g., good, poor, restless, etc.\', \'duration\': \'&lt;string&gt; # e.g., 6 hours, phrases like "all night", etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, evening etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}}\n                                    If no relevant attribute exists for an event, return an empty object {}.\n                                    \n                        \n                        ---\n                                    Keyword evidence (Ki):\n                                    Additional facts: A keyword matching algorithm without context detected keyword(s) (\'pain\',).\n                                    Use this only as a pointer. If context contradicts, ignore.\n                        ---\n                        Output Schema (strict):\n                        {\n                                    "events": [\n                                        {\n                                        "event_id": "&lt; A unique id eg.: e1 | e2 |...&gt;"\n                                        "event_type": "&lt;Pain | Sleep | Excretion | Eating | Family&gt;",\n                                        "text_quote": "&lt;fragement from the text indicating the event_type&gt;",\n                "attributes": {\n                    "&lt;attribute_name&gt;": "&lt;attribute_value&gt;"\n                }\n                                        }\n                                    ],\n                                    "order": [\n                                        ["e1", "before" | "after" | "simultaneous", "e2" ]\n                                    ]\n                                    }\n                        \n                            Rules:\n                                - Ensure the output is valid JSON (parseable).\n                                - "eventS" must always be an array (can be empty).\n                                - Multiple instances of the same event type appear with different ids.\n                                - Events appear in the array in the same order in which they appear in the text.\n                                - Their partial orders can be expressed using the "order" section.\n                                - Do not include extra keys, comments, or text.\n                                - Each object in "events" must contain "event_type", "text_quote", and "attributes".\n                                - If an event attribute type has no value mentioned, return "attributes": {"&lt; attribute name &gt;:Unknown"} for each attribute type defined for the event type \n                        \n                        \n                        \n                ---\n                Examples:\n                \n                text: "Patient ate breakfast this morning. He seems less anxious."\n                output: {\n                "events": [\n                    {"event_id": "e1",\n                    "event_type": "Eating",\n                    "text_quote":"Patient ate breakfast this morning",\n                    "attributes": {"food": "breakfast", \n                                   "amount": "Unknown",\n                                   "method": "Unknown",\n                                   "negation": "false",\n                                   "time":"morning",\n                                   "caused_by":"Unknown"}\n                    }\n                ],\n                "order":[]\n                }\n                \n                text: "Patient reported severe abdominal pain."\n                output: {\n                "events": [\n                    {"event_id": "e1",\n                    "event_type": "Pain",\n                    "text_quote": "severe abdominal Pain",\n                    "attributes": {"severity": "severe", \n                                   "location": "abdominal",\n                                   "duration": "Unknown",\n                                   "negation": "false",\n                                   "time":"Unknown",\n                                   "caused_by":"Unknown"}\n                    }\n                ],\n                "order":[]\n                }\n                \n                text: "Patient called his son around 3 pm."\n                output: {\n                "events": [\n                    {"event_id": "e1",\n                    "event_type": "Family",\n                    "text_quote": "called his son around 3 pm",\n                    "attributes": {"interaction": "call", \n                                    "relation": "son",\n                                    "negation": "false",\n                                    "time":"3 pm",\n                                    "caused_by":"Unknown"}\n                    }\n                ],\n                "order":[]\n                }\n                \n                text: "Patient had a loose stool overnight."\n                output: {\n                "events": [\n                    {"event_id": "e1",\n                    "event_type": "Excretion",\n                    "text_quote": "loose stool overnight",\n                    "attributes": {"type": "stool", \n                                   "quality": "loose", \n                                   "frequency":"overnight", \n                                   "negation": "false",\n                                   "time":"night",\n                                   "caused_by":"Unknown"}\n                    }\n                ],\n                "order":[]\n                }\n                \n                text: "Patient was able to sleep well last night."\n                output: {\n                "events": [\n                    {"event_id": "e1",\n                    "event_type": "Sleep",\n                    "text_quote": "sleep well last night",\n                    "attributes": {"quality": "well",\n                                    "duration": "Unknown", \n                                    "negation": "false",\n                                    "time":"night",\n                                    "caused_by":"Unknown"}\n                    }\n                ],\n                "order":[]\n                }\n                \n                text: "The patient couldn\'t sleep due to severe pain."\n                output: {\n                "events": [\n                    {"event_id": "e1",\n                    "event_type": "Sleep",\n                    "text_quote": "couldn\'t sleep",\n                    "attributes": {"quality": "poor", \n                                    "duration": "Unknown",\n                                    "negation": "true",\n                                    "time":"Unknown",\n                                    "caused_by":"Pain"}\n                    },\n                    {"event_id": "e2",\n                    "event_type": "Pain",\n                    "text_quote": "severe pain",\n                    "attributes": {"severity": "severe", \n                                    "location": "Unknown", \n                                    "duration": "Unknown", \n                                    "time":"Unknown",\n                                    "caused_by":"Unknown"}\n                    }\n                ],\n                "order":["e1", "after", "e2"]\n                }\n                \n                text: "The patient complained of severe back pain, was given Tylenol, but the pain persisted and he was then prescribed stronger morphine."\n                output: {\n                "events": [\n                    {"event_id": "e1",\n                    "event_type": "Pain",\n                    "text_quote": "complained of severe back pain",\n                    "attributes": {"severity": "severe", \n                                    "location": "back",\n                                    "duration": "Unknown", \n                                    "time":"Unknown",\n                                    "caused_by":"Unknown"}\n                    },\n                    {"event_id": "e2",\n                    "event_type": "Pain",\n                    "text_quote": "pain persisted",\n                    "attributes": {"severity": "severe", \n                                   "location": "back",\n                                   "duration": "persistent", \n                                   "time":"after Tylenol",\n                                   "caused_by":"Unknown"}\n                    }\n                ],\n                "order":[["e1", "before", "e2"]]\n                }\n                \n                        ', 'event_detection_time': 13.210118529968895}</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
           <t>['Pain', 'Eating', 'Excretion', 'Sleep']</t>
         </is>
       </c>
-      <c r="G7" t="inlineStr">
-        <is>
-          <t>[{'Pain': {'severity': 'Unknown', 'location': 'low back', 'duration': 'some releif', 'time': 'Unknown', 'caused_by': 'Unknown'}}, {'Eating': {'food': 'cl liquids', 'amount': 'Unknown', 'method': 'oral', 'time': 'Unknown', 'caused_by': 'Unknown'}}, {'Excretion': {'type': 'stool', 'frequency': 'none', 'quality': 'Unknown', 'time': 'Unknown', 'caused_by': 'Unknown'}}, {'Sleep': {'quality': 'restless', 'duration': 'Unknown', 'time': 'Unknown', 'caused_by': 'Unknown'}}]</t>
-        </is>
-      </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>['low back pain some releif c tylenol and sitting on side of bed', 'taking cl liquids,pos bs ,no stool', 'taking cl liquids,pos bs ,no stool', 'patient restless']</t>
+          <t>[{'Pain': {'severity': 'Unknown', 'location': 'low back', 'duration': 'Unknown', 'negation': 'false', 'time': 'Unknown', 'caused_by': 'Unknown'}}, {'Eating': {'food': 'cl liquids', 'amount': 'Unknown', 'method': 'oral', 'negation': 'false', 'time': 'Unknown', 'caused_by': 'Unknown'}}, {'Excretion': {'type': 'stool', 'frequency': 'none', 'quality': 'Unknown', 'negation': 'true', 'time': 'Unknown', 'caused_by': 'Unknown'}}, {'Sleep': {'quality': 'poor', 'duration': 'Unknown', 'negation': 'false', 'time': 'Unknown', 'caused_by': 'Unknown'}}]</t>
         </is>
       </c>
       <c r="I7" t="inlineStr">
         <is>
-          <t>{'text': '84 yr old c dissecting aortic aneurysm .\n\nsr c blocked beats .bp labile ranging 160 to 77 systolic.labetolol drip for short time .to have mri this pm. k, mg repleted .milrinone continues on .375.amniodarone dc iv .patient feels nauseous when bp under 110\n\nbs diminished ,7.38/32/115/20 on 6lnp\n\ntaking cl liquids,pos bs ,no stool\n\nhuo 10 to 20,creat\n\npatient restless.co low back pain some releif c tylenol and sitting on side of bed .\n\nlabile bp unexplained ,need mri to check aneurysm\n\nfollow hct,lytes\naim bp 110 to 120\nmri this pm\n\naim bp 110 to 120 sys\n\n', 'event': ['Pain', 'Excretion', 'Eating', 'Sleep'], 'phrase': '', 'raw_output': '{\n  "events": [\n    {\n      "event_type": "Pain",\n      "text_quote": "co low back pain some releif c tylenol and sitting on side of bed .",\n      "attributes": {\n        "severity": "Unknown",\n        "location": "low back",\n        "duration": "Unknown",\n        "negation": false,\n        "time": "Unknown",\n        "caused_by": "Unknown"\n      }\n    },\n    {\n      "event_type": "Excretion",\n      "text_quote": "taking cl liquids,pos bs ,no stool",\n      "attributes": {\n        "type": "stool",\n        "frequency": "0",\n        "quality": "Unknown",\n        "negation": true,\n        "time": "Unknown",\n        "caused_by": "Unknown"\n      }\n    },\n    {\n      "event_type": "Eating",\n      "text_quote": "taking cl liquids,pos bs ,no stool",\n      "attributes": {\n        "food": "liquids",\n        "amount": "Unknown",\n        "method": "oral",\n        "negation": false,\n        "time": "Unknown",\n        "caused_by": "Unknown"\n      }\n    },\n    {\n      "event_type": "Sleep",\n      "text_quote": "patient restless.",\n      "attributes": {\n        "quality": "restless",\n        "duration": "Unknown",\n        "negation": false,\n        "time": "Unknown",\n        "caused_by": "Unknown"\n      }\n    }\n  ]\n}', 'attributes': [{'Pain': {'severity': 'Unknown', 'location': 'low back', 'duration': 'Unknown', 'negation': False, 'time': 'Unknown', 'caused_by': 'Unknown'}}, {'Excretion': {'type': 'stool', 'frequency': '0', 'quality': 'Unknown', 'negation': True, 'time': 'Unknown', 'caused_by': 'Unknown'}}, {'Eating': {'food': 'liquids', 'amount': 'Unknown', 'method': 'oral', 'negation': False, 'time': 'Unknown', 'caused_by': 'Unknown'}}, {'Sleep': {'quality': 'restless', 'duration': 'Unknown', 'negation': False, 'time': 'Unknown', 'caused_by': 'Unknown'}}], 'text_quotes': ['co low back pain some releif c tylenol and sitting on side of bed .', 'taking cl liquids,pos bs ,no stool', 'taking cl liquids,pos bs ,no stool', 'patient restless.'], 'event_name_prompt': 'Given the text: 84 yr old c dissecting aortic aneurysm .\n\nsr c blocked beats .bp labile ranging 160 to 77 systolic.labetolol drip for short time .to have mri this pm. k, mg repleted .milrinone continues on .375.amniodarone dc iv .patient feels nauseous when bp under 110\n\nbs diminished ,7.38/32/115/20 on 6lnp\n\ntaking cl liquids,pos bs ,no stool\n\nhuo 10 to 20,creat\n\npatient restless.co low back pain some releif c tylenol and sitting on side of bed .\n\nlabile bp unexplained ,need mri to check aneurysm\n\nfollow hct,lytes\naim bp 110 to 120\nmri this pm\n\naim bp 110 to 120 sys\n\n, \n                        and the following event types with their definitions: Eating : The patient takes food into their body by mouth.\nExcretion : The patient discharges waste matter from their body.\nFamily : The patient has a visit, call, or communication with a family member.\nPain : The patient reports or shows signs of pain.\nSleep : The patient sleeps or the sleep’s quality or quantity is described.\nUnknown : choose "Unknown" if none of the other event type are applicable. \n                        ---\n                        Your task:\n                        0. Identify ALL events in the text (zero, one, or more).\n1. For each event, assign an event_type from the list above.\n2. If multiple event of same type is mentioned, assign the event_type multiple times\n3. Extract attributes for each event using ONLY the allowed attributes listed below.\n4. Use keyword evidence (Ki) ONLY if it is consistent with the text context.\n5. Output strictly valid JSON following the schema below.\n                        ---\n                        Classification Rules:\n                        - A text may contain multiple events of the same or different types.\n- Create a separate event object for each event mention.\n- If the text is explicitly a NEGATION (e.g., "denies pain"), do not extract that event.\n- If the text describes a FUTURE or HYPOTHETICAL event (e.g., "will eat tomorrow"), ignore it.\n- A valid event should have occurred in the recent past or is occurring during the time of writing of the text.\n- If no events are found or if unsure, return {"events": []}\n                        \n                        ---\n                                    Attributes allowed:\n                                    {\'Eating\': {\'food\': \'&lt;string&gt; # e.g., pancakes, porridge, etc.\', \'amount\': \'&lt;string&gt; # e.g., 1, 2 bowls, etc.\', \'method\': \'&lt;string&gt;  # e.g., oral, tube, etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, after shower, etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}, \'Excretion\': {\'type\': \'&lt;string&gt; # e.g., urine, stool, etc.\', \'frequency\': \'&lt;string&gt; # e.g., 2x, once, etc.\', \'quality\': \'&lt;string&gt; # e.g., loose, hard, etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, after shower, etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}, \'Family\': {\'interaction\': \'&lt;string&gt; # e.g., visit, call, communication, etc.\', \'relation\': \'&lt;string&gt; # e.g., mother, son, etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, after shower, etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}, \'Pain\': {\'severity\': \'&lt;string&gt; # e.g., mild, moderate, severe, numeric scale if present, etc.\', \'location\': \'&lt;string&gt; # e.g., right knee, head, etc.\', \'duration\': \'&lt;string&gt; # e.g., all night, 3 hours, etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, after shower, etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}, \'Sleep\': {\'quality\': \'&lt;string&gt; # e.g., good, poor, restless, etc.\', \'duration\': \'&lt;string&gt; # e.g., 6 hours, phrases like "all night", etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, after shower, etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}}\n                                    If no relevant attribute exists for an event, return an empty object {}.\n                                    \n                        \n                        ---\n                                    Keyword evidence (Ki):\n                                    Additional facts: A keyword matching algorithm without context detected keyword(s) [\'pain\'].\n                                    Use this only as a pointer. If context contradicts, ignore.\n                        ---\n                        Output Schema (strict):\n                        {\n                                    "events": [\n                                        {\n                                        "event_type": "&lt;Pain | Sleep | Excretion | Eating | Family&gt;",\n                                        "text_quote": "&lt;fragement from the text indicating &gt;",\n                "attributes": {\n                    "&lt;attribute_name&gt;": "&lt;attribute_value&gt;"\n                }\n                                        }\n                                    ]\n                                    }\n                        \n                            Rules:\n                                - Ensure the output is valid JSON (parseable).\n                                - "eventS" must always be an array (can be empty).\n                                - Multiple instances of the same event type appear as individual elements in the event array.\n                                - Events appear in the array in the same order in which they appear in the text.\n                                - Do not include extra keys, comments, or text.\n                                - Each object in "events" must contain "event_type", "text_quote", and "attributes".\n                                -If an event attribute type has no value mentioned, return "attributes": {"&lt; attribute name &gt;:Unknown"} for each attribute type defined for the event type \n                        \n                        \n                        \n                        ', 'event_detection_time': 10.960092339999392}</t>
+          <t>['low back pain some releif c tylenol and sitting on side of bed', 'taking cl liquids,pos bs ,no stool', 'no stool', 'patient restless']</t>
         </is>
       </c>
       <c r="J7" t="inlineStr">
         <is>
-          <t>['Pain', 'Excretion', 'Eating', 'Sleep']</t>
+          <t>[[]]</t>
         </is>
       </c>
       <c r="K7" t="inlineStr">
         <is>
-          <t>[{'Pain': {'severity': 'Unknown', 'location': 'low back', 'duration': 'Unknown', 'negation': False, 'time': 'Unknown', 'caused_by': 'Unknown'}}, {'Excretion': {'type': 'stool', 'frequency': '0', 'quality': 'Unknown', 'negation': True, 'time': 'Unknown', 'caused_by': 'Unknown'}}, {'Eating': {'food': 'liquids', 'amount': 'Unknown', 'method': 'oral', 'negation': False, 'time': 'Unknown', 'caused_by': 'Unknown'}}, {'Sleep': {'quality': 'restless', 'duration': 'Unknown', 'negation': False, 'time': 'Unknown', 'caused_by': 'Unknown'}}]</t>
+          <t>{'text': '84 yr old c dissecting aortic aneurysm .\n\nsr c blocked beats .bp labile ranging 160 to 77 systolic.labetolol drip for short time .to have mri this pm. k, mg repleted .milrinone continues on .375.amniodarone dc iv .patient feels nauseous when bp under 110\n\nbs diminished ,7.38/32/115/20 on 6lnp\n\ntaking cl liquids,pos bs ,no stool\n\nhuo 10 to 20,creat\n\npatient restless.co low back pain some releif c tylenol and sitting on side of bed .\n\nlabile bp unexplained ,need mri to check aneurysm\n\nfollow hct,lytes\naim bp 110 to 120\nmri this pm\n\naim bp 110 to 120 sys\n\n', 'event': ['Pain', 'Excretion', 'Eating', 'Pain', 'Sleep'], 'event_id': ['e1', 'e2', 'e3', 'e4', 'e5'], 'phrase': '', 'raw_output': '{\n  "events": [\n    {\n      "event_id": "e1",\n      "event_type": "Pain",\n      "text_quote": "co low back pain some releif c tylenol and sitting on side of bed .",\n      "attributes": {\n        "severity": "Unknown",\n        "location": "low back",\n        "duration": "Unknown",\n        "negation": false,\n        "time": "Unknown",\n        "caused_by": "Unknown"\n      }\n    },\n    {\n      "event_id": "e2",\n      "event_type": "Excretion",\n      "text_quote": "taking cl liquids,pos bs ,no stool",\n      "attributes": {\n        "type": "stool",\n        "frequency": "Unknown",\n        "quality": "None",\n        "negation": true,\n        "time": "Unknown",\n        "caused_by": "Unknown"\n      }\n    },\n    {\n      "event_id": "e3",\n      "event_type": "Eating",\n      "text_quote": "taking cl liquids,pos bs ,no stool",\n      "attributes": {\n        "food": "liquids",\n        "amount": "Unknown",\n        "method": "oral",\n        "negation": false,\n        "time": "Unknown",\n        "caused_by": "Unknown"\n      }\n    },\n    {\n      "event_id": "e4",\n      "event_type": "Pain",\n      "text_quote": "patient feels nauseous when bp under 110",\n      "attributes": {\n        "severity": "Unknown",\n        "location": "Unknown",\n        "duration": "Unknown",\n        "negation": false,\n        "time": "Unknown",\n        "caused_by": "bp under 110"\n      }\n    },\n    {\n      "event_id": "e5",\n      "event_type": "Sleep",\n      "text_quote": "patient restless.",\n      "attributes": {\n        "quality": "restless",\n        "duration": "Unknown",\n        "negation": false,\n        "time": "Unknown",\n        "caused_by": "Unknown"\n      }\n    }\n  ],\n  "order": [\n    ["e1", "before", "e2"],\n    ["e2", "simultaneous", "e3"],\n    ["e3", "after", "e4"],\n    ["e4", "before", "e5"]\n  ]\n}', 'attributes': [{'Pain': {'severity': 'Unknown', 'location': 'low back', 'duration': 'Unknown', 'negation': False, 'time': 'Unknown', 'caused_by': 'Unknown'}}, {'Excretion': {'type': 'stool', 'frequency': 'Unknown', 'quality': 'None', 'negation': True, 'time': 'Unknown', 'caused_by': 'Unknown'}}, {'Eating': {'food': 'liquids', 'amount': 'Unknown', 'method': 'oral', 'negation': False, 'time': 'Unknown', 'caused_by': 'Unknown'}}, {'Pain': {'severity': 'Unknown', 'location': 'Unknown', 'duration': 'Unknown', 'negation': False, 'time': 'Unknown', 'caused_by': 'bp under 110'}}, {'Sleep': {'quality': 'restless', 'duration': 'Unknown', 'negation': False, 'time': 'Unknown', 'caused_by': 'Unknown'}}], 'orders': [[['e1', 'before', 'e2'], ['e2', 'simultaneous', 'e3'], ['e3', 'after', 'e4'], ['e4', 'before', 'e5']]], 'text_quotes': ['co low back pain some releif c tylenol and sitting on side of bed .', 'taking cl liquids,pos bs ,no stool', 'taking cl liquids,pos bs ,no stool', 'patient feels nauseous when bp under 110', 'patient restless.'], 'event_name_prompt': 'Given the text: 84 yr old c dissecting aortic aneurysm .\n\nsr c blocked beats .bp labile ranging 160 to 77 systolic.labetolol drip for short time .to have mri this pm. k, mg repleted .milrinone continues on .375.amniodarone dc iv .patient feels nauseous when bp under 110\n\nbs diminished ,7.38/32/115/20 on 6lnp\n\ntaking cl liquids,pos bs ,no stool\n\nhuo 10 to 20,creat\n\npatient restless.co low back pain some releif c tylenol and sitting on side of bed .\n\nlabile bp unexplained ,need mri to check aneurysm\n\nfollow hct,lytes\naim bp 110 to 120\nmri this pm\n\naim bp 110 to 120 sys\n\n, \n                        and the following event types with their definitions: Eating : The patient takes food into their body by mouth.\nExcretion : The patient discharges waste matter from their body.\nFamily : The patient has a visit, call, or communication with a family member.\nPain : The patient reports or shows signs of pain.\nSleep : The patient sleeps or the sleep’s quality or quantity is described.\nUnknown : choose "Unknown" if none of the other event type are applicable. \n                        ---\n                        Your task:\n                        0. Identify ALL events in the text (zero, one, or more).\n1. For each event, assign an event_type from the list above.\n2. If multiple event of same type is mentioned, assign the event_type multiple times\n3. Extract attributes for each event using ONLY the allowed attributes listed below.\n4. Use keyword evidence (Ki) ONLY if it is consistent with the text context.\n5. Output strictly valid JSON following the schema below.\n                        ---\n                        Classification Rules:\n                        - A text may contain multiple events of the same or different types.\n- Create a separate event object for each event mention.\n- If the text is explicitly a NEGATION (e.g., "denies pain"), do not extract that event.\n- If the text describes a FUTURE or HYPOTHETICAL event (e.g., "will eat tomorrow"), ignore it.\n- A valid event should have occurred in the recent past or is occurring during the time of writing of the text.\n- If no events are found or if unsure, return {"events": []}\n                        \n                        ---\n                                    Attributes allowed:\n                                    {\'Eating\': {\'food\': \'&lt;string&gt; # e.g., pancakes, porridge, etc.\', \'amount\': \'&lt;string&gt; # e.g., 1, 2 bowls, etc.\', \'method\': \'&lt;string&gt;  # e.g., oral, tube, etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, evening etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}, \'Excretion\': {\'type\': \'&lt;string&gt; # e.g., urine, stool, etc.\', \'frequency\': \'&lt;string&gt; # e.g., 2x, once, etc.\', \'quality\': \'&lt;string&gt; # e.g., loose, hard, etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, evening etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}, \'Family\': {\'interaction\': \'&lt;string&gt; # e.g., visit, call, communication, etc.\', \'relation\': \'&lt;string&gt; # e.g., mother, son, etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, evening etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}, \'Pain\': {\'severity\': \'&lt;string&gt; # e.g., mild, moderate, severe, numeric scale if present, etc.\', \'location\': \'&lt;string&gt; # e.g., right knee, head, etc.\', \'duration\': \'&lt;string&gt; # e.g., all night, 3 hours, etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, evening etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}, \'Sleep\': {\'quality\': \'&lt;string&gt; # e.g., good, poor, restless, etc.\', \'duration\': \'&lt;string&gt; # e.g., 6 hours, phrases like "all night", etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, evening etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}}\n                                    If no relevant attribute exists for an event, return an empty object {}.\n                                    \n                        \n                        ---\n                                    Keyword evidence (Ki):\n                                    Additional facts: A keyword matching algorithm without context detected keyword(s) (\'pain\',).\n                                    Use this only as a pointer. If context contradicts, ignore.\n                        ---\n                        Output Schema (strict):\n                        {\n                                    "events": [\n                                        {\n                                        "event_id": "&lt; A unique id eg.: e1 | e2 |...&gt;"\n                                        "event_type": "&lt;Pain | Sleep | Excretion | Eating | Family&gt;",\n                                        "text_quote": "&lt;fragement from the text indicating the event_type&gt;",\n                "attributes": {\n                    "&lt;attribute_name&gt;": "&lt;attribute_value&gt;"\n                }\n                                        }\n                                    ],\n                                    "order": [\n                                        ["e1", "before" | "after" | "simultaneous", "e2" ]\n                                    ]\n                                    }\n                        \n                            Rules:\n                                - Ensure the output is valid JSON (parseable).\n                                - "eventS" must always be an array (can be empty).\n                                - Multiple instances of the same event type appear with different ids.\n                                - Events appear in the array in the same order in which they appear in the text.\n                                - Their partial orders can be expressed using the "order" section.\n                                - Do not include extra keys, comments, or text.\n                                - Each object in "events" must contain "event_type", "text_quote", and "attributes".\n                                - If an event attribute type has no value mentioned, return "attributes": {"&lt; attribute name &gt;:Unknown"} for each attribute type defined for the event type \n                        \n                        \n                        \n                        ', 'event_detection_time': 16.51165822701296}</t>
         </is>
       </c>
       <c r="L7" t="inlineStr">
         <is>
-          <t>['co low back pain some releif c tylenol and sitting on side of bed .', 'taking cl liquids,pos bs ,no stool', 'taking cl liquids,pos bs ,no stool', 'patient restless.']</t>
+          <t>['Pain', 'Excretion', 'Eating', 'Pain', 'Sleep']</t>
         </is>
       </c>
       <c r="M7" t="inlineStr">
         <is>
-          <t>{'text': '84 yr old c dissecting aortic aneurysm .\n\nsr c blocked beats .bp labile ranging 160 to 77 systolic.labetolol drip for short time .to have mri this pm. k, mg repleted .milrinone continues on .375.amniodarone dc iv .patient feels nauseous when bp under 110\n\nbs diminished ,7.38/32/115/20 on 6lnp\n\ntaking cl liquids,pos bs ,no stool\n\nhuo 10 to 20,creat\n\npatient restless.co low back pain some releif c tylenol and sitting on side of bed .\n\nlabile bp unexplained ,need mri to check aneurysm\n\nfollow hct,lytes\naim bp 110 to 120\nmri this pm\n\naim bp 110 to 120 sys\n\n', 'event': ['Pain', 'Eating', 'Excretion', 'Sleep'], 'phrase': '', 'raw_output': '{\n  "events": [\n    {\n      "event_type": "Pain",\n      "text_quote": "low back pain some releif c tylenol and sitting on side of bed",\n      "attributes": {\n        "severity": "Unknown",\n        "location": "low back",\n        "duration": "some releif",\n        "time": "Unknown",\n        "caused_by": "Unknown"\n      }\n    },\n    {\n      "event_type": "Eating",\n      "text_quote": "taking cl liquids,pos bs ,no stool",\n      "attributes": {\n        "food": "cl liquids",\n        "amount": "Unknown",\n        "method": "oral",\n        "time": "Unknown",\n        "caused_by": "Unknown"\n      }\n    },\n    {\n      "event_type": "Excretion",\n      "text_quote": "taking cl liquids,pos bs ,no stool",\n      "attributes": {\n        "type": "stool",\n        "frequency": "none",\n        "quality": "Unknown",\n        "time": "Unknown",\n        "caused_by": "Unknown"\n      }\n    },\n    {\n      "event_type": "Sleep",\n      "text_quote": "patient restless",\n      "attributes": {\n        "quality": "restless",\n        "duration": "Unknown",\n        "time": "Unknown",\n        "caused_by": "Unknown"\n      }\n    }\n  ]\n}', 'attributes': [{'Pain': {'severity': 'Unknown', 'location': 'low back', 'duration': 'some releif', 'time': 'Unknown', 'caused_by': 'Unknown'}}, {'Eating': {'food': 'cl liquids', 'amount': 'Unknown', 'method': 'oral', 'time': 'Unknown', 'caused_by': 'Unknown'}}, {'Excretion': {'type': 'stool', 'frequency': 'none', 'quality': 'Unknown', 'time': 'Unknown', 'caused_by': 'Unknown'}}, {'Sleep': {'quality': 'restless', 'duration': 'Unknown', 'time': 'Unknown', 'caused_by': 'Unknown'}}], 'text_quotes': ['low back pain some releif c tylenol and sitting on side of bed', 'taking cl liquids,pos bs ,no stool', 'taking cl liquids,pos bs ,no stool', 'patient restless'], 'event_name_prompt': 'Given the text: 84 yr old c dissecting aortic aneurysm .\n\nsr c blocked beats .bp labile ranging 160 to 77 systolic.labetolol drip for short time .to have mri this pm. k, mg repleted .milrinone continues on .375.amniodarone dc iv .patient feels nauseous when bp under 110\n\nbs diminished ,7.38/32/115/20 on 6lnp\n\ntaking cl liquids,pos bs ,no stool\n\nhuo 10 to 20,creat\n\npatient restless.co low back pain some releif c tylenol and sitting on side of bed .\n\nlabile bp unexplained ,need mri to check aneurysm\n\nfollow hct,lytes\naim bp 110 to 120\nmri this pm\n\naim bp 110 to 120 sys\n\n, \n                        and the following event types with their definitions: Eating : The patient takes food into their body by mouth.\nExcretion : The patient discharges waste matter from their body.\nFamily : The patient has a visit, call, or communication with a family member.\nPain : The patient reports or shows signs of pain.\nSleep : The patient sleeps or the sleep’s quality or quantity is described.\nUnknown : choose "Unknown" if none of the other event type are applicable. \n                        ---\n                        Your task:\n                        0. Identify ALL events in the text (zero, one, or more).\n1. For each event, assign an event_type from the list above.\n2. If multiple event of same type is mentioned, assign the event_type multiple times\n3. Extract attributes for each event using ONLY the allowed attributes listed below.\n4. Output strictly valid JSON following the schema below.\n                        ---\n                        Classification Rules:\n                        - A text may contain multiple events of the same or different types.\n- Create a separate event object for each event mention.\n- If the text is explicitly a NEGATION (e.g., "denies pain"), do not extract that event.\n- If the text describes a FUTURE or HYPOTHETICAL event (e.g., "will eat tomorrow"), ignore it.\n- A valid event should have occurred in the recent past or is occurring during the time of writing of the text.\n- If no events are found or if unsure, return {"events": []}\n                        \n                        ---\n                                    Attributes allowed:\n                                    {\'Eating\': {\'food\': \'&lt;string&gt; # e.g., pancakes, porridge, etc.\', \'amount\': \'&lt;string&gt; # e.g., 1, 2 bowls, etc.\', \'method\': \'&lt;string&gt;  # e.g., oral, tube, etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, after shower, etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}, \'Excretion\': {\'type\': \'&lt;string&gt; # e.g., urine, stool, etc.\', \'frequency\': \'&lt;string&gt; # e.g., 2x, once, etc.\', \'quality\': \'&lt;string&gt; # e.g., loose, hard, etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, after shower, etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}, \'Family\': {\'interaction\': \'&lt;string&gt; # e.g., visit, call, communication, etc.\', \'relation\': \'&lt;string&gt; # e.g., mother, son, etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, after shower, etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}, \'Pain\': {\'severity\': \'&lt;string&gt; # e.g., mild, moderate, severe, numeric scale if present, etc.\', \'location\': \'&lt;string&gt; # e.g., right knee, head, etc.\', \'duration\': \'&lt;string&gt; # e.g., all night, 3 hours, etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, after shower, etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}, \'Sleep\': {\'quality\': \'&lt;string&gt; # e.g., good, poor, restless, etc.\', \'duration\': \'&lt;string&gt; # e.g., 6 hours, phrases like "all night", etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, after shower, etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}}\n                                    If no relevant attribute exists for an event, return an empty object {}.\n                                    \n                        \n                        \n                        ---\n                        Output Schema (strict):\n                        {\n                                    "events": [\n                                        {\n                                        "event_type": "&lt;Pain | Sleep | Excretion | Eating | Family&gt;",\n                                        "text_quote": "&lt;fragement from the text indicating &gt;",\n                "attributes": {\n                    "&lt;attribute_name&gt;": "&lt;attribute_value&gt;"\n                }\n                                        }\n                                    ]\n                                    }\n                        \n                            Rules:\n                                - Ensure the output is valid JSON (parseable).\n                                - "eventS" must always be an array (can be empty).\n                                - Multiple instances of the same event type appear as individual elements in the event array.\n                                - Events appear in the array in the same order in which they appear in the text.\n                                - Do not include extra keys, comments, or text.\n                                - Each object in "events" must contain "event_type", "text_quote", and "attributes".\n                                -If an event attribute type has no value mentioned, return "attributes": {"&lt; attribute name &gt;:Unknown"} for each attribute type defined for the event type \n                        \n                        \n                        \n                ---\n                Examples:\n                \n                text: "Patient ate breakfast this morning. He seems less anxious."\n                output: {\n                "events": [\n                    {\n                    "event_type": "Eating",\n                    "text_quote":"Patient ate breakfast this morning",\n                    "attributes": {"food": "breakfast", \n                                   "amount": "Unknown",\n                                   "method": "Unknown",\n                                   "time":"morning",\n                                   "caused_by":"Unknown"}\n                    }\n                ]\n                }\n                \n                text: "Patient reported severe abdominal pain."\n                output: {\n                "events": [\n                    {\n                    "event_type": "Pain",\n                    "text_quote": "severe abdominal Pain",\n                    "attributes": {"severity": "severe", \n                                   "location": "abdominal",\n                                   "duration": "Unknown",\n                                   "time":"Unknown",\n                                   "caused_by":"Unknown"}\n                    }\n                ]\n                }\n                \n                text: "Patient called his son around 3 pm."\n                output: {\n                "events": [\n                    {\n                    "event_type": "Family",\n                    "text_quote": "called his son around 3 pm",\n                    "attributes": {"interaction": "call", \n                                    "relation": "son",\n                                    "time":"3 pm",\n                                    "caused_by":"Unknown"}\n                    }\n                ]\n                }\n                \n                text: "Patient had a loose stool overnight."\n                output: {\n                "events": [\n                    {\n                    "event_type": "Excretion",\n                    "text_quote": "loose stool overnight",\n                    "attributes": {"type": "stool", \n                                   "quality": "loose", \n                                   "frequency":"overnight", \n                                   "time":"night",\n                                   "caused_by":"Unknown"}\n                    }\n                ]\n                }\n                \n                text: "Patient was able to sleep well last night."\n                output: {\n                "events": [\n                    {\n                    "event_type": "Sleep",\n                    "text_quote": "sleep well last night",\n                    "attributes": {"quality": "well",\n                                    "duration": "Unknown", \n                                    "time":"night",\n                                    "caused_by":"Unknown"}\n                    }\n                ]\n                }\n                \n                text: "The patient couldn\'t sleep due to severe pain."\n                output: {\n                "events": [\n                    {\n                    "event_type": "Sleep",\n                    "text_quote": "couldn\'t sleep",\n                    "attributes": {"quality": "poor", \n                                    "duration": "Unknown",\n                                   "time":"Unknown",\n                                   "caused_by":"Pain"}\n                    },\n                    {\n                    "event_type": "Pain",\n                    "text_quote": "severe pain",\n                    "attributes": {"severity": "severe", \n                                    "location": "Unknown", \n                                    "duration": "Unknown", \n                                   "time":"before Sleep",\n                                   "caused_by":"Unknown"}\n                    }\n                ]\n                }\n                \n                text: "The patient complained of severe back pain, was given Tylenol, but the pain persisted and he was then prescribed stronger morphine."\n                output: {\n                "events": [\n                    {\n                    "event_type": "Pain",\n                    "text_quote": "complained of severe back pain",\n                    "attributes": {"severity": "severe", \n                                    "location": "back",\n                                    "duration": "Unknown", \n                                    "time":"Unknown",\n                                    "caused_by":"Unknown"}\n                    },\n                    {\n                    "event_type": "Pain",\n                    "text_quote": "pain persisted",\n                    "attributes": {"severity": "severe", \n                                   "location": "back",\n                                   "duration": "persistent", \n                                   "time":"after Tylenol",\n                                   "caused_by":"Unknown"}\n                    }\n                ]\n                }\n                \n                        ', 'event_detection_time': 10.875866931004566}</t>
+          <t>[{'Pain': {'severity': 'Unknown', 'location': 'low back', 'duration': 'Unknown', 'negation': False, 'time': 'Unknown', 'caused_by': 'Unknown'}}, {'Excretion': {'type': 'stool', 'frequency': 'Unknown', 'quality': 'None', 'negation': True, 'time': 'Unknown', 'caused_by': 'Unknown'}}, {'Eating': {'food': 'liquids', 'amount': 'Unknown', 'method': 'oral', 'negation': False, 'time': 'Unknown', 'caused_by': 'Unknown'}}, {'Pain': {'severity': 'Unknown', 'location': 'Unknown', 'duration': 'Unknown', 'negation': False, 'time': 'Unknown', 'caused_by': 'bp under 110'}}, {'Sleep': {'quality': 'restless', 'duration': 'Unknown', 'negation': False, 'time': 'Unknown', 'caused_by': 'Unknown'}}]</t>
         </is>
       </c>
       <c r="N7" t="inlineStr">
         <is>
-          <t>['Pain', 'Eating', 'Excretion', 'Sleep']</t>
+          <t>['co low back pain some releif c tylenol and sitting on side of bed .', 'taking cl liquids,pos bs ,no stool', 'taking cl liquids,pos bs ,no stool', 'patient feels nauseous when bp under 110', 'patient restless.']</t>
         </is>
       </c>
       <c r="O7" t="inlineStr">
         <is>
-          <t>[{'Pain': {'severity': 'Unknown', 'location': 'low back', 'duration': 'some releif', 'time': 'Unknown', 'caused_by': 'Unknown'}}, {'Eating': {'food': 'cl liquids', 'amount': 'Unknown', 'method': 'oral', 'time': 'Unknown', 'caused_by': 'Unknown'}}, {'Excretion': {'type': 'stool', 'frequency': 'none', 'quality': 'Unknown', 'time': 'Unknown', 'caused_by': 'Unknown'}}, {'Sleep': {'quality': 'restless', 'duration': 'Unknown', 'time': 'Unknown', 'caused_by': 'Unknown'}}]</t>
-        </is>
-      </c>
-      <c r="P7" t="inlineStr">
-        <is>
-          <t>['low back pain some releif c tylenol and sitting on side of bed', 'taking cl liquids,pos bs ,no stool', 'taking cl liquids,pos bs ,no stool', 'patient restless']</t>
-        </is>
-      </c>
-      <c r="Q7" t="n">
-        <v>0.002961268999570166</v>
-      </c>
-      <c r="R7" t="inlineStr">
+          <t>[[['e1', 'before', 'e2'], ['e2', 'simultaneous', 'e3'], ['e3', 'after', 'e4'], ['e4', 'before', 'e5']]]</t>
+        </is>
+      </c>
+      <c r="P7" t="n">
+        <v>0.002378008000960108</v>
+      </c>
+      <c r="Q7" t="inlineStr">
         <is>
           <t>Sleep</t>
         </is>
       </c>
-      <c r="S7" t="b">
+      <c r="R7" t="b">
+        <v>0</v>
+      </c>
+      <c r="S7" t="n">
         <v>0</v>
       </c>
       <c r="T7" t="n">
         <v>0</v>
       </c>
-      <c r="U7" t="n">
-        <v>0</v>
-      </c>
-      <c r="V7" t="inlineStr">
+      <c r="U7" t="inlineStr">
         <is>
           <t>('pain',)</t>
         </is>
       </c>
+      <c r="V7" t="n">
+        <v>13.2101185299689</v>
+      </c>
       <c r="W7" t="n">
-        <v>10.98690803500358</v>
+        <v>16.51165822701296</v>
       </c>
       <c r="X7" t="n">
-        <v>10.96009233999939</v>
+        <v>0</v>
       </c>
       <c r="Y7" t="n">
-        <v>10.87586693100457</v>
+        <v>1</v>
       </c>
       <c r="Z7" t="n">
-        <v>0</v>
-      </c>
-      <c r="AA7" t="n">
-        <v>1</v>
-      </c>
-      <c r="AB7" t="n">
-        <v>1</v>
-      </c>
-      <c r="AC7" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8" t="n">
-        <v>1310484</v>
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>1310484</t>
+        </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>['Sleep', 'Excretion', 'Pain', 'Unknown']</t>
+          <t>('Pain', 'Sleep', 'Unknown', 'Excretion')</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>['asleep', 'sleep', 'urine', 'pain']</t>
+          <t>('pain', 'urine', 'sleep', 'asleep')</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
@@ -1431,120 +1366,111 @@
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>{'text': 'ccu npn 7p-7a\ns: "its just like in the army, hurry up and wait"\no: see carevue and update for complete assessment data\n\ncv: diastolic blood pressure labile, transiently on labetalol for bp 150s, ranging 79-150/, down significantly when asleep but patient. awakens easily and is coherent, map &gt;60, md aware, cont to closely monitor. c/o mild back pain, per patient. tolerable. assists with turning, sits @ bedside. heart rate 60s-70s nsr, no ectopy. dps/pts weak palp and verified by dopplar, radial pulses palp. hct stable @ 38, am labs pending. awaiting mri abdomen to eval extension of dissection, ? involvement of renal arteries\n\nresp: no c/o sob, breathing comfortably on 6l nc with spo2 94-97%. rr 18-24. ls clear @ apices, diminished with occasional scattered rales @ bases r&gt;l.\n\ngi/gu: abd soft, nontender, nondistended. +bs, -bm. tol pos and meds. foley draining minimal amts clear amber urine, 15-40cc/heart rate, +725cc yesterday. am bun/cr pending.\n\nid: afebrile, tmax 99.0 pr. wbc 8\n\nneruo: a&amp;ox3, easliy arousable despite low bp, appropriately discouraged re: lack of sleep but otherwise pleasant.\n\na: 84yo with h/o type a dissection, repaired in \'[**77**], admitted now with type b dissection extending to bifurcation and ? renal artery involvement; hosp. course c/b cardiogenic shock (ci 1.7, ^ 2.9 with milrinone), arf and labile bp.\np: follow up am labs, q12hr hct, monitor pain, mri abdomen. labetalol/pressors to maintain diastolic blood pressure 100-120.\n', 'event': ['Pain', 'Sleep', 'Excretion'], 'phrase': '', 'raw_output': '{\n  "events": [\n    {\n      "event_type": "Pain",\n      "text_quote": "c/o mild back pain, per patient. tolerable.",\n      "attributes": {\n        "severity": "mild",\n        "location": "back",\n        "duration": "Unknown",\n        "time": "Unknown",\n        "caused_by": "Unknown"\n      }\n    },\n    {\n      "event_type": "Sleep",\n      "text_quote": "awakens easily and is coherent, map &gt;60, md aware, cont to closely monitor. down significantly when asleep but patient.",\n      "attributes": {\n        "quality": "Unknown",\n        "duration": "Unknown",\n        "time": "Unknown",\n        "caused_by": "Unknown"\n      }\n    },\n    {\n      "event_type": "Excretion",\n      "text_quote": "foley draining minimal amts clear amber urine, 15-40cc/heart rate, +725cc yesterday.",\n      "attributes": {\n        "type": "urine",\n        "frequency": "minimal",\n        "quality": "clear amber",\n        "time": "Unknown",\n        "caused_by": "Unknown"\n      }\n    }\n  ]\n}', 'attributes': [{'Pain': {'severity': 'mild', 'location': 'back', 'duration': 'Unknown', 'time': 'Unknown', 'caused_by': 'Unknown'}}, {'Sleep': {'quality': 'Unknown', 'duration': 'Unknown', 'time': 'Unknown', 'caused_by': 'Unknown'}}, {'Excretion': {'type': 'urine', 'frequency': 'minimal', 'quality': 'clear amber', 'time': 'Unknown', 'caused_by': 'Unknown'}}], 'text_quotes': ['c/o mild back pain, per patient. tolerable.', 'awakens easily and is coherent, map &gt;60, md aware, cont to closely monitor. down significantly when asleep but patient.', 'foley draining minimal amts clear amber urine, 15-40cc/heart rate, +725cc yesterday.'], 'event_name_prompt': 'Given the text: ccu npn 7p-7a\ns: "its just like in the army, hurry up and wait"\no: see carevue and update for complete assessment data\n\ncv: diastolic blood pressure labile, transiently on labetalol for bp 150s, ranging 79-150/, down significantly when asleep but patient. awakens easily and is coherent, map &gt;60, md aware, cont to closely monitor. c/o mild back pain, per patient. tolerable. assists with turning, sits @ bedside. heart rate 60s-70s nsr, no ectopy. dps/pts weak palp and verified by dopplar, radial pulses palp. hct stable @ 38, am labs pending. awaiting mri abdomen to eval extension of dissection, ? involvement of renal arteries\n\nresp: no c/o sob, breathing comfortably on 6l nc with spo2 94-97%. rr 18-24. ls clear @ apices, diminished with occasional scattered rales @ bases r&gt;l.\n\ngi/gu: abd soft, nontender, nondistended. +bs, -bm. tol pos and meds. foley draining minimal amts clear amber urine, 15-40cc/heart rate, +725cc yesterday. am bun/cr pending.\n\nid: afebrile, tmax 99.0 pr. wbc 8\n\nneruo: a&amp;ox3, easliy arousable despite low bp, appropriately discouraged re: lack of sleep but otherwise pleasant.\n\na: 84yo with h/o type a dissection, repaired in \'[**77**], admitted now with type b dissection extending to bifurcation and ? renal artery involvement; hosp. course c/b cardiogenic shock (ci 1.7, ^ 2.9 with milrinone), arf and labile bp.\np: follow up am labs, q12hr hct, monitor pain, mri abdomen. labetalol/pressors to maintain diastolic blood pressure 100-120.\n, \n                        and the following event types with their definitions: Eating : The patient takes food into their body by mouth.\nExcretion : The patient discharges waste matter from their body.\nFamily : The patient has a visit, call, or communication with a family member.\nPain : The patient reports or shows signs of pain.\nSleep : The patient sleeps or the sleep’s quality or quantity is described.\nUnknown : choose "Unknown" if none of the other event type are applicable. \n                        ---\n                        Your task:\n                        0. Identify ALL events in the text (zero, one, or more).\n1. For each event, assign an event_type from the list above.\n2. If multiple event of same type is mentioned, assign the event_type multiple times\n3. Extract attributes for each event using ONLY the allowed attributes listed below.\n4. Use keyword evidence (Ki) ONLY if it is consistent with the text context.\n5. Output strictly valid JSON following the schema below.\n                        ---\n                        Classification Rules:\n                        - A text may contain multiple events of the same or different types.\n- Create a separate event object for each event mention.\n- If the text is explicitly a NEGATION (e.g., "denies pain"), do not extract that event.\n- If the text describes a FUTURE or HYPOTHETICAL event (e.g., "will eat tomorrow"), ignore it.\n- A valid event should have occurred in the recent past or is occurring during the time of writing of the text.\n- If no events are found or if unsure, return {"events": []}\n                        \n                        ---\n                                    Attributes allowed:\n                                    {\'Eating\': {\'food\': \'&lt;string&gt; # e.g., pancakes, porridge, etc.\', \'amount\': \'&lt;string&gt; # e.g., 1, 2 bowls, etc.\', \'method\': \'&lt;string&gt;  # e.g., oral, tube, etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, after shower, etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}, \'Excretion\': {\'type\': \'&lt;string&gt; # e.g., urine, stool, etc.\', \'frequency\': \'&lt;string&gt; # e.g., 2x, once, etc.\', \'quality\': \'&lt;string&gt; # e.g., loose, hard, etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, after shower, etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}, \'Family\': {\'interaction\': \'&lt;string&gt; # e.g., visit, call, communication, etc.\', \'relation\': \'&lt;string&gt; # e.g., mother, son, etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, after shower, etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}, \'Pain\': {\'severity\': \'&lt;string&gt; # e.g., mild, moderate, severe, numeric scale if present, etc.\', \'location\': \'&lt;string&gt; # e.g., right knee, head, etc.\', \'duration\': \'&lt;string&gt; # e.g., all night, 3 hours, etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, after shower, etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}, \'Sleep\': {\'quality\': \'&lt;string&gt; # e.g., good, poor, restless, etc.\', \'duration\': \'&lt;string&gt; # e.g., 6 hours, phrases like "all night", etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, after shower, etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}}\n                                    If no relevant attribute exists for an event, return an empty object {}.\n                                    \n                        \n                        ---\n                                    Keyword evidence (Ki):\n                                    Additional facts: A keyword matching algorithm without context detected keyword(s) [\'asleep\', \'sleep\', \'urine\', \'pain\'].\n                                    Use this only as a pointer. If context contradicts, ignore.\n                        ---\n                        Output Schema (strict):\n                        {\n                                    "events": [\n                                        {\n                                        "event_type": "&lt;Pain | Sleep | Excretion | Eating | Family&gt;",\n                                        "text_quote": "&lt;fragement from the text indicating &gt;",\n                "attributes": {\n                    "&lt;attribute_name&gt;": "&lt;attribute_value&gt;"\n                }\n                                        }\n                                    ]\n                                    }\n                        \n                            Rules:\n                                - Ensure the output is valid JSON (parseable).\n                                - "eventS" must always be an array (can be empty).\n                                - Multiple instances of the same event type appear as individual elements in the event array.\n                                - Events appear in the array in the same order in which they appear in the text.\n                                - Do not include extra keys, comments, or text.\n                                - Each object in "events" must contain "event_type", "text_quote", and "attributes".\n                                -If an event attribute type has no value mentioned, return "attributes": {"&lt; attribute name &gt;:Unknown"} for each attribute type defined for the event type \n                        \n                        \n                        \n                ---\n                Examples:\n                \n                text: "Patient ate breakfast this morning. He seems less anxious."\n                output: {\n                "events": [\n                    {\n                    "event_type": "Eating",\n                    "text_quote":"Patient ate breakfast this morning",\n                    "attributes": {"food": "breakfast", \n                                   "amount": "Unknown",\n                                   "method": "Unknown",\n                                   "time":"morning",\n                                   "caused_by":"Unknown"}\n                    }\n                ]\n                }\n                \n                text: "Patient reported severe abdominal pain."\n                output: {\n                "events": [\n                    {\n                    "event_type": "Pain",\n                    "text_quote": "severe abdominal Pain",\n                    "attributes": {"severity": "severe", \n                                   "location": "abdominal",\n                                   "duration": "Unknown",\n                                   "time":"Unknown",\n                                   "caused_by":"Unknown"}\n                    }\n                ]\n                }\n                \n                text: "Patient called his son around 3 pm."\n                output: {\n                "events": [\n                    {\n                    "event_type": "Family",\n                    "text_quote": "called his son around 3 pm",\n                    "attributes": {"interaction": "call", \n                                    "relation": "son",\n                                    "time":"3 pm",\n                                    "caused_by":"Unknown"}\n                    }\n                ]\n                }\n                \n                text: "Patient had a loose stool overnight."\n                output: {\n                "events": [\n                    {\n                    "event_type": "Excretion",\n                    "text_quote": "loose stool overnight",\n                    "attributes": {"type": "stool", \n                                   "quality": "loose", \n                                   "frequency":"overnight", \n                                   "time":"night",\n                                   "caused_by":"Unknown"}\n                    }\n                ]\n                }\n                \n                text: "Patient was able to sleep well last night."\n                output: {\n                "events": [\n                    {\n                    "event_type": "Sleep",\n                    "text_quote": "sleep well last night",\n                    "attributes": {"quality": "well",\n                                    "duration": "Unknown", \n                                    "time":"night",\n                                    "caused_by":"Unknown"}\n                    }\n                ]\n                }\n                \n                text: "The patient couldn\'t sleep due to severe pain."\n                output: {\n                "events": [\n                    {\n                    "event_type": "Sleep",\n                    "text_quote": "couldn\'t sleep",\n                    "attributes": {"quality": "poor", \n                                    "duration": "Unknown",\n                                   "time":"Unknown",\n                                   "caused_by":"Pain"}\n                    },\n                    {\n                    "event_type": "Pain",\n                    "text_quote": "severe pain",\n                    "attributes": {"severity": "severe", \n                                    "location": "Unknown", \n                                    "duration": "Unknown", \n                                   "time":"before Sleep",\n                                   "caused_by":"Unknown"}\n                    }\n                ]\n                }\n                \n                text: "The patient complained of severe back pain, was given Tylenol, but the pain persisted and he was then prescribed stronger morphine."\n                output: {\n                "events": [\n                    {\n                    "event_type": "Pain",\n                    "text_quote": "complained of severe back pain",\n                    "attributes": {"severity": "severe", \n                                    "location": "back",\n                                    "duration": "Unknown", \n                                    "time":"Unknown",\n                                    "caused_by":"Unknown"}\n                    },\n                    {\n                    "event_type": "Pain",\n                    "text_quote": "pain persisted",\n                    "attributes": {"severity": "severe", \n                                   "location": "back",\n                                   "duration": "persistent", \n                                   "time":"after Tylenol",\n                                   "caused_by":"Unknown"}\n                    }\n                ]\n                }\n                \n                        ', 'event_detection_time': 10.067598346999148}</t>
+          <t>['pain', 'urine', 'sleep', 'asleep']</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
+          <t>{'text': 'ccu npn 7p-7a\ns: "its just like in the army, hurry up and wait"\no: see carevue and update for complete assessment data\n\ncv: diastolic blood pressure labile, transiently on labetalol for bp 150s, ranging 79-150/, down significantly when asleep but patient. awakens easily and is coherent, map &gt;60, md aware, cont to closely monitor. c/o mild back pain, per patient. tolerable. assists with turning, sits @ bedside. heart rate 60s-70s nsr, no ectopy. dps/pts weak palp and verified by dopplar, radial pulses palp. hct stable @ 38, am labs pending. awaiting mri abdomen to eval extension of dissection, ? involvement of renal arteries\n\nresp: no c/o sob, breathing comfortably on 6l nc with spo2 94-97%. rr 18-24. ls clear @ apices, diminished with occasional scattered rales @ bases r&gt;l.\n\ngi/gu: abd soft, nontender, nondistended. +bs, -bm. tol pos and meds. foley draining minimal amts clear amber urine, 15-40cc/heart rate, +725cc yesterday. am bun/cr pending.\n\nid: afebrile, tmax 99.0 pr. wbc 8\n\nneruo: a&amp;ox3, easliy arousable despite low bp, appropriately discouraged re: lack of sleep but otherwise pleasant.\n\na: 84yo with h/o type a dissection, repaired in \'[**77**], admitted now with type b dissection extending to bifurcation and ? renal artery involvement; hosp. course c/b cardiogenic shock (ci 1.7, ^ 2.9 with milrinone), arf and labile bp.\np: follow up am labs, q12hr hct, monitor pain, mri abdomen. labetalol/pressors to maintain diastolic blood pressure 100-120.\n', 'event': ['Pain', 'Sleep', 'Excretion'], 'event_id': ['e1', 'e2', 'e3'], 'phrase': '', 'raw_output': '{\n  "events": [\n    {\n      "event_id": "e1",\n      "event_type": "Pain",\n      "text_quote": "c/o mild back pain, per patient. tolerable.",\n      "attributes": {\n        "severity": "mild",\n        "location": "back",\n        "duration": "Unknown",\n        "negation": "false",\n        "time": "Unknown",\n        "caused_by": "Unknown"\n      }\n    },\n    {\n      "event_id": "e2",\n      "event_type": "Sleep",\n      "text_quote": "awakens easily and is coherent, map &gt;60, md aware, cont to closely monitor. down significantly when asleep but patient.",\n      "attributes": {\n        "quality": "Unknown",\n        "duration": "Unknown",\n        "negation": "false",\n        "time": "asleep",\n        "caused_by": "Unknown"\n      }\n    },\n    {\n      "event_id": "e3",\n      "event_type": "Excretion",\n      "text_quote": "foley draining minimal amts clear amber urine, 15-40cc/heart rate, +725cc yesterday.",\n      "attributes": {\n        "type": "urine",\n        "frequency": "minimal",\n        "quality": "clear amber",\n        "negation": "false",\n        "time": "Unknown",\n        "caused_by": "Unknown"\n      }\n    }\n  ],\n  "order": []\n}', 'attributes': [{'Pain': {'severity': 'mild', 'location': 'back', 'duration': 'Unknown', 'negation': 'false', 'time': 'Unknown', 'caused_by': 'Unknown'}}, {'Sleep': {'quality': 'Unknown', 'duration': 'Unknown', 'negation': 'false', 'time': 'asleep', 'caused_by': 'Unknown'}}, {'Excretion': {'type': 'urine', 'frequency': 'minimal', 'quality': 'clear amber', 'negation': 'false', 'time': 'Unknown', 'caused_by': 'Unknown'}}], 'orders': [[]], 'text_quotes': ['c/o mild back pain, per patient. tolerable.', 'awakens easily and is coherent, map &gt;60, md aware, cont to closely monitor. down significantly when asleep but patient.', 'foley draining minimal amts clear amber urine, 15-40cc/heart rate, +725cc yesterday.'], 'event_name_prompt': 'Given the text: ccu npn 7p-7a\ns: "its just like in the army, hurry up and wait"\no: see carevue and update for complete assessment data\n\ncv: diastolic blood pressure labile, transiently on labetalol for bp 150s, ranging 79-150/, down significantly when asleep but patient. awakens easily and is coherent, map &gt;60, md aware, cont to closely monitor. c/o mild back pain, per patient. tolerable. assists with turning, sits @ bedside. heart rate 60s-70s nsr, no ectopy. dps/pts weak palp and verified by dopplar, radial pulses palp. hct stable @ 38, am labs pending. awaiting mri abdomen to eval extension of dissection, ? involvement of renal arteries\n\nresp: no c/o sob, breathing comfortably on 6l nc with spo2 94-97%. rr 18-24. ls clear @ apices, diminished with occasional scattered rales @ bases r&gt;l.\n\ngi/gu: abd soft, nontender, nondistended. +bs, -bm. tol pos and meds. foley draining minimal amts clear amber urine, 15-40cc/heart rate, +725cc yesterday. am bun/cr pending.\n\nid: afebrile, tmax 99.0 pr. wbc 8\n\nneruo: a&amp;ox3, easliy arousable despite low bp, appropriately discouraged re: lack of sleep but otherwise pleasant.\n\na: 84yo with h/o type a dissection, repaired in \'[**77**], admitted now with type b dissection extending to bifurcation and ? renal artery involvement; hosp. course c/b cardiogenic shock (ci 1.7, ^ 2.9 with milrinone), arf and labile bp.\np: follow up am labs, q12hr hct, monitor pain, mri abdomen. labetalol/pressors to maintain diastolic blood pressure 100-120.\n, \n                        and the following event types with their definitions: Eating : The patient takes food into their body by mouth.\nExcretion : The patient discharges waste matter from their body.\nFamily : The patient has a visit, call, or communication with a family member.\nPain : The patient reports or shows signs of pain.\nSleep : The patient sleeps or the sleep’s quality or quantity is described.\nUnknown : choose "Unknown" if none of the other event type are applicable. \n                        ---\n                        Your task:\n                        0. Identify ALL events in the text (zero, one, or more).\n1. For each event, assign an event_type from the list above.\n2. If multiple event of same type is mentioned, assign the event_type multiple times\n3. Extract attributes for each event using ONLY the allowed attributes listed below.\n4. Use keyword evidence (Ki) ONLY if it is consistent with the text context.\n5. Output strictly valid JSON following the schema below.\n                        ---\n                        Classification Rules:\n                        - A text may contain multiple events of the same or different types.\n- Create a separate event object for each event mention.\n- If the text is explicitly a NEGATION (e.g., "denies pain"), do not extract that event.\n- If the text describes a FUTURE or HYPOTHETICAL event (e.g., "will eat tomorrow"), ignore it.\n- A valid event should have occurred in the recent past or is occurring during the time of writing of the text.\n- If no events are found or if unsure, return {"events": []}\n                        \n                        ---\n                                    Attributes allowed:\n                                    {\'Eating\': {\'food\': \'&lt;string&gt; # e.g., pancakes, porridge, etc.\', \'amount\': \'&lt;string&gt; # e.g., 1, 2 bowls, etc.\', \'method\': \'&lt;string&gt;  # e.g., oral, tube, etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, evening etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}, \'Excretion\': {\'type\': \'&lt;string&gt; # e.g., urine, stool, etc.\', \'frequency\': \'&lt;string&gt; # e.g., 2x, once, etc.\', \'quality\': \'&lt;string&gt; # e.g., loose, hard, etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, evening etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}, \'Family\': {\'interaction\': \'&lt;string&gt; # e.g., visit, call, communication, etc.\', \'relation\': \'&lt;string&gt; # e.g., mother, son, etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, evening etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}, \'Pain\': {\'severity\': \'&lt;string&gt; # e.g., mild, moderate, severe, numeric scale if present, etc.\', \'location\': \'&lt;string&gt; # e.g., right knee, head, etc.\', \'duration\': \'&lt;string&gt; # e.g., all night, 3 hours, etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, evening etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}, \'Sleep\': {\'quality\': \'&lt;string&gt; # e.g., good, poor, restless, etc.\', \'duration\': \'&lt;string&gt; # e.g., 6 hours, phrases like "all night", etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, evening etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}}\n                                    If no relevant attribute exists for an event, return an empty object {}.\n                                    \n                        \n                        ---\n                                    Keyword evidence (Ki):\n                                    Additional facts: A keyword matching algorithm without context detected keyword(s) (\'pain\', \'urine\', \'sleep\', \'asleep\').\n                                    Use this only as a pointer. If context contradicts, ignore.\n                        ---\n                        Output Schema (strict):\n                        {\n                                    "events": [\n                                        {\n                                        "event_id": "&lt; A unique id eg.: e1 | e2 |...&gt;"\n                                        "event_type": "&lt;Pain | Sleep | Excretion | Eating | Family&gt;",\n                                        "text_quote": "&lt;fragement from the text indicating the event_type&gt;",\n                "attributes": {\n                    "&lt;attribute_name&gt;": "&lt;attribute_value&gt;"\n                }\n                                        }\n                                    ],\n                                    "order": [\n                                        ["e1", "before" | "after" | "simultaneous", "e2" ]\n                                    ]\n                                    }\n                        \n                            Rules:\n                                - Ensure the output is valid JSON (parseable).\n                                - "eventS" must always be an array (can be empty).\n                                - Multiple instances of the same event type appear with different ids.\n                                - Events appear in the array in the same order in which they appear in the text.\n                                - Their partial orders can be expressed using the "order" section.\n                                - Do not include extra keys, comments, or text.\n                                - Each object in "events" must contain "event_type", "text_quote", and "attributes".\n                                - If an event attribute type has no value mentioned, return "attributes": {"&lt; attribute name &gt;:Unknown"} for each attribute type defined for the event type \n                        \n                        \n                        \n                ---\n                Examples:\n                \n                text: "Patient ate breakfast this morning. He seems less anxious."\n                output: {\n                "events": [\n                    {"event_id": "e1",\n                    "event_type": "Eating",\n                    "text_quote":"Patient ate breakfast this morning",\n                    "attributes": {"food": "breakfast", \n                                   "amount": "Unknown",\n                                   "method": "Unknown",\n                                   "negation": "false",\n                                   "time":"morning",\n                                   "caused_by":"Unknown"}\n                    }\n                ],\n                "order":[]\n                }\n                \n                text: "Patient reported severe abdominal pain."\n                output: {\n                "events": [\n                    {"event_id": "e1",\n                    "event_type": "Pain",\n                    "text_quote": "severe abdominal Pain",\n                    "attributes": {"severity": "severe", \n                                   "location": "abdominal",\n                                   "duration": "Unknown",\n                                   "negation": "false",\n                                   "time":"Unknown",\n                                   "caused_by":"Unknown"}\n                    }\n                ],\n                "order":[]\n                }\n                \n                text: "Patient called his son around 3 pm."\n                output: {\n                "events": [\n                    {"event_id": "e1",\n                    "event_type": "Family",\n                    "text_quote": "called his son around 3 pm",\n                    "attributes": {"interaction": "call", \n                                    "relation": "son",\n                                    "negation": "false",\n                                    "time":"3 pm",\n                                    "caused_by":"Unknown"}\n                    }\n                ],\n                "order":[]\n                }\n                \n                text: "Patient had a loose stool overnight."\n                output: {\n                "events": [\n                    {"event_id": "e1",\n                    "event_type": "Excretion",\n                    "text_quote": "loose stool overnight",\n                    "attributes": {"type": "stool", \n                                   "quality": "loose", \n                                   "frequency":"overnight", \n                                   "negation": "false",\n                                   "time":"night",\n                                   "caused_by":"Unknown"}\n                    }\n                ],\n                "order":[]\n                }\n                \n                text: "Patient was able to sleep well last night."\n                output: {\n                "events": [\n                    {"event_id": "e1",\n                    "event_type": "Sleep",\n                    "text_quote": "sleep well last night",\n                    "attributes": {"quality": "well",\n                                    "duration": "Unknown", \n                                    "negation": "false",\n                                    "time":"night",\n                                    "caused_by":"Unknown"}\n                    }\n                ],\n                "order":[]\n                }\n                \n                text: "The patient couldn\'t sleep due to severe pain."\n                output: {\n                "events": [\n                    {"event_id": "e1",\n                    "event_type": "Sleep",\n                    "text_quote": "couldn\'t sleep",\n                    "attributes": {"quality": "poor", \n                                    "duration": "Unknown",\n                                    "negation": "true",\n                                    "time":"Unknown",\n                                    "caused_by":"Pain"}\n                    },\n                    {"event_id": "e2",\n                    "event_type": "Pain",\n                    "text_quote": "severe pain",\n                    "attributes": {"severity": "severe", \n                                    "location": "Unknown", \n                                    "duration": "Unknown", \n                                    "time":"Unknown",\n                                    "caused_by":"Unknown"}\n                    }\n                ],\n                "order":["e1", "after", "e2"]\n                }\n                \n                text: "The patient complained of severe back pain, was given Tylenol, but the pain persisted and he was then prescribed stronger morphine."\n                output: {\n                "events": [\n                    {"event_id": "e1",\n                    "event_type": "Pain",\n                    "text_quote": "complained of severe back pain",\n                    "attributes": {"severity": "severe", \n                                    "location": "back",\n                                    "duration": "Unknown", \n                                    "time":"Unknown",\n                                    "caused_by":"Unknown"}\n                    },\n                    {"event_id": "e2",\n                    "event_type": "Pain",\n                    "text_quote": "pain persisted",\n                    "attributes": {"severity": "severe", \n                                   "location": "back",\n                                   "duration": "persistent", \n                                   "time":"after Tylenol",\n                                   "caused_by":"Unknown"}\n                    }\n                ],\n                "order":[["e1", "before", "e2"]]\n                }\n                \n                        ', 'event_detection_time': 12.070597011013888}</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
           <t>['Pain', 'Sleep', 'Excretion']</t>
         </is>
       </c>
-      <c r="G8" t="inlineStr">
-        <is>
-          <t>[{'Pain': {'severity': 'mild', 'location': 'back', 'duration': 'Unknown', 'time': 'Unknown', 'caused_by': 'Unknown'}}, {'Sleep': {'quality': 'Unknown', 'duration': 'Unknown', 'time': 'Unknown', 'caused_by': 'Unknown'}}, {'Excretion': {'type': 'urine', 'frequency': 'minimal', 'quality': 'clear amber', 'time': 'Unknown', 'caused_by': 'Unknown'}}]</t>
-        </is>
-      </c>
       <c r="H8" t="inlineStr">
         <is>
+          <t>[{'Pain': {'severity': 'mild', 'location': 'back', 'duration': 'Unknown', 'negation': 'false', 'time': 'Unknown', 'caused_by': 'Unknown'}}, {'Sleep': {'quality': 'Unknown', 'duration': 'Unknown', 'negation': 'false', 'time': 'asleep', 'caused_by': 'Unknown'}}, {'Excretion': {'type': 'urine', 'frequency': 'minimal', 'quality': 'clear amber', 'negation': 'false', 'time': 'Unknown', 'caused_by': 'Unknown'}}]</t>
+        </is>
+      </c>
+      <c r="I8" t="inlineStr">
+        <is>
           <t>['c/o mild back pain, per patient. tolerable.', 'awakens easily and is coherent, map &gt;60, md aware, cont to closely monitor. down significantly when asleep but patient.', 'foley draining minimal amts clear amber urine, 15-40cc/heart rate, +725cc yesterday.']</t>
         </is>
       </c>
-      <c r="I8" t="inlineStr">
-        <is>
-          <t>{'text': 'ccu npn 7p-7a\ns: "its just like in the army, hurry up and wait"\no: see carevue and update for complete assessment data\n\ncv: diastolic blood pressure labile, transiently on labetalol for bp 150s, ranging 79-150/, down significantly when asleep but patient. awakens easily and is coherent, map &gt;60, md aware, cont to closely monitor. c/o mild back pain, per patient. tolerable. assists with turning, sits @ bedside. heart rate 60s-70s nsr, no ectopy. dps/pts weak palp and verified by dopplar, radial pulses palp. hct stable @ 38, am labs pending. awaiting mri abdomen to eval extension of dissection, ? involvement of renal arteries\n\nresp: no c/o sob, breathing comfortably on 6l nc with spo2 94-97%. rr 18-24. ls clear @ apices, diminished with occasional scattered rales @ bases r&gt;l.\n\ngi/gu: abd soft, nontender, nondistended. +bs, -bm. tol pos and meds. foley draining minimal amts clear amber urine, 15-40cc/heart rate, +725cc yesterday. am bun/cr pending.\n\nid: afebrile, tmax 99.0 pr. wbc 8\n\nneruo: a&amp;ox3, easliy arousable despite low bp, appropriately discouraged re: lack of sleep but otherwise pleasant.\n\na: 84yo with h/o type a dissection, repaired in \'[**77**], admitted now with type b dissection extending to bifurcation and ? renal artery involvement; hosp. course c/b cardiogenic shock (ci 1.7, ^ 2.9 with milrinone), arf and labile bp.\np: follow up am labs, q12hr hct, monitor pain, mri abdomen. labetalol/pressors to maintain diastolic blood pressure 100-120.\n', 'event': ['Pain', 'Sleep', 'Excretion', 'Sleep'], 'phrase': '', 'raw_output': '{\n  "events": [\n    {\n      "event_type": "Pain",\n      "text_quote": "c/o mild back pain, per patient. tolerable.",\n      "attributes": {\n        "severity": "mild",\n        "location": "back",\n        "duration": "Unknown",\n        "negation": false,\n        "time": "Unknown",\n        "caused_by": "Unknown"\n      }\n    },\n    {\n      "event_type": "Sleep",\n      "text_quote": "awakens easily and is coherent, map &gt;60, md aware, cont to closely monitor. down significantly when asleep but patient.",\n      "attributes": {\n        "quality": "Unknown",\n        "duration": "Unknown",\n        "negation": false,\n        "time": "Unknown",\n        "caused_by": "Unknown"\n      }\n    },\n    {\n      "event_type": "Excretion",\n      "text_quote": "foley draining minimal amts clear amber urine, 15-40cc/heart rate, +725cc yesterday.",\n      "attributes": {\n        "type": "urine",\n        "frequency": "Unknown",\n        "quality": "clear amber",\n        "negation": false,\n        "time": "yesterday",\n        "caused_by": "Unknown"\n      }\n    },\n    {\n      "event_type": "Sleep",\n      "text_quote": "appropriately discouraged re: lack of sleep but otherwise pleasant.",\n      "attributes": {\n        "quality": "poor",\n        "duration": "Unknown",\n        "negation": false,\n        "time": "Unknown",\n        "caused_by": "Unknown"\n      }\n    }\n  ]\n}', 'attributes': [{'Pain': {'severity': 'mild', 'location': 'back', 'duration': 'Unknown', 'negation': False, 'time': 'Unknown', 'caused_by': 'Unknown'}}, {'Sleep': {'quality': 'Unknown', 'duration': 'Unknown', 'negation': False, 'time': 'Unknown', 'caused_by': 'Unknown'}}, {'Excretion': {'type': 'urine', 'frequency': 'Unknown', 'quality': 'clear amber', 'negation': False, 'time': 'yesterday', 'caused_by': 'Unknown'}}, {'Sleep': {'quality': 'poor', 'duration': 'Unknown', 'negation': False, 'time': 'Unknown', 'caused_by': 'Unknown'}}], 'text_quotes': ['c/o mild back pain, per patient. tolerable.', 'awakens easily and is coherent, map &gt;60, md aware, cont to closely monitor. down significantly when asleep but patient.', 'foley draining minimal amts clear amber urine, 15-40cc/heart rate, +725cc yesterday.', 'appropriately discouraged re: lack of sleep but otherwise pleasant.'], 'event_name_prompt': 'Given the text: ccu npn 7p-7a\ns: "its just like in the army, hurry up and wait"\no: see carevue and update for complete assessment data\n\ncv: diastolic blood pressure labile, transiently on labetalol for bp 150s, ranging 79-150/, down significantly when asleep but patient. awakens easily and is coherent, map &gt;60, md aware, cont to closely monitor. c/o mild back pain, per patient. tolerable. assists with turning, sits @ bedside. heart rate 60s-70s nsr, no ectopy. dps/pts weak palp and verified by dopplar, radial pulses palp. hct stable @ 38, am labs pending. awaiting mri abdomen to eval extension of dissection, ? involvement of renal arteries\n\nresp: no c/o sob, breathing comfortably on 6l nc with spo2 94-97%. rr 18-24. ls clear @ apices, diminished with occasional scattered rales @ bases r&gt;l.\n\ngi/gu: abd soft, nontender, nondistended. +bs, -bm. tol pos and meds. foley draining minimal amts clear amber urine, 15-40cc/heart rate, +725cc yesterday. am bun/cr pending.\n\nid: afebrile, tmax 99.0 pr. wbc 8\n\nneruo: a&amp;ox3, easliy arousable despite low bp, appropriately discouraged re: lack of sleep but otherwise pleasant.\n\na: 84yo with h/o type a dissection, repaired in \'[**77**], admitted now with type b dissection extending to bifurcation and ? renal artery involvement; hosp. course c/b cardiogenic shock (ci 1.7, ^ 2.9 with milrinone), arf and labile bp.\np: follow up am labs, q12hr hct, monitor pain, mri abdomen. labetalol/pressors to maintain diastolic blood pressure 100-120.\n, \n                        and the following event types with their definitions: Eating : The patient takes food into their body by mouth.\nExcretion : The patient discharges waste matter from their body.\nFamily : The patient has a visit, call, or communication with a family member.\nPain : The patient reports or shows signs of pain.\nSleep : The patient sleeps or the sleep’s quality or quantity is described.\nUnknown : choose "Unknown" if none of the other event type are applicable. \n                        ---\n                        Your task:\n                        0. Identify ALL events in the text (zero, one, or more).\n1. For each event, assign an event_type from the list above.\n2. If multiple event of same type is mentioned, assign the event_type multiple times\n3. Extract attributes for each event using ONLY the allowed attributes listed below.\n4. Use keyword evidence (Ki) ONLY if it is consistent with the text context.\n5. Output strictly valid JSON following the schema below.\n                        ---\n                        Classification Rules:\n                        - A text may contain multiple events of the same or different types.\n- Create a separate event object for each event mention.\n- If the text is explicitly a NEGATION (e.g., "denies pain"), do not extract that event.\n- If the text describes a FUTURE or HYPOTHETICAL event (e.g., "will eat tomorrow"), ignore it.\n- A valid event should have occurred in the recent past or is occurring during the time of writing of the text.\n- If no events are found or if unsure, return {"events": []}\n                        \n                        ---\n                                    Attributes allowed:\n                                    {\'Eating\': {\'food\': \'&lt;string&gt; # e.g., pancakes, porridge, etc.\', \'amount\': \'&lt;string&gt; # e.g., 1, 2 bowls, etc.\', \'method\': \'&lt;string&gt;  # e.g., oral, tube, etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, after shower, etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}, \'Excretion\': {\'type\': \'&lt;string&gt; # e.g., urine, stool, etc.\', \'frequency\': \'&lt;string&gt; # e.g., 2x, once, etc.\', \'quality\': \'&lt;string&gt; # e.g., loose, hard, etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, after shower, etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}, \'Family\': {\'interaction\': \'&lt;string&gt; # e.g., visit, call, communication, etc.\', \'relation\': \'&lt;string&gt; # e.g., mother, son, etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, after shower, etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}, \'Pain\': {\'severity\': \'&lt;string&gt; # e.g., mild, moderate, severe, numeric scale if present, etc.\', \'location\': \'&lt;string&gt; # e.g., right knee, head, etc.\', \'duration\': \'&lt;string&gt; # e.g., all night, 3 hours, etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, after shower, etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}, \'Sleep\': {\'quality\': \'&lt;string&gt; # e.g., good, poor, restless, etc.\', \'duration\': \'&lt;string&gt; # e.g., 6 hours, phrases like "all night", etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, after shower, etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}}\n                                    If no relevant attribute exists for an event, return an empty object {}.\n                                    \n                        \n                        ---\n                                    Keyword evidence (Ki):\n                                    Additional facts: A keyword matching algorithm without context detected keyword(s) [\'asleep\', \'sleep\', \'urine\', \'pain\'].\n                                    Use this only as a pointer. If context contradicts, ignore.\n                        ---\n                        Output Schema (strict):\n                        {\n                                    "events": [\n                                        {\n                                        "event_type": "&lt;Pain | Sleep | Excretion | Eating | Family&gt;",\n                                        "text_quote": "&lt;fragement from the text indicating &gt;",\n                "attributes": {\n                    "&lt;attribute_name&gt;": "&lt;attribute_value&gt;"\n                }\n                                        }\n                                    ]\n                                    }\n                        \n                            Rules:\n                                - Ensure the output is valid JSON (parseable).\n                                - "eventS" must always be an array (can be empty).\n                                - Multiple instances of the same event type appear as individual elements in the event array.\n                                - Events appear in the array in the same order in which they appear in the text.\n                                - Do not include extra keys, comments, or text.\n                                - Each object in "events" must contain "event_type", "text_quote", and "attributes".\n                                -If an event attribute type has no value mentioned, return "attributes": {"&lt; attribute name &gt;:Unknown"} for each attribute type defined for the event type \n                        \n                        \n                        \n                        ', 'event_detection_time': 12.072494338004617}</t>
-        </is>
-      </c>
       <c r="J8" t="inlineStr">
         <is>
+          <t>[[]]</t>
+        </is>
+      </c>
+      <c r="K8" t="inlineStr">
+        <is>
+          <t>{'text': 'ccu npn 7p-7a\ns: "its just like in the army, hurry up and wait"\no: see carevue and update for complete assessment data\n\ncv: diastolic blood pressure labile, transiently on labetalol for bp 150s, ranging 79-150/, down significantly when asleep but patient. awakens easily and is coherent, map &gt;60, md aware, cont to closely monitor. c/o mild back pain, per patient. tolerable. assists with turning, sits @ bedside. heart rate 60s-70s nsr, no ectopy. dps/pts weak palp and verified by dopplar, radial pulses palp. hct stable @ 38, am labs pending. awaiting mri abdomen to eval extension of dissection, ? involvement of renal arteries\n\nresp: no c/o sob, breathing comfortably on 6l nc with spo2 94-97%. rr 18-24. ls clear @ apices, diminished with occasional scattered rales @ bases r&gt;l.\n\ngi/gu: abd soft, nontender, nondistended. +bs, -bm. tol pos and meds. foley draining minimal amts clear amber urine, 15-40cc/heart rate, +725cc yesterday. am bun/cr pending.\n\nid: afebrile, tmax 99.0 pr. wbc 8\n\nneruo: a&amp;ox3, easliy arousable despite low bp, appropriately discouraged re: lack of sleep but otherwise pleasant.\n\na: 84yo with h/o type a dissection, repaired in \'[**77**], admitted now with type b dissection extending to bifurcation and ? renal artery involvement; hosp. course c/b cardiogenic shock (ci 1.7, ^ 2.9 with milrinone), arf and labile bp.\np: follow up am labs, q12hr hct, monitor pain, mri abdomen. labetalol/pressors to maintain diastolic blood pressure 100-120.\n', 'event': ['Pain', 'Sleep', 'Excretion', 'Sleep'], 'event_id': ['e1', 'e2', 'e3', 'e4'], 'phrase': '', 'raw_output': '{\n  "events": [\n    {\n      "event_id": "e1",\n      "event_type": "Pain",\n      "text_quote": "c/o mild back pain, per patient. tolerable.",\n      "attributes": {\n        "severity": "mild",\n        "location": "back",\n        "duration": "Unknown",\n        "negation": false,\n        "time": "Unknown",\n        "caused_by": "Unknown"\n      }\n    },\n    {\n      "event_id": "e2",\n      "event_type": "Sleep",\n      "text_quote": "down significantly when asleep but patient. awakens easily and is coherent, map &gt;60, md aware, cont to closely monitor.",\n      "attributes": {\n        "quality": "Unknown",\n        "duration": "Unknown",\n        "negation": false,\n        "time": "Unknown",\n        "caused_by": "Unknown"\n      }\n    },\n    {\n      "event_id": "e3",\n      "event_type": "Excretion",\n      "text_quote": "foley draining minimal amts clear amber urine, 15-40cc/heart rate, +725cc yesterday.",\n      "attributes": {\n        "type": "urine",\n        "frequency": "Unknown",\n        "quality": "clear amber",\n        "negation": false,\n        "time": "yesterday",\n        "caused_by": "Unknown"\n      }\n    },\n    {\n      "event_id": "e4",\n      "event_type": "Sleep",\n      "text_quote": "appropriately discouraged re: lack of sleep but otherwise pleasant.",\n      "attributes": {\n        "quality": "poor",\n        "duration": "Unknown",\n        "negation": false,\n        "time": "Unknown",\n        "caused_by": "Unknown"\n      }\n    }\n  ],\n  "order": [\n    ["e1", "before", "e2"],\n    ["e2", "before", "e3"],\n    ["e3", "before", "e4"]\n  ]\n}', 'attributes': [{'Pain': {'severity': 'mild', 'location': 'back', 'duration': 'Unknown', 'negation': False, 'time': 'Unknown', 'caused_by': 'Unknown'}}, {'Sleep': {'quality': 'Unknown', 'duration': 'Unknown', 'negation': False, 'time': 'Unknown', 'caused_by': 'Unknown'}}, {'Excretion': {'type': 'urine', 'frequency': 'Unknown', 'quality': 'clear amber', 'negation': False, 'time': 'yesterday', 'caused_by': 'Unknown'}}, {'Sleep': {'quality': 'poor', 'duration': 'Unknown', 'negation': False, 'time': 'Unknown', 'caused_by': 'Unknown'}}], 'orders': [[['e1', 'before', 'e2'], ['e2', 'before', 'e3'], ['e3', 'before', 'e4']]], 'text_quotes': ['c/o mild back pain, per patient. tolerable.', 'down significantly when asleep but patient. awakens easily and is coherent, map &gt;60, md aware, cont to closely monitor.', 'foley draining minimal amts clear amber urine, 15-40cc/heart rate, +725cc yesterday.', 'appropriately discouraged re: lack of sleep but otherwise pleasant.'], 'event_name_prompt': 'Given the text: ccu npn 7p-7a\ns: "its just like in the army, hurry up and wait"\no: see carevue and update for complete assessment data\n\ncv: diastolic blood pressure labile, transiently on labetalol for bp 150s, ranging 79-150/, down significantly when asleep but patient. awakens easily and is coherent, map &gt;60, md aware, cont to closely monitor. c/o mild back pain, per patient. tolerable. assists with turning, sits @ bedside. heart rate 60s-70s nsr, no ectopy. dps/pts weak palp and verified by dopplar, radial pulses palp. hct stable @ 38, am labs pending. awaiting mri abdomen to eval extension of dissection, ? involvement of renal arteries\n\nresp: no c/o sob, breathing comfortably on 6l nc with spo2 94-97%. rr 18-24. ls clear @ apices, diminished with occasional scattered rales @ bases r&gt;l.\n\ngi/gu: abd soft, nontender, nondistended. +bs, -bm. tol pos and meds. foley draining minimal amts clear amber urine, 15-40cc/heart rate, +725cc yesterday. am bun/cr pending.\n\nid: afebrile, tmax 99.0 pr. wbc 8\n\nneruo: a&amp;ox3, easliy arousable despite low bp, appropriately discouraged re: lack of sleep but otherwise pleasant.\n\na: 84yo with h/o type a dissection, repaired in \'[**77**], admitted now with type b dissection extending to bifurcation and ? renal artery involvement; hosp. course c/b cardiogenic shock (ci 1.7, ^ 2.9 with milrinone), arf and labile bp.\np: follow up am labs, q12hr hct, monitor pain, mri abdomen. labetalol/pressors to maintain diastolic blood pressure 100-120.\n, \n                        and the following event types with their definitions: Eating : The patient takes food into their body by mouth.\nExcretion : The patient discharges waste matter from their body.\nFamily : The patient has a visit, call, or communication with a family member.\nPain : The patient reports or shows signs of pain.\nSleep : The patient sleeps or the sleep’s quality or quantity is described.\nUnknown : choose "Unknown" if none of the other event type are applicable. \n                        ---\n                        Your task:\n                        0. Identify ALL events in the text (zero, one, or more).\n1. For each event, assign an event_type from the list above.\n2. If multiple event of same type is mentioned, assign the event_type multiple times\n3. Extract attributes for each event using ONLY the allowed attributes listed below.\n4. Use keyword evidence (Ki) ONLY if it is consistent with the text context.\n5. Output strictly valid JSON following the schema below.\n                        ---\n                        Classification Rules:\n                        - A text may contain multiple events of the same or different types.\n- Create a separate event object for each event mention.\n- If the text is explicitly a NEGATION (e.g., "denies pain"), do not extract that event.\n- If the text describes a FUTURE or HYPOTHETICAL event (e.g., "will eat tomorrow"), ignore it.\n- A valid event should have occurred in the recent past or is occurring during the time of writing of the text.\n- If no events are found or if unsure, return {"events": []}\n                        \n                        ---\n                                    Attributes allowed:\n                                    {\'Eating\': {\'food\': \'&lt;string&gt; # e.g., pancakes, porridge, etc.\', \'amount\': \'&lt;string&gt; # e.g., 1, 2 bowls, etc.\', \'method\': \'&lt;string&gt;  # e.g., oral, tube, etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, evening etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}, \'Excretion\': {\'type\': \'&lt;string&gt; # e.g., urine, stool, etc.\', \'frequency\': \'&lt;string&gt; # e.g., 2x, once, etc.\', \'quality\': \'&lt;string&gt; # e.g., loose, hard, etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, evening etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}, \'Family\': {\'interaction\': \'&lt;string&gt; # e.g., visit, call, communication, etc.\', \'relation\': \'&lt;string&gt; # e.g., mother, son, etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, evening etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}, \'Pain\': {\'severity\': \'&lt;string&gt; # e.g., mild, moderate, severe, numeric scale if present, etc.\', \'location\': \'&lt;string&gt; # e.g., right knee, head, etc.\', \'duration\': \'&lt;string&gt; # e.g., all night, 3 hours, etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, evening etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}, \'Sleep\': {\'quality\': \'&lt;string&gt; # e.g., good, poor, restless, etc.\', \'duration\': \'&lt;string&gt; # e.g., 6 hours, phrases like "all night", etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, evening etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}}\n                                    If no relevant attribute exists for an event, return an empty object {}.\n                                    \n                        \n                        ---\n                                    Keyword evidence (Ki):\n                                    Additional facts: A keyword matching algorithm without context detected keyword(s) (\'pain\', \'urine\', \'sleep\', \'asleep\').\n                                    Use this only as a pointer. If context contradicts, ignore.\n                        ---\n                        Output Schema (strict):\n                        {\n                                    "events": [\n                                        {\n                                        "event_id": "&lt; A unique id eg.: e1 | e2 |...&gt;"\n                                        "event_type": "&lt;Pain | Sleep | Excretion | Eating | Family&gt;",\n                                        "text_quote": "&lt;fragement from the text indicating the event_type&gt;",\n                "attributes": {\n                    "&lt;attribute_name&gt;": "&lt;attribute_value&gt;"\n                }\n                                        }\n                                    ],\n                                    "order": [\n                                        ["e1", "before" | "after" | "simultaneous", "e2" ]\n                                    ]\n                                    }\n                        \n                            Rules:\n                                - Ensure the output is valid JSON (parseable).\n                                - "eventS" must always be an array (can be empty).\n                                - Multiple instances of the same event type appear with different ids.\n                                - Events appear in the array in the same order in which they appear in the text.\n                                - Their partial orders can be expressed using the "order" section.\n                                - Do not include extra keys, comments, or text.\n                                - Each object in "events" must contain "event_type", "text_quote", and "attributes".\n                                - If an event attribute type has no value mentioned, return "attributes": {"&lt; attribute name &gt;:Unknown"} for each attribute type defined for the event type \n                        \n                        \n                        \n                        ', 'event_detection_time': 14.451204492012039}</t>
+        </is>
+      </c>
+      <c r="L8" t="inlineStr">
+        <is>
           <t>['Pain', 'Sleep', 'Excretion', 'Sleep']</t>
         </is>
       </c>
-      <c r="K8" t="inlineStr">
+      <c r="M8" t="inlineStr">
         <is>
           <t>[{'Pain': {'severity': 'mild', 'location': 'back', 'duration': 'Unknown', 'negation': False, 'time': 'Unknown', 'caused_by': 'Unknown'}}, {'Sleep': {'quality': 'Unknown', 'duration': 'Unknown', 'negation': False, 'time': 'Unknown', 'caused_by': 'Unknown'}}, {'Excretion': {'type': 'urine', 'frequency': 'Unknown', 'quality': 'clear amber', 'negation': False, 'time': 'yesterday', 'caused_by': 'Unknown'}}, {'Sleep': {'quality': 'poor', 'duration': 'Unknown', 'negation': False, 'time': 'Unknown', 'caused_by': 'Unknown'}}]</t>
         </is>
       </c>
-      <c r="L8" t="inlineStr">
-        <is>
-          <t>['c/o mild back pain, per patient. tolerable.', 'awakens easily and is coherent, map &gt;60, md aware, cont to closely monitor. down significantly when asleep but patient.', 'foley draining minimal amts clear amber urine, 15-40cc/heart rate, +725cc yesterday.', 'appropriately discouraged re: lack of sleep but otherwise pleasant.']</t>
-        </is>
-      </c>
-      <c r="M8" t="inlineStr">
-        <is>
-          <t>{'text': 'ccu npn 7p-7a\ns: "its just like in the army, hurry up and wait"\no: see carevue and update for complete assessment data\n\ncv: diastolic blood pressure labile, transiently on labetalol for bp 150s, ranging 79-150/, down significantly when asleep but patient. awakens easily and is coherent, map &gt;60, md aware, cont to closely monitor. c/o mild back pain, per patient. tolerable. assists with turning, sits @ bedside. heart rate 60s-70s nsr, no ectopy. dps/pts weak palp and verified by dopplar, radial pulses palp. hct stable @ 38, am labs pending. awaiting mri abdomen to eval extension of dissection, ? involvement of renal arteries\n\nresp: no c/o sob, breathing comfortably on 6l nc with spo2 94-97%. rr 18-24. ls clear @ apices, diminished with occasional scattered rales @ bases r&gt;l.\n\ngi/gu: abd soft, nontender, nondistended. +bs, -bm. tol pos and meds. foley draining minimal amts clear amber urine, 15-40cc/heart rate, +725cc yesterday. am bun/cr pending.\n\nid: afebrile, tmax 99.0 pr. wbc 8\n\nneruo: a&amp;ox3, easliy arousable despite low bp, appropriately discouraged re: lack of sleep but otherwise pleasant.\n\na: 84yo with h/o type a dissection, repaired in \'[**77**], admitted now with type b dissection extending to bifurcation and ? renal artery involvement; hosp. course c/b cardiogenic shock (ci 1.7, ^ 2.9 with milrinone), arf and labile bp.\np: follow up am labs, q12hr hct, monitor pain, mri abdomen. labetalol/pressors to maintain diastolic blood pressure 100-120.\n', 'event': ['Pain', 'Sleep', 'Excretion'], 'phrase': '', 'raw_output': '{\n  "events": [\n    {\n      "event_type": "Pain",\n      "text_quote": "c/o mild back pain, per patient. tolerable.",\n      "attributes": {\n        "severity": "mild",\n        "location": "back",\n        "duration": "Unknown",\n        "time": "Unknown",\n        "caused_by": "Unknown"\n      }\n    },\n    {\n      "event_type": "Sleep",\n      "text_quote": "down significantly when asleep but patient. awakens easily and is coherent",\n      "attributes": {\n        "quality": "good",\n        "duration": "Unknown",\n        "time": "Unknown",\n        "caused_by": "Unknown"\n      }\n    },\n    {\n      "event_type": "Excretion",\n      "text_quote": "foley draining minimal amts clear amber urine, 15-40cc/heart rate, +725cc yesterday.",\n      "attributes": {\n        "type": "urine",\n        "frequency": "minimal",\n        "quality": "clear amber",\n        "time": "Unknown",\n        "caused_by": "Unknown"\n      }\n    }\n  ]\n}', 'attributes': [{'Pain': {'severity': 'mild', 'location': 'back', 'duration': 'Unknown', 'time': 'Unknown', 'caused_by': 'Unknown'}}, {'Sleep': {'quality': 'good', 'duration': 'Unknown', 'time': 'Unknown', 'caused_by': 'Unknown'}}, {'Excretion': {'type': 'urine', 'frequency': 'minimal', 'quality': 'clear amber', 'time': 'Unknown', 'caused_by': 'Unknown'}}], 'text_quotes': ['c/o mild back pain, per patient. tolerable.', 'down significantly when asleep but patient. awakens easily and is coherent', 'foley draining minimal amts clear amber urine, 15-40cc/heart rate, +725cc yesterday.'], 'event_name_prompt': 'Given the text: ccu npn 7p-7a\ns: "its just like in the army, hurry up and wait"\no: see carevue and update for complete assessment data\n\ncv: diastolic blood pressure labile, transiently on labetalol for bp 150s, ranging 79-150/, down significantly when asleep but patient. awakens easily and is coherent, map &gt;60, md aware, cont to closely monitor. c/o mild back pain, per patient. tolerable. assists with turning, sits @ bedside. heart rate 60s-70s nsr, no ectopy. dps/pts weak palp and verified by dopplar, radial pulses palp. hct stable @ 38, am labs pending. awaiting mri abdomen to eval extension of dissection, ? involvement of renal arteries\n\nresp: no c/o sob, breathing comfortably on 6l nc with spo2 94-97%. rr 18-24. ls clear @ apices, diminished with occasional scattered rales @ bases r&gt;l.\n\ngi/gu: abd soft, nontender, nondistended. +bs, -bm. tol pos and meds. foley draining minimal amts clear amber urine, 15-40cc/heart rate, +725cc yesterday. am bun/cr pending.\n\nid: afebrile, tmax 99.0 pr. wbc 8\n\nneruo: a&amp;ox3, easliy arousable despite low bp, appropriately discouraged re: lack of sleep but otherwise pleasant.\n\na: 84yo with h/o type a dissection, repaired in \'[**77**], admitted now with type b dissection extending to bifurcation and ? renal artery involvement; hosp. course c/b cardiogenic shock (ci 1.7, ^ 2.9 with milrinone), arf and labile bp.\np: follow up am labs, q12hr hct, monitor pain, mri abdomen. labetalol/pressors to maintain diastolic blood pressure 100-120.\n, \n                        and the following event types with their definitions: Eating : The patient takes food into their body by mouth.\nExcretion : The patient discharges waste matter from their body.\nFamily : The patient has a visit, call, or communication with a family member.\nPain : The patient reports or shows signs of pain.\nSleep : The patient sleeps or the sleep’s quality or quantity is described.\nUnknown : choose "Unknown" if none of the other event type are applicable. \n                        ---\n                        Your task:\n                        0. Identify ALL events in the text (zero, one, or more).\n1. For each event, assign an event_type from the list above.\n2. If multiple event of same type is mentioned, assign the event_type multiple times\n3. Extract attributes for each event using ONLY the allowed attributes listed below.\n4. Output strictly valid JSON following the schema below.\n                        ---\n                        Classification Rules:\n                        - A text may contain multiple events of the same or different types.\n- Create a separate event object for each event mention.\n- If the text is explicitly a NEGATION (e.g., "denies pain"), do not extract that event.\n- If the text describes a FUTURE or HYPOTHETICAL event (e.g., "will eat tomorrow"), ignore it.\n- A valid event should have occurred in the recent past or is occurring during the time of writing of the text.\n- If no events are found or if unsure, return {"events": []}\n                        \n                        ---\n                                    Attributes allowed:\n                                    {\'Eating\': {\'food\': \'&lt;string&gt; # e.g., pancakes, porridge, etc.\', \'amount\': \'&lt;string&gt; # e.g., 1, 2 bowls, etc.\', \'method\': \'&lt;string&gt;  # e.g., oral, tube, etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, after shower, etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}, \'Excretion\': {\'type\': \'&lt;string&gt; # e.g., urine, stool, etc.\', \'frequency\': \'&lt;string&gt; # e.g., 2x, once, etc.\', \'quality\': \'&lt;string&gt; # e.g., loose, hard, etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, after shower, etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}, \'Family\': {\'interaction\': \'&lt;string&gt; # e.g., visit, call, communication, etc.\', \'relation\': \'&lt;string&gt; # e.g., mother, son, etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, after shower, etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}, \'Pain\': {\'severity\': \'&lt;string&gt; # e.g., mild, moderate, severe, numeric scale if present, etc.\', \'location\': \'&lt;string&gt; # e.g., right knee, head, etc.\', \'duration\': \'&lt;string&gt; # e.g., all night, 3 hours, etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, after shower, etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}, \'Sleep\': {\'quality\': \'&lt;string&gt; # e.g., good, poor, restless, etc.\', \'duration\': \'&lt;string&gt; # e.g., 6 hours, phrases like "all night", etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, after shower, etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}}\n                                    If no relevant attribute exists for an event, return an empty object {}.\n                                    \n                        \n                        \n                        ---\n                        Output Schema (strict):\n                        {\n                                    "events": [\n                                        {\n                                        "event_type": "&lt;Pain | Sleep | Excretion | Eating | Family&gt;",\n                                        "text_quote": "&lt;fragement from the text indicating &gt;",\n                "attributes": {\n                    "&lt;attribute_name&gt;": "&lt;attribute_value&gt;"\n                }\n                                        }\n                                    ]\n                                    }\n                        \n                            Rules:\n                                - Ensure the output is valid JSON (parseable).\n                                - "eventS" must always be an array (can be empty).\n                                - Multiple instances of the same event type appear as individual elements in the event array.\n                                - Events appear in the array in the same order in which they appear in the text.\n                                - Do not include extra keys, comments, or text.\n                                - Each object in "events" must contain "event_type", "text_quote", and "attributes".\n                                -If an event attribute type has no value mentioned, return "attributes": {"&lt; attribute name &gt;:Unknown"} for each attribute type defined for the event type \n                        \n                        \n                        \n                ---\n                Examples:\n                \n                text: "Patient ate breakfast this morning. He seems less anxious."\n                output: {\n                "events": [\n                    {\n                    "event_type": "Eating",\n                    "text_quote":"Patient ate breakfast this morning",\n                    "attributes": {"food": "breakfast", \n                                   "amount": "Unknown",\n                                   "method": "Unknown",\n                                   "time":"morning",\n                                   "caused_by":"Unknown"}\n                    }\n                ]\n                }\n                \n                text: "Patient reported severe abdominal pain."\n                output: {\n                "events": [\n                    {\n                    "event_type": "Pain",\n                    "text_quote": "severe abdominal Pain",\n                    "attributes": {"severity": "severe", \n                                   "location": "abdominal",\n                                   "duration": "Unknown",\n                                   "time":"Unknown",\n                                   "caused_by":"Unknown"}\n                    }\n                ]\n                }\n                \n                text: "Patient called his son around 3 pm."\n                output: {\n                "events": [\n                    {\n                    "event_type": "Family",\n                    "text_quote": "called his son around 3 pm",\n                    "attributes": {"interaction": "call", \n                                    "relation": "son",\n                                    "time":"3 pm",\n                                    "caused_by":"Unknown"}\n                    }\n                ]\n                }\n                \n                text: "Patient had a loose stool overnight."\n                output: {\n                "events": [\n                    {\n                    "event_type": "Excretion",\n                    "text_quote": "loose stool overnight",\n                    "attributes": {"type": "stool", \n                                   "quality": "loose", \n                                   "frequency":"overnight", \n                                   "time":"night",\n                                   "caused_by":"Unknown"}\n                    }\n                ]\n                }\n                \n                text: "Patient was able to sleep well last night."\n                output: {\n                "events": [\n                    {\n                    "event_type": "Sleep",\n                    "text_quote": "sleep well last night",\n                    "attributes": {"quality": "well",\n                                    "duration": "Unknown", \n                                    "time":"night",\n                                    "caused_by":"Unknown"}\n                    }\n                ]\n                }\n                \n                text: "The patient couldn\'t sleep due to severe pain."\n                output: {\n                "events": [\n                    {\n                    "event_type": "Sleep",\n                    "text_quote": "couldn\'t sleep",\n                    "attributes": {"quality": "poor", \n                                    "duration": "Unknown",\n                                   "time":"Unknown",\n                                   "caused_by":"Pain"}\n                    },\n                    {\n                    "event_type": "Pain",\n                    "text_quote": "severe pain",\n                    "attributes": {"severity": "severe", \n                                    "location": "Unknown", \n                                    "duration": "Unknown", \n                                   "time":"before Sleep",\n                                   "caused_by":"Unknown"}\n                    }\n                ]\n                }\n                \n                text: "The patient complained of severe back pain, was given Tylenol, but the pain persisted and he was then prescribed stronger morphine."\n                output: {\n                "events": [\n                    {\n                    "event_type": "Pain",\n                    "text_quote": "complained of severe back pain",\n                    "attributes": {"severity": "severe", \n                                    "location": "back",\n                                    "duration": "Unknown", \n                                    "time":"Unknown",\n                                    "caused_by":"Unknown"}\n                    },\n                    {\n                    "event_type": "Pain",\n                    "text_quote": "pain persisted",\n                    "attributes": {"severity": "severe", \n                                   "location": "back",\n                                   "duration": "persistent", \n                                   "time":"after Tylenol",\n                                   "caused_by":"Unknown"}\n                    }\n                ]\n                }\n                \n                        ', 'event_detection_time': 9.583147113997256}</t>
-        </is>
-      </c>
       <c r="N8" t="inlineStr">
         <is>
-          <t>['Pain', 'Sleep', 'Excretion']</t>
+          <t>['c/o mild back pain, per patient. tolerable.', 'down significantly when asleep but patient. awakens easily and is coherent, map &gt;60, md aware, cont to closely monitor.', 'foley draining minimal amts clear amber urine, 15-40cc/heart rate, +725cc yesterday.', 'appropriately discouraged re: lack of sleep but otherwise pleasant.']</t>
         </is>
       </c>
       <c r="O8" t="inlineStr">
         <is>
-          <t>[{'Pain': {'severity': 'mild', 'location': 'back', 'duration': 'Unknown', 'time': 'Unknown', 'caused_by': 'Unknown'}}, {'Sleep': {'quality': 'good', 'duration': 'Unknown', 'time': 'Unknown', 'caused_by': 'Unknown'}}, {'Excretion': {'type': 'urine', 'frequency': 'minimal', 'quality': 'clear amber', 'time': 'Unknown', 'caused_by': 'Unknown'}}]</t>
-        </is>
-      </c>
-      <c r="P8" t="inlineStr">
-        <is>
-          <t>['c/o mild back pain, per patient. tolerable.', 'down significantly when asleep but patient. awakens easily and is coherent', 'foley draining minimal amts clear amber urine, 15-40cc/heart rate, +725cc yesterday.']</t>
-        </is>
-      </c>
-      <c r="Q8" t="n">
-        <v>0.003000100999997812</v>
-      </c>
-      <c r="R8" t="inlineStr">
+          <t>[[['e1', 'before', 'e2'], ['e2', 'before', 'e3'], ['e3', 'before', 'e4']]]</t>
+        </is>
+      </c>
+      <c r="P8" t="n">
+        <v>0.002408244999969611</v>
+      </c>
+      <c r="Q8" t="inlineStr">
         <is>
           <t>Sleep</t>
         </is>
       </c>
-      <c r="S8" t="b">
-        <v>0</v>
+      <c r="R8" t="b">
+        <v>0</v>
+      </c>
+      <c r="S8" t="n">
+        <v>1</v>
       </c>
       <c r="T8" t="n">
         <v>1</v>
       </c>
-      <c r="U8" t="n">
-        <v>1</v>
-      </c>
-      <c r="V8" t="inlineStr">
+      <c r="U8" t="inlineStr">
         <is>
           <t>('pain', 'urine', 'sleep', 'asleep')</t>
         </is>
       </c>
+      <c r="V8" t="n">
+        <v>12.07059701101389</v>
+      </c>
       <c r="W8" t="n">
-        <v>10.06759834699915</v>
+        <v>14.45120449201204</v>
       </c>
       <c r="X8" t="n">
-        <v>12.07249433800462</v>
+        <v>1</v>
       </c>
       <c r="Y8" t="n">
-        <v>9.583147113997256</v>
+        <v>1</v>
       </c>
       <c r="Z8" t="n">
-        <v>1</v>
-      </c>
-      <c r="AA8" t="n">
-        <v>1</v>
-      </c>
-      <c r="AB8" t="n">
-        <v>1</v>
-      </c>
-      <c r="AC8" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="9">
-      <c r="A9" t="n">
-        <v>1310486</v>
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>1310486</t>
+        </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>['Unknown', 'Sleep', 'Pain', 'Excretion', 'Family']</t>
+          <t>('Pain', 'Unknown', 'Excretion', 'Family', 'Sleep')</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>['aches', 'urine', 'son', 'sleeping', 'asleep', 'sleep', 'family']</t>
+          <t>('asleep', 'aches', 'sleep', 'son', 'family', 'urine', 'sleeping')</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
@@ -1566,120 +1492,111 @@
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>{'text': "ccu nursing progress note 7pm 3/21-7am [**3-14**]\ns:  i can't sleep at night at home either.  i walk around alot.\n\no:  patient sleeping only in short intervals, but states that this is normal for him.  sitting on side of bed to relieve generalized aches.\n\nt max 97.7\n\ncv - heart rate 56-62 sb/sr with no vea.  bp continues to be labile 80-150/59-70.  found that patient was initially on 1mg/min labetelol.  attempting to titrate down and while patient was asleep, labetolol was briefly off per bp.  but as patient is awake, labetolol resumed and increased up to 1mg/min for goal diastolic blood pressure 100-120/.  milrinone cont 0.375mcgs/kg/min and is unchanged.  pulses +1/+2 bilaterally.  mri tonight with no documented results.\n\nresp - ls are decreased at bases l&gt;r and o2 on 6ln/p.  patient denies sob.  patient is a mouth breather, so sat will decrease to 92% while patient is asleep, otherwise 95-97%.\n\ngu - foley patent cloudy amber urine 15-40cc/heart rate.\n\ngi - abd is soft with +bs.  no stool tonight.  tolerating by mouth's without difficulty.\n\nskin - l hand old iv site +2 edema, reddened with approx 2-3cm area of bruising noted.  covered with dsd. ho aware.  l elbow reddened contusion noted as well as area of pressure r buttocks.  areas washed with soap and water and left open to air.\n\nsocial - wife and son [**name (ni) **] patient this evening and have spoken and were updated by ho.\n\na:  84yom with aortic dissection c/b hypotension, cardiogenic shock now is stable on milrinone and labetolol.\n\np:  check am pnd lytes, hct and replete pro re nata, ? change iv labetolol to by mouth beta blocker, monitor bp response, cont pulse checks, monitor skin integrity and encourage turning and positioning to lessen pressure areas, cont to keep patient and family informed of all plans, treatments and goals.\n", 'event': ['Sleep', 'Pain', 'Sleep', 'Excretion', 'Family'], 'phrase': '', 'raw_output': '{\n  "events": [\n    {\n      "event_type": "Sleep",\n      "text_quote": "i can\'t sleep at night at home either.",\n      "attributes": {"quality": "poor", \n                     "duration": "Unknown", \n                     "time":"night",\n                     "caused_by":"Unknown"}\n    },\n    {\n      "event_type": "Pain",\n      "text_quote": "sitting on side of bed to relieve generalized aches.",\n      "attributes": {"severity": "Unknown", \n                     "location": "generalized", \n                     "duration": "Unknown", \n                     "time":"Unknown",\n                     "caused_by":"Unknown"}\n    },\n    {\n      "event_type": "Sleep",\n      "text_quote": "patient sleeping only in short intervals, but states that this is normal for him.",\n      "attributes": {"quality": "poor", \n                     "duration": "short intervals", \n                     "time":"Unknown",\n                     "caused_by":"Unknown"}\n    },\n    {\n      "event_type": "Excretion",\n      "text_quote": "foley patent cloudy amber urine 15-40cc/heart rate.",\n      "attributes": {"type": "urine", \n                     "quality": "cloudy amber", \n                     "frequency":"15-40cc/heart rate", \n                     "time":"Unknown",\n                     "caused_by":"Unknown"}\n    },\n    {\n      "event_type": "Family",\n      "text_quote": "wife and son [**name (ni) **] patient this evening and have spoken and were updated by ho.",\n      "attributes": {"interaction": "visit", \n                     "relation": "wife, son", \n                     "time":"evening",\n                     "caused_by":"Unknown"}\n    }\n  ]\n}', 'attributes': [{'Sleep': {'quality': 'poor', 'duration': 'Unknown', 'time': 'night', 'caused_by': 'Unknown'}}, {'Pain': {'severity': 'Unknown', 'location': 'generalized', 'duration': 'Unknown', 'time': 'Unknown', 'caused_by': 'Unknown'}}, {'Sleep': {'quality': 'poor', 'duration': 'short intervals', 'time': 'Unknown', 'caused_by': 'Unknown'}}, {'Excretion': {'type': 'urine', 'quality': 'cloudy amber', 'frequency': '15-40cc/heart rate', 'time': 'Unknown', 'caused_by': 'Unknown'}}, {'Family': {'interaction': 'visit', 'relation': 'wife, son', 'time': 'evening', 'caused_by': 'Unknown'}}], 'text_quotes': ["i can't sleep at night at home either.", 'sitting on side of bed to relieve generalized aches.', 'patient sleeping only in short intervals, but states that this is normal for him.', 'foley patent cloudy amber urine 15-40cc/heart rate.', 'wife and son [**name (ni) **] patient this evening and have spoken and were updated by ho.'], 'event_name_prompt': 'Given the text: ccu nursing progress note 7pm 3/21-7am [**3-14**]\ns:  i can\'t sleep at night at home either.  i walk around alot.\n\no:  patient sleeping only in short intervals, but states that this is normal for him.  sitting on side of bed to relieve generalized aches.\n\nt max 97.7\n\ncv - heart rate 56-62 sb/sr with no vea.  bp continues to be labile 80-150/59-70.  found that patient was initially on 1mg/min labetelol.  attempting to titrate down and while patient was asleep, labetolol was briefly off per bp.  but as patient is awake, labetolol resumed and increased up to 1mg/min for goal diastolic blood pressure 100-120/.  milrinone cont 0.375mcgs/kg/min and is unchanged.  pulses +1/+2 bilaterally.  mri tonight with no documented results.\n\nresp - ls are decreased at bases l&gt;r and o2 on 6ln/p.  patient denies sob.  patient is a mouth breather, so sat will decrease to 92% while patient is asleep, otherwise 95-97%.\n\ngu - foley patent cloudy amber urine 15-40cc/heart rate.\n\ngi - abd is soft with +bs.  no stool tonight.  tolerating by mouth\'s without difficulty.\n\nskin - l hand old iv site +2 edema, reddened with approx 2-3cm area of bruising noted.  covered with dsd. ho aware.  l elbow reddened contusion noted as well as area of pressure r buttocks.  areas washed with soap and water and left open to air.\n\nsocial - wife and son [**name (ni) **] patient this evening and have spoken and were updated by ho.\n\na:  84yom with aortic dissection c/b hypotension, cardiogenic shock now is stable on milrinone and labetolol.\n\np:  check am pnd lytes, hct and replete pro re nata, ? change iv labetolol to by mouth beta blocker, monitor bp response, cont pulse checks, monitor skin integrity and encourage turning and positioning to lessen pressure areas, cont to keep patient and family informed of all plans, treatments and goals.\n, \n                        and the following event types with their definitions: Eating : The patient takes food into their body by mouth.\nExcretion : The patient discharges waste matter from their body.\nFamily : The patient has a visit, call, or communication with a family member.\nPain : The patient reports or shows signs of pain.\nSleep : The patient sleeps or the sleep’s quality or quantity is described.\nUnknown : choose "Unknown" if none of the other event type are applicable. \n                        ---\n                        Your task:\n                        0. Identify ALL events in the text (zero, one, or more).\n1. For each event, assign an event_type from the list above.\n2. If multiple event of same type is mentioned, assign the event_type multiple times\n3. Extract attributes for each event using ONLY the allowed attributes listed below.\n4. Use keyword evidence (Ki) ONLY if it is consistent with the text context.\n5. Output strictly valid JSON following the schema below.\n                        ---\n                        Classification Rules:\n                        - A text may contain multiple events of the same or different types.\n- Create a separate event object for each event mention.\n- If the text is explicitly a NEGATION (e.g., "denies pain"), do not extract that event.\n- If the text describes a FUTURE or HYPOTHETICAL event (e.g., "will eat tomorrow"), ignore it.\n- A valid event should have occurred in the recent past or is occurring during the time of writing of the text.\n- If no events are found or if unsure, return {"events": []}\n                        \n                        ---\n                                    Attributes allowed:\n                                    {\'Eating\': {\'food\': \'&lt;string&gt; # e.g., pancakes, porridge, etc.\', \'amount\': \'&lt;string&gt; # e.g., 1, 2 bowls, etc.\', \'method\': \'&lt;string&gt;  # e.g., oral, tube, etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, after shower, etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}, \'Excretion\': {\'type\': \'&lt;string&gt; # e.g., urine, stool, etc.\', \'frequency\': \'&lt;string&gt; # e.g., 2x, once, etc.\', \'quality\': \'&lt;string&gt; # e.g., loose, hard, etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, after shower, etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}, \'Family\': {\'interaction\': \'&lt;string&gt; # e.g., visit, call, communication, etc.\', \'relation\': \'&lt;string&gt; # e.g., mother, son, etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, after shower, etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}, \'Pain\': {\'severity\': \'&lt;string&gt; # e.g., mild, moderate, severe, numeric scale if present, etc.\', \'location\': \'&lt;string&gt; # e.g., right knee, head, etc.\', \'duration\': \'&lt;string&gt; # e.g., all night, 3 hours, etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, after shower, etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}, \'Sleep\': {\'quality\': \'&lt;string&gt; # e.g., good, poor, restless, etc.\', \'duration\': \'&lt;string&gt; # e.g., 6 hours, phrases like "all night", etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, after shower, etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}}\n                                    If no relevant attribute exists for an event, return an empty object {}.\n                                    \n                        \n                        ---\n                                    Keyword evidence (Ki):\n                                    Additional facts: A keyword matching algorithm without context detected keyword(s) [\'aches\', \'urine\', \'son\', \'sleeping\', \'asleep\', \'sleep\', \'family\'].\n                                    Use this only as a pointer. If context contradicts, ignore.\n                        ---\n                        Output Schema (strict):\n                        {\n                                    "events": [\n                                        {\n                                        "event_type": "&lt;Pain | Sleep | Excretion | Eating | Family&gt;",\n                                        "text_quote": "&lt;fragement from the text indicating &gt;",\n                "attributes": {\n                    "&lt;attribute_name&gt;": "&lt;attribute_value&gt;"\n                }\n                                        }\n                                    ]\n                                    }\n                        \n                            Rules:\n                                - Ensure the output is valid JSON (parseable).\n                                - "eventS" must always be an array (can be empty).\n                                - Multiple instances of the same event type appear as individual elements in the event array.\n                                - Events appear in the array in the same order in which they appear in the text.\n                                - Do not include extra keys, comments, or text.\n                                - Each object in "events" must contain "event_type", "text_quote", and "attributes".\n                                -If an event attribute type has no value mentioned, return "attributes": {"&lt; attribute name &gt;:Unknown"} for each attribute type defined for the event type \n                        \n                        \n                        \n                ---\n                Examples:\n                \n                text: "Patient ate breakfast this morning. He seems less anxious."\n                output: {\n                "events": [\n                    {\n                    "event_type": "Eating",\n                    "text_quote":"Patient ate breakfast this morning",\n                    "attributes": {"food": "breakfast", \n                                   "amount": "Unknown",\n                                   "method": "Unknown",\n                                   "time":"morning",\n                                   "caused_by":"Unknown"}\n                    }\n                ]\n                }\n                \n                text: "Patient reported severe abdominal pain."\n                output: {\n                "events": [\n                    {\n                    "event_type": "Pain",\n                    "text_quote": "severe abdominal Pain",\n                    "attributes": {"severity": "severe", \n                                   "location": "abdominal",\n                                   "duration": "Unknown",\n                                   "time":"Unknown",\n                                   "caused_by":"Unknown"}\n                    }\n                ]\n                }\n                \n                text: "Patient called his son around 3 pm."\n                output: {\n                "events": [\n                    {\n                    "event_type": "Family",\n                    "text_quote": "called his son around 3 pm",\n                    "attributes": {"interaction": "call", \n                                    "relation": "son",\n                                    "time":"3 pm",\n                                    "caused_by":"Unknown"}\n                    }\n                ]\n                }\n                \n                text: "Patient had a loose stool overnight."\n                output: {\n                "events": [\n                    {\n                    "event_type": "Excretion",\n                    "text_quote": "loose stool overnight",\n                    "attributes": {"type": "stool", \n                                   "quality": "loose", \n                                   "frequency":"overnight", \n                                   "time":"night",\n                                   "caused_by":"Unknown"}\n                    }\n                ]\n                }\n                \n                text: "Patient was able to sleep well last night."\n                output: {\n                "events": [\n                    {\n                    "event_type": "Sleep",\n                    "text_quote": "sleep well last night",\n                    "attributes": {"quality": "well",\n                                    "duration": "Unknown", \n                                    "time":"night",\n                                    "caused_by":"Unknown"}\n                    }\n                ]\n                }\n                \n                text: "The patient couldn\'t sleep due to severe pain."\n                output: {\n                "events": [\n                    {\n                    "event_type": "Sleep",\n                    "text_quote": "couldn\'t sleep",\n                    "attributes": {"quality": "poor", \n                                    "duration": "Unknown",\n                                   "time":"Unknown",\n                                   "caused_by":"Pain"}\n                    },\n                    {\n                    "event_type": "Pain",\n                    "text_quote": "severe pain",\n                    "attributes": {"severity": "severe", \n                                    "location": "Unknown", \n                                    "duration": "Unknown", \n                                   "time":"before Sleep",\n                                   "caused_by":"Unknown"}\n                    }\n                ]\n                }\n                \n                text: "The patient complained of severe back pain, was given Tylenol, but the pain persisted and he was then prescribed stronger morphine."\n                output: {\n                "events": [\n                    {\n                    "event_type": "Pain",\n                    "text_quote": "complained of severe back pain",\n                    "attributes": {"severity": "severe", \n                                    "location": "back",\n                                    "duration": "Unknown", \n                                    "time":"Unknown",\n                                    "caused_by":"Unknown"}\n                    },\n                    {\n                    "event_type": "Pain",\n                    "text_quote": "pain persisted",\n                    "attributes": {"severity": "severe", \n                                   "location": "back",\n                                   "duration": "persistent", \n                                   "time":"after Tylenol",\n                                   "caused_by":"Unknown"}\n                    }\n                ]\n                }\n                \n                        ', 'event_detection_time': 13.660997304992634}</t>
+          <t>['asleep', 'sleep', 'son', 'family', 'urine', 'ache', 'sleeping']</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
+          <t>{'text': "ccu nursing progress note 7pm 3/21-7am [**3-14**]\ns:  i can't sleep at night at home either.  i walk around alot.\n\no:  patient sleeping only in short intervals, but states that this is normal for him.  sitting on side of bed to relieve generalized aches.\n\nt max 97.7\n\ncv - heart rate 56-62 sb/sr with no vea.  bp continues to be labile 80-150/59-70.  found that patient was initially on 1mg/min labetelol.  attempting to titrate down and while patient was asleep, labetolol was briefly off per bp.  but as patient is awake, labetolol resumed and increased up to 1mg/min for goal diastolic blood pressure 100-120/.  milrinone cont 0.375mcgs/kg/min and is unchanged.  pulses +1/+2 bilaterally.  mri tonight with no documented results.\n\nresp - ls are decreased at bases l&gt;r and o2 on 6ln/p.  patient denies sob.  patient is a mouth breather, so sat will decrease to 92% while patient is asleep, otherwise 95-97%.\n\ngu - foley patent cloudy amber urine 15-40cc/heart rate.\n\ngi - abd is soft with +bs.  no stool tonight.  tolerating by mouth's without difficulty.\n\nskin - l hand old iv site +2 edema, reddened with approx 2-3cm area of bruising noted.  covered with dsd. ho aware.  l elbow reddened contusion noted as well as area of pressure r buttocks.  areas washed with soap and water and left open to air.\n\nsocial - wife and son [**name (ni) **] patient this evening and have spoken and were updated by ho.\n\na:  84yom with aortic dissection c/b hypotension, cardiogenic shock now is stable on milrinone and labetolol.\n\np:  check am pnd lytes, hct and replete pro re nata, ? change iv labetolol to by mouth beta blocker, monitor bp response, cont pulse checks, monitor skin integrity and encourage turning and positioning to lessen pressure areas, cont to keep patient and family informed of all plans, treatments and goals.\n", 'event': ['Sleep', 'Pain', 'Sleep', 'Excretion', 'Family'], 'event_id': ['e1', 'e2', 'e3', 'e4', 'e5'], 'phrase': '', 'raw_output': '{\n  "events": [\n    {\n      "event_id": "e1",\n      "event_type": "Sleep",\n      "text_quote": "i can\'t sleep at night at home either.",\n      "attributes": {\n        "quality": "poor",\n        "duration": "Unknown",\n        "negation": "false",\n        "time": "night",\n        "caused_by": "Unknown"\n      }\n    },\n    {\n      "event_id": "e2",\n      "event_type": "Pain",\n      "text_quote": "sitting on side of bed to relieve generalized aches.",\n      "attributes": {\n        "severity": "Unknown",\n        "location": "generalized",\n        "duration": "Unknown",\n        "negation": "false",\n        "time": "Unknown",\n        "caused_by": "Unknown"\n      }\n    },\n    {\n      "event_id": "e3",\n      "event_type": "Sleep",\n      "text_quote": "patient sleeping only in short intervals, but states that this is normal for him.",\n      "attributes": {\n        "quality": "poor",\n        "duration": "short intervals",\n        "negation": "false",\n        "time": "Unknown",\n        "caused_by": "Unknown"\n      }\n    },\n    {\n      "event_id": "e4",\n      "event_type": "Excretion",\n      "text_quote": "foley patent cloudy amber urine 15-40cc/heart rate.",\n      "attributes": {\n        "type": "urine",\n        "frequency": "Unknown",\n        "quality": "cloudy amber",\n        "negation": "false",\n        "time": "Unknown",\n        "caused_by": "Unknown"\n      }\n    },\n    {\n      "event_id": "e5",\n      "event_type": "Family",\n      "text_quote": "wife and son [**name (ni) **] patient this evening and have spoken and were updated by ho.",\n      "attributes": {\n        "interaction": "visit",\n        "relation": "wife and son",\n        "negation": "false",\n        "time": "evening",\n        "caused_by": "Unknown"\n      }\n    }\n  ],\n  "order": []\n}', 'attributes': [{'Sleep': {'quality': 'poor', 'duration': 'Unknown', 'negation': 'false', 'time': 'night', 'caused_by': 'Unknown'}}, {'Pain': {'severity': 'Unknown', 'location': 'generalized', 'duration': 'Unknown', 'negation': 'false', 'time': 'Unknown', 'caused_by': 'Unknown'}}, {'Sleep': {'quality': 'poor', 'duration': 'short intervals', 'negation': 'false', 'time': 'Unknown', 'caused_by': 'Unknown'}}, {'Excretion': {'type': 'urine', 'frequency': 'Unknown', 'quality': 'cloudy amber', 'negation': 'false', 'time': 'Unknown', 'caused_by': 'Unknown'}}, {'Family': {'interaction': 'visit', 'relation': 'wife and son', 'negation': 'false', 'time': 'evening', 'caused_by': 'Unknown'}}], 'orders': [[]], 'text_quotes': ["i can't sleep at night at home either.", 'sitting on side of bed to relieve generalized aches.', 'patient sleeping only in short intervals, but states that this is normal for him.', 'foley patent cloudy amber urine 15-40cc/heart rate.', 'wife and son [**name (ni) **] patient this evening and have spoken and were updated by ho.'], 'event_name_prompt': 'Given the text: ccu nursing progress note 7pm 3/21-7am [**3-14**]\ns:  i can\'t sleep at night at home either.  i walk around alot.\n\no:  patient sleeping only in short intervals, but states that this is normal for him.  sitting on side of bed to relieve generalized aches.\n\nt max 97.7\n\ncv - heart rate 56-62 sb/sr with no vea.  bp continues to be labile 80-150/59-70.  found that patient was initially on 1mg/min labetelol.  attempting to titrate down and while patient was asleep, labetolol was briefly off per bp.  but as patient is awake, labetolol resumed and increased up to 1mg/min for goal diastolic blood pressure 100-120/.  milrinone cont 0.375mcgs/kg/min and is unchanged.  pulses +1/+2 bilaterally.  mri tonight with no documented results.\n\nresp - ls are decreased at bases l&gt;r and o2 on 6ln/p.  patient denies sob.  patient is a mouth breather, so sat will decrease to 92% while patient is asleep, otherwise 95-97%.\n\ngu - foley patent cloudy amber urine 15-40cc/heart rate.\n\ngi - abd is soft with +bs.  no stool tonight.  tolerating by mouth\'s without difficulty.\n\nskin - l hand old iv site +2 edema, reddened with approx 2-3cm area of bruising noted.  covered with dsd. ho aware.  l elbow reddened contusion noted as well as area of pressure r buttocks.  areas washed with soap and water and left open to air.\n\nsocial - wife and son [**name (ni) **] patient this evening and have spoken and were updated by ho.\n\na:  84yom with aortic dissection c/b hypotension, cardiogenic shock now is stable on milrinone and labetolol.\n\np:  check am pnd lytes, hct and replete pro re nata, ? change iv labetolol to by mouth beta blocker, monitor bp response, cont pulse checks, monitor skin integrity and encourage turning and positioning to lessen pressure areas, cont to keep patient and family informed of all plans, treatments and goals.\n, \n                        and the following event types with their definitions: Eating : The patient takes food into their body by mouth.\nExcretion : The patient discharges waste matter from their body.\nFamily : The patient has a visit, call, or communication with a family member.\nPain : The patient reports or shows signs of pain.\nSleep : The patient sleeps or the sleep’s quality or quantity is described.\nUnknown : choose "Unknown" if none of the other event type are applicable. \n                        ---\n                        Your task:\n                        0. Identify ALL events in the text (zero, one, or more).\n1. For each event, assign an event_type from the list above.\n2. If multiple event of same type is mentioned, assign the event_type multiple times\n3. Extract attributes for each event using ONLY the allowed attributes listed below.\n4. Use keyword evidence (Ki) ONLY if it is consistent with the text context.\n5. Output strictly valid JSON following the schema below.\n                        ---\n                        Classification Rules:\n                        - A text may contain multiple events of the same or different types.\n- Create a separate event object for each event mention.\n- If the text is explicitly a NEGATION (e.g., "denies pain"), do not extract that event.\n- If the text describes a FUTURE or HYPOTHETICAL event (e.g., "will eat tomorrow"), ignore it.\n- A valid event should have occurred in the recent past or is occurring during the time of writing of the text.\n- If no events are found or if unsure, return {"events": []}\n                        \n                        ---\n                                    Attributes allowed:\n                                    {\'Eating\': {\'food\': \'&lt;string&gt; # e.g., pancakes, porridge, etc.\', \'amount\': \'&lt;string&gt; # e.g., 1, 2 bowls, etc.\', \'method\': \'&lt;string&gt;  # e.g., oral, tube, etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, evening etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}, \'Excretion\': {\'type\': \'&lt;string&gt; # e.g., urine, stool, etc.\', \'frequency\': \'&lt;string&gt; # e.g., 2x, once, etc.\', \'quality\': \'&lt;string&gt; # e.g., loose, hard, etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, evening etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}, \'Family\': {\'interaction\': \'&lt;string&gt; # e.g., visit, call, communication, etc.\', \'relation\': \'&lt;string&gt; # e.g., mother, son, etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, evening etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}, \'Pain\': {\'severity\': \'&lt;string&gt; # e.g., mild, moderate, severe, numeric scale if present, etc.\', \'location\': \'&lt;string&gt; # e.g., right knee, head, etc.\', \'duration\': \'&lt;string&gt; # e.g., all night, 3 hours, etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, evening etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}, \'Sleep\': {\'quality\': \'&lt;string&gt; # e.g., good, poor, restless, etc.\', \'duration\': \'&lt;string&gt; # e.g., 6 hours, phrases like "all night", etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, evening etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}}\n                                    If no relevant attribute exists for an event, return an empty object {}.\n                                    \n                        \n                        ---\n                                    Keyword evidence (Ki):\n                                    Additional facts: A keyword matching algorithm without context detected keyword(s) (\'asleep\', \'aches\', \'sleep\', \'son\', \'family\', \'urine\', \'sleeping\').\n                                    Use this only as a pointer. If context contradicts, ignore.\n                        ---\n                        Output Schema (strict):\n                        {\n                                    "events": [\n                                        {\n                                        "event_id": "&lt; A unique id eg.: e1 | e2 |...&gt;"\n                                        "event_type": "&lt;Pain | Sleep | Excretion | Eating | Family&gt;",\n                                        "text_quote": "&lt;fragement from the text indicating the event_type&gt;",\n                "attributes": {\n                    "&lt;attribute_name&gt;": "&lt;attribute_value&gt;"\n                }\n                                        }\n                                    ],\n                                    "order": [\n                                        ["e1", "before" | "after" | "simultaneous", "e2" ]\n                                    ]\n                                    }\n                        \n                            Rules:\n                                - Ensure the output is valid JSON (parseable).\n                                - "eventS" must always be an array (can be empty).\n                                - Multiple instances of the same event type appear with different ids.\n                                - Events appear in the array in the same order in which they appear in the text.\n                                - Their partial orders can be expressed using the "order" section.\n                                - Do not include extra keys, comments, or text.\n                                - Each object in "events" must contain "event_type", "text_quote", and "attributes".\n                                - If an event attribute type has no value mentioned, return "attributes": {"&lt; attribute name &gt;:Unknown"} for each attribute type defined for the event type \n                        \n                        \n                        \n                ---\n                Examples:\n                \n                text: "Patient ate breakfast this morning. He seems less anxious."\n                output: {\n                "events": [\n                    {"event_id": "e1",\n                    "event_type": "Eating",\n                    "text_quote":"Patient ate breakfast this morning",\n                    "attributes": {"food": "breakfast", \n                                   "amount": "Unknown",\n                                   "method": "Unknown",\n                                   "negation": "false",\n                                   "time":"morning",\n                                   "caused_by":"Unknown"}\n                    }\n                ],\n                "order":[]\n                }\n                \n                text: "Patient reported severe abdominal pain."\n                output: {\n                "events": [\n                    {"event_id": "e1",\n                    "event_type": "Pain",\n                    "text_quote": "severe abdominal Pain",\n                    "attributes": {"severity": "severe", \n                                   "location": "abdominal",\n                                   "duration": "Unknown",\n                                   "negation": "false",\n                                   "time":"Unknown",\n                                   "caused_by":"Unknown"}\n                    }\n                ],\n                "order":[]\n                }\n                \n                text: "Patient called his son around 3 pm."\n                output: {\n                "events": [\n                    {"event_id": "e1",\n                    "event_type": "Family",\n                    "text_quote": "called his son around 3 pm",\n                    "attributes": {"interaction": "call", \n                                    "relation": "son",\n                                    "negation": "false",\n                                    "time":"3 pm",\n                                    "caused_by":"Unknown"}\n                    }\n                ],\n                "order":[]\n                }\n                \n                text: "Patient had a loose stool overnight."\n                output: {\n                "events": [\n                    {"event_id": "e1",\n                    "event_type": "Excretion",\n                    "text_quote": "loose stool overnight",\n                    "attributes": {"type": "stool", \n                                   "quality": "loose", \n                                   "frequency":"overnight", \n                                   "negation": "false",\n                                   "time":"night",\n                                   "caused_by":"Unknown"}\n                    }\n                ],\n                "order":[]\n                }\n                \n                text: "Patient was able to sleep well last night."\n                output: {\n                "events": [\n                    {"event_id": "e1",\n                    "event_type": "Sleep",\n                    "text_quote": "sleep well last night",\n                    "attributes": {"quality": "well",\n                                    "duration": "Unknown", \n                                    "negation": "false",\n                                    "time":"night",\n                                    "caused_by":"Unknown"}\n                    }\n                ],\n                "order":[]\n                }\n                \n                text: "The patient couldn\'t sleep due to severe pain."\n                output: {\n                "events": [\n                    {"event_id": "e1",\n                    "event_type": "Sleep",\n                    "text_quote": "couldn\'t sleep",\n                    "attributes": {"quality": "poor", \n                                    "duration": "Unknown",\n                                    "negation": "true",\n                                    "time":"Unknown",\n                                    "caused_by":"Pain"}\n                    },\n                    {"event_id": "e2",\n                    "event_type": "Pain",\n                    "text_quote": "severe pain",\n                    "attributes": {"severity": "severe", \n                                    "location": "Unknown", \n                                    "duration": "Unknown", \n                                    "time":"Unknown",\n                                    "caused_by":"Unknown"}\n                    }\n                ],\n                "order":["e1", "after", "e2"]\n                }\n                \n                text: "The patient complained of severe back pain, was given Tylenol, but the pain persisted and he was then prescribed stronger morphine."\n                output: {\n                "events": [\n                    {"event_id": "e1",\n                    "event_type": "Pain",\n                    "text_quote": "complained of severe back pain",\n                    "attributes": {"severity": "severe", \n                                    "location": "back",\n                                    "duration": "Unknown", \n                                    "time":"Unknown",\n                                    "caused_by":"Unknown"}\n                    },\n                    {"event_id": "e2",\n                    "event_type": "Pain",\n                    "text_quote": "pain persisted",\n                    "attributes": {"severity": "severe", \n                                   "location": "back",\n                                   "duration": "persistent", \n                                   "time":"after Tylenol",\n                                   "caused_by":"Unknown"}\n                    }\n                ],\n                "order":[["e1", "before", "e2"]]\n                }\n                \n                        ', 'event_detection_time': 17.087886700988747}</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
           <t>['Sleep', 'Pain', 'Sleep', 'Excretion', 'Family']</t>
         </is>
       </c>
-      <c r="G9" t="inlineStr">
-        <is>
-          <t>[{'Sleep': {'quality': 'poor', 'duration': 'Unknown', 'time': 'night', 'caused_by': 'Unknown'}}, {'Pain': {'severity': 'Unknown', 'location': 'generalized', 'duration': 'Unknown', 'time': 'Unknown', 'caused_by': 'Unknown'}}, {'Sleep': {'quality': 'poor', 'duration': 'short intervals', 'time': 'Unknown', 'caused_by': 'Unknown'}}, {'Excretion': {'type': 'urine', 'quality': 'cloudy amber', 'frequency': '15-40cc/heart rate', 'time': 'Unknown', 'caused_by': 'Unknown'}}, {'Family': {'interaction': 'visit', 'relation': 'wife, son', 'time': 'evening', 'caused_by': 'Unknown'}}]</t>
-        </is>
-      </c>
       <c r="H9" t="inlineStr">
         <is>
+          <t>[{'Sleep': {'quality': 'poor', 'duration': 'Unknown', 'negation': 'false', 'time': 'night', 'caused_by': 'Unknown'}}, {'Pain': {'severity': 'Unknown', 'location': 'generalized', 'duration': 'Unknown', 'negation': 'false', 'time': 'Unknown', 'caused_by': 'Unknown'}}, {'Sleep': {'quality': 'poor', 'duration': 'short intervals', 'negation': 'false', 'time': 'Unknown', 'caused_by': 'Unknown'}}, {'Excretion': {'type': 'urine', 'frequency': 'Unknown', 'quality': 'cloudy amber', 'negation': 'false', 'time': 'Unknown', 'caused_by': 'Unknown'}}, {'Family': {'interaction': 'visit', 'relation': 'wife and son', 'negation': 'false', 'time': 'evening', 'caused_by': 'Unknown'}}]</t>
+        </is>
+      </c>
+      <c r="I9" t="inlineStr">
+        <is>
           <t>["i can't sleep at night at home either.", 'sitting on side of bed to relieve generalized aches.', 'patient sleeping only in short intervals, but states that this is normal for him.', 'foley patent cloudy amber urine 15-40cc/heart rate.', 'wife and son [**name (ni) **] patient this evening and have spoken and were updated by ho.']</t>
         </is>
       </c>
-      <c r="I9" t="inlineStr">
-        <is>
-          <t>{'text': "ccu nursing progress note 7pm 3/21-7am [**3-14**]\ns:  i can't sleep at night at home either.  i walk around alot.\n\no:  patient sleeping only in short intervals, but states that this is normal for him.  sitting on side of bed to relieve generalized aches.\n\nt max 97.7\n\ncv - heart rate 56-62 sb/sr with no vea.  bp continues to be labile 80-150/59-70.  found that patient was initially on 1mg/min labetelol.  attempting to titrate down and while patient was asleep, labetolol was briefly off per bp.  but as patient is awake, labetolol resumed and increased up to 1mg/min for goal diastolic blood pressure 100-120/.  milrinone cont 0.375mcgs/kg/min and is unchanged.  pulses +1/+2 bilaterally.  mri tonight with no documented results.\n\nresp - ls are decreased at bases l&gt;r and o2 on 6ln/p.  patient denies sob.  patient is a mouth breather, so sat will decrease to 92% while patient is asleep, otherwise 95-97%.\n\ngu - foley patent cloudy amber urine 15-40cc/heart rate.\n\ngi - abd is soft with +bs.  no stool tonight.  tolerating by mouth's without difficulty.\n\nskin - l hand old iv site +2 edema, reddened with approx 2-3cm area of bruising noted.  covered with dsd. ho aware.  l elbow reddened contusion noted as well as area of pressure r buttocks.  areas washed with soap and water and left open to air.\n\nsocial - wife and son [**name (ni) **] patient this evening and have spoken and were updated by ho.\n\na:  84yom with aortic dissection c/b hypotension, cardiogenic shock now is stable on milrinone and labetolol.\n\np:  check am pnd lytes, hct and replete pro re nata, ? change iv labetolol to by mouth beta blocker, monitor bp response, cont pulse checks, monitor skin integrity and encourage turning and positioning to lessen pressure areas, cont to keep patient and family informed of all plans, treatments and goals.\n", 'event': ['Sleep', 'Pain', 'Excretion', 'Family', 'Sleep'], 'phrase': '', 'raw_output': '{\n  "events": [\n    {\n      "event_type": "Sleep",\n      "text_quote": "patient sleeping only in short intervals, but states that this is normal for him.",\n      "attributes": {\n        "quality": "poor",\n        "duration": "short intervals",\n        "negation": false,\n        "time": "night"\n      }\n    },\n    {\n      "event_type": "Pain",\n      "text_quote": "sitting on side of bed to relieve generalized aches.",\n      "attributes": {\n        "severity": "Unknown",\n        "location": "generalized",\n        "duration": "Unknown",\n        "negation": false,\n        "time": "night"\n      }\n    },\n    {\n      "event_type": "Excretion",\n      "text_quote": "foley patent cloudy amber urine 15-40cc/heart rate.",\n      "attributes": {\n        "type": "urine",\n        "frequency": "Unknown",\n        "quality": "cloudy amber",\n        "negation": false,\n        "time": "night"\n      }\n    },\n    {\n      "event_type": "Family",\n      "text_quote": "wife and son [**name (ni) **] patient this evening and have spoken and were updated by ho.",\n      "attributes": {\n        "interaction": "visit",\n        "relation": "wife, son",\n        "negation": false,\n        "time": "evening"\n      }\n    },\n    {\n      "event_type": "Sleep",\n      "text_quote": "i can\'t sleep at night at home either.",\n      "attributes": {\n        "quality": "poor",\n        "duration": "Unknown",\n        "negation": false,\n        "time": "night"\n      }\n    }\n  ]\n}', 'attributes': [{'Sleep': {'quality': 'poor', 'duration': 'short intervals', 'negation': False, 'time': 'night'}}, {'Pain': {'severity': 'Unknown', 'location': 'generalized', 'duration': 'Unknown', 'negation': False, 'time': 'night'}}, {'Excretion': {'type': 'urine', 'frequency': 'Unknown', 'quality': 'cloudy amber', 'negation': False, 'time': 'night'}}, {'Family': {'interaction': 'visit', 'relation': 'wife, son', 'negation': False, 'time': 'evening'}}, {'Sleep': {'quality': 'poor', 'duration': 'Unknown', 'negation': False, 'time': 'night'}}], 'text_quotes': ['patient sleeping only in short intervals, but states that this is normal for him.', 'sitting on side of bed to relieve generalized aches.', 'foley patent cloudy amber urine 15-40cc/heart rate.', 'wife and son [**name (ni) **] patient this evening and have spoken and were updated by ho.', "i can't sleep at night at home either."], 'event_name_prompt': 'Given the text: ccu nursing progress note 7pm 3/21-7am [**3-14**]\ns:  i can\'t sleep at night at home either.  i walk around alot.\n\no:  patient sleeping only in short intervals, but states that this is normal for him.  sitting on side of bed to relieve generalized aches.\n\nt max 97.7\n\ncv - heart rate 56-62 sb/sr with no vea.  bp continues to be labile 80-150/59-70.  found that patient was initially on 1mg/min labetelol.  attempting to titrate down and while patient was asleep, labetolol was briefly off per bp.  but as patient is awake, labetolol resumed and increased up to 1mg/min for goal diastolic blood pressure 100-120/.  milrinone cont 0.375mcgs/kg/min and is unchanged.  pulses +1/+2 bilaterally.  mri tonight with no documented results.\n\nresp - ls are decreased at bases l&gt;r and o2 on 6ln/p.  patient denies sob.  patient is a mouth breather, so sat will decrease to 92% while patient is asleep, otherwise 95-97%.\n\ngu - foley patent cloudy amber urine 15-40cc/heart rate.\n\ngi - abd is soft with +bs.  no stool tonight.  tolerating by mouth\'s without difficulty.\n\nskin - l hand old iv site +2 edema, reddened with approx 2-3cm area of bruising noted.  covered with dsd. ho aware.  l elbow reddened contusion noted as well as area of pressure r buttocks.  areas washed with soap and water and left open to air.\n\nsocial - wife and son [**name (ni) **] patient this evening and have spoken and were updated by ho.\n\na:  84yom with aortic dissection c/b hypotension, cardiogenic shock now is stable on milrinone and labetolol.\n\np:  check am pnd lytes, hct and replete pro re nata, ? change iv labetolol to by mouth beta blocker, monitor bp response, cont pulse checks, monitor skin integrity and encourage turning and positioning to lessen pressure areas, cont to keep patient and family informed of all plans, treatments and goals.\n, \n                        and the following event types with their definitions: Eating : The patient takes food into their body by mouth.\nExcretion : The patient discharges waste matter from their body.\nFamily : The patient has a visit, call, or communication with a family member.\nPain : The patient reports or shows signs of pain.\nSleep : The patient sleeps or the sleep’s quality or quantity is described.\nUnknown : choose "Unknown" if none of the other event type are applicable. \n                        ---\n                        Your task:\n                        0. Identify ALL events in the text (zero, one, or more).\n1. For each event, assign an event_type from the list above.\n2. If multiple event of same type is mentioned, assign the event_type multiple times\n3. Extract attributes for each event using ONLY the allowed attributes listed below.\n4. Use keyword evidence (Ki) ONLY if it is consistent with the text context.\n5. Output strictly valid JSON following the schema below.\n                        ---\n                        Classification Rules:\n                        - A text may contain multiple events of the same or different types.\n- Create a separate event object for each event mention.\n- If the text is explicitly a NEGATION (e.g., "denies pain"), do not extract that event.\n- If the text describes a FUTURE or HYPOTHETICAL event (e.g., "will eat tomorrow"), ignore it.\n- A valid event should have occurred in the recent past or is occurring during the time of writing of the text.\n- If no events are found or if unsure, return {"events": []}\n                        \n                        ---\n                                    Attributes allowed:\n                                    {\'Eating\': {\'food\': \'&lt;string&gt; # e.g., pancakes, porridge, etc.\', \'amount\': \'&lt;string&gt; # e.g., 1, 2 bowls, etc.\', \'method\': \'&lt;string&gt;  # e.g., oral, tube, etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, after shower, etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}, \'Excretion\': {\'type\': \'&lt;string&gt; # e.g., urine, stool, etc.\', \'frequency\': \'&lt;string&gt; # e.g., 2x, once, etc.\', \'quality\': \'&lt;string&gt; # e.g., loose, hard, etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, after shower, etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}, \'Family\': {\'interaction\': \'&lt;string&gt; # e.g., visit, call, communication, etc.\', \'relation\': \'&lt;string&gt; # e.g., mother, son, etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, after shower, etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}, \'Pain\': {\'severity\': \'&lt;string&gt; # e.g., mild, moderate, severe, numeric scale if present, etc.\', \'location\': \'&lt;string&gt; # e.g., right knee, head, etc.\', \'duration\': \'&lt;string&gt; # e.g., all night, 3 hours, etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, after shower, etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}, \'Sleep\': {\'quality\': \'&lt;string&gt; # e.g., good, poor, restless, etc.\', \'duration\': \'&lt;string&gt; # e.g., 6 hours, phrases like "all night", etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, after shower, etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}}\n                                    If no relevant attribute exists for an event, return an empty object {}.\n                                    \n                        \n                        ---\n                                    Keyword evidence (Ki):\n                                    Additional facts: A keyword matching algorithm without context detected keyword(s) [\'aches\', \'urine\', \'son\', \'sleeping\', \'asleep\', \'sleep\', \'family\'].\n                                    Use this only as a pointer. If context contradicts, ignore.\n                        ---\n                        Output Schema (strict):\n                        {\n                                    "events": [\n                                        {\n                                        "event_type": "&lt;Pain | Sleep | Excretion | Eating | Family&gt;",\n                                        "text_quote": "&lt;fragement from the text indicating &gt;",\n                "attributes": {\n                    "&lt;attribute_name&gt;": "&lt;attribute_value&gt;"\n                }\n                                        }\n                                    ]\n                                    }\n                        \n                            Rules:\n                                - Ensure the output is valid JSON (parseable).\n                                - "eventS" must always be an array (can be empty).\n                                - Multiple instances of the same event type appear as individual elements in the event array.\n                                - Events appear in the array in the same order in which they appear in the text.\n                                - Do not include extra keys, comments, or text.\n                                - Each object in "events" must contain "event_type", "text_quote", and "attributes".\n                                -If an event attribute type has no value mentioned, return "attributes": {"&lt; attribute name &gt;:Unknown"} for each attribute type defined for the event type \n                        \n                        \n                        \n                        ', 'event_detection_time': 12.861335912006325}</t>
-        </is>
-      </c>
       <c r="J9" t="inlineStr">
         <is>
-          <t>['Sleep', 'Pain', 'Excretion', 'Family', 'Sleep']</t>
+          <t>[[]]</t>
         </is>
       </c>
       <c r="K9" t="inlineStr">
         <is>
-          <t>[{'Sleep': {'quality': 'poor', 'duration': 'short intervals', 'negation': False, 'time': 'night'}}, {'Pain': {'severity': 'Unknown', 'location': 'generalized', 'duration': 'Unknown', 'negation': False, 'time': 'night'}}, {'Excretion': {'type': 'urine', 'frequency': 'Unknown', 'quality': 'cloudy amber', 'negation': False, 'time': 'night'}}, {'Family': {'interaction': 'visit', 'relation': 'wife, son', 'negation': False, 'time': 'evening'}}, {'Sleep': {'quality': 'poor', 'duration': 'Unknown', 'negation': False, 'time': 'night'}}]</t>
+          <t>{'text': "ccu nursing progress note 7pm 3/21-7am [**3-14**]\ns:  i can't sleep at night at home either.  i walk around alot.\n\no:  patient sleeping only in short intervals, but states that this is normal for him.  sitting on side of bed to relieve generalized aches.\n\nt max 97.7\n\ncv - heart rate 56-62 sb/sr with no vea.  bp continues to be labile 80-150/59-70.  found that patient was initially on 1mg/min labetelol.  attempting to titrate down and while patient was asleep, labetolol was briefly off per bp.  but as patient is awake, labetolol resumed and increased up to 1mg/min for goal diastolic blood pressure 100-120/.  milrinone cont 0.375mcgs/kg/min and is unchanged.  pulses +1/+2 bilaterally.  mri tonight with no documented results.\n\nresp - ls are decreased at bases l&gt;r and o2 on 6ln/p.  patient denies sob.  patient is a mouth breather, so sat will decrease to 92% while patient is asleep, otherwise 95-97%.\n\ngu - foley patent cloudy amber urine 15-40cc/heart rate.\n\ngi - abd is soft with +bs.  no stool tonight.  tolerating by mouth's without difficulty.\n\nskin - l hand old iv site +2 edema, reddened with approx 2-3cm area of bruising noted.  covered with dsd. ho aware.  l elbow reddened contusion noted as well as area of pressure r buttocks.  areas washed with soap and water and left open to air.\n\nsocial - wife and son [**name (ni) **] patient this evening and have spoken and were updated by ho.\n\na:  84yom with aortic dissection c/b hypotension, cardiogenic shock now is stable on milrinone and labetolol.\n\np:  check am pnd lytes, hct and replete pro re nata, ? change iv labetolol to by mouth beta blocker, monitor bp response, cont pulse checks, monitor skin integrity and encourage turning and positioning to lessen pressure areas, cont to keep patient and family informed of all plans, treatments and goals.\n", 'event': ['Sleep', 'Pain', 'Family', 'Excretion', 'Sleep', 'Sleep'], 'event_id': ['e1', 'e2', 'e3', 'e4', 'e5', 'e6'], 'phrase': '', 'raw_output': '{\n  "events": [\n    {\n      "event_id": "e1",\n      "event_type": "Sleep",\n      "text_quote": "patient sleeping only in short intervals, but states that this is normal for him.",\n      "attributes": {\n        "quality": "poor",\n        "duration": "short intervals",\n        "negation": false,\n        "time": "night"\n      }\n    },\n    {\n      "event_id": "e2",\n      "event_type": "Pain",\n      "text_quote": "sitting on side of bed to relieve generalized aches.",\n      "attributes": {\n        "severity": "Unknown",\n        "location": "generalized",\n        "duration": "Unknown",\n        "negation": false,\n        "time": "night"\n      }\n    },\n    {\n      "event_id": "e3",\n      "event_type": "Family",\n      "text_quote": "wife and son [**name (ni) **] patient this evening and have spoken and were updated by ho.",\n      "attributes": {\n        "interaction": "visit",\n        "relation": "wife, son",\n        "negation": false,\n        "time": "evening"\n      }\n    },\n    {\n      "event_id": "e4",\n      "event_type": "Excretion",\n      "text_quote": "foley patent cloudy amber urine 15-40cc/heart rate.",\n      "attributes": {\n        "type": "urine",\n        "frequency": "Unknown",\n        "quality": "cloudy amber",\n        "negation": false,\n        "time": "night"\n      }\n    },\n    {\n      "event_id": "e5",\n      "event_type": "Sleep",\n      "text_quote": "i can\'t sleep at night at home either.",\n      "attributes": {\n        "quality": "poor",\n        "duration": "Unknown",\n        "negation": false,\n        "time": "night"\n      }\n    },\n    {\n      "event_id": "e6",\n      "event_type": "Sleep",\n      "text_quote": "sat will decrease to 92% while patient is asleep, otherwise 95-97%.",\n      "attributes": {\n        "quality": "Unknown",\n        "duration": "Unknown",\n        "negation": false,\n        "time": "night"\n      }\n    }\n  ],\n  "order": [\n    ["e1", "before", "e2"],\n    ["e2", "before", "e3"],\n    ["e3", "before", "e4"],\n    ["e4", "before", "e5"],\n    ["e5", "before", "e6"]\n  ]\n}', 'attributes': [{'Sleep': {'quality': 'poor', 'duration': 'short intervals', 'negation': False, 'time': 'night'}}, {'Pain': {'severity': 'Unknown', 'location': 'generalized', 'duration': 'Unknown', 'negation': False, 'time': 'night'}}, {'Family': {'interaction': 'visit', 'relation': 'wife, son', 'negation': False, 'time': 'evening'}}, {'Excretion': {'type': 'urine', 'frequency': 'Unknown', 'quality': 'cloudy amber', 'negation': False, 'time': 'night'}}, {'Sleep': {'quality': 'poor', 'duration': 'Unknown', 'negation': False, 'time': 'night'}}, {'Sleep': {'quality': 'Unknown', 'duration': 'Unknown', 'negation': False, 'time': 'night'}}], 'orders': [[['e1', 'before', 'e2'], ['e2', 'before', 'e3'], ['e3', 'before', 'e4'], ['e4', 'before', 'e5'], ['e5', 'before', 'e6']]], 'text_quotes': ['patient sleeping only in short intervals, but states that this is normal for him.', 'sitting on side of bed to relieve generalized aches.', 'wife and son [**name (ni) **] patient this evening and have spoken and were updated by ho.', 'foley patent cloudy amber urine 15-40cc/heart rate.', "i can't sleep at night at home either.", 'sat will decrease to 92% while patient is asleep, otherwise 95-97%.'], 'event_name_prompt': 'Given the text: ccu nursing progress note 7pm 3/21-7am [**3-14**]\ns:  i can\'t sleep at night at home either.  i walk around alot.\n\no:  patient sleeping only in short intervals, but states that this is normal for him.  sitting on side of bed to relieve generalized aches.\n\nt max 97.7\n\ncv - heart rate 56-62 sb/sr with no vea.  bp continues to be labile 80-150/59-70.  found that patient was initially on 1mg/min labetelol.  attempting to titrate down and while patient was asleep, labetolol was briefly off per bp.  but as patient is awake, labetolol resumed and increased up to 1mg/min for goal diastolic blood pressure 100-120/.  milrinone cont 0.375mcgs/kg/min and is unchanged.  pulses +1/+2 bilaterally.  mri tonight with no documented results.\n\nresp - ls are decreased at bases l&gt;r and o2 on 6ln/p.  patient denies sob.  patient is a mouth breather, so sat will decrease to 92% while patient is asleep, otherwise 95-97%.\n\ngu - foley patent cloudy amber urine 15-40cc/heart rate.\n\ngi - abd is soft with +bs.  no stool tonight.  tolerating by mouth\'s without difficulty.\n\nskin - l hand old iv site +2 edema, reddened with approx 2-3cm area of bruising noted.  covered with dsd. ho aware.  l elbow reddened contusion noted as well as area of pressure r buttocks.  areas washed with soap and water and left open to air.\n\nsocial - wife and son [**name (ni) **] patient this evening and have spoken and were updated by ho.\n\na:  84yom with aortic dissection c/b hypotension, cardiogenic shock now is stable on milrinone and labetolol.\n\np:  check am pnd lytes, hct and replete pro re nata, ? change iv labetolol to by mouth beta blocker, monitor bp response, cont pulse checks, monitor skin integrity and encourage turning and positioning to lessen pressure areas, cont to keep patient and family informed of all plans, treatments and goals.\n, \n                        and the following event types with their definitions: Eating : The patient takes food into their body by mouth.\nExcretion : The patient discharges waste matter from their body.\nFamily : The patient has a visit, call, or communication with a family member.\nPain : The patient reports or shows signs of pain.\nSleep : The patient sleeps or the sleep’s quality or quantity is described.\nUnknown : choose "Unknown" if none of the other event type are applicable. \n                        ---\n                        Your task:\n                        0. Identify ALL events in the text (zero, one, or more).\n1. For each event, assign an event_type from the list above.\n2. If multiple event of same type is mentioned, assign the event_type multiple times\n3. Extract attributes for each event using ONLY the allowed attributes listed below.\n4. Use keyword evidence (Ki) ONLY if it is consistent with the text context.\n5. Output strictly valid JSON following the schema below.\n                        ---\n                        Classification Rules:\n                        - A text may contain multiple events of the same or different types.\n- Create a separate event object for each event mention.\n- If the text is explicitly a NEGATION (e.g., "denies pain"), do not extract that event.\n- If the text describes a FUTURE or HYPOTHETICAL event (e.g., "will eat tomorrow"), ignore it.\n- A valid event should have occurred in the recent past or is occurring during the time of writing of the text.\n- If no events are found or if unsure, return {"events": []}\n                        \n                        ---\n                                    Attributes allowed:\n                                    {\'Eating\': {\'food\': \'&lt;string&gt; # e.g., pancakes, porridge, etc.\', \'amount\': \'&lt;string&gt; # e.g., 1, 2 bowls, etc.\', \'method\': \'&lt;string&gt;  # e.g., oral, tube, etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, evening etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}, \'Excretion\': {\'type\': \'&lt;string&gt; # e.g., urine, stool, etc.\', \'frequency\': \'&lt;string&gt; # e.g., 2x, once, etc.\', \'quality\': \'&lt;string&gt; # e.g., loose, hard, etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, evening etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}, \'Family\': {\'interaction\': \'&lt;string&gt; # e.g., visit, call, communication, etc.\', \'relation\': \'&lt;string&gt; # e.g., mother, son, etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, evening etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}, \'Pain\': {\'severity\': \'&lt;string&gt; # e.g., mild, moderate, severe, numeric scale if present, etc.\', \'location\': \'&lt;string&gt; # e.g., right knee, head, etc.\', \'duration\': \'&lt;string&gt; # e.g., all night, 3 hours, etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, evening etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}, \'Sleep\': {\'quality\': \'&lt;string&gt; # e.g., good, poor, restless, etc.\', \'duration\': \'&lt;string&gt; # e.g., 6 hours, phrases like "all night", etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, evening etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}}\n                                    If no relevant attribute exists for an event, return an empty object {}.\n                                    \n                        \n                        ---\n                                    Keyword evidence (Ki):\n                                    Additional facts: A keyword matching algorithm without context detected keyword(s) (\'asleep\', \'aches\', \'sleep\', \'son\', \'family\', \'urine\', \'sleeping\').\n                                    Use this only as a pointer. If context contradicts, ignore.\n                        ---\n                        Output Schema (strict):\n                        {\n                                    "events": [\n                                        {\n                                        "event_id": "&lt; A unique id eg.: e1 | e2 |...&gt;"\n                                        "event_type": "&lt;Pain | Sleep | Excretion | Eating | Family&gt;",\n                                        "text_quote": "&lt;fragement from the text indicating the event_type&gt;",\n                "attributes": {\n                    "&lt;attribute_name&gt;": "&lt;attribute_value&gt;"\n                }\n                                        }\n                                    ],\n                                    "order": [\n                                        ["e1", "before" | "after" | "simultaneous", "e2" ]\n                                    ]\n                                    }\n                        \n                            Rules:\n                                - Ensure the output is valid JSON (parseable).\n                                - "eventS" must always be an array (can be empty).\n                                - Multiple instances of the same event type appear with different ids.\n                                - Events appear in the array in the same order in which they appear in the text.\n                                - Their partial orders can be expressed using the "order" section.\n                                - Do not include extra keys, comments, or text.\n                                - Each object in "events" must contain "event_type", "text_quote", and "attributes".\n                                - If an event attribute type has no value mentioned, return "attributes": {"&lt; attribute name &gt;:Unknown"} for each attribute type defined for the event type \n                        \n                        \n                        \n                        ', 'event_detection_time': 18.639292717038188}</t>
         </is>
       </c>
       <c r="L9" t="inlineStr">
         <is>
-          <t>['patient sleeping only in short intervals, but states that this is normal for him.', 'sitting on side of bed to relieve generalized aches.', 'foley patent cloudy amber urine 15-40cc/heart rate.', 'wife and son [**name (ni) **] patient this evening and have spoken and were updated by ho.', "i can't sleep at night at home either."]</t>
+          <t>['Sleep', 'Pain', 'Family', 'Excretion', 'Sleep', 'Sleep']</t>
         </is>
       </c>
       <c r="M9" t="inlineStr">
         <is>
-          <t>{'text': "ccu nursing progress note 7pm 3/21-7am [**3-14**]\ns:  i can't sleep at night at home either.  i walk around alot.\n\no:  patient sleeping only in short intervals, but states that this is normal for him.  sitting on side of bed to relieve generalized aches.\n\nt max 97.7\n\ncv - heart rate 56-62 sb/sr with no vea.  bp continues to be labile 80-150/59-70.  found that patient was initially on 1mg/min labetelol.  attempting to titrate down and while patient was asleep, labetolol was briefly off per bp.  but as patient is awake, labetolol resumed and increased up to 1mg/min for goal diastolic blood pressure 100-120/.  milrinone cont 0.375mcgs/kg/min and is unchanged.  pulses +1/+2 bilaterally.  mri tonight with no documented results.\n\nresp - ls are decreased at bases l&gt;r and o2 on 6ln/p.  patient denies sob.  patient is a mouth breather, so sat will decrease to 92% while patient is asleep, otherwise 95-97%.\n\ngu - foley patent cloudy amber urine 15-40cc/heart rate.\n\ngi - abd is soft with +bs.  no stool tonight.  tolerating by mouth's without difficulty.\n\nskin - l hand old iv site +2 edema, reddened with approx 2-3cm area of bruising noted.  covered with dsd. ho aware.  l elbow reddened contusion noted as well as area of pressure r buttocks.  areas washed with soap and water and left open to air.\n\nsocial - wife and son [**name (ni) **] patient this evening and have spoken and were updated by ho.\n\na:  84yom with aortic dissection c/b hypotension, cardiogenic shock now is stable on milrinone and labetolol.\n\np:  check am pnd lytes, hct and replete pro re nata, ? change iv labetolol to by mouth beta blocker, monitor bp response, cont pulse checks, monitor skin integrity and encourage turning and positioning to lessen pressure areas, cont to keep patient and family informed of all plans, treatments and goals.\n", 'event': ['Sleep', 'Pain', 'Sleep', 'Excretion', 'Family'], 'phrase': '', 'raw_output': '{\n  "events": [\n    {\n      "event_type": "Sleep",\n      "text_quote": "i can\'t sleep at night at home either.",\n      "attributes": {"quality": "poor", \n                     "duration": "Unknown", \n                     "time":"night",\n                     "caused_by":"Unknown"}\n    },\n    {\n      "event_type": "Pain",\n      "text_quote": "sitting on side of bed to relieve generalized aches.",\n      "attributes": {"severity": "mild", \n                     "location": "generalized", \n                     "duration": "Unknown", \n                     "time":"Unknown",\n                     "caused_by":"Unknown"}\n    },\n    {\n      "event_type": "Sleep",\n      "text_quote": "patient sleeping only in short intervals, but states that this is normal for him.",\n      "attributes": {"quality": "poor", \n                     "duration": "short intervals", \n                     "time":"Unknown",\n                     "caused_by":"Unknown"}\n    },\n    {\n      "event_type": "Excretion",\n      "text_quote": "foley patent cloudy amber urine 15-40cc/heart rate.",\n      "attributes": {"type": "urine", \n                     "quality": "cloudy amber", \n                     "frequency":"15-40cc/heart rate", \n                     "time":"Unknown",\n                     "caused_by":"Unknown"}\n    },\n    {\n      "event_type": "Family",\n      "text_quote": "wife and son [**name (ni) **] patient this evening and have spoken and were updated by ho.",\n      "attributes": {"interaction": "visit", \n                     "relation": "wife, son", \n                     "time":"evening",\n                     "caused_by":"Unknown"}\n    }\n  ]\n}', 'attributes': [{'Sleep': {'quality': 'poor', 'duration': 'Unknown', 'time': 'night', 'caused_by': 'Unknown'}}, {'Pain': {'severity': 'mild', 'location': 'generalized', 'duration': 'Unknown', 'time': 'Unknown', 'caused_by': 'Unknown'}}, {'Sleep': {'quality': 'poor', 'duration': 'short intervals', 'time': 'Unknown', 'caused_by': 'Unknown'}}, {'Excretion': {'type': 'urine', 'quality': 'cloudy amber', 'frequency': '15-40cc/heart rate', 'time': 'Unknown', 'caused_by': 'Unknown'}}, {'Family': {'interaction': 'visit', 'relation': 'wife, son', 'time': 'evening', 'caused_by': 'Unknown'}}], 'text_quotes': ["i can't sleep at night at home either.", 'sitting on side of bed to relieve generalized aches.', 'patient sleeping only in short intervals, but states that this is normal for him.', 'foley patent cloudy amber urine 15-40cc/heart rate.', 'wife and son [**name (ni) **] patient this evening and have spoken and were updated by ho.'], 'event_name_prompt': 'Given the text: ccu nursing progress note 7pm 3/21-7am [**3-14**]\ns:  i can\'t sleep at night at home either.  i walk around alot.\n\no:  patient sleeping only in short intervals, but states that this is normal for him.  sitting on side of bed to relieve generalized aches.\n\nt max 97.7\n\ncv - heart rate 56-62 sb/sr with no vea.  bp continues to be labile 80-150/59-70.  found that patient was initially on 1mg/min labetelol.  attempting to titrate down and while patient was asleep, labetolol was briefly off per bp.  but as patient is awake, labetolol resumed and increased up to 1mg/min for goal diastolic blood pressure 100-120/.  milrinone cont 0.375mcgs/kg/min and is unchanged.  pulses +1/+2 bilaterally.  mri tonight with no documented results.\n\nresp - ls are decreased at bases l&gt;r and o2 on 6ln/p.  patient denies sob.  patient is a mouth breather, so sat will decrease to 92% while patient is asleep, otherwise 95-97%.\n\ngu - foley patent cloudy amber urine 15-40cc/heart rate.\n\ngi - abd is soft with +bs.  no stool tonight.  tolerating by mouth\'s without difficulty.\n\nskin - l hand old iv site +2 edema, reddened with approx 2-3cm area of bruising noted.  covered with dsd. ho aware.  l elbow reddened contusion noted as well as area of pressure r buttocks.  areas washed with soap and water and left open to air.\n\nsocial - wife and son [**name (ni) **] patient this evening and have spoken and were updated by ho.\n\na:  84yom with aortic dissection c/b hypotension, cardiogenic shock now is stable on milrinone and labetolol.\n\np:  check am pnd lytes, hct and replete pro re nata, ? change iv labetolol to by mouth beta blocker, monitor bp response, cont pulse checks, monitor skin integrity and encourage turning and positioning to lessen pressure areas, cont to keep patient and family informed of all plans, treatments and goals.\n, \n                        and the following event types with their definitions: Eating : The patient takes food into their body by mouth.\nExcretion : The patient discharges waste matter from their body.\nFamily : The patient has a visit, call, or communication with a family member.\nPain : The patient reports or shows signs of pain.\nSleep : The patient sleeps or the sleep’s quality or quantity is described.\nUnknown : choose "Unknown" if none of the other event type are applicable. \n                        ---\n                        Your task:\n                        0. Identify ALL events in the text (zero, one, or more).\n1. For each event, assign an event_type from the list above.\n2. If multiple event of same type is mentioned, assign the event_type multiple times\n3. Extract attributes for each event using ONLY the allowed attributes listed below.\n4. Output strictly valid JSON following the schema below.\n                        ---\n                        Classification Rules:\n                        - A text may contain multiple events of the same or different types.\n- Create a separate event object for each event mention.\n- If the text is explicitly a NEGATION (e.g., "denies pain"), do not extract that event.\n- If the text describes a FUTURE or HYPOTHETICAL event (e.g., "will eat tomorrow"), ignore it.\n- A valid event should have occurred in the recent past or is occurring during the time of writing of the text.\n- If no events are found or if unsure, return {"events": []}\n                        \n                        ---\n                                    Attributes allowed:\n                                    {\'Eating\': {\'food\': \'&lt;string&gt; # e.g., pancakes, porridge, etc.\', \'amount\': \'&lt;string&gt; # e.g., 1, 2 bowls, etc.\', \'method\': \'&lt;string&gt;  # e.g., oral, tube, etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, after shower, etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}, \'Excretion\': {\'type\': \'&lt;string&gt; # e.g., urine, stool, etc.\', \'frequency\': \'&lt;string&gt; # e.g., 2x, once, etc.\', \'quality\': \'&lt;string&gt; # e.g., loose, hard, etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, after shower, etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}, \'Family\': {\'interaction\': \'&lt;string&gt; # e.g., visit, call, communication, etc.\', \'relation\': \'&lt;string&gt; # e.g., mother, son, etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, after shower, etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}, \'Pain\': {\'severity\': \'&lt;string&gt; # e.g., mild, moderate, severe, numeric scale if present, etc.\', \'location\': \'&lt;string&gt; # e.g., right knee, head, etc.\', \'duration\': \'&lt;string&gt; # e.g., all night, 3 hours, etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, after shower, etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}, \'Sleep\': {\'quality\': \'&lt;string&gt; # e.g., good, poor, restless, etc.\', \'duration\': \'&lt;string&gt; # e.g., 6 hours, phrases like "all night", etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, after shower, etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}}\n                                    If no relevant attribute exists for an event, return an empty object {}.\n                                    \n                        \n                        \n                        ---\n                        Output Schema (strict):\n                        {\n                                    "events": [\n                                        {\n                                        "event_type": "&lt;Pain | Sleep | Excretion | Eating | Family&gt;",\n                                        "text_quote": "&lt;fragement from the text indicating &gt;",\n                "attributes": {\n                    "&lt;attribute_name&gt;": "&lt;attribute_value&gt;"\n                }\n                                        }\n                                    ]\n                                    }\n                        \n                            Rules:\n                                - Ensure the output is valid JSON (parseable).\n                                - "eventS" must always be an array (can be empty).\n                                - Multiple instances of the same event type appear as individual elements in the event array.\n                                - Events appear in the array in the same order in which they appear in the text.\n                                - Do not include extra keys, comments, or text.\n                                - Each object in "events" must contain "event_type", "text_quote", and "attributes".\n                                -If an event attribute type has no value mentioned, return "attributes": {"&lt; attribute name &gt;:Unknown"} for each attribute type defined for the event type \n                        \n                        \n                        \n                ---\n                Examples:\n                \n                text: "Patient ate breakfast this morning. He seems less anxious."\n                output: {\n                "events": [\n                    {\n                    "event_type": "Eating",\n                    "text_quote":"Patient ate breakfast this morning",\n                    "attributes": {"food": "breakfast", \n                                   "amount": "Unknown",\n                                   "method": "Unknown",\n                                   "time":"morning",\n                                   "caused_by":"Unknown"}\n                    }\n                ]\n                }\n                \n                text: "Patient reported severe abdominal pain."\n                output: {\n                "events": [\n                    {\n                    "event_type": "Pain",\n                    "text_quote": "severe abdominal Pain",\n                    "attributes": {"severity": "severe", \n                                   "location": "abdominal",\n                                   "duration": "Unknown",\n                                   "time":"Unknown",\n                                   "caused_by":"Unknown"}\n                    }\n                ]\n                }\n                \n                text: "Patient called his son around 3 pm."\n                output: {\n                "events": [\n                    {\n                    "event_type": "Family",\n                    "text_quote": "called his son around 3 pm",\n                    "attributes": {"interaction": "call", \n                                    "relation": "son",\n                                    "time":"3 pm",\n                                    "caused_by":"Unknown"}\n                    }\n                ]\n                }\n                \n                text: "Patient had a loose stool overnight."\n                output: {\n                "events": [\n                    {\n                    "event_type": "Excretion",\n                    "text_quote": "loose stool overnight",\n                    "attributes": {"type": "stool", \n                                   "quality": "loose", \n                                   "frequency":"overnight", \n                                   "time":"night",\n                                   "caused_by":"Unknown"}\n                    }\n                ]\n                }\n                \n                text: "Patient was able to sleep well last night."\n                output: {\n                "events": [\n                    {\n                    "event_type": "Sleep",\n                    "text_quote": "sleep well last night",\n                    "attributes": {"quality": "well",\n                                    "duration": "Unknown", \n                                    "time":"night",\n                                    "caused_by":"Unknown"}\n                    }\n                ]\n                }\n                \n                text: "The patient couldn\'t sleep due to severe pain."\n                output: {\n                "events": [\n                    {\n                    "event_type": "Sleep",\n                    "text_quote": "couldn\'t sleep",\n                    "attributes": {"quality": "poor", \n                                    "duration": "Unknown",\n                                   "time":"Unknown",\n                                   "caused_by":"Pain"}\n                    },\n                    {\n                    "event_type": "Pain",\n                    "text_quote": "severe pain",\n                    "attributes": {"severity": "severe", \n                                    "location": "Unknown", \n                                    "duration": "Unknown", \n                                   "time":"before Sleep",\n                                   "caused_by":"Unknown"}\n                    }\n                ]\n                }\n                \n                text: "The patient complained of severe back pain, was given Tylenol, but the pain persisted and he was then prescribed stronger morphine."\n                output: {\n                "events": [\n                    {\n                    "event_type": "Pain",\n                    "text_quote": "complained of severe back pain",\n                    "attributes": {"severity": "severe", \n                                    "location": "back",\n                                    "duration": "Unknown", \n                                    "time":"Unknown",\n                                    "caused_by":"Unknown"}\n                    },\n                    {\n                    "event_type": "Pain",\n                    "text_quote": "pain persisted",\n                    "attributes": {"severity": "severe", \n                                   "location": "back",\n                                   "duration": "persistent", \n                                   "time":"after Tylenol",\n                                   "caused_by":"Unknown"}\n                    }\n                ]\n                }\n                \n                        ', 'event_detection_time': 13.636018894001609}</t>
+          <t>[{'Sleep': {'quality': 'poor', 'duration': 'short intervals', 'negation': False, 'time': 'night'}}, {'Pain': {'severity': 'Unknown', 'location': 'generalized', 'duration': 'Unknown', 'negation': False, 'time': 'night'}}, {'Family': {'interaction': 'visit', 'relation': 'wife, son', 'negation': False, 'time': 'evening'}}, {'Excretion': {'type': 'urine', 'frequency': 'Unknown', 'quality': 'cloudy amber', 'negation': False, 'time': 'night'}}, {'Sleep': {'quality': 'poor', 'duration': 'Unknown', 'negation': False, 'time': 'night'}}, {'Sleep': {'quality': 'Unknown', 'duration': 'Unknown', 'negation': False, 'time': 'night'}}]</t>
         </is>
       </c>
       <c r="N9" t="inlineStr">
         <is>
-          <t>['Sleep', 'Pain', 'Sleep', 'Excretion', 'Family']</t>
+          <t>['patient sleeping only in short intervals, but states that this is normal for him.', 'sitting on side of bed to relieve generalized aches.', 'wife and son [**name (ni) **] patient this evening and have spoken and were updated by ho.', 'foley patent cloudy amber urine 15-40cc/heart rate.', "i can't sleep at night at home either.", 'sat will decrease to 92% while patient is asleep, otherwise 95-97%.']</t>
         </is>
       </c>
       <c r="O9" t="inlineStr">
         <is>
-          <t>[{'Sleep': {'quality': 'poor', 'duration': 'Unknown', 'time': 'night', 'caused_by': 'Unknown'}}, {'Pain': {'severity': 'mild', 'location': 'generalized', 'duration': 'Unknown', 'time': 'Unknown', 'caused_by': 'Unknown'}}, {'Sleep': {'quality': 'poor', 'duration': 'short intervals', 'time': 'Unknown', 'caused_by': 'Unknown'}}, {'Excretion': {'type': 'urine', 'quality': 'cloudy amber', 'frequency': '15-40cc/heart rate', 'time': 'Unknown', 'caused_by': 'Unknown'}}, {'Family': {'interaction': 'visit', 'relation': 'wife, son', 'time': 'evening', 'caused_by': 'Unknown'}}]</t>
-        </is>
-      </c>
-      <c r="P9" t="inlineStr">
-        <is>
-          <t>["i can't sleep at night at home either.", 'sitting on side of bed to relieve generalized aches.', 'patient sleeping only in short intervals, but states that this is normal for him.', 'foley patent cloudy amber urine 15-40cc/heart rate.', 'wife and son [**name (ni) **] patient this evening and have spoken and were updated by ho.']</t>
-        </is>
-      </c>
-      <c r="Q9" t="n">
-        <v>0.003180572000928805</v>
-      </c>
-      <c r="R9" t="inlineStr">
+          <t>[[['e1', 'before', 'e2'], ['e2', 'before', 'e3'], ['e3', 'before', 'e4'], ['e4', 'before', 'e5'], ['e5', 'before', 'e6']]]</t>
+        </is>
+      </c>
+      <c r="P9" t="n">
+        <v>0.002477226000337396</v>
+      </c>
+      <c r="Q9" t="inlineStr">
         <is>
           <t>Sleep</t>
         </is>
       </c>
-      <c r="S9" t="b">
-        <v>0</v>
+      <c r="R9" t="b">
+        <v>0</v>
+      </c>
+      <c r="S9" t="n">
+        <v>1</v>
       </c>
       <c r="T9" t="n">
         <v>1</v>
       </c>
-      <c r="U9" t="n">
-        <v>1</v>
-      </c>
-      <c r="V9" t="inlineStr">
+      <c r="U9" t="inlineStr">
         <is>
           <t>('asleep', 'sleep', 'son', 'family', 'urine', 'ache', 'sleeping')</t>
         </is>
       </c>
+      <c r="V9" t="n">
+        <v>17.08788670098875</v>
+      </c>
       <c r="W9" t="n">
-        <v>13.66099730499263</v>
+        <v>18.63929271703819</v>
       </c>
       <c r="X9" t="n">
-        <v>12.86133591200633</v>
+        <v>1</v>
       </c>
       <c r="Y9" t="n">
-        <v>13.63601889400161</v>
+        <v>1</v>
       </c>
       <c r="Z9" t="n">
-        <v>1</v>
-      </c>
-      <c r="AA9" t="n">
-        <v>1</v>
-      </c>
-      <c r="AB9" t="n">
-        <v>1</v>
-      </c>
-      <c r="AC9" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="10">
-      <c r="A10" t="n">
-        <v>1310487</v>
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>1310487</t>
+        </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>['Eating', 'Family', 'Unknown']</t>
+          <t>('Family', 'Eating', 'Unknown')</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>['family', 'daughter', 'eat']</t>
+          <t>('eat', 'family', 'daughter')</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
@@ -1699,120 +1616,111 @@
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>{'text': 'ccu npn 7a-7p\ns: " i don\'t eat much anymore...i\'male fine just looking out the window.\n\no: please see careview for vs and additional data.\n\ncv: heart rate 54-68 sb/nsr, no ectopy noted.  patient continues on labetalol and milrinone gtts.  labetalol drops titrated from off to 1.2 mg/min, milrinone titrated from 0.375 mcg/kg/min to 0.33 mcg/kg/min-milrinone to be titrated further overnoc.  patient abp 98-164/49-70-&gt; patient systolic 100-125 for most of shift, bp labile-fluctuates with wakening. pulses palp. hct 35 this am, to be redrawn this eve. patient to go to cath lab tomorrow am, per cardiac [**doctor first name **] note in chart-to examine hemodynamics and coronaries. mri results for aortic dissection status pending.\n\nresp: patient ls clear to coarse to diminished at bases, oxygen saturation 93-100 % on 6l n.c, rr 15-20, patient denies sob appears comfortable.\n\ngi/gu: patient abd soft, +bs x 4, no stool this shift.  patient with foley cath draining amber cloudy u/o to dark yellow clearing u/o, approx 15-40 cc/heart rate-patient to get lasix this eve.\n\nneuro: patient a&amp;o x 3, patient moves self to dangling on side of bed.  patient cooperative with care, patient quiet but responds appropriately to questions and engages in conversation with initiation. patient dozing intermittently throughout day.\n\nid: patient afebrile.\n\nsocial: patient wife and daughter in to visit patient today, aware of plan of care.\n\na/p: 84 year old male with aortic dissection-repair in 03, c/b cardiogenic shock, labile bp and arf-continues on labetalol drops d/t labile bp, milrinone drops titrating down, awaiting mri results-patient to cath lab tomorrrow am.  as discussed per interdisciplinary rounds, continue to monitor hemodynamics-titrate labetalol-change over to by mouth beta-blocker as patient condition tol.  continue to follow hct, lytes and update team on patient condition.  continue to monitor resp status, renal func and u/o.  continue to provide emotional support to patient and family.\n\n\n', 'event': ['Eating', 'Family', 'Sleep', 'Excretion', 'Excretion'], 'phrase': '', 'raw_output': '{\n  "events": [\n    {\n      "event_type": "Eating",\n      "text_quote": "i don\'t eat much anymore...",\n      "attributes": {\n        "food": "Unknown",\n        "amount": "little",\n        "method": "Unknown",\n        "negation": "false",\n        "time": "Unknown",\n        "caused_by": "Unknown"\n      }\n    },\n    {\n      "event_type": "Family",\n      "text_quote": "patient wife and daughter in to visit patient today",\n      "attributes": {\n        "interaction": "visit",\n        "relation": "wife, daughter",\n        "negation": "false",\n        "time": "today",\n        "caused_by": "Unknown"\n      }\n    },\n    {\n      "event_type": "Sleep",\n      "text_quote": "patient dozing intermittently throughout day",\n      "attributes": {\n        "quality": "intermittent",\n        "duration": "throughout the day",\n        "negation": "false",\n        "time": "day",\n        "caused_by": "Unknown"\n      }\n    },\n    {\n      "event_type": "Excretion",\n      "text_quote": "patient with foley cath draining amber cloudy u/o to dark yellow clearing u/o, approx 15-40 cc/heart rate",\n      "attributes": {\n        "type": "urine",\n        "frequency": "approx 15-40 cc/heart rate",\n        "quality": "amber cloudy to dark yellow clearing",\n        "negation": "false",\n        "time": "Unknown",\n        "caused_by": "Unknown"\n      }\n    },\n    {\n      "event_type": "Excretion",\n      "text_quote": "no stool this shift",\n      "attributes": {\n        "type": "stool",\n        "frequency": "none",\n        "quality": "Unknown",\n        "negation": "true",\n        "time": "this shift",\n        "caused_by": "Unknown"\n      }\n    }\n  ]\n}', 'attributes': [{'Eating': {'food': 'Unknown', 'amount': 'little', 'method': 'Unknown', 'negation': 'false', 'time': 'Unknown', 'caused_by': 'Unknown'}}, {'Family': {'interaction': 'visit', 'relation': 'wife, daughter', 'negation': 'false', 'time': 'today', 'caused_by': 'Unknown'}}, {'Sleep': {'quality': 'intermittent', 'duration': 'throughout the day', 'negation': 'false', 'time': 'day', 'caused_by': 'Unknown'}}, {'Excretion': {'type': 'urine', 'frequency': 'approx 15-40 cc/heart rate', 'quality': 'amber cloudy to dark yellow clearing', 'negation': 'false', 'time': 'Unknown', 'caused_by': 'Unknown'}}, {'Excretion': {'type': 'stool', 'frequency': 'none', 'quality': 'Unknown', 'negation': 'true', 'time': 'this shift', 'caused_by': 'Unknown'}}], 'text_quotes': ["i don't eat much anymore...", 'patient wife and daughter in to visit patient today', 'patient dozing intermittently throughout day', 'patient with foley cath draining amber cloudy u/o to dark yellow clearing u/o, approx 15-40 cc/heart rate', 'no stool this shift'], 'event_name_prompt': 'Given the text: ccu npn 7a-7p\ns: " i don\'t eat much anymore...i\'male fine just looking out the window.\n\no: please see careview for vs and additional data.\n\ncv: heart rate 54-68 sb/nsr, no ectopy noted.  patient continues on labetalol and milrinone gtts.  labetalol drops titrated from off to 1.2 mg/min, milrinone titrated from 0.375 mcg/kg/min to 0.33 mcg/kg/min-milrinone to be titrated further overnoc.  patient abp 98-164/49-70-&gt; patient systolic 100-125 for most of shift, bp labile-fluctuates with wakening. pulses palp. hct 35 this am, to be redrawn this eve. patient to go to cath lab tomorrow am, per cardiac [**doctor first name **] note in chart-to examine hemodynamics and coronaries. mri results for aortic dissection status pending.\n\nresp: patient ls clear to coarse to diminished at bases, oxygen saturation 93-100 % on 6l n.c, rr 15-20, patient denies sob appears comfortable.\n\ngi/gu: patient abd soft, +bs x 4, no stool this shift.  patient with foley cath draining amber cloudy u/o to dark yellow clearing u/o, approx 15-40 cc/heart rate-patient to get lasix this eve.\n\nneuro: patient a&amp;o x 3, patient moves self to dangling on side of bed.  patient cooperative with care, patient quiet but responds appropriately to questions and engages in conversation with initiation. patient dozing intermittently throughout day.\n\nid: patient afebrile.\n\nsocial: patient wife and daughter in to visit patient today, aware of plan of care.\n\na/p: 84 year old male with aortic dissection-repair in 03, c/b cardiogenic shock, labile bp and arf-continues on labetalol drops d/t labile bp, milrinone drops titrating down, awaiting mri results-patient to cath lab tomorrrow am.  as discussed per interdisciplinary rounds, continue to monitor hemodynamics-titrate labetalol-change over to by mouth beta-blocker as patient condition tol.  continue to follow hct, lytes and update team on patient condition.  continue to monitor resp status, renal func and u/o.  continue to provide emotional support to patient and family.\n\n\n, \n                        and the following event types with their definitions: Eating : The patient takes food into their body by mouth.\nExcretion : The patient discharges waste matter from their body.\nFamily : The patient has a visit, call, or communication with a family member.\nPain : The patient reports or shows signs of pain.\nSleep : The patient sleeps or the sleep’s quality or quantity is described.\nUnknown : choose "Unknown" if none of the other event type are applicable. \n                        ---\n                        Your task:\n                        0. Identify ALL events in the text (zero, one, or more).\n1. For each event, assign an event_type from the list above.\n2. If multiple event of same type is mentioned, assign the event_type multiple times\n3. Extract attributes for each event using ONLY the allowed attributes listed below.\n4. Use keyword evidence (Ki) ONLY if it is consistent with the text context.\n5. Output strictly valid JSON following the schema below.\n                        ---\n                        Classification Rules:\n                        - A text may contain multiple events of the same or different types.\n- Create a separate event object for each event mention.\n- If the text is explicitly a NEGATION (e.g., "denies pain"), do not extract that event.\n- If the text describes a FUTURE or HYPOTHETICAL event (e.g., "will eat tomorrow"), ignore it.\n- A valid event should have occurred in the recent past or is occurring during the time of writing of the text.\n- If no events are found or if unsure, return {"events": []}\n                        \n                        ---\n                                    Attributes allowed:\n                                    {\'Eating\': {\'food\': \'&lt;string&gt; # e.g., pancakes, porridge, etc.\', \'amount\': \'&lt;string&gt; # e.g., 1, 2 bowls, etc.\', \'method\': \'&lt;string&gt;  # e.g., oral, tube, etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, after shower, etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}, \'Excretion\': {\'type\': \'&lt;string&gt; # e.g., urine, stool, etc.\', \'frequency\': \'&lt;string&gt; # e.g., 2x, once, etc.\', \'quality\': \'&lt;string&gt; # e.g., loose, hard, etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, after shower, etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}, \'Family\': {\'interaction\': \'&lt;string&gt; # e.g., visit, call, communication, etc.\', \'relation\': \'&lt;string&gt; # e.g., mother, son, etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, after shower, etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}, \'Pain\': {\'severity\': \'&lt;string&gt; # e.g., mild, moderate, severe, numeric scale if present, etc.\', \'location\': \'&lt;string&gt; # e.g., right knee, head, etc.\', \'duration\': \'&lt;string&gt; # e.g., all night, 3 hours, etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, after shower, etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}, \'Sleep\': {\'quality\': \'&lt;string&gt; # e.g., good, poor, restless, etc.\', \'duration\': \'&lt;string&gt; # e.g., 6 hours, phrases like "all night", etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, after shower, etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}}\n                                    If no relevant attribute exists for an event, return an empty object {}.\n                                    \n                        \n                        ---\n                                    Keyword evidence (Ki):\n                                    Additional facts: A keyword matching algorithm without context detected keyword(s) [\'family\', \'daughter\', \'eat\'].\n                                    Use this only as a pointer. If context contradicts, ignore.\n                        ---\n                        Output Schema (strict):\n                        {\n                                    "events": [\n                                        {\n                                        "event_type": "&lt;Pain | Sleep | Excretion | Eating | Family&gt;",\n                                        "text_quote": "&lt;fragement from the text indicating &gt;",\n                "attributes": {\n                    "&lt;attribute_name&gt;": "&lt;attribute_value&gt;"\n                }\n                                        }\n                                    ]\n                                    }\n                        \n                            Rules:\n                                - Ensure the output is valid JSON (parseable).\n                                - "eventS" must always be an array (can be empty).\n                                - Multiple instances of the same event type appear as individual elements in the event array.\n                                - Events appear in the array in the same order in which they appear in the text.\n                                - Do not include extra keys, comments, or text.\n                                - Each object in "events" must contain "event_type", "text_quote", and "attributes".\n                                -If an event attribute type has no value mentioned, return "attributes": {"&lt; attribute name &gt;:Unknown"} for each attribute type defined for the event type \n                        \n                        \n                        \n                ---\n                Examples:\n                \n                text: "Patient ate breakfast this morning. He seems less anxious."\n                output: {\n                "events": [\n                    {\n                    "event_type": "Eating",\n                    "text_quote":"Patient ate breakfast this morning",\n                    "attributes": {"food": "breakfast", \n                                   "amount": "Unknown",\n                                   "method": "Unknown",\n                                   "time":"morning",\n                                   "caused_by":"Unknown"}\n                    }\n                ]\n                }\n                \n                text: "Patient reported severe abdominal pain."\n                output: {\n                "events": [\n                    {\n                    "event_type": "Pain",\n                    "text_quote": "severe abdominal Pain",\n                    "attributes": {"severity": "severe", \n                                   "location": "abdominal",\n                                   "duration": "Unknown",\n                                   "time":"Unknown",\n                                   "caused_by":"Unknown"}\n                    }\n                ]\n                }\n                \n                text: "Patient called his son around 3 pm."\n                output: {\n                "events": [\n                    {\n                    "event_type": "Family",\n                    "text_quote": "called his son around 3 pm",\n                    "attributes": {"interaction": "call", \n                                    "relation": "son",\n                                    "time":"3 pm",\n                                    "caused_by":"Unknown"}\n                    }\n                ]\n                }\n                \n                text: "Patient had a loose stool overnight."\n                output: {\n                "events": [\n                    {\n                    "event_type": "Excretion",\n                    "text_quote": "loose stool overnight",\n                    "attributes": {"type": "stool", \n                                   "quality": "loose", \n                                   "frequency":"overnight", \n                                   "time":"night",\n                                   "caused_by":"Unknown"}\n                    }\n                ]\n                }\n                \n                text: "Patient was able to sleep well last night."\n                output: {\n                "events": [\n                    {\n                    "event_type": "Sleep",\n                    "text_quote": "sleep well last night",\n                    "attributes": {"quality": "well",\n                                    "duration": "Unknown", \n                                    "time":"night",\n                                    "caused_by":"Unknown"}\n                    }\n                ]\n                }\n                \n                text: "The patient couldn\'t sleep due to severe pain."\n                output: {\n                "events": [\n                    {\n                    "event_type": "Sleep",\n                    "text_quote": "couldn\'t sleep",\n                    "attributes": {"quality": "poor", \n                                    "duration": "Unknown",\n                                   "time":"Unknown",\n                                   "caused_by":"Pain"}\n                    },\n                    {\n                    "event_type": "Pain",\n                    "text_quote": "severe pain",\n                    "attributes": {"severity": "severe", \n                                    "location": "Unknown", \n                                    "duration": "Unknown", \n                                   "time":"before Sleep",\n                                   "caused_by":"Unknown"}\n                    }\n                ]\n                }\n                \n                text: "The patient complained of severe back pain, was given Tylenol, but the pain persisted and he was then prescribed stronger morphine."\n                output: {\n                "events": [\n                    {\n                    "event_type": "Pain",\n                    "text_quote": "complained of severe back pain",\n                    "attributes": {"severity": "severe", \n                                    "location": "back",\n                                    "duration": "Unknown", \n                                    "time":"Unknown",\n                                    "caused_by":"Unknown"}\n                    },\n                    {\n                    "event_type": "Pain",\n                    "text_quote": "pain persisted",\n                    "attributes": {"severity": "severe", \n                                   "location": "back",\n                                   "duration": "persistent", \n                                   "time":"after Tylenol",\n                                   "caused_by":"Unknown"}\n                    }\n                ]\n                }\n                \n                        ', 'event_detection_time': 15.26224031500169}</t>
+          <t>['eat', 'family', 'daughter']</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>['Eating', 'Family', 'Sleep', 'Excretion', 'Excretion']</t>
+          <t>{'text': 'ccu npn 7a-7p\ns: " i don\'t eat much anymore...i\'male fine just looking out the window.\n\no: please see careview for vs and additional data.\n\ncv: heart rate 54-68 sb/nsr, no ectopy noted.  patient continues on labetalol and milrinone gtts.  labetalol drops titrated from off to 1.2 mg/min, milrinone titrated from 0.375 mcg/kg/min to 0.33 mcg/kg/min-milrinone to be titrated further overnoc.  patient abp 98-164/49-70-&gt; patient systolic 100-125 for most of shift, bp labile-fluctuates with wakening. pulses palp. hct 35 this am, to be redrawn this eve. patient to go to cath lab tomorrow am, per cardiac [**doctor first name **] note in chart-to examine hemodynamics and coronaries. mri results for aortic dissection status pending.\n\nresp: patient ls clear to coarse to diminished at bases, oxygen saturation 93-100 % on 6l n.c, rr 15-20, patient denies sob appears comfortable.\n\ngi/gu: patient abd soft, +bs x 4, no stool this shift.  patient with foley cath draining amber cloudy u/o to dark yellow clearing u/o, approx 15-40 cc/heart rate-patient to get lasix this eve.\n\nneuro: patient a&amp;o x 3, patient moves self to dangling on side of bed.  patient cooperative with care, patient quiet but responds appropriately to questions and engages in conversation with initiation. patient dozing intermittently throughout day.\n\nid: patient afebrile.\n\nsocial: patient wife and daughter in to visit patient today, aware of plan of care.\n\na/p: 84 year old male with aortic dissection-repair in 03, c/b cardiogenic shock, labile bp and arf-continues on labetalol drops d/t labile bp, milrinone drops titrating down, awaiting mri results-patient to cath lab tomorrrow am.  as discussed per interdisciplinary rounds, continue to monitor hemodynamics-titrate labetalol-change over to by mouth beta-blocker as patient condition tol.  continue to follow hct, lytes and update team on patient condition.  continue to monitor resp status, renal func and u/o.  continue to provide emotional support to patient and family.\n\n\n', 'event': ['Eating', 'Family', 'Sleep', 'Excretion'], 'event_id': ['e1', 'e2', 'e3', 'e4'], 'phrase': '', 'raw_output': '{\n  "events": [\n    {\n      "event_id": "e1",\n      "event_type": "Eating",\n      "text_quote": "i don\'t eat much anymore",\n      "attributes": {\n        "food": "Unknown",\n        "amount": "Unknown",\n        "method": "Unknown",\n        "negation": "true",\n        "time": "Unknown",\n        "caused_by": "Unknown"\n      }\n    },\n    {\n      "event_id": "e2",\n      "event_type": "Family",\n      "text_quote": "patient wife and daughter in to visit patient today",\n      "attributes": {\n        "interaction": "visit",\n        "relation": "wife, daughter",\n        "negation": "false",\n        "time": "today",\n        "caused_by": "Unknown"\n      }\n    },\n    {\n      "event_id": "e3",\n      "event_type": "Sleep",\n      "text_quote": "patient dozing intermittently throughout day",\n      "attributes": {\n        "quality": "intermittent",\n        "duration": "throughout the day",\n        "negation": "false",\n        "time": "day",\n        "caused_by": "Unknown"\n      }\n    },\n    {\n      "event_id": "e4",\n      "event_type": "Excretion",\n      "text_quote": "patient with foley cath draining amber cloudy u/o to dark yellow clearing u/o, approx 15-40 cc/heart rate",\n      "attributes": {\n        "type": "urine",\n        "frequency": "approx 15-40 cc/heart rate",\n        "quality": "amber cloudy to dark yellow clearing",\n        "negation": "false",\n        "time": "Unknown",\n        "caused_by": "Unknown"\n      }\n    }\n  ],\n  "order": []\n}', 'attributes': [{'Eating': {'food': 'Unknown', 'amount': 'Unknown', 'method': 'Unknown', 'negation': 'true', 'time': 'Unknown', 'caused_by': 'Unknown'}}, {'Family': {'interaction': 'visit', 'relation': 'wife, daughter', 'negation': 'false', 'time': 'today', 'caused_by': 'Unknown'}}, {'Sleep': {'quality': 'intermittent', 'duration': 'throughout the day', 'negation': 'false', 'time': 'day', 'caused_by': 'Unknown'}}, {'Excretion': {'type': 'urine', 'frequency': 'approx 15-40 cc/heart rate', 'quality': 'amber cloudy to dark yellow clearing', 'negation': 'false', 'time': 'Unknown', 'caused_by': 'Unknown'}}], 'orders': [[]], 'text_quotes': ["i don't eat much anymore", 'patient wife and daughter in to visit patient today', 'patient dozing intermittently throughout day', 'patient with foley cath draining amber cloudy u/o to dark yellow clearing u/o, approx 15-40 cc/heart rate'], 'event_name_prompt': 'Given the text: ccu npn 7a-7p\ns: " i don\'t eat much anymore...i\'male fine just looking out the window.\n\no: please see careview for vs and additional data.\n\ncv: heart rate 54-68 sb/nsr, no ectopy noted.  patient continues on labetalol and milrinone gtts.  labetalol drops titrated from off to 1.2 mg/min, milrinone titrated from 0.375 mcg/kg/min to 0.33 mcg/kg/min-milrinone to be titrated further overnoc.  patient abp 98-164/49-70-&gt; patient systolic 100-125 for most of shift, bp labile-fluctuates with wakening. pulses palp. hct 35 this am, to be redrawn this eve. patient to go to cath lab tomorrow am, per cardiac [**doctor first name **] note in chart-to examine hemodynamics and coronaries. mri results for aortic dissection status pending.\n\nresp: patient ls clear to coarse to diminished at bases, oxygen saturation 93-100 % on 6l n.c, rr 15-20, patient denies sob appears comfortable.\n\ngi/gu: patient abd soft, +bs x 4, no stool this shift.  patient with foley cath draining amber cloudy u/o to dark yellow clearing u/o, approx 15-40 cc/heart rate-patient to get lasix this eve.\n\nneuro: patient a&amp;o x 3, patient moves self to dangling on side of bed.  patient cooperative with care, patient quiet but responds appropriately to questions and engages in conversation with initiation. patient dozing intermittently throughout day.\n\nid: patient afebrile.\n\nsocial: patient wife and daughter in to visit patient today, aware of plan of care.\n\na/p: 84 year old male with aortic dissection-repair in 03, c/b cardiogenic shock, labile bp and arf-continues on labetalol drops d/t labile bp, milrinone drops titrating down, awaiting mri results-patient to cath lab tomorrrow am.  as discussed per interdisciplinary rounds, continue to monitor hemodynamics-titrate labetalol-change over to by mouth beta-blocker as patient condition tol.  continue to follow hct, lytes and update team on patient condition.  continue to monitor resp status, renal func and u/o.  continue to provide emotional support to patient and family.\n\n\n, \n                        and the following event types with their definitions: Eating : The patient takes food into their body by mouth.\nExcretion : The patient discharges waste matter from their body.\nFamily : The patient has a visit, call, or communication with a family member.\nPain : The patient reports or shows signs of pain.\nSleep : The patient sleeps or the sleep’s quality or quantity is described.\nUnknown : choose "Unknown" if none of the other event type are applicable. \n                        ---\n                        Your task:\n                        0. Identify ALL events in the text (zero, one, or more).\n1. For each event, assign an event_type from the list above.\n2. If multiple event of same type is mentioned, assign the event_type multiple times\n3. Extract attributes for each event using ONLY the allowed attributes listed below.\n4. Use keyword evidence (Ki) ONLY if it is consistent with the text context.\n5. Output strictly valid JSON following the schema below.\n                        ---\n                        Classification Rules:\n                        - A text may contain multiple events of the same or different types.\n- Create a separate event object for each event mention.\n- If the text is explicitly a NEGATION (e.g., "denies pain"), do not extract that event.\n- If the text describes a FUTURE or HYPOTHETICAL event (e.g., "will eat tomorrow"), ignore it.\n- A valid event should have occurred in the recent past or is occurring during the time of writing of the text.\n- If no events are found or if unsure, return {"events": []}\n                        \n                        ---\n                                    Attributes allowed:\n                                    {\'Eating\': {\'food\': \'&lt;string&gt; # e.g., pancakes, porridge, etc.\', \'amount\': \'&lt;string&gt; # e.g., 1, 2 bowls, etc.\', \'method\': \'&lt;string&gt;  # e.g., oral, tube, etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, evening etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}, \'Excretion\': {\'type\': \'&lt;string&gt; # e.g., urine, stool, etc.\', \'frequency\': \'&lt;string&gt; # e.g., 2x, once, etc.\', \'quality\': \'&lt;string&gt; # e.g., loose, hard, etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, evening etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}, \'Family\': {\'interaction\': \'&lt;string&gt; # e.g., visit, call, communication, etc.\', \'relation\': \'&lt;string&gt; # e.g., mother, son, etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, evening etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}, \'Pain\': {\'severity\': \'&lt;string&gt; # e.g., mild, moderate, severe, numeric scale if present, etc.\', \'location\': \'&lt;string&gt; # e.g., right knee, head, etc.\', \'duration\': \'&lt;string&gt; # e.g., all night, 3 hours, etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, evening etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}, \'Sleep\': {\'quality\': \'&lt;string&gt; # e.g., good, poor, restless, etc.\', \'duration\': \'&lt;string&gt; # e.g., 6 hours, phrases like "all night", etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, evening etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}}\n                                    If no relevant attribute exists for an event, return an empty object {}.\n                                    \n                        \n                        ---\n                                    Keyword evidence (Ki):\n                                    Additional facts: A keyword matching algorithm without context detected keyword(s) (\'eat\', \'family\', \'daughter\').\n                                    Use this only as a pointer. If context contradicts, ignore.\n                        ---\n                        Output Schema (strict):\n                        {\n                                    "events": [\n                                        {\n                                        "event_id": "&lt; A unique id eg.: e1 | e2 |...&gt;"\n                                        "event_type": "&lt;Pain | Sleep | Excretion | Eating | Family&gt;",\n                                        "text_quote": "&lt;fragement from the text indicating the event_type&gt;",\n                "attributes": {\n                    "&lt;attribute_name&gt;": "&lt;attribute_value&gt;"\n                }\n                                        }\n                                    ],\n                                    "order": [\n                                        ["e1", "before" | "after" | "simultaneous", "e2" ]\n                                    ]\n                                    }\n                        \n                            Rules:\n                                - Ensure the output is valid JSON (parseable).\n                                - "eventS" must always be an array (can be empty).\n                                - Multiple instances of the same event type appear with different ids.\n                                - Events appear in the array in the same order in which they appear in the text.\n                                - Their partial orders can be expressed using the "order" section.\n                                - Do not include extra keys, comments, or text.\n                                - Each object in "events" must contain "event_type", "text_quote", and "attributes".\n                                - If an event attribute type has no value mentioned, return "attributes": {"&lt; attribute name &gt;:Unknown"} for each attribute type defined for the event type \n                        \n                        \n                        \n                ---\n                Examples:\n                \n                text: "Patient ate breakfast this morning. He seems less anxious."\n                output: {\n                "events": [\n                    {"event_id": "e1",\n                    "event_type": "Eating",\n                    "text_quote":"Patient ate breakfast this morning",\n                    "attributes": {"food": "breakfast", \n                                   "amount": "Unknown",\n                                   "method": "Unknown",\n                                   "negation": "false",\n                                   "time":"morning",\n                                   "caused_by":"Unknown"}\n                    }\n                ],\n                "order":[]\n                }\n                \n                text: "Patient reported severe abdominal pain."\n                output: {\n                "events": [\n                    {"event_id": "e1",\n                    "event_type": "Pain",\n                    "text_quote": "severe abdominal Pain",\n                    "attributes": {"severity": "severe", \n                                   "location": "abdominal",\n                                   "duration": "Unknown",\n                                   "negation": "false",\n                                   "time":"Unknown",\n                                   "caused_by":"Unknown"}\n                    }\n                ],\n                "order":[]\n                }\n                \n                text: "Patient called his son around 3 pm."\n                output: {\n                "events": [\n                    {"event_id": "e1",\n                    "event_type": "Family",\n                    "text_quote": "called his son around 3 pm",\n                    "attributes": {"interaction": "call", \n                                    "relation": "son",\n                                    "negation": "false",\n                                    "time":"3 pm",\n                                    "caused_by":"Unknown"}\n                    }\n                ],\n                "order":[]\n                }\n                \n                text: "Patient had a loose stool overnight."\n                output: {\n                "events": [\n                    {"event_id": "e1",\n                    "event_type": "Excretion",\n                    "text_quote": "loose stool overnight",\n                    "attributes": {"type": "stool", \n                                   "quality": "loose", \n                                   "frequency":"overnight", \n                                   "negation": "false",\n                                   "time":"night",\n                                   "caused_by":"Unknown"}\n                    }\n                ],\n                "order":[]\n                }\n                \n                text: "Patient was able to sleep well last night."\n                output: {\n                "events": [\n                    {"event_id": "e1",\n                    "event_type": "Sleep",\n                    "text_quote": "sleep well last night",\n                    "attributes": {"quality": "well",\n                                    "duration": "Unknown", \n                                    "negation": "false",\n                                    "time":"night",\n                                    "caused_by":"Unknown"}\n                    }\n                ],\n                "order":[]\n                }\n                \n                text: "The patient couldn\'t sleep due to severe pain."\n                output: {\n                "events": [\n                    {"event_id": "e1",\n                    "event_type": "Sleep",\n                    "text_quote": "couldn\'t sleep",\n                    "attributes": {"quality": "poor", \n                                    "duration": "Unknown",\n                                    "negation": "true",\n                                    "time":"Unknown",\n                                    "caused_by":"Pain"}\n                    },\n                    {"event_id": "e2",\n                    "event_type": "Pain",\n                    "text_quote": "severe pain",\n                    "attributes": {"severity": "severe", \n                                    "location": "Unknown", \n                                    "duration": "Unknown", \n                                    "time":"Unknown",\n                                    "caused_by":"Unknown"}\n                    }\n                ],\n                "order":["e1", "after", "e2"]\n                }\n                \n                text: "The patient complained of severe back pain, was given Tylenol, but the pain persisted and he was then prescribed stronger morphine."\n                output: {\n                "events": [\n                    {"event_id": "e1",\n                    "event_type": "Pain",\n                    "text_quote": "complained of severe back pain",\n                    "attributes": {"severity": "severe", \n                                    "location": "back",\n                                    "duration": "Unknown", \n                                    "time":"Unknown",\n                                    "caused_by":"Unknown"}\n                    },\n                    {"event_id": "e2",\n                    "event_type": "Pain",\n                    "text_quote": "pain persisted",\n                    "attributes": {"severity": "severe", \n                                   "location": "back",\n                                   "duration": "persistent", \n                                   "time":"after Tylenol",\n                                   "caused_by":"Unknown"}\n                    }\n                ],\n                "order":[["e1", "before", "e2"]]\n                }\n                \n                        ', 'event_detection_time': 14.486266430991236}</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>[{'Eating': {'food': 'Unknown', 'amount': 'little', 'method': 'Unknown', 'negation': 'false', 'time': 'Unknown', 'caused_by': 'Unknown'}}, {'Family': {'interaction': 'visit', 'relation': 'wife, daughter', 'negation': 'false', 'time': 'today', 'caused_by': 'Unknown'}}, {'Sleep': {'quality': 'intermittent', 'duration': 'throughout the day', 'negation': 'false', 'time': 'day', 'caused_by': 'Unknown'}}, {'Excretion': {'type': 'urine', 'frequency': 'approx 15-40 cc/heart rate', 'quality': 'amber cloudy to dark yellow clearing', 'negation': 'false', 'time': 'Unknown', 'caused_by': 'Unknown'}}, {'Excretion': {'type': 'stool', 'frequency': 'none', 'quality': 'Unknown', 'negation': 'true', 'time': 'this shift', 'caused_by': 'Unknown'}}]</t>
+          <t>['Eating', 'Family', 'Sleep', 'Excretion']</t>
         </is>
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>["i don't eat much anymore...", 'patient wife and daughter in to visit patient today', 'patient dozing intermittently throughout day', 'patient with foley cath draining amber cloudy u/o to dark yellow clearing u/o, approx 15-40 cc/heart rate', 'no stool this shift']</t>
+          <t>[{'Eating': {'food': 'Unknown', 'amount': 'Unknown', 'method': 'Unknown', 'negation': 'true', 'time': 'Unknown', 'caused_by': 'Unknown'}}, {'Family': {'interaction': 'visit', 'relation': 'wife, daughter', 'negation': 'false', 'time': 'today', 'caused_by': 'Unknown'}}, {'Sleep': {'quality': 'intermittent', 'duration': 'throughout the day', 'negation': 'false', 'time': 'day', 'caused_by': 'Unknown'}}, {'Excretion': {'type': 'urine', 'frequency': 'approx 15-40 cc/heart rate', 'quality': 'amber cloudy to dark yellow clearing', 'negation': 'false', 'time': 'Unknown', 'caused_by': 'Unknown'}}]</t>
         </is>
       </c>
       <c r="I10" t="inlineStr">
         <is>
-          <t>{'text': 'ccu npn 7a-7p\ns: " i don\'t eat much anymore...i\'male fine just looking out the window.\n\no: please see careview for vs and additional data.\n\ncv: heart rate 54-68 sb/nsr, no ectopy noted.  patient continues on labetalol and milrinone gtts.  labetalol drops titrated from off to 1.2 mg/min, milrinone titrated from 0.375 mcg/kg/min to 0.33 mcg/kg/min-milrinone to be titrated further overnoc.  patient abp 98-164/49-70-&gt; patient systolic 100-125 for most of shift, bp labile-fluctuates with wakening. pulses palp. hct 35 this am, to be redrawn this eve. patient to go to cath lab tomorrow am, per cardiac [**doctor first name **] note in chart-to examine hemodynamics and coronaries. mri results for aortic dissection status pending.\n\nresp: patient ls clear to coarse to diminished at bases, oxygen saturation 93-100 % on 6l n.c, rr 15-20, patient denies sob appears comfortable.\n\ngi/gu: patient abd soft, +bs x 4, no stool this shift.  patient with foley cath draining amber cloudy u/o to dark yellow clearing u/o, approx 15-40 cc/heart rate-patient to get lasix this eve.\n\nneuro: patient a&amp;o x 3, patient moves self to dangling on side of bed.  patient cooperative with care, patient quiet but responds appropriately to questions and engages in conversation with initiation. patient dozing intermittently throughout day.\n\nid: patient afebrile.\n\nsocial: patient wife and daughter in to visit patient today, aware of plan of care.\n\na/p: 84 year old male with aortic dissection-repair in 03, c/b cardiogenic shock, labile bp and arf-continues on labetalol drops d/t labile bp, milrinone drops titrating down, awaiting mri results-patient to cath lab tomorrrow am.  as discussed per interdisciplinary rounds, continue to monitor hemodynamics-titrate labetalol-change over to by mouth beta-blocker as patient condition tol.  continue to follow hct, lytes and update team on patient condition.  continue to monitor resp status, renal func and u/o.  continue to provide emotional support to patient and family.\n\n\n', 'event': ['Eating', 'Family', 'Sleep', 'Excretion', 'Excretion'], 'phrase': '', 'raw_output': '{\n  "events": [\n    {\n      "event_type": "Eating",\n      "text_quote": "i don\'t eat much anymore...",\n      "attributes": {\n        "food": "Unknown",\n        "amount": "Unknown",\n        "method": "Unknown",\n        "negation": true,\n        "time": "Unknown",\n        "caused_by": "Unknown"\n      }\n    },\n    {\n      "event_type": "Family",\n      "text_quote": "patient wife and daughter in to visit patient today, aware of plan of care.",\n      "attributes": {\n        "interaction": "visit",\n        "relation": "wife and daughter",\n        "negation": false,\n        "time": "today",\n        "caused_by": "Unknown"\n      }\n    },\n    {\n      "event_type": "Sleep",\n      "text_quote": "patient dozing intermittently throughout day.",\n      "attributes": {\n        "quality": "intermittent",\n        "duration": "throughout the day",\n        "negation": false,\n        "time": "day",\n        "caused_by": "Unknown"\n      }\n    },\n    {\n      "event_type": "Excretion",\n      "text_quote": "patient with foley cath draining amber cloudy u/o to dark yellow clearing u/o, approx 15-40 cc/heart rate-patient to get lasix this eve.",\n      "attributes": {\n        "type": "urine",\n        "frequency": "Unknown",\n        "quality": "amber cloudy to dark yellow clearing",\n        "negation": false,\n        "time": "eve",\n        "caused_by": "foley cath"\n      }\n    },\n    {\n      "event_type": "Excretion",\n      "text_quote": "patient abd soft, +bs x 4, no stool this shift.",\n      "attributes": {\n        "type": "stool",\n        "frequency": "none",\n        "quality": "Unknown",\n        "negation": true,\n        "time": "this shift",\n        "caused_by": "Unknown"\n      }\n    }\n  ]\n}', 'attributes': [{'Eating': {'food': 'Unknown', 'amount': 'Unknown', 'method': 'Unknown', 'negation': True, 'time': 'Unknown', 'caused_by': 'Unknown'}}, {'Family': {'interaction': 'visit', 'relation': 'wife and daughter', 'negation': False, 'time': 'today', 'caused_by': 'Unknown'}}, {'Sleep': {'quality': 'intermittent', 'duration': 'throughout the day', 'negation': False, 'time': 'day', 'caused_by': 'Unknown'}}, {'Excretion': {'type': 'urine', 'frequency': 'Unknown', 'quality': 'amber cloudy to dark yellow clearing', 'negation': False, 'time': 'eve', 'caused_by': 'foley cath'}}, {'Excretion': {'type': 'stool', 'frequency': 'none', 'quality': 'Unknown', 'negation': True, 'time': 'this shift', 'caused_by': 'Unknown'}}], 'text_quotes': ["i don't eat much anymore...", 'patient wife and daughter in to visit patient today, aware of plan of care.', 'patient dozing intermittently throughout day.', 'patient with foley cath draining amber cloudy u/o to dark yellow clearing u/o, approx 15-40 cc/heart rate-patient to get lasix this eve.', 'patient abd soft, +bs x 4, no stool this shift.'], 'event_name_prompt': 'Given the text: ccu npn 7a-7p\ns: " i don\'t eat much anymore...i\'male fine just looking out the window.\n\no: please see careview for vs and additional data.\n\ncv: heart rate 54-68 sb/nsr, no ectopy noted.  patient continues on labetalol and milrinone gtts.  labetalol drops titrated from off to 1.2 mg/min, milrinone titrated from 0.375 mcg/kg/min to 0.33 mcg/kg/min-milrinone to be titrated further overnoc.  patient abp 98-164/49-70-&gt; patient systolic 100-125 for most of shift, bp labile-fluctuates with wakening. pulses palp. hct 35 this am, to be redrawn this eve. patient to go to cath lab tomorrow am, per cardiac [**doctor first name **] note in chart-to examine hemodynamics and coronaries. mri results for aortic dissection status pending.\n\nresp: patient ls clear to coarse to diminished at bases, oxygen saturation 93-100 % on 6l n.c, rr 15-20, patient denies sob appears comfortable.\n\ngi/gu: patient abd soft, +bs x 4, no stool this shift.  patient with foley cath draining amber cloudy u/o to dark yellow clearing u/o, approx 15-40 cc/heart rate-patient to get lasix this eve.\n\nneuro: patient a&amp;o x 3, patient moves self to dangling on side of bed.  patient cooperative with care, patient quiet but responds appropriately to questions and engages in conversation with initiation. patient dozing intermittently throughout day.\n\nid: patient afebrile.\n\nsocial: patient wife and daughter in to visit patient today, aware of plan of care.\n\na/p: 84 year old male with aortic dissection-repair in 03, c/b cardiogenic shock, labile bp and arf-continues on labetalol drops d/t labile bp, milrinone drops titrating down, awaiting mri results-patient to cath lab tomorrrow am.  as discussed per interdisciplinary rounds, continue to monitor hemodynamics-titrate labetalol-change over to by mouth beta-blocker as patient condition tol.  continue to follow hct, lytes and update team on patient condition.  continue to monitor resp status, renal func and u/o.  continue to provide emotional support to patient and family.\n\n\n, \n                        and the following event types with their definitions: Eating : The patient takes food into their body by mouth.\nExcretion : The patient discharges waste matter from their body.\nFamily : The patient has a visit, call, or communication with a family member.\nPain : The patient reports or shows signs of pain.\nSleep : The patient sleeps or the sleep’s quality or quantity is described.\nUnknown : choose "Unknown" if none of the other event type are applicable. \n                        ---\n                        Your task:\n                        0. Identify ALL events in the text (zero, one, or more).\n1. For each event, assign an event_type from the list above.\n2. If multiple event of same type is mentioned, assign the event_type multiple times\n3. Extract attributes for each event using ONLY the allowed attributes listed below.\n4. Use keyword evidence (Ki) ONLY if it is consistent with the text context.\n5. Output strictly valid JSON following the schema below.\n                        ---\n                        Classification Rules:\n                        - A text may contain multiple events of the same or different types.\n- Create a separate event object for each event mention.\n- If the text is explicitly a NEGATION (e.g., "denies pain"), do not extract that event.\n- If the text describes a FUTURE or HYPOTHETICAL event (e.g., "will eat tomorrow"), ignore it.\n- A valid event should have occurred in the recent past or is occurring during the time of writing of the text.\n- If no events are found or if unsure, return {"events": []}\n                        \n                        ---\n                                    Attributes allowed:\n                                    {\'Eating\': {\'food\': \'&lt;string&gt; # e.g., pancakes, porridge, etc.\', \'amount\': \'&lt;string&gt; # e.g., 1, 2 bowls, etc.\', \'method\': \'&lt;string&gt;  # e.g., oral, tube, etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, after shower, etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}, \'Excretion\': {\'type\': \'&lt;string&gt; # e.g., urine, stool, etc.\', \'frequency\': \'&lt;string&gt; # e.g., 2x, once, etc.\', \'quality\': \'&lt;string&gt; # e.g., loose, hard, etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, after shower, etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}, \'Family\': {\'interaction\': \'&lt;string&gt; # e.g., visit, call, communication, etc.\', \'relation\': \'&lt;string&gt; # e.g., mother, son, etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, after shower, etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}, \'Pain\': {\'severity\': \'&lt;string&gt; # e.g., mild, moderate, severe, numeric scale if present, etc.\', \'location\': \'&lt;string&gt; # e.g., right knee, head, etc.\', \'duration\': \'&lt;string&gt; # e.g., all night, 3 hours, etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, after shower, etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}, \'Sleep\': {\'quality\': \'&lt;string&gt; # e.g., good, poor, restless, etc.\', \'duration\': \'&lt;string&gt; # e.g., 6 hours, phrases like "all night", etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, after shower, etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}}\n                                    If no relevant attribute exists for an event, return an empty object {}.\n                                    \n                        \n                        ---\n                                    Keyword evidence (Ki):\n                                    Additional facts: A keyword matching algorithm without context detected keyword(s) [\'family\', \'daughter\', \'eat\'].\n                                    Use this only as a pointer. If context contradicts, ignore.\n                        ---\n                        Output Schema (strict):\n                        {\n                                    "events": [\n                                        {\n                                        "event_type": "&lt;Pain | Sleep | Excretion | Eating | Family&gt;",\n                                        "text_quote": "&lt;fragement from the text indicating &gt;",\n                "attributes": {\n                    "&lt;attribute_name&gt;": "&lt;attribute_value&gt;"\n                }\n                                        }\n                                    ]\n                                    }\n                        \n                            Rules:\n                                - Ensure the output is valid JSON (parseable).\n                                - "eventS" must always be an array (can be empty).\n                                - Multiple instances of the same event type appear as individual elements in the event array.\n                                - Events appear in the array in the same order in which they appear in the text.\n                                - Do not include extra keys, comments, or text.\n                                - Each object in "events" must contain "event_type", "text_quote", and "attributes".\n                                -If an event attribute type has no value mentioned, return "attributes": {"&lt; attribute name &gt;:Unknown"} for each attribute type defined for the event type \n                        \n                        \n                        \n                        ', 'event_detection_time': 14.756375787997968}</t>
+          <t>["i don't eat much anymore", 'patient wife and daughter in to visit patient today', 'patient dozing intermittently throughout day', 'patient with foley cath draining amber cloudy u/o to dark yellow clearing u/o, approx 15-40 cc/heart rate']</t>
         </is>
       </c>
       <c r="J10" t="inlineStr">
         <is>
-          <t>['Eating', 'Family', 'Sleep', 'Excretion', 'Excretion']</t>
+          <t>[[]]</t>
         </is>
       </c>
       <c r="K10" t="inlineStr">
         <is>
-          <t>[{'Eating': {'food': 'Unknown', 'amount': 'Unknown', 'method': 'Unknown', 'negation': True, 'time': 'Unknown', 'caused_by': 'Unknown'}}, {'Family': {'interaction': 'visit', 'relation': 'wife and daughter', 'negation': False, 'time': 'today', 'caused_by': 'Unknown'}}, {'Sleep': {'quality': 'intermittent', 'duration': 'throughout the day', 'negation': False, 'time': 'day', 'caused_by': 'Unknown'}}, {'Excretion': {'type': 'urine', 'frequency': 'Unknown', 'quality': 'amber cloudy to dark yellow clearing', 'negation': False, 'time': 'eve', 'caused_by': 'foley cath'}}, {'Excretion': {'type': 'stool', 'frequency': 'none', 'quality': 'Unknown', 'negation': True, 'time': 'this shift', 'caused_by': 'Unknown'}}]</t>
+          <t>{'text': 'ccu npn 7a-7p\ns: " i don\'t eat much anymore...i\'male fine just looking out the window.\n\no: please see careview for vs and additional data.\n\ncv: heart rate 54-68 sb/nsr, no ectopy noted.  patient continues on labetalol and milrinone gtts.  labetalol drops titrated from off to 1.2 mg/min, milrinone titrated from 0.375 mcg/kg/min to 0.33 mcg/kg/min-milrinone to be titrated further overnoc.  patient abp 98-164/49-70-&gt; patient systolic 100-125 for most of shift, bp labile-fluctuates with wakening. pulses palp. hct 35 this am, to be redrawn this eve. patient to go to cath lab tomorrow am, per cardiac [**doctor first name **] note in chart-to examine hemodynamics and coronaries. mri results for aortic dissection status pending.\n\nresp: patient ls clear to coarse to diminished at bases, oxygen saturation 93-100 % on 6l n.c, rr 15-20, patient denies sob appears comfortable.\n\ngi/gu: patient abd soft, +bs x 4, no stool this shift.  patient with foley cath draining amber cloudy u/o to dark yellow clearing u/o, approx 15-40 cc/heart rate-patient to get lasix this eve.\n\nneuro: patient a&amp;o x 3, patient moves self to dangling on side of bed.  patient cooperative with care, patient quiet but responds appropriately to questions and engages in conversation with initiation. patient dozing intermittently throughout day.\n\nid: patient afebrile.\n\nsocial: patient wife and daughter in to visit patient today, aware of plan of care.\n\na/p: 84 year old male with aortic dissection-repair in 03, c/b cardiogenic shock, labile bp and arf-continues on labetalol drops d/t labile bp, milrinone drops titrating down, awaiting mri results-patient to cath lab tomorrrow am.  as discussed per interdisciplinary rounds, continue to monitor hemodynamics-titrate labetalol-change over to by mouth beta-blocker as patient condition tol.  continue to follow hct, lytes and update team on patient condition.  continue to monitor resp status, renal func and u/o.  continue to provide emotional support to patient and family.\n\n\n', 'event': ['Eating', 'Excretion', 'Family', 'Sleep'], 'event_id': ['e1', 'e2', 'e3', 'e4'], 'phrase': '', 'raw_output': '{\n  "events": [\n    {\n      "event_id": "e1",\n      "event_type": "Eating",\n      "text_quote": "i don\'t eat much anymore...",\n      "attributes": {\n        "food": "Unknown",\n        "amount": "Unknown",\n        "method": "oral",\n        "negation": true,\n        "time": "Unknown",\n        "caused_by": "Unknown"\n      }\n    },\n    {\n      "event_id": "e2",\n      "event_type": "Excretion",\n      "text_quote": "patient with foley cath draining amber cloudy u/o to dark yellow clearing u/o, approx 15-40 cc/heart rate",\n      "attributes": {\n        "type": "urine",\n        "frequency": "Unknown",\n        "quality": "cloudy to clear",\n        "negation": false,\n        "time": "Unknown",\n        "caused_by": "Unknown"\n      }\n    },\n    {\n      "event_id": "e3",\n      "event_type": "Family",\n      "text_quote": "patient wife and daughter in to visit patient today, aware of plan of care.",\n      "attributes": {\n        "interaction": "visit",\n        "relation": "wife and daughter",\n        "negation": false,\n        "time": "today",\n        "caused_by": "Unknown"\n      }\n    },\n    {\n      "event_id": "e4",\n      "event_type": "Sleep",\n      "text_quote": "patient dozing intermittently throughout day.",\n      "attributes": {\n        "quality": "intermittent",\n        "duration": "throughout the day",\n        "negation": false,\n        "time": "day",\n        "caused_by": "Unknown"\n      }\n    }\n  ],\n  "order": [\n    ["e1", "before", "e2"],\n    ["e2", "before", "e3"],\n    ["e3", "before", "e4"]\n  ]\n}', 'attributes': [{'Eating': {'food': 'Unknown', 'amount': 'Unknown', 'method': 'oral', 'negation': True, 'time': 'Unknown', 'caused_by': 'Unknown'}}, {'Excretion': {'type': 'urine', 'frequency': 'Unknown', 'quality': 'cloudy to clear', 'negation': False, 'time': 'Unknown', 'caused_by': 'Unknown'}}, {'Family': {'interaction': 'visit', 'relation': 'wife and daughter', 'negation': False, 'time': 'today', 'caused_by': 'Unknown'}}, {'Sleep': {'quality': 'intermittent', 'duration': 'throughout the day', 'negation': False, 'time': 'day', 'caused_by': 'Unknown'}}], 'orders': [[['e1', 'before', 'e2'], ['e2', 'before', 'e3'], ['e3', 'before', 'e4']]], 'text_quotes': ["i don't eat much anymore...", 'patient with foley cath draining amber cloudy u/o to dark yellow clearing u/o, approx 15-40 cc/heart rate', 'patient wife and daughter in to visit patient today, aware of plan of care.', 'patient dozing intermittently throughout day.'], 'event_name_prompt': 'Given the text: ccu npn 7a-7p\ns: " i don\'t eat much anymore...i\'male fine just looking out the window.\n\no: please see careview for vs and additional data.\n\ncv: heart rate 54-68 sb/nsr, no ectopy noted.  patient continues on labetalol and milrinone gtts.  labetalol drops titrated from off to 1.2 mg/min, milrinone titrated from 0.375 mcg/kg/min to 0.33 mcg/kg/min-milrinone to be titrated further overnoc.  patient abp 98-164/49-70-&gt; patient systolic 100-125 for most of shift, bp labile-fluctuates with wakening. pulses palp. hct 35 this am, to be redrawn this eve. patient to go to cath lab tomorrow am, per cardiac [**doctor first name **] note in chart-to examine hemodynamics and coronaries. mri results for aortic dissection status pending.\n\nresp: patient ls clear to coarse to diminished at bases, oxygen saturation 93-100 % on 6l n.c, rr 15-20, patient denies sob appears comfortable.\n\ngi/gu: patient abd soft, +bs x 4, no stool this shift.  patient with foley cath draining amber cloudy u/o to dark yellow clearing u/o, approx 15-40 cc/heart rate-patient to get lasix this eve.\n\nneuro: patient a&amp;o x 3, patient moves self to dangling on side of bed.  patient cooperative with care, patient quiet but responds appropriately to questions and engages in conversation with initiation. patient dozing intermittently throughout day.\n\nid: patient afebrile.\n\nsocial: patient wife and daughter in to visit patient today, aware of plan of care.\n\na/p: 84 year old male with aortic dissection-repair in 03, c/b cardiogenic shock, labile bp and arf-continues on labetalol drops d/t labile bp, milrinone drops titrating down, awaiting mri results-patient to cath lab tomorrrow am.  as discussed per interdisciplinary rounds, continue to monitor hemodynamics-titrate labetalol-change over to by mouth beta-blocker as patient condition tol.  continue to follow hct, lytes and update team on patient condition.  continue to monitor resp status, renal func and u/o.  continue to provide emotional support to patient and family.\n\n\n, \n                        and the following event types with their definitions: Eating : The patient takes food into their body by mouth.\nExcretion : The patient discharges waste matter from their body.\nFamily : The patient has a visit, call, or communication with a family member.\nPain : The patient reports or shows signs of pain.\nSleep : The patient sleeps or the sleep’s quality or quantity is described.\nUnknown : choose "Unknown" if none of the other event type are applicable. \n                        ---\n                        Your task:\n                        0. Identify ALL events in the text (zero, one, or more).\n1. For each event, assign an event_type from the list above.\n2. If multiple event of same type is mentioned, assign the event_type multiple times\n3. Extract attributes for each event using ONLY the allowed attributes listed below.\n4. Use keyword evidence (Ki) ONLY if it is consistent with the text context.\n5. Output strictly valid JSON following the schema below.\n                        ---\n                        Classification Rules:\n                        - A text may contain multiple events of the same or different types.\n- Create a separate event object for each event mention.\n- If the text is explicitly a NEGATION (e.g., "denies pain"), do not extract that event.\n- If the text describes a FUTURE or HYPOTHETICAL event (e.g., "will eat tomorrow"), ignore it.\n- A valid event should have occurred in the recent past or is occurring during the time of writing of the text.\n- If no events are found or if unsure, return {"events": []}\n                        \n                        ---\n                                    Attributes allowed:\n                                    {\'Eating\': {\'food\': \'&lt;string&gt; # e.g., pancakes, porridge, etc.\', \'amount\': \'&lt;string&gt; # e.g., 1, 2 bowls, etc.\', \'method\': \'&lt;string&gt;  # e.g., oral, tube, etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, evening etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}, \'Excretion\': {\'type\': \'&lt;string&gt; # e.g., urine, stool, etc.\', \'frequency\': \'&lt;string&gt; # e.g., 2x, once, etc.\', \'quality\': \'&lt;string&gt; # e.g., loose, hard, etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, evening etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}, \'Family\': {\'interaction\': \'&lt;string&gt; # e.g., visit, call, communication, etc.\', \'relation\': \'&lt;string&gt; # e.g., mother, son, etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, evening etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}, \'Pain\': {\'severity\': \'&lt;string&gt; # e.g., mild, moderate, severe, numeric scale if present, etc.\', \'location\': \'&lt;string&gt; # e.g., right knee, head, etc.\', \'duration\': \'&lt;string&gt; # e.g., all night, 3 hours, etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, evening etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}, \'Sleep\': {\'quality\': \'&lt;string&gt; # e.g., good, poor, restless, etc.\', \'duration\': \'&lt;string&gt; # e.g., 6 hours, phrases like "all night", etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, evening etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}}\n                                    If no relevant attribute exists for an event, return an empty object {}.\n                                    \n                        \n                        ---\n                                    Keyword evidence (Ki):\n                                    Additional facts: A keyword matching algorithm without context detected keyword(s) (\'eat\', \'family\', \'daughter\').\n                                    Use this only as a pointer. If context contradicts, ignore.\n                        ---\n                        Output Schema (strict):\n                        {\n                                    "events": [\n                                        {\n                                        "event_id": "&lt; A unique id eg.: e1 | e2 |...&gt;"\n                                        "event_type": "&lt;Pain | Sleep | Excretion | Eating | Family&gt;",\n                                        "text_quote": "&lt;fragement from the text indicating the event_type&gt;",\n                "attributes": {\n                    "&lt;attribute_name&gt;": "&lt;attribute_value&gt;"\n                }\n                                        }\n                                    ],\n                                    "order": [\n                                        ["e1", "before" | "after" | "simultaneous", "e2" ]\n                                    ]\n                                    }\n                        \n                            Rules:\n                                - Ensure the output is valid JSON (parseable).\n                                - "eventS" must always be an array (can be empty).\n                                - Multiple instances of the same event type appear with different ids.\n                                - Events appear in the array in the same order in which they appear in the text.\n                                - Their partial orders can be expressed using the "order" section.\n                                - Do not include extra keys, comments, or text.\n                                - Each object in "events" must contain "event_type", "text_quote", and "attributes".\n                                - If an event attribute type has no value mentioned, return "attributes": {"&lt; attribute name &gt;:Unknown"} for each attribute type defined for the event type \n                        \n                        \n                        \n                        ', 'event_detection_time': 14.192327663011383}</t>
         </is>
       </c>
       <c r="L10" t="inlineStr">
         <is>
-          <t>["i don't eat much anymore...", 'patient wife and daughter in to visit patient today, aware of plan of care.', 'patient dozing intermittently throughout day.', 'patient with foley cath draining amber cloudy u/o to dark yellow clearing u/o, approx 15-40 cc/heart rate-patient to get lasix this eve.', 'patient abd soft, +bs x 4, no stool this shift.']</t>
+          <t>['Eating', 'Excretion', 'Family', 'Sleep']</t>
         </is>
       </c>
       <c r="M10" t="inlineStr">
         <is>
-          <t>{'text': 'ccu npn 7a-7p\ns: " i don\'t eat much anymore...i\'male fine just looking out the window.\n\no: please see careview for vs and additional data.\n\ncv: heart rate 54-68 sb/nsr, no ectopy noted.  patient continues on labetalol and milrinone gtts.  labetalol drops titrated from off to 1.2 mg/min, milrinone titrated from 0.375 mcg/kg/min to 0.33 mcg/kg/min-milrinone to be titrated further overnoc.  patient abp 98-164/49-70-&gt; patient systolic 100-125 for most of shift, bp labile-fluctuates with wakening. pulses palp. hct 35 this am, to be redrawn this eve. patient to go to cath lab tomorrow am, per cardiac [**doctor first name **] note in chart-to examine hemodynamics and coronaries. mri results for aortic dissection status pending.\n\nresp: patient ls clear to coarse to diminished at bases, oxygen saturation 93-100 % on 6l n.c, rr 15-20, patient denies sob appears comfortable.\n\ngi/gu: patient abd soft, +bs x 4, no stool this shift.  patient with foley cath draining amber cloudy u/o to dark yellow clearing u/o, approx 15-40 cc/heart rate-patient to get lasix this eve.\n\nneuro: patient a&amp;o x 3, patient moves self to dangling on side of bed.  patient cooperative with care, patient quiet but responds appropriately to questions and engages in conversation with initiation. patient dozing intermittently throughout day.\n\nid: patient afebrile.\n\nsocial: patient wife and daughter in to visit patient today, aware of plan of care.\n\na/p: 84 year old male with aortic dissection-repair in 03, c/b cardiogenic shock, labile bp and arf-continues on labetalol drops d/t labile bp, milrinone drops titrating down, awaiting mri results-patient to cath lab tomorrrow am.  as discussed per interdisciplinary rounds, continue to monitor hemodynamics-titrate labetalol-change over to by mouth beta-blocker as patient condition tol.  continue to follow hct, lytes and update team on patient condition.  continue to monitor resp status, renal func and u/o.  continue to provide emotional support to patient and family.\n\n\n', 'event': ['Eating', 'Family', 'Sleep', 'Excretion'], 'phrase': '', 'raw_output': '{\n  "events": [\n    {\n      "event_type": "Eating",\n      "text_quote": "i don\'t eat much anymore...",\n      "attributes": {"food": "Unknown", \n                     "amount": "Unknown",\n                     "method": "Unknown",\n                     "time":"Unknown",\n                     "caused_by":"Unknown"}\n    },\n    {\n      "event_type": "Family",\n      "text_quote": "patient wife and daughter in to visit patient today",\n      "attributes": {"interaction": "visit", \n                     "relation": "wife, daughter",\n                     "time":"today",\n                     "caused_by":"Unknown"}\n    },\n    {\n      "event_type": "Sleep",\n      "text_quote": "patient dozing intermittently throughout day",\n      "attributes": {"quality": "intermittent", \n                     "duration": "throughout the day",\n                     "time":"day",\n                     "caused_by":"Unknown"}\n    },\n    {\n      "event_type": "Excretion",\n      "text_quote": "patient with foley cath draining amber cloudy u/o to dark yellow clearing u/o, approx 15-40 cc/heart rate",\n      "attributes": {"type": "urine", \n                     "frequency": "approx 15-40 cc/heart rate",\n                     "quality": "amber cloudy to dark yellow clearing",\n                     "time":"Unknown",\n                     "caused_by":"Unknown"}\n    }\n  ]\n}', 'attributes': [{'Eating': {'food': 'Unknown', 'amount': 'Unknown', 'method': 'Unknown', 'time': 'Unknown', 'caused_by': 'Unknown'}}, {'Family': {'interaction': 'visit', 'relation': 'wife, daughter', 'time': 'today', 'caused_by': 'Unknown'}}, {'Sleep': {'quality': 'intermittent', 'duration': 'throughout the day', 'time': 'day', 'caused_by': 'Unknown'}}, {'Excretion': {'type': 'urine', 'frequency': 'approx 15-40 cc/heart rate', 'quality': 'amber cloudy to dark yellow clearing', 'time': 'Unknown', 'caused_by': 'Unknown'}}], 'text_quotes': ["i don't eat much anymore...", 'patient wife and daughter in to visit patient today', 'patient dozing intermittently throughout day', 'patient with foley cath draining amber cloudy u/o to dark yellow clearing u/o, approx 15-40 cc/heart rate'], 'event_name_prompt': 'Given the text: ccu npn 7a-7p\ns: " i don\'t eat much anymore...i\'male fine just looking out the window.\n\no: please see careview for vs and additional data.\n\ncv: heart rate 54-68 sb/nsr, no ectopy noted.  patient continues on labetalol and milrinone gtts.  labetalol drops titrated from off to 1.2 mg/min, milrinone titrated from 0.375 mcg/kg/min to 0.33 mcg/kg/min-milrinone to be titrated further overnoc.  patient abp 98-164/49-70-&gt; patient systolic 100-125 for most of shift, bp labile-fluctuates with wakening. pulses palp. hct 35 this am, to be redrawn this eve. patient to go to cath lab tomorrow am, per cardiac [**doctor first name **] note in chart-to examine hemodynamics and coronaries. mri results for aortic dissection status pending.\n\nresp: patient ls clear to coarse to diminished at bases, oxygen saturation 93-100 % on 6l n.c, rr 15-20, patient denies sob appears comfortable.\n\ngi/gu: patient abd soft, +bs x 4, no stool this shift.  patient with foley cath draining amber cloudy u/o to dark yellow clearing u/o, approx 15-40 cc/heart rate-patient to get lasix this eve.\n\nneuro: patient a&amp;o x 3, patient moves self to dangling on side of bed.  patient cooperative with care, patient quiet but responds appropriately to questions and engages in conversation with initiation. patient dozing intermittently throughout day.\n\nid: patient afebrile.\n\nsocial: patient wife and daughter in to visit patient today, aware of plan of care.\n\na/p: 84 year old male with aortic dissection-repair in 03, c/b cardiogenic shock, labile bp and arf-continues on labetalol drops d/t labile bp, milrinone drops titrating down, awaiting mri results-patient to cath lab tomorrrow am.  as discussed per interdisciplinary rounds, continue to monitor hemodynamics-titrate labetalol-change over to by mouth beta-blocker as patient condition tol.  continue to follow hct, lytes and update team on patient condition.  continue to monitor resp status, renal func and u/o.  continue to provide emotional support to patient and family.\n\n\n, \n                        and the following event types with their definitions: Eating : The patient takes food into their body by mouth.\nExcretion : The patient discharges waste matter from their body.\nFamily : The patient has a visit, call, or communication with a family member.\nPain : The patient reports or shows signs of pain.\nSleep : The patient sleeps or the sleep’s quality or quantity is described.\nUnknown : choose "Unknown" if none of the other event type are applicable. \n                        ---\n                        Your task:\n                        0. Identify ALL events in the text (zero, one, or more).\n1. For each event, assign an event_type from the list above.\n2. If multiple event of same type is mentioned, assign the event_type multiple times\n3. Extract attributes for each event using ONLY the allowed attributes listed below.\n4. Output strictly valid JSON following the schema below.\n                        ---\n                        Classification Rules:\n                        - A text may contain multiple events of the same or different types.\n- Create a separate event object for each event mention.\n- If the text is explicitly a NEGATION (e.g., "denies pain"), do not extract that event.\n- If the text describes a FUTURE or HYPOTHETICAL event (e.g., "will eat tomorrow"), ignore it.\n- A valid event should have occurred in the recent past or is occurring during the time of writing of the text.\n- If no events are found or if unsure, return {"events": []}\n                        \n                        ---\n                                    Attributes allowed:\n                                    {\'Eating\': {\'food\': \'&lt;string&gt; # e.g., pancakes, porridge, etc.\', \'amount\': \'&lt;string&gt; # e.g., 1, 2 bowls, etc.\', \'method\': \'&lt;string&gt;  # e.g., oral, tube, etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, after shower, etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}, \'Excretion\': {\'type\': \'&lt;string&gt; # e.g., urine, stool, etc.\', \'frequency\': \'&lt;string&gt; # e.g., 2x, once, etc.\', \'quality\': \'&lt;string&gt; # e.g., loose, hard, etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, after shower, etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}, \'Family\': {\'interaction\': \'&lt;string&gt; # e.g., visit, call, communication, etc.\', \'relation\': \'&lt;string&gt; # e.g., mother, son, etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, after shower, etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}, \'Pain\': {\'severity\': \'&lt;string&gt; # e.g., mild, moderate, severe, numeric scale if present, etc.\', \'location\': \'&lt;string&gt; # e.g., right knee, head, etc.\', \'duration\': \'&lt;string&gt; # e.g., all night, 3 hours, etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, after shower, etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}, \'Sleep\': {\'quality\': \'&lt;string&gt; # e.g., good, poor, restless, etc.\', \'duration\': \'&lt;string&gt; # e.g., 6 hours, phrases like "all night", etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, after shower, etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}}\n                                    If no relevant attribute exists for an event, return an empty object {}.\n                                    \n                        \n                        \n                        ---\n                        Output Schema (strict):\n                        {\n                                    "events": [\n                                        {\n                                        "event_type": "&lt;Pain | Sleep | Excretion | Eating | Family&gt;",\n                                        "text_quote": "&lt;fragement from the text indicating &gt;",\n                "attributes": {\n                    "&lt;attribute_name&gt;": "&lt;attribute_value&gt;"\n                }\n                                        }\n                                    ]\n                                    }\n                        \n                            Rules:\n                                - Ensure the output is valid JSON (parseable).\n                                - "eventS" must always be an array (can be empty).\n                                - Multiple instances of the same event type appear as individual elements in the event array.\n                                - Events appear in the array in the same order in which they appear in the text.\n                                - Do not include extra keys, comments, or text.\n                                - Each object in "events" must contain "event_type", "text_quote", and "attributes".\n                                -If an event attribute type has no value mentioned, return "attributes": {"&lt; attribute name &gt;:Unknown"} for each attribute type defined for the event type \n                        \n                        \n                        \n                ---\n                Examples:\n                \n                text: "Patient ate breakfast this morning. He seems less anxious."\n                output: {\n                "events": [\n                    {\n                    "event_type": "Eating",\n                    "text_quote":"Patient ate breakfast this morning",\n                    "attributes": {"food": "breakfast", \n                                   "amount": "Unknown",\n                                   "method": "Unknown",\n                                   "time":"morning",\n                                   "caused_by":"Unknown"}\n                    }\n                ]\n                }\n                \n                text: "Patient reported severe abdominal pain."\n                output: {\n                "events": [\n                    {\n                    "event_type": "Pain",\n                    "text_quote": "severe abdominal Pain",\n                    "attributes": {"severity": "severe", \n                                   "location": "abdominal",\n                                   "duration": "Unknown",\n                                   "time":"Unknown",\n                                   "caused_by":"Unknown"}\n                    }\n                ]\n                }\n                \n                text: "Patient called his son around 3 pm."\n                output: {\n                "events": [\n                    {\n                    "event_type": "Family",\n                    "text_quote": "called his son around 3 pm",\n                    "attributes": {"interaction": "call", \n                                    "relation": "son",\n                                    "time":"3 pm",\n                                    "caused_by":"Unknown"}\n                    }\n                ]\n                }\n                \n                text: "Patient had a loose stool overnight."\n                output: {\n                "events": [\n                    {\n                    "event_type": "Excretion",\n                    "text_quote": "loose stool overnight",\n                    "attributes": {"type": "stool", \n                                   "quality": "loose", \n                                   "frequency":"overnight", \n                                   "time":"night",\n                                   "caused_by":"Unknown"}\n                    }\n                ]\n                }\n                \n                text: "Patient was able to sleep well last night."\n                output: {\n                "events": [\n                    {\n                    "event_type": "Sleep",\n                    "text_quote": "sleep well last night",\n                    "attributes": {"quality": "well",\n                                    "duration": "Unknown", \n                                    "time":"night",\n                                    "caused_by":"Unknown"}\n                    }\n                ]\n                }\n                \n                text: "The patient couldn\'t sleep due to severe pain."\n                output: {\n                "events": [\n                    {\n                    "event_type": "Sleep",\n                    "text_quote": "couldn\'t sleep",\n                    "attributes": {"quality": "poor", \n                                    "duration": "Unknown",\n                                   "time":"Unknown",\n                                   "caused_by":"Pain"}\n                    },\n                    {\n                    "event_type": "Pain",\n                    "text_quote": "severe pain",\n                    "attributes": {"severity": "severe", \n                                    "location": "Unknown", \n                                    "duration": "Unknown", \n                                   "time":"before Sleep",\n                                   "caused_by":"Unknown"}\n                    }\n                ]\n                }\n                \n                text: "The patient complained of severe back pain, was given Tylenol, but the pain persisted and he was then prescribed stronger morphine."\n                output: {\n                "events": [\n                    {\n                    "event_type": "Pain",\n                    "text_quote": "complained of severe back pain",\n                    "attributes": {"severity": "severe", \n                                    "location": "back",\n                                    "duration": "Unknown", \n                                    "time":"Unknown",\n                                    "caused_by":"Unknown"}\n                    },\n                    {\n                    "event_type": "Pain",\n                    "text_quote": "pain persisted",\n                    "attributes": {"severity": "severe", \n                                   "location": "back",\n                                   "duration": "persistent", \n                                   "time":"after Tylenol",\n                                   "caused_by":"Unknown"}\n                    }\n                ]\n                }\n                \n                        ', 'event_detection_time': 11.282679026990081}</t>
+          <t>[{'Eating': {'food': 'Unknown', 'amount': 'Unknown', 'method': 'oral', 'negation': True, 'time': 'Unknown', 'caused_by': 'Unknown'}}, {'Excretion': {'type': 'urine', 'frequency': 'Unknown', 'quality': 'cloudy to clear', 'negation': False, 'time': 'Unknown', 'caused_by': 'Unknown'}}, {'Family': {'interaction': 'visit', 'relation': 'wife and daughter', 'negation': False, 'time': 'today', 'caused_by': 'Unknown'}}, {'Sleep': {'quality': 'intermittent', 'duration': 'throughout the day', 'negation': False, 'time': 'day', 'caused_by': 'Unknown'}}]</t>
         </is>
       </c>
       <c r="N10" t="inlineStr">
         <is>
-          <t>['Eating', 'Family', 'Sleep', 'Excretion']</t>
+          <t>["i don't eat much anymore...", 'patient with foley cath draining amber cloudy u/o to dark yellow clearing u/o, approx 15-40 cc/heart rate', 'patient wife and daughter in to visit patient today, aware of plan of care.', 'patient dozing intermittently throughout day.']</t>
         </is>
       </c>
       <c r="O10" t="inlineStr">
         <is>
-          <t>[{'Eating': {'food': 'Unknown', 'amount': 'Unknown', 'method': 'Unknown', 'time': 'Unknown', 'caused_by': 'Unknown'}}, {'Family': {'interaction': 'visit', 'relation': 'wife, daughter', 'time': 'today', 'caused_by': 'Unknown'}}, {'Sleep': {'quality': 'intermittent', 'duration': 'throughout the day', 'time': 'day', 'caused_by': 'Unknown'}}, {'Excretion': {'type': 'urine', 'frequency': 'approx 15-40 cc/heart rate', 'quality': 'amber cloudy to dark yellow clearing', 'time': 'Unknown', 'caused_by': 'Unknown'}}]</t>
-        </is>
-      </c>
-      <c r="P10" t="inlineStr">
-        <is>
-          <t>["i don't eat much anymore...", 'patient wife and daughter in to visit patient today', 'patient dozing intermittently throughout day', 'patient with foley cath draining amber cloudy u/o to dark yellow clearing u/o, approx 15-40 cc/heart rate']</t>
-        </is>
-      </c>
-      <c r="Q10" t="n">
-        <v>0.003039491000890848</v>
-      </c>
-      <c r="R10" t="inlineStr">
+          <t>[[['e1', 'before', 'e2'], ['e2', 'before', 'e3'], ['e3', 'before', 'e4']]]</t>
+        </is>
+      </c>
+      <c r="P10" t="n">
+        <v>0.002431813001749106</v>
+      </c>
+      <c r="Q10" t="inlineStr">
         <is>
           <t>Sleep</t>
         </is>
       </c>
-      <c r="S10" t="b">
-        <v>0</v>
+      <c r="R10" t="b">
+        <v>0</v>
+      </c>
+      <c r="S10" t="n">
+        <v>1</v>
       </c>
       <c r="T10" t="n">
-        <v>1</v>
-      </c>
-      <c r="U10" t="n">
-        <v>0</v>
-      </c>
-      <c r="V10" t="inlineStr">
+        <v>0</v>
+      </c>
+      <c r="U10" t="inlineStr">
         <is>
           <t>('eat', 'family', 'daughter')</t>
         </is>
       </c>
+      <c r="V10" t="n">
+        <v>14.48626643099124</v>
+      </c>
       <c r="W10" t="n">
-        <v>15.26224031500169</v>
+        <v>14.19232766301138</v>
       </c>
       <c r="X10" t="n">
-        <v>14.75637578799797</v>
+        <v>0</v>
       </c>
       <c r="Y10" t="n">
-        <v>11.28267902699008</v>
+        <v>1</v>
       </c>
       <c r="Z10" t="n">
-        <v>0</v>
-      </c>
-      <c r="AA10" t="n">
-        <v>1</v>
-      </c>
-      <c r="AB10" t="n">
-        <v>1</v>
-      </c>
-      <c r="AC10" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="11">
-      <c r="A11" t="n">
-        <v>1310488</v>
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>1310488</t>
+        </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>['Pain', 'Family', 'Unknown']</t>
+          <t>('Pain', 'Family', 'Unknown')</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>['family', 'pain']</t>
+          <t>('pain', 'family')</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
@@ -1835,120 +1743,111 @@
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>{'text': 'ccu npn 7p-7a\ns: "when am i going to be able to get out of bed and walk around?"\no: see carevue and update for complete assessment data\nhpi: 84yo admitted [**3-10**] w/sob and backpain found to have type b aortic dissection descending from thoracic aorta to l common iliac artery. h/o htn, type a dissection \'[**77**] status post emergent surgical repair c/b embolic cva. tee [**3-10**] showed global hypokinesis with newly depressed lvef 25% (from 60% on \'[**77**]). current hospitalization c/b new onset rapid a flutter v. a tach with 2:1 conduction, cardioversion to nsr [**3-10**] c/b hypotension requiring neo, arf with cr up to 2.7, extremely labile bp requiring both labetalol and neo at times. pa line placed [**3-11**] revealed ci of 1.7, up to 3 after starting milrinone, was self d/c\'d [**3-12**].\nros:\ncv: cont labetolol 0.5-1.5mg/min to maintain diastolic blood pressure 100-120, ranging 90s-150s/ depending on level of alertness. milrinone weaned to 0.25mcg/kg/min. heart rate sb 58-60, no ectopy, hct stable, am labs pending. no c/o cp/sob. distal pulses palp/dop, bp equal bilat ues. plan for cath today to eval coronaries and hemodynamics.\n\nresp: nc frequently dislodged, spo2 on ra 89-96%. ls clear, diminished @ bases with fine rales 1/4 up posteriorly. bilat atelectasis appreciated on mri.\n\ngi/gu: abd soft, nontender, nondistended, +bs/-bm, tolerating by mouth meds with sips. npo after mn for cath [**3-15**].  foley draining cyu, excellent response to 60mg lasix ivp given @ [**2174**]. +325 yesterday, -850 since mn. am bun/cr pending. mri revealing that renal artery perfusion is not inhibited by dissection.\n\nid: afebrile although warm to touch. tmax 98.6 by mouth. wbc 5.8(5.6)\n\nskin: multiple areas of ecchymosis. r hand 22g piv erythematous, nontender, flushes easily, left in d/t poor peripheral access. lac also needs to be d/c\'d (in on [**3-10**]). l hand edematous from ? infiltration of old iv site.\n\nneuro: a&amp;ox3, dangling at bedside at times and c/o restlessness (baseline). tylenol for back pain with relief.\n\na: 84yo with type b descending arotic dissection, bp cont labile and cont to require labetalol. also cont on milrinone. improving renal sts, responded well to diuresis.\np: to cath today to eval hemodynamic sts, follow up am labs. monitor fluid sts. teaching re: procedure, continue to support patient. and family. ? start by mouth bb.\n', 'event': ['Pain', 'Pain', 'Sleep', 'Family'], 'phrase': '', 'raw_output': '{\n  "events": [\n    {\n      "event_type": "Pain",\n      "text_quote": "when am i going to be able to get out of bed and walk around?",\n      "attributes": {"severity": "Unknown", \n                     "location": "back",\n                     "duration": "Unknown", \n                     "time":"Unknown",\n                     "caused_by":"Unknown"}\n    },\n    {\n      "event_type": "Pain",\n      "text_quote": "tylenol for back pain with relief.",\n      "attributes": {"severity": "Unknown", \n                     "location": "back",\n                     "duration": "Unknown", \n                     "time":"Unknown",\n                     "caused_by":"Tylenol"}\n    },\n    {\n      "event_type": "Sleep",\n      "text_quote": "a&amp;ox3, dangling at bedside at times and c/o restlessness (baseline).",\n      "attributes": {"quality": "restless", \n                     "duration": "Unknown", \n                     "time":"Unknown",\n                     "caused_by":"Unknown"}\n    },\n    {\n      "event_type": "Family",\n      "text_quote": "continue to support patient. and family.",\n      "attributes": {"interaction": "support", \n                     "relation": "family",\n                     "time":"Unknown",\n                     "caused_by":"Unknown"}\n    }\n  ]\n}', 'attributes': [{'Pain': {'severity': 'Unknown', 'location': 'back', 'duration': 'Unknown', 'time': 'Unknown', 'caused_by': 'Unknown'}}, {'Pain': {'severity': 'Unknown', 'location': 'back', 'duration': 'Unknown', 'time': 'Unknown', 'caused_by': 'Tylenol'}}, {'Sleep': {'quality': 'restless', 'duration': 'Unknown', 'time': 'Unknown', 'caused_by': 'Unknown'}}, {'Family': {'interaction': 'support', 'relation': 'family', 'time': 'Unknown', 'caused_by': 'Unknown'}}], 'text_quotes': ['when am i going to be able to get out of bed and walk around?', 'tylenol for back pain with relief.', 'a&amp;ox3, dangling at bedside at times and c/o restlessness (baseline).', 'continue to support patient. and family.'], 'event_name_prompt': 'Given the text: ccu npn 7p-7a\ns: "when am i going to be able to get out of bed and walk around?"\no: see carevue and update for complete assessment data\nhpi: 84yo admitted [**3-10**] w/sob and backpain found to have type b aortic dissection descending from thoracic aorta to l common iliac artery. h/o htn, type a dissection \'[**77**] status post emergent surgical repair c/b embolic cva. tee [**3-10**] showed global hypokinesis with newly depressed lvef 25% (from 60% on \'[**77**]). current hospitalization c/b new onset rapid a flutter v. a tach with 2:1 conduction, cardioversion to nsr [**3-10**] c/b hypotension requiring neo, arf with cr up to 2.7, extremely labile bp requiring both labetalol and neo at times. pa line placed [**3-11**] revealed ci of 1.7, up to 3 after starting milrinone, was self d/c\'d [**3-12**].\nros:\ncv: cont labetolol 0.5-1.5mg/min to maintain diastolic blood pressure 100-120, ranging 90s-150s/ depending on level of alertness. milrinone weaned to 0.25mcg/kg/min. heart rate sb 58-60, no ectopy, hct stable, am labs pending. no c/o cp/sob. distal pulses palp/dop, bp equal bilat ues. plan for cath today to eval coronaries and hemodynamics.\n\nresp: nc frequently dislodged, spo2 on ra 89-96%. ls clear, diminished @ bases with fine rales 1/4 up posteriorly. bilat atelectasis appreciated on mri.\n\ngi/gu: abd soft, nontender, nondistended, +bs/-bm, tolerating by mouth meds with sips. npo after mn for cath [**3-15**].  foley draining cyu, excellent response to 60mg lasix ivp given @ [**2174**]. +325 yesterday, -850 since mn. am bun/cr pending. mri revealing that renal artery perfusion is not inhibited by dissection.\n\nid: afebrile although warm to touch. tmax 98.6 by mouth. wbc 5.8(5.6)\n\nskin: multiple areas of ecchymosis. r hand 22g piv erythematous, nontender, flushes easily, left in d/t poor peripheral access. lac also needs to be d/c\'d (in on [**3-10**]). l hand edematous from ? infiltration of old iv site.\n\nneuro: a&amp;ox3, dangling at bedside at times and c/o restlessness (baseline). tylenol for back pain with relief.\n\na: 84yo with type b descending arotic dissection, bp cont labile and cont to require labetalol. also cont on milrinone. improving renal sts, responded well to diuresis.\np: to cath today to eval hemodynamic sts, follow up am labs. monitor fluid sts. teaching re: procedure, continue to support patient. and family. ? start by mouth bb.\n, \n                        and the following event types with their definitions: Eating : The patient takes food into their body by mouth.\nExcretion : The patient discharges waste matter from their body.\nFamily : The patient has a visit, call, or communication with a family member.\nPain : The patient reports or shows signs of pain.\nSleep : The patient sleeps or the sleep’s quality or quantity is described.\nUnknown : choose "Unknown" if none of the other event type are applicable. \n                        ---\n                        Your task:\n                        0. Identify ALL events in the text (zero, one, or more).\n1. For each event, assign an event_type from the list above.\n2. If multiple event of same type is mentioned, assign the event_type multiple times\n3. Extract attributes for each event using ONLY the allowed attributes listed below.\n4. Use keyword evidence (Ki) ONLY if it is consistent with the text context.\n5. Output strictly valid JSON following the schema below.\n                        ---\n                        Classification Rules:\n                        - A text may contain multiple events of the same or different types.\n- Create a separate event object for each event mention.\n- If the text is explicitly a NEGATION (e.g., "denies pain"), do not extract that event.\n- If the text describes a FUTURE or HYPOTHETICAL event (e.g., "will eat tomorrow"), ignore it.\n- A valid event should have occurred in the recent past or is occurring during the time of writing of the text.\n- If no events are found or if unsure, return {"events": []}\n                        \n                        ---\n                                    Attributes allowed:\n                                    {\'Eating\': {\'food\': \'&lt;string&gt; # e.g., pancakes, porridge, etc.\', \'amount\': \'&lt;string&gt; # e.g., 1, 2 bowls, etc.\', \'method\': \'&lt;string&gt;  # e.g., oral, tube, etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, after shower, etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}, \'Excretion\': {\'type\': \'&lt;string&gt; # e.g., urine, stool, etc.\', \'frequency\': \'&lt;string&gt; # e.g., 2x, once, etc.\', \'quality\': \'&lt;string&gt; # e.g., loose, hard, etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, after shower, etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}, \'Family\': {\'interaction\': \'&lt;string&gt; # e.g., visit, call, communication, etc.\', \'relation\': \'&lt;string&gt; # e.g., mother, son, etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, after shower, etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}, \'Pain\': {\'severity\': \'&lt;string&gt; # e.g., mild, moderate, severe, numeric scale if present, etc.\', \'location\': \'&lt;string&gt; # e.g., right knee, head, etc.\', \'duration\': \'&lt;string&gt; # e.g., all night, 3 hours, etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, after shower, etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}, \'Sleep\': {\'quality\': \'&lt;string&gt; # e.g., good, poor, restless, etc.\', \'duration\': \'&lt;string&gt; # e.g., 6 hours, phrases like "all night", etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, after shower, etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}}\n                                    If no relevant attribute exists for an event, return an empty object {}.\n                                    \n                        \n                        ---\n                                    Keyword evidence (Ki):\n                                    Additional facts: A keyword matching algorithm without context detected keyword(s) [\'family\', \'pain\'].\n                                    Use this only as a pointer. If context contradicts, ignore.\n                        ---\n                        Output Schema (strict):\n                        {\n                                    "events": [\n                                        {\n                                        "event_type": "&lt;Pain | Sleep | Excretion | Eating | Family&gt;",\n                                        "text_quote": "&lt;fragement from the text indicating &gt;",\n                "attributes": {\n                    "&lt;attribute_name&gt;": "&lt;attribute_value&gt;"\n                }\n                                        }\n                                    ]\n                                    }\n                        \n                            Rules:\n                                - Ensure the output is valid JSON (parseable).\n                                - "eventS" must always be an array (can be empty).\n                                - Multiple instances of the same event type appear as individual elements in the event array.\n                                - Events appear in the array in the same order in which they appear in the text.\n                                - Do not include extra keys, comments, or text.\n                                - Each object in "events" must contain "event_type", "text_quote", and "attributes".\n                                -If an event attribute type has no value mentioned, return "attributes": {"&lt; attribute name &gt;:Unknown"} for each attribute type defined for the event type \n                        \n                        \n                        \n                ---\n                Examples:\n                \n                text: "Patient ate breakfast this morning. He seems less anxious."\n                output: {\n                "events": [\n                    {\n                    "event_type": "Eating",\n                    "text_quote":"Patient ate breakfast this morning",\n                    "attributes": {"food": "breakfast", \n                                   "amount": "Unknown",\n                                   "method": "Unknown",\n                                   "time":"morning",\n                                   "caused_by":"Unknown"}\n                    }\n                ]\n                }\n                \n                text: "Patient reported severe abdominal pain."\n                output: {\n                "events": [\n                    {\n                    "event_type": "Pain",\n                    "text_quote": "severe abdominal Pain",\n                    "attributes": {"severity": "severe", \n                                   "location": "abdominal",\n                                   "duration": "Unknown",\n                                   "time":"Unknown",\n                                   "caused_by":"Unknown"}\n                    }\n                ]\n                }\n                \n                text: "Patient called his son around 3 pm."\n                output: {\n                "events": [\n                    {\n                    "event_type": "Family",\n                    "text_quote": "called his son around 3 pm",\n                    "attributes": {"interaction": "call", \n                                    "relation": "son",\n                                    "time":"3 pm",\n                                    "caused_by":"Unknown"}\n                    }\n                ]\n                }\n                \n                text: "Patient had a loose stool overnight."\n                output: {\n                "events": [\n                    {\n                    "event_type": "Excretion",\n                    "text_quote": "loose stool overnight",\n                    "attributes": {"type": "stool", \n                                   "quality": "loose", \n                                   "frequency":"overnight", \n                                   "time":"night",\n                                   "caused_by":"Unknown"}\n                    }\n                ]\n                }\n                \n                text: "Patient was able to sleep well last night."\n                output: {\n                "events": [\n                    {\n                    "event_type": "Sleep",\n                    "text_quote": "sleep well last night",\n                    "attributes": {"quality": "well",\n                                    "duration": "Unknown", \n                                    "time":"night",\n                                    "caused_by":"Unknown"}\n                    }\n                ]\n                }\n                \n                text: "The patient couldn\'t sleep due to severe pain."\n                output: {\n                "events": [\n                    {\n                    "event_type": "Sleep",\n                    "text_quote": "couldn\'t sleep",\n                    "attributes": {"quality": "poor", \n                                    "duration": "Unknown",\n                                   "time":"Unknown",\n                                   "caused_by":"Pain"}\n                    },\n                    {\n                    "event_type": "Pain",\n                    "text_quote": "severe pain",\n                    "attributes": {"severity": "severe", \n                                    "location": "Unknown", \n                                    "duration": "Unknown", \n                                   "time":"before Sleep",\n                                   "caused_by":"Unknown"}\n                    }\n                ]\n                }\n                \n                text: "The patient complained of severe back pain, was given Tylenol, but the pain persisted and he was then prescribed stronger morphine."\n                output: {\n                "events": [\n                    {\n                    "event_type": "Pain",\n                    "text_quote": "complained of severe back pain",\n                    "attributes": {"severity": "severe", \n                                    "location": "back",\n                                    "duration": "Unknown", \n                                    "time":"Unknown",\n                                    "caused_by":"Unknown"}\n                    },\n                    {\n                    "event_type": "Pain",\n                    "text_quote": "pain persisted",\n                    "attributes": {"severity": "severe", \n                                   "location": "back",\n                                   "duration": "persistent", \n                                   "time":"after Tylenol",\n                                   "caused_by":"Unknown"}\n                    }\n                ]\n                }\n                \n                        ', 'event_detection_time': 11.212815274004242}</t>
+          <t>['pain', 'family']</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>['Pain', 'Pain', 'Sleep', 'Family']</t>
+          <t>{'text': 'ccu npn 7p-7a\ns: "when am i going to be able to get out of bed and walk around?"\no: see carevue and update for complete assessment data\nhpi: 84yo admitted [**3-10**] w/sob and backpain found to have type b aortic dissection descending from thoracic aorta to l common iliac artery. h/o htn, type a dissection \'[**77**] status post emergent surgical repair c/b embolic cva. tee [**3-10**] showed global hypokinesis with newly depressed lvef 25% (from 60% on \'[**77**]). current hospitalization c/b new onset rapid a flutter v. a tach with 2:1 conduction, cardioversion to nsr [**3-10**] c/b hypotension requiring neo, arf with cr up to 2.7, extremely labile bp requiring both labetalol and neo at times. pa line placed [**3-11**] revealed ci of 1.7, up to 3 after starting milrinone, was self d/c\'d [**3-12**].\nros:\ncv: cont labetolol 0.5-1.5mg/min to maintain diastolic blood pressure 100-120, ranging 90s-150s/ depending on level of alertness. milrinone weaned to 0.25mcg/kg/min. heart rate sb 58-60, no ectopy, hct stable, am labs pending. no c/o cp/sob. distal pulses palp/dop, bp equal bilat ues. plan for cath today to eval coronaries and hemodynamics.\n\nresp: nc frequently dislodged, spo2 on ra 89-96%. ls clear, diminished @ bases with fine rales 1/4 up posteriorly. bilat atelectasis appreciated on mri.\n\ngi/gu: abd soft, nontender, nondistended, +bs/-bm, tolerating by mouth meds with sips. npo after mn for cath [**3-15**].  foley draining cyu, excellent response to 60mg lasix ivp given @ [**2174**]. +325 yesterday, -850 since mn. am bun/cr pending. mri revealing that renal artery perfusion is not inhibited by dissection.\n\nid: afebrile although warm to touch. tmax 98.6 by mouth. wbc 5.8(5.6)\n\nskin: multiple areas of ecchymosis. r hand 22g piv erythematous, nontender, flushes easily, left in d/t poor peripheral access. lac also needs to be d/c\'d (in on [**3-10**]). l hand edematous from ? infiltration of old iv site.\n\nneuro: a&amp;ox3, dangling at bedside at times and c/o restlessness (baseline). tylenol for back pain with relief.\n\na: 84yo with type b descending arotic dissection, bp cont labile and cont to require labetalol. also cont on milrinone. improving renal sts, responded well to diuresis.\np: to cath today to eval hemodynamic sts, follow up am labs. monitor fluid sts. teaching re: procedure, continue to support patient. and family. ? start by mouth bb.\n', 'event': ['Pain', 'Sleep', 'Excretion', 'Family', 'Eating'], 'event_id': ['e1', 'e2', 'e3', 'e4', 'e5'], 'phrase': '', 'raw_output': '{\n  "events": [\n    {\n      "event_id": "e1",\n      "event_type": "Pain",\n      "text_quote": "back pain with relief",\n      "attributes": {\n        "severity": "Unknown",\n        "location": "back",\n        "duration": "Unknown",\n        "negation": "false",\n        "time": "Unknown",\n        "caused_by": "Tylenol"\n      }\n    },\n    {\n      "event_id": "e2",\n      "event_type": "Sleep",\n      "text_quote": "dangling at bedside at times and c/o restlessness (baseline)",\n      "attributes": {\n        "quality": "restless",\n        "duration": "Unknown",\n        "negation": "false",\n        "time": "Unknown",\n        "caused_by": "Unknown"\n      }\n    },\n    {\n      "event_id": "e3",\n      "event_type": "Excretion",\n      "text_quote": "+325 yesterday, -850 since mn.",\n      "attributes": {\n        "type": "urine",\n        "frequency": "Unknown",\n        "quality": "Unknown",\n        "negation": "false",\n        "time": "yesterday and morning",\n        "caused_by": "60mg lasix ivp"\n      }\n    },\n    {\n      "event_id": "e4",\n      "event_type": "Family",\n      "text_quote": "continue to support patient. and family.",\n      "attributes": {\n        "interaction": "Unknown",\n        "relation": "Unknown",\n        "negation": "false",\n        "time": "Unknown",\n        "caused_by": "Unknown"\n      }\n    },\n    {\n      "event_id": "e5",\n      "event_type": "Eating",\n      "text_quote": "tolerating by mouth meds with sips.",\n      "attributes": {\n        "food": "Unknown",\n        "amount": "sips",\n        "method": "oral",\n        "negation": "false",\n        "time": "Unknown",\n        "caused_by": "Unknown"\n      }\n    }\n  ],\n  "order": []\n}', 'attributes': [{'Pain': {'severity': 'Unknown', 'location': 'back', 'duration': 'Unknown', 'negation': 'false', 'time': 'Unknown', 'caused_by': 'Tylenol'}}, {'Sleep': {'quality': 'restless', 'duration': 'Unknown', 'negation': 'false', 'time': 'Unknown', 'caused_by': 'Unknown'}}, {'Excretion': {'type': 'urine', 'frequency': 'Unknown', 'quality': 'Unknown', 'negation': 'false', 'time': 'yesterday and morning', 'caused_by': '60mg lasix ivp'}}, {'Family': {'interaction': 'Unknown', 'relation': 'Unknown', 'negation': 'false', 'time': 'Unknown', 'caused_by': 'Unknown'}}, {'Eating': {'food': 'Unknown', 'amount': 'sips', 'method': 'oral', 'negation': 'false', 'time': 'Unknown', 'caused_by': 'Unknown'}}], 'orders': [[]], 'text_quotes': ['back pain with relief', 'dangling at bedside at times and c/o restlessness (baseline)', '+325 yesterday, -850 since mn.', 'continue to support patient. and family.', 'tolerating by mouth meds with sips.'], 'event_name_prompt': 'Given the text: ccu npn 7p-7a\ns: "when am i going to be able to get out of bed and walk around?"\no: see carevue and update for complete assessment data\nhpi: 84yo admitted [**3-10**] w/sob and backpain found to have type b aortic dissection descending from thoracic aorta to l common iliac artery. h/o htn, type a dissection \'[**77**] status post emergent surgical repair c/b embolic cva. tee [**3-10**] showed global hypokinesis with newly depressed lvef 25% (from 60% on \'[**77**]). current hospitalization c/b new onset rapid a flutter v. a tach with 2:1 conduction, cardioversion to nsr [**3-10**] c/b hypotension requiring neo, arf with cr up to 2.7, extremely labile bp requiring both labetalol and neo at times. pa line placed [**3-11**] revealed ci of 1.7, up to 3 after starting milrinone, was self d/c\'d [**3-12**].\nros:\ncv: cont labetolol 0.5-1.5mg/min to maintain diastolic blood pressure 100-120, ranging 90s-150s/ depending on level of alertness. milrinone weaned to 0.25mcg/kg/min. heart rate sb 58-60, no ectopy, hct stable, am labs pending. no c/o cp/sob. distal pulses palp/dop, bp equal bilat ues. plan for cath today to eval coronaries and hemodynamics.\n\nresp: nc frequently dislodged, spo2 on ra 89-96%. ls clear, diminished @ bases with fine rales 1/4 up posteriorly. bilat atelectasis appreciated on mri.\n\ngi/gu: abd soft, nontender, nondistended, +bs/-bm, tolerating by mouth meds with sips. npo after mn for cath [**3-15**].  foley draining cyu, excellent response to 60mg lasix ivp given @ [**2174**]. +325 yesterday, -850 since mn. am bun/cr pending. mri revealing that renal artery perfusion is not inhibited by dissection.\n\nid: afebrile although warm to touch. tmax 98.6 by mouth. wbc 5.8(5.6)\n\nskin: multiple areas of ecchymosis. r hand 22g piv erythematous, nontender, flushes easily, left in d/t poor peripheral access. lac also needs to be d/c\'d (in on [**3-10**]). l hand edematous from ? infiltration of old iv site.\n\nneuro: a&amp;ox3, dangling at bedside at times and c/o restlessness (baseline). tylenol for back pain with relief.\n\na: 84yo with type b descending arotic dissection, bp cont labile and cont to require labetalol. also cont on milrinone. improving renal sts, responded well to diuresis.\np: to cath today to eval hemodynamic sts, follow up am labs. monitor fluid sts. teaching re: procedure, continue to support patient. and family. ? start by mouth bb.\n, \n                        and the following event types with their definitions: Eating : The patient takes food into their body by mouth.\nExcretion : The patient discharges waste matter from their body.\nFamily : The patient has a visit, call, or communication with a family member.\nPain : The patient reports or shows signs of pain.\nSleep : The patient sleeps or the sleep’s quality or quantity is described.\nUnknown : choose "Unknown" if none of the other event type are applicable. \n                        ---\n                        Your task:\n                        0. Identify ALL events in the text (zero, one, or more).\n1. For each event, assign an event_type from the list above.\n2. If multiple event of same type is mentioned, assign the event_type multiple times\n3. Extract attributes for each event using ONLY the allowed attributes listed below.\n4. Use keyword evidence (Ki) ONLY if it is consistent with the text context.\n5. Output strictly valid JSON following the schema below.\n                        ---\n                        Classification Rules:\n                        - A text may contain multiple events of the same or different types.\n- Create a separate event object for each event mention.\n- If the text is explicitly a NEGATION (e.g., "denies pain"), do not extract that event.\n- If the text describes a FUTURE or HYPOTHETICAL event (e.g., "will eat tomorrow"), ignore it.\n- A valid event should have occurred in the recent past or is occurring during the time of writing of the text.\n- If no events are found or if unsure, return {"events": []}\n                        \n                        ---\n                                    Attributes allowed:\n                                    {\'Eating\': {\'food\': \'&lt;string&gt; # e.g., pancakes, porridge, etc.\', \'amount\': \'&lt;string&gt; # e.g., 1, 2 bowls, etc.\', \'method\': \'&lt;string&gt;  # e.g., oral, tube, etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, evening etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}, \'Excretion\': {\'type\': \'&lt;string&gt; # e.g., urine, stool, etc.\', \'frequency\': \'&lt;string&gt; # e.g., 2x, once, etc.\', \'quality\': \'&lt;string&gt; # e.g., loose, hard, etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, evening etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}, \'Family\': {\'interaction\': \'&lt;string&gt; # e.g., visit, call, communication, etc.\', \'relation\': \'&lt;string&gt; # e.g., mother, son, etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, evening etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}, \'Pain\': {\'severity\': \'&lt;string&gt; # e.g., mild, moderate, severe, numeric scale if present, etc.\', \'location\': \'&lt;string&gt; # e.g., right knee, head, etc.\', \'duration\': \'&lt;string&gt; # e.g., all night, 3 hours, etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, evening etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}, \'Sleep\': {\'quality\': \'&lt;string&gt; # e.g., good, poor, restless, etc.\', \'duration\': \'&lt;string&gt; # e.g., 6 hours, phrases like "all night", etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, evening etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}}\n                                    If no relevant attribute exists for an event, return an empty object {}.\n                                    \n                        \n                        ---\n                                    Keyword evidence (Ki):\n                                    Additional facts: A keyword matching algorithm without context detected keyword(s) (\'pain\', \'family\').\n                                    Use this only as a pointer. If context contradicts, ignore.\n                        ---\n                        Output Schema (strict):\n                        {\n                                    "events": [\n                                        {\n                                        "event_id": "&lt; A unique id eg.: e1 | e2 |...&gt;"\n                                        "event_type": "&lt;Pain | Sleep | Excretion | Eating | Family&gt;",\n                                        "text_quote": "&lt;fragement from the text indicating the event_type&gt;",\n                "attributes": {\n                    "&lt;attribute_name&gt;": "&lt;attribute_value&gt;"\n                }\n                                        }\n                                    ],\n                                    "order": [\n                                        ["e1", "before" | "after" | "simultaneous", "e2" ]\n                                    ]\n                                    }\n                        \n                            Rules:\n                                - Ensure the output is valid JSON (parseable).\n                                - "eventS" must always be an array (can be empty).\n                                - Multiple instances of the same event type appear with different ids.\n                                - Events appear in the array in the same order in which they appear in the text.\n                                - Their partial orders can be expressed using the "order" section.\n                                - Do not include extra keys, comments, or text.\n                                - Each object in "events" must contain "event_type", "text_quote", and "attributes".\n                                - If an event attribute type has no value mentioned, return "attributes": {"&lt; attribute name &gt;:Unknown"} for each attribute type defined for the event type \n                        \n                        \n                        \n                ---\n                Examples:\n                \n                text: "Patient ate breakfast this morning. He seems less anxious."\n                output: {\n                "events": [\n                    {"event_id": "e1",\n                    "event_type": "Eating",\n                    "text_quote":"Patient ate breakfast this morning",\n                    "attributes": {"food": "breakfast", \n                                   "amount": "Unknown",\n                                   "method": "Unknown",\n                                   "negation": "false",\n                                   "time":"morning",\n                                   "caused_by":"Unknown"}\n                    }\n                ],\n                "order":[]\n                }\n                \n                text: "Patient reported severe abdominal pain."\n                output: {\n                "events": [\n                    {"event_id": "e1",\n                    "event_type": "Pain",\n                    "text_quote": "severe abdominal Pain",\n                    "attributes": {"severity": "severe", \n                                   "location": "abdominal",\n                                   "duration": "Unknown",\n                                   "negation": "false",\n                                   "time":"Unknown",\n                                   "caused_by":"Unknown"}\n                    }\n                ],\n                "order":[]\n                }\n                \n                text: "Patient called his son around 3 pm."\n                output: {\n                "events": [\n                    {"event_id": "e1",\n                    "event_type": "Family",\n                    "text_quote": "called his son around 3 pm",\n                    "attributes": {"interaction": "call", \n                                    "relation": "son",\n                                    "negation": "false",\n                                    "time":"3 pm",\n                                    "caused_by":"Unknown"}\n                    }\n                ],\n                "order":[]\n                }\n                \n                text: "Patient had a loose stool overnight."\n                output: {\n                "events": [\n                    {"event_id": "e1",\n                    "event_type": "Excretion",\n                    "text_quote": "loose stool overnight",\n                    "attributes": {"type": "stool", \n                                   "quality": "loose", \n                                   "frequency":"overnight", \n                                   "negation": "false",\n                                   "time":"night",\n                                   "caused_by":"Unknown"}\n                    }\n                ],\n                "order":[]\n                }\n                \n                text: "Patient was able to sleep well last night."\n                output: {\n                "events": [\n                    {"event_id": "e1",\n                    "event_type": "Sleep",\n                    "text_quote": "sleep well last night",\n                    "attributes": {"quality": "well",\n                                    "duration": "Unknown", \n                                    "negation": "false",\n                                    "time":"night",\n                                    "caused_by":"Unknown"}\n                    }\n                ],\n                "order":[]\n                }\n                \n                text: "The patient couldn\'t sleep due to severe pain."\n                output: {\n                "events": [\n                    {"event_id": "e1",\n                    "event_type": "Sleep",\n                    "text_quote": "couldn\'t sleep",\n                    "attributes": {"quality": "poor", \n                                    "duration": "Unknown",\n                                    "negation": "true",\n                                    "time":"Unknown",\n                                    "caused_by":"Pain"}\n                    },\n                    {"event_id": "e2",\n                    "event_type": "Pain",\n                    "text_quote": "severe pain",\n                    "attributes": {"severity": "severe", \n                                    "location": "Unknown", \n                                    "duration": "Unknown", \n                                    "time":"Unknown",\n                                    "caused_by":"Unknown"}\n                    }\n                ],\n                "order":["e1", "after", "e2"]\n                }\n                \n                text: "The patient complained of severe back pain, was given Tylenol, but the pain persisted and he was then prescribed stronger morphine."\n                output: {\n                "events": [\n                    {"event_id": "e1",\n                    "event_type": "Pain",\n                    "text_quote": "complained of severe back pain",\n                    "attributes": {"severity": "severe", \n                                    "location": "back",\n                                    "duration": "Unknown", \n                                    "time":"Unknown",\n                                    "caused_by":"Unknown"}\n                    },\n                    {"event_id": "e2",\n                    "event_type": "Pain",\n                    "text_quote": "pain persisted",\n                    "attributes": {"severity": "severe", \n                                   "location": "back",\n                                   "duration": "persistent", \n                                   "time":"after Tylenol",\n                                   "caused_by":"Unknown"}\n                    }\n                ],\n                "order":[["e1", "before", "e2"]]\n                }\n                \n                        ', 'event_detection_time': 16.602070035994984}</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>[{'Pain': {'severity': 'Unknown', 'location': 'back', 'duration': 'Unknown', 'time': 'Unknown', 'caused_by': 'Unknown'}}, {'Pain': {'severity': 'Unknown', 'location': 'back', 'duration': 'Unknown', 'time': 'Unknown', 'caused_by': 'Tylenol'}}, {'Sleep': {'quality': 'restless', 'duration': 'Unknown', 'time': 'Unknown', 'caused_by': 'Unknown'}}, {'Family': {'interaction': 'support', 'relation': 'family', 'time': 'Unknown', 'caused_by': 'Unknown'}}]</t>
+          <t>['Pain', 'Sleep', 'Excretion', 'Family', 'Eating']</t>
         </is>
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>['when am i going to be able to get out of bed and walk around?', 'tylenol for back pain with relief.', 'a&amp;ox3, dangling at bedside at times and c/o restlessness (baseline).', 'continue to support patient. and family.']</t>
+          <t>[{'Pain': {'severity': 'Unknown', 'location': 'back', 'duration': 'Unknown', 'negation': 'false', 'time': 'Unknown', 'caused_by': 'Tylenol'}}, {'Sleep': {'quality': 'restless', 'duration': 'Unknown', 'negation': 'false', 'time': 'Unknown', 'caused_by': 'Unknown'}}, {'Excretion': {'type': 'urine', 'frequency': 'Unknown', 'quality': 'Unknown', 'negation': 'false', 'time': 'yesterday and morning', 'caused_by': '60mg lasix ivp'}}, {'Family': {'interaction': 'Unknown', 'relation': 'Unknown', 'negation': 'false', 'time': 'Unknown', 'caused_by': 'Unknown'}}, {'Eating': {'food': 'Unknown', 'amount': 'sips', 'method': 'oral', 'negation': 'false', 'time': 'Unknown', 'caused_by': 'Unknown'}}]</t>
         </is>
       </c>
       <c r="I11" t="inlineStr">
         <is>
-          <t>{'text': 'ccu npn 7p-7a\ns: "when am i going to be able to get out of bed and walk around?"\no: see carevue and update for complete assessment data\nhpi: 84yo admitted [**3-10**] w/sob and backpain found to have type b aortic dissection descending from thoracic aorta to l common iliac artery. h/o htn, type a dissection \'[**77**] status post emergent surgical repair c/b embolic cva. tee [**3-10**] showed global hypokinesis with newly depressed lvef 25% (from 60% on \'[**77**]). current hospitalization c/b new onset rapid a flutter v. a tach with 2:1 conduction, cardioversion to nsr [**3-10**] c/b hypotension requiring neo, arf with cr up to 2.7, extremely labile bp requiring both labetalol and neo at times. pa line placed [**3-11**] revealed ci of 1.7, up to 3 after starting milrinone, was self d/c\'d [**3-12**].\nros:\ncv: cont labetolol 0.5-1.5mg/min to maintain diastolic blood pressure 100-120, ranging 90s-150s/ depending on level of alertness. milrinone weaned to 0.25mcg/kg/min. heart rate sb 58-60, no ectopy, hct stable, am labs pending. no c/o cp/sob. distal pulses palp/dop, bp equal bilat ues. plan for cath today to eval coronaries and hemodynamics.\n\nresp: nc frequently dislodged, spo2 on ra 89-96%. ls clear, diminished @ bases with fine rales 1/4 up posteriorly. bilat atelectasis appreciated on mri.\n\ngi/gu: abd soft, nontender, nondistended, +bs/-bm, tolerating by mouth meds with sips. npo after mn for cath [**3-15**].  foley draining cyu, excellent response to 60mg lasix ivp given @ [**2174**]. +325 yesterday, -850 since mn. am bun/cr pending. mri revealing that renal artery perfusion is not inhibited by dissection.\n\nid: afebrile although warm to touch. tmax 98.6 by mouth. wbc 5.8(5.6)\n\nskin: multiple areas of ecchymosis. r hand 22g piv erythematous, nontender, flushes easily, left in d/t poor peripheral access. lac also needs to be d/c\'d (in on [**3-10**]). l hand edematous from ? infiltration of old iv site.\n\nneuro: a&amp;ox3, dangling at bedside at times and c/o restlessness (baseline). tylenol for back pain with relief.\n\na: 84yo with type b descending arotic dissection, bp cont labile and cont to require labetalol. also cont on milrinone. improving renal sts, responded well to diuresis.\np: to cath today to eval hemodynamic sts, follow up am labs. monitor fluid sts. teaching re: procedure, continue to support patient. and family. ? start by mouth bb.\n', 'event': ['Pain', 'Family', 'Sleep', 'Excretion', 'Eating', 'Excretion'], 'phrase': '', 'raw_output': '{\n  "events": [\n    {\n      "event_type": "Pain",\n      "text_quote": "tylenol for back pain with relief.",\n      "attributes": {\n        "severity": "Unknown",\n        "location": "back",\n        "duration": "Unknown",\n        "negation": false,\n        "time": "Unknown",\n        "caused_by": "Unknown"\n      }\n    },\n    {\n      "event_type": "Family",\n      "text_quote": "continue to support patient. and family.",\n      "attributes": {\n        "interaction": "Unknown",\n        "relation": "Unknown",\n        "negation": false,\n        "time": "Unknown",\n        "caused_by": "Unknown"\n      }\n    },\n    {\n      "event_type": "Sleep",\n      "text_quote": "a&amp;ox3, dangling at bedside at times and c/o restlessness (baseline).",\n      "attributes": {\n        "quality": "restless",\n        "duration": "Unknown",\n        "negation": false,\n        "time": "Unknown",\n        "caused_by": "Unknown"\n      }\n    },\n    {\n      "event_type": "Excretion",\n      "text_quote": "+325 yesterday, -850 since mn.",\n      "attributes": {\n        "type": "urine",\n        "frequency": "Unknown",\n        "quality": "Unknown",\n        "negation": false,\n        "time": "yesterday and morning",\n        "caused_by": "60mg lasix ivp"\n      }\n    },\n    {\n      "event_type": "Eating",\n      "text_quote": "tolerating by mouth meds with sips.",\n      "attributes": {\n        "food": "Unknown",\n        "amount": "sips",\n        "method": "oral",\n        "negation": false,\n        "time": "Unknown",\n        "caused_by": "Unknown"\n      }\n    },\n    {\n      "event_type": "Excretion",\n      "text_quote": "foley draining cyu, excellent response to 60mg lasix ivp given @ [2174].",\n      "attributes": {\n        "type": "urine",\n        "frequency": "Unknown",\n        "quality": "Unknown",\n        "negation": false,\n        "time": "[2174]",\n        "caused_by": "60mg lasix ivp"\n      }\n    }\n  ]\n}', 'attributes': [{'Pain': {'severity': 'Unknown', 'location': 'back', 'duration': 'Unknown', 'negation': False, 'time': 'Unknown', 'caused_by': 'Unknown'}}, {'Family': {'interaction': 'Unknown', 'relation': 'Unknown', 'negation': False, 'time': 'Unknown', 'caused_by': 'Unknown'}}, {'Sleep': {'quality': 'restless', 'duration': 'Unknown', 'negation': False, 'time': 'Unknown', 'caused_by': 'Unknown'}}, {'Excretion': {'type': 'urine', 'frequency': 'Unknown', 'quality': 'Unknown', 'negation': False, 'time': 'yesterday and morning', 'caused_by': '60mg lasix ivp'}}, {'Eating': {'food': 'Unknown', 'amount': 'sips', 'method': 'oral', 'negation': False, 'time': 'Unknown', 'caused_by': 'Unknown'}}, {'Excretion': {'type': 'urine', 'frequency': 'Unknown', 'quality': 'Unknown', 'negation': False, 'time': '[2174]', 'caused_by': '60mg lasix ivp'}}], 'text_quotes': ['tylenol for back pain with relief.', 'continue to support patient. and family.', 'a&amp;ox3, dangling at bedside at times and c/o restlessness (baseline).', '+325 yesterday, -850 since mn.', 'tolerating by mouth meds with sips.', 'foley draining cyu, excellent response to 60mg lasix ivp given @ [2174].'], 'event_name_prompt': 'Given the text: ccu npn 7p-7a\ns: "when am i going to be able to get out of bed and walk around?"\no: see carevue and update for complete assessment data\nhpi: 84yo admitted [**3-10**] w/sob and backpain found to have type b aortic dissection descending from thoracic aorta to l common iliac artery. h/o htn, type a dissection \'[**77**] status post emergent surgical repair c/b embolic cva. tee [**3-10**] showed global hypokinesis with newly depressed lvef 25% (from 60% on \'[**77**]). current hospitalization c/b new onset rapid a flutter v. a tach with 2:1 conduction, cardioversion to nsr [**3-10**] c/b hypotension requiring neo, arf with cr up to 2.7, extremely labile bp requiring both labetalol and neo at times. pa line placed [**3-11**] revealed ci of 1.7, up to 3 after starting milrinone, was self d/c\'d [**3-12**].\nros:\ncv: cont labetolol 0.5-1.5mg/min to maintain diastolic blood pressure 100-120, ranging 90s-150s/ depending on level of alertness. milrinone weaned to 0.25mcg/kg/min. heart rate sb 58-60, no ectopy, hct stable, am labs pending. no c/o cp/sob. distal pulses palp/dop, bp equal bilat ues. plan for cath today to eval coronaries and hemodynamics.\n\nresp: nc frequently dislodged, spo2 on ra 89-96%. ls clear, diminished @ bases with fine rales 1/4 up posteriorly. bilat atelectasis appreciated on mri.\n\ngi/gu: abd soft, nontender, nondistended, +bs/-bm, tolerating by mouth meds with sips. npo after mn for cath [**3-15**].  foley draining cyu, excellent response to 60mg lasix ivp given @ [**2174**]. +325 yesterday, -850 since mn. am bun/cr pending. mri revealing that renal artery perfusion is not inhibited by dissection.\n\nid: afebrile although warm to touch. tmax 98.6 by mouth. wbc 5.8(5.6)\n\nskin: multiple areas of ecchymosis. r hand 22g piv erythematous, nontender, flushes easily, left in d/t poor peripheral access. lac also needs to be d/c\'d (in on [**3-10**]). l hand edematous from ? infiltration of old iv site.\n\nneuro: a&amp;ox3, dangling at bedside at times and c/o restlessness (baseline). tylenol for back pain with relief.\n\na: 84yo with type b descending arotic dissection, bp cont labile and cont to require labetalol. also cont on milrinone. improving renal sts, responded well to diuresis.\np: to cath today to eval hemodynamic sts, follow up am labs. monitor fluid sts. teaching re: procedure, continue to support patient. and family. ? start by mouth bb.\n, \n                        and the following event types with their definitions: Eating : The patient takes food into their body by mouth.\nExcretion : The patient discharges waste matter from their body.\nFamily : The patient has a visit, call, or communication with a family member.\nPain : The patient reports or shows signs of pain.\nSleep : The patient sleeps or the sleep’s quality or quantity is described.\nUnknown : choose "Unknown" if none of the other event type are applicable. \n                        ---\n                        Your task:\n                        0. Identify ALL events in the text (zero, one, or more).\n1. For each event, assign an event_type from the list above.\n2. If multiple event of same type is mentioned, assign the event_type multiple times\n3. Extract attributes for each event using ONLY the allowed attributes listed below.\n4. Use keyword evidence (Ki) ONLY if it is consistent with the text context.\n5. Output strictly valid JSON following the schema below.\n                        ---\n                        Classification Rules:\n                        - A text may contain multiple events of the same or different types.\n- Create a separate event object for each event mention.\n- If the text is explicitly a NEGATION (e.g., "denies pain"), do not extract that event.\n- If the text describes a FUTURE or HYPOTHETICAL event (e.g., "will eat tomorrow"), ignore it.\n- A valid event should have occurred in the recent past or is occurring during the time of writing of the text.\n- If no events are found or if unsure, return {"events": []}\n                        \n                        ---\n                                    Attributes allowed:\n                                    {\'Eating\': {\'food\': \'&lt;string&gt; # e.g., pancakes, porridge, etc.\', \'amount\': \'&lt;string&gt; # e.g., 1, 2 bowls, etc.\', \'method\': \'&lt;string&gt;  # e.g., oral, tube, etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, after shower, etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}, \'Excretion\': {\'type\': \'&lt;string&gt; # e.g., urine, stool, etc.\', \'frequency\': \'&lt;string&gt; # e.g., 2x, once, etc.\', \'quality\': \'&lt;string&gt; # e.g., loose, hard, etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, after shower, etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}, \'Family\': {\'interaction\': \'&lt;string&gt; # e.g., visit, call, communication, etc.\', \'relation\': \'&lt;string&gt; # e.g., mother, son, etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, after shower, etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}, \'Pain\': {\'severity\': \'&lt;string&gt; # e.g., mild, moderate, severe, numeric scale if present, etc.\', \'location\': \'&lt;string&gt; # e.g., right knee, head, etc.\', \'duration\': \'&lt;string&gt; # e.g., all night, 3 hours, etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, after shower, etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}, \'Sleep\': {\'quality\': \'&lt;string&gt; # e.g., good, poor, restless, etc.\', \'duration\': \'&lt;string&gt; # e.g., 6 hours, phrases like "all night", etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, after shower, etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}}\n                                    If no relevant attribute exists for an event, return an empty object {}.\n                                    \n                        \n                        ---\n                                    Keyword evidence (Ki):\n                                    Additional facts: A keyword matching algorithm without context detected keyword(s) [\'family\', \'pain\'].\n                                    Use this only as a pointer. If context contradicts, ignore.\n                        ---\n                        Output Schema (strict):\n                        {\n                                    "events": [\n                                        {\n                                        "event_type": "&lt;Pain | Sleep | Excretion | Eating | Family&gt;",\n                                        "text_quote": "&lt;fragement from the text indicating &gt;",\n                "attributes": {\n                    "&lt;attribute_name&gt;": "&lt;attribute_value&gt;"\n                }\n                                        }\n                                    ]\n                                    }\n                        \n                            Rules:\n                                - Ensure the output is valid JSON (parseable).\n                                - "eventS" must always be an array (can be empty).\n                                - Multiple instances of the same event type appear as individual elements in the event array.\n                                - Events appear in the array in the same order in which they appear in the text.\n                                - Do not include extra keys, comments, or text.\n                                - Each object in "events" must contain "event_type", "text_quote", and "attributes".\n                                -If an event attribute type has no value mentioned, return "attributes": {"&lt; attribute name &gt;:Unknown"} for each attribute type defined for the event type \n                        \n                        \n                        \n                        ', 'event_detection_time': 16.90746971098997}</t>
+          <t>['back pain with relief', 'dangling at bedside at times and c/o restlessness (baseline)', '+325 yesterday, -850 since mn.', 'continue to support patient. and family.', 'tolerating by mouth meds with sips.']</t>
         </is>
       </c>
       <c r="J11" t="inlineStr">
         <is>
-          <t>['Pain', 'Family', 'Sleep', 'Excretion', 'Eating', 'Excretion']</t>
+          <t>[[]]</t>
         </is>
       </c>
       <c r="K11" t="inlineStr">
         <is>
-          <t>[{'Pain': {'severity': 'Unknown', 'location': 'back', 'duration': 'Unknown', 'negation': False, 'time': 'Unknown', 'caused_by': 'Unknown'}}, {'Family': {'interaction': 'Unknown', 'relation': 'Unknown', 'negation': False, 'time': 'Unknown', 'caused_by': 'Unknown'}}, {'Sleep': {'quality': 'restless', 'duration': 'Unknown', 'negation': False, 'time': 'Unknown', 'caused_by': 'Unknown'}}, {'Excretion': {'type': 'urine', 'frequency': 'Unknown', 'quality': 'Unknown', 'negation': False, 'time': 'yesterday and morning', 'caused_by': '60mg lasix ivp'}}, {'Eating': {'food': 'Unknown', 'amount': 'sips', 'method': 'oral', 'negation': False, 'time': 'Unknown', 'caused_by': 'Unknown'}}, {'Excretion': {'type': 'urine', 'frequency': 'Unknown', 'quality': 'Unknown', 'negation': False, 'time': '[2174]', 'caused_by': '60mg lasix ivp'}}]</t>
+          <t>{'text': 'ccu npn 7p-7a\ns: "when am i going to be able to get out of bed and walk around?"\no: see carevue and update for complete assessment data\nhpi: 84yo admitted [**3-10**] w/sob and backpain found to have type b aortic dissection descending from thoracic aorta to l common iliac artery. h/o htn, type a dissection \'[**77**] status post emergent surgical repair c/b embolic cva. tee [**3-10**] showed global hypokinesis with newly depressed lvef 25% (from 60% on \'[**77**]). current hospitalization c/b new onset rapid a flutter v. a tach with 2:1 conduction, cardioversion to nsr [**3-10**] c/b hypotension requiring neo, arf with cr up to 2.7, extremely labile bp requiring both labetalol and neo at times. pa line placed [**3-11**] revealed ci of 1.7, up to 3 after starting milrinone, was self d/c\'d [**3-12**].\nros:\ncv: cont labetolol 0.5-1.5mg/min to maintain diastolic blood pressure 100-120, ranging 90s-150s/ depending on level of alertness. milrinone weaned to 0.25mcg/kg/min. heart rate sb 58-60, no ectopy, hct stable, am labs pending. no c/o cp/sob. distal pulses palp/dop, bp equal bilat ues. plan for cath today to eval coronaries and hemodynamics.\n\nresp: nc frequently dislodged, spo2 on ra 89-96%. ls clear, diminished @ bases with fine rales 1/4 up posteriorly. bilat atelectasis appreciated on mri.\n\ngi/gu: abd soft, nontender, nondistended, +bs/-bm, tolerating by mouth meds with sips. npo after mn for cath [**3-15**].  foley draining cyu, excellent response to 60mg lasix ivp given @ [**2174**]. +325 yesterday, -850 since mn. am bun/cr pending. mri revealing that renal artery perfusion is not inhibited by dissection.\n\nid: afebrile although warm to touch. tmax 98.6 by mouth. wbc 5.8(5.6)\n\nskin: multiple areas of ecchymosis. r hand 22g piv erythematous, nontender, flushes easily, left in d/t poor peripheral access. lac also needs to be d/c\'d (in on [**3-10**]). l hand edematous from ? infiltration of old iv site.\n\nneuro: a&amp;ox3, dangling at bedside at times and c/o restlessness (baseline). tylenol for back pain with relief.\n\na: 84yo with type b descending arotic dissection, bp cont labile and cont to require labetalol. also cont on milrinone. improving renal sts, responded well to diuresis.\np: to cath today to eval hemodynamic sts, follow up am labs. monitor fluid sts. teaching re: procedure, continue to support patient. and family. ? start by mouth bb.\n', 'event': ['Pain', 'Excretion', 'Excretion', 'Family', 'Sleep', 'Eating', 'Eating'], 'event_id': ['e1', 'e2', 'e3', 'e4', 'e5', 'e6', 'e7'], 'phrase': '', 'raw_output': '{\n  "events": [\n    {\n      "event_id": "e1",\n      "event_type": "Pain",\n      "text_quote": "tylenol for back pain with relief.",\n      "attributes": {\n        "severity": "Unknown",\n        "location": "back",\n        "duration": "Unknown",\n        "negation": false,\n        "time": "Unknown",\n        "caused_by": "Unknown"\n      }\n    },\n    {\n      "event_id": "e2",\n      "event_type": "Excretion",\n      "text_quote": "+325 yesterday, -850 since mn.",\n      "attributes": {\n        "type": "urine",\n        "frequency": "Unknown",\n        "quality": "Unknown",\n        "negation": false,\n        "time": "yesterday and morning",\n        "caused_by": "60mg lasix ivp"\n      }\n    },\n    {\n      "event_id": "e3",\n      "event_type": "Excretion",\n      "text_quote": "+325 yesterday, -850 since mn.",\n      "attributes": {\n        "type": "urine",\n        "frequency": "Unknown",\n        "quality": "Unknown",\n        "negation": false,\n        "time": "yesterday and morning",\n        "caused_by": "60mg lasix ivp"\n      }\n    },\n    {\n      "event_id": "e4",\n      "event_type": "Family",\n      "text_quote": "continue to support patient. and family.",\n      "attributes": {\n        "interaction": "Unknown",\n        "relation": "Unknown",\n        "negation": false,\n        "time": "Unknown",\n        "caused_by": "Unknown"\n      }\n    },\n    {\n      "event_id": "e5",\n      "event_type": "Sleep",\n      "text_quote": "a&amp;ox3, dangling at bedside at times and c/o restlessness (baseline).",\n      "attributes": {\n        "quality": "restless",\n        "duration": "Unknown",\n        "negation": false,\n        "time": "Unknown",\n        "caused_by": "Unknown"\n      }\n    },\n    {\n      "event_id": "e6",\n      "event_type": "Eating",\n      "text_quote": "tolerating by mouth meds with sips.",\n      "attributes": {\n        "food": "Unknown",\n        "amount": "Unknown",\n        "method": "oral",\n        "negation": false,\n        "time": "Unknown",\n        "caused_by": "Unknown"\n      }\n    },\n    {\n      "event_id": "e7",\n      "event_type": "Eating",\n      "text_quote": "npo after mn for cath [3-15].",\n      "attributes": {\n        "food": "Unknown",\n        "amount": "Unknown",\n        "method": "Unknown",\n        "negation": true,\n        "time": "after morning",\n        "caused_by": "cath"\n      }\n    }\n  ],\n  "order": [\n    ["e1", "before", "e2"],\n    ["e2", "simultaneous", "e3"],\n    ["e3", "before", "e4"],\n    ["e4", "after", "e5"],\n    ["e5", "before", "e6"],\n    ["e6", "before", "e7"]\n  ]\n}', 'attributes': [{'Pain': {'severity': 'Unknown', 'location': 'back', 'duration': 'Unknown', 'negation': False, 'time': 'Unknown', 'caused_by': 'Unknown'}}, {'Excretion': {'type': 'urine', 'frequency': 'Unknown', 'quality': 'Unknown', 'negation': False, 'time': 'yesterday and morning', 'caused_by': '60mg lasix ivp'}}, {'Excretion': {'type': 'urine', 'frequency': 'Unknown', 'quality': 'Unknown', 'negation': False, 'time': 'yesterday and morning', 'caused_by': '60mg lasix ivp'}}, {'Family': {'interaction': 'Unknown', 'relation': 'Unknown', 'negation': False, 'time': 'Unknown', 'caused_by': 'Unknown'}}, {'Sleep': {'quality': 'restless', 'duration': 'Unknown', 'negation': False, 'time': 'Unknown', 'caused_by': 'Unknown'}}, {'Eating': {'food': 'Unknown', 'amount': 'Unknown', 'method': 'oral', 'negation': False, 'time': 'Unknown', 'caused_by': 'Unknown'}}, {'Eating': {'food': 'Unknown', 'amount': 'Unknown', 'method': 'Unknown', 'negation': True, 'time': 'after morning', 'caused_by': 'cath'}}], 'orders': [[['e1', 'before', 'e2'], ['e2', 'simultaneous', 'e3'], ['e3', 'before', 'e4'], ['e4', 'after', 'e5'], ['e5', 'before', 'e6'], ['e6', 'before', 'e7']]], 'text_quotes': ['tylenol for back pain with relief.', '+325 yesterday, -850 since mn.', '+325 yesterday, -850 since mn.', 'continue to support patient. and family.', 'a&amp;ox3, dangling at bedside at times and c/o restlessness (baseline).', 'tolerating by mouth meds with sips.', 'npo after mn for cath [3-15].'], 'event_name_prompt': 'Given the text: ccu npn 7p-7a\ns: "when am i going to be able to get out of bed and walk around?"\no: see carevue and update for complete assessment data\nhpi: 84yo admitted [**3-10**] w/sob and backpain found to have type b aortic dissection descending from thoracic aorta to l common iliac artery. h/o htn, type a dissection \'[**77**] status post emergent surgical repair c/b embolic cva. tee [**3-10**] showed global hypokinesis with newly depressed lvef 25% (from 60% on \'[**77**]). current hospitalization c/b new onset rapid a flutter v. a tach with 2:1 conduction, cardioversion to nsr [**3-10**] c/b hypotension requiring neo, arf with cr up to 2.7, extremely labile bp requiring both labetalol and neo at times. pa line placed [**3-11**] revealed ci of 1.7, up to 3 after starting milrinone, was self d/c\'d [**3-12**].\nros:\ncv: cont labetolol 0.5-1.5mg/min to maintain diastolic blood pressure 100-120, ranging 90s-150s/ depending on level of alertness. milrinone weaned to 0.25mcg/kg/min. heart rate sb 58-60, no ectopy, hct stable, am labs pending. no c/o cp/sob. distal pulses palp/dop, bp equal bilat ues. plan for cath today to eval coronaries and hemodynamics.\n\nresp: nc frequently dislodged, spo2 on ra 89-96%. ls clear, diminished @ bases with fine rales 1/4 up posteriorly. bilat atelectasis appreciated on mri.\n\ngi/gu: abd soft, nontender, nondistended, +bs/-bm, tolerating by mouth meds with sips. npo after mn for cath [**3-15**].  foley draining cyu, excellent response to 60mg lasix ivp given @ [**2174**]. +325 yesterday, -850 since mn. am bun/cr pending. mri revealing that renal artery perfusion is not inhibited by dissection.\n\nid: afebrile although warm to touch. tmax 98.6 by mouth. wbc 5.8(5.6)\n\nskin: multiple areas of ecchymosis. r hand 22g piv erythematous, nontender, flushes easily, left in d/t poor peripheral access. lac also needs to be d/c\'d (in on [**3-10**]). l hand edematous from ? infiltration of old iv site.\n\nneuro: a&amp;ox3, dangling at bedside at times and c/o restlessness (baseline). tylenol for back pain with relief.\n\na: 84yo with type b descending arotic dissection, bp cont labile and cont to require labetalol. also cont on milrinone. improving renal sts, responded well to diuresis.\np: to cath today to eval hemodynamic sts, follow up am labs. monitor fluid sts. teaching re: procedure, continue to support patient. and family. ? start by mouth bb.\n, \n                        and the following event types with their definitions: Eating : The patient takes food into their body by mouth.\nExcretion : The patient discharges waste matter from their body.\nFamily : The patient has a visit, call, or communication with a family member.\nPain : The patient reports or shows signs of pain.\nSleep : The patient sleeps or the sleep’s quality or quantity is described.\nUnknown : choose "Unknown" if none of the other event type are applicable. \n                        ---\n                        Your task:\n                        0. Identify ALL events in the text (zero, one, or more).\n1. For each event, assign an event_type from the list above.\n2. If multiple event of same type is mentioned, assign the event_type multiple times\n3. Extract attributes for each event using ONLY the allowed attributes listed below.\n4. Use keyword evidence (Ki) ONLY if it is consistent with the text context.\n5. Output strictly valid JSON following the schema below.\n                        ---\n                        Classification Rules:\n                        - A text may contain multiple events of the same or different types.\n- Create a separate event object for each event mention.\n- If the text is explicitly a NEGATION (e.g., "denies pain"), do not extract that event.\n- If the text describes a FUTURE or HYPOTHETICAL event (e.g., "will eat tomorrow"), ignore it.\n- A valid event should have occurred in the recent past or is occurring during the time of writing of the text.\n- If no events are found or if unsure, return {"events": []}\n                        \n                        ---\n                                    Attributes allowed:\n                                    {\'Eating\': {\'food\': \'&lt;string&gt; # e.g., pancakes, porridge, etc.\', \'amount\': \'&lt;string&gt; # e.g., 1, 2 bowls, etc.\', \'method\': \'&lt;string&gt;  # e.g., oral, tube, etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, evening etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}, \'Excretion\': {\'type\': \'&lt;string&gt; # e.g., urine, stool, etc.\', \'frequency\': \'&lt;string&gt; # e.g., 2x, once, etc.\', \'quality\': \'&lt;string&gt; # e.g., loose, hard, etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, evening etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}, \'Family\': {\'interaction\': \'&lt;string&gt; # e.g., visit, call, communication, etc.\', \'relation\': \'&lt;string&gt; # e.g., mother, son, etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, evening etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}, \'Pain\': {\'severity\': \'&lt;string&gt; # e.g., mild, moderate, severe, numeric scale if present, etc.\', \'location\': \'&lt;string&gt; # e.g., right knee, head, etc.\', \'duration\': \'&lt;string&gt; # e.g., all night, 3 hours, etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, evening etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}, \'Sleep\': {\'quality\': \'&lt;string&gt; # e.g., good, poor, restless, etc.\', \'duration\': \'&lt;string&gt; # e.g., 6 hours, phrases like "all night", etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, evening etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}}\n                                    If no relevant attribute exists for an event, return an empty object {}.\n                                    \n                        \n                        ---\n                                    Keyword evidence (Ki):\n                                    Additional facts: A keyword matching algorithm without context detected keyword(s) (\'pain\', \'family\').\n                                    Use this only as a pointer. If context contradicts, ignore.\n                        ---\n                        Output Schema (strict):\n                        {\n                                    "events": [\n                                        {\n                                        "event_id": "&lt; A unique id eg.: e1 | e2 |...&gt;"\n                                        "event_type": "&lt;Pain | Sleep | Excretion | Eating | Family&gt;",\n                                        "text_quote": "&lt;fragement from the text indicating the event_type&gt;",\n                "attributes": {\n                    "&lt;attribute_name&gt;": "&lt;attribute_value&gt;"\n                }\n                                        }\n                                    ],\n                                    "order": [\n                                        ["e1", "before" | "after" | "simultaneous", "e2" ]\n                                    ]\n                                    }\n                        \n                            Rules:\n                                - Ensure the output is valid JSON (parseable).\n                                - "eventS" must always be an array (can be empty).\n                                - Multiple instances of the same event type appear with different ids.\n                                - Events appear in the array in the same order in which they appear in the text.\n                                - Their partial orders can be expressed using the "order" section.\n                                - Do not include extra keys, comments, or text.\n                                - Each object in "events" must contain "event_type", "text_quote", and "attributes".\n                                - If an event attribute type has no value mentioned, return "attributes": {"&lt; attribute name &gt;:Unknown"} for each attribute type defined for the event type \n                        \n                        \n                        \n                        ', 'event_detection_time': 23.403584696003236}</t>
         </is>
       </c>
       <c r="L11" t="inlineStr">
         <is>
-          <t>['tylenol for back pain with relief.', 'continue to support patient. and family.', 'a&amp;ox3, dangling at bedside at times and c/o restlessness (baseline).', '+325 yesterday, -850 since mn.', 'tolerating by mouth meds with sips.', 'foley draining cyu, excellent response to 60mg lasix ivp given @ [2174].']</t>
+          <t>['Pain', 'Excretion', 'Excretion', 'Family', 'Sleep', 'Eating', 'Eating']</t>
         </is>
       </c>
       <c r="M11" t="inlineStr">
         <is>
-          <t>{'text': 'ccu npn 7p-7a\ns: "when am i going to be able to get out of bed and walk around?"\no: see carevue and update for complete assessment data\nhpi: 84yo admitted [**3-10**] w/sob and backpain found to have type b aortic dissection descending from thoracic aorta to l common iliac artery. h/o htn, type a dissection \'[**77**] status post emergent surgical repair c/b embolic cva. tee [**3-10**] showed global hypokinesis with newly depressed lvef 25% (from 60% on \'[**77**]). current hospitalization c/b new onset rapid a flutter v. a tach with 2:1 conduction, cardioversion to nsr [**3-10**] c/b hypotension requiring neo, arf with cr up to 2.7, extremely labile bp requiring both labetalol and neo at times. pa line placed [**3-11**] revealed ci of 1.7, up to 3 after starting milrinone, was self d/c\'d [**3-12**].\nros:\ncv: cont labetolol 0.5-1.5mg/min to maintain diastolic blood pressure 100-120, ranging 90s-150s/ depending on level of alertness. milrinone weaned to 0.25mcg/kg/min. heart rate sb 58-60, no ectopy, hct stable, am labs pending. no c/o cp/sob. distal pulses palp/dop, bp equal bilat ues. plan for cath today to eval coronaries and hemodynamics.\n\nresp: nc frequently dislodged, spo2 on ra 89-96%. ls clear, diminished @ bases with fine rales 1/4 up posteriorly. bilat atelectasis appreciated on mri.\n\ngi/gu: abd soft, nontender, nondistended, +bs/-bm, tolerating by mouth meds with sips. npo after mn for cath [**3-15**].  foley draining cyu, excellent response to 60mg lasix ivp given @ [**2174**]. +325 yesterday, -850 since mn. am bun/cr pending. mri revealing that renal artery perfusion is not inhibited by dissection.\n\nid: afebrile although warm to touch. tmax 98.6 by mouth. wbc 5.8(5.6)\n\nskin: multiple areas of ecchymosis. r hand 22g piv erythematous, nontender, flushes easily, left in d/t poor peripheral access. lac also needs to be d/c\'d (in on [**3-10**]). l hand edematous from ? infiltration of old iv site.\n\nneuro: a&amp;ox3, dangling at bedside at times and c/o restlessness (baseline). tylenol for back pain with relief.\n\na: 84yo with type b descending arotic dissection, bp cont labile and cont to require labetalol. also cont on milrinone. improving renal sts, responded well to diuresis.\np: to cath today to eval hemodynamic sts, follow up am labs. monitor fluid sts. teaching re: procedure, continue to support patient. and family. ? start by mouth bb.\n', 'event': ['Pain', 'Sleep', 'Excretion', 'Excretion', 'Eating', 'Family'], 'phrase': '', 'raw_output': '{\n  "events": [\n    {\n      "event_type": "Pain",\n      "text_quote": "c/o back pain",\n      "attributes": {\n        "severity": "Unknown",\n        "location": "back",\n        "duration": "Unknown",\n        "time": "Unknown",\n        "caused_by": "Unknown"\n      }\n    },\n    {\n      "event_type": "Sleep",\n      "text_quote": "a&amp;ox3, dangling at bedside at times and c/o restlessness (baseline)",\n      "attributes": {\n        "quality": "restless",\n        "duration": "Unknown",\n        "time": "Unknown",\n        "caused_by": "Unknown"\n      }\n    },\n    {\n      "event_type": "Excretion",\n      "text_quote": "+325 yesterday, -850 since mn.",\n      "attributes": {\n        "type": "urine",\n        "frequency": "Unknown",\n        "quality": "Unknown",\n        "time": "yesterday and morning",\n        "caused_by": "Unknown"\n      }\n    },\n    {\n      "event_type": "Excretion",\n      "text_quote": "+325 yesterday, -850 since mn.",\n      "attributes": {\n        "type": "urine",\n        "frequency": "Unknown",\n        "quality": "Unknown",\n        "time": "yesterday and morning",\n        "caused_by": "Unknown"\n      }\n    },\n    {\n      "event_type": "Eating",\n      "text_quote": "tolerating by mouth meds with sips.",\n      "attributes": {\n        "food": "meds",\n        "amount": "Unknown",\n        "method": "oral",\n        "time": "Unknown",\n        "caused_by": "Unknown"\n      }\n    },\n    {\n      "event_type": "Family",\n      "text_quote": "continue to support patient. and family.",\n      "attributes": {\n        "interaction": "support",\n        "relation": "family",\n        "time": "Unknown",\n        "caused_by": "Unknown"\n      }\n    }\n  ]\n}', 'attributes': [{'Pain': {'severity': 'Unknown', 'location': 'back', 'duration': 'Unknown', 'time': 'Unknown', 'caused_by': 'Unknown'}}, {'Sleep': {'quality': 'restless', 'duration': 'Unknown', 'time': 'Unknown', 'caused_by': 'Unknown'}}, {'Excretion': {'type': 'urine', 'frequency': 'Unknown', 'quality': 'Unknown', 'time': 'yesterday and morning', 'caused_by': 'Unknown'}}, {'Excretion': {'type': 'urine', 'frequency': 'Unknown', 'quality': 'Unknown', 'time': 'yesterday and morning', 'caused_by': 'Unknown'}}, {'Eating': {'food': 'meds', 'amount': 'Unknown', 'method': 'oral', 'time': 'Unknown', 'caused_by': 'Unknown'}}, {'Family': {'interaction': 'support', 'relation': 'family', 'time': 'Unknown', 'caused_by': 'Unknown'}}], 'text_quotes': ['c/o back pain', 'a&amp;ox3, dangling at bedside at times and c/o restlessness (baseline)', '+325 yesterday, -850 since mn.', '+325 yesterday, -850 since mn.', 'tolerating by mouth meds with sips.', 'continue to support patient. and family.'], 'event_name_prompt': 'Given the text: ccu npn 7p-7a\ns: "when am i going to be able to get out of bed and walk around?"\no: see carevue and update for complete assessment data\nhpi: 84yo admitted [**3-10**] w/sob and backpain found to have type b aortic dissection descending from thoracic aorta to l common iliac artery. h/o htn, type a dissection \'[**77**] status post emergent surgical repair c/b embolic cva. tee [**3-10**] showed global hypokinesis with newly depressed lvef 25% (from 60% on \'[**77**]). current hospitalization c/b new onset rapid a flutter v. a tach with 2:1 conduction, cardioversion to nsr [**3-10**] c/b hypotension requiring neo, arf with cr up to 2.7, extremely labile bp requiring both labetalol and neo at times. pa line placed [**3-11**] revealed ci of 1.7, up to 3 after starting milrinone, was self d/c\'d [**3-12**].\nros:\ncv: cont labetolol 0.5-1.5mg/min to maintain diastolic blood pressure 100-120, ranging 90s-150s/ depending on level of alertness. milrinone weaned to 0.25mcg/kg/min. heart rate sb 58-60, no ectopy, hct stable, am labs pending. no c/o cp/sob. distal pulses palp/dop, bp equal bilat ues. plan for cath today to eval coronaries and hemodynamics.\n\nresp: nc frequently dislodged, spo2 on ra 89-96%. ls clear, diminished @ bases with fine rales 1/4 up posteriorly. bilat atelectasis appreciated on mri.\n\ngi/gu: abd soft, nontender, nondistended, +bs/-bm, tolerating by mouth meds with sips. npo after mn for cath [**3-15**].  foley draining cyu, excellent response to 60mg lasix ivp given @ [**2174**]. +325 yesterday, -850 since mn. am bun/cr pending. mri revealing that renal artery perfusion is not inhibited by dissection.\n\nid: afebrile although warm to touch. tmax 98.6 by mouth. wbc 5.8(5.6)\n\nskin: multiple areas of ecchymosis. r hand 22g piv erythematous, nontender, flushes easily, left in d/t poor peripheral access. lac also needs to be d/c\'d (in on [**3-10**]). l hand edematous from ? infiltration of old iv site.\n\nneuro: a&amp;ox3, dangling at bedside at times and c/o restlessness (baseline). tylenol for back pain with relief.\n\na: 84yo with type b descending arotic dissection, bp cont labile and cont to require labetalol. also cont on milrinone. improving renal sts, responded well to diuresis.\np: to cath today to eval hemodynamic sts, follow up am labs. monitor fluid sts. teaching re: procedure, continue to support patient. and family. ? start by mouth bb.\n, \n                        and the following event types with their definitions: Eating : The patient takes food into their body by mouth.\nExcretion : The patient discharges waste matter from their body.\nFamily : The patient has a visit, call, or communication with a family member.\nPain : The patient reports or shows signs of pain.\nSleep : The patient sleeps or the sleep’s quality or quantity is described.\nUnknown : choose "Unknown" if none of the other event type are applicable. \n                        ---\n                        Your task:\n                        0. Identify ALL events in the text (zero, one, or more).\n1. For each event, assign an event_type from the list above.\n2. If multiple event of same type is mentioned, assign the event_type multiple times\n3. Extract attributes for each event using ONLY the allowed attributes listed below.\n4. Output strictly valid JSON following the schema below.\n                        ---\n                        Classification Rules:\n                        - A text may contain multiple events of the same or different types.\n- Create a separate event object for each event mention.\n- If the text is explicitly a NEGATION (e.g., "denies pain"), do not extract that event.\n- If the text describes a FUTURE or HYPOTHETICAL event (e.g., "will eat tomorrow"), ignore it.\n- A valid event should have occurred in the recent past or is occurring during the time of writing of the text.\n- If no events are found or if unsure, return {"events": []}\n                        \n                        ---\n                                    Attributes allowed:\n                                    {\'Eating\': {\'food\': \'&lt;string&gt; # e.g., pancakes, porridge, etc.\', \'amount\': \'&lt;string&gt; # e.g., 1, 2 bowls, etc.\', \'method\': \'&lt;string&gt;  # e.g., oral, tube, etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, after shower, etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}, \'Excretion\': {\'type\': \'&lt;string&gt; # e.g., urine, stool, etc.\', \'frequency\': \'&lt;string&gt; # e.g., 2x, once, etc.\', \'quality\': \'&lt;string&gt; # e.g., loose, hard, etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, after shower, etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}, \'Family\': {\'interaction\': \'&lt;string&gt; # e.g., visit, call, communication, etc.\', \'relation\': \'&lt;string&gt; # e.g., mother, son, etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, after shower, etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}, \'Pain\': {\'severity\': \'&lt;string&gt; # e.g., mild, moderate, severe, numeric scale if present, etc.\', \'location\': \'&lt;string&gt; # e.g., right knee, head, etc.\', \'duration\': \'&lt;string&gt; # e.g., all night, 3 hours, etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, after shower, etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}, \'Sleep\': {\'quality\': \'&lt;string&gt; # e.g., good, poor, restless, etc.\', \'duration\': \'&lt;string&gt; # e.g., 6 hours, phrases like "all night", etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, after shower, etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}}\n                                    If no relevant attribute exists for an event, return an empty object {}.\n                                    \n                        \n                        \n                        ---\n                        Output Schema (strict):\n                        {\n                                    "events": [\n                                        {\n                                        "event_type": "&lt;Pain | Sleep | Excretion | Eating | Family&gt;",\n                                        "text_quote": "&lt;fragement from the text indicating &gt;",\n                "attributes": {\n                    "&lt;attribute_name&gt;": "&lt;attribute_value&gt;"\n                }\n                                        }\n                                    ]\n                                    }\n                        \n                            Rules:\n                                - Ensure the output is valid JSON (parseable).\n                                - "eventS" must always be an array (can be empty).\n                                - Multiple instances of the same event type appear as individual elements in the event array.\n                                - Events appear in the array in the same order in which they appear in the text.\n                                - Do not include extra keys, comments, or text.\n                                - Each object in "events" must contain "event_type", "text_quote", and "attributes".\n                                -If an event attribute type has no value mentioned, return "attributes": {"&lt; attribute name &gt;:Unknown"} for each attribute type defined for the event type \n                        \n                        \n                        \n                ---\n                Examples:\n                \n                text: "Patient ate breakfast this morning. He seems less anxious."\n                output: {\n                "events": [\n                    {\n                    "event_type": "Eating",\n                    "text_quote":"Patient ate breakfast this morning",\n                    "attributes": {"food": "breakfast", \n                                   "amount": "Unknown",\n                                   "method": "Unknown",\n                                   "time":"morning",\n                                   "caused_by":"Unknown"}\n                    }\n                ]\n                }\n                \n                text: "Patient reported severe abdominal pain."\n                output: {\n                "events": [\n                    {\n                    "event_type": "Pain",\n                    "text_quote": "severe abdominal Pain",\n                    "attributes": {"severity": "severe", \n                                   "location": "abdominal",\n                                   "duration": "Unknown",\n                                   "time":"Unknown",\n                                   "caused_by":"Unknown"}\n                    }\n                ]\n                }\n                \n                text: "Patient called his son around 3 pm."\n                output: {\n                "events": [\n                    {\n                    "event_type": "Family",\n                    "text_quote": "called his son around 3 pm",\n                    "attributes": {"interaction": "call", \n                                    "relation": "son",\n                                    "time":"3 pm",\n                                    "caused_by":"Unknown"}\n                    }\n                ]\n                }\n                \n                text: "Patient had a loose stool overnight."\n                output: {\n                "events": [\n                    {\n                    "event_type": "Excretion",\n                    "text_quote": "loose stool overnight",\n                    "attributes": {"type": "stool", \n                                   "quality": "loose", \n                                   "frequency":"overnight", \n                                   "time":"night",\n                                   "caused_by":"Unknown"}\n                    }\n                ]\n                }\n                \n                text: "Patient was able to sleep well last night."\n                output: {\n                "events": [\n                    {\n                    "event_type": "Sleep",\n                    "text_quote": "sleep well last night",\n                    "attributes": {"quality": "well",\n                                    "duration": "Unknown", \n                                    "time":"night",\n                                    "caused_by":"Unknown"}\n                    }\n                ]\n                }\n                \n                text: "The patient couldn\'t sleep due to severe pain."\n                output: {\n                "events": [\n                    {\n                    "event_type": "Sleep",\n                    "text_quote": "couldn\'t sleep",\n                    "attributes": {"quality": "poor", \n                                    "duration": "Unknown",\n                                   "time":"Unknown",\n                                   "caused_by":"Pain"}\n                    },\n                    {\n                    "event_type": "Pain",\n                    "text_quote": "severe pain",\n                    "attributes": {"severity": "severe", \n                                    "location": "Unknown", \n                                    "duration": "Unknown", \n                                   "time":"before Sleep",\n                                   "caused_by":"Unknown"}\n                    }\n                ]\n                }\n                \n                text: "The patient complained of severe back pain, was given Tylenol, but the pain persisted and he was then prescribed stronger morphine."\n                output: {\n                "events": [\n                    {\n                    "event_type": "Pain",\n                    "text_quote": "complained of severe back pain",\n                    "attributes": {"severity": "severe", \n                                    "location": "back",\n                                    "duration": "Unknown", \n                                    "time":"Unknown",\n                                    "caused_by":"Unknown"}\n                    },\n                    {\n                    "event_type": "Pain",\n                    "text_quote": "pain persisted",\n                    "attributes": {"severity": "severe", \n                                   "location": "back",\n                                   "duration": "persistent", \n                                   "time":"after Tylenol",\n                                   "caused_by":"Unknown"}\n                    }\n                ]\n                }\n                \n                        ', 'event_detection_time': 15.737997104006354}</t>
+          <t>[{'Pain': {'severity': 'Unknown', 'location': 'back', 'duration': 'Unknown', 'negation': False, 'time': 'Unknown', 'caused_by': 'Unknown'}}, {'Excretion': {'type': 'urine', 'frequency': 'Unknown', 'quality': 'Unknown', 'negation': False, 'time': 'yesterday and morning', 'caused_by': '60mg lasix ivp'}}, {'Excretion': {'type': 'urine', 'frequency': 'Unknown', 'quality': 'Unknown', 'negation': False, 'time': 'yesterday and morning', 'caused_by': '60mg lasix ivp'}}, {'Family': {'interaction': 'Unknown', 'relation': 'Unknown', 'negation': False, 'time': 'Unknown', 'caused_by': 'Unknown'}}, {'Sleep': {'quality': 'restless', 'duration': 'Unknown', 'negation': False, 'time': 'Unknown', 'caused_by': 'Unknown'}}, {'Eating': {'food': 'Unknown', 'amount': 'Unknown', 'method': 'oral', 'negation': False, 'time': 'Unknown', 'caused_by': 'Unknown'}}, {'Eating': {'food': 'Unknown', 'amount': 'Unknown', 'method': 'Unknown', 'negation': True, 'time': 'after morning', 'caused_by': 'cath'}}]</t>
         </is>
       </c>
       <c r="N11" t="inlineStr">
         <is>
-          <t>['Pain', 'Sleep', 'Excretion', 'Excretion', 'Eating', 'Family']</t>
+          <t>['tylenol for back pain with relief.', '+325 yesterday, -850 since mn.', '+325 yesterday, -850 since mn.', 'continue to support patient. and family.', 'a&amp;ox3, dangling at bedside at times and c/o restlessness (baseline).', 'tolerating by mouth meds with sips.', 'npo after mn for cath [3-15].']</t>
         </is>
       </c>
       <c r="O11" t="inlineStr">
         <is>
-          <t>[{'Pain': {'severity': 'Unknown', 'location': 'back', 'duration': 'Unknown', 'time': 'Unknown', 'caused_by': 'Unknown'}}, {'Sleep': {'quality': 'restless', 'duration': 'Unknown', 'time': 'Unknown', 'caused_by': 'Unknown'}}, {'Excretion': {'type': 'urine', 'frequency': 'Unknown', 'quality': 'Unknown', 'time': 'yesterday and morning', 'caused_by': 'Unknown'}}, {'Excretion': {'type': 'urine', 'frequency': 'Unknown', 'quality': 'Unknown', 'time': 'yesterday and morning', 'caused_by': 'Unknown'}}, {'Eating': {'food': 'meds', 'amount': 'Unknown', 'method': 'oral', 'time': 'Unknown', 'caused_by': 'Unknown'}}, {'Family': {'interaction': 'support', 'relation': 'family', 'time': 'Unknown', 'caused_by': 'Unknown'}}]</t>
-        </is>
-      </c>
-      <c r="P11" t="inlineStr">
-        <is>
-          <t>['c/o back pain', 'a&amp;ox3, dangling at bedside at times and c/o restlessness (baseline)', '+325 yesterday, -850 since mn.', '+325 yesterday, -850 since mn.', 'tolerating by mouth meds with sips.', 'continue to support patient. and family.']</t>
-        </is>
-      </c>
-      <c r="Q11" t="n">
-        <v>0.002954564999527065</v>
-      </c>
-      <c r="R11" t="inlineStr">
+          <t>[[['e1', 'before', 'e2'], ['e2', 'simultaneous', 'e3'], ['e3', 'before', 'e4'], ['e4', 'after', 'e5'], ['e5', 'before', 'e6'], ['e6', 'before', 'e7']]]</t>
+        </is>
+      </c>
+      <c r="P11" t="n">
+        <v>0.00233298199964338</v>
+      </c>
+      <c r="Q11" t="inlineStr">
         <is>
           <t>Sleep</t>
         </is>
       </c>
-      <c r="S11" t="b">
+      <c r="R11" t="b">
+        <v>0</v>
+      </c>
+      <c r="S11" t="n">
         <v>0</v>
       </c>
       <c r="T11" t="n">
         <v>0</v>
       </c>
-      <c r="U11" t="n">
-        <v>0</v>
-      </c>
-      <c r="V11" t="inlineStr">
+      <c r="U11" t="inlineStr">
         <is>
           <t>('pain', 'family')</t>
         </is>
       </c>
+      <c r="V11" t="n">
+        <v>16.60207003599498</v>
+      </c>
       <c r="W11" t="n">
-        <v>11.21281527400424</v>
+        <v>23.40358469600324</v>
       </c>
       <c r="X11" t="n">
-        <v>16.90746971098997</v>
+        <v>0</v>
       </c>
       <c r="Y11" t="n">
-        <v>15.73799710400635</v>
+        <v>1</v>
       </c>
       <c r="Z11" t="n">
-        <v>0</v>
-      </c>
-      <c r="AA11" t="n">
-        <v>1</v>
-      </c>
-      <c r="AB11" t="n">
-        <v>1</v>
-      </c>
-      <c r="AC11" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="12">
-      <c r="A12" t="n">
-        <v>1310489</v>
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>1310489</t>
+        </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>['Eating', 'Unknown', 'Sleep', 'Excretion', 'Family']</t>
+          <t>('Eating', 'Unknown', 'Excretion', 'Family', 'Sleep')</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>['urine', 'son', 'eat', 'family', 'sleep']</t>
+          <t>('eat', 'sleep', 'son', 'family', 'urine')</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
@@ -1969,120 +1868,111 @@
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>{'text': 'ccu progress note:\n\ns: "my son doesn\'t help at all at home, all he does is eat and sleep"\n\no:  please see flow sheet for objective data\n\ncv: tele: sinus brady w/no ectopy. heart rate 50-57, abp 103-148/50-68. milrinone and labetelol drips dc\'d. started on by mouth labetelol diastolic blood pressure 140\'s given hydralazine 10 mg by mouth given with little effect. diastolic blood pressure goal to 120. hct 39.6- k 3.8, 40 meq kcl given. repeat k 4.3. mg 2.\n\nresp: o2 5l nc. ls diminished at the bases. no labored breathing, zero retractions, sp02 92-97%.\n\ngi/gu: abd soft, non-distended, bs present x4. bm x1 mod brown formed stool. by mouth intake fair. gu: foley draining clear, yellow urine. lasix 80 mg iv given with good effect. negative 1900cc\'s since twelve a.male. bun 38, crea 2.1.\n\nneuro: patient a&amp;o x 3, moving all extremities, follows commands, restless at times. verbalized overwhelming responsibilities at home, social worker consulted.\n\niv access: picc line placed right upper arm (single lumen).\n\na) successfully weaned off of labetalol and milrinone drips. patient tolerated by mouth labetalol and hydralazine well. ? cath tomorrow.\n\np) monitor vital signs, lung sounds, i &amp; o, labs. keep diastolic blood pressure therapeutic range w/in 110-120. continute to monitor urinary output with follow-up labs. offer emotional support and update family on plan of care.\n\n                                                      [**first name8 (namepattern2) 1309**] [**last name (namepattern1) 9102**], sn\n\n\n', 'event': ['Family', 'Eating', 'Sleep'], 'phrase': '', 'raw_output': '{\n  "events": [\n    {\n      "event_type": "Family",\n      "text_quote": "my son doesn\'t help at all at home, all he does is eat and sleep",\n      "attributes": {"interaction": "Unknown", \n                     "relation": "son",\n                     "time":"Unknown",\n                     "caused_by":"Unknown"}\n    },\n    {\n      "event_type": "Eating",\n      "text_quote": "all he does is eat and sleep",\n      "attributes": {"food": "Unknown", \n                     "amount": "Unknown",\n                     "method": "Unknown",\n                     "time":"Unknown",\n                     "caused_by":"Unknown"}\n    },\n    {\n      "event_type": "Sleep",\n      "text_quote": "all he does is eat and sleep",\n      "attributes": {"quality": "Unknown", \n                     "duration": "Unknown", \n                     "time":"Unknown",\n                     "caused_by":"Unknown"}\n    }\n  ]\n}', 'attributes': [{'Family': {'interaction': 'Unknown', 'relation': 'son', 'time': 'Unknown', 'caused_by': 'Unknown'}}, {'Eating': {'food': 'Unknown', 'amount': 'Unknown', 'method': 'Unknown', 'time': 'Unknown', 'caused_by': 'Unknown'}}, {'Sleep': {'quality': 'Unknown', 'duration': 'Unknown', 'time': 'Unknown', 'caused_by': 'Unknown'}}], 'text_quotes': ["my son doesn't help at all at home, all he does is eat and sleep", 'all he does is eat and sleep', 'all he does is eat and sleep'], 'event_name_prompt': 'Given the text: ccu progress note:\n\ns: "my son doesn\'t help at all at home, all he does is eat and sleep"\n\no:  please see flow sheet for objective data\n\ncv: tele: sinus brady w/no ectopy. heart rate 50-57, abp 103-148/50-68. milrinone and labetelol drips dc\'d. started on by mouth labetelol diastolic blood pressure 140\'s given hydralazine 10 mg by mouth given with little effect. diastolic blood pressure goal to 120. hct 39.6- k 3.8, 40 meq kcl given. repeat k 4.3. mg 2.\n\nresp: o2 5l nc. ls diminished at the bases. no labored breathing, zero retractions, sp02 92-97%.\n\ngi/gu: abd soft, non-distended, bs present x4. bm x1 mod brown formed stool. by mouth intake fair. gu: foley draining clear, yellow urine. lasix 80 mg iv given with good effect. negative 1900cc\'s since twelve a.male. bun 38, crea 2.1.\n\nneuro: patient a&amp;o x 3, moving all extremities, follows commands, restless at times. verbalized overwhelming responsibilities at home, social worker consulted.\n\niv access: picc line placed right upper arm (single lumen).\n\na) successfully weaned off of labetalol and milrinone drips. patient tolerated by mouth labetalol and hydralazine well. ? cath tomorrow.\n\np) monitor vital signs, lung sounds, i &amp; o, labs. keep diastolic blood pressure therapeutic range w/in 110-120. continute to monitor urinary output with follow-up labs. offer emotional support and update family on plan of care.\n\n                                                      [**first name8 (namepattern2) 1309**] [**last name (namepattern1) 9102**], sn\n\n\n, \n                        and the following event types with their definitions: Eating : The patient takes food into their body by mouth.\nExcretion : The patient discharges waste matter from their body.\nFamily : The patient has a visit, call, or communication with a family member.\nPain : The patient reports or shows signs of pain.\nSleep : The patient sleeps or the sleep’s quality or quantity is described.\nUnknown : choose "Unknown" if none of the other event type are applicable. \n                        ---\n                        Your task:\n                        0. Identify ALL events in the text (zero, one, or more).\n1. For each event, assign an event_type from the list above.\n2. If multiple event of same type is mentioned, assign the event_type multiple times\n3. Extract attributes for each event using ONLY the allowed attributes listed below.\n4. Use keyword evidence (Ki) ONLY if it is consistent with the text context.\n5. Output strictly valid JSON following the schema below.\n                        ---\n                        Classification Rules:\n                        - A text may contain multiple events of the same or different types.\n- Create a separate event object for each event mention.\n- If the text is explicitly a NEGATION (e.g., "denies pain"), do not extract that event.\n- If the text describes a FUTURE or HYPOTHETICAL event (e.g., "will eat tomorrow"), ignore it.\n- A valid event should have occurred in the recent past or is occurring during the time of writing of the text.\n- If no events are found or if unsure, return {"events": []}\n                        \n                        ---\n                                    Attributes allowed:\n                                    {\'Eating\': {\'food\': \'&lt;string&gt; # e.g., pancakes, porridge, etc.\', \'amount\': \'&lt;string&gt; # e.g., 1, 2 bowls, etc.\', \'method\': \'&lt;string&gt;  # e.g., oral, tube, etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, after shower, etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}, \'Excretion\': {\'type\': \'&lt;string&gt; # e.g., urine, stool, etc.\', \'frequency\': \'&lt;string&gt; # e.g., 2x, once, etc.\', \'quality\': \'&lt;string&gt; # e.g., loose, hard, etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, after shower, etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}, \'Family\': {\'interaction\': \'&lt;string&gt; # e.g., visit, call, communication, etc.\', \'relation\': \'&lt;string&gt; # e.g., mother, son, etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, after shower, etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}, \'Pain\': {\'severity\': \'&lt;string&gt; # e.g., mild, moderate, severe, numeric scale if present, etc.\', \'location\': \'&lt;string&gt; # e.g., right knee, head, etc.\', \'duration\': \'&lt;string&gt; # e.g., all night, 3 hours, etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, after shower, etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}, \'Sleep\': {\'quality\': \'&lt;string&gt; # e.g., good, poor, restless, etc.\', \'duration\': \'&lt;string&gt; # e.g., 6 hours, phrases like "all night", etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, after shower, etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}}\n                                    If no relevant attribute exists for an event, return an empty object {}.\n                                    \n                        \n                        ---\n                                    Keyword evidence (Ki):\n                                    Additional facts: A keyword matching algorithm without context detected keyword(s) [\'urine\', \'son\', \'eat\', \'family\', \'sleep\'].\n                                    Use this only as a pointer. If context contradicts, ignore.\n                        ---\n                        Output Schema (strict):\n                        {\n                                    "events": [\n                                        {\n                                        "event_type": "&lt;Pain | Sleep | Excretion | Eating | Family&gt;",\n                                        "text_quote": "&lt;fragement from the text indicating &gt;",\n                "attributes": {\n                    "&lt;attribute_name&gt;": "&lt;attribute_value&gt;"\n                }\n                                        }\n                                    ]\n                                    }\n                        \n                            Rules:\n                                - Ensure the output is valid JSON (parseable).\n                                - "eventS" must always be an array (can be empty).\n                                - Multiple instances of the same event type appear as individual elements in the event array.\n                                - Events appear in the array in the same order in which they appear in the text.\n                                - Do not include extra keys, comments, or text.\n                                - Each object in "events" must contain "event_type", "text_quote", and "attributes".\n                                -If an event attribute type has no value mentioned, return "attributes": {"&lt; attribute name &gt;:Unknown"} for each attribute type defined for the event type \n                        \n                        \n                        \n                ---\n                Examples:\n                \n                text: "Patient ate breakfast this morning. He seems less anxious."\n                output: {\n                "events": [\n                    {\n                    "event_type": "Eating",\n                    "text_quote":"Patient ate breakfast this morning",\n                    "attributes": {"food": "breakfast", \n                                   "amount": "Unknown",\n                                   "method": "Unknown",\n                                   "time":"morning",\n                                   "caused_by":"Unknown"}\n                    }\n                ]\n                }\n                \n                text: "Patient reported severe abdominal pain."\n                output: {\n                "events": [\n                    {\n                    "event_type": "Pain",\n                    "text_quote": "severe abdominal Pain",\n                    "attributes": {"severity": "severe", \n                                   "location": "abdominal",\n                                   "duration": "Unknown",\n                                   "time":"Unknown",\n                                   "caused_by":"Unknown"}\n                    }\n                ]\n                }\n                \n                text: "Patient called his son around 3 pm."\n                output: {\n                "events": [\n                    {\n                    "event_type": "Family",\n                    "text_quote": "called his son around 3 pm",\n                    "attributes": {"interaction": "call", \n                                    "relation": "son",\n                                    "time":"3 pm",\n                                    "caused_by":"Unknown"}\n                    }\n                ]\n                }\n                \n                text: "Patient had a loose stool overnight."\n                output: {\n                "events": [\n                    {\n                    "event_type": "Excretion",\n                    "text_quote": "loose stool overnight",\n                    "attributes": {"type": "stool", \n                                   "quality": "loose", \n                                   "frequency":"overnight", \n                                   "time":"night",\n                                   "caused_by":"Unknown"}\n                    }\n                ]\n                }\n                \n                text: "Patient was able to sleep well last night."\n                output: {\n                "events": [\n                    {\n                    "event_type": "Sleep",\n                    "text_quote": "sleep well last night",\n                    "attributes": {"quality": "well",\n                                    "duration": "Unknown", \n                                    "time":"night",\n                                    "caused_by":"Unknown"}\n                    }\n                ]\n                }\n                \n                text: "The patient couldn\'t sleep due to severe pain."\n                output: {\n                "events": [\n                    {\n                    "event_type": "Sleep",\n                    "text_quote": "couldn\'t sleep",\n                    "attributes": {"quality": "poor", \n                                    "duration": "Unknown",\n                                   "time":"Unknown",\n                                   "caused_by":"Pain"}\n                    },\n                    {\n                    "event_type": "Pain",\n                    "text_quote": "severe pain",\n                    "attributes": {"severity": "severe", \n                                    "location": "Unknown", \n                                    "duration": "Unknown", \n                                   "time":"before Sleep",\n                                   "caused_by":"Unknown"}\n                    }\n                ]\n                }\n                \n                text: "The patient complained of severe back pain, was given Tylenol, but the pain persisted and he was then prescribed stronger morphine."\n                output: {\n                "events": [\n                    {\n                    "event_type": "Pain",\n                    "text_quote": "complained of severe back pain",\n                    "attributes": {"severity": "severe", \n                                    "location": "back",\n                                    "duration": "Unknown", \n                                    "time":"Unknown",\n                                    "caused_by":"Unknown"}\n                    },\n                    {\n                    "event_type": "Pain",\n                    "text_quote": "pain persisted",\n                    "attributes": {"severity": "severe", \n                                   "location": "back",\n                                   "duration": "persistent", \n                                   "time":"after Tylenol",\n                                   "caused_by":"Unknown"}\n                    }\n                ]\n                }\n                \n                        ', 'event_detection_time': 8.453074363991618}</t>
+          <t>['eat', 'sleep', 'son', 'family', 'urine']</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>['Family', 'Eating', 'Sleep']</t>
+          <t>{'text': 'ccu progress note:\n\ns: "my son doesn\'t help at all at home, all he does is eat and sleep"\n\no:  please see flow sheet for objective data\n\ncv: tele: sinus brady w/no ectopy. heart rate 50-57, abp 103-148/50-68. milrinone and labetelol drips dc\'d. started on by mouth labetelol diastolic blood pressure 140\'s given hydralazine 10 mg by mouth given with little effect. diastolic blood pressure goal to 120. hct 39.6- k 3.8, 40 meq kcl given. repeat k 4.3. mg 2.\n\nresp: o2 5l nc. ls diminished at the bases. no labored breathing, zero retractions, sp02 92-97%.\n\ngi/gu: abd soft, non-distended, bs present x4. bm x1 mod brown formed stool. by mouth intake fair. gu: foley draining clear, yellow urine. lasix 80 mg iv given with good effect. negative 1900cc\'s since twelve a.male. bun 38, crea 2.1.\n\nneuro: patient a&amp;o x 3, moving all extremities, follows commands, restless at times. verbalized overwhelming responsibilities at home, social worker consulted.\n\niv access: picc line placed right upper arm (single lumen).\n\na) successfully weaned off of labetalol and milrinone drips. patient tolerated by mouth labetalol and hydralazine well. ? cath tomorrow.\n\np) monitor vital signs, lung sounds, i &amp; o, labs. keep diastolic blood pressure therapeutic range w/in 110-120. continute to monitor urinary output with follow-up labs. offer emotional support and update family on plan of care.\n\n                                                      [**first name8 (namepattern2) 1309**] [**last name (namepattern1) 9102**], sn\n\n\n', 'event': ['Eating', 'Sleep', 'Family', 'Excretion', 'Excretion', 'Family'], 'event_id': ['e1', 'e2', 'e3', 'e4', 'e5', 'e6'], 'phrase': '', 'raw_output': '{\n  "events": [\n    {\n      "event_id": "e1",\n      "event_type": "Eating",\n      "text_quote": "all he does is eat and sleep",\n      "attributes": {\n        "food": "Unknown",\n        "amount": "Unknown",\n        "method": "Unknown",\n        "negation": "false",\n        "time": "Unknown",\n        "caused_by": "Unknown"\n      }\n    },\n    {\n      "event_id": "e2",\n      "event_type": "Sleep",\n      "text_quote": "all he does is eat and sleep",\n      "attributes": {\n        "quality": "Unknown",\n        "duration": "Unknown",\n        "negation": "false",\n        "time": "Unknown",\n        "caused_by": "Unknown"\n      }\n    },\n    {\n      "event_id": "e3",\n      "event_type": "Family",\n      "text_quote": "my son doesn\'t help at all at home",\n      "attributes": {\n        "interaction": "visit",\n        "relation": "son",\n        "negation": "false",\n        "time": "Unknown",\n        "caused_by": "Unknown"\n      }\n    },\n    {\n      "event_id": "e4",\n      "event_type": "Excretion",\n      "text_quote": "bm x1 mod brown formed stool",\n      "attributes": {\n        "type": "stool",\n        "frequency": "x1",\n        "quality": "mod brown formed",\n        "negation": "false",\n        "time": "Unknown",\n        "caused_by": "Unknown"\n      }\n    },\n    {\n      "event_id": "e5",\n      "event_type": "Excretion",\n      "text_quote": "foley draining clear, yellow urine",\n      "attributes": {\n        "type": "urine",\n        "frequency": "Unknown",\n        "quality": "clear, yellow",\n        "negation": "false",\n        "time": "Unknown",\n        "caused_by": "Unknown"\n      }\n    },\n    {\n      "event_id": "e6",\n      "event_type": "Family",\n      "text_quote": "verbalized overwhelming responsibilities at home, social worker consulted",\n      "attributes": {\n        "interaction": "consultation",\n        "relation": "social worker",\n        "negation": "false",\n        "time": "Unknown",\n        "caused_by": "Unknown"\n      }\n    }\n  ],\n  "order": []\n}', 'attributes': [{'Eating': {'food': 'Unknown', 'amount': 'Unknown', 'method': 'Unknown', 'negation': 'false', 'time': 'Unknown', 'caused_by': 'Unknown'}}, {'Sleep': {'quality': 'Unknown', 'duration': 'Unknown', 'negation': 'false', 'time': 'Unknown', 'caused_by': 'Unknown'}}, {'Family': {'interaction': 'visit', 'relation': 'son', 'negation': 'false', 'time': 'Unknown', 'caused_by': 'Unknown'}}, {'Excretion': {'type': 'stool', 'frequency': 'x1', 'quality': 'mod brown formed', 'negation': 'false', 'time': 'Unknown', 'caused_by': 'Unknown'}}, {'Excretion': {'type': 'urine', 'frequency': 'Unknown', 'quality': 'clear, yellow', 'negation': 'false', 'time': 'Unknown', 'caused_by': 'Unknown'}}, {'Family': {'interaction': 'consultation', 'relation': 'social worker', 'negation': 'false', 'time': 'Unknown', 'caused_by': 'Unknown'}}], 'orders': [[]], 'text_quotes': ['all he does is eat and sleep', 'all he does is eat and sleep', "my son doesn't help at all at home", 'bm x1 mod brown formed stool', 'foley draining clear, yellow urine', 'verbalized overwhelming responsibilities at home, social worker consulted'], 'event_name_prompt': 'Given the text: ccu progress note:\n\ns: "my son doesn\'t help at all at home, all he does is eat and sleep"\n\no:  please see flow sheet for objective data\n\ncv: tele: sinus brady w/no ectopy. heart rate 50-57, abp 103-148/50-68. milrinone and labetelol drips dc\'d. started on by mouth labetelol diastolic blood pressure 140\'s given hydralazine 10 mg by mouth given with little effect. diastolic blood pressure goal to 120. hct 39.6- k 3.8, 40 meq kcl given. repeat k 4.3. mg 2.\n\nresp: o2 5l nc. ls diminished at the bases. no labored breathing, zero retractions, sp02 92-97%.\n\ngi/gu: abd soft, non-distended, bs present x4. bm x1 mod brown formed stool. by mouth intake fair. gu: foley draining clear, yellow urine. lasix 80 mg iv given with good effect. negative 1900cc\'s since twelve a.male. bun 38, crea 2.1.\n\nneuro: patient a&amp;o x 3, moving all extremities, follows commands, restless at times. verbalized overwhelming responsibilities at home, social worker consulted.\n\niv access: picc line placed right upper arm (single lumen).\n\na) successfully weaned off of labetalol and milrinone drips. patient tolerated by mouth labetalol and hydralazine well. ? cath tomorrow.\n\np) monitor vital signs, lung sounds, i &amp; o, labs. keep diastolic blood pressure therapeutic range w/in 110-120. continute to monitor urinary output with follow-up labs. offer emotional support and update family on plan of care.\n\n                                                      [**first name8 (namepattern2) 1309**] [**last name (namepattern1) 9102**], sn\n\n\n, \n                        and the following event types with their definitions: Eating : The patient takes food into their body by mouth.\nExcretion : The patient discharges waste matter from their body.\nFamily : The patient has a visit, call, or communication with a family member.\nPain : The patient reports or shows signs of pain.\nSleep : The patient sleeps or the sleep’s quality or quantity is described.\nUnknown : choose "Unknown" if none of the other event type are applicable. \n                        ---\n                        Your task:\n                        0. Identify ALL events in the text (zero, one, or more).\n1. For each event, assign an event_type from the list above.\n2. If multiple event of same type is mentioned, assign the event_type multiple times\n3. Extract attributes for each event using ONLY the allowed attributes listed below.\n4. Use keyword evidence (Ki) ONLY if it is consistent with the text context.\n5. Output strictly valid JSON following the schema below.\n                        ---\n                        Classification Rules:\n                        - A text may contain multiple events of the same or different types.\n- Create a separate event object for each event mention.\n- If the text is explicitly a NEGATION (e.g., "denies pain"), do not extract that event.\n- If the text describes a FUTURE or HYPOTHETICAL event (e.g., "will eat tomorrow"), ignore it.\n- A valid event should have occurred in the recent past or is occurring during the time of writing of the text.\n- If no events are found or if unsure, return {"events": []}\n                        \n                        ---\n                                    Attributes allowed:\n                                    {\'Eating\': {\'food\': \'&lt;string&gt; # e.g., pancakes, porridge, etc.\', \'amount\': \'&lt;string&gt; # e.g., 1, 2 bowls, etc.\', \'method\': \'&lt;string&gt;  # e.g., oral, tube, etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, evening etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}, \'Excretion\': {\'type\': \'&lt;string&gt; # e.g., urine, stool, etc.\', \'frequency\': \'&lt;string&gt; # e.g., 2x, once, etc.\', \'quality\': \'&lt;string&gt; # e.g., loose, hard, etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, evening etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}, \'Family\': {\'interaction\': \'&lt;string&gt; # e.g., visit, call, communication, etc.\', \'relation\': \'&lt;string&gt; # e.g., mother, son, etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, evening etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}, \'Pain\': {\'severity\': \'&lt;string&gt; # e.g., mild, moderate, severe, numeric scale if present, etc.\', \'location\': \'&lt;string&gt; # e.g., right knee, head, etc.\', \'duration\': \'&lt;string&gt; # e.g., all night, 3 hours, etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, evening etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}, \'Sleep\': {\'quality\': \'&lt;string&gt; # e.g., good, poor, restless, etc.\', \'duration\': \'&lt;string&gt; # e.g., 6 hours, phrases like "all night", etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, evening etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}}\n                                    If no relevant attribute exists for an event, return an empty object {}.\n                                    \n                        \n                        ---\n                                    Keyword evidence (Ki):\n                                    Additional facts: A keyword matching algorithm without context detected keyword(s) (\'eat\', \'sleep\', \'son\', \'family\', \'urine\').\n                                    Use this only as a pointer. If context contradicts, ignore.\n                        ---\n                        Output Schema (strict):\n                        {\n                                    "events": [\n                                        {\n                                        "event_id": "&lt; A unique id eg.: e1 | e2 |...&gt;"\n                                        "event_type": "&lt;Pain | Sleep | Excretion | Eating | Family&gt;",\n                                        "text_quote": "&lt;fragement from the text indicating the event_type&gt;",\n                "attributes": {\n                    "&lt;attribute_name&gt;": "&lt;attribute_value&gt;"\n                }\n                                        }\n                                    ],\n                                    "order": [\n                                        ["e1", "before" | "after" | "simultaneous", "e2" ]\n                                    ]\n                                    }\n                        \n                            Rules:\n                                - Ensure the output is valid JSON (parseable).\n                                - "eventS" must always be an array (can be empty).\n                                - Multiple instances of the same event type appear with different ids.\n                                - Events appear in the array in the same order in which they appear in the text.\n                                - Their partial orders can be expressed using the "order" section.\n                                - Do not include extra keys, comments, or text.\n                                - Each object in "events" must contain "event_type", "text_quote", and "attributes".\n                                - If an event attribute type has no value mentioned, return "attributes": {"&lt; attribute name &gt;:Unknown"} for each attribute type defined for the event type \n                        \n                        \n                        \n                ---\n                Examples:\n                \n                text: "Patient ate breakfast this morning. He seems less anxious."\n                output: {\n                "events": [\n                    {"event_id": "e1",\n                    "event_type": "Eating",\n                    "text_quote":"Patient ate breakfast this morning",\n                    "attributes": {"food": "breakfast", \n                                   "amount": "Unknown",\n                                   "method": "Unknown",\n                                   "negation": "false",\n                                   "time":"morning",\n                                   "caused_by":"Unknown"}\n                    }\n                ],\n                "order":[]\n                }\n                \n                text: "Patient reported severe abdominal pain."\n                output: {\n                "events": [\n                    {"event_id": "e1",\n                    "event_type": "Pain",\n                    "text_quote": "severe abdominal Pain",\n                    "attributes": {"severity": "severe", \n                                   "location": "abdominal",\n                                   "duration": "Unknown",\n                                   "negation": "false",\n                                   "time":"Unknown",\n                                   "caused_by":"Unknown"}\n                    }\n                ],\n                "order":[]\n                }\n                \n                text: "Patient called his son around 3 pm."\n                output: {\n                "events": [\n                    {"event_id": "e1",\n                    "event_type": "Family",\n                    "text_quote": "called his son around 3 pm",\n                    "attributes": {"interaction": "call", \n                                    "relation": "son",\n                                    "negation": "false",\n                                    "time":"3 pm",\n                                    "caused_by":"Unknown"}\n                    }\n                ],\n                "order":[]\n                }\n                \n                text: "Patient had a loose stool overnight."\n                output: {\n                "events": [\n                    {"event_id": "e1",\n                    "event_type": "Excretion",\n                    "text_quote": "loose stool overnight",\n                    "attributes": {"type": "stool", \n                                   "quality": "loose", \n                                   "frequency":"overnight", \n                                   "negation": "false",\n                                   "time":"night",\n                                   "caused_by":"Unknown"}\n                    }\n                ],\n                "order":[]\n                }\n                \n                text: "Patient was able to sleep well last night."\n                output: {\n                "events": [\n                    {"event_id": "e1",\n                    "event_type": "Sleep",\n                    "text_quote": "sleep well last night",\n                    "attributes": {"quality": "well",\n                                    "duration": "Unknown", \n                                    "negation": "false",\n                                    "time":"night",\n                                    "caused_by":"Unknown"}\n                    }\n                ],\n                "order":[]\n                }\n                \n                text: "The patient couldn\'t sleep due to severe pain."\n                output: {\n                "events": [\n                    {"event_id": "e1",\n                    "event_type": "Sleep",\n                    "text_quote": "couldn\'t sleep",\n                    "attributes": {"quality": "poor", \n                                    "duration": "Unknown",\n                                    "negation": "true",\n                                    "time":"Unknown",\n                                    "caused_by":"Pain"}\n                    },\n                    {"event_id": "e2",\n                    "event_type": "Pain",\n                    "text_quote": "severe pain",\n                    "attributes": {"severity": "severe", \n                                    "location": "Unknown", \n                                    "duration": "Unknown", \n                                    "time":"Unknown",\n                                    "caused_by":"Unknown"}\n                    }\n                ],\n                "order":["e1", "after", "e2"]\n                }\n                \n                text: "The patient complained of severe back pain, was given Tylenol, but the pain persisted and he was then prescribed stronger morphine."\n                output: {\n                "events": [\n                    {"event_id": "e1",\n                    "event_type": "Pain",\n                    "text_quote": "complained of severe back pain",\n                    "attributes": {"severity": "severe", \n                                    "location": "back",\n                                    "duration": "Unknown", \n                                    "time":"Unknown",\n                                    "caused_by":"Unknown"}\n                    },\n                    {"event_id": "e2",\n                    "event_type": "Pain",\n                    "text_quote": "pain persisted",\n                    "attributes": {"severity": "severe", \n                                   "location": "back",\n                                   "duration": "persistent", \n                                   "time":"after Tylenol",\n                                   "caused_by":"Unknown"}\n                    }\n                ],\n                "order":[["e1", "before", "e2"]]\n                }\n                \n                        ', 'event_detection_time': 18.577292246976867}</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>[{'Family': {'interaction': 'Unknown', 'relation': 'son', 'time': 'Unknown', 'caused_by': 'Unknown'}}, {'Eating': {'food': 'Unknown', 'amount': 'Unknown', 'method': 'Unknown', 'time': 'Unknown', 'caused_by': 'Unknown'}}, {'Sleep': {'quality': 'Unknown', 'duration': 'Unknown', 'time': 'Unknown', 'caused_by': 'Unknown'}}]</t>
+          <t>['Eating', 'Sleep', 'Family', 'Excretion', 'Excretion', 'Family']</t>
         </is>
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>["my son doesn't help at all at home, all he does is eat and sleep", 'all he does is eat and sleep', 'all he does is eat and sleep']</t>
+          <t>[{'Eating': {'food': 'Unknown', 'amount': 'Unknown', 'method': 'Unknown', 'negation': 'false', 'time': 'Unknown', 'caused_by': 'Unknown'}}, {'Sleep': {'quality': 'Unknown', 'duration': 'Unknown', 'negation': 'false', 'time': 'Unknown', 'caused_by': 'Unknown'}}, {'Family': {'interaction': 'visit', 'relation': 'son', 'negation': 'false', 'time': 'Unknown', 'caused_by': 'Unknown'}}, {'Excretion': {'type': 'stool', 'frequency': 'x1', 'quality': 'mod brown formed', 'negation': 'false', 'time': 'Unknown', 'caused_by': 'Unknown'}}, {'Excretion': {'type': 'urine', 'frequency': 'Unknown', 'quality': 'clear, yellow', 'negation': 'false', 'time': 'Unknown', 'caused_by': 'Unknown'}}, {'Family': {'interaction': 'consultation', 'relation': 'social worker', 'negation': 'false', 'time': 'Unknown', 'caused_by': 'Unknown'}}]</t>
         </is>
       </c>
       <c r="I12" t="inlineStr">
         <is>
-          <t>{'text': 'ccu progress note:\n\ns: "my son doesn\'t help at all at home, all he does is eat and sleep"\n\no:  please see flow sheet for objective data\n\ncv: tele: sinus brady w/no ectopy. heart rate 50-57, abp 103-148/50-68. milrinone and labetelol drips dc\'d. started on by mouth labetelol diastolic blood pressure 140\'s given hydralazine 10 mg by mouth given with little effect. diastolic blood pressure goal to 120. hct 39.6- k 3.8, 40 meq kcl given. repeat k 4.3. mg 2.\n\nresp: o2 5l nc. ls diminished at the bases. no labored breathing, zero retractions, sp02 92-97%.\n\ngi/gu: abd soft, non-distended, bs present x4. bm x1 mod brown formed stool. by mouth intake fair. gu: foley draining clear, yellow urine. lasix 80 mg iv given with good effect. negative 1900cc\'s since twelve a.male. bun 38, crea 2.1.\n\nneuro: patient a&amp;o x 3, moving all extremities, follows commands, restless at times. verbalized overwhelming responsibilities at home, social worker consulted.\n\niv access: picc line placed right upper arm (single lumen).\n\na) successfully weaned off of labetalol and milrinone drips. patient tolerated by mouth labetalol and hydralazine well. ? cath tomorrow.\n\np) monitor vital signs, lung sounds, i &amp; o, labs. keep diastolic blood pressure therapeutic range w/in 110-120. continute to monitor urinary output with follow-up labs. offer emotional support and update family on plan of care.\n\n                                                      [**first name8 (namepattern2) 1309**] [**last name (namepattern1) 9102**], sn\n\n\n', 'event': ['Eating', 'Sleep', 'Family', 'Excretion', 'Excretion', 'Excretion'], 'phrase': '', 'raw_output': '{\n  "events": [\n    {\n      "event_type": "Eating",\n      "text_quote": "all he does is eat and sleep",\n      "attributes": {\n        "food": "Unknown",\n        "amount": "Unknown",\n        "method": "Unknown",\n        "negation": false,\n        "time": "Unknown",\n        "caused_by": "Unknown"\n      }\n    },\n    {\n      "event_type": "Sleep",\n      "text_quote": "all he does is eat and sleep",\n      "attributes": {\n        "quality": "Unknown",\n        "duration": "Unknown",\n        "negation": false,\n        "time": "Unknown",\n        "caused_by": "Unknown"\n      }\n    },\n    {\n      "event_type": "Family",\n      "text_quote": "my son doesn\'t help at all at home",\n      "attributes": {\n        "interaction": "Unknown",\n        "relation": "son",\n        "negation": false,\n        "time": "Unknown",\n        "caused_by": "Unknown"\n      }\n    },\n    {\n      "event_type": "Excretion",\n      "text_quote": "bm x1 mod brown formed stool.",\n      "attributes": {\n        "type": "stool",\n        "frequency": "once",\n        "quality": "mod brown formed",\n        "negation": false,\n        "time": "Unknown",\n        "caused_by": "Unknown"\n      }\n    },\n    {\n      "event_type": "Excretion",\n      "text_quote": "Foley draining clear, yellow urine.",\n      "attributes": {\n        "type": "urine",\n        "frequency": "Unknown",\n        "quality": "clear, yellow",\n        "negation": false,\n        "time": "Unknown",\n        "caused_by": "Unknown"\n      }\n    },\n    {\n      "event_type": "Excretion",\n      "text_quote": "negative 1900cc\'s since twelve a.m.",\n      "attributes": {\n        "type": "urine",\n        "frequency": "Unknown",\n        "quality": "Unknown",\n        "negation": false,\n        "time": "since twelve a.m.",\n        "caused_by": "Unknown"\n      }\n    }\n  ]\n}', 'attributes': [{'Eating': {'food': 'Unknown', 'amount': 'Unknown', 'method': 'Unknown', 'negation': False, 'time': 'Unknown', 'caused_by': 'Unknown'}}, {'Sleep': {'quality': 'Unknown', 'duration': 'Unknown', 'negation': False, 'time': 'Unknown', 'caused_by': 'Unknown'}}, {'Family': {'interaction': 'Unknown', 'relation': 'son', 'negation': False, 'time': 'Unknown', 'caused_by': 'Unknown'}}, {'Excretion': {'type': 'stool', 'frequency': 'once', 'quality': 'mod brown formed', 'negation': False, 'time': 'Unknown', 'caused_by': 'Unknown'}}, {'Excretion': {'type': 'urine', 'frequency': 'Unknown', 'quality': 'clear, yellow', 'negation': False, 'time': 'Unknown', 'caused_by': 'Unknown'}}, {'Excretion': {'type': 'urine', 'frequency': 'Unknown', 'quality': 'Unknown', 'negation': False, 'time': 'since twelve a.m.', 'caused_by': 'Unknown'}}], 'text_quotes': ['all he does is eat and sleep', 'all he does is eat and sleep', "my son doesn't help at all at home", 'bm x1 mod brown formed stool.', 'Foley draining clear, yellow urine.', "negative 1900cc's since twelve a.m."], 'event_name_prompt': 'Given the text: ccu progress note:\n\ns: "my son doesn\'t help at all at home, all he does is eat and sleep"\n\no:  please see flow sheet for objective data\n\ncv: tele: sinus brady w/no ectopy. heart rate 50-57, abp 103-148/50-68. milrinone and labetelol drips dc\'d. started on by mouth labetelol diastolic blood pressure 140\'s given hydralazine 10 mg by mouth given with little effect. diastolic blood pressure goal to 120. hct 39.6- k 3.8, 40 meq kcl given. repeat k 4.3. mg 2.\n\nresp: o2 5l nc. ls diminished at the bases. no labored breathing, zero retractions, sp02 92-97%.\n\ngi/gu: abd soft, non-distended, bs present x4. bm x1 mod brown formed stool. by mouth intake fair. gu: foley draining clear, yellow urine. lasix 80 mg iv given with good effect. negative 1900cc\'s since twelve a.male. bun 38, crea 2.1.\n\nneuro: patient a&amp;o x 3, moving all extremities, follows commands, restless at times. verbalized overwhelming responsibilities at home, social worker consulted.\n\niv access: picc line placed right upper arm (single lumen).\n\na) successfully weaned off of labetalol and milrinone drips. patient tolerated by mouth labetalol and hydralazine well. ? cath tomorrow.\n\np) monitor vital signs, lung sounds, i &amp; o, labs. keep diastolic blood pressure therapeutic range w/in 110-120. continute to monitor urinary output with follow-up labs. offer emotional support and update family on plan of care.\n\n                                                      [**first name8 (namepattern2) 1309**] [**last name (namepattern1) 9102**], sn\n\n\n, \n                        and the following event types with their definitions: Eating : The patient takes food into their body by mouth.\nExcretion : The patient discharges waste matter from their body.\nFamily : The patient has a visit, call, or communication with a family member.\nPain : The patient reports or shows signs of pain.\nSleep : The patient sleeps or the sleep’s quality or quantity is described.\nUnknown : choose "Unknown" if none of the other event type are applicable. \n                        ---\n                        Your task:\n                        0. Identify ALL events in the text (zero, one, or more).\n1. For each event, assign an event_type from the list above.\n2. If multiple event of same type is mentioned, assign the event_type multiple times\n3. Extract attributes for each event using ONLY the allowed attributes listed below.\n4. Use keyword evidence (Ki) ONLY if it is consistent with the text context.\n5. Output strictly valid JSON following the schema below.\n                        ---\n                        Classification Rules:\n                        - A text may contain multiple events of the same or different types.\n- Create a separate event object for each event mention.\n- If the text is explicitly a NEGATION (e.g., "denies pain"), do not extract that event.\n- If the text describes a FUTURE or HYPOTHETICAL event (e.g., "will eat tomorrow"), ignore it.\n- A valid event should have occurred in the recent past or is occurring during the time of writing of the text.\n- If no events are found or if unsure, return {"events": []}\n                        \n                        ---\n                                    Attributes allowed:\n                                    {\'Eating\': {\'food\': \'&lt;string&gt; # e.g., pancakes, porridge, etc.\', \'amount\': \'&lt;string&gt; # e.g., 1, 2 bowls, etc.\', \'method\': \'&lt;string&gt;  # e.g., oral, tube, etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, after shower, etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}, \'Excretion\': {\'type\': \'&lt;string&gt; # e.g., urine, stool, etc.\', \'frequency\': \'&lt;string&gt; # e.g., 2x, once, etc.\', \'quality\': \'&lt;string&gt; # e.g., loose, hard, etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, after shower, etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}, \'Family\': {\'interaction\': \'&lt;string&gt; # e.g., visit, call, communication, etc.\', \'relation\': \'&lt;string&gt; # e.g., mother, son, etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, after shower, etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}, \'Pain\': {\'severity\': \'&lt;string&gt; # e.g., mild, moderate, severe, numeric scale if present, etc.\', \'location\': \'&lt;string&gt; # e.g., right knee, head, etc.\', \'duration\': \'&lt;string&gt; # e.g., all night, 3 hours, etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, after shower, etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}, \'Sleep\': {\'quality\': \'&lt;string&gt; # e.g., good, poor, restless, etc.\', \'duration\': \'&lt;string&gt; # e.g., 6 hours, phrases like "all night", etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, after shower, etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}}\n                                    If no relevant attribute exists for an event, return an empty object {}.\n                                    \n                        \n                        ---\n                                    Keyword evidence (Ki):\n                                    Additional facts: A keyword matching algorithm without context detected keyword(s) [\'urine\', \'son\', \'eat\', \'family\', \'sleep\'].\n                                    Use this only as a pointer. If context contradicts, ignore.\n                        ---\n                        Output Schema (strict):\n                        {\n                                    "events": [\n                                        {\n                                        "event_type": "&lt;Pain | Sleep | Excretion | Eating | Family&gt;",\n                                        "text_quote": "&lt;fragement from the text indicating &gt;",\n                "attributes": {\n                    "&lt;attribute_name&gt;": "&lt;attribute_value&gt;"\n                }\n                                        }\n                                    ]\n                                    }\n                        \n                            Rules:\n                                - Ensure the output is valid JSON (parseable).\n                                - "eventS" must always be an array (can be empty).\n                                - Multiple instances of the same event type appear as individual elements in the event array.\n                                - Events appear in the array in the same order in which they appear in the text.\n                                - Do not include extra keys, comments, or text.\n                                - Each object in "events" must contain "event_type", "text_quote", and "attributes".\n                                -If an event attribute type has no value mentioned, return "attributes": {"&lt; attribute name &gt;:Unknown"} for each attribute type defined for the event type \n                        \n                        \n                        \n                        ', 'event_detection_time': 15.665367870999034}</t>
+          <t>['all he does is eat and sleep', 'all he does is eat and sleep', "my son doesn't help at all at home", 'bm x1 mod brown formed stool', 'foley draining clear, yellow urine', 'verbalized overwhelming responsibilities at home, social worker consulted']</t>
         </is>
       </c>
       <c r="J12" t="inlineStr">
         <is>
-          <t>['Eating', 'Sleep', 'Family', 'Excretion', 'Excretion', 'Excretion']</t>
+          <t>[[]]</t>
         </is>
       </c>
       <c r="K12" t="inlineStr">
         <is>
-          <t>[{'Eating': {'food': 'Unknown', 'amount': 'Unknown', 'method': 'Unknown', 'negation': False, 'time': 'Unknown', 'caused_by': 'Unknown'}}, {'Sleep': {'quality': 'Unknown', 'duration': 'Unknown', 'negation': False, 'time': 'Unknown', 'caused_by': 'Unknown'}}, {'Family': {'interaction': 'Unknown', 'relation': 'son', 'negation': False, 'time': 'Unknown', 'caused_by': 'Unknown'}}, {'Excretion': {'type': 'stool', 'frequency': 'once', 'quality': 'mod brown formed', 'negation': False, 'time': 'Unknown', 'caused_by': 'Unknown'}}, {'Excretion': {'type': 'urine', 'frequency': 'Unknown', 'quality': 'clear, yellow', 'negation': False, 'time': 'Unknown', 'caused_by': 'Unknown'}}, {'Excretion': {'type': 'urine', 'frequency': 'Unknown', 'quality': 'Unknown', 'negation': False, 'time': 'since twelve a.m.', 'caused_by': 'Unknown'}}]</t>
+          <t>{'text': 'ccu progress note:\n\ns: "my son doesn\'t help at all at home, all he does is eat and sleep"\n\no:  please see flow sheet for objective data\n\ncv: tele: sinus brady w/no ectopy. heart rate 50-57, abp 103-148/50-68. milrinone and labetelol drips dc\'d. started on by mouth labetelol diastolic blood pressure 140\'s given hydralazine 10 mg by mouth given with little effect. diastolic blood pressure goal to 120. hct 39.6- k 3.8, 40 meq kcl given. repeat k 4.3. mg 2.\n\nresp: o2 5l nc. ls diminished at the bases. no labored breathing, zero retractions, sp02 92-97%.\n\ngi/gu: abd soft, non-distended, bs present x4. bm x1 mod brown formed stool. by mouth intake fair. gu: foley draining clear, yellow urine. lasix 80 mg iv given with good effect. negative 1900cc\'s since twelve a.male. bun 38, crea 2.1.\n\nneuro: patient a&amp;o x 3, moving all extremities, follows commands, restless at times. verbalized overwhelming responsibilities at home, social worker consulted.\n\niv access: picc line placed right upper arm (single lumen).\n\na) successfully weaned off of labetalol and milrinone drips. patient tolerated by mouth labetalol and hydralazine well. ? cath tomorrow.\n\np) monitor vital signs, lung sounds, i &amp; o, labs. keep diastolic blood pressure therapeutic range w/in 110-120. continute to monitor urinary output with follow-up labs. offer emotional support and update family on plan of care.\n\n                                                      [**first name8 (namepattern2) 1309**] [**last name (namepattern1) 9102**], sn\n\n\n', 'event': ['Eating', 'Sleep', 'Family', 'Excretion', 'Excretion', 'Family'], 'event_id': ['e1', 'e2', 'e3', 'e4', 'e5', 'e6'], 'phrase': '', 'raw_output': '{\n  "events": [\n    {\n      "event_id": "e1",\n      "event_type": "Eating",\n      "text_quote": "all he does is eat and sleep",\n      "attributes": {\n        "food": "Unknown",\n        "amount": "Unknown",\n        "method": "oral",\n        "negation": false,\n        "time": "Unknown",\n        "caused_by": "Unknown"\n      }\n    },\n    {\n      "event_id": "e2",\n      "event_type": "Sleep",\n      "text_quote": "all he does is eat and sleep",\n      "attributes": {\n        "quality": "Unknown",\n        "duration": "Unknown",\n        "negation": false,\n        "time": "Unknown",\n        "caused_by": "Unknown"\n      }\n    },\n    {\n      "event_id": "e3",\n      "event_type": "Family",\n      "text_quote": "my son doesn\'t help at all at home",\n      "attributes": {\n        "interaction": "Unknown",\n        "relation": "son",\n        "negation": false,\n        "time": "Unknown",\n        "caused_by": "Unknown"\n      }\n    },\n    {\n      "event_id": "e4",\n      "event_type": "Excretion",\n      "text_quote": "bm x1 mod brown formed stool",\n      "attributes": {\n        "type": "stool",\n        "frequency": "once",\n        "quality": "moderate, brown, formed",\n        "negation": false,\n        "time": "Unknown",\n        "caused_by": "Unknown"\n      }\n    },\n    {\n      "event_id": "e5",\n      "event_type": "Excretion",\n      "text_quote": "foley draining clear, yellow urine",\n      "attributes": {\n        "type": "urine",\n        "frequency": "Unknown",\n        "quality": "clear, yellow",\n        "negation": false,\n        "time": "Unknown",\n        "caused_by": "Unknown"\n      }\n    },\n    {\n      "event_id": "e6",\n      "event_type": "Family",\n      "text_quote": "verbalized overwhelming responsibilities at home, social worker consulted",\n      "attributes": {\n        "interaction": "consultation",\n        "relation": "Unknown",\n        "negation": false,\n        "time": "Unknown",\n        "caused_by": "Unknown"\n      }\n    }\n  ],\n  "order": [\n    ["e1", "simultaneous", "e2"],\n    ["e3", "before", "e4"],\n    ["e4", "before", "e5"],\n    ["e5", "before", "e6"]\n  ]\n}', 'attributes': [{'Eating': {'food': 'Unknown', 'amount': 'Unknown', 'method': 'oral', 'negation': False, 'time': 'Unknown', 'caused_by': 'Unknown'}}, {'Sleep': {'quality': 'Unknown', 'duration': 'Unknown', 'negation': False, 'time': 'Unknown', 'caused_by': 'Unknown'}}, {'Family': {'interaction': 'Unknown', 'relation': 'son', 'negation': False, 'time': 'Unknown', 'caused_by': 'Unknown'}}, {'Excretion': {'type': 'stool', 'frequency': 'once', 'quality': 'moderate, brown, formed', 'negation': False, 'time': 'Unknown', 'caused_by': 'Unknown'}}, {'Excretion': {'type': 'urine', 'frequency': 'Unknown', 'quality': 'clear, yellow', 'negation': False, 'time': 'Unknown', 'caused_by': 'Unknown'}}, {'Family': {'interaction': 'consultation', 'relation': 'Unknown', 'negation': False, 'time': 'Unknown', 'caused_by': 'Unknown'}}], 'orders': [[['e1', 'simultaneous', 'e2'], ['e3', 'before', 'e4'], ['e4', 'before', 'e5'], ['e5', 'before', 'e6']]], 'text_quotes': ['all he does is eat and sleep', 'all he does is eat and sleep', "my son doesn't help at all at home", 'bm x1 mod brown formed stool', 'foley draining clear, yellow urine', 'verbalized overwhelming responsibilities at home, social worker consulted'], 'event_name_prompt': 'Given the text: ccu progress note:\n\ns: "my son doesn\'t help at all at home, all he does is eat and sleep"\n\no:  please see flow sheet for objective data\n\ncv: tele: sinus brady w/no ectopy. heart rate 50-57, abp 103-148/50-68. milrinone and labetelol drips dc\'d. started on by mouth labetelol diastolic blood pressure 140\'s given hydralazine 10 mg by mouth given with little effect. diastolic blood pressure goal to 120. hct 39.6- k 3.8, 40 meq kcl given. repeat k 4.3. mg 2.\n\nresp: o2 5l nc. ls diminished at the bases. no labored breathing, zero retractions, sp02 92-97%.\n\ngi/gu: abd soft, non-distended, bs present x4. bm x1 mod brown formed stool. by mouth intake fair. gu: foley draining clear, yellow urine. lasix 80 mg iv given with good effect. negative 1900cc\'s since twelve a.male. bun 38, crea 2.1.\n\nneuro: patient a&amp;o x 3, moving all extremities, follows commands, restless at times. verbalized overwhelming responsibilities at home, social worker consulted.\n\niv access: picc line placed right upper arm (single lumen).\n\na) successfully weaned off of labetalol and milrinone drips. patient tolerated by mouth labetalol and hydralazine well. ? cath tomorrow.\n\np) monitor vital signs, lung sounds, i &amp; o, labs. keep diastolic blood pressure therapeutic range w/in 110-120. continute to monitor urinary output with follow-up labs. offer emotional support and update family on plan of care.\n\n                                                      [**first name8 (namepattern2) 1309**] [**last name (namepattern1) 9102**], sn\n\n\n, \n                        and the following event types with their definitions: Eating : The patient takes food into their body by mouth.\nExcretion : The patient discharges waste matter from their body.\nFamily : The patient has a visit, call, or communication with a family member.\nPain : The patient reports or shows signs of pain.\nSleep : The patient sleeps or the sleep’s quality or quantity is described.\nUnknown : choose "Unknown" if none of the other event type are applicable. \n                        ---\n                        Your task:\n                        0. Identify ALL events in the text (zero, one, or more).\n1. For each event, assign an event_type from the list above.\n2. If multiple event of same type is mentioned, assign the event_type multiple times\n3. Extract attributes for each event using ONLY the allowed attributes listed below.\n4. Use keyword evidence (Ki) ONLY if it is consistent with the text context.\n5. Output strictly valid JSON following the schema below.\n                        ---\n                        Classification Rules:\n                        - A text may contain multiple events of the same or different types.\n- Create a separate event object for each event mention.\n- If the text is explicitly a NEGATION (e.g., "denies pain"), do not extract that event.\n- If the text describes a FUTURE or HYPOTHETICAL event (e.g., "will eat tomorrow"), ignore it.\n- A valid event should have occurred in the recent past or is occurring during the time of writing of the text.\n- If no events are found or if unsure, return {"events": []}\n                        \n                        ---\n                                    Attributes allowed:\n                                    {\'Eating\': {\'food\': \'&lt;string&gt; # e.g., pancakes, porridge, etc.\', \'amount\': \'&lt;string&gt; # e.g., 1, 2 bowls, etc.\', \'method\': \'&lt;string&gt;  # e.g., oral, tube, etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, evening etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}, \'Excretion\': {\'type\': \'&lt;string&gt; # e.g., urine, stool, etc.\', \'frequency\': \'&lt;string&gt; # e.g., 2x, once, etc.\', \'quality\': \'&lt;string&gt; # e.g., loose, hard, etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, evening etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}, \'Family\': {\'interaction\': \'&lt;string&gt; # e.g., visit, call, communication, etc.\', \'relation\': \'&lt;string&gt; # e.g., mother, son, etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, evening etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}, \'Pain\': {\'severity\': \'&lt;string&gt; # e.g., mild, moderate, severe, numeric scale if present, etc.\', \'location\': \'&lt;string&gt; # e.g., right knee, head, etc.\', \'duration\': \'&lt;string&gt; # e.g., all night, 3 hours, etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, evening etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}, \'Sleep\': {\'quality\': \'&lt;string&gt; # e.g., good, poor, restless, etc.\', \'duration\': \'&lt;string&gt; # e.g., 6 hours, phrases like "all night", etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, evening etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}}\n                                    If no relevant attribute exists for an event, return an empty object {}.\n                                    \n                        \n                        ---\n                                    Keyword evidence (Ki):\n                                    Additional facts: A keyword matching algorithm without context detected keyword(s) (\'eat\', \'sleep\', \'son\', \'family\', \'urine\').\n                                    Use this only as a pointer. If context contradicts, ignore.\n                        ---\n                        Output Schema (strict):\n                        {\n                                    "events": [\n                                        {\n                                        "event_id": "&lt; A unique id eg.: e1 | e2 |...&gt;"\n                                        "event_type": "&lt;Pain | Sleep | Excretion | Eating | Family&gt;",\n                                        "text_quote": "&lt;fragement from the text indicating the event_type&gt;",\n                "attributes": {\n                    "&lt;attribute_name&gt;": "&lt;attribute_value&gt;"\n                }\n                                        }\n                                    ],\n                                    "order": [\n                                        ["e1", "before" | "after" | "simultaneous", "e2" ]\n                                    ]\n                                    }\n                        \n                            Rules:\n                                - Ensure the output is valid JSON (parseable).\n                                - "eventS" must always be an array (can be empty).\n                                - Multiple instances of the same event type appear with different ids.\n                                - Events appear in the array in the same order in which they appear in the text.\n                                - Their partial orders can be expressed using the "order" section.\n                                - Do not include extra keys, comments, or text.\n                                - Each object in "events" must contain "event_type", "text_quote", and "attributes".\n                                - If an event attribute type has no value mentioned, return "attributes": {"&lt; attribute name &gt;:Unknown"} for each attribute type defined for the event type \n                        \n                        \n                        \n                        ', 'event_detection_time': 18.80097839399241}</t>
         </is>
       </c>
       <c r="L12" t="inlineStr">
         <is>
-          <t>['all he does is eat and sleep', 'all he does is eat and sleep', "my son doesn't help at all at home", 'bm x1 mod brown formed stool.', 'Foley draining clear, yellow urine.', "negative 1900cc's since twelve a.m."]</t>
+          <t>['Eating', 'Sleep', 'Family', 'Excretion', 'Excretion', 'Family']</t>
         </is>
       </c>
       <c r="M12" t="inlineStr">
         <is>
-          <t>{'text': 'ccu progress note:\n\ns: "my son doesn\'t help at all at home, all he does is eat and sleep"\n\no:  please see flow sheet for objective data\n\ncv: tele: sinus brady w/no ectopy. heart rate 50-57, abp 103-148/50-68. milrinone and labetelol drips dc\'d. started on by mouth labetelol diastolic blood pressure 140\'s given hydralazine 10 mg by mouth given with little effect. diastolic blood pressure goal to 120. hct 39.6- k 3.8, 40 meq kcl given. repeat k 4.3. mg 2.\n\nresp: o2 5l nc. ls diminished at the bases. no labored breathing, zero retractions, sp02 92-97%.\n\ngi/gu: abd soft, non-distended, bs present x4. bm x1 mod brown formed stool. by mouth intake fair. gu: foley draining clear, yellow urine. lasix 80 mg iv given with good effect. negative 1900cc\'s since twelve a.male. bun 38, crea 2.1.\n\nneuro: patient a&amp;o x 3, moving all extremities, follows commands, restless at times. verbalized overwhelming responsibilities at home, social worker consulted.\n\niv access: picc line placed right upper arm (single lumen).\n\na) successfully weaned off of labetalol and milrinone drips. patient tolerated by mouth labetalol and hydralazine well. ? cath tomorrow.\n\np) monitor vital signs, lung sounds, i &amp; o, labs. keep diastolic blood pressure therapeutic range w/in 110-120. continute to monitor urinary output with follow-up labs. offer emotional support and update family on plan of care.\n\n                                                      [**first name8 (namepattern2) 1309**] [**last name (namepattern1) 9102**], sn\n\n\n', 'event': ['Eating', 'Sleep', 'Excretion', 'Excretion', 'Family'], 'phrase': '', 'raw_output': '{\n  "events": [\n    {\n      "event_type": "Eating",\n      "text_quote": "all he does is eat and sleep",\n      "attributes": {"food": "Unknown", \n                     "amount": "Unknown",\n                     "method": "Unknown",\n                     "time":"Unknown",\n                     "caused_by":"Unknown"}\n    },\n    {\n      "event_type": "Sleep",\n      "text_quote": "all he does is eat and sleep",\n      "attributes": {"quality": "Unknown", \n                     "duration": "Unknown", \n                     "time":"Unknown",\n                     "caused_by":"Unknown"}\n    },\n    {\n      "event_type": "Excretion",\n      "text_quote": "bm x1 mod brown formed stool.",\n      "attributes": {"type": "stool", \n                     "quality": "formed", \n                     "frequency":"x1", \n                     "time":"Unknown",\n                     "caused_by":"Unknown"}\n    },\n    {\n      "event_type": "Excretion",\n      "text_quote": "Foley draining clear, yellow urine.",\n      "attributes": {"type": "urine", \n                     "quality": "clear, yellow", \n                     "frequency":"Unknown", \n                     "time":"Unknown",\n                     "caused_by":"Unknown"}\n    },\n    {\n      "event_type": "Family",\n      "text_quote": "my son doesn\'t help at all at home",\n      "attributes": {"interaction": "visit", \n                     "relation": "son",\n                     "time":"Unknown",\n                     "caused_by":"Unknown"}\n    }\n  ]\n}', 'attributes': [{'Eating': {'food': 'Unknown', 'amount': 'Unknown', 'method': 'Unknown', 'time': 'Unknown', 'caused_by': 'Unknown'}}, {'Sleep': {'quality': 'Unknown', 'duration': 'Unknown', 'time': 'Unknown', 'caused_by': 'Unknown'}}, {'Excretion': {'type': 'stool', 'quality': 'formed', 'frequency': 'x1', 'time': 'Unknown', 'caused_by': 'Unknown'}}, {'Excretion': {'type': 'urine', 'quality': 'clear, yellow', 'frequency': 'Unknown', 'time': 'Unknown', 'caused_by': 'Unknown'}}, {'Family': {'interaction': 'visit', 'relation': 'son', 'time': 'Unknown', 'caused_by': 'Unknown'}}], 'text_quotes': ['all he does is eat and sleep', 'all he does is eat and sleep', 'bm x1 mod brown formed stool.', 'Foley draining clear, yellow urine.', "my son doesn't help at all at home"], 'event_name_prompt': 'Given the text: ccu progress note:\n\ns: "my son doesn\'t help at all at home, all he does is eat and sleep"\n\no:  please see flow sheet for objective data\n\ncv: tele: sinus brady w/no ectopy. heart rate 50-57, abp 103-148/50-68. milrinone and labetelol drips dc\'d. started on by mouth labetelol diastolic blood pressure 140\'s given hydralazine 10 mg by mouth given with little effect. diastolic blood pressure goal to 120. hct 39.6- k 3.8, 40 meq kcl given. repeat k 4.3. mg 2.\n\nresp: o2 5l nc. ls diminished at the bases. no labored breathing, zero retractions, sp02 92-97%.\n\ngi/gu: abd soft, non-distended, bs present x4. bm x1 mod brown formed stool. by mouth intake fair. gu: foley draining clear, yellow urine. lasix 80 mg iv given with good effect. negative 1900cc\'s since twelve a.male. bun 38, crea 2.1.\n\nneuro: patient a&amp;o x 3, moving all extremities, follows commands, restless at times. verbalized overwhelming responsibilities at home, social worker consulted.\n\niv access: picc line placed right upper arm (single lumen).\n\na) successfully weaned off of labetalol and milrinone drips. patient tolerated by mouth labetalol and hydralazine well. ? cath tomorrow.\n\np) monitor vital signs, lung sounds, i &amp; o, labs. keep diastolic blood pressure therapeutic range w/in 110-120. continute to monitor urinary output with follow-up labs. offer emotional support and update family on plan of care.\n\n                                                      [**first name8 (namepattern2) 1309**] [**last name (namepattern1) 9102**], sn\n\n\n, \n                        and the following event types with their definitions: Eating : The patient takes food into their body by mouth.\nExcretion : The patient discharges waste matter from their body.\nFamily : The patient has a visit, call, or communication with a family member.\nPain : The patient reports or shows signs of pain.\nSleep : The patient sleeps or the sleep’s quality or quantity is described.\nUnknown : choose "Unknown" if none of the other event type are applicable. \n                        ---\n                        Your task:\n                        0. Identify ALL events in the text (zero, one, or more).\n1. For each event, assign an event_type from the list above.\n2. If multiple event of same type is mentioned, assign the event_type multiple times\n3. Extract attributes for each event using ONLY the allowed attributes listed below.\n4. Output strictly valid JSON following the schema below.\n                        ---\n                        Classification Rules:\n                        - A text may contain multiple events of the same or different types.\n- Create a separate event object for each event mention.\n- If the text is explicitly a NEGATION (e.g., "denies pain"), do not extract that event.\n- If the text describes a FUTURE or HYPOTHETICAL event (e.g., "will eat tomorrow"), ignore it.\n- A valid event should have occurred in the recent past or is occurring during the time of writing of the text.\n- If no events are found or if unsure, return {"events": []}\n                        \n                        ---\n                                    Attributes allowed:\n                                    {\'Eating\': {\'food\': \'&lt;string&gt; # e.g., pancakes, porridge, etc.\', \'amount\': \'&lt;string&gt; # e.g., 1, 2 bowls, etc.\', \'method\': \'&lt;string&gt;  # e.g., oral, tube, etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, after shower, etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}, \'Excretion\': {\'type\': \'&lt;string&gt; # e.g., urine, stool, etc.\', \'frequency\': \'&lt;string&gt; # e.g., 2x, once, etc.\', \'quality\': \'&lt;string&gt; # e.g., loose, hard, etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, after shower, etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}, \'Family\': {\'interaction\': \'&lt;string&gt; # e.g., visit, call, communication, etc.\', \'relation\': \'&lt;string&gt; # e.g., mother, son, etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, after shower, etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}, \'Pain\': {\'severity\': \'&lt;string&gt; # e.g., mild, moderate, severe, numeric scale if present, etc.\', \'location\': \'&lt;string&gt; # e.g., right knee, head, etc.\', \'duration\': \'&lt;string&gt; # e.g., all night, 3 hours, etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, after shower, etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}, \'Sleep\': {\'quality\': \'&lt;string&gt; # e.g., good, poor, restless, etc.\', \'duration\': \'&lt;string&gt; # e.g., 6 hours, phrases like "all night", etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, after shower, etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}}\n                                    If no relevant attribute exists for an event, return an empty object {}.\n                                    \n                        \n                        \n                        ---\n                        Output Schema (strict):\n                        {\n                                    "events": [\n                                        {\n                                        "event_type": "&lt;Pain | Sleep | Excretion | Eating | Family&gt;",\n                                        "text_quote": "&lt;fragement from the text indicating &gt;",\n                "attributes": {\n                    "&lt;attribute_name&gt;": "&lt;attribute_value&gt;"\n                }\n                                        }\n                                    ]\n                                    }\n                        \n                            Rules:\n                                - Ensure the output is valid JSON (parseable).\n                                - "eventS" must always be an array (can be empty).\n                                - Multiple instances of the same event type appear as individual elements in the event array.\n                                - Events appear in the array in the same order in which they appear in the text.\n                                - Do not include extra keys, comments, or text.\n                                - Each object in "events" must contain "event_type", "text_quote", and "attributes".\n                                -If an event attribute type has no value mentioned, return "attributes": {"&lt; attribute name &gt;:Unknown"} for each attribute type defined for the event type \n                        \n                        \n                        \n                ---\n                Examples:\n                \n                text: "Patient ate breakfast this morning. He seems less anxious."\n                output: {\n                "events": [\n                    {\n                    "event_type": "Eating",\n                    "text_quote":"Patient ate breakfast this morning",\n                    "attributes": {"food": "breakfast", \n                                   "amount": "Unknown",\n                                   "method": "Unknown",\n                                   "time":"morning",\n                                   "caused_by":"Unknown"}\n                    }\n                ]\n                }\n                \n                text: "Patient reported severe abdominal pain."\n                output: {\n                "events": [\n                    {\n                    "event_type": "Pain",\n                    "text_quote": "severe abdominal Pain",\n                    "attributes": {"severity": "severe", \n                                   "location": "abdominal",\n                                   "duration": "Unknown",\n                                   "time":"Unknown",\n                                   "caused_by":"Unknown"}\n                    }\n                ]\n                }\n                \n                text: "Patient called his son around 3 pm."\n                output: {\n                "events": [\n                    {\n                    "event_type": "Family",\n                    "text_quote": "called his son around 3 pm",\n                    "attributes": {"interaction": "call", \n                                    "relation": "son",\n                                    "time":"3 pm",\n                                    "caused_by":"Unknown"}\n                    }\n                ]\n                }\n                \n                text: "Patient had a loose stool overnight."\n                output: {\n                "events": [\n                    {\n                    "event_type": "Excretion",\n                    "text_quote": "loose stool overnight",\n                    "attributes": {"type": "stool", \n                                   "quality": "loose", \n                                   "frequency":"overnight", \n                                   "time":"night",\n                                   "caused_by":"Unknown"}\n                    }\n                ]\n                }\n                \n                text: "Patient was able to sleep well last night."\n                output: {\n                "events": [\n                    {\n                    "event_type": "Sleep",\n                    "text_quote": "sleep well last night",\n                    "attributes": {"quality": "well",\n                                    "duration": "Unknown", \n                                    "time":"night",\n                                    "caused_by":"Unknown"}\n                    }\n                ]\n                }\n                \n                text: "The patient couldn\'t sleep due to severe pain."\n                output: {\n                "events": [\n                    {\n                    "event_type": "Sleep",\n                    "text_quote": "couldn\'t sleep",\n                    "attributes": {"quality": "poor", \n                                    "duration": "Unknown",\n                                   "time":"Unknown",\n                                   "caused_by":"Pain"}\n                    },\n                    {\n                    "event_type": "Pain",\n                    "text_quote": "severe pain",\n                    "attributes": {"severity": "severe", \n                                    "location": "Unknown", \n                                    "duration": "Unknown", \n                                   "time":"before Sleep",\n                                   "caused_by":"Unknown"}\n                    }\n                ]\n                }\n                \n                text: "The patient complained of severe back pain, was given Tylenol, but the pain persisted and he was then prescribed stronger morphine."\n                output: {\n                "events": [\n                    {\n                    "event_type": "Pain",\n                    "text_quote": "complained of severe back pain",\n                    "attributes": {"severity": "severe", \n                                    "location": "back",\n                                    "duration": "Unknown", \n                                    "time":"Unknown",\n                                    "caused_by":"Unknown"}\n                    },\n                    {\n                    "event_type": "Pain",\n                    "text_quote": "pain persisted",\n                    "attributes": {"severity": "severe", \n                                   "location": "back",\n                                   "duration": "persistent", \n                                   "time":"after Tylenol",\n                                   "caused_by":"Unknown"}\n                    }\n                ]\n                }\n                \n                        ', 'event_detection_time': 12.248596679986804}</t>
+          <t>[{'Eating': {'food': 'Unknown', 'amount': 'Unknown', 'method': 'oral', 'negation': False, 'time': 'Unknown', 'caused_by': 'Unknown'}}, {'Sleep': {'quality': 'Unknown', 'duration': 'Unknown', 'negation': False, 'time': 'Unknown', 'caused_by': 'Unknown'}}, {'Family': {'interaction': 'Unknown', 'relation': 'son', 'negation': False, 'time': 'Unknown', 'caused_by': 'Unknown'}}, {'Excretion': {'type': 'stool', 'frequency': 'once', 'quality': 'moderate, brown, formed', 'negation': False, 'time': 'Unknown', 'caused_by': 'Unknown'}}, {'Excretion': {'type': 'urine', 'frequency': 'Unknown', 'quality': 'clear, yellow', 'negation': False, 'time': 'Unknown', 'caused_by': 'Unknown'}}, {'Family': {'interaction': 'consultation', 'relation': 'Unknown', 'negation': False, 'time': 'Unknown', 'caused_by': 'Unknown'}}]</t>
         </is>
       </c>
       <c r="N12" t="inlineStr">
         <is>
-          <t>['Eating', 'Sleep', 'Excretion', 'Excretion', 'Family']</t>
+          <t>['all he does is eat and sleep', 'all he does is eat and sleep', "my son doesn't help at all at home", 'bm x1 mod brown formed stool', 'foley draining clear, yellow urine', 'verbalized overwhelming responsibilities at home, social worker consulted']</t>
         </is>
       </c>
       <c r="O12" t="inlineStr">
         <is>
-          <t>[{'Eating': {'food': 'Unknown', 'amount': 'Unknown', 'method': 'Unknown', 'time': 'Unknown', 'caused_by': 'Unknown'}}, {'Sleep': {'quality': 'Unknown', 'duration': 'Unknown', 'time': 'Unknown', 'caused_by': 'Unknown'}}, {'Excretion': {'type': 'stool', 'quality': 'formed', 'frequency': 'x1', 'time': 'Unknown', 'caused_by': 'Unknown'}}, {'Excretion': {'type': 'urine', 'quality': 'clear, yellow', 'frequency': 'Unknown', 'time': 'Unknown', 'caused_by': 'Unknown'}}, {'Family': {'interaction': 'visit', 'relation': 'son', 'time': 'Unknown', 'caused_by': 'Unknown'}}]</t>
-        </is>
-      </c>
-      <c r="P12" t="inlineStr">
-        <is>
-          <t>['all he does is eat and sleep', 'all he does is eat and sleep', 'bm x1 mod brown formed stool.', 'Foley draining clear, yellow urine.', "my son doesn't help at all at home"]</t>
-        </is>
-      </c>
-      <c r="Q12" t="n">
-        <v>0.003127771000436042</v>
-      </c>
-      <c r="R12" t="inlineStr">
+          <t>[[['e1', 'simultaneous', 'e2'], ['e3', 'before', 'e4'], ['e4', 'before', 'e5'], ['e5', 'before', 'e6']]]</t>
+        </is>
+      </c>
+      <c r="P12" t="n">
+        <v>0.002387193002505228</v>
+      </c>
+      <c r="Q12" t="inlineStr">
         <is>
           <t>Sleep</t>
         </is>
       </c>
-      <c r="S12" t="b">
+      <c r="R12" t="b">
+        <v>0</v>
+      </c>
+      <c r="S12" t="n">
         <v>0</v>
       </c>
       <c r="T12" t="n">
-        <v>0</v>
-      </c>
-      <c r="U12" t="n">
-        <v>1</v>
-      </c>
-      <c r="V12" t="inlineStr">
+        <v>1</v>
+      </c>
+      <c r="U12" t="inlineStr">
         <is>
           <t>('eat', 'sleep', 'son', 'family', 'urine')</t>
         </is>
       </c>
+      <c r="V12" t="n">
+        <v>18.57729224697687</v>
+      </c>
       <c r="W12" t="n">
-        <v>8.453074363991618</v>
+        <v>18.80097839399241</v>
       </c>
       <c r="X12" t="n">
-        <v>15.66536787099903</v>
+        <v>1</v>
       </c>
       <c r="Y12" t="n">
-        <v>12.2485966799868</v>
+        <v>1</v>
       </c>
       <c r="Z12" t="n">
-        <v>1</v>
-      </c>
-      <c r="AA12" t="n">
-        <v>1</v>
-      </c>
-      <c r="AB12" t="n">
-        <v>1</v>
-      </c>
-      <c r="AC12" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="13">
-      <c r="A13" t="n">
-        <v>1310490</v>
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>1310490</t>
+        </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>['Sleep', 'Pain', 'Unknown']</t>
+          <t>('Pain', 'Sleep', 'Unknown')</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>['sleeping', 'sleep', 'slept', 'pain']</t>
+          <t>('pain', 'sleep', 'slept', 'sleeping')</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
@@ -2103,120 +1993,111 @@
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>{'text': 'ccu npn 7p-7a\ns: "i feel better today, [**initials (namepattern4) **] [**last name (namepattern4) **] some"\no: see carevue for complete assessment data\ncv: off labetalol and milrinone, tolerating standing labetalol by mouth and by mouth hydral, bp consistently 130s-140s&gt;120, around 0500 up to 160s, intern notified. heart rate sb 45-55, no ectopy. am labs pending. distal pulses palp/dop. no c/o cp/sob.\n\nresp: spo2 &gt;93% on 5l nc, @ times on ra with spo2 89-97%, noted ~20sec apenic pauses while sleeping (corresponding to subsequent ^diastolic blood pressure). lscta, diminished @ bases, fine bibasilar rales.\n\ngi/gu: abd soft, nontender, nondistended, +bs/-bm. tol pos npo after mn for tenative cath today (unlikely per resident). foley draining cyu, recieved additional 80mg lasix ivp @ mn with good diuresis, -2l yesterday, -1l thus far today.\n\nid: afebrile, tmax 97.9 by mouth. no abx.\n\nskin: cont ecchymotic in areas, l hand edema resolving. no b/d noted. turns by self in bed.\n\nneuro: slept through night, tylenol pro re nata for back pain.\n\na: 84yo with type b dissection off gtts today with spb consistently &gt;goal of 120 despite by mouth labetolol, hydralazine and diuresis with lasix.\n\np: cont to monitor bp, ? ^ by mouth meds. npo for ? cath today to eval hemodynamics and coronaries.  monitor resp sts/sleep apnea. follow up am labs. ? c/o to floor v. cath today.\n', 'event': ['Sleep', 'Pain', 'Excretion', 'Excretion', 'Eating', 'Eating'], 'phrase': '', 'raw_output': '{\n  "events": [\n    {\n      "event_type": "Sleep",\n      "text_quote": "slept through night",\n      "attributes": {\n        "quality": "good",\n        "duration": "all night",\n        "time": "night",\n        "caused_by": "Unknown"\n      }\n    },\n    {\n      "event_type": "Pain",\n      "text_quote": "back pain",\n      "attributes": {\n        "severity": "Unknown",\n        "location": "back",\n        "duration": "Unknown",\n        "time": "Unknown",\n        "caused_by": "Unknown"\n      }\n    },\n    {\n      "event_type": "Excretion",\n      "text_quote": "+bs/-bm, foley draining cyu",\n      "attributes": {\n        "type": "urine",\n        "frequency": "Unknown",\n        "quality": "Unknown",\n        "time": "Unknown",\n        "caused_by": "Unknown"\n      }\n    },\n    {\n      "event_type": "Excretion",\n      "text_quote": "-2l yesterday, -1l thus far today",\n      "attributes": {\n        "type": "urine",\n        "frequency": " Unknown",\n        "quality": "Unknown",\n        "time": "yesterday and today",\n        "caused_by": "lasix"\n      }\n    },\n    {\n      "event_type": "Eating",\n      "text_quote": "npo for ? cath today",\n      "attributes": {\n        "food": "Unknown",\n        "amount": "Unknown",\n        "method": "Unknown",\n        "time": "today",\n        "caused_by": "cath"\n      }\n    },\n    {\n      "event_type": "Eating",\n      "text_quote": "tol pos npo after mn for tenative cath today",\n      "attributes": {\n        "food": "Unknown",\n        "amount": "Unknown",\n        "method": "Unknown",\n        "time": "after morning",\n        "caused_by": "cath"\n      }\n    }\n  ]\n}', 'attributes': [{'Sleep': {'quality': 'good', 'duration': 'all night', 'time': 'night', 'caused_by': 'Unknown'}}, {'Pain': {'severity': 'Unknown', 'location': 'back', 'duration': 'Unknown', 'time': 'Unknown', 'caused_by': 'Unknown'}}, {'Excretion': {'type': 'urine', 'frequency': 'Unknown', 'quality': 'Unknown', 'time': 'Unknown', 'caused_by': 'Unknown'}}, {'Excretion': {'type': 'urine', 'frequency': ' Unknown', 'quality': 'Unknown', 'time': 'yesterday and today', 'caused_by': 'lasix'}}, {'Eating': {'food': 'Unknown', 'amount': 'Unknown', 'method': 'Unknown', 'time': 'today', 'caused_by': 'cath'}}, {'Eating': {'food': 'Unknown', 'amount': 'Unknown', 'method': 'Unknown', 'time': 'after morning', 'caused_by': 'cath'}}], 'text_quotes': ['slept through night', 'back pain', '+bs/-bm, foley draining cyu', '-2l yesterday, -1l thus far today', 'npo for ? cath today', 'tol pos npo after mn for tenative cath today'], 'event_name_prompt': 'Given the text: ccu npn 7p-7a\ns: "i feel better today, [**initials (namepattern4) **] [**last name (namepattern4) **] some"\no: see carevue for complete assessment data\ncv: off labetalol and milrinone, tolerating standing labetalol by mouth and by mouth hydral, bp consistently 130s-140s&gt;120, around 0500 up to 160s, intern notified. heart rate sb 45-55, no ectopy. am labs pending. distal pulses palp/dop. no c/o cp/sob.\n\nresp: spo2 &gt;93% on 5l nc, @ times on ra with spo2 89-97%, noted ~20sec apenic pauses while sleeping (corresponding to subsequent ^diastolic blood pressure). lscta, diminished @ bases, fine bibasilar rales.\n\ngi/gu: abd soft, nontender, nondistended, +bs/-bm. tol pos npo after mn for tenative cath today (unlikely per resident). foley draining cyu, recieved additional 80mg lasix ivp @ mn with good diuresis, -2l yesterday, -1l thus far today.\n\nid: afebrile, tmax 97.9 by mouth. no abx.\n\nskin: cont ecchymotic in areas, l hand edema resolving. no b/d noted. turns by self in bed.\n\nneuro: slept through night, tylenol pro re nata for back pain.\n\na: 84yo with type b dissection off gtts today with spb consistently &gt;goal of 120 despite by mouth labetolol, hydralazine and diuresis with lasix.\n\np: cont to monitor bp, ? ^ by mouth meds. npo for ? cath today to eval hemodynamics and coronaries.  monitor resp sts/sleep apnea. follow up am labs. ? c/o to floor v. cath today.\n, \n                        and the following event types with their definitions: Eating : The patient takes food into their body by mouth.\nExcretion : The patient discharges waste matter from their body.\nFamily : The patient has a visit, call, or communication with a family member.\nPain : The patient reports or shows signs of pain.\nSleep : The patient sleeps or the sleep’s quality or quantity is described.\nUnknown : choose "Unknown" if none of the other event type are applicable. \n                        ---\n                        Your task:\n                        0. Identify ALL events in the text (zero, one, or more).\n1. For each event, assign an event_type from the list above.\n2. If multiple event of same type is mentioned, assign the event_type multiple times\n3. Extract attributes for each event using ONLY the allowed attributes listed below.\n4. Use keyword evidence (Ki) ONLY if it is consistent with the text context.\n5. Output strictly valid JSON following the schema below.\n                        ---\n                        Classification Rules:\n                        - A text may contain multiple events of the same or different types.\n- Create a separate event object for each event mention.\n- If the text is explicitly a NEGATION (e.g., "denies pain"), do not extract that event.\n- If the text describes a FUTURE or HYPOTHETICAL event (e.g., "will eat tomorrow"), ignore it.\n- A valid event should have occurred in the recent past or is occurring during the time of writing of the text.\n- If no events are found or if unsure, return {"events": []}\n                        \n                        ---\n                                    Attributes allowed:\n                                    {\'Eating\': {\'food\': \'&lt;string&gt; # e.g., pancakes, porridge, etc.\', \'amount\': \'&lt;string&gt; # e.g., 1, 2 bowls, etc.\', \'method\': \'&lt;string&gt;  # e.g., oral, tube, etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, after shower, etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}, \'Excretion\': {\'type\': \'&lt;string&gt; # e.g., urine, stool, etc.\', \'frequency\': \'&lt;string&gt; # e.g., 2x, once, etc.\', \'quality\': \'&lt;string&gt; # e.g., loose, hard, etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, after shower, etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}, \'Family\': {\'interaction\': \'&lt;string&gt; # e.g., visit, call, communication, etc.\', \'relation\': \'&lt;string&gt; # e.g., mother, son, etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, after shower, etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}, \'Pain\': {\'severity\': \'&lt;string&gt; # e.g., mild, moderate, severe, numeric scale if present, etc.\', \'location\': \'&lt;string&gt; # e.g., right knee, head, etc.\', \'duration\': \'&lt;string&gt; # e.g., all night, 3 hours, etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, after shower, etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}, \'Sleep\': {\'quality\': \'&lt;string&gt; # e.g., good, poor, restless, etc.\', \'duration\': \'&lt;string&gt; # e.g., 6 hours, phrases like "all night", etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, after shower, etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}}\n                                    If no relevant attribute exists for an event, return an empty object {}.\n                                    \n                        \n                        ---\n                                    Keyword evidence (Ki):\n                                    Additional facts: A keyword matching algorithm without context detected keyword(s) [\'sleeping\', \'sleep\', \'slept\', \'pain\'].\n                                    Use this only as a pointer. If context contradicts, ignore.\n                        ---\n                        Output Schema (strict):\n                        {\n                                    "events": [\n                                        {\n                                        "event_type": "&lt;Pain | Sleep | Excretion | Eating | Family&gt;",\n                                        "text_quote": "&lt;fragement from the text indicating &gt;",\n                "attributes": {\n                    "&lt;attribute_name&gt;": "&lt;attribute_value&gt;"\n                }\n                                        }\n                                    ]\n                                    }\n                        \n                            Rules:\n                                - Ensure the output is valid JSON (parseable).\n                                - "eventS" must always be an array (can be empty).\n                                - Multiple instances of the same event type appear as individual elements in the event array.\n                                - Events appear in the array in the same order in which they appear in the text.\n                                - Do not include extra keys, comments, or text.\n                                - Each object in "events" must contain "event_type", "text_quote", and "attributes".\n                                -If an event attribute type has no value mentioned, return "attributes": {"&lt; attribute name &gt;:Unknown"} for each attribute type defined for the event type \n                        \n                        \n                        \n                ---\n                Examples:\n                \n                text: "Patient ate breakfast this morning. He seems less anxious."\n                output: {\n                "events": [\n                    {\n                    "event_type": "Eating",\n                    "text_quote":"Patient ate breakfast this morning",\n                    "attributes": {"food": "breakfast", \n                                   "amount": "Unknown",\n                                   "method": "Unknown",\n                                   "time":"morning",\n                                   "caused_by":"Unknown"}\n                    }\n                ]\n                }\n                \n                text: "Patient reported severe abdominal pain."\n                output: {\n                "events": [\n                    {\n                    "event_type": "Pain",\n                    "text_quote": "severe abdominal Pain",\n                    "attributes": {"severity": "severe", \n                                   "location": "abdominal",\n                                   "duration": "Unknown",\n                                   "time":"Unknown",\n                                   "caused_by":"Unknown"}\n                    }\n                ]\n                }\n                \n                text: "Patient called his son around 3 pm."\n                output: {\n                "events": [\n                    {\n                    "event_type": "Family",\n                    "text_quote": "called his son around 3 pm",\n                    "attributes": {"interaction": "call", \n                                    "relation": "son",\n                                    "time":"3 pm",\n                                    "caused_by":"Unknown"}\n                    }\n                ]\n                }\n                \n                text: "Patient had a loose stool overnight."\n                output: {\n                "events": [\n                    {\n                    "event_type": "Excretion",\n                    "text_quote": "loose stool overnight",\n                    "attributes": {"type": "stool", \n                                   "quality": "loose", \n                                   "frequency":"overnight", \n                                   "time":"night",\n                                   "caused_by":"Unknown"}\n                    }\n                ]\n                }\n                \n                text: "Patient was able to sleep well last night."\n                output: {\n                "events": [\n                    {\n                    "event_type": "Sleep",\n                    "text_quote": "sleep well last night",\n                    "attributes": {"quality": "well",\n                                    "duration": "Unknown", \n                                    "time":"night",\n                                    "caused_by":"Unknown"}\n                    }\n                ]\n                }\n                \n                text: "The patient couldn\'t sleep due to severe pain."\n                output: {\n                "events": [\n                    {\n                    "event_type": "Sleep",\n                    "text_quote": "couldn\'t sleep",\n                    "attributes": {"quality": "poor", \n                                    "duration": "Unknown",\n                                   "time":"Unknown",\n                                   "caused_by":"Pain"}\n                    },\n                    {\n                    "event_type": "Pain",\n                    "text_quote": "severe pain",\n                    "attributes": {"severity": "severe", \n                                    "location": "Unknown", \n                                    "duration": "Unknown", \n                                   "time":"before Sleep",\n                                   "caused_by":"Unknown"}\n                    }\n                ]\n                }\n                \n                text: "The patient complained of severe back pain, was given Tylenol, but the pain persisted and he was then prescribed stronger morphine."\n                output: {\n                "events": [\n                    {\n                    "event_type": "Pain",\n                    "text_quote": "complained of severe back pain",\n                    "attributes": {"severity": "severe", \n                                    "location": "back",\n                                    "duration": "Unknown", \n                                    "time":"Unknown",\n                                    "caused_by":"Unknown"}\n                    },\n                    {\n                    "event_type": "Pain",\n                    "text_quote": "pain persisted",\n                    "attributes": {"severity": "severe", \n                                   "location": "back",\n                                   "duration": "persistent", \n                                   "time":"after Tylenol",\n                                   "caused_by":"Unknown"}\n                    }\n                ]\n                }\n                \n                        ', 'event_detection_time': 15.500614459000644}</t>
+          <t>['pain', 'sleep', 'sleeping']</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>['Sleep', 'Pain', 'Excretion', 'Excretion', 'Eating', 'Eating']</t>
+          <t>{'text': 'ccu npn 7p-7a\ns: "i feel better today, [**initials (namepattern4) **] [**last name (namepattern4) **] some"\no: see carevue for complete assessment data\ncv: off labetalol and milrinone, tolerating standing labetalol by mouth and by mouth hydral, bp consistently 130s-140s&gt;120, around 0500 up to 160s, intern notified. heart rate sb 45-55, no ectopy. am labs pending. distal pulses palp/dop. no c/o cp/sob.\n\nresp: spo2 &gt;93% on 5l nc, @ times on ra with spo2 89-97%, noted ~20sec apenic pauses while sleeping (corresponding to subsequent ^diastolic blood pressure). lscta, diminished @ bases, fine bibasilar rales.\n\ngi/gu: abd soft, nontender, nondistended, +bs/-bm. tol pos npo after mn for tenative cath today (unlikely per resident). foley draining cyu, recieved additional 80mg lasix ivp @ mn with good diuresis, -2l yesterday, -1l thus far today.\n\nid: afebrile, tmax 97.9 by mouth. no abx.\n\nskin: cont ecchymotic in areas, l hand edema resolving. no b/d noted. turns by self in bed.\n\nneuro: slept through night, tylenol pro re nata for back pain.\n\na: 84yo with type b dissection off gtts today with spb consistently &gt;goal of 120 despite by mouth labetolol, hydralazine and diuresis with lasix.\n\np: cont to monitor bp, ? ^ by mouth meds. npo for ? cath today to eval hemodynamics and coronaries.  monitor resp sts/sleep apnea. follow up am labs. ? c/o to floor v. cath today.\n', 'event': ['Sleep', 'Pain', 'Excretion', 'Excretion', 'Sleep'], 'event_id': ['e1', 'e2', 'e3', 'e4', 'e5'], 'phrase': '', 'raw_output': '{\n  "events": [\n    {\n      "event_id": "e1",\n      "event_type": "Sleep",\n      "text_quote": "slept through night",\n      "attributes": {\n        "quality": "Unknown",\n        "duration": "all night",\n        "negation": "false",\n        "time": "night",\n        "caused_by": "Unknown"\n      }\n    },\n    {\n      "event_id": "e2",\n      "event_type": "Pain",\n      "text_quote": "back pain",\n      "attributes": {\n        "severity": "Unknown",\n        "location": "back",\n        "duration": "Unknown",\n        "negation": "false",\n        "time": "Unknown",\n        "caused_by": "Unknown"\n      }\n    },\n    {\n      "event_id": "e3",\n      "event_type": "Excretion",\n      "text_quote": "+bs/-bm, foley draining cyu",\n      "attributes": {\n        "type": "urine",\n        "frequency": "Unknown",\n        "quality": "Unknown",\n        "negation": "false",\n        "time": "Unknown",\n        "caused_by": "Unknown"\n      }\n    },\n    {\n      "event_id": "e4",\n      "event_type": "Excretion",\n      "text_quote": "-2l yesterday, -1l thus far today",\n      "attributes": {\n        "type": "urine",\n        "frequency": "Unknown",\n        "quality": "Unknown",\n        "negation": "false",\n        "time": "yesterday and today",\n        "caused_by": "lasix"\n      }\n    },\n    {\n      "event_id": "e5",\n      "event_type": "Sleep",\n      "text_quote": "~20sec apenic pauses while sleeping",\n      "attributes": {\n        "quality": "poor",\n        "duration": "Unknown",\n        "negation": "false",\n        "time": "Unknown",\n        "caused_by": "Unknown"\n      }\n    }\n  ],\n  "order": []\n}', 'attributes': [{'Sleep': {'quality': 'Unknown', 'duration': 'all night', 'negation': 'false', 'time': 'night', 'caused_by': 'Unknown'}}, {'Pain': {'severity': 'Unknown', 'location': 'back', 'duration': 'Unknown', 'negation': 'false', 'time': 'Unknown', 'caused_by': 'Unknown'}}, {'Excretion': {'type': 'urine', 'frequency': 'Unknown', 'quality': 'Unknown', 'negation': 'false', 'time': 'Unknown', 'caused_by': 'Unknown'}}, {'Excretion': {'type': 'urine', 'frequency': 'Unknown', 'quality': 'Unknown', 'negation': 'false', 'time': 'yesterday and today', 'caused_by': 'lasix'}}, {'Sleep': {'quality': 'poor', 'duration': 'Unknown', 'negation': 'false', 'time': 'Unknown', 'caused_by': 'Unknown'}}], 'orders': [[]], 'text_quotes': ['slept through night', 'back pain', '+bs/-bm, foley draining cyu', '-2l yesterday, -1l thus far today', '~20sec apenic pauses while sleeping'], 'event_name_prompt': 'Given the text: ccu npn 7p-7a\ns: "i feel better today, [**initials (namepattern4) **] [**last name (namepattern4) **] some"\no: see carevue for complete assessment data\ncv: off labetalol and milrinone, tolerating standing labetalol by mouth and by mouth hydral, bp consistently 130s-140s&gt;120, around 0500 up to 160s, intern notified. heart rate sb 45-55, no ectopy. am labs pending. distal pulses palp/dop. no c/o cp/sob.\n\nresp: spo2 &gt;93% on 5l nc, @ times on ra with spo2 89-97%, noted ~20sec apenic pauses while sleeping (corresponding to subsequent ^diastolic blood pressure). lscta, diminished @ bases, fine bibasilar rales.\n\ngi/gu: abd soft, nontender, nondistended, +bs/-bm. tol pos npo after mn for tenative cath today (unlikely per resident). foley draining cyu, recieved additional 80mg lasix ivp @ mn with good diuresis, -2l yesterday, -1l thus far today.\n\nid: afebrile, tmax 97.9 by mouth. no abx.\n\nskin: cont ecchymotic in areas, l hand edema resolving. no b/d noted. turns by self in bed.\n\nneuro: slept through night, tylenol pro re nata for back pain.\n\na: 84yo with type b dissection off gtts today with spb consistently &gt;goal of 120 despite by mouth labetolol, hydralazine and diuresis with lasix.\n\np: cont to monitor bp, ? ^ by mouth meds. npo for ? cath today to eval hemodynamics and coronaries.  monitor resp sts/sleep apnea. follow up am labs. ? c/o to floor v. cath today.\n, \n                        and the following event types with their definitions: Eating : The patient takes food into their body by mouth.\nExcretion : The patient discharges waste matter from their body.\nFamily : The patient has a visit, call, or communication with a family member.\nPain : The patient reports or shows signs of pain.\nSleep : The patient sleeps or the sleep’s quality or quantity is described.\nUnknown : choose "Unknown" if none of the other event type are applicable. \n                        ---\n                        Your task:\n                        0. Identify ALL events in the text (zero, one, or more).\n1. For each event, assign an event_type from the list above.\n2. If multiple event of same type is mentioned, assign the event_type multiple times\n3. Extract attributes for each event using ONLY the allowed attributes listed below.\n4. Use keyword evidence (Ki) ONLY if it is consistent with the text context.\n5. Output strictly valid JSON following the schema below.\n                        ---\n                        Classification Rules:\n                        - A text may contain multiple events of the same or different types.\n- Create a separate event object for each event mention.\n- If the text is explicitly a NEGATION (e.g., "denies pain"), do not extract that event.\n- If the text describes a FUTURE or HYPOTHETICAL event (e.g., "will eat tomorrow"), ignore it.\n- A valid event should have occurred in the recent past or is occurring during the time of writing of the text.\n- If no events are found or if unsure, return {"events": []}\n                        \n                        ---\n                                    Attributes allowed:\n                                    {\'Eating\': {\'food\': \'&lt;string&gt; # e.g., pancakes, porridge, etc.\', \'amount\': \'&lt;string&gt; # e.g., 1, 2 bowls, etc.\', \'method\': \'&lt;string&gt;  # e.g., oral, tube, etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, evening etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}, \'Excretion\': {\'type\': \'&lt;string&gt; # e.g., urine, stool, etc.\', \'frequency\': \'&lt;string&gt; # e.g., 2x, once, etc.\', \'quality\': \'&lt;string&gt; # e.g., loose, hard, etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, evening etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}, \'Family\': {\'interaction\': \'&lt;string&gt; # e.g., visit, call, communication, etc.\', \'relation\': \'&lt;string&gt; # e.g., mother, son, etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, evening etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}, \'Pain\': {\'severity\': \'&lt;string&gt; # e.g., mild, moderate, severe, numeric scale if present, etc.\', \'location\': \'&lt;string&gt; # e.g., right knee, head, etc.\', \'duration\': \'&lt;string&gt; # e.g., all night, 3 hours, etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, evening etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}, \'Sleep\': {\'quality\': \'&lt;string&gt; # e.g., good, poor, restless, etc.\', \'duration\': \'&lt;string&gt; # e.g., 6 hours, phrases like "all night", etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, evening etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}}\n                                    If no relevant attribute exists for an event, return an empty object {}.\n                                    \n                        \n                        ---\n                                    Keyword evidence (Ki):\n                                    Additional facts: A keyword matching algorithm without context detected keyword(s) (\'pain\', \'sleep\', \'slept\', \'sleeping\').\n                                    Use this only as a pointer. If context contradicts, ignore.\n                        ---\n                        Output Schema (strict):\n                        {\n                                    "events": [\n                                        {\n                                        "event_id": "&lt; A unique id eg.: e1 | e2 |...&gt;"\n                                        "event_type": "&lt;Pain | Sleep | Excretion | Eating | Family&gt;",\n                                        "text_quote": "&lt;fragement from the text indicating the event_type&gt;",\n                "attributes": {\n                    "&lt;attribute_name&gt;": "&lt;attribute_value&gt;"\n                }\n                                        }\n                                    ],\n                                    "order": [\n                                        ["e1", "before" | "after" | "simultaneous", "e2" ]\n                                    ]\n                                    }\n                        \n                            Rules:\n                                - Ensure the output is valid JSON (parseable).\n                                - "eventS" must always be an array (can be empty).\n                                - Multiple instances of the same event type appear with different ids.\n                                - Events appear in the array in the same order in which they appear in the text.\n                                - Their partial orders can be expressed using the "order" section.\n                                - Do not include extra keys, comments, or text.\n                                - Each object in "events" must contain "event_type", "text_quote", and "attributes".\n                                - If an event attribute type has no value mentioned, return "attributes": {"&lt; attribute name &gt;:Unknown"} for each attribute type defined for the event type \n                        \n                        \n                        \n                ---\n                Examples:\n                \n                text: "Patient ate breakfast this morning. He seems less anxious."\n                output: {\n                "events": [\n                    {"event_id": "e1",\n                    "event_type": "Eating",\n                    "text_quote":"Patient ate breakfast this morning",\n                    "attributes": {"food": "breakfast", \n                                   "amount": "Unknown",\n                                   "method": "Unknown",\n                                   "negation": "false",\n                                   "time":"morning",\n                                   "caused_by":"Unknown"}\n                    }\n                ],\n                "order":[]\n                }\n                \n                text: "Patient reported severe abdominal pain."\n                output: {\n                "events": [\n                    {"event_id": "e1",\n                    "event_type": "Pain",\n                    "text_quote": "severe abdominal Pain",\n                    "attributes": {"severity": "severe", \n                                   "location": "abdominal",\n                                   "duration": "Unknown",\n                                   "negation": "false",\n                                   "time":"Unknown",\n                                   "caused_by":"Unknown"}\n                    }\n                ],\n                "order":[]\n                }\n                \n                text: "Patient called his son around 3 pm."\n                output: {\n                "events": [\n                    {"event_id": "e1",\n                    "event_type": "Family",\n                    "text_quote": "called his son around 3 pm",\n                    "attributes": {"interaction": "call", \n                                    "relation": "son",\n                                    "negation": "false",\n                                    "time":"3 pm",\n                                    "caused_by":"Unknown"}\n                    }\n                ],\n                "order":[]\n                }\n                \n                text: "Patient had a loose stool overnight."\n                output: {\n                "events": [\n                    {"event_id": "e1",\n                    "event_type": "Excretion",\n                    "text_quote": "loose stool overnight",\n                    "attributes": {"type": "stool", \n                                   "quality": "loose", \n                                   "frequency":"overnight", \n                                   "negation": "false",\n                                   "time":"night",\n                                   "caused_by":"Unknown"}\n                    }\n                ],\n                "order":[]\n                }\n                \n                text: "Patient was able to sleep well last night."\n                output: {\n                "events": [\n                    {"event_id": "e1",\n                    "event_type": "Sleep",\n                    "text_quote": "sleep well last night",\n                    "attributes": {"quality": "well",\n                                    "duration": "Unknown", \n                                    "negation": "false",\n                                    "time":"night",\n                                    "caused_by":"Unknown"}\n                    }\n                ],\n                "order":[]\n                }\n                \n                text: "The patient couldn\'t sleep due to severe pain."\n                output: {\n                "events": [\n                    {"event_id": "e1",\n                    "event_type": "Sleep",\n                    "text_quote": "couldn\'t sleep",\n                    "attributes": {"quality": "poor", \n                                    "duration": "Unknown",\n                                    "negation": "true",\n                                    "time":"Unknown",\n                                    "caused_by":"Pain"}\n                    },\n                    {"event_id": "e2",\n                    "event_type": "Pain",\n                    "text_quote": "severe pain",\n                    "attributes": {"severity": "severe", \n                                    "location": "Unknown", \n                                    "duration": "Unknown", \n                                    "time":"Unknown",\n                                    "caused_by":"Unknown"}\n                    }\n                ],\n                "order":["e1", "after", "e2"]\n                }\n                \n                text: "The patient complained of severe back pain, was given Tylenol, but the pain persisted and he was then prescribed stronger morphine."\n                output: {\n                "events": [\n                    {"event_id": "e1",\n                    "event_type": "Pain",\n                    "text_quote": "complained of severe back pain",\n                    "attributes": {"severity": "severe", \n                                    "location": "back",\n                                    "duration": "Unknown", \n                                    "time":"Unknown",\n                                    "caused_by":"Unknown"}\n                    },\n                    {"event_id": "e2",\n                    "event_type": "Pain",\n                    "text_quote": "pain persisted",\n                    "attributes": {"severity": "severe", \n                                   "location": "back",\n                                   "duration": "persistent", \n                                   "time":"after Tylenol",\n                                   "caused_by":"Unknown"}\n                    }\n                ],\n                "order":[["e1", "before", "e2"]]\n                }\n                \n                        ', 'event_detection_time': 15.952894961985294}</t>
         </is>
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>[{'Sleep': {'quality': 'good', 'duration': 'all night', 'time': 'night', 'caused_by': 'Unknown'}}, {'Pain': {'severity': 'Unknown', 'location': 'back', 'duration': 'Unknown', 'time': 'Unknown', 'caused_by': 'Unknown'}}, {'Excretion': {'type': 'urine', 'frequency': 'Unknown', 'quality': 'Unknown', 'time': 'Unknown', 'caused_by': 'Unknown'}}, {'Excretion': {'type': 'urine', 'frequency': ' Unknown', 'quality': 'Unknown', 'time': 'yesterday and today', 'caused_by': 'lasix'}}, {'Eating': {'food': 'Unknown', 'amount': 'Unknown', 'method': 'Unknown', 'time': 'today', 'caused_by': 'cath'}}, {'Eating': {'food': 'Unknown', 'amount': 'Unknown', 'method': 'Unknown', 'time': 'after morning', 'caused_by': 'cath'}}]</t>
+          <t>['Sleep', 'Pain', 'Excretion', 'Excretion', 'Sleep']</t>
         </is>
       </c>
       <c r="H13" t="inlineStr">
         <is>
-          <t>['slept through night', 'back pain', '+bs/-bm, foley draining cyu', '-2l yesterday, -1l thus far today', 'npo for ? cath today', 'tol pos npo after mn for tenative cath today']</t>
+          <t>[{'Sleep': {'quality': 'Unknown', 'duration': 'all night', 'negation': 'false', 'time': 'night', 'caused_by': 'Unknown'}}, {'Pain': {'severity': 'Unknown', 'location': 'back', 'duration': 'Unknown', 'negation': 'false', 'time': 'Unknown', 'caused_by': 'Unknown'}}, {'Excretion': {'type': 'urine', 'frequency': 'Unknown', 'quality': 'Unknown', 'negation': 'false', 'time': 'Unknown', 'caused_by': 'Unknown'}}, {'Excretion': {'type': 'urine', 'frequency': 'Unknown', 'quality': 'Unknown', 'negation': 'false', 'time': 'yesterday and today', 'caused_by': 'lasix'}}, {'Sleep': {'quality': 'poor', 'duration': 'Unknown', 'negation': 'false', 'time': 'Unknown', 'caused_by': 'Unknown'}}]</t>
         </is>
       </c>
       <c r="I13" t="inlineStr">
         <is>
-          <t>{'text': 'ccu npn 7p-7a\ns: "i feel better today, [**initials (namepattern4) **] [**last name (namepattern4) **] some"\no: see carevue for complete assessment data\ncv: off labetalol and milrinone, tolerating standing labetalol by mouth and by mouth hydral, bp consistently 130s-140s&gt;120, around 0500 up to 160s, intern notified. heart rate sb 45-55, no ectopy. am labs pending. distal pulses palp/dop. no c/o cp/sob.\n\nresp: spo2 &gt;93% on 5l nc, @ times on ra with spo2 89-97%, noted ~20sec apenic pauses while sleeping (corresponding to subsequent ^diastolic blood pressure). lscta, diminished @ bases, fine bibasilar rales.\n\ngi/gu: abd soft, nontender, nondistended, +bs/-bm. tol pos npo after mn for tenative cath today (unlikely per resident). foley draining cyu, recieved additional 80mg lasix ivp @ mn with good diuresis, -2l yesterday, -1l thus far today.\n\nid: afebrile, tmax 97.9 by mouth. no abx.\n\nskin: cont ecchymotic in areas, l hand edema resolving. no b/d noted. turns by self in bed.\n\nneuro: slept through night, tylenol pro re nata for back pain.\n\na: 84yo with type b dissection off gtts today with spb consistently &gt;goal of 120 despite by mouth labetolol, hydralazine and diuresis with lasix.\n\np: cont to monitor bp, ? ^ by mouth meds. npo for ? cath today to eval hemodynamics and coronaries.  monitor resp sts/sleep apnea. follow up am labs. ? c/o to floor v. cath today.\n', 'event': ['Sleep', 'Pain', 'Excretion', 'Excretion', 'Eating', 'Sleep'], 'phrase': '', 'raw_output': '{\n  "events": [\n    {\n      "event_type": "Sleep",\n      "text_quote": "slept through night",\n      "attributes": {\n        "quality": "Unknown",\n        "duration": "all night",\n        "negation": false,\n        "time": "night",\n        "caused_by": "Unknown"\n      }\n    },\n    {\n      "event_type": "Pain",\n      "text_quote": "tylenol pro re nata for back pain",\n      "attributes": {\n        "severity": "Unknown",\n        "location": "back",\n        "duration": "Unknown",\n        "negation": false,\n        "time": "Unknown",\n        "caused_by": "Unknown"\n      }\n    },\n    {\n      "event_type": "Excretion",\n      "text_quote": "+bs/-bm, foley draining cyu, recieved additional 80mg lasix ivp @ mn with good diuresis, -2l yesterday, -1l thus far today.",\n      "attributes": {\n        "type": "urine",\n        "frequency": "Unknown",\n        "quality": "Unknown",\n        "negation": false,\n        "time": "yesterday and today",\n        "caused_by": "lasix"\n      }\n    },\n    {\n      "event_type": "Excretion",\n      "text_quote": "+bs/-bm, foley draining cyu, recieved additional 80mg lasix ivp @ mn with good diuresis, -2l yesterday, -1l thus far today.",\n      "attributes": {\n        "type": "stool",\n        "frequency": "Unknown",\n        "quality": "Unknown",\n        "negation": false,\n        "time": "Unknown",\n        "caused_by": "Unknown"\n      }\n    },\n    {\n      "event_type": "Eating",\n      "text_quote": "tol pos npo after mn for tenative cath today (unlikely per resident)",\n      "attributes": {\n        "food": "Unknown",\n        "amount": "Unknown",\n        "method": "oral",\n        "negation": true,\n        "time": "after morning",\n        "caused_by": "Unknown"\n      }\n    },\n    {\n      "event_type": "Sleep",\n      "text_quote": "noted ~20sec apenic pauses while sleeping (corresponding to subsequent ^diastolic blood pressure)",\n      "attributes": {\n        "quality": "poor",\n        "duration": "~20 seconds",\n        "negation": false,\n        "time": "Unknown",\n        "caused_by": "Unknown"\n      }\n    }\n  ]\n}', 'attributes': [{'Sleep': {'quality': 'Unknown', 'duration': 'all night', 'negation': False, 'time': 'night', 'caused_by': 'Unknown'}}, {'Pain': {'severity': 'Unknown', 'location': 'back', 'duration': 'Unknown', 'negation': False, 'time': 'Unknown', 'caused_by': 'Unknown'}}, {'Excretion': {'type': 'urine', 'frequency': 'Unknown', 'quality': 'Unknown', 'negation': False, 'time': 'yesterday and today', 'caused_by': 'lasix'}}, {'Excretion': {'type': 'stool', 'frequency': 'Unknown', 'quality': 'Unknown', 'negation': False, 'time': 'Unknown', 'caused_by': 'Unknown'}}, {'Eating': {'food': 'Unknown', 'amount': 'Unknown', 'method': 'oral', 'negation': True, 'time': 'after morning', 'caused_by': 'Unknown'}}, {'Sleep': {'quality': 'poor', 'duration': '~20 seconds', 'negation': False, 'time': 'Unknown', 'caused_by': 'Unknown'}}], 'text_quotes': ['slept through night', 'tylenol pro re nata for back pain', '+bs/-bm, foley draining cyu, recieved additional 80mg lasix ivp @ mn with good diuresis, -2l yesterday, -1l thus far today.', '+bs/-bm, foley draining cyu, recieved additional 80mg lasix ivp @ mn with good diuresis, -2l yesterday, -1l thus far today.', 'tol pos npo after mn for tenative cath today (unlikely per resident)', 'noted ~20sec apenic pauses while sleeping (corresponding to subsequent ^diastolic blood pressure)'], 'event_name_prompt': 'Given the text: ccu npn 7p-7a\ns: "i feel better today, [**initials (namepattern4) **] [**last name (namepattern4) **] some"\no: see carevue for complete assessment data\ncv: off labetalol and milrinone, tolerating standing labetalol by mouth and by mouth hydral, bp consistently 130s-140s&gt;120, around 0500 up to 160s, intern notified. heart rate sb 45-55, no ectopy. am labs pending. distal pulses palp/dop. no c/o cp/sob.\n\nresp: spo2 &gt;93% on 5l nc, @ times on ra with spo2 89-97%, noted ~20sec apenic pauses while sleeping (corresponding to subsequent ^diastolic blood pressure). lscta, diminished @ bases, fine bibasilar rales.\n\ngi/gu: abd soft, nontender, nondistended, +bs/-bm. tol pos npo after mn for tenative cath today (unlikely per resident). foley draining cyu, recieved additional 80mg lasix ivp @ mn with good diuresis, -2l yesterday, -1l thus far today.\n\nid: afebrile, tmax 97.9 by mouth. no abx.\n\nskin: cont ecchymotic in areas, l hand edema resolving. no b/d noted. turns by self in bed.\n\nneuro: slept through night, tylenol pro re nata for back pain.\n\na: 84yo with type b dissection off gtts today with spb consistently &gt;goal of 120 despite by mouth labetolol, hydralazine and diuresis with lasix.\n\np: cont to monitor bp, ? ^ by mouth meds. npo for ? cath today to eval hemodynamics and coronaries.  monitor resp sts/sleep apnea. follow up am labs. ? c/o to floor v. cath today.\n, \n                        and the following event types with their definitions: Eating : The patient takes food into their body by mouth.\nExcretion : The patient discharges waste matter from their body.\nFamily : The patient has a visit, call, or communication with a family member.\nPain : The patient reports or shows signs of pain.\nSleep : The patient sleeps or the sleep’s quality or quantity is described.\nUnknown : choose "Unknown" if none of the other event type are applicable. \n                        ---\n                        Your task:\n                        0. Identify ALL events in the text (zero, one, or more).\n1. For each event, assign an event_type from the list above.\n2. If multiple event of same type is mentioned, assign the event_type multiple times\n3. Extract attributes for each event using ONLY the allowed attributes listed below.\n4. Use keyword evidence (Ki) ONLY if it is consistent with the text context.\n5. Output strictly valid JSON following the schema below.\n                        ---\n                        Classification Rules:\n                        - A text may contain multiple events of the same or different types.\n- Create a separate event object for each event mention.\n- If the text is explicitly a NEGATION (e.g., "denies pain"), do not extract that event.\n- If the text describes a FUTURE or HYPOTHETICAL event (e.g., "will eat tomorrow"), ignore it.\n- A valid event should have occurred in the recent past or is occurring during the time of writing of the text.\n- If no events are found or if unsure, return {"events": []}\n                        \n                        ---\n                                    Attributes allowed:\n                                    {\'Eating\': {\'food\': \'&lt;string&gt; # e.g., pancakes, porridge, etc.\', \'amount\': \'&lt;string&gt; # e.g., 1, 2 bowls, etc.\', \'method\': \'&lt;string&gt;  # e.g., oral, tube, etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, after shower, etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}, \'Excretion\': {\'type\': \'&lt;string&gt; # e.g., urine, stool, etc.\', \'frequency\': \'&lt;string&gt; # e.g., 2x, once, etc.\', \'quality\': \'&lt;string&gt; # e.g., loose, hard, etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, after shower, etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}, \'Family\': {\'interaction\': \'&lt;string&gt; # e.g., visit, call, communication, etc.\', \'relation\': \'&lt;string&gt; # e.g., mother, son, etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, after shower, etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}, \'Pain\': {\'severity\': \'&lt;string&gt; # e.g., mild, moderate, severe, numeric scale if present, etc.\', \'location\': \'&lt;string&gt; # e.g., right knee, head, etc.\', \'duration\': \'&lt;string&gt; # e.g., all night, 3 hours, etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, after shower, etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}, \'Sleep\': {\'quality\': \'&lt;string&gt; # e.g., good, poor, restless, etc.\', \'duration\': \'&lt;string&gt; # e.g., 6 hours, phrases like "all night", etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, after shower, etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}}\n                                    If no relevant attribute exists for an event, return an empty object {}.\n                                    \n                        \n                        ---\n                                    Keyword evidence (Ki):\n                                    Additional facts: A keyword matching algorithm without context detected keyword(s) [\'sleeping\', \'sleep\', \'slept\', \'pain\'].\n                                    Use this only as a pointer. If context contradicts, ignore.\n                        ---\n                        Output Schema (strict):\n                        {\n                                    "events": [\n                                        {\n                                        "event_type": "&lt;Pain | Sleep | Excretion | Eating | Family&gt;",\n                                        "text_quote": "&lt;fragement from the text indicating &gt;",\n                "attributes": {\n                    "&lt;attribute_name&gt;": "&lt;attribute_value&gt;"\n                }\n                                        }\n                                    ]\n                                    }\n                        \n                            Rules:\n                                - Ensure the output is valid JSON (parseable).\n                                - "eventS" must always be an array (can be empty).\n                                - Multiple instances of the same event type appear as individual elements in the event array.\n                                - Events appear in the array in the same order in which they appear in the text.\n                                - Do not include extra keys, comments, or text.\n                                - Each object in "events" must contain "event_type", "text_quote", and "attributes".\n                                -If an event attribute type has no value mentioned, return "attributes": {"&lt; attribute name &gt;:Unknown"} for each attribute type defined for the event type \n                        \n                        \n                        \n                        ', 'event_detection_time': 18.069861648997176}</t>
+          <t>['slept through night', 'back pain', '+bs/-bm, foley draining cyu', '-2l yesterday, -1l thus far today', '~20sec apenic pauses while sleeping']</t>
         </is>
       </c>
       <c r="J13" t="inlineStr">
         <is>
-          <t>['Sleep', 'Pain', 'Excretion', 'Excretion', 'Eating', 'Sleep']</t>
+          <t>[[]]</t>
         </is>
       </c>
       <c r="K13" t="inlineStr">
         <is>
-          <t>[{'Sleep': {'quality': 'Unknown', 'duration': 'all night', 'negation': False, 'time': 'night', 'caused_by': 'Unknown'}}, {'Pain': {'severity': 'Unknown', 'location': 'back', 'duration': 'Unknown', 'negation': False, 'time': 'Unknown', 'caused_by': 'Unknown'}}, {'Excretion': {'type': 'urine', 'frequency': 'Unknown', 'quality': 'Unknown', 'negation': False, 'time': 'yesterday and today', 'caused_by': 'lasix'}}, {'Excretion': {'type': 'stool', 'frequency': 'Unknown', 'quality': 'Unknown', 'negation': False, 'time': 'Unknown', 'caused_by': 'Unknown'}}, {'Eating': {'food': 'Unknown', 'amount': 'Unknown', 'method': 'oral', 'negation': True, 'time': 'after morning', 'caused_by': 'Unknown'}}, {'Sleep': {'quality': 'poor', 'duration': '~20 seconds', 'negation': False, 'time': 'Unknown', 'caused_by': 'Unknown'}}]</t>
+          <t>{'text': 'ccu npn 7p-7a\ns: "i feel better today, [**initials (namepattern4) **] [**last name (namepattern4) **] some"\no: see carevue for complete assessment data\ncv: off labetalol and milrinone, tolerating standing labetalol by mouth and by mouth hydral, bp consistently 130s-140s&gt;120, around 0500 up to 160s, intern notified. heart rate sb 45-55, no ectopy. am labs pending. distal pulses palp/dop. no c/o cp/sob.\n\nresp: spo2 &gt;93% on 5l nc, @ times on ra with spo2 89-97%, noted ~20sec apenic pauses while sleeping (corresponding to subsequent ^diastolic blood pressure). lscta, diminished @ bases, fine bibasilar rales.\n\ngi/gu: abd soft, nontender, nondistended, +bs/-bm. tol pos npo after mn for tenative cath today (unlikely per resident). foley draining cyu, recieved additional 80mg lasix ivp @ mn with good diuresis, -2l yesterday, -1l thus far today.\n\nid: afebrile, tmax 97.9 by mouth. no abx.\n\nskin: cont ecchymotic in areas, l hand edema resolving. no b/d noted. turns by self in bed.\n\nneuro: slept through night, tylenol pro re nata for back pain.\n\na: 84yo with type b dissection off gtts today with spb consistently &gt;goal of 120 despite by mouth labetolol, hydralazine and diuresis with lasix.\n\np: cont to monitor bp, ? ^ by mouth meds. npo for ? cath today to eval hemodynamics and coronaries.  monitor resp sts/sleep apnea. follow up am labs. ? c/o to floor v. cath today.\n', 'event': ['Sleep', 'Pain', 'Excretion', 'Eating', 'Sleep'], 'event_id': ['e1', 'e2', 'e3', 'e4', 'e5'], 'phrase': '', 'raw_output': '{\n  "events": [\n    {\n      "event_id": "e1",\n      "event_type": "Sleep",\n      "text_quote": "slept through night",\n      "attributes": {\n        "quality": "Unknown",\n        "duration": "all night",\n        "negation": false,\n        "time": "night",\n        "caused_by": "Unknown"\n      }\n    },\n    {\n      "event_id": "e2",\n      "event_type": "Pain",\n      "text_quote": "tylenol pro re nata for back pain",\n      "attributes": {\n        "severity": "Unknown",\n        "location": "back",\n        "duration": "Unknown",\n        "negation": false,\n        "time": "Unknown",\n        "caused_by": "Unknown"\n      }\n    },\n    {\n      "event_id": "e3",\n      "event_type": "Excretion",\n      "text_quote": "+bs/-bm, foley draining cyu, recieved additional 80mg lasix ivp @ mn with good diuresis, -2l yesterday, -1l thus far today",\n      "attributes": {\n        "type": "urine",\n        "frequency": "Unknown",\n        "quality": "Unknown",\n        "negation": false,\n        "time": "yesterday and today",\n        "caused_by": "lasix"\n      }\n    },\n    {\n      "event_id": "e4",\n      "event_type": "Eating",\n      "text_quote": "tol pos npo after mn for tenative cath today (unlikely per resident)",\n      "attributes": {\n        "food": "Unknown",\n        "amount": "Unknown",\n        "method": "oral",\n        "negation": true,\n        "time": "after morning",\n        "caused_by": "Unknown"\n      }\n    },\n    {\n      "event_id": "e5",\n      "event_type": "Sleep",\n      "text_quote": "~20sec apenic pauses while sleeping (corresponding to subsequent ^diastolic blood pressure)",\n      "attributes": {\n        "quality": "restless",\n        "duration": "Unknown",\n        "negation": false,\n        "time": "Unknown",\n        "caused_by": "Unknown"\n      }\n    }\n  ],\n  "order": [\n    ["e1", "before", "e2"],\n    ["e2", "before", "e3"],\n    ["e3", "before", "e4"],\n    ["e4", "before", "e5"]\n  ]\n}', 'attributes': [{'Sleep': {'quality': 'Unknown', 'duration': 'all night', 'negation': False, 'time': 'night', 'caused_by': 'Unknown'}}, {'Pain': {'severity': 'Unknown', 'location': 'back', 'duration': 'Unknown', 'negation': False, 'time': 'Unknown', 'caused_by': 'Unknown'}}, {'Excretion': {'type': 'urine', 'frequency': 'Unknown', 'quality': 'Unknown', 'negation': False, 'time': 'yesterday and today', 'caused_by': 'lasix'}}, {'Eating': {'food': 'Unknown', 'amount': 'Unknown', 'method': 'oral', 'negation': True, 'time': 'after morning', 'caused_by': 'Unknown'}}, {'Sleep': {'quality': 'restless', 'duration': 'Unknown', 'negation': False, 'time': 'Unknown', 'caused_by': 'Unknown'}}], 'orders': [[['e1', 'before', 'e2'], ['e2', 'before', 'e3'], ['e3', 'before', 'e4'], ['e4', 'before', 'e5']]], 'text_quotes': ['slept through night', 'tylenol pro re nata for back pain', '+bs/-bm, foley draining cyu, recieved additional 80mg lasix ivp @ mn with good diuresis, -2l yesterday, -1l thus far today', 'tol pos npo after mn for tenative cath today (unlikely per resident)', '~20sec apenic pauses while sleeping (corresponding to subsequent ^diastolic blood pressure)'], 'event_name_prompt': 'Given the text: ccu npn 7p-7a\ns: "i feel better today, [**initials (namepattern4) **] [**last name (namepattern4) **] some"\no: see carevue for complete assessment data\ncv: off labetalol and milrinone, tolerating standing labetalol by mouth and by mouth hydral, bp consistently 130s-140s&gt;120, around 0500 up to 160s, intern notified. heart rate sb 45-55, no ectopy. am labs pending. distal pulses palp/dop. no c/o cp/sob.\n\nresp: spo2 &gt;93% on 5l nc, @ times on ra with spo2 89-97%, noted ~20sec apenic pauses while sleeping (corresponding to subsequent ^diastolic blood pressure). lscta, diminished @ bases, fine bibasilar rales.\n\ngi/gu: abd soft, nontender, nondistended, +bs/-bm. tol pos npo after mn for tenative cath today (unlikely per resident). foley draining cyu, recieved additional 80mg lasix ivp @ mn with good diuresis, -2l yesterday, -1l thus far today.\n\nid: afebrile, tmax 97.9 by mouth. no abx.\n\nskin: cont ecchymotic in areas, l hand edema resolving. no b/d noted. turns by self in bed.\n\nneuro: slept through night, tylenol pro re nata for back pain.\n\na: 84yo with type b dissection off gtts today with spb consistently &gt;goal of 120 despite by mouth labetolol, hydralazine and diuresis with lasix.\n\np: cont to monitor bp, ? ^ by mouth meds. npo for ? cath today to eval hemodynamics and coronaries.  monitor resp sts/sleep apnea. follow up am labs. ? c/o to floor v. cath today.\n, \n                        and the following event types with their definitions: Eating : The patient takes food into their body by mouth.\nExcretion : The patient discharges waste matter from their body.\nFamily : The patient has a visit, call, or communication with a family member.\nPain : The patient reports or shows signs of pain.\nSleep : The patient sleeps or the sleep’s quality or quantity is described.\nUnknown : choose "Unknown" if none of the other event type are applicable. \n                        ---\n                        Your task:\n                        0. Identify ALL events in the text (zero, one, or more).\n1. For each event, assign an event_type from the list above.\n2. If multiple event of same type is mentioned, assign the event_type multiple times\n3. Extract attributes for each event using ONLY the allowed attributes listed below.\n4. Use keyword evidence (Ki) ONLY if it is consistent with the text context.\n5. Output strictly valid JSON following the schema below.\n                        ---\n                        Classification Rules:\n                        - A text may contain multiple events of the same or different types.\n- Create a separate event object for each event mention.\n- If the text is explicitly a NEGATION (e.g., "denies pain"), do not extract that event.\n- If the text describes a FUTURE or HYPOTHETICAL event (e.g., "will eat tomorrow"), ignore it.\n- A valid event should have occurred in the recent past or is occurring during the time of writing of the text.\n- If no events are found or if unsure, return {"events": []}\n                        \n                        ---\n                                    Attributes allowed:\n                                    {\'Eating\': {\'food\': \'&lt;string&gt; # e.g., pancakes, porridge, etc.\', \'amount\': \'&lt;string&gt; # e.g., 1, 2 bowls, etc.\', \'method\': \'&lt;string&gt;  # e.g., oral, tube, etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, evening etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}, \'Excretion\': {\'type\': \'&lt;string&gt; # e.g., urine, stool, etc.\', \'frequency\': \'&lt;string&gt; # e.g., 2x, once, etc.\', \'quality\': \'&lt;string&gt; # e.g., loose, hard, etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, evening etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}, \'Family\': {\'interaction\': \'&lt;string&gt; # e.g., visit, call, communication, etc.\', \'relation\': \'&lt;string&gt; # e.g., mother, son, etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, evening etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}, \'Pain\': {\'severity\': \'&lt;string&gt; # e.g., mild, moderate, severe, numeric scale if present, etc.\', \'location\': \'&lt;string&gt; # e.g., right knee, head, etc.\', \'duration\': \'&lt;string&gt; # e.g., all night, 3 hours, etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, evening etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}, \'Sleep\': {\'quality\': \'&lt;string&gt; # e.g., good, poor, restless, etc.\', \'duration\': \'&lt;string&gt; # e.g., 6 hours, phrases like "all night", etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, evening etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}}\n                                    If no relevant attribute exists for an event, return an empty object {}.\n                                    \n                        \n                        ---\n                                    Keyword evidence (Ki):\n                                    Additional facts: A keyword matching algorithm without context detected keyword(s) (\'pain\', \'sleep\', \'slept\', \'sleeping\').\n                                    Use this only as a pointer. If context contradicts, ignore.\n                        ---\n                        Output Schema (strict):\n                        {\n                                    "events": [\n                                        {\n                                        "event_id": "&lt; A unique id eg.: e1 | e2 |...&gt;"\n                                        "event_type": "&lt;Pain | Sleep | Excretion | Eating | Family&gt;",\n                                        "text_quote": "&lt;fragement from the text indicating the event_type&gt;",\n                "attributes": {\n                    "&lt;attribute_name&gt;": "&lt;attribute_value&gt;"\n                }\n                                        }\n                                    ],\n                                    "order": [\n                                        ["e1", "before" | "after" | "simultaneous", "e2" ]\n                                    ]\n                                    }\n                        \n                            Rules:\n                                - Ensure the output is valid JSON (parseable).\n                                - "eventS" must always be an array (can be empty).\n                                - Multiple instances of the same event type appear with different ids.\n                                - Events appear in the array in the same order in which they appear in the text.\n                                - Their partial orders can be expressed using the "order" section.\n                                - Do not include extra keys, comments, or text.\n                                - Each object in "events" must contain "event_type", "text_quote", and "attributes".\n                                - If an event attribute type has no value mentioned, return "attributes": {"&lt; attribute name &gt;:Unknown"} for each attribute type defined for the event type \n                        \n                        \n                        \n                        ', 'event_detection_time': 17.73115080303978}</t>
         </is>
       </c>
       <c r="L13" t="inlineStr">
         <is>
-          <t>['slept through night', 'tylenol pro re nata for back pain', '+bs/-bm, foley draining cyu, recieved additional 80mg lasix ivp @ mn with good diuresis, -2l yesterday, -1l thus far today.', '+bs/-bm, foley draining cyu, recieved additional 80mg lasix ivp @ mn with good diuresis, -2l yesterday, -1l thus far today.', 'tol pos npo after mn for tenative cath today (unlikely per resident)', 'noted ~20sec apenic pauses while sleeping (corresponding to subsequent ^diastolic blood pressure)']</t>
+          <t>['Sleep', 'Pain', 'Excretion', 'Eating', 'Sleep']</t>
         </is>
       </c>
       <c r="M13" t="inlineStr">
         <is>
-          <t>{'text': 'ccu npn 7p-7a\ns: "i feel better today, [**initials (namepattern4) **] [**last name (namepattern4) **] some"\no: see carevue for complete assessment data\ncv: off labetalol and milrinone, tolerating standing labetalol by mouth and by mouth hydral, bp consistently 130s-140s&gt;120, around 0500 up to 160s, intern notified. heart rate sb 45-55, no ectopy. am labs pending. distal pulses palp/dop. no c/o cp/sob.\n\nresp: spo2 &gt;93% on 5l nc, @ times on ra with spo2 89-97%, noted ~20sec apenic pauses while sleeping (corresponding to subsequent ^diastolic blood pressure). lscta, diminished @ bases, fine bibasilar rales.\n\ngi/gu: abd soft, nontender, nondistended, +bs/-bm. tol pos npo after mn for tenative cath today (unlikely per resident). foley draining cyu, recieved additional 80mg lasix ivp @ mn with good diuresis, -2l yesterday, -1l thus far today.\n\nid: afebrile, tmax 97.9 by mouth. no abx.\n\nskin: cont ecchymotic in areas, l hand edema resolving. no b/d noted. turns by self in bed.\n\nneuro: slept through night, tylenol pro re nata for back pain.\n\na: 84yo with type b dissection off gtts today with spb consistently &gt;goal of 120 despite by mouth labetolol, hydralazine and diuresis with lasix.\n\np: cont to monitor bp, ? ^ by mouth meds. npo for ? cath today to eval hemodynamics and coronaries.  monitor resp sts/sleep apnea. follow up am labs. ? c/o to floor v. cath today.\n', 'event': ['Sleep', 'Pain', 'Excretion', 'Excretion', 'Eating', 'Eating'], 'phrase': '', 'raw_output': '{\n  "events": [\n    {\n      "event_type": "Sleep",\n      "text_quote": "slept through night",\n      "attributes": {\n        "quality": "good",\n        "duration": "all night",\n        "time": "night",\n        "caused_by": "Unknown"\n      }\n    },\n    {\n      "event_type": "Pain",\n      "text_quote": "back pain",\n      "attributes": {\n        "severity": "Unknown",\n        "location": "back",\n        "duration": "Unknown",\n        "time": "Unknown",\n        "caused_by": "Unknown"\n      }\n    },\n    {\n      "event_type": "Excretion",\n      "text_quote": "+bs/-bm, foley draining cyu",\n      "attributes": {\n        "type": "urine",\n        "frequency": "Unknown",\n        "quality": "Unknown",\n        "time": "Unknown",\n        "caused_by": "Unknown"\n      }\n    },\n    {\n      "event_type": "Excretion",\n      "text_quote": "-2l yesterday, -1l thus far today",\n      "attributes": {\n        "type": "urine",\n        "frequency": " Unknown",\n        "quality": "Unknown",\n        "time": "yesterday and today",\n        "caused_by": "lasix"\n      }\n    },\n    {\n      "event_type": "Eating",\n      "text_quote": "npo for ? cath today",\n      "attributes": {\n        "food": "Unknown",\n        "amount": "Unknown",\n        "method": "oral",\n        "time": "today",\n        "caused_by": "cath"\n      }\n    },\n    {\n      "event_type": "Eating",\n      "text_quote": "tol pos npo after mn for tenative cath today",\n      "attributes": {\n        "food": "Unknown",\n        "amount": "Unknown",\n        "method": "oral",\n        "time": "after morning",\n        "caused_by": "cath"\n      }\n    }\n  ]\n}', 'attributes': [{'Sleep': {'quality': 'good', 'duration': 'all night', 'time': 'night', 'caused_by': 'Unknown'}}, {'Pain': {'severity': 'Unknown', 'location': 'back', 'duration': 'Unknown', 'time': 'Unknown', 'caused_by': 'Unknown'}}, {'Excretion': {'type': 'urine', 'frequency': 'Unknown', 'quality': 'Unknown', 'time': 'Unknown', 'caused_by': 'Unknown'}}, {'Excretion': {'type': 'urine', 'frequency': ' Unknown', 'quality': 'Unknown', 'time': 'yesterday and today', 'caused_by': 'lasix'}}, {'Eating': {'food': 'Unknown', 'amount': 'Unknown', 'method': 'oral', 'time': 'today', 'caused_by': 'cath'}}, {'Eating': {'food': 'Unknown', 'amount': 'Unknown', 'method': 'oral', 'time': 'after morning', 'caused_by': 'cath'}}], 'text_quotes': ['slept through night', 'back pain', '+bs/-bm, foley draining cyu', '-2l yesterday, -1l thus far today', 'npo for ? cath today', 'tol pos npo after mn for tenative cath today'], 'event_name_prompt': 'Given the text: ccu npn 7p-7a\ns: "i feel better today, [**initials (namepattern4) **] [**last name (namepattern4) **] some"\no: see carevue for complete assessment data\ncv: off labetalol and milrinone, tolerating standing labetalol by mouth and by mouth hydral, bp consistently 130s-140s&gt;120, around 0500 up to 160s, intern notified. heart rate sb 45-55, no ectopy. am labs pending. distal pulses palp/dop. no c/o cp/sob.\n\nresp: spo2 &gt;93% on 5l nc, @ times on ra with spo2 89-97%, noted ~20sec apenic pauses while sleeping (corresponding to subsequent ^diastolic blood pressure). lscta, diminished @ bases, fine bibasilar rales.\n\ngi/gu: abd soft, nontender, nondistended, +bs/-bm. tol pos npo after mn for tenative cath today (unlikely per resident). foley draining cyu, recieved additional 80mg lasix ivp @ mn with good diuresis, -2l yesterday, -1l thus far today.\n\nid: afebrile, tmax 97.9 by mouth. no abx.\n\nskin: cont ecchymotic in areas, l hand edema resolving. no b/d noted. turns by self in bed.\n\nneuro: slept through night, tylenol pro re nata for back pain.\n\na: 84yo with type b dissection off gtts today with spb consistently &gt;goal of 120 despite by mouth labetolol, hydralazine and diuresis with lasix.\n\np: cont to monitor bp, ? ^ by mouth meds. npo for ? cath today to eval hemodynamics and coronaries.  monitor resp sts/sleep apnea. follow up am labs. ? c/o to floor v. cath today.\n, \n                        and the following event types with their definitions: Eating : The patient takes food into their body by mouth.\nExcretion : The patient discharges waste matter from their body.\nFamily : The patient has a visit, call, or communication with a family member.\nPain : The patient reports or shows signs of pain.\nSleep : The patient sleeps or the sleep’s quality or quantity is described.\nUnknown : choose "Unknown" if none of the other event type are applicable. \n                        ---\n                        Your task:\n                        0. Identify ALL events in the text (zero, one, or more).\n1. For each event, assign an event_type from the list above.\n2. If multiple event of same type is mentioned, assign the event_type multiple times\n3. Extract attributes for each event using ONLY the allowed attributes listed below.\n4. Output strictly valid JSON following the schema below.\n                        ---\n                        Classification Rules:\n                        - A text may contain multiple events of the same or different types.\n- Create a separate event object for each event mention.\n- If the text is explicitly a NEGATION (e.g., "denies pain"), do not extract that event.\n- If the text describes a FUTURE or HYPOTHETICAL event (e.g., "will eat tomorrow"), ignore it.\n- A valid event should have occurred in the recent past or is occurring during the time of writing of the text.\n- If no events are found or if unsure, return {"events": []}\n                        \n                        ---\n                                    Attributes allowed:\n                                    {\'Eating\': {\'food\': \'&lt;string&gt; # e.g., pancakes, porridge, etc.\', \'amount\': \'&lt;string&gt; # e.g., 1, 2 bowls, etc.\', \'method\': \'&lt;string&gt;  # e.g., oral, tube, etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, after shower, etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}, \'Excretion\': {\'type\': \'&lt;string&gt; # e.g., urine, stool, etc.\', \'frequency\': \'&lt;string&gt; # e.g., 2x, once, etc.\', \'quality\': \'&lt;string&gt; # e.g., loose, hard, etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, after shower, etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}, \'Family\': {\'interaction\': \'&lt;string&gt; # e.g., visit, call, communication, etc.\', \'relation\': \'&lt;string&gt; # e.g., mother, son, etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, after shower, etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}, \'Pain\': {\'severity\': \'&lt;string&gt; # e.g., mild, moderate, severe, numeric scale if present, etc.\', \'location\': \'&lt;string&gt; # e.g., right knee, head, etc.\', \'duration\': \'&lt;string&gt; # e.g., all night, 3 hours, etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, after shower, etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}, \'Sleep\': {\'quality\': \'&lt;string&gt; # e.g., good, poor, restless, etc.\', \'duration\': \'&lt;string&gt; # e.g., 6 hours, phrases like "all night", etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, after shower, etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}}\n                                    If no relevant attribute exists for an event, return an empty object {}.\n                                    \n                        \n                        \n                        ---\n                        Output Schema (strict):\n                        {\n                                    "events": [\n                                        {\n                                        "event_type": "&lt;Pain | Sleep | Excretion | Eating | Family&gt;",\n                                        "text_quote": "&lt;fragement from the text indicating &gt;",\n                "attributes": {\n                    "&lt;attribute_name&gt;": "&lt;attribute_value&gt;"\n                }\n                                        }\n                                    ]\n                                    }\n                        \n                            Rules:\n                                - Ensure the output is valid JSON (parseable).\n                                - "eventS" must always be an array (can be empty).\n                                - Multiple instances of the same event type appear as individual elements in the event array.\n                                - Events appear in the array in the same order in which they appear in the text.\n                                - Do not include extra keys, comments, or text.\n                                - Each object in "events" must contain "event_type", "text_quote", and "attributes".\n                                -If an event attribute type has no value mentioned, return "attributes": {"&lt; attribute name &gt;:Unknown"} for each attribute type defined for the event type \n                        \n                        \n                        \n                ---\n                Examples:\n                \n                text: "Patient ate breakfast this morning. He seems less anxious."\n                output: {\n                "events": [\n                    {\n                    "event_type": "Eating",\n                    "text_quote":"Patient ate breakfast this morning",\n                    "attributes": {"food": "breakfast", \n                                   "amount": "Unknown",\n                                   "method": "Unknown",\n                                   "time":"morning",\n                                   "caused_by":"Unknown"}\n                    }\n                ]\n                }\n                \n                text: "Patient reported severe abdominal pain."\n                output: {\n                "events": [\n                    {\n                    "event_type": "Pain",\n                    "text_quote": "severe abdominal Pain",\n                    "attributes": {"severity": "severe", \n                                   "location": "abdominal",\n                                   "duration": "Unknown",\n                                   "time":"Unknown",\n                                   "caused_by":"Unknown"}\n                    }\n                ]\n                }\n                \n                text: "Patient called his son around 3 pm."\n                output: {\n                "events": [\n                    {\n                    "event_type": "Family",\n                    "text_quote": "called his son around 3 pm",\n                    "attributes": {"interaction": "call", \n                                    "relation": "son",\n                                    "time":"3 pm",\n                                    "caused_by":"Unknown"}\n                    }\n                ]\n                }\n                \n                text: "Patient had a loose stool overnight."\n                output: {\n                "events": [\n                    {\n                    "event_type": "Excretion",\n                    "text_quote": "loose stool overnight",\n                    "attributes": {"type": "stool", \n                                   "quality": "loose", \n                                   "frequency":"overnight", \n                                   "time":"night",\n                                   "caused_by":"Unknown"}\n                    }\n                ]\n                }\n                \n                text: "Patient was able to sleep well last night."\n                output: {\n                "events": [\n                    {\n                    "event_type": "Sleep",\n                    "text_quote": "sleep well last night",\n                    "attributes": {"quality": "well",\n                                    "duration": "Unknown", \n                                    "time":"night",\n                                    "caused_by":"Unknown"}\n                    }\n                ]\n                }\n                \n                text: "The patient couldn\'t sleep due to severe pain."\n                output: {\n                "events": [\n                    {\n                    "event_type": "Sleep",\n                    "text_quote": "couldn\'t sleep",\n                    "attributes": {"quality": "poor", \n                                    "duration": "Unknown",\n                                   "time":"Unknown",\n                                   "caused_by":"Pain"}\n                    },\n                    {\n                    "event_type": "Pain",\n                    "text_quote": "severe pain",\n                    "attributes": {"severity": "severe", \n                                    "location": "Unknown", \n                                    "duration": "Unknown", \n                                   "time":"before Sleep",\n                                   "caused_by":"Unknown"}\n                    }\n                ]\n                }\n                \n                text: "The patient complained of severe back pain, was given Tylenol, but the pain persisted and he was then prescribed stronger morphine."\n                output: {\n                "events": [\n                    {\n                    "event_type": "Pain",\n                    "text_quote": "complained of severe back pain",\n                    "attributes": {"severity": "severe", \n                                    "location": "back",\n                                    "duration": "Unknown", \n                                    "time":"Unknown",\n                                    "caused_by":"Unknown"}\n                    },\n                    {\n                    "event_type": "Pain",\n                    "text_quote": "pain persisted",\n                    "attributes": {"severity": "severe", \n                                   "location": "back",\n                                   "duration": "persistent", \n                                   "time":"after Tylenol",\n                                   "caused_by":"Unknown"}\n                    }\n                ]\n                }\n                \n                        ', 'event_detection_time': 15.352820611995412}</t>
+          <t>[{'Sleep': {'quality': 'Unknown', 'duration': 'all night', 'negation': False, 'time': 'night', 'caused_by': 'Unknown'}}, {'Pain': {'severity': 'Unknown', 'location': 'back', 'duration': 'Unknown', 'negation': False, 'time': 'Unknown', 'caused_by': 'Unknown'}}, {'Excretion': {'type': 'urine', 'frequency': 'Unknown', 'quality': 'Unknown', 'negation': False, 'time': 'yesterday and today', 'caused_by': 'lasix'}}, {'Eating': {'food': 'Unknown', 'amount': 'Unknown', 'method': 'oral', 'negation': True, 'time': 'after morning', 'caused_by': 'Unknown'}}, {'Sleep': {'quality': 'restless', 'duration': 'Unknown', 'negation': False, 'time': 'Unknown', 'caused_by': 'Unknown'}}]</t>
         </is>
       </c>
       <c r="N13" t="inlineStr">
         <is>
-          <t>['Sleep', 'Pain', 'Excretion', 'Excretion', 'Eating', 'Eating']</t>
+          <t>['slept through night', 'tylenol pro re nata for back pain', '+bs/-bm, foley draining cyu, recieved additional 80mg lasix ivp @ mn with good diuresis, -2l yesterday, -1l thus far today', 'tol pos npo after mn for tenative cath today (unlikely per resident)', '~20sec apenic pauses while sleeping (corresponding to subsequent ^diastolic blood pressure)']</t>
         </is>
       </c>
       <c r="O13" t="inlineStr">
         <is>
-          <t>[{'Sleep': {'quality': 'good', 'duration': 'all night', 'time': 'night', 'caused_by': 'Unknown'}}, {'Pain': {'severity': 'Unknown', 'location': 'back', 'duration': 'Unknown', 'time': 'Unknown', 'caused_by': 'Unknown'}}, {'Excretion': {'type': 'urine', 'frequency': 'Unknown', 'quality': 'Unknown', 'time': 'Unknown', 'caused_by': 'Unknown'}}, {'Excretion': {'type': 'urine', 'frequency': ' Unknown', 'quality': 'Unknown', 'time': 'yesterday and today', 'caused_by': 'lasix'}}, {'Eating': {'food': 'Unknown', 'amount': 'Unknown', 'method': 'oral', 'time': 'today', 'caused_by': 'cath'}}, {'Eating': {'food': 'Unknown', 'amount': 'Unknown', 'method': 'oral', 'time': 'after morning', 'caused_by': 'cath'}}]</t>
-        </is>
-      </c>
-      <c r="P13" t="inlineStr">
-        <is>
-          <t>['slept through night', 'back pain', '+bs/-bm, foley draining cyu', '-2l yesterday, -1l thus far today', 'npo for ? cath today', 'tol pos npo after mn for tenative cath today']</t>
-        </is>
-      </c>
-      <c r="Q13" t="n">
-        <v>0.00302272999942943</v>
-      </c>
-      <c r="R13" t="inlineStr">
+          <t>[[['e1', 'before', 'e2'], ['e2', 'before', 'e3'], ['e3', 'before', 'e4'], ['e4', 'before', 'e5']]]</t>
+        </is>
+      </c>
+      <c r="P13" t="n">
+        <v>0.002382867001870181</v>
+      </c>
+      <c r="Q13" t="inlineStr">
         <is>
           <t>Sleep</t>
         </is>
       </c>
-      <c r="S13" t="b">
-        <v>0</v>
+      <c r="R13" t="b">
+        <v>0</v>
+      </c>
+      <c r="S13" t="n">
+        <v>1</v>
       </c>
       <c r="T13" t="n">
         <v>1</v>
       </c>
-      <c r="U13" t="n">
-        <v>1</v>
-      </c>
-      <c r="V13" t="inlineStr">
+      <c r="U13" t="inlineStr">
         <is>
           <t>('pain', 'sleep', 'sleeping')</t>
         </is>
       </c>
+      <c r="V13" t="n">
+        <v>15.95289496198529</v>
+      </c>
       <c r="W13" t="n">
-        <v>15.50061445900064</v>
+        <v>17.73115080303978</v>
       </c>
       <c r="X13" t="n">
-        <v>18.06986164899718</v>
+        <v>1</v>
       </c>
       <c r="Y13" t="n">
-        <v>15.35282061199541</v>
+        <v>1</v>
       </c>
       <c r="Z13" t="n">
-        <v>1</v>
-      </c>
-      <c r="AA13" t="n">
-        <v>1</v>
-      </c>
-      <c r="AB13" t="n">
-        <v>1</v>
-      </c>
-      <c r="AC13" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="14">
-      <c r="A14" t="n">
-        <v>1325547</v>
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>1325547</t>
+        </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>['Sleep', 'Family', 'Unknown']</t>
+          <t>('Family', 'Sleep', 'Unknown')</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>['family', 'sleeping']</t>
+          <t>('family', 'sleeping')</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
@@ -2235,118 +2116,111 @@
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>{'text': 'nursing progress note [**2085**]-2300\ns: "my breathing feels better when i sit up"\n\no: please see carevue for complete objective data.\n\n39 year old female admitted for cardiomyopathy and heart failure. ef-15%.\n\nnsr with freq pvc\'s, no runs of vt since admission. diastolic blood pressure 110-120\'s, started on carvedilol 6.25. heparin sc. pulses palp, no c/o cp. k-6.1, hemolyzed, repeat pending. echo done.\n\nlung clr with rales in bases. c/o sob when lying flat. sats 95 when awake, dropped to high 80\'s when sleeping. placed on 2l nc, sats in mid 90\'s. had cxr.\n\nnas diet, bs present, had guaiac - bm and voided. placed foley and gave lasix 20mg iv. patient on 1500cc fluid restriction.\n\nafebrile, wbc-10.4. 2 piv\'s.\n\nmonitor uo and fluid restriction. monitor response to cardiac meds. follow up c labs and tests. emotionally support patient and family.\n\n\n\n\n\n\n', 'event': ['Sleep', 'Excretion', 'Excretion', 'Eating', 'Family', 'Pain', 'Sleep', 'Sleep'], 'phrase': '', 'raw_output': '{\n  "events": [\n    {\n      "event_type": "Sleep",\n      "text_quote": "sats dropped to high 80\'s when sleeping",\n      "attributes": {\n        "quality": "poor",\n        "duration": "Unknown",\n        "time": "Unknown",\n        "caused_by": "Unknown"\n      }\n    },\n    {\n      "event_type": "Excretion",\n      "text_quote": "had guaiac - bm and voided",\n      "attributes": {\n        "type": "stool",\n        "frequency": "Unknown",\n        "quality": "Unknown",\n        "negation": "false",\n        "time": "Unknown",\n        "caused_by": "Unknown"\n      }\n    },\n    {\n      "event_type": "Excretion",\n      "text_quote": "had guaiac - bm and voided",\n      "attributes": {\n        "type": "urine",\n        "frequency": "Unknown",\n        "quality": "Unknown",\n        "negation": "false",\n        "time": "Unknown",\n        "caused_by": "Unknown"\n      }\n    },\n    {\n      "event_type": "Eating",\n      "text_quote": "nas diet, bs present",\n      "attributes": {\n        "food": "Unknown",\n        "amount": "Unknown",\n        "method": "oral",\n        "negation": "false",\n        "time": "Unknown",\n        "caused_by": "Unknown"\n      }\n    },\n    {\n      "event_type": "Family",\n      "text_quote": "emotionally support patient and family",\n      "attributes": {\n        "interaction": "support",\n        "relation": "family",\n        "negation": "false",\n        "time": "Unknown",\n        "caused_by": "Unknown"\n      }\n    },\n    {\n      "event_type": "Pain",\n      "text_quote": "c/o sob when lying flat",\n      "attributes": {\n        "severity": "Unknown",\n        "location": "chest",\n        "duration": "Unknown",\n        "negation": "false",\n        "time": "when lying flat",\n        "caused_by": "Unknown"\n      }\n    },\n    {\n      "event_type": "Sleep",\n      "text_quote": "sats 95 when awake, dropped to high 80\'s when sleeping",\n      "attributes": {\n        "quality": "poor",\n        "duration": "Unknown",\n        "negation": "false",\n        "time": "when sleeping",\n        "caused_by": "Unknown"\n      }\n    },\n    {\n      "event_type": "Sleep",\n      "text_quote": "sats 95 when awake, dropped to high 80\'s when sleeping",\n      "attributes": {\n        "quality": "good",\n        "duration": "Unknown",\n        "negation": "false",\n        "time": "when awake",\n        "caused_by": "Unknown"\n      }\n    }\n  ]\n}', 'attributes': [{'Sleep': {'quality': 'poor', 'duration': 'Unknown', 'time': 'Unknown', 'caused_by': 'Unknown'}}, {'Excretion': {'type': 'stool', 'frequency': 'Unknown', 'quality': 'Unknown', 'negation': 'false', 'time': 'Unknown', 'caused_by': 'Unknown'}}, {'Excretion': {'type': 'urine', 'frequency': 'Unknown', 'quality': 'Unknown', 'negation': 'false', 'time': 'Unknown', 'caused_by': 'Unknown'}}, {'Eating': {'food': 'Unknown', 'amount': 'Unknown', 'method': 'oral', 'negation': 'false', 'time': 'Unknown', 'caused_by': 'Unknown'}}, {'Family': {'interaction': 'support', 'relation': 'family', 'negation': 'false', 'time': 'Unknown', 'caused_by': 'Unknown'}}, {'Pain': {'severity': 'Unknown', 'location': 'chest', 'duration': 'Unknown', 'negation': 'false', 'time': 'when lying flat', 'caused_by': 'Unknown'}}, {'Sleep': {'quality': 'poor', 'duration': 'Unknown', 'negation': 'false', 'time': 'when sleeping', 'caused_by': 'Unknown'}}, {'Sleep': {'quality': 'good', 'duration': 'Unknown', 'negation': 'false', 'time': 'when awake', 'caused_by': 'Unknown'}}], 'text_quotes': ["sats dropped to high 80's when sleeping", 'had guaiac - bm and voided', 'had guaiac - bm and voided', 'nas diet, bs present', 'emotionally support patient and family', 'c/o sob when lying flat', "sats 95 when awake, dropped to high 80's when sleeping", "sats 95 when awake, dropped to high 80's when sleeping"], 'event_name_prompt': 'Given the text: nursing progress note [**2085**]-2300\ns: "my breathing feels better when i sit up"\n\no: please see carevue for complete objective data.\n\n39 year old female admitted for cardiomyopathy and heart failure. ef-15%.\n\nnsr with freq pvc\'s, no runs of vt since admission. diastolic blood pressure 110-120\'s, started on carvedilol 6.25. heparin sc. pulses palp, no c/o cp. k-6.1, hemolyzed, repeat pending. echo done.\n\nlung clr with rales in bases. c/o sob when lying flat. sats 95 when awake, dropped to high 80\'s when sleeping. placed on 2l nc, sats in mid 90\'s. had cxr.\n\nnas diet, bs present, had guaiac - bm and voided. placed foley and gave lasix 20mg iv. patient on 1500cc fluid restriction.\n\nafebrile, wbc-10.4. 2 piv\'s.\n\nmonitor uo and fluid restriction. monitor response to cardiac meds. follow up c labs and tests. emotionally support patient and family.\n\n\n\n\n\n\n, \n                        and the following event types with their definitions: Eating : The patient takes food into their body by mouth.\nExcretion : The patient discharges waste matter from their body.\nFamily : The patient has a visit, call, or communication with a family member.\nPain : The patient reports or shows signs of pain.\nSleep : The patient sleeps or the sleep’s quality or quantity is described.\nUnknown : choose "Unknown" if none of the other event type are applicable. \n                        ---\n                        Your task:\n                        0. Identify ALL events in the text (zero, one, or more).\n1. For each event, assign an event_type from the list above.\n2. If multiple event of same type is mentioned, assign the event_type multiple times\n3. Extract attributes for each event using ONLY the allowed attributes listed below.\n4. Use keyword evidence (Ki) ONLY if it is consistent with the text context.\n5. Output strictly valid JSON following the schema below.\n                        ---\n                        Classification Rules:\n                        - A text may contain multiple events of the same or different types.\n- Create a separate event object for each event mention.\n- If the text is explicitly a NEGATION (e.g., "denies pain"), do not extract that event.\n- If the text describes a FUTURE or HYPOTHETICAL event (e.g., "will eat tomorrow"), ignore it.\n- A valid event should have occurred in the recent past or is occurring during the time of writing of the text.\n- If no events are found or if unsure, return {"events": []}\n                        \n                        ---\n                                    Attributes allowed:\n                                    {\'Eating\': {\'food\': \'&lt;string&gt; # e.g., pancakes, porridge, etc.\', \'amount\': \'&lt;string&gt; # e.g., 1, 2 bowls, etc.\', \'method\': \'&lt;string&gt;  # e.g., oral, tube, etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, after shower, etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}, \'Excretion\': {\'type\': \'&lt;string&gt; # e.g., urine, stool, etc.\', \'frequency\': \'&lt;string&gt; # e.g., 2x, once, etc.\', \'quality\': \'&lt;string&gt; # e.g., loose, hard, etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, after shower, etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}, \'Family\': {\'interaction\': \'&lt;string&gt; # e.g., visit, call, communication, etc.\', \'relation\': \'&lt;string&gt; # e.g., mother, son, etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, after shower, etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}, \'Pain\': {\'severity\': \'&lt;string&gt; # e.g., mild, moderate, severe, numeric scale if present, etc.\', \'location\': \'&lt;string&gt; # e.g., right knee, head, etc.\', \'duration\': \'&lt;string&gt; # e.g., all night, 3 hours, etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, after shower, etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}, \'Sleep\': {\'quality\': \'&lt;string&gt; # e.g., good, poor, restless, etc.\', \'duration\': \'&lt;string&gt; # e.g., 6 hours, phrases like "all night", etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, after shower, etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}}\n                                    If no relevant attribute exists for an event, return an empty object {}.\n                                    \n                        \n                        ---\n                                    Keyword evidence (Ki):\n                                    Additional facts: A keyword matching algorithm without context detected keyword(s) [\'family\', \'sleeping\'].\n                                    Use this only as a pointer. If context contradicts, ignore.\n                        ---\n                        Output Schema (strict):\n                        {\n                                    "events": [\n                                        {\n                                        "event_type": "&lt;Pain | Sleep | Excretion | Eating | Family&gt;",\n                                        "text_quote": "&lt;fragement from the text indicating &gt;",\n                "attributes": {\n                    "&lt;attribute_name&gt;": "&lt;attribute_value&gt;"\n                }\n                                        }\n                                    ]\n                                    }\n                        \n                            Rules:\n                                - Ensure the output is valid JSON (parseable).\n                                - "eventS" must always be an array (can be empty).\n                                - Multiple instances of the same event type appear as individual elements in the event array.\n                                - Events appear in the array in the same order in which they appear in the text.\n                                - Do not include extra keys, comments, or text.\n                                - Each object in "events" must contain "event_type", "text_quote", and "attributes".\n                                -If an event attribute type has no value mentioned, return "attributes": {"&lt; attribute name &gt;:Unknown"} for each attribute type defined for the event type \n                        \n                        \n                        \n                ---\n                Examples:\n                \n                text: "Patient ate breakfast this morning. He seems less anxious."\n                output: {\n                "events": [\n                    {\n                    "event_type": "Eating",\n                    "text_quote":"Patient ate breakfast this morning",\n                    "attributes": {"food": "breakfast", \n                                   "amount": "Unknown",\n                                   "method": "Unknown",\n                                   "time":"morning",\n                                   "caused_by":"Unknown"}\n                    }\n                ]\n                }\n                \n                text: "Patient reported severe abdominal pain."\n                output: {\n                "events": [\n                    {\n                    "event_type": "Pain",\n                    "text_quote": "severe abdominal Pain",\n                    "attributes": {"severity": "severe", \n                                   "location": "abdominal",\n                                   "duration": "Unknown",\n                                   "time":"Unknown",\n                                   "caused_by":"Unknown"}\n                    }\n                ]\n                }\n                \n                text: "Patient called his son around 3 pm."\n                output: {\n                "events": [\n                    {\n                    "event_type": "Family",\n                    "text_quote": "called his son around 3 pm",\n                    "attributes": {"interaction": "call", \n                                    "relation": "son",\n                                    "time":"3 pm",\n                                    "caused_by":"Unknown"}\n                    }\n                ]\n                }\n                \n                text: "Patient had a loose stool overnight."\n                output: {\n                "events": [\n                    {\n                    "event_type": "Excretion",\n                    "text_quote": "loose stool overnight",\n                    "attributes": {"type": "stool", \n                                   "quality": "loose", \n                                   "frequency":"overnight", \n                                   "time":"night",\n                                   "caused_by":"Unknown"}\n                    }\n                ]\n                }\n                \n                text: "Patient was able to sleep well last night."\n                output: {\n                "events": [\n                    {\n                    "event_type": "Sleep",\n                    "text_quote": "sleep well last night",\n                    "attributes": {"quality": "well",\n                                    "duration": "Unknown", \n                                    "time":"night",\n                                    "caused_by":"Unknown"}\n                    }\n                ]\n                }\n                \n                text: "The patient couldn\'t sleep due to severe pain."\n                output: {\n                "events": [\n                    {\n                    "event_type": "Sleep",\n                    "text_quote": "couldn\'t sleep",\n                    "attributes": {"quality": "poor", \n                                    "duration": "Unknown",\n                                   "time":"Unknown",\n                                   "caused_by":"Pain"}\n                    },\n                    {\n                    "event_type": "Pain",\n                    "text_quote": "severe pain",\n                    "attributes": {"severity": "severe", \n                                    "location": "Unknown", \n                                    "duration": "Unknown", \n                                   "time":"before Sleep",\n                                   "caused_by":"Unknown"}\n                    }\n                ]\n                }\n                \n                text: "The patient complained of severe back pain, was given Tylenol, but the pain persisted and he was then prescribed stronger morphine."\n                output: {\n                "events": [\n                    {\n                    "event_type": "Pain",\n                    "text_quote": "complained of severe back pain",\n                    "attributes": {"severity": "severe", \n                                    "location": "back",\n                                    "duration": "Unknown", \n                                    "time":"Unknown",\n                                    "caused_by":"Unknown"}\n                    },\n                    {\n                    "event_type": "Pain",\n                    "text_quote": "pain persisted",\n                    "attributes": {"severity": "severe", \n                                   "location": "back",\n                                   "duration": "persistent", \n                                   "time":"after Tylenol",\n                                   "caused_by":"Unknown"}\n                    }\n                ]\n                }\n                \n                        ', 'event_detection_time': 20.917169795997324}</t>
+          <t>['family', 'sleeping']</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>['Sleep', 'Excretion', 'Excretion', 'Eating', 'Family', 'Pain', 'Sleep', 'Sleep']</t>
+          <t>{'text': 'nursing progress note [**2085**]-2300\ns: "my breathing feels better when i sit up"\n\no: please see carevue for complete objective data.\n\n39 year old female admitted for cardiomyopathy and heart failure. ef-15%.\n\nnsr with freq pvc\'s, no runs of vt since admission. diastolic blood pressure 110-120\'s, started on carvedilol 6.25. heparin sc. pulses palp, no c/o cp. k-6.1, hemolyzed, repeat pending. echo done.\n\nlung clr with rales in bases. c/o sob when lying flat. sats 95 when awake, dropped to high 80\'s when sleeping. placed on 2l nc, sats in mid 90\'s. had cxr.\n\nnas diet, bs present, had guaiac - bm and voided. placed foley and gave lasix 20mg iv. patient on 1500cc fluid restriction.\n\nafebrile, wbc-10.4. 2 piv\'s.\n\nmonitor uo and fluid restriction. monitor response to cardiac meds. follow up c labs and tests. emotionally support patient and family.\n\n\n\n\n\n\n', 'event': ['Sleep', 'Excretion', 'Excretion', 'Family', 'Eating', 'Pain'], 'event_id': ['e1', 'e2', 'e3', 'e4', 'e5', 'e6'], 'phrase': '', 'raw_output': '{\n  "events": [\n    {\n      "event_id": "e1",\n      "event_type": "Sleep",\n      "text_quote": "sats dropped to high 80\'s when sleeping",\n      "attributes": {\n        "quality": "poor",\n        "duration": "Unknown",\n        "negation": "false",\n        "time": "Unknown",\n        "caused_by": "Unknown"\n      }\n    },\n    {\n      "event_id": "e2",\n      "event_type": "Excretion",\n      "text_quote": "had guaiac - bm and voided",\n      "attributes": {\n        "type": "stool",\n        "frequency": "Unknown",\n        "quality": "Unknown",\n        "negation": "false",\n        "time": "Unknown",\n        "caused_by": "Unknown"\n      }\n    },\n    {\n      "event_id": "e3",\n      "event_type": "Excretion",\n      "text_quote": "had guaiac - bm and voided",\n      "attributes": {\n        "type": "urine",\n        "frequency": "Unknown",\n        "quality": "Unknown",\n        "negation": "false",\n        "time": "Unknown",\n        "caused_by": "Unknown"\n      }\n    },\n    {\n      "event_id": "e4",\n      "event_type": "Family",\n      "text_quote": "emotionally support patient and family",\n      "attributes": {\n        "interaction": "Unknown",\n        "relation": "Unknown",\n        "negation": "false",\n        "time": "Unknown",\n        "caused_by": "Unknown"\n      }\n    },\n    {\n      "event_id": "e5",\n      "event_type": "Eating",\n      "text_quote": "nas diet, bs present",\n      "attributes": {\n        "food": "Unknown",\n        "amount": "Unknown",\n        "method": "oral",\n        "negation": "false",\n        "time": "Unknown",\n        "caused_by": "Unknown"\n      }\n    },\n    {\n      "event_id": "e6",\n      "event_type": "Pain",\n      "text_quote": "c/o sob when lying flat",\n      "attributes": {\n        "severity": "Unknown",\n        "location": "chest",\n        "duration": "Unknown",\n        "negation": "false",\n        "time": "Unknown",\n        "caused_by": "Unknown"\n      }\n    }\n  ],\n  "order": []\n}', 'attributes': [{'Sleep': {'quality': 'poor', 'duration': 'Unknown', 'negation': 'false', 'time': 'Unknown', 'caused_by': 'Unknown'}}, {'Excretion': {'type': 'stool', 'frequency': 'Unknown', 'quality': 'Unknown', 'negation': 'false', 'time': 'Unknown', 'caused_by': 'Unknown'}}, {'Excretion': {'type': 'urine', 'frequency': 'Unknown', 'quality': 'Unknown', 'negation': 'false', 'time': 'Unknown', 'caused_by': 'Unknown'}}, {'Family': {'interaction': 'Unknown', 'relation': 'Unknown', 'negation': 'false', 'time': 'Unknown', 'caused_by': 'Unknown'}}, {'Eating': {'food': 'Unknown', 'amount': 'Unknown', 'method': 'oral', 'negation': 'false', 'time': 'Unknown', 'caused_by': 'Unknown'}}, {'Pain': {'severity': 'Unknown', 'location': 'chest', 'duration': 'Unknown', 'negation': 'false', 'time': 'Unknown', 'caused_by': 'Unknown'}}], 'orders': [[]], 'text_quotes': ["sats dropped to high 80's when sleeping", 'had guaiac - bm and voided', 'had guaiac - bm and voided', 'emotionally support patient and family', 'nas diet, bs present', 'c/o sob when lying flat'], 'event_name_prompt': 'Given the text: nursing progress note [**2085**]-2300\ns: "my breathing feels better when i sit up"\n\no: please see carevue for complete objective data.\n\n39 year old female admitted for cardiomyopathy and heart failure. ef-15%.\n\nnsr with freq pvc\'s, no runs of vt since admission. diastolic blood pressure 110-120\'s, started on carvedilol 6.25. heparin sc. pulses palp, no c/o cp. k-6.1, hemolyzed, repeat pending. echo done.\n\nlung clr with rales in bases. c/o sob when lying flat. sats 95 when awake, dropped to high 80\'s when sleeping. placed on 2l nc, sats in mid 90\'s. had cxr.\n\nnas diet, bs present, had guaiac - bm and voided. placed foley and gave lasix 20mg iv. patient on 1500cc fluid restriction.\n\nafebrile, wbc-10.4. 2 piv\'s.\n\nmonitor uo and fluid restriction. monitor response to cardiac meds. follow up c labs and tests. emotionally support patient and family.\n\n\n\n\n\n\n, \n                        and the following event types with their definitions: Eating : The patient takes food into their body by mouth.\nExcretion : The patient discharges waste matter from their body.\nFamily : The patient has a visit, call, or communication with a family member.\nPain : The patient reports or shows signs of pain.\nSleep : The patient sleeps or the sleep’s quality or quantity is described.\nUnknown : choose "Unknown" if none of the other event type are applicable. \n                        ---\n                        Your task:\n                        0. Identify ALL events in the text (zero, one, or more).\n1. For each event, assign an event_type from the list above.\n2. If multiple event of same type is mentioned, assign the event_type multiple times\n3. Extract attributes for each event using ONLY the allowed attributes listed below.\n4. Use keyword evidence (Ki) ONLY if it is consistent with the text context.\n5. Output strictly valid JSON following the schema below.\n                        ---\n                        Classification Rules:\n                        - A text may contain multiple events of the same or different types.\n- Create a separate event object for each event mention.\n- If the text is explicitly a NEGATION (e.g., "denies pain"), do not extract that event.\n- If the text describes a FUTURE or HYPOTHETICAL event (e.g., "will eat tomorrow"), ignore it.\n- A valid event should have occurred in the recent past or is occurring during the time of writing of the text.\n- If no events are found or if unsure, return {"events": []}\n                        \n                        ---\n                                    Attributes allowed:\n                                    {\'Eating\': {\'food\': \'&lt;string&gt; # e.g., pancakes, porridge, etc.\', \'amount\': \'&lt;string&gt; # e.g., 1, 2 bowls, etc.\', \'method\': \'&lt;string&gt;  # e.g., oral, tube, etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, evening etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}, \'Excretion\': {\'type\': \'&lt;string&gt; # e.g., urine, stool, etc.\', \'frequency\': \'&lt;string&gt; # e.g., 2x, once, etc.\', \'quality\': \'&lt;string&gt; # e.g., loose, hard, etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, evening etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}, \'Family\': {\'interaction\': \'&lt;string&gt; # e.g., visit, call, communication, etc.\', \'relation\': \'&lt;string&gt; # e.g., mother, son, etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, evening etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}, \'Pain\': {\'severity\': \'&lt;string&gt; # e.g., mild, moderate, severe, numeric scale if present, etc.\', \'location\': \'&lt;string&gt; # e.g., right knee, head, etc.\', \'duration\': \'&lt;string&gt; # e.g., all night, 3 hours, etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, evening etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}, \'Sleep\': {\'quality\': \'&lt;string&gt; # e.g., good, poor, restless, etc.\', \'duration\': \'&lt;string&gt; # e.g., 6 hours, phrases like "all night", etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, evening etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}}\n                                    If no relevant attribute exists for an event, return an empty object {}.\n                                    \n                        \n                        ---\n                                    Keyword evidence (Ki):\n                                    Additional facts: A keyword matching algorithm without context detected keyword(s) (\'family\', \'sleeping\').\n                                    Use this only as a pointer. If context contradicts, ignore.\n                        ---\n                        Output Schema (strict):\n                        {\n                                    "events": [\n                                        {\n                                        "event_id": "&lt; A unique id eg.: e1 | e2 |...&gt;"\n                                        "event_type": "&lt;Pain | Sleep | Excretion | Eating | Family&gt;",\n                                        "text_quote": "&lt;fragement from the text indicating the event_type&gt;",\n                "attributes": {\n                    "&lt;attribute_name&gt;": "&lt;attribute_value&gt;"\n                }\n                                        }\n                                    ],\n                                    "order": [\n                                        ["e1", "before" | "after" | "simultaneous", "e2" ]\n                                    ]\n                                    }\n                        \n                            Rules:\n                                - Ensure the output is valid JSON (parseable).\n                                - "eventS" must always be an array (can be empty).\n                                - Multiple instances of the same event type appear with different ids.\n                                - Events appear in the array in the same order in which they appear in the text.\n                                - Their partial orders can be expressed using the "order" section.\n                                - Do not include extra keys, comments, or text.\n                                - Each object in "events" must contain "event_type", "text_quote", and "attributes".\n                                - If an event attribute type has no value mentioned, return "attributes": {"&lt; attribute name &gt;:Unknown"} for each attribute type defined for the event type \n                        \n                        \n                        \n                ---\n                Examples:\n                \n                text: "Patient ate breakfast this morning. He seems less anxious."\n                output: {\n                "events": [\n                    {"event_id": "e1",\n                    "event_type": "Eating",\n                    "text_quote":"Patient ate breakfast this morning",\n                    "attributes": {"food": "breakfast", \n                                   "amount": "Unknown",\n                                   "method": "Unknown",\n                                   "negation": "false",\n                                   "time":"morning",\n                                   "caused_by":"Unknown"}\n                    }\n                ],\n                "order":[]\n                }\n                \n                text: "Patient reported severe abdominal pain."\n                output: {\n                "events": [\n                    {"event_id": "e1",\n                    "event_type": "Pain",\n                    "text_quote": "severe abdominal Pain",\n                    "attributes": {"severity": "severe", \n                                   "location": "abdominal",\n                                   "duration": "Unknown",\n                                   "negation": "false",\n                                   "time":"Unknown",\n                                   "caused_by":"Unknown"}\n                    }\n                ],\n                "order":[]\n                }\n                \n                text: "Patient called his son around 3 pm."\n                output: {\n                "events": [\n                    {"event_id": "e1",\n                    "event_type": "Family",\n                    "text_quote": "called his son around 3 pm",\n                    "attributes": {"interaction": "call", \n                                    "relation": "son",\n                                    "negation": "false",\n                                    "time":"3 pm",\n                                    "caused_by":"Unknown"}\n                    }\n                ],\n                "order":[]\n                }\n                \n                text: "Patient had a loose stool overnight."\n                output: {\n                "events": [\n                    {"event_id": "e1",\n                    "event_type": "Excretion",\n                    "text_quote": "loose stool overnight",\n                    "attributes": {"type": "stool", \n                                   "quality": "loose", \n                                   "frequency":"overnight", \n                                   "negation": "false",\n                                   "time":"night",\n                                   "caused_by":"Unknown"}\n                    }\n                ],\n                "order":[]\n                }\n                \n                text: "Patient was able to sleep well last night."\n                output: {\n                "events": [\n                    {"event_id": "e1",\n                    "event_type": "Sleep",\n                    "text_quote": "sleep well last night",\n                    "attributes": {"quality": "well",\n                                    "duration": "Unknown", \n                                    "negation": "false",\n                                    "time":"night",\n                                    "caused_by":"Unknown"}\n                    }\n                ],\n                "order":[]\n                }\n                \n                text: "The patient couldn\'t sleep due to severe pain."\n                output: {\n                "events": [\n                    {"event_id": "e1",\n                    "event_type": "Sleep",\n                    "text_quote": "couldn\'t sleep",\n                    "attributes": {"quality": "poor", \n                                    "duration": "Unknown",\n                                    "negation": "true",\n                                    "time":"Unknown",\n                                    "caused_by":"Pain"}\n                    },\n                    {"event_id": "e2",\n                    "event_type": "Pain",\n                    "text_quote": "severe pain",\n                    "attributes": {"severity": "severe", \n                                    "location": "Unknown", \n                                    "duration": "Unknown", \n                                    "time":"Unknown",\n                                    "caused_by":"Unknown"}\n                    }\n                ],\n                "order":["e1", "after", "e2"]\n                }\n                \n                text: "The patient complained of severe back pain, was given Tylenol, but the pain persisted and he was then prescribed stronger morphine."\n                output: {\n                "events": [\n                    {"event_id": "e1",\n                    "event_type": "Pain",\n                    "text_quote": "complained of severe back pain",\n                    "attributes": {"severity": "severe", \n                                    "location": "back",\n                                    "duration": "Unknown", \n                                    "time":"Unknown",\n                                    "caused_by":"Unknown"}\n                    },\n                    {"event_id": "e2",\n                    "event_type": "Pain",\n                    "text_quote": "pain persisted",\n                    "attributes": {"severity": "severe", \n                                   "location": "back",\n                                   "duration": "persistent", \n                                   "time":"after Tylenol",\n                                   "caused_by":"Unknown"}\n                    }\n                ],\n                "order":[["e1", "before", "e2"]]\n                }\n                \n                        ', 'event_detection_time': 18.33578487095656}</t>
         </is>
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>[{'Sleep': {'quality': 'poor', 'duration': 'Unknown', 'time': 'Unknown', 'caused_by': 'Unknown'}}, {'Excretion': {'type': 'stool', 'frequency': 'Unknown', 'quality': 'Unknown', 'negation': 'false', 'time': 'Unknown', 'caused_by': 'Unknown'}}, {'Excretion': {'type': 'urine', 'frequency': 'Unknown', 'quality': 'Unknown', 'negation': 'false', 'time': 'Unknown', 'caused_by': 'Unknown'}}, {'Eating': {'food': 'Unknown', 'amount': 'Unknown', 'method': 'oral', 'negation': 'false', 'time': 'Unknown', 'caused_by': 'Unknown'}}, {'Family': {'interaction': 'support', 'relation': 'family', 'negation': 'false', 'time': 'Unknown', 'caused_by': 'Unknown'}}, {'Pain': {'severity': 'Unknown', 'location': 'chest', 'duration': 'Unknown', 'negation': 'false', 'time': 'when lying flat', 'caused_by': 'Unknown'}}, {'Sleep': {'quality': 'poor', 'duration': 'Unknown', 'negation': 'false', 'time': 'when sleeping', 'caused_by': 'Unknown'}}, {'Sleep': {'quality': 'good', 'duration': 'Unknown', 'negation': 'false', 'time': 'when awake', 'caused_by': 'Unknown'}}]</t>
+          <t>['Sleep', 'Excretion', 'Excretion', 'Family', 'Eating', 'Pain']</t>
         </is>
       </c>
       <c r="H14" t="inlineStr">
         <is>
-          <t>["sats dropped to high 80's when sleeping", 'had guaiac - bm and voided', 'had guaiac - bm and voided', 'nas diet, bs present', 'emotionally support patient and family', 'c/o sob when lying flat', "sats 95 when awake, dropped to high 80's when sleeping", "sats 95 when awake, dropped to high 80's when sleeping"]</t>
+          <t>[{'Sleep': {'quality': 'poor', 'duration': 'Unknown', 'negation': 'false', 'time': 'Unknown', 'caused_by': 'Unknown'}}, {'Excretion': {'type': 'stool', 'frequency': 'Unknown', 'quality': 'Unknown', 'negation': 'false', 'time': 'Unknown', 'caused_by': 'Unknown'}}, {'Excretion': {'type': 'urine', 'frequency': 'Unknown', 'quality': 'Unknown', 'negation': 'false', 'time': 'Unknown', 'caused_by': 'Unknown'}}, {'Family': {'interaction': 'Unknown', 'relation': 'Unknown', 'negation': 'false', 'time': 'Unknown', 'caused_by': 'Unknown'}}, {'Eating': {'food': 'Unknown', 'amount': 'Unknown', 'method': 'oral', 'negation': 'false', 'time': 'Unknown', 'caused_by': 'Unknown'}}, {'Pain': {'severity': 'Unknown', 'location': 'chest', 'duration': 'Unknown', 'negation': 'false', 'time': 'Unknown', 'caused_by': 'Unknown'}}]</t>
         </is>
       </c>
       <c r="I14" t="inlineStr">
         <is>
-          <t>{'text': 'nursing progress note [**2085**]-2300\ns: "my breathing feels better when i sit up"\n\no: please see carevue for complete objective data.\n\n39 year old female admitted for cardiomyopathy and heart failure. ef-15%.\n\nnsr with freq pvc\'s, no runs of vt since admission. diastolic blood pressure 110-120\'s, started on carvedilol 6.25. heparin sc. pulses palp, no c/o cp. k-6.1, hemolyzed, repeat pending. echo done.\n\nlung clr with rales in bases. c/o sob when lying flat. sats 95 when awake, dropped to high 80\'s when sleeping. placed on 2l nc, sats in mid 90\'s. had cxr.\n\nnas diet, bs present, had guaiac - bm and voided. placed foley and gave lasix 20mg iv. patient on 1500cc fluid restriction.\n\nafebrile, wbc-10.4. 2 piv\'s.\n\nmonitor uo and fluid restriction. monitor response to cardiac meds. follow up c labs and tests. emotionally support patient and family.\n\n\n\n\n\n\n', 'event': ['Sleep', 'Excretion', 'Excretion', 'Family', 'Eating', 'Pain', 'Sleep'], 'phrase': '', 'raw_output': '{\n  "events": [\n    {\n      "event_type": "Sleep",\n      "text_quote": "sats dropped to high 80\'s when sleeping",\n      "attributes": {\n        "quality": "poor",\n        "duration": "Unknown",\n        "negation": false,\n        "time": "when sleeping",\n        "caused_by": "Unknown"\n      }\n    },\n    {\n      "event_type": "Excretion",\n      "text_quote": "had guaiac - bm and voided",\n      "attributes": {\n        "type": "stool",\n        "frequency": "Unknown",\n        "quality": "Unknown",\n        "negation": false,\n        "time": "Unknown",\n        "caused_by": "Unknown"\n      }\n    },\n    {\n      "event_type": "Excretion",\n      "text_quote": "had guaiac - bm and voided",\n      "attributes": {\n        "type": "urine",\n        "frequency": "Unknown",\n        "quality": "Unknown",\n        "negation": false,\n        "time": "Unknown",\n        "caused_by": "Unknown"\n      }\n    },\n    {\n      "event_type": "Family",\n      "text_quote": "emotionally support patient and family",\n      "attributes": {\n        "interaction": "communication",\n        "relation": "Unknown",\n        "negation": false,\n        "time": "Unknown",\n        "caused_by": "Unknown"\n      }\n    },\n    {\n      "event_type": "Eating",\n      "text_quote": "nas diet, bs present",\n      "attributes": {\n        "food": "Unknown",\n        "amount": "Unknown",\n        "method": "oral",\n        "negation": false,\n        "time": "Unknown",\n        "caused_by": "Unknown"\n      }\n    },\n    {\n      "event_type": "Pain",\n      "text_quote": "c/o sob when lying flat",\n      "attributes": {\n        "severity": "Unknown",\n        "location": "chest",\n        "duration": "Unknown",\n        "negation": false,\n        "time": "when lying flat",\n        "caused_by": "Unknown"\n      }\n    },\n    {\n      "event_type": "Sleep",\n      "text_quote": "sats 95 when awake, dropped to high 80\'s when sleeping",\n      "attributes": {\n        "quality": "good",\n        "duration": "Unknown",\n        "negation": false,\n        "time": "when awake",\n        "caused_by": "Unknown"\n      }\n    }\n  ]\n}', 'attributes': [{'Sleep': {'quality': 'poor', 'duration': 'Unknown', 'negation': False, 'time': 'when sleeping', 'caused_by': 'Unknown'}}, {'Excretion': {'type': 'stool', 'frequency': 'Unknown', 'quality': 'Unknown', 'negation': False, 'time': 'Unknown', 'caused_by': 'Unknown'}}, {'Excretion': {'type': 'urine', 'frequency': 'Unknown', 'quality': 'Unknown', 'negation': False, 'time': 'Unknown', 'caused_by': 'Unknown'}}, {'Family': {'interaction': 'communication', 'relation': 'Unknown', 'negation': False, 'time': 'Unknown', 'caused_by': 'Unknown'}}, {'Eating': {'food': 'Unknown', 'amount': 'Unknown', 'method': 'oral', 'negation': False, 'time': 'Unknown', 'caused_by': 'Unknown'}}, {'Pain': {'severity': 'Unknown', 'location': 'chest', 'duration': 'Unknown', 'negation': False, 'time': 'when lying flat', 'caused_by': 'Unknown'}}, {'Sleep': {'quality': 'good', 'duration': 'Unknown', 'negation': False, 'time': 'when awake', 'caused_by': 'Unknown'}}], 'text_quotes': ["sats dropped to high 80's when sleeping", 'had guaiac - bm and voided', 'had guaiac - bm and voided', 'emotionally support patient and family', 'nas diet, bs present', 'c/o sob when lying flat', "sats 95 when awake, dropped to high 80's when sleeping"], 'event_name_prompt': 'Given the text: nursing progress note [**2085**]-2300\ns: "my breathing feels better when i sit up"\n\no: please see carevue for complete objective data.\n\n39 year old female admitted for cardiomyopathy and heart failure. ef-15%.\n\nnsr with freq pvc\'s, no runs of vt since admission. diastolic blood pressure 110-120\'s, started on carvedilol 6.25. heparin sc. pulses palp, no c/o cp. k-6.1, hemolyzed, repeat pending. echo done.\n\nlung clr with rales in bases. c/o sob when lying flat. sats 95 when awake, dropped to high 80\'s when sleeping. placed on 2l nc, sats in mid 90\'s. had cxr.\n\nnas diet, bs present, had guaiac - bm and voided. placed foley and gave lasix 20mg iv. patient on 1500cc fluid restriction.\n\nafebrile, wbc-10.4. 2 piv\'s.\n\nmonitor uo and fluid restriction. monitor response to cardiac meds. follow up c labs and tests. emotionally support patient and family.\n\n\n\n\n\n\n, \n                        and the following event types with their definitions: Eating : The patient takes food into their body by mouth.\nExcretion : The patient discharges waste matter from their body.\nFamily : The patient has a visit, call, or communication with a family member.\nPain : The patient reports or shows signs of pain.\nSleep : The patient sleeps or the sleep’s quality or quantity is described.\nUnknown : choose "Unknown" if none of the other event type are applicable. \n                        ---\n                        Your task:\n                        0. Identify ALL events in the text (zero, one, or more).\n1. For each event, assign an event_type from the list above.\n2. If multiple event of same type is mentioned, assign the event_type multiple times\n3. Extract attributes for each event using ONLY the allowed attributes listed below.\n4. Use keyword evidence (Ki) ONLY if it is consistent with the text context.\n5. Output strictly valid JSON following the schema below.\n                        ---\n                        Classification Rules:\n                        - A text may contain multiple events of the same or different types.\n- Create a separate event object for each event mention.\n- If the text is explicitly a NEGATION (e.g., "denies pain"), do not extract that event.\n- If the text describes a FUTURE or HYPOTHETICAL event (e.g., "will eat tomorrow"), ignore it.\n- A valid event should have occurred in the recent past or is occurring during the time of writing of the text.\n- If no events are found or if unsure, return {"events": []}\n                        \n                        ---\n                                    Attributes allowed:\n                                    {\'Eating\': {\'food\': \'&lt;string&gt; # e.g., pancakes, porridge, etc.\', \'amount\': \'&lt;string&gt; # e.g., 1, 2 bowls, etc.\', \'method\': \'&lt;string&gt;  # e.g., oral, tube, etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, after shower, etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}, \'Excretion\': {\'type\': \'&lt;string&gt; # e.g., urine, stool, etc.\', \'frequency\': \'&lt;string&gt; # e.g., 2x, once, etc.\', \'quality\': \'&lt;string&gt; # e.g., loose, hard, etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, after shower, etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}, \'Family\': {\'interaction\': \'&lt;string&gt; # e.g., visit, call, communication, etc.\', \'relation\': \'&lt;string&gt; # e.g., mother, son, etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, after shower, etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}, \'Pain\': {\'severity\': \'&lt;string&gt; # e.g., mild, moderate, severe, numeric scale if present, etc.\', \'location\': \'&lt;string&gt; # e.g., right knee, head, etc.\', \'duration\': \'&lt;string&gt; # e.g., all night, 3 hours, etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, after shower, etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}, \'Sleep\': {\'quality\': \'&lt;string&gt; # e.g., good, poor, restless, etc.\', \'duration\': \'&lt;string&gt; # e.g., 6 hours, phrases like "all night", etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, after shower, etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}}\n                                    If no relevant attribute exists for an event, return an empty object {}.\n                                    \n                        \n                        ---\n                                    Keyword evidence (Ki):\n                                    Additional facts: A keyword matching algorithm without context detected keyword(s) [\'family\', \'sleeping\'].\n                                    Use this only as a pointer. If context contradicts, ignore.\n                        ---\n                        Output Schema (strict):\n                        {\n                                    "events": [\n                                        {\n                                        "event_type": "&lt;Pain | Sleep | Excretion | Eating | Family&gt;",\n                                        "text_quote": "&lt;fragement from the text indicating &gt;",\n                "attributes": {\n                    "&lt;attribute_name&gt;": "&lt;attribute_value&gt;"\n                }\n                                        }\n                                    ]\n                                    }\n                        \n                            Rules:\n                                - Ensure the output is valid JSON (parseable).\n                                - "eventS" must always be an array (can be empty).\n                                - Multiple instances of the same event type appear as individual elements in the event array.\n                                - Events appear in the array in the same order in which they appear in the text.\n                                - Do not include extra keys, comments, or text.\n                                - Each object in "events" must contain "event_type", "text_quote", and "attributes".\n                                -If an event attribute type has no value mentioned, return "attributes": {"&lt; attribute name &gt;:Unknown"} for each attribute type defined for the event type \n                        \n                        \n                        \n                        ', 'event_detection_time': 17.639792390997172}</t>
+          <t>["sats dropped to high 80's when sleeping", 'had guaiac - bm and voided', 'had guaiac - bm and voided', 'emotionally support patient and family', 'nas diet, bs present', 'c/o sob when lying flat']</t>
         </is>
       </c>
       <c r="J14" t="inlineStr">
         <is>
-          <t>['Sleep', 'Excretion', 'Excretion', 'Family', 'Eating', 'Pain', 'Sleep']</t>
+          <t>[[]]</t>
         </is>
       </c>
       <c r="K14" t="inlineStr">
         <is>
-          <t>[{'Sleep': {'quality': 'poor', 'duration': 'Unknown', 'negation': False, 'time': 'when sleeping', 'caused_by': 'Unknown'}}, {'Excretion': {'type': 'stool', 'frequency': 'Unknown', 'quality': 'Unknown', 'negation': False, 'time': 'Unknown', 'caused_by': 'Unknown'}}, {'Excretion': {'type': 'urine', 'frequency': 'Unknown', 'quality': 'Unknown', 'negation': False, 'time': 'Unknown', 'caused_by': 'Unknown'}}, {'Family': {'interaction': 'communication', 'relation': 'Unknown', 'negation': False, 'time': 'Unknown', 'caused_by': 'Unknown'}}, {'Eating': {'food': 'Unknown', 'amount': 'Unknown', 'method': 'oral', 'negation': False, 'time': 'Unknown', 'caused_by': 'Unknown'}}, {'Pain': {'severity': 'Unknown', 'location': 'chest', 'duration': 'Unknown', 'negation': False, 'time': 'when lying flat', 'caused_by': 'Unknown'}}, {'Sleep': {'quality': 'good', 'duration': 'Unknown', 'negation': False, 'time': 'when awake', 'caused_by': 'Unknown'}}]</t>
+          <t>{'text': 'nursing progress note [**2085**]-2300\ns: "my breathing feels better when i sit up"\n\no: please see carevue for complete objective data.\n\n39 year old female admitted for cardiomyopathy and heart failure. ef-15%.\n\nnsr with freq pvc\'s, no runs of vt since admission. diastolic blood pressure 110-120\'s, started on carvedilol 6.25. heparin sc. pulses palp, no c/o cp. k-6.1, hemolyzed, repeat pending. echo done.\n\nlung clr with rales in bases. c/o sob when lying flat. sats 95 when awake, dropped to high 80\'s when sleeping. placed on 2l nc, sats in mid 90\'s. had cxr.\n\nnas diet, bs present, had guaiac - bm and voided. placed foley and gave lasix 20mg iv. patient on 1500cc fluid restriction.\n\nafebrile, wbc-10.4. 2 piv\'s.\n\nmonitor uo and fluid restriction. monitor response to cardiac meds. follow up c labs and tests. emotionally support patient and family.\n\n\n\n\n\n\n', 'event': ['Sleep', 'Excretion', 'Excretion', 'Family', 'Eating', 'Pain'], 'event_id': ['e1', 'e2', 'e3', 'e4', 'e5', 'e6'], 'phrase': '', 'raw_output': '{\n  "events": [\n    {\n      "event_id": "e1",\n      "event_type": "Sleep",\n      "text_quote": "sats dropped to high 80\'s when sleeping",\n      "attributes": {\n        "quality": "Unknown",\n        "duration": "Unknown",\n        "negation": false,\n        "time": "when sleeping",\n        "caused_by": "Unknown"\n      }\n    },\n    {\n      "event_id": "e2",\n      "event_type": "Excretion",\n      "text_quote": "had guaiac - bm and voided",\n      "attributes": {\n        "type": "stool",\n        "frequency": "Unknown",\n        "quality": "Unknown",\n        "negation": false,\n        "time": "Unknown",\n        "caused_by": "Unknown"\n      }\n    },\n    {\n      "event_id": "e3",\n      "event_type": "Excretion",\n      "text_quote": "had guaiac - bm and voided",\n      "attributes": {\n        "type": "urine",\n        "frequency": "Unknown",\n        "quality": "Unknown",\n        "negation": false,\n        "time": "Unknown",\n        "caused_by": "Unknown"\n      }\n    },\n    {\n      "event_id": "e4",\n      "event_type": "Family",\n      "text_quote": "emotionally support patient and family",\n      "attributes": {\n        "interaction": "Unknown",\n        "relation": "Unknown",\n        "negation": false,\n        "time": "Unknown",\n        "caused_by": "Unknown"\n      }\n    },\n    {\n      "event_id": "e5",\n      "event_type": "Eating",\n      "text_quote": "nas diet, bs present",\n      "attributes": {\n        "food": "Unknown",\n        "amount": "Unknown",\n        "method": "oral",\n        "negation": false,\n        "time": "Unknown",\n        "caused_by": "Unknown"\n      }\n    },\n    {\n      "event_id": "e6",\n      "event_type": "Pain",\n      "text_quote": "c/o sob when lying flat",\n      "attributes": {\n        "severity": "Unknown",\n        "location": "chest",\n        "duration": "Unknown",\n        "negation": false,\n        "time": "when lying flat",\n        "caused_by": "Unknown"\n      }\n    }\n  ],\n  "order": [\n    ["e1", "before", "e2"],\n    ["e2", "simultaneous", "e3"],\n    ["e3", "after", "e4"],\n    ["e4", "after", "e5"],\n    ["e5", "after", "e6"]\n  ]\n}', 'attributes': [{'Sleep': {'quality': 'Unknown', 'duration': 'Unknown', 'negation': False, 'time': 'when sleeping', 'caused_by': 'Unknown'}}, {'Excretion': {'type': 'stool', 'frequency': 'Unknown', 'quality': 'Unknown', 'negation': False, 'time': 'Unknown', 'caused_by': 'Unknown'}}, {'Excretion': {'type': 'urine', 'frequency': 'Unknown', 'quality': 'Unknown', 'negation': False, 'time': 'Unknown', 'caused_by': 'Unknown'}}, {'Family': {'interaction': 'Unknown', 'relation': 'Unknown', 'negation': False, 'time': 'Unknown', 'caused_by': 'Unknown'}}, {'Eating': {'food': 'Unknown', 'amount': 'Unknown', 'method': 'oral', 'negation': False, 'time': 'Unknown', 'caused_by': 'Unknown'}}, {'Pain': {'severity': 'Unknown', 'location': 'chest', 'duration': 'Unknown', 'negation': False, 'time': 'when lying flat', 'caused_by': 'Unknown'}}], 'orders': [[['e1', 'before', 'e2'], ['e2', 'simultaneous', 'e3'], ['e3', 'after', 'e4'], ['e4', 'after', 'e5'], ['e5', 'after', 'e6']]], 'text_quotes': ["sats dropped to high 80's when sleeping", 'had guaiac - bm and voided', 'had guaiac - bm and voided', 'emotionally support patient and family', 'nas diet, bs present', 'c/o sob when lying flat'], 'event_name_prompt': 'Given the text: nursing progress note [**2085**]-2300\ns: "my breathing feels better when i sit up"\n\no: please see carevue for complete objective data.\n\n39 year old female admitted for cardiomyopathy and heart failure. ef-15%.\n\nnsr with freq pvc\'s, no runs of vt since admission. diastolic blood pressure 110-120\'s, started on carvedilol 6.25. heparin sc. pulses palp, no c/o cp. k-6.1, hemolyzed, repeat pending. echo done.\n\nlung clr with rales in bases. c/o sob when lying flat. sats 95 when awake, dropped to high 80\'s when sleeping. placed on 2l nc, sats in mid 90\'s. had cxr.\n\nnas diet, bs present, had guaiac - bm and voided. placed foley and gave lasix 20mg iv. patient on 1500cc fluid restriction.\n\nafebrile, wbc-10.4. 2 piv\'s.\n\nmonitor uo and fluid restriction. monitor response to cardiac meds. follow up c labs and tests. emotionally support patient and family.\n\n\n\n\n\n\n, \n                        and the following event types with their definitions: Eating : The patient takes food into their body by mouth.\nExcretion : The patient discharges waste matter from their body.\nFamily : The patient has a visit, call, or communication with a family member.\nPain : The patient reports or shows signs of pain.\nSleep : The patient sleeps or the sleep’s quality or quantity is described.\nUnknown : choose "Unknown" if none of the other event type are applicable. \n                        ---\n                        Your task:\n                        0. Identify ALL events in the text (zero, one, or more).\n1. For each event, assign an event_type from the list above.\n2. If multiple event of same type is mentioned, assign the event_type multiple times\n3. Extract attributes for each event using ONLY the allowed attributes listed below.\n4. Use keyword evidence (Ki) ONLY if it is consistent with the text context.\n5. Output strictly valid JSON following the schema below.\n                        ---\n                        Classification Rules:\n                        - A text may contain multiple events of the same or different types.\n- Create a separate event object for each event mention.\n- If the text is explicitly a NEGATION (e.g., "denies pain"), do not extract that event.\n- If the text describes a FUTURE or HYPOTHETICAL event (e.g., "will eat tomorrow"), ignore it.\n- A valid event should have occurred in the recent past or is occurring during the time of writing of the text.\n- If no events are found or if unsure, return {"events": []}\n                        \n                        ---\n                                    Attributes allowed:\n                                    {\'Eating\': {\'food\': \'&lt;string&gt; # e.g., pancakes, porridge, etc.\', \'amount\': \'&lt;string&gt; # e.g., 1, 2 bowls, etc.\', \'method\': \'&lt;string&gt;  # e.g., oral, tube, etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, evening etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}, \'Excretion\': {\'type\': \'&lt;string&gt; # e.g., urine, stool, etc.\', \'frequency\': \'&lt;string&gt; # e.g., 2x, once, etc.\', \'quality\': \'&lt;string&gt; # e.g., loose, hard, etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, evening etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}, \'Family\': {\'interaction\': \'&lt;string&gt; # e.g., visit, call, communication, etc.\', \'relation\': \'&lt;string&gt; # e.g., mother, son, etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, evening etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}, \'Pain\': {\'severity\': \'&lt;string&gt; # e.g., mild, moderate, severe, numeric scale if present, etc.\', \'location\': \'&lt;string&gt; # e.g., right knee, head, etc.\', \'duration\': \'&lt;string&gt; # e.g., all night, 3 hours, etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, evening etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}, \'Sleep\': {\'quality\': \'&lt;string&gt; # e.g., good, poor, restless, etc.\', \'duration\': \'&lt;string&gt; # e.g., 6 hours, phrases like "all night", etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, evening etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}}\n                                    If no relevant attribute exists for an event, return an empty object {}.\n                                    \n                        \n                        ---\n                                    Keyword evidence (Ki):\n                                    Additional facts: A keyword matching algorithm without context detected keyword(s) (\'family\', \'sleeping\').\n                                    Use this only as a pointer. If context contradicts, ignore.\n                        ---\n                        Output Schema (strict):\n                        {\n                                    "events": [\n                                        {\n                                        "event_id": "&lt; A unique id eg.: e1 | e2 |...&gt;"\n                                        "event_type": "&lt;Pain | Sleep | Excretion | Eating | Family&gt;",\n                                        "text_quote": "&lt;fragement from the text indicating the event_type&gt;",\n                "attributes": {\n                    "&lt;attribute_name&gt;": "&lt;attribute_value&gt;"\n                }\n                                        }\n                                    ],\n                                    "order": [\n                                        ["e1", "before" | "after" | "simultaneous", "e2" ]\n                                    ]\n                                    }\n                        \n                            Rules:\n                                - Ensure the output is valid JSON (parseable).\n                                - "eventS" must always be an array (can be empty).\n                                - Multiple instances of the same event type appear with different ids.\n                                - Events appear in the array in the same order in which they appear in the text.\n                                - Their partial orders can be expressed using the "order" section.\n                                - Do not include extra keys, comments, or text.\n                                - Each object in "events" must contain "event_type", "text_quote", and "attributes".\n                                - If an event attribute type has no value mentioned, return "attributes": {"&lt; attribute name &gt;:Unknown"} for each attribute type defined for the event type \n                        \n                        \n                        \n                        ', 'event_detection_time': 18.958092350978404}</t>
         </is>
       </c>
       <c r="L14" t="inlineStr">
         <is>
-          <t>["sats dropped to high 80's when sleeping", 'had guaiac - bm and voided', 'had guaiac - bm and voided', 'emotionally support patient and family', 'nas diet, bs present', 'c/o sob when lying flat', "sats 95 when awake, dropped to high 80's when sleeping"]</t>
+          <t>['Sleep', 'Excretion', 'Excretion', 'Family', 'Eating', 'Pain']</t>
         </is>
       </c>
       <c r="M14" t="inlineStr">
         <is>
-          <t>{'text': 'nursing progress note [**2085**]-2300\ns: "my breathing feels better when i sit up"\n\no: please see carevue for complete objective data.\n\n39 year old female admitted for cardiomyopathy and heart failure. ef-15%.\n\nnsr with freq pvc\'s, no runs of vt since admission. diastolic blood pressure 110-120\'s, started on carvedilol 6.25. heparin sc. pulses palp, no c/o cp. k-6.1, hemolyzed, repeat pending. echo done.\n\nlung clr with rales in bases. c/o sob when lying flat. sats 95 when awake, dropped to high 80\'s when sleeping. placed on 2l nc, sats in mid 90\'s. had cxr.\n\nnas diet, bs present, had guaiac - bm and voided. placed foley and gave lasix 20mg iv. patient on 1500cc fluid restriction.\n\nafebrile, wbc-10.4. 2 piv\'s.\n\nmonitor uo and fluid restriction. monitor response to cardiac meds. follow up c labs and tests. emotionally support patient and family.\n\n\n\n\n\n\n', 'event': ['Sleep', 'Excretion', 'Excretion', 'Eating', 'Family', 'Pain', 'Sleep'], 'phrase': '', 'raw_output': '{\n  "events": [\n    {\n      "event_type": "Sleep",\n      "text_quote": "sats dropped to high 80\'s when sleeping",\n      "attributes": {\n        "quality": "poor",\n        "duration": "Unknown",\n        "time": "Unknown",\n        "caused_by": "Unknown"\n      }\n    },\n    {\n      "event_type": "Excretion",\n      "text_quote": "had guaiac - bm and voided",\n      "attributes": {\n        "type": "stool",\n        "frequency": "Unknown",\n        "quality": "Unknown",\n        "negation": "false",\n        "time": "Unknown",\n        "caused_by": "Unknown"\n      }\n    },\n    {\n      "event_type": "Excretion",\n      "text_quote": "had guaiac - bm and voided",\n      "attributes": {\n        "type": "urine",\n        "frequency": "Unknown",\n        "quality": "Unknown",\n        "negation": "false",\n        "time": "Unknown",\n        "caused_by": "Unknown"\n      }\n    },\n    {\n      "event_type": "Eating",\n      "text_quote": "nas diet, bs present",\n      "attributes": {\n        "food": "Unknown",\n        "amount": "Unknown",\n        "method": "oral",\n        "negation": "false",\n        "time": "Unknown",\n        "caused_by": "Unknown"\n      }\n    },\n    {\n      "event_type": "Family",\n      "text_quote": "emotionally support patient and family",\n      "attributes": {\n        "interaction": "support",\n        "relation": "family",\n        "negation": "false",\n        "time": "Unknown",\n        "caused_by": "Unknown"\n      }\n    },\n    {\n      "event_type": "Pain",\n      "text_quote": "c/o sob when lying flat",\n      "attributes": {\n        "severity": "Unknown",\n        "location": "chest",\n        "duration": "Unknown",\n        "negation": "false",\n        "time": "when lying flat",\n        "caused_by": "Unknown"\n      }\n    },\n    {\n      "event_type": "Sleep",\n      "text_quote": "sats 95 when awake, dropped to high 80\'s when sleeping",\n      "attributes": {\n        "quality": "good",\n        "duration": "Unknown",\n        "negation": "false",\n        "time": "when awake",\n        "caused_by": "Unknown"\n      }\n    }\n  ]\n}', 'attributes': [{'Sleep': {'quality': 'poor', 'duration': 'Unknown', 'time': 'Unknown', 'caused_by': 'Unknown'}}, {'Excretion': {'type': 'stool', 'frequency': 'Unknown', 'quality': 'Unknown', 'negation': 'false', 'time': 'Unknown', 'caused_by': 'Unknown'}}, {'Excretion': {'type': 'urine', 'frequency': 'Unknown', 'quality': 'Unknown', 'negation': 'false', 'time': 'Unknown', 'caused_by': 'Unknown'}}, {'Eating': {'food': 'Unknown', 'amount': 'Unknown', 'method': 'oral', 'negation': 'false', 'time': 'Unknown', 'caused_by': 'Unknown'}}, {'Family': {'interaction': 'support', 'relation': 'family', 'negation': 'false', 'time': 'Unknown', 'caused_by': 'Unknown'}}, {'Pain': {'severity': 'Unknown', 'location': 'chest', 'duration': 'Unknown', 'negation': 'false', 'time': 'when lying flat', 'caused_by': 'Unknown'}}, {'Sleep': {'quality': 'good', 'duration': 'Unknown', 'negation': 'false', 'time': 'when awake', 'caused_by': 'Unknown'}}], 'text_quotes': ["sats dropped to high 80's when sleeping", 'had guaiac - bm and voided', 'had guaiac - bm and voided', 'nas diet, bs present', 'emotionally support patient and family', 'c/o sob when lying flat', "sats 95 when awake, dropped to high 80's when sleeping"], 'event_name_prompt': 'Given the text: nursing progress note [**2085**]-2300\ns: "my breathing feels better when i sit up"\n\no: please see carevue for complete objective data.\n\n39 year old female admitted for cardiomyopathy and heart failure. ef-15%.\n\nnsr with freq pvc\'s, no runs of vt since admission. diastolic blood pressure 110-120\'s, started on carvedilol 6.25. heparin sc. pulses palp, no c/o cp. k-6.1, hemolyzed, repeat pending. echo done.\n\nlung clr with rales in bases. c/o sob when lying flat. sats 95 when awake, dropped to high 80\'s when sleeping. placed on 2l nc, sats in mid 90\'s. had cxr.\n\nnas diet, bs present, had guaiac - bm and voided. placed foley and gave lasix 20mg iv. patient on 1500cc fluid restriction.\n\nafebrile, wbc-10.4. 2 piv\'s.\n\nmonitor uo and fluid restriction. monitor response to cardiac meds. follow up c labs and tests. emotionally support patient and family.\n\n\n\n\n\n\n, \n                        and the following event types with their definitions: Eating : The patient takes food into their body by mouth.\nExcretion : The patient discharges waste matter from their body.\nFamily : The patient has a visit, call, or communication with a family member.\nPain : The patient reports or shows signs of pain.\nSleep : The patient sleeps or the sleep’s quality or quantity is described.\nUnknown : choose "Unknown" if none of the other event type are applicable. \n                        ---\n                        Your task:\n                        0. Identify ALL events in the text (zero, one, or more).\n1. For each event, assign an event_type from the list above.\n2. If multiple event of same type is mentioned, assign the event_type multiple times\n3. Extract attributes for each event using ONLY the allowed attributes listed below.\n4. Output strictly valid JSON following the schema below.\n                        ---\n                        Classification Rules:\n                        - A text may contain multiple events of the same or different types.\n- Create a separate event object for each event mention.\n- If the text is explicitly a NEGATION (e.g., "denies pain"), do not extract that event.\n- If the text describes a FUTURE or HYPOTHETICAL event (e.g., "will eat tomorrow"), ignore it.\n- A valid event should have occurred in the recent past or is occurring during the time of writing of the text.\n- If no events are found or if unsure, return {"events": []}\n                        \n                        ---\n                                    Attributes allowed:\n                                    {\'Eating\': {\'food\': \'&lt;string&gt; # e.g., pancakes, porridge, etc.\', \'amount\': \'&lt;string&gt; # e.g., 1, 2 bowls, etc.\', \'method\': \'&lt;string&gt;  # e.g., oral, tube, etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, after shower, etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}, \'Excretion\': {\'type\': \'&lt;string&gt; # e.g., urine, stool, etc.\', \'frequency\': \'&lt;string&gt; # e.g., 2x, once, etc.\', \'quality\': \'&lt;string&gt; # e.g., loose, hard, etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, after shower, etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}, \'Family\': {\'interaction\': \'&lt;string&gt; # e.g., visit, call, communication, etc.\', \'relation\': \'&lt;string&gt; # e.g., mother, son, etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, after shower, etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}, \'Pain\': {\'severity\': \'&lt;string&gt; # e.g., mild, moderate, severe, numeric scale if present, etc.\', \'location\': \'&lt;string&gt; # e.g., right knee, head, etc.\', \'duration\': \'&lt;string&gt; # e.g., all night, 3 hours, etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, after shower, etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}, \'Sleep\': {\'quality\': \'&lt;string&gt; # e.g., good, poor, restless, etc.\', \'duration\': \'&lt;string&gt; # e.g., 6 hours, phrases like "all night", etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, after shower, etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}}\n                                    If no relevant attribute exists for an event, return an empty object {}.\n                                    \n                        \n                        \n                        ---\n                        Output Schema (strict):\n                        {\n                                    "events": [\n                                        {\n                                        "event_type": "&lt;Pain | Sleep | Excretion | Eating | Family&gt;",\n                                        "text_quote": "&lt;fragement from the text indicating &gt;",\n                "attributes": {\n                    "&lt;attribute_name&gt;": "&lt;attribute_value&gt;"\n                }\n                                        }\n                                    ]\n                                    }\n                        \n                            Rules:\n                                - Ensure the output is valid JSON (parseable).\n                                - "eventS" must always be an array (can be empty).\n                                - Multiple instances of the same event type appear as individual elements in the event array.\n                                - Events appear in the array in the same order in which they appear in the text.\n                                - Do not include extra keys, comments, or text.\n                                - Each object in "events" must contain "event_type", "text_quote", and "attributes".\n                                -If an event attribute type has no value mentioned, return "attributes": {"&lt; attribute name &gt;:Unknown"} for each attribute type defined for the event type \n                        \n                        \n                        \n                ---\n                Examples:\n                \n                text: "Patient ate breakfast this morning. He seems less anxious."\n                output: {\n                "events": [\n                    {\n                    "event_type": "Eating",\n                    "text_quote":"Patient ate breakfast this morning",\n                    "attributes": {"food": "breakfast", \n                                   "amount": "Unknown",\n                                   "method": "Unknown",\n                                   "time":"morning",\n                                   "caused_by":"Unknown"}\n                    }\n                ]\n                }\n                \n                text: "Patient reported severe abdominal pain."\n                output: {\n                "events": [\n                    {\n                    "event_type": "Pain",\n                    "text_quote": "severe abdominal Pain",\n                    "attributes": {"severity": "severe", \n                                   "location": "abdominal",\n                                   "duration": "Unknown",\n                                   "time":"Unknown",\n                                   "caused_by":"Unknown"}\n                    }\n                ]\n                }\n                \n                text: "Patient called his son around 3 pm."\n                output: {\n                "events": [\n                    {\n                    "event_type": "Family",\n                    "text_quote": "called his son around 3 pm",\n                    "attributes": {"interaction": "call", \n                                    "relation": "son",\n                                    "time":"3 pm",\n                                    "caused_by":"Unknown"}\n                    }\n                ]\n                }\n                \n                text: "Patient had a loose stool overnight."\n                output: {\n                "events": [\n                    {\n                    "event_type": "Excretion",\n                    "text_quote": "loose stool overnight",\n                    "attributes": {"type": "stool", \n                                   "quality": "loose", \n                                   "frequency":"overnight", \n                                   "time":"night",\n                                   "caused_by":"Unknown"}\n                    }\n                ]\n                }\n                \n                text: "Patient was able to sleep well last night."\n                output: {\n                "events": [\n                    {\n                    "event_type": "Sleep",\n                    "text_quote": "sleep well last night",\n                    "attributes": {"quality": "well",\n                                    "duration": "Unknown", \n                                    "time":"night",\n                                    "caused_by":"Unknown"}\n                    }\n                ]\n                }\n                \n                text: "The patient couldn\'t sleep due to severe pain."\n                output: {\n                "events": [\n                    {\n                    "event_type": "Sleep",\n                    "text_quote": "couldn\'t sleep",\n                    "attributes": {"quality": "poor", \n                                    "duration": "Unknown",\n                                   "time":"Unknown",\n                                   "caused_by":"Pain"}\n                    },\n                    {\n                    "event_type": "Pain",\n                    "text_quote": "severe pain",\n                    "attributes": {"severity": "severe", \n                                    "location": "Unknown", \n                                    "duration": "Unknown", \n                                   "time":"before Sleep",\n                                   "caused_by":"Unknown"}\n                    }\n                ]\n                }\n                \n                text: "The patient complained of severe back pain, was given Tylenol, but the pain persisted and he was then prescribed stronger morphine."\n                output: {\n                "events": [\n                    {\n                    "event_type": "Pain",\n                    "text_quote": "complained of severe back pain",\n                    "attributes": {"severity": "severe", \n                                    "location": "back",\n                                    "duration": "Unknown", \n                                    "time":"Unknown",\n                                    "caused_by":"Unknown"}\n                    },\n                    {\n                    "event_type": "Pain",\n                    "text_quote": "pain persisted",\n                    "attributes": {"severity": "severe", \n                                   "location": "back",\n                                   "duration": "persistent", \n                                   "time":"after Tylenol",\n                                   "caused_by":"Unknown"}\n                    }\n                ]\n                }\n                \n                        ', 'event_detection_time': 18.352297778998036}</t>
+          <t>[{'Sleep': {'quality': 'Unknown', 'duration': 'Unknown', 'negation': False, 'time': 'when sleeping', 'caused_by': 'Unknown'}}, {'Excretion': {'type': 'stool', 'frequency': 'Unknown', 'quality': 'Unknown', 'negation': False, 'time': 'Unknown', 'caused_by': 'Unknown'}}, {'Excretion': {'type': 'urine', 'frequency': 'Unknown', 'quality': 'Unknown', 'negation': False, 'time': 'Unknown', 'caused_by': 'Unknown'}}, {'Family': {'interaction': 'Unknown', 'relation': 'Unknown', 'negation': False, 'time': 'Unknown', 'caused_by': 'Unknown'}}, {'Eating': {'food': 'Unknown', 'amount': 'Unknown', 'method': 'oral', 'negation': False, 'time': 'Unknown', 'caused_by': 'Unknown'}}, {'Pain': {'severity': 'Unknown', 'location': 'chest', 'duration': 'Unknown', 'negation': False, 'time': 'when lying flat', 'caused_by': 'Unknown'}}]</t>
         </is>
       </c>
       <c r="N14" t="inlineStr">
         <is>
-          <t>['Sleep', 'Excretion', 'Excretion', 'Eating', 'Family', 'Pain', 'Sleep']</t>
+          <t>["sats dropped to high 80's when sleeping", 'had guaiac - bm and voided', 'had guaiac - bm and voided', 'emotionally support patient and family', 'nas diet, bs present', 'c/o sob when lying flat']</t>
         </is>
       </c>
       <c r="O14" t="inlineStr">
         <is>
-          <t>[{'Sleep': {'quality': 'poor', 'duration': 'Unknown', 'time': 'Unknown', 'caused_by': 'Unknown'}}, {'Excretion': {'type': 'stool', 'frequency': 'Unknown', 'quality': 'Unknown', 'negation': 'false', 'time': 'Unknown', 'caused_by': 'Unknown'}}, {'Excretion': {'type': 'urine', 'frequency': 'Unknown', 'quality': 'Unknown', 'negation': 'false', 'time': 'Unknown', 'caused_by': 'Unknown'}}, {'Eating': {'food': 'Unknown', 'amount': 'Unknown', 'method': 'oral', 'negation': 'false', 'time': 'Unknown', 'caused_by': 'Unknown'}}, {'Family': {'interaction': 'support', 'relation': 'family', 'negation': 'false', 'time': 'Unknown', 'caused_by': 'Unknown'}}, {'Pain': {'severity': 'Unknown', 'location': 'chest', 'duration': 'Unknown', 'negation': 'false', 'time': 'when lying flat', 'caused_by': 'Unknown'}}, {'Sleep': {'quality': 'good', 'duration': 'Unknown', 'negation': 'false', 'time': 'when awake', 'caused_by': 'Unknown'}}]</t>
-        </is>
-      </c>
-      <c r="P14" t="inlineStr">
-        <is>
-          <t>["sats dropped to high 80's when sleeping", 'had guaiac - bm and voided', 'had guaiac - bm and voided', 'nas diet, bs present', 'emotionally support patient and family', 'c/o sob when lying flat', "sats 95 when awake, dropped to high 80's when sleeping"]</t>
-        </is>
-      </c>
-      <c r="Q14" t="inlineStr"/>
-      <c r="R14" t="inlineStr">
+          <t>[[['e1', 'before', 'e2'], ['e2', 'simultaneous', 'e3'], ['e3', 'after', 'e4'], ['e4', 'after', 'e5'], ['e5', 'after', 'e6']]]</t>
+        </is>
+      </c>
+      <c r="P14" t="n">
+        <v>2.246000804007053e-06</v>
+      </c>
+      <c r="Q14" t="inlineStr">
         <is>
           <t>Sleep</t>
         </is>
       </c>
-      <c r="S14" t="b">
-        <v>0</v>
+      <c r="R14" t="b">
+        <v>0</v>
+      </c>
+      <c r="S14" t="n">
+        <v>1</v>
       </c>
       <c r="T14" t="n">
         <v>1</v>
       </c>
-      <c r="U14" t="n">
-        <v>1</v>
-      </c>
-      <c r="V14" t="inlineStr">
+      <c r="U14" t="inlineStr">
         <is>
           <t>('family', 'sleeping')</t>
         </is>
       </c>
+      <c r="V14" t="n">
+        <v>18.33578487095656</v>
+      </c>
       <c r="W14" t="n">
-        <v>20.91716979599732</v>
+        <v>18.9580923509784</v>
       </c>
       <c r="X14" t="n">
-        <v>17.63979239099717</v>
+        <v>1</v>
       </c>
       <c r="Y14" t="n">
-        <v>18.35229777899804</v>
+        <v>1</v>
       </c>
       <c r="Z14" t="n">
-        <v>1</v>
-      </c>
-      <c r="AA14" t="n">
-        <v>1</v>
-      </c>
-      <c r="AB14" t="n">
-        <v>1</v>
-      </c>
-      <c r="AC14" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="15">
-      <c r="A15" t="n">
-        <v>1325548</v>
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>1325548</t>
+        </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>['Sleep', 'Pain', 'Family', 'Unknown']</t>
+          <t>('Family', 'Sleep', 'Pain', 'Unknown')</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>['slept', 'husband', 'pain']</t>
+          <t>('pain', 'husband', 'slept')</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
@@ -2364,120 +2238,111 @@
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>{'text': "39 year old female history of coughing past few weeks. patient was found to have cardiomyopathy and is in heart failure. patient was taking coreg 3.125mg [**hospital1 **] and lasix 40 mg qd at home. patient was tolerating by mouth meds until [**6-12**] a.male. she felt weak and dizzy. patient ef was 15%. ? cardiomyopathy from viral illness diagnosed on [**6-8**]. pts husband is a nurse [**first name (titles) 14**] [**last name (titles) 2**] he requested patient be transferred here from [**hospital 1227**] hosp.\n\ncv:nsr/st c freq/occa pvc's. patient has 5 runs of vt each with 8-10 beats of vt. patient received her captopril 6.25mg at 2200 and received lasix 20mg at 2200 and since has had very low bp in the 80's. beta blocker has been on hold until bp maps are greater than 65. maps now 64. heart rate 104-80. hct 42.2, k 4.3. small pericardial effusion and sever global vent hypokinesis found on echo.\n\nresp: patient has nonproductive cough for past few weeks. patient has benzonatate ordered for coughing patient received one this a.male and it helped with her coughing. patient ls coarse at bases. no o2 maintaining oxygen saturation of 97%. sob with exertion.\n\nneuro:patient has a history of depression and patient does appear sad. patient is alert and oriented x3. patient lives at [**location 10814**] with husband and two children. patient has complained that she hasnt slept in days.\n\ngu:patient tolerating sips of water. bs +, + bm guaic -.\n\ngi:1500cc a day fluid restriction. patient responded well to lasix -600cc.\n\na:39yo female with new onset of cardiomyopathy witha ef of 15%.\n\np: patient [**month (only) 108**] need cardiaccath to evaluate coronary arteries. fluid restriction. keep pain free patient was taking percocet for chest pain at home. emotional support.\n", 'event': ['Pain', 'Sleep', 'Family', 'Excretion', 'Eating'], 'phrase': '', 'raw_output': '{\n  "events": [\n    {\n      "event_type": "Pain",\n      "text_quote": "chest pain at home",\n      "attributes": {\n        "severity": "Unknown",\n        "location": "chest",\n        "duration": "Unknown",\n        "time": "at home",\n        "caused_by": "Unknown"\n      }\n    },\n    {\n      "event_type": "Sleep",\n      "text_quote": "she hasn\'t slept in days",\n      "attributes": {\n        "quality": "poor",\n        "duration": "days",\n        "time": "Unknown",\n        "caused_by": "Unknown"\n      }\n    },\n    {\n      "event_type": "Family",\n      "text_quote": "pts husband is a nurse",\n      "attributes": {\n        "interaction": "Unknown",\n        "relation": "husband",\n        "negation": "false",\n        "time": "Unknown",\n        "caused_by": "Unknown"\n      }\n    },\n    {\n      "event_type": "Excretion",\n      "text_quote": "+ bm guaic -",\n      "attributes": {\n        "type": "stool",\n        "frequency": "Unknown",\n        "quality": "Unknown",\n        "negation": "false",\n        "time": "Unknown",\n        "caused_by": "Unknown"\n      }\n    },\n    {\n      "event_type": "Eating",\n      "text_quote": "patient tolerating sips of water",\n      "attributes": {\n        "food": "water",\n        "amount": "sips",\n        "method": "oral",\n        "negation": "false",\n        "time": "Unknown",\n        "caused_by": "Unknown"\n      }\n    }\n  ]\n}', 'attributes': [{'Pain': {'severity': 'Unknown', 'location': 'chest', 'duration': 'Unknown', 'time': 'at home', 'caused_by': 'Unknown'}}, {'Sleep': {'quality': 'poor', 'duration': 'days', 'time': 'Unknown', 'caused_by': 'Unknown'}}, {'Family': {'interaction': 'Unknown', 'relation': 'husband', 'negation': 'false', 'time': 'Unknown', 'caused_by': 'Unknown'}}, {'Excretion': {'type': 'stool', 'frequency': 'Unknown', 'quality': 'Unknown', 'negation': 'false', 'time': 'Unknown', 'caused_by': 'Unknown'}}, {'Eating': {'food': 'water', 'amount': 'sips', 'method': 'oral', 'negation': 'false', 'time': 'Unknown', 'caused_by': 'Unknown'}}], 'text_quotes': ['chest pain at home', "she hasn't slept in days", 'pts husband is a nurse', '+ bm guaic -', 'patient tolerating sips of water'], 'event_name_prompt': 'Given the text: 39 year old female history of coughing past few weeks. patient was found to have cardiomyopathy and is in heart failure. patient was taking coreg 3.125mg [**hospital1 **] and lasix 40 mg qd at home. patient was tolerating by mouth meds until [**6-12**] a.male. she felt weak and dizzy. patient ef was 15%. ? cardiomyopathy from viral illness diagnosed on [**6-8**]. pts husband is a nurse [**first name (titles) 14**] [**last name (titles) 2**] he requested patient be transferred here from [**hospital 1227**] hosp.\n\ncv:nsr/st c freq/occa pvc\'s. patient has 5 runs of vt each with 8-10 beats of vt. patient received her captopril 6.25mg at 2200 and received lasix 20mg at 2200 and since has had very low bp in the 80\'s. beta blocker has been on hold until bp maps are greater than 65. maps now 64. heart rate 104-80. hct 42.2, k 4.3. small pericardial effusion and sever global vent hypokinesis found on echo.\n\nresp: patient has nonproductive cough for past few weeks. patient has benzonatate ordered for coughing patient received one this a.male and it helped with her coughing. patient ls coarse at bases. no o2 maintaining oxygen saturation of 97%. sob with exertion.\n\nneuro:patient has a history of depression and patient does appear sad. patient is alert and oriented x3. patient lives at [**location 10814**] with husband and two children. patient has complained that she hasnt slept in days.\n\ngu:patient tolerating sips of water. bs +, + bm guaic -.\n\ngi:1500cc a day fluid restriction. patient responded well to lasix -600cc.\n\na:39yo female with new onset of cardiomyopathy witha ef of 15%.\n\np: patient [**month (only) 108**] need cardiaccath to evaluate coronary arteries. fluid restriction. keep pain free patient was taking percocet for chest pain at home. emotional support.\n, \n                        and the following event types with their definitions: Eating : The patient takes food into their body by mouth.\nExcretion : The patient discharges waste matter from their body.\nFamily : The patient has a visit, call, or communication with a family member.\nPain : The patient reports or shows signs of pain.\nSleep : The patient sleeps or the sleep’s quality or quantity is described.\nUnknown : choose "Unknown" if none of the other event type are applicable. \n                        ---\n                        Your task:\n                        0. Identify ALL events in the text (zero, one, or more).\n1. For each event, assign an event_type from the list above.\n2. If multiple event of same type is mentioned, assign the event_type multiple times\n3. Extract attributes for each event using ONLY the allowed attributes listed below.\n4. Use keyword evidence (Ki) ONLY if it is consistent with the text context.\n5. Output strictly valid JSON following the schema below.\n                        ---\n                        Classification Rules:\n                        - A text may contain multiple events of the same or different types.\n- Create a separate event object for each event mention.\n- If the text is explicitly a NEGATION (e.g., "denies pain"), do not extract that event.\n- If the text describes a FUTURE or HYPOTHETICAL event (e.g., "will eat tomorrow"), ignore it.\n- A valid event should have occurred in the recent past or is occurring during the time of writing of the text.\n- If no events are found or if unsure, return {"events": []}\n                        \n                        ---\n                                    Attributes allowed:\n                                    {\'Eating\': {\'food\': \'&lt;string&gt; # e.g., pancakes, porridge, etc.\', \'amount\': \'&lt;string&gt; # e.g., 1, 2 bowls, etc.\', \'method\': \'&lt;string&gt;  # e.g., oral, tube, etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, after shower, etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}, \'Excretion\': {\'type\': \'&lt;string&gt; # e.g., urine, stool, etc.\', \'frequency\': \'&lt;string&gt; # e.g., 2x, once, etc.\', \'quality\': \'&lt;string&gt; # e.g., loose, hard, etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, after shower, etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}, \'Family\': {\'interaction\': \'&lt;string&gt; # e.g., visit, call, communication, etc.\', \'relation\': \'&lt;string&gt; # e.g., mother, son, etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, after shower, etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}, \'Pain\': {\'severity\': \'&lt;string&gt; # e.g., mild, moderate, severe, numeric scale if present, etc.\', \'location\': \'&lt;string&gt; # e.g., right knee, head, etc.\', \'duration\': \'&lt;string&gt; # e.g., all night, 3 hours, etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, after shower, etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}, \'Sleep\': {\'quality\': \'&lt;string&gt; # e.g., good, poor, restless, etc.\', \'duration\': \'&lt;string&gt; # e.g., 6 hours, phrases like "all night", etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, after shower, etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}}\n                                    If no relevant attribute exists for an event, return an empty object {}.\n                                    \n                        \n                        ---\n                                    Keyword evidence (Ki):\n                                    Additional facts: A keyword matching algorithm without context detected keyword(s) [\'slept\', \'husband\', \'pain\'].\n                                    Use this only as a pointer. If context contradicts, ignore.\n                        ---\n                        Output Schema (strict):\n                        {\n                                    "events": [\n                                        {\n                                        "event_type": "&lt;Pain | Sleep | Excretion | Eating | Family&gt;",\n                                        "text_quote": "&lt;fragement from the text indicating &gt;",\n                "attributes": {\n                    "&lt;attribute_name&gt;": "&lt;attribute_value&gt;"\n                }\n                                        }\n                                    ]\n                                    }\n                        \n                            Rules:\n                                - Ensure the output is valid JSON (parseable).\n                                - "eventS" must always be an array (can be empty).\n                                - Multiple instances of the same event type appear as individual elements in the event array.\n                                - Events appear in the array in the same order in which they appear in the text.\n                                - Do not include extra keys, comments, or text.\n                                - Each object in "events" must contain "event_type", "text_quote", and "attributes".\n                                -If an event attribute type has no value mentioned, return "attributes": {"&lt; attribute name &gt;:Unknown"} for each attribute type defined for the event type \n                        \n                        \n                        \n                ---\n                Examples:\n                \n                text: "Patient ate breakfast this morning. He seems less anxious."\n                output: {\n                "events": [\n                    {\n                    "event_type": "Eating",\n                    "text_quote":"Patient ate breakfast this morning",\n                    "attributes": {"food": "breakfast", \n                                   "amount": "Unknown",\n                                   "method": "Unknown",\n                                   "time":"morning",\n                                   "caused_by":"Unknown"}\n                    }\n                ]\n                }\n                \n                text: "Patient reported severe abdominal pain."\n                output: {\n                "events": [\n                    {\n                    "event_type": "Pain",\n                    "text_quote": "severe abdominal Pain",\n                    "attributes": {"severity": "severe", \n                                   "location": "abdominal",\n                                   "duration": "Unknown",\n                                   "time":"Unknown",\n                                   "caused_by":"Unknown"}\n                    }\n                ]\n                }\n                \n                text: "Patient called his son around 3 pm."\n                output: {\n                "events": [\n                    {\n                    "event_type": "Family",\n                    "text_quote": "called his son around 3 pm",\n                    "attributes": {"interaction": "call", \n                                    "relation": "son",\n                                    "time":"3 pm",\n                                    "caused_by":"Unknown"}\n                    }\n                ]\n                }\n                \n                text: "Patient had a loose stool overnight."\n                output: {\n                "events": [\n                    {\n                    "event_type": "Excretion",\n                    "text_quote": "loose stool overnight",\n                    "attributes": {"type": "stool", \n                                   "quality": "loose", \n                                   "frequency":"overnight", \n                                   "time":"night",\n                                   "caused_by":"Unknown"}\n                    }\n                ]\n                }\n                \n                text: "Patient was able to sleep well last night."\n                output: {\n                "events": [\n                    {\n                    "event_type": "Sleep",\n                    "text_quote": "sleep well last night",\n                    "attributes": {"quality": "well",\n                                    "duration": "Unknown", \n                                    "time":"night",\n                                    "caused_by":"Unknown"}\n                    }\n                ]\n                }\n                \n                text: "The patient couldn\'t sleep due to severe pain."\n                output: {\n                "events": [\n                    {\n                    "event_type": "Sleep",\n                    "text_quote": "couldn\'t sleep",\n                    "attributes": {"quality": "poor", \n                                    "duration": "Unknown",\n                                   "time":"Unknown",\n                                   "caused_by":"Pain"}\n                    },\n                    {\n                    "event_type": "Pain",\n                    "text_quote": "severe pain",\n                    "attributes": {"severity": "severe", \n                                    "location": "Unknown", \n                                    "duration": "Unknown", \n                                   "time":"before Sleep",\n                                   "caused_by":"Unknown"}\n                    }\n                ]\n                }\n                \n                text: "The patient complained of severe back pain, was given Tylenol, but the pain persisted and he was then prescribed stronger morphine."\n                output: {\n                "events": [\n                    {\n                    "event_type": "Pain",\n                    "text_quote": "complained of severe back pain",\n                    "attributes": {"severity": "severe", \n                                    "location": "back",\n                                    "duration": "Unknown", \n                                    "time":"Unknown",\n                                    "caused_by":"Unknown"}\n                    },\n                    {\n                    "event_type": "Pain",\n                    "text_quote": "pain persisted",\n                    "attributes": {"severity": "severe", \n                                   "location": "back",\n                                   "duration": "persistent", \n                                   "time":"after Tylenol",\n                                   "caused_by":"Unknown"}\n                    }\n                ]\n                }\n                \n                        ', 'event_detection_time': 13.499786435000715}</t>
+          <t>['pain', 'husband', 'sleep']</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
         <is>
+          <t>{'text': "39 year old female history of coughing past few weeks. patient was found to have cardiomyopathy and is in heart failure. patient was taking coreg 3.125mg [**hospital1 **] and lasix 40 mg qd at home. patient was tolerating by mouth meds until [**6-12**] a.male. she felt weak and dizzy. patient ef was 15%. ? cardiomyopathy from viral illness diagnosed on [**6-8**]. pts husband is a nurse [**first name (titles) 14**] [**last name (titles) 2**] he requested patient be transferred here from [**hospital 1227**] hosp.\n\ncv:nsr/st c freq/occa pvc's. patient has 5 runs of vt each with 8-10 beats of vt. patient received her captopril 6.25mg at 2200 and received lasix 20mg at 2200 and since has had very low bp in the 80's. beta blocker has been on hold until bp maps are greater than 65. maps now 64. heart rate 104-80. hct 42.2, k 4.3. small pericardial effusion and sever global vent hypokinesis found on echo.\n\nresp: patient has nonproductive cough for past few weeks. patient has benzonatate ordered for coughing patient received one this a.male and it helped with her coughing. patient ls coarse at bases. no o2 maintaining oxygen saturation of 97%. sob with exertion.\n\nneuro:patient has a history of depression and patient does appear sad. patient is alert and oriented x3. patient lives at [**location 10814**] with husband and two children. patient has complained that she hasnt slept in days.\n\ngu:patient tolerating sips of water. bs +, + bm guaic -.\n\ngi:1500cc a day fluid restriction. patient responded well to lasix -600cc.\n\na:39yo female with new onset of cardiomyopathy witha ef of 15%.\n\np: patient [**month (only) 108**] need cardiaccath to evaluate coronary arteries. fluid restriction. keep pain free patient was taking percocet for chest pain at home. emotional support.\n", 'event': ['Pain', 'Sleep', 'Family', 'Excretion', 'Eating'], 'event_id': ['e1', 'e2', 'e3', 'e4', 'e5'], 'phrase': '', 'raw_output': '{\n  "events": [\n    {\n      "event_id": "e1",\n      "event_type": "Pain",\n      "text_quote": "chest pain at home",\n      "attributes": {\n        "severity": "Unknown",\n        "location": "chest",\n        "duration": "Unknown",\n        "negation": "false",\n        "time": "at home",\n        "caused_by": "Unknown"\n      }\n    },\n    {\n      "event_id": "e2",\n      "event_type": "Sleep",\n      "text_quote": "she hasn\'t slept in days",\n      "attributes": {\n        "quality": "poor",\n        "duration": "days",\n        "negation": "true",\n        "time": "Unknown",\n        "caused_by": "Unknown"\n      }\n    },\n    {\n      "event_id": "e3",\n      "event_type": "Family",\n      "text_quote": "pts husband is a nurse",\n      "attributes": {\n        "interaction": "Unknown",\n        "relation": "husband",\n        "negation": "false",\n        "time": "Unknown",\n        "caused_by": "Unknown"\n      }\n    },\n    {\n      "event_id": "e4",\n      "event_type": "Excretion",\n      "text_quote": "+ bm guaic -",\n      "attributes": {\n        "type": "stool",\n        "frequency": "Unknown",\n        "quality": "Unknown",\n        "negation": "false",\n        "time": "Unknown",\n        "caused_by": "Unknown"\n      }\n    },\n    {\n      "event_id": "e5",\n      "event_type": "Eating",\n      "text_quote": "patient tolerating sips of water",\n      "attributes": {\n        "food": "water",\n        "amount": "sips",\n        "method": "oral",\n        "negation": "false",\n        "time": "Unknown",\n        "caused_by": "Unknown"\n      }\n    }\n  ],\n  "order": []\n}', 'attributes': [{'Pain': {'severity': 'Unknown', 'location': 'chest', 'duration': 'Unknown', 'negation': 'false', 'time': 'at home', 'caused_by': 'Unknown'}}, {'Sleep': {'quality': 'poor', 'duration': 'days', 'negation': 'true', 'time': 'Unknown', 'caused_by': 'Unknown'}}, {'Family': {'interaction': 'Unknown', 'relation': 'husband', 'negation': 'false', 'time': 'Unknown', 'caused_by': 'Unknown'}}, {'Excretion': {'type': 'stool', 'frequency': 'Unknown', 'quality': 'Unknown', 'negation': 'false', 'time': 'Unknown', 'caused_by': 'Unknown'}}, {'Eating': {'food': 'water', 'amount': 'sips', 'method': 'oral', 'negation': 'false', 'time': 'Unknown', 'caused_by': 'Unknown'}}], 'orders': [[]], 'text_quotes': ['chest pain at home', "she hasn't slept in days", 'pts husband is a nurse', '+ bm guaic -', 'patient tolerating sips of water'], 'event_name_prompt': 'Given the text: 39 year old female history of coughing past few weeks. patient was found to have cardiomyopathy and is in heart failure. patient was taking coreg 3.125mg [**hospital1 **] and lasix 40 mg qd at home. patient was tolerating by mouth meds until [**6-12**] a.male. she felt weak and dizzy. patient ef was 15%. ? cardiomyopathy from viral illness diagnosed on [**6-8**]. pts husband is a nurse [**first name (titles) 14**] [**last name (titles) 2**] he requested patient be transferred here from [**hospital 1227**] hosp.\n\ncv:nsr/st c freq/occa pvc\'s. patient has 5 runs of vt each with 8-10 beats of vt. patient received her captopril 6.25mg at 2200 and received lasix 20mg at 2200 and since has had very low bp in the 80\'s. beta blocker has been on hold until bp maps are greater than 65. maps now 64. heart rate 104-80. hct 42.2, k 4.3. small pericardial effusion and sever global vent hypokinesis found on echo.\n\nresp: patient has nonproductive cough for past few weeks. patient has benzonatate ordered for coughing patient received one this a.male and it helped with her coughing. patient ls coarse at bases. no o2 maintaining oxygen saturation of 97%. sob with exertion.\n\nneuro:patient has a history of depression and patient does appear sad. patient is alert and oriented x3. patient lives at [**location 10814**] with husband and two children. patient has complained that she hasnt slept in days.\n\ngu:patient tolerating sips of water. bs +, + bm guaic -.\n\ngi:1500cc a day fluid restriction. patient responded well to lasix -600cc.\n\na:39yo female with new onset of cardiomyopathy witha ef of 15%.\n\np: patient [**month (only) 108**] need cardiaccath to evaluate coronary arteries. fluid restriction. keep pain free patient was taking percocet for chest pain at home. emotional support.\n, \n                        and the following event types with their definitions: Eating : The patient takes food into their body by mouth.\nExcretion : The patient discharges waste matter from their body.\nFamily : The patient has a visit, call, or communication with a family member.\nPain : The patient reports or shows signs of pain.\nSleep : The patient sleeps or the sleep’s quality or quantity is described.\nUnknown : choose "Unknown" if none of the other event type are applicable. \n                        ---\n                        Your task:\n                        0. Identify ALL events in the text (zero, one, or more).\n1. For each event, assign an event_type from the list above.\n2. If multiple event of same type is mentioned, assign the event_type multiple times\n3. Extract attributes for each event using ONLY the allowed attributes listed below.\n4. Use keyword evidence (Ki) ONLY if it is consistent with the text context.\n5. Output strictly valid JSON following the schema below.\n                        ---\n                        Classification Rules:\n                        - A text may contain multiple events of the same or different types.\n- Create a separate event object for each event mention.\n- If the text is explicitly a NEGATION (e.g., "denies pain"), do not extract that event.\n- If the text describes a FUTURE or HYPOTHETICAL event (e.g., "will eat tomorrow"), ignore it.\n- A valid event should have occurred in the recent past or is occurring during the time of writing of the text.\n- If no events are found or if unsure, return {"events": []}\n                        \n                        ---\n                                    Attributes allowed:\n                                    {\'Eating\': {\'food\': \'&lt;string&gt; # e.g., pancakes, porridge, etc.\', \'amount\': \'&lt;string&gt; # e.g., 1, 2 bowls, etc.\', \'method\': \'&lt;string&gt;  # e.g., oral, tube, etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, evening etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}, \'Excretion\': {\'type\': \'&lt;string&gt; # e.g., urine, stool, etc.\', \'frequency\': \'&lt;string&gt; # e.g., 2x, once, etc.\', \'quality\': \'&lt;string&gt; # e.g., loose, hard, etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, evening etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}, \'Family\': {\'interaction\': \'&lt;string&gt; # e.g., visit, call, communication, etc.\', \'relation\': \'&lt;string&gt; # e.g., mother, son, etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, evening etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}, \'Pain\': {\'severity\': \'&lt;string&gt; # e.g., mild, moderate, severe, numeric scale if present, etc.\', \'location\': \'&lt;string&gt; # e.g., right knee, head, etc.\', \'duration\': \'&lt;string&gt; # e.g., all night, 3 hours, etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, evening etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}, \'Sleep\': {\'quality\': \'&lt;string&gt; # e.g., good, poor, restless, etc.\', \'duration\': \'&lt;string&gt; # e.g., 6 hours, phrases like "all night", etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, evening etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}}\n                                    If no relevant attribute exists for an event, return an empty object {}.\n                                    \n                        \n                        ---\n                                    Keyword evidence (Ki):\n                                    Additional facts: A keyword matching algorithm without context detected keyword(s) (\'pain\', \'husband\', \'slept\').\n                                    Use this only as a pointer. If context contradicts, ignore.\n                        ---\n                        Output Schema (strict):\n                        {\n                                    "events": [\n                                        {\n                                        "event_id": "&lt; A unique id eg.: e1 | e2 |...&gt;"\n                                        "event_type": "&lt;Pain | Sleep | Excretion | Eating | Family&gt;",\n                                        "text_quote": "&lt;fragement from the text indicating the event_type&gt;",\n                "attributes": {\n                    "&lt;attribute_name&gt;": "&lt;attribute_value&gt;"\n                }\n                                        }\n                                    ],\n                                    "order": [\n                                        ["e1", "before" | "after" | "simultaneous", "e2" ]\n                                    ]\n                                    }\n                        \n                            Rules:\n                                - Ensure the output is valid JSON (parseable).\n                                - "eventS" must always be an array (can be empty).\n                                - Multiple instances of the same event type appear with different ids.\n                                - Events appear in the array in the same order in which they appear in the text.\n                                - Their partial orders can be expressed using the "order" section.\n                                - Do not include extra keys, comments, or text.\n                                - Each object in "events" must contain "event_type", "text_quote", and "attributes".\n                                - If an event attribute type has no value mentioned, return "attributes": {"&lt; attribute name &gt;:Unknown"} for each attribute type defined for the event type \n                        \n                        \n                        \n                ---\n                Examples:\n                \n                text: "Patient ate breakfast this morning. He seems less anxious."\n                output: {\n                "events": [\n                    {"event_id": "e1",\n                    "event_type": "Eating",\n                    "text_quote":"Patient ate breakfast this morning",\n                    "attributes": {"food": "breakfast", \n                                   "amount": "Unknown",\n                                   "method": "Unknown",\n                                   "negation": "false",\n                                   "time":"morning",\n                                   "caused_by":"Unknown"}\n                    }\n                ],\n                "order":[]\n                }\n                \n                text: "Patient reported severe abdominal pain."\n                output: {\n                "events": [\n                    {"event_id": "e1",\n                    "event_type": "Pain",\n                    "text_quote": "severe abdominal Pain",\n                    "attributes": {"severity": "severe", \n                                   "location": "abdominal",\n                                   "duration": "Unknown",\n                                   "negation": "false",\n                                   "time":"Unknown",\n                                   "caused_by":"Unknown"}\n                    }\n                ],\n                "order":[]\n                }\n                \n                text: "Patient called his son around 3 pm."\n                output: {\n                "events": [\n                    {"event_id": "e1",\n                    "event_type": "Family",\n                    "text_quote": "called his son around 3 pm",\n                    "attributes": {"interaction": "call", \n                                    "relation": "son",\n                                    "negation": "false",\n                                    "time":"3 pm",\n                                    "caused_by":"Unknown"}\n                    }\n                ],\n                "order":[]\n                }\n                \n                text: "Patient had a loose stool overnight."\n                output: {\n                "events": [\n                    {"event_id": "e1",\n                    "event_type": "Excretion",\n                    "text_quote": "loose stool overnight",\n                    "attributes": {"type": "stool", \n                                   "quality": "loose", \n                                   "frequency":"overnight", \n                                   "negation": "false",\n                                   "time":"night",\n                                   "caused_by":"Unknown"}\n                    }\n                ],\n                "order":[]\n                }\n                \n                text: "Patient was able to sleep well last night."\n                output: {\n                "events": [\n                    {"event_id": "e1",\n                    "event_type": "Sleep",\n                    "text_quote": "sleep well last night",\n                    "attributes": {"quality": "well",\n                                    "duration": "Unknown", \n                                    "negation": "false",\n                                    "time":"night",\n                                    "caused_by":"Unknown"}\n                    }\n                ],\n                "order":[]\n                }\n                \n                text: "The patient couldn\'t sleep due to severe pain."\n                output: {\n                "events": [\n                    {"event_id": "e1",\n                    "event_type": "Sleep",\n                    "text_quote": "couldn\'t sleep",\n                    "attributes": {"quality": "poor", \n                                    "duration": "Unknown",\n                                    "negation": "true",\n                                    "time":"Unknown",\n                                    "caused_by":"Pain"}\n                    },\n                    {"event_id": "e2",\n                    "event_type": "Pain",\n                    "text_quote": "severe pain",\n                    "attributes": {"severity": "severe", \n                                    "location": "Unknown", \n                                    "duration": "Unknown", \n                                    "time":"Unknown",\n                                    "caused_by":"Unknown"}\n                    }\n                ],\n                "order":["e1", "after", "e2"]\n                }\n                \n                text: "The patient complained of severe back pain, was given Tylenol, but the pain persisted and he was then prescribed stronger morphine."\n                output: {\n                "events": [\n                    {"event_id": "e1",\n                    "event_type": "Pain",\n                    "text_quote": "complained of severe back pain",\n                    "attributes": {"severity": "severe", \n                                    "location": "back",\n                                    "duration": "Unknown", \n                                    "time":"Unknown",\n                                    "caused_by":"Unknown"}\n                    },\n                    {"event_id": "e2",\n                    "event_type": "Pain",\n                    "text_quote": "pain persisted",\n                    "attributes": {"severity": "severe", \n                                   "location": "back",\n                                   "duration": "persistent", \n                                   "time":"after Tylenol",\n                                   "caused_by":"Unknown"}\n                    }\n                ],\n                "order":[["e1", "before", "e2"]]\n                }\n                \n                        ', 'event_detection_time': 15.790015444043092}</t>
+        </is>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
           <t>['Pain', 'Sleep', 'Family', 'Excretion', 'Eating']</t>
         </is>
       </c>
-      <c r="G15" t="inlineStr">
-        <is>
-          <t>[{'Pain': {'severity': 'Unknown', 'location': 'chest', 'duration': 'Unknown', 'time': 'at home', 'caused_by': 'Unknown'}}, {'Sleep': {'quality': 'poor', 'duration': 'days', 'time': 'Unknown', 'caused_by': 'Unknown'}}, {'Family': {'interaction': 'Unknown', 'relation': 'husband', 'negation': 'false', 'time': 'Unknown', 'caused_by': 'Unknown'}}, {'Excretion': {'type': 'stool', 'frequency': 'Unknown', 'quality': 'Unknown', 'negation': 'false', 'time': 'Unknown', 'caused_by': 'Unknown'}}, {'Eating': {'food': 'water', 'amount': 'sips', 'method': 'oral', 'negation': 'false', 'time': 'Unknown', 'caused_by': 'Unknown'}}]</t>
-        </is>
-      </c>
       <c r="H15" t="inlineStr">
         <is>
+          <t>[{'Pain': {'severity': 'Unknown', 'location': 'chest', 'duration': 'Unknown', 'negation': 'false', 'time': 'at home', 'caused_by': 'Unknown'}}, {'Sleep': {'quality': 'poor', 'duration': 'days', 'negation': 'true', 'time': 'Unknown', 'caused_by': 'Unknown'}}, {'Family': {'interaction': 'Unknown', 'relation': 'husband', 'negation': 'false', 'time': 'Unknown', 'caused_by': 'Unknown'}}, {'Excretion': {'type': 'stool', 'frequency': 'Unknown', 'quality': 'Unknown', 'negation': 'false', 'time': 'Unknown', 'caused_by': 'Unknown'}}, {'Eating': {'food': 'water', 'amount': 'sips', 'method': 'oral', 'negation': 'false', 'time': 'Unknown', 'caused_by': 'Unknown'}}]</t>
+        </is>
+      </c>
+      <c r="I15" t="inlineStr">
+        <is>
           <t>['chest pain at home', "she hasn't slept in days", 'pts husband is a nurse', '+ bm guaic -', 'patient tolerating sips of water']</t>
         </is>
       </c>
-      <c r="I15" t="inlineStr">
-        <is>
-          <t>{'text': "39 year old female history of coughing past few weeks. patient was found to have cardiomyopathy and is in heart failure. patient was taking coreg 3.125mg [**hospital1 **] and lasix 40 mg qd at home. patient was tolerating by mouth meds until [**6-12**] a.male. she felt weak and dizzy. patient ef was 15%. ? cardiomyopathy from viral illness diagnosed on [**6-8**]. pts husband is a nurse [**first name (titles) 14**] [**last name (titles) 2**] he requested patient be transferred here from [**hospital 1227**] hosp.\n\ncv:nsr/st c freq/occa pvc's. patient has 5 runs of vt each with 8-10 beats of vt. patient received her captopril 6.25mg at 2200 and received lasix 20mg at 2200 and since has had very low bp in the 80's. beta blocker has been on hold until bp maps are greater than 65. maps now 64. heart rate 104-80. hct 42.2, k 4.3. small pericardial effusion and sever global vent hypokinesis found on echo.\n\nresp: patient has nonproductive cough for past few weeks. patient has benzonatate ordered for coughing patient received one this a.male and it helped with her coughing. patient ls coarse at bases. no o2 maintaining oxygen saturation of 97%. sob with exertion.\n\nneuro:patient has a history of depression and patient does appear sad. patient is alert and oriented x3. patient lives at [**location 10814**] with husband and two children. patient has complained that she hasnt slept in days.\n\ngu:patient tolerating sips of water. bs +, + bm guaic -.\n\ngi:1500cc a day fluid restriction. patient responded well to lasix -600cc.\n\na:39yo female with new onset of cardiomyopathy witha ef of 15%.\n\np: patient [**month (only) 108**] need cardiaccath to evaluate coronary arteries. fluid restriction. keep pain free patient was taking percocet for chest pain at home. emotional support.\n", 'event': ['Pain', 'Sleep', 'Family', 'Excretion', 'Eating'], 'phrase': '', 'raw_output': '{\n  "events": [\n    {\n      "event_type": "Pain",\n      "text_quote": "patient was taking percocet for chest pain at home.",\n      "attributes": {\n        "severity": "Unknown",\n        "location": "chest",\n        "duration": "Unknown",\n        "negation": false,\n        "time": "at home",\n        "caused_by": "Unknown"\n      }\n    },\n    {\n      "event_type": "Sleep",\n      "text_quote": "patient has complained that she hasn\'t slept in days.",\n      "attributes": {\n        "quality": "poor",\n        "duration": "days",\n        "negation": false,\n        "time": "Unknown",\n        "caused_by": "Unknown"\n      }\n    },\n    {\n      "event_type": "Family",\n      "text_quote": "pts husband is a nurse [**first name (titles) 14**] [**last name (titles) 2**]",\n      "attributes": {\n        "interaction": "Unknown",\n        "relation": "husband",\n        "negation": false,\n        "time": "Unknown",\n        "caused_by": "Unknown"\n      }\n    },\n    {\n      "event_type": "Excretion",\n      "text_quote": "gu:patient tolerating sips of water. bs +, + bm guaic -.",\n      "attributes": {\n        "type": "stool",\n        "frequency": "Unknown",\n        "quality": "positive for blood",\n        "negation": false,\n        "time": "Unknown",\n        "caused_by": "Unknown"\n      }\n    },\n    {\n      "event_type": "Eating",\n      "text_quote": "patient tolerating sips of water.",\n      "attributes": {\n        "food": "water",\n        "amount": "sips",\n        "method": "oral",\n        "negation": false,\n        "time": "Unknown",\n        "caused_by": "Unknown"\n      }\n    }\n  ]\n}', 'attributes': [{'Pain': {'severity': 'Unknown', 'location': 'chest', 'duration': 'Unknown', 'negation': False, 'time': 'at home', 'caused_by': 'Unknown'}}, {'Sleep': {'quality': 'poor', 'duration': 'days', 'negation': False, 'time': 'Unknown', 'caused_by': 'Unknown'}}, {'Family': {'interaction': 'Unknown', 'relation': 'husband', 'negation': False, 'time': 'Unknown', 'caused_by': 'Unknown'}}, {'Excretion': {'type': 'stool', 'frequency': 'Unknown', 'quality': 'positive for blood', 'negation': False, 'time': 'Unknown', 'caused_by': 'Unknown'}}, {'Eating': {'food': 'water', 'amount': 'sips', 'method': 'oral', 'negation': False, 'time': 'Unknown', 'caused_by': 'Unknown'}}], 'text_quotes': ['patient was taking percocet for chest pain at home.', "patient has complained that she hasn't slept in days.", 'pts husband is a nurse [**first name (titles) 14**] [**last name (titles) 2**]', 'gu:patient tolerating sips of water. bs +, + bm guaic -.', 'patient tolerating sips of water.'], 'event_name_prompt': 'Given the text: 39 year old female history of coughing past few weeks. patient was found to have cardiomyopathy and is in heart failure. patient was taking coreg 3.125mg [**hospital1 **] and lasix 40 mg qd at home. patient was tolerating by mouth meds until [**6-12**] a.male. she felt weak and dizzy. patient ef was 15%. ? cardiomyopathy from viral illness diagnosed on [**6-8**]. pts husband is a nurse [**first name (titles) 14**] [**last name (titles) 2**] he requested patient be transferred here from [**hospital 1227**] hosp.\n\ncv:nsr/st c freq/occa pvc\'s. patient has 5 runs of vt each with 8-10 beats of vt. patient received her captopril 6.25mg at 2200 and received lasix 20mg at 2200 and since has had very low bp in the 80\'s. beta blocker has been on hold until bp maps are greater than 65. maps now 64. heart rate 104-80. hct 42.2, k 4.3. small pericardial effusion and sever global vent hypokinesis found on echo.\n\nresp: patient has nonproductive cough for past few weeks. patient has benzonatate ordered for coughing patient received one this a.male and it helped with her coughing. patient ls coarse at bases. no o2 maintaining oxygen saturation of 97%. sob with exertion.\n\nneuro:patient has a history of depression and patient does appear sad. patient is alert and oriented x3. patient lives at [**location 10814**] with husband and two children. patient has complained that she hasnt slept in days.\n\ngu:patient tolerating sips of water. bs +, + bm guaic -.\n\ngi:1500cc a day fluid restriction. patient responded well to lasix -600cc.\n\na:39yo female with new onset of cardiomyopathy witha ef of 15%.\n\np: patient [**month (only) 108**] need cardiaccath to evaluate coronary arteries. fluid restriction. keep pain free patient was taking percocet for chest pain at home. emotional support.\n, \n                        and the following event types with their definitions: Eating : The patient takes food into their body by mouth.\nExcretion : The patient discharges waste matter from their body.\nFamily : The patient has a visit, call, or communication with a family member.\nPain : The patient reports or shows signs of pain.\nSleep : The patient sleeps or the sleep’s quality or quantity is described.\nUnknown : choose "Unknown" if none of the other event type are applicable. \n                        ---\n                        Your task:\n                        0. Identify ALL events in the text (zero, one, or more).\n1. For each event, assign an event_type from the list above.\n2. If multiple event of same type is mentioned, assign the event_type multiple times\n3. Extract attributes for each event using ONLY the allowed attributes listed below.\n4. Use keyword evidence (Ki) ONLY if it is consistent with the text context.\n5. Output strictly valid JSON following the schema below.\n                        ---\n                        Classification Rules:\n                        - A text may contain multiple events of the same or different types.\n- Create a separate event object for each event mention.\n- If the text is explicitly a NEGATION (e.g., "denies pain"), do not extract that event.\n- If the text describes a FUTURE or HYPOTHETICAL event (e.g., "will eat tomorrow"), ignore it.\n- A valid event should have occurred in the recent past or is occurring during the time of writing of the text.\n- If no events are found or if unsure, return {"events": []}\n                        \n                        ---\n                                    Attributes allowed:\n                                    {\'Eating\': {\'food\': \'&lt;string&gt; # e.g., pancakes, porridge, etc.\', \'amount\': \'&lt;string&gt; # e.g., 1, 2 bowls, etc.\', \'method\': \'&lt;string&gt;  # e.g., oral, tube, etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, after shower, etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}, \'Excretion\': {\'type\': \'&lt;string&gt; # e.g., urine, stool, etc.\', \'frequency\': \'&lt;string&gt; # e.g., 2x, once, etc.\', \'quality\': \'&lt;string&gt; # e.g., loose, hard, etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, after shower, etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}, \'Family\': {\'interaction\': \'&lt;string&gt; # e.g., visit, call, communication, etc.\', \'relation\': \'&lt;string&gt; # e.g., mother, son, etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, after shower, etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}, \'Pain\': {\'severity\': \'&lt;string&gt; # e.g., mild, moderate, severe, numeric scale if present, etc.\', \'location\': \'&lt;string&gt; # e.g., right knee, head, etc.\', \'duration\': \'&lt;string&gt; # e.g., all night, 3 hours, etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, after shower, etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}, \'Sleep\': {\'quality\': \'&lt;string&gt; # e.g., good, poor, restless, etc.\', \'duration\': \'&lt;string&gt; # e.g., 6 hours, phrases like "all night", etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, after shower, etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}}\n                                    If no relevant attribute exists for an event, return an empty object {}.\n                                    \n                        \n                        ---\n                                    Keyword evidence (Ki):\n                                    Additional facts: A keyword matching algorithm without context detected keyword(s) [\'slept\', \'husband\', \'pain\'].\n                                    Use this only as a pointer. If context contradicts, ignore.\n                        ---\n                        Output Schema (strict):\n                        {\n                                    "events": [\n                                        {\n                                        "event_type": "&lt;Pain | Sleep | Excretion | Eating | Family&gt;",\n                                        "text_quote": "&lt;fragement from the text indicating &gt;",\n                "attributes": {\n                    "&lt;attribute_name&gt;": "&lt;attribute_value&gt;"\n                }\n                                        }\n                                    ]\n                                    }\n                        \n                            Rules:\n                                - Ensure the output is valid JSON (parseable).\n                                - "eventS" must always be an array (can be empty).\n                                - Multiple instances of the same event type appear as individual elements in the event array.\n                                - Events appear in the array in the same order in which they appear in the text.\n                                - Do not include extra keys, comments, or text.\n                                - Each object in "events" must contain "event_type", "text_quote", and "attributes".\n                                -If an event attribute type has no value mentioned, return "attributes": {"&lt; attribute name &gt;:Unknown"} for each attribute type defined for the event type \n                        \n                        \n                        \n                        ', 'event_detection_time': 14.345665834989632}</t>
-        </is>
-      </c>
       <c r="J15" t="inlineStr">
         <is>
+          <t>[[]]</t>
+        </is>
+      </c>
+      <c r="K15" t="inlineStr">
+        <is>
+          <t>{'text': "39 year old female history of coughing past few weeks. patient was found to have cardiomyopathy and is in heart failure. patient was taking coreg 3.125mg [**hospital1 **] and lasix 40 mg qd at home. patient was tolerating by mouth meds until [**6-12**] a.male. she felt weak and dizzy. patient ef was 15%. ? cardiomyopathy from viral illness diagnosed on [**6-8**]. pts husband is a nurse [**first name (titles) 14**] [**last name (titles) 2**] he requested patient be transferred here from [**hospital 1227**] hosp.\n\ncv:nsr/st c freq/occa pvc's. patient has 5 runs of vt each with 8-10 beats of vt. patient received her captopril 6.25mg at 2200 and received lasix 20mg at 2200 and since has had very low bp in the 80's. beta blocker has been on hold until bp maps are greater than 65. maps now 64. heart rate 104-80. hct 42.2, k 4.3. small pericardial effusion and sever global vent hypokinesis found on echo.\n\nresp: patient has nonproductive cough for past few weeks. patient has benzonatate ordered for coughing patient received one this a.male and it helped with her coughing. patient ls coarse at bases. no o2 maintaining oxygen saturation of 97%. sob with exertion.\n\nneuro:patient has a history of depression and patient does appear sad. patient is alert and oriented x3. patient lives at [**location 10814**] with husband and two children. patient has complained that she hasnt slept in days.\n\ngu:patient tolerating sips of water. bs +, + bm guaic -.\n\ngi:1500cc a day fluid restriction. patient responded well to lasix -600cc.\n\na:39yo female with new onset of cardiomyopathy witha ef of 15%.\n\np: patient [**month (only) 108**] need cardiaccath to evaluate coronary arteries. fluid restriction. keep pain free patient was taking percocet for chest pain at home. emotional support.\n", 'event': ['Pain', 'Sleep', 'Family', 'Excretion', 'Eating'], 'event_id': ['e1', 'e2', 'e3', 'e4', 'e5'], 'phrase': '', 'raw_output': '{\n  "events": [\n    {\n      "event_id": "e1",\n      "event_type": "Pain",\n      "text_quote": "patient was taking percocet for chest pain at home.",\n      "attributes": {\n        "severity": "Unknown",\n        "location": "chest",\n        "duration": "Unknown",\n        "negation": false,\n        "time": "at home",\n        "caused_by": "Unknown"\n      }\n    },\n    {\n      "event_id": "e2",\n      "event_type": "Sleep",\n      "text_quote": "patient has complained that she hasn\'t slept in days.",\n      "attributes": {\n        "quality": "poor",\n        "duration": "days",\n        "negation": false,\n        "time": "Unknown",\n        "caused_by": "Unknown"\n      }\n    },\n    {\n      "event_id": "e3",\n      "event_type": "Family",\n      "text_quote": "pts husband is a nurse [**first name (titles) 14**] [**last name (titles) 2**]",\n      "attributes": {\n        "interaction": "Unknown",\n        "relation": "husband",\n        "negation": false,\n        "time": "Unknown",\n        "caused_by": "Unknown"\n      }\n    },\n    {\n      "event_id": "e4",\n      "event_type": "Excretion",\n      "text_quote": "gu:patient tolerating sips of water. bs +, + bm guaic -.",\n      "attributes": {\n        "type": "stool",\n        "frequency": "Unknown",\n        "quality": "+",\n        "negation": false,\n        "time": "Unknown",\n        "caused_by": "Unknown"\n      }\n    },\n    {\n      "event_id": "e5",\n      "event_type": "Eating",\n      "text_quote": "patient tolerating sips of water.",\n      "attributes": {\n        "food": "water",\n        "amount": "sips",\n        "method": "oral",\n        "negation": false,\n        "time": "Unknown",\n        "caused_by": "Unknown"\n      }\n    }\n  ],\n  "order": [\n    ["e1", "before", "e2"],\n    ["e2", "before", "e3"],\n    ["e3", "before", "e4"],\n    ["e4", "before", "e5"]\n  ]\n}', 'attributes': [{'Pain': {'severity': 'Unknown', 'location': 'chest', 'duration': 'Unknown', 'negation': False, 'time': 'at home', 'caused_by': 'Unknown'}}, {'Sleep': {'quality': 'poor', 'duration': 'days', 'negation': False, 'time': 'Unknown', 'caused_by': 'Unknown'}}, {'Family': {'interaction': 'Unknown', 'relation': 'husband', 'negation': False, 'time': 'Unknown', 'caused_by': 'Unknown'}}, {'Excretion': {'type': 'stool', 'frequency': 'Unknown', 'quality': '+', 'negation': False, 'time': 'Unknown', 'caused_by': 'Unknown'}}, {'Eating': {'food': 'water', 'amount': 'sips', 'method': 'oral', 'negation': False, 'time': 'Unknown', 'caused_by': 'Unknown'}}], 'orders': [[['e1', 'before', 'e2'], ['e2', 'before', 'e3'], ['e3', 'before', 'e4'], ['e4', 'before', 'e5']]], 'text_quotes': ['patient was taking percocet for chest pain at home.', "patient has complained that she hasn't slept in days.", 'pts husband is a nurse [**first name (titles) 14**] [**last name (titles) 2**]', 'gu:patient tolerating sips of water. bs +, + bm guaic -.', 'patient tolerating sips of water.'], 'event_name_prompt': 'Given the text: 39 year old female history of coughing past few weeks. patient was found to have cardiomyopathy and is in heart failure. patient was taking coreg 3.125mg [**hospital1 **] and lasix 40 mg qd at home. patient was tolerating by mouth meds until [**6-12**] a.male. she felt weak and dizzy. patient ef was 15%. ? cardiomyopathy from viral illness diagnosed on [**6-8**]. pts husband is a nurse [**first name (titles) 14**] [**last name (titles) 2**] he requested patient be transferred here from [**hospital 1227**] hosp.\n\ncv:nsr/st c freq/occa pvc\'s. patient has 5 runs of vt each with 8-10 beats of vt. patient received her captopril 6.25mg at 2200 and received lasix 20mg at 2200 and since has had very low bp in the 80\'s. beta blocker has been on hold until bp maps are greater than 65. maps now 64. heart rate 104-80. hct 42.2, k 4.3. small pericardial effusion and sever global vent hypokinesis found on echo.\n\nresp: patient has nonproductive cough for past few weeks. patient has benzonatate ordered for coughing patient received one this a.male and it helped with her coughing. patient ls coarse at bases. no o2 maintaining oxygen saturation of 97%. sob with exertion.\n\nneuro:patient has a history of depression and patient does appear sad. patient is alert and oriented x3. patient lives at [**location 10814**] with husband and two children. patient has complained that she hasnt slept in days.\n\ngu:patient tolerating sips of water. bs +, + bm guaic -.\n\ngi:1500cc a day fluid restriction. patient responded well to lasix -600cc.\n\na:39yo female with new onset of cardiomyopathy witha ef of 15%.\n\np: patient [**month (only) 108**] need cardiaccath to evaluate coronary arteries. fluid restriction. keep pain free patient was taking percocet for chest pain at home. emotional support.\n, \n                        and the following event types with their definitions: Eating : The patient takes food into their body by mouth.\nExcretion : The patient discharges waste matter from their body.\nFamily : The patient has a visit, call, or communication with a family member.\nPain : The patient reports or shows signs of pain.\nSleep : The patient sleeps or the sleep’s quality or quantity is described.\nUnknown : choose "Unknown" if none of the other event type are applicable. \n                        ---\n                        Your task:\n                        0. Identify ALL events in the text (zero, one, or more).\n1. For each event, assign an event_type from the list above.\n2. If multiple event of same type is mentioned, assign the event_type multiple times\n3. Extract attributes for each event using ONLY the allowed attributes listed below.\n4. Use keyword evidence (Ki) ONLY if it is consistent with the text context.\n5. Output strictly valid JSON following the schema below.\n                        ---\n                        Classification Rules:\n                        - A text may contain multiple events of the same or different types.\n- Create a separate event object for each event mention.\n- If the text is explicitly a NEGATION (e.g., "denies pain"), do not extract that event.\n- If the text describes a FUTURE or HYPOTHETICAL event (e.g., "will eat tomorrow"), ignore it.\n- A valid event should have occurred in the recent past or is occurring during the time of writing of the text.\n- If no events are found or if unsure, return {"events": []}\n                        \n                        ---\n                                    Attributes allowed:\n                                    {\'Eating\': {\'food\': \'&lt;string&gt; # e.g., pancakes, porridge, etc.\', \'amount\': \'&lt;string&gt; # e.g., 1, 2 bowls, etc.\', \'method\': \'&lt;string&gt;  # e.g., oral, tube, etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, evening etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}, \'Excretion\': {\'type\': \'&lt;string&gt; # e.g., urine, stool, etc.\', \'frequency\': \'&lt;string&gt; # e.g., 2x, once, etc.\', \'quality\': \'&lt;string&gt; # e.g., loose, hard, etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, evening etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}, \'Family\': {\'interaction\': \'&lt;string&gt; # e.g., visit, call, communication, etc.\', \'relation\': \'&lt;string&gt; # e.g., mother, son, etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, evening etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}, \'Pain\': {\'severity\': \'&lt;string&gt; # e.g., mild, moderate, severe, numeric scale if present, etc.\', \'location\': \'&lt;string&gt; # e.g., right knee, head, etc.\', \'duration\': \'&lt;string&gt; # e.g., all night, 3 hours, etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, evening etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}, \'Sleep\': {\'quality\': \'&lt;string&gt; # e.g., good, poor, restless, etc.\', \'duration\': \'&lt;string&gt; # e.g., 6 hours, phrases like "all night", etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, evening etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}}\n                                    If no relevant attribute exists for an event, return an empty object {}.\n                                    \n                        \n                        ---\n                                    Keyword evidence (Ki):\n                                    Additional facts: A keyword matching algorithm without context detected keyword(s) (\'pain\', \'husband\', \'slept\').\n                                    Use this only as a pointer. If context contradicts, ignore.\n                        ---\n                        Output Schema (strict):\n                        {\n                                    "events": [\n                                        {\n                                        "event_id": "&lt; A unique id eg.: e1 | e2 |...&gt;"\n                                        "event_type": "&lt;Pain | Sleep | Excretion | Eating | Family&gt;",\n                                        "text_quote": "&lt;fragement from the text indicating the event_type&gt;",\n                "attributes": {\n                    "&lt;attribute_name&gt;": "&lt;attribute_value&gt;"\n                }\n                                        }\n                                    ],\n                                    "order": [\n                                        ["e1", "before" | "after" | "simultaneous", "e2" ]\n                                    ]\n                                    }\n                        \n                            Rules:\n                                - Ensure the output is valid JSON (parseable).\n                                - "eventS" must always be an array (can be empty).\n                                - Multiple instances of the same event type appear with different ids.\n                                - Events appear in the array in the same order in which they appear in the text.\n                                - Their partial orders can be expressed using the "order" section.\n                                - Do not include extra keys, comments, or text.\n                                - Each object in "events" must contain "event_type", "text_quote", and "attributes".\n                                - If an event attribute type has no value mentioned, return "attributes": {"&lt; attribute name &gt;:Unknown"} for each attribute type defined for the event type \n                        \n                        \n                        \n                        ', 'event_detection_time': 17.291625529993325}</t>
+        </is>
+      </c>
+      <c r="L15" t="inlineStr">
+        <is>
           <t>['Pain', 'Sleep', 'Family', 'Excretion', 'Eating']</t>
         </is>
       </c>
-      <c r="K15" t="inlineStr">
-        <is>
-          <t>[{'Pain': {'severity': 'Unknown', 'location': 'chest', 'duration': 'Unknown', 'negation': False, 'time': 'at home', 'caused_by': 'Unknown'}}, {'Sleep': {'quality': 'poor', 'duration': 'days', 'negation': False, 'time': 'Unknown', 'caused_by': 'Unknown'}}, {'Family': {'interaction': 'Unknown', 'relation': 'husband', 'negation': False, 'time': 'Unknown', 'caused_by': 'Unknown'}}, {'Excretion': {'type': 'stool', 'frequency': 'Unknown', 'quality': 'positive for blood', 'negation': False, 'time': 'Unknown', 'caused_by': 'Unknown'}}, {'Eating': {'food': 'water', 'amount': 'sips', 'method': 'oral', 'negation': False, 'time': 'Unknown', 'caused_by': 'Unknown'}}]</t>
-        </is>
-      </c>
-      <c r="L15" t="inlineStr">
+      <c r="M15" t="inlineStr">
+        <is>
+          <t>[{'Pain': {'severity': 'Unknown', 'location': 'chest', 'duration': 'Unknown', 'negation': False, 'time': 'at home', 'caused_by': 'Unknown'}}, {'Sleep': {'quality': 'poor', 'duration': 'days', 'negation': False, 'time': 'Unknown', 'caused_by': 'Unknown'}}, {'Family': {'interaction': 'Unknown', 'relation': 'husband', 'negation': False, 'time': 'Unknown', 'caused_by': 'Unknown'}}, {'Excretion': {'type': 'stool', 'frequency': 'Unknown', 'quality': '+', 'negation': False, 'time': 'Unknown', 'caused_by': 'Unknown'}}, {'Eating': {'food': 'water', 'amount': 'sips', 'method': 'oral', 'negation': False, 'time': 'Unknown', 'caused_by': 'Unknown'}}]</t>
+        </is>
+      </c>
+      <c r="N15" t="inlineStr">
         <is>
           <t>['patient was taking percocet for chest pain at home.', "patient has complained that she hasn't slept in days.", 'pts husband is a nurse [**first name (titles) 14**] [**last name (titles) 2**]', 'gu:patient tolerating sips of water. bs +, + bm guaic -.', 'patient tolerating sips of water.']</t>
         </is>
       </c>
-      <c r="M15" t="inlineStr">
-        <is>
-          <t>{'text': "39 year old female history of coughing past few weeks. patient was found to have cardiomyopathy and is in heart failure. patient was taking coreg 3.125mg [**hospital1 **] and lasix 40 mg qd at home. patient was tolerating by mouth meds until [**6-12**] a.male. she felt weak and dizzy. patient ef was 15%. ? cardiomyopathy from viral illness diagnosed on [**6-8**]. pts husband is a nurse [**first name (titles) 14**] [**last name (titles) 2**] he requested patient be transferred here from [**hospital 1227**] hosp.\n\ncv:nsr/st c freq/occa pvc's. patient has 5 runs of vt each with 8-10 beats of vt. patient received her captopril 6.25mg at 2200 and received lasix 20mg at 2200 and since has had very low bp in the 80's. beta blocker has been on hold until bp maps are greater than 65. maps now 64. heart rate 104-80. hct 42.2, k 4.3. small pericardial effusion and sever global vent hypokinesis found on echo.\n\nresp: patient has nonproductive cough for past few weeks. patient has benzonatate ordered for coughing patient received one this a.male and it helped with her coughing. patient ls coarse at bases. no o2 maintaining oxygen saturation of 97%. sob with exertion.\n\nneuro:patient has a history of depression and patient does appear sad. patient is alert and oriented x3. patient lives at [**location 10814**] with husband and two children. patient has complained that she hasnt slept in days.\n\ngu:patient tolerating sips of water. bs +, + bm guaic -.\n\ngi:1500cc a day fluid restriction. patient responded well to lasix -600cc.\n\na:39yo female with new onset of cardiomyopathy witha ef of 15%.\n\np: patient [**month (only) 108**] need cardiaccath to evaluate coronary arteries. fluid restriction. keep pain free patient was taking percocet for chest pain at home. emotional support.\n", 'event': ['Pain', 'Sleep', 'Family', 'Eating', 'Excretion', 'Excretion'], 'phrase': '', 'raw_output': '{\n  "events": [\n    {\n      "event_type": "Pain",\n      "text_quote": "chest pain at home",\n      "attributes": {\n        "severity": "Unknown",\n        "location": "chest",\n        "duration": "Unknown",\n        "time": "at home",\n        "caused_by": "Unknown"\n      }\n    },\n    {\n      "event_type": "Sleep",\n      "text_quote": "she hasn\'t slept in days",\n      "attributes": {\n        "quality": "poor",\n        "duration": "days",\n        "negation": "true",\n        "time": "Unknown",\n        "caused_by": "Unknown"\n      }\n    },\n    {\n      "event_type": "Family",\n      "text_quote": "patient\'s husband is a nurse",\n      "attributes": {\n        "interaction": "Unknown",\n        "relation": "husband",\n        "negation": "false",\n        "time": "Unknown",\n        "caused_by": "Unknown"\n      }\n    },\n    {\n      "event_type": "Eating",\n      "text_quote": "patient tolerating sips of water",\n      "attributes": {\n        "food": "water",\n        "amount": "sips",\n        "method": "oral",\n        "negation": "false",\n        "time": "Unknown",\n        "caused_by": "Unknown"\n      }\n    },\n    {\n      "event_type": "Excretion",\n      "text_quote": "patient responded well to lasix -600cc",\n      "attributes": {\n        "type": "urine",\n        "frequency": "-600cc",\n        "quality": "Unknown",\n        "negation": "false",\n        "time": "Unknown",\n        "caused_by": "lasix"\n      }\n    },\n    {\n      "event_type": "Excretion",\n      "text_quote": "+ bm guaic -",\n      "attributes": {\n        "type": "stool",\n        "frequency": "Unknown",\n        "quality": "Unknown",\n        "negation": "false",\n        "time": "Unknown",\n        "caused_by": "Unknown"\n      }\n    }\n  ]\n}', 'attributes': [{'Pain': {'severity': 'Unknown', 'location': 'chest', 'duration': 'Unknown', 'time': 'at home', 'caused_by': 'Unknown'}}, {'Sleep': {'quality': 'poor', 'duration': 'days', 'negation': 'true', 'time': 'Unknown', 'caused_by': 'Unknown'}}, {'Family': {'interaction': 'Unknown', 'relation': 'husband', 'negation': 'false', 'time': 'Unknown', 'caused_by': 'Unknown'}}, {'Eating': {'food': 'water', 'amount': 'sips', 'method': 'oral', 'negation': 'false', 'time': 'Unknown', 'caused_by': 'Unknown'}}, {'Excretion': {'type': 'urine', 'frequency': '-600cc', 'quality': 'Unknown', 'negation': 'false', 'time': 'Unknown', 'caused_by': 'lasix'}}, {'Excretion': {'type': 'stool', 'frequency': 'Unknown', 'quality': 'Unknown', 'negation': 'false', 'time': 'Unknown', 'caused_by': 'Unknown'}}], 'text_quotes': ['chest pain at home', "she hasn't slept in days", "patient's husband is a nurse", 'patient tolerating sips of water', 'patient responded well to lasix -600cc', '+ bm guaic -'], 'event_name_prompt': 'Given the text: 39 year old female history of coughing past few weeks. patient was found to have cardiomyopathy and is in heart failure. patient was taking coreg 3.125mg [**hospital1 **] and lasix 40 mg qd at home. patient was tolerating by mouth meds until [**6-12**] a.male. she felt weak and dizzy. patient ef was 15%. ? cardiomyopathy from viral illness diagnosed on [**6-8**]. pts husband is a nurse [**first name (titles) 14**] [**last name (titles) 2**] he requested patient be transferred here from [**hospital 1227**] hosp.\n\ncv:nsr/st c freq/occa pvc\'s. patient has 5 runs of vt each with 8-10 beats of vt. patient received her captopril 6.25mg at 2200 and received lasix 20mg at 2200 and since has had very low bp in the 80\'s. beta blocker has been on hold until bp maps are greater than 65. maps now 64. heart rate 104-80. hct 42.2, k 4.3. small pericardial effusion and sever global vent hypokinesis found on echo.\n\nresp: patient has nonproductive cough for past few weeks. patient has benzonatate ordered for coughing patient received one this a.male and it helped with her coughing. patient ls coarse at bases. no o2 maintaining oxygen saturation of 97%. sob with exertion.\n\nneuro:patient has a history of depression and patient does appear sad. patient is alert and oriented x3. patient lives at [**location 10814**] with husband and two children. patient has complained that she hasnt slept in days.\n\ngu:patient tolerating sips of water. bs +, + bm guaic -.\n\ngi:1500cc a day fluid restriction. patient responded well to lasix -600cc.\n\na:39yo female with new onset of cardiomyopathy witha ef of 15%.\n\np: patient [**month (only) 108**] need cardiaccath to evaluate coronary arteries. fluid restriction. keep pain free patient was taking percocet for chest pain at home. emotional support.\n, \n                        and the following event types with their definitions: Eating : The patient takes food into their body by mouth.\nExcretion : The patient discharges waste matter from their body.\nFamily : The patient has a visit, call, or communication with a family member.\nPain : The patient reports or shows signs of pain.\nSleep : The patient sleeps or the sleep’s quality or quantity is described.\nUnknown : choose "Unknown" if none of the other event type are applicable. \n                        ---\n                        Your task:\n                        0. Identify ALL events in the text (zero, one, or more).\n1. For each event, assign an event_type from the list above.\n2. If multiple event of same type is mentioned, assign the event_type multiple times\n3. Extract attributes for each event using ONLY the allowed attributes listed below.\n4. Output strictly valid JSON following the schema below.\n                        ---\n                        Classification Rules:\n                        - A text may contain multiple events of the same or different types.\n- Create a separate event object for each event mention.\n- If the text is explicitly a NEGATION (e.g., "denies pain"), do not extract that event.\n- If the text describes a FUTURE or HYPOTHETICAL event (e.g., "will eat tomorrow"), ignore it.\n- A valid event should have occurred in the recent past or is occurring during the time of writing of the text.\n- If no events are found or if unsure, return {"events": []}\n                        \n                        ---\n                                    Attributes allowed:\n                                    {\'Eating\': {\'food\': \'&lt;string&gt; # e.g., pancakes, porridge, etc.\', \'amount\': \'&lt;string&gt; # e.g., 1, 2 bowls, etc.\', \'method\': \'&lt;string&gt;  # e.g., oral, tube, etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, after shower, etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}, \'Excretion\': {\'type\': \'&lt;string&gt; # e.g., urine, stool, etc.\', \'frequency\': \'&lt;string&gt; # e.g., 2x, once, etc.\', \'quality\': \'&lt;string&gt; # e.g., loose, hard, etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, after shower, etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}, \'Family\': {\'interaction\': \'&lt;string&gt; # e.g., visit, call, communication, etc.\', \'relation\': \'&lt;string&gt; # e.g., mother, son, etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, after shower, etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}, \'Pain\': {\'severity\': \'&lt;string&gt; # e.g., mild, moderate, severe, numeric scale if present, etc.\', \'location\': \'&lt;string&gt; # e.g., right knee, head, etc.\', \'duration\': \'&lt;string&gt; # e.g., all night, 3 hours, etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, after shower, etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}, \'Sleep\': {\'quality\': \'&lt;string&gt; # e.g., good, poor, restless, etc.\', \'duration\': \'&lt;string&gt; # e.g., 6 hours, phrases like "all night", etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, after shower, etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}}\n                                    If no relevant attribute exists for an event, return an empty object {}.\n                                    \n                        \n                        \n                        ---\n                        Output Schema (strict):\n                        {\n                                    "events": [\n                                        {\n                                        "event_type": "&lt;Pain | Sleep | Excretion | Eating | Family&gt;",\n                                        "text_quote": "&lt;fragement from the text indicating &gt;",\n                "attributes": {\n                    "&lt;attribute_name&gt;": "&lt;attribute_value&gt;"\n                }\n                                        }\n                                    ]\n                                    }\n                        \n                            Rules:\n                                - Ensure the output is valid JSON (parseable).\n                                - "eventS" must always be an array (can be empty).\n                                - Multiple instances of the same event type appear as individual elements in the event array.\n                                - Events appear in the array in the same order in which they appear in the text.\n                                - Do not include extra keys, comments, or text.\n                                - Each object in "events" must contain "event_type", "text_quote", and "attributes".\n                                -If an event attribute type has no value mentioned, return "attributes": {"&lt; attribute name &gt;:Unknown"} for each attribute type defined for the event type \n                        \n                        \n                        \n                ---\n                Examples:\n                \n                text: "Patient ate breakfast this morning. He seems less anxious."\n                output: {\n                "events": [\n                    {\n                    "event_type": "Eating",\n                    "text_quote":"Patient ate breakfast this morning",\n                    "attributes": {"food": "breakfast", \n                                   "amount": "Unknown",\n                                   "method": "Unknown",\n                                   "time":"morning",\n                                   "caused_by":"Unknown"}\n                    }\n                ]\n                }\n                \n                text: "Patient reported severe abdominal pain."\n                output: {\n                "events": [\n                    {\n                    "event_type": "Pain",\n                    "text_quote": "severe abdominal Pain",\n                    "attributes": {"severity": "severe", \n                                   "location": "abdominal",\n                                   "duration": "Unknown",\n                                   "time":"Unknown",\n                                   "caused_by":"Unknown"}\n                    }\n                ]\n                }\n                \n                text: "Patient called his son around 3 pm."\n                output: {\n                "events": [\n                    {\n                    "event_type": "Family",\n                    "text_quote": "called his son around 3 pm",\n                    "attributes": {"interaction": "call", \n                                    "relation": "son",\n                                    "time":"3 pm",\n                                    "caused_by":"Unknown"}\n                    }\n                ]\n                }\n                \n                text: "Patient had a loose stool overnight."\n                output: {\n                "events": [\n                    {\n                    "event_type": "Excretion",\n                    "text_quote": "loose stool overnight",\n                    "attributes": {"type": "stool", \n                                   "quality": "loose", \n                                   "frequency":"overnight", \n                                   "time":"night",\n                                   "caused_by":"Unknown"}\n                    }\n                ]\n                }\n                \n                text: "Patient was able to sleep well last night."\n                output: {\n                "events": [\n                    {\n                    "event_type": "Sleep",\n                    "text_quote": "sleep well last night",\n                    "attributes": {"quality": "well",\n                                    "duration": "Unknown", \n                                    "time":"night",\n                                    "caused_by":"Unknown"}\n                    }\n                ]\n                }\n                \n                text: "The patient couldn\'t sleep due to severe pain."\n                output: {\n                "events": [\n                    {\n                    "event_type": "Sleep",\n                    "text_quote": "couldn\'t sleep",\n                    "attributes": {"quality": "poor", \n                                    "duration": "Unknown",\n                                   "time":"Unknown",\n                                   "caused_by":"Pain"}\n                    },\n                    {\n                    "event_type": "Pain",\n                    "text_quote": "severe pain",\n                    "attributes": {"severity": "severe", \n                                    "location": "Unknown", \n                                    "duration": "Unknown", \n                                   "time":"before Sleep",\n                                   "caused_by":"Unknown"}\n                    }\n                ]\n                }\n                \n                text: "The patient complained of severe back pain, was given Tylenol, but the pain persisted and he was then prescribed stronger morphine."\n                output: {\n                "events": [\n                    {\n                    "event_type": "Pain",\n                    "text_quote": "complained of severe back pain",\n                    "attributes": {"severity": "severe", \n                                    "location": "back",\n                                    "duration": "Unknown", \n                                    "time":"Unknown",\n                                    "caused_by":"Unknown"}\n                    },\n                    {\n                    "event_type": "Pain",\n                    "text_quote": "pain persisted",\n                    "attributes": {"severity": "severe", \n                                   "location": "back",\n                                   "duration": "persistent", \n                                   "time":"after Tylenol",\n                                   "caused_by":"Unknown"}\n                    }\n                ]\n                }\n                \n                        ', 'event_detection_time': 16.121050052999635}</t>
-        </is>
-      </c>
-      <c r="N15" t="inlineStr">
-        <is>
-          <t>['Pain', 'Sleep', 'Family', 'Eating', 'Excretion', 'Excretion']</t>
-        </is>
-      </c>
       <c r="O15" t="inlineStr">
         <is>
-          <t>[{'Pain': {'severity': 'Unknown', 'location': 'chest', 'duration': 'Unknown', 'time': 'at home', 'caused_by': 'Unknown'}}, {'Sleep': {'quality': 'poor', 'duration': 'days', 'negation': 'true', 'time': 'Unknown', 'caused_by': 'Unknown'}}, {'Family': {'interaction': 'Unknown', 'relation': 'husband', 'negation': 'false', 'time': 'Unknown', 'caused_by': 'Unknown'}}, {'Eating': {'food': 'water', 'amount': 'sips', 'method': 'oral', 'negation': 'false', 'time': 'Unknown', 'caused_by': 'Unknown'}}, {'Excretion': {'type': 'urine', 'frequency': '-600cc', 'quality': 'Unknown', 'negation': 'false', 'time': 'Unknown', 'caused_by': 'lasix'}}, {'Excretion': {'type': 'stool', 'frequency': 'Unknown', 'quality': 'Unknown', 'negation': 'false', 'time': 'Unknown', 'caused_by': 'Unknown'}}]</t>
-        </is>
-      </c>
-      <c r="P15" t="inlineStr">
-        <is>
-          <t>['chest pain at home', "she hasn't slept in days", "patient's husband is a nurse", 'patient tolerating sips of water', 'patient responded well to lasix -600cc', '+ bm guaic -']</t>
-        </is>
-      </c>
-      <c r="Q15" t="n">
-        <v>0.003042565000214381</v>
-      </c>
-      <c r="R15" t="inlineStr">
+          <t>[[['e1', 'before', 'e2'], ['e2', 'before', 'e3'], ['e3', 'before', 'e4'], ['e4', 'before', 'e5']]]</t>
+        </is>
+      </c>
+      <c r="P15" t="n">
+        <v>0.002408535001450218</v>
+      </c>
+      <c r="Q15" t="inlineStr">
         <is>
           <t>Sleep</t>
         </is>
       </c>
-      <c r="S15" t="b">
+      <c r="R15" t="b">
+        <v>0</v>
+      </c>
+      <c r="S15" t="n">
         <v>0</v>
       </c>
       <c r="T15" t="n">
-        <v>0</v>
-      </c>
-      <c r="U15" t="n">
-        <v>1</v>
-      </c>
-      <c r="V15" t="inlineStr">
+        <v>1</v>
+      </c>
+      <c r="U15" t="inlineStr">
         <is>
           <t>('pain', 'husband', 'sleep')</t>
         </is>
       </c>
+      <c r="V15" t="n">
+        <v>15.79001544404309</v>
+      </c>
       <c r="W15" t="n">
-        <v>13.49978643500071</v>
+        <v>17.29162552999333</v>
       </c>
       <c r="X15" t="n">
-        <v>14.34566583498963</v>
+        <v>1</v>
       </c>
       <c r="Y15" t="n">
-        <v>16.12105005299964</v>
+        <v>1</v>
       </c>
       <c r="Z15" t="n">
-        <v>1</v>
-      </c>
-      <c r="AA15" t="n">
-        <v>1</v>
-      </c>
-      <c r="AB15" t="n">
-        <v>1</v>
-      </c>
-      <c r="AC15" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="16">
-      <c r="A16" t="n">
-        <v>1325549</v>
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>1325549</t>
+        </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>['Eating', 'Unknown', 'Sleep', 'Excretion', 'Family']</t>
+          <t>('Eating', 'Unknown', 'Excretion', 'Family', 'Sleep')</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>['urine', 'eaten', 'brother', 'sleeping', 'mother', 'sleep', 'family', 'sisters', 'husband']</t>
+          <t>('mother', 'sleep', 'husband', 'family', 'urine', 'sisters', 'eaten', 'brother', 'sleeping')</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
@@ -2499,120 +2364,111 @@
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>{'text': 'ccu nsg note: alt in cv/cardiomyopathy\ns: "i think i do feel better".\no: for complete vs see ccu flow sheet\nthis 39y old woman comes to [**hospital1 2**] from osh with ~3mo history of sob and 3 week history of increasing sob, fever, lower extremity edema and severe exercise intolerance. echo shows ef of 10% with cardiomyopathy of unknown origen. she started captopril overnight with previous carvedolol dose d/c.\ncv: patient initially had bp in low 100s, but by 10pm dinamap and auscultated bp were unobtainable. doppler \rbps  weree  in the mid 80s with heart rate in the low 100s st with frequent pvcs. urine output also dropped and lungs were more congested with near constant coughing. it was decided to send here to the cath lab for swan placement. prior to going multiple radial aline attempts were made with no success. attempts in cath lab also failed and r 4f femoral aline was placed. in lab she had swan placed thru r ij. ra was 12, rv 45/16, pa 43/21 with wedge 17. co was 3.2 with index 1.53. she was boluses with 50mic/kilo of milrinone and started on drip at .375mic/kilo. patient returned to ccu ~1430 with aline in r groin, rij swan and milrinone running. co/ci have improved and at 1800 numbers were 6.0/2.83/853. paps have ranged 40s/14-20 with wedge 14 and ra [**6-2**]. heart rate has increased to  108-120s with frequent pvcs, runs of ventricular trigemininy and episodes of alternans from systole seen by aline tracing. at 1530 anesthesia was able to place a l radial aline and at 1600 femoral aline was removed. there is no ooze or hematoma and all pulses palpable. all extremities remain cool. extremities were dusky this am, but color has improved since milrinone added. she received lasix 20mg ivp at 1530. bp now low 100s to 1-teens /60-70s. cough has greatly improved. nimc transplant team has been notified and if patient needs immediate intervention she will be transfered there, if not she will stay here and see them as outpatient if cardiomyopathy does not adequately resolve.\nid: temp on return from lab was 101.7. tylenol given and bc x 2 and urine sent. wbc 16.1 (10.4 this am).\nresp: breath sounds in am were crackles primarily at bases but by 10am she has decreased breath sounds throughout with experitory squeeking noise. she was sating 98-100% but coughing very frequently despite anti-tussives. since returning from the lab her breathing has much improved with only decreased bs at bases. she is sating 97% on 3l np. and gas was 7.47/29/80/22.\ngi: apetite poor and she has eaten nothing today. no bm\nrenal: she has had fair response to lasix and is presently ~900cc neg for the day.\nms/comfort: patient was very anxious about going to lab and also have so many sticks for aline. she received ativan .5mg iv pre and post lab with good results. she also received morphine 2mg iv upon return from lab to help with discomfort.  she has finally been sleeping since line was pulled.\nsocial: her mother sisters and brother and [**name2 (ni) 10815**] were in to visit as well as her husband. [**name (ni) **] husband will sleep here tonight. family aware of severity of patient condition but\n', 'event': ['Eating', 'Excretion', 'Family', 'Pain', 'Sleep'], 'phrase': '', 'raw_output': '{\n  "events": [\n    {\n      "event_type": "Eating",\n      "text_quote": "she has eaten nothing today.",\n      "attributes": {"food": "Unknown", \n                     "amount": "0", \n                     "method": "Unknown", \n                     "negation": true, \n                     "time": "today", \n                     "caused_by": "Unknown"}\n    },\n    {\n      "event_type": "Excretion",\n      "text_quote": "she has had fair response to lasix and is presently ~900cc neg for the day.",\n      "attributes": {"type": "urine", \n                     "frequency": "~900cc", \n                     "quality": "Unknown", \n                     "negation": false, \n                     "time": "today", \n                     "caused_by": "lasix"}\n    },\n    {\n      "event_type": "Family",\n      "text_quote": "her mother sisters and brother and [**name2 (ni) 10815**] were in to visit as well as her husband.",\n      "attributes": {"interaction": "visit", \n                     "relation": "mother, sisters, brother, husband", \n                     "negation": false, \n                     "time": "Unknown", \n                     "caused_by": "Unknown"}\n    },\n    {\n      "event_type": "Pain",\n      "text_quote": "she received morphine 2mg iv upon return from lab to help with discomfort.",\n      "attributes": {"severity": "Unknown", \n                     "location": "Unknown", \n                     "duration": "Unknown", \n                     "negation": false, \n                     "time": "upon return from lab", \n                     "caused_by": "discomfort"}\n    },\n    {\n      "event_type": "Sleep",\n      "text_quote": "she has finally been sleeping since line was pulled.",\n      "attributes": {"quality": "Unknown", \n                     "duration": "since line was pulled", \n                     "negation": false, \n                     "time": "since line was pulled", \n                     "caused_by": "line was pulled"}\n    }\n  ]\n}', 'attributes': [{'Eating': {'food': 'Unknown', 'amount': '0', 'method': 'Unknown', 'negation': True, 'time': 'today', 'caused_by': 'Unknown'}}, {'Excretion': {'type': 'urine', 'frequency': '~900cc', 'quality': 'Unknown', 'negation': False, 'time': 'today', 'caused_by': 'lasix'}}, {'Family': {'interaction': 'visit', 'relation': 'mother, sisters, brother, husband', 'negation': False, 'time': 'Unknown', 'caused_by': 'Unknown'}}, {'Pain': {'severity': 'Unknown', 'location': 'Unknown', 'duration': 'Unknown', 'negation': False, 'time': 'upon return from lab', 'caused_by': 'discomfort'}}, {'Sleep': {'quality': 'Unknown', 'duration': 'since line was pulled', 'negation': False, 'time': 'since line was pulled', 'caused_by': 'line was pulled'}}], 'text_quotes': ['she has eaten nothing today.', 'she has had fair response to lasix and is presently ~900cc neg for the day.', 'her mother sisters and brother and [**name2 (ni) 10815**] were in to visit as well as her husband.', 'she received morphine 2mg iv upon return from lab to help with discomfort.', 'she has finally been sleeping since line was pulled.'], 'event_name_prompt': 'Given the text: ccu nsg note: alt in cv/cardiomyopathy\ns: "i think i do feel better".\no: for complete vs see ccu flow sheet\nthis 39y old woman comes to [**hospital1 2**] from osh with ~3mo history of sob and 3 week history of increasing sob, fever, lower extremity edema and severe exercise intolerance. echo shows ef of 10% with cardiomyopathy of unknown origen. she started captopril overnight with previous carvedolol dose d/c.\ncv: patient initially had bp in low 100s, but by 10pm dinamap and auscultated bp were unobtainable. doppler \rbps  weree  in the mid 80s with heart rate in the low 100s st with frequent pvcs. urine output also dropped and lungs were more congested with near constant coughing. it was decided to send here to the cath lab for swan placement. prior to going multiple radial aline attempts were made with no success. attempts in cath lab also failed and r 4f femoral aline was placed. in lab she had swan placed thru r ij. ra was 12, rv 45/16, pa 43/21 with wedge 17. co was 3.2 with index 1.53. she was boluses with 50mic/kilo of milrinone and started on drip at .375mic/kilo. patient returned to ccu ~1430 with aline in r groin, rij swan and milrinone running. co/ci have improved and at 1800 numbers were 6.0/2.83/853. paps have ranged 40s/14-20 with wedge 14 and ra [**6-2**]. heart rate has increased to  108-120s with frequent pvcs, runs of ventricular trigemininy and episodes of alternans from systole seen by aline tracing. at 1530 anesthesia was able to place a l radial aline and at 1600 femoral aline was removed. there is no ooze or hematoma and all pulses palpable. all extremities remain cool. extremities were dusky this am, but color has improved since milrinone added. she received lasix 20mg ivp at 1530. bp now low 100s to 1-teens /60-70s. cough has greatly improved. nimc transplant team has been notified and if patient needs immediate intervention she will be transfered there, if not she will stay here and see them as outpatient if cardiomyopathy does not adequately resolve.\nid: temp on return from lab was 101.7. tylenol given and bc x 2 and urine sent. wbc 16.1 (10.4 this am).\nresp: breath sounds in am were crackles primarily at bases but by 10am she has decreased breath sounds throughout with experitory squeeking noise. she was sating 98-100% but coughing very frequently despite anti-tussives. since returning from the lab her breathing has much improved with only decreased bs at bases. she is sating 97% on 3l np. and gas was 7.47/29/80/22.\ngi: apetite poor and she has eaten nothing today. no bm\nrenal: she has had fair response to lasix and is presently ~900cc neg for the day.\nms/comfort: patient was very anxious about going to lab and also have so many sticks for aline. she received ativan .5mg iv pre and post lab with good results. she also received morphine 2mg iv upon return from lab to help with discomfort.  she has finally been sleeping since line was pulled.\nsocial: her mother sisters and brother and [**name2 (ni) 10815**] were in to visit as well as her husband. [**name (ni) **] husband will sleep here tonight. family aware of severity of patient condition but\n, \n                        and the following event types with their definitions: Eating : The patient takes food into their body by mouth.\nExcretion : The patient discharges waste matter from their body.\nFamily : The patient has a visit, call, or communication with a family member.\nPain : The patient reports or shows signs of pain.\nSleep : The patient sleeps or the sleep’s quality or quantity is described.\nUnknown : choose "Unknown" if none of the other event type are applicable. \n                        ---\n                        Your task:\n                        0. Identify ALL events in the text (zero, one, or more).\n1. For each event, assign an event_type from the list above.\n2. If multiple event of same type is mentioned, assign the event_type multiple times\n3. Extract attributes for each event using ONLY the allowed attributes listed below.\n4. Use keyword evidence (Ki) ONLY if it is consistent with the text context.\n5. Output strictly valid JSON following the schema below.\n                        ---\n                        Classification Rules:\n                        - A text may contain multiple events of the same or different types.\n- Create a separate event object for each event mention.\n- If the text is explicitly a NEGATION (e.g., "denies pain"), do not extract that event.\n- If the text describes a FUTURE or HYPOTHETICAL event (e.g., "will eat tomorrow"), ignore it.\n- A valid event should have occurred in the recent past or is occurring during the time of writing of the text.\n- If no events are found or if unsure, return {"events": []}\n                        \n                        ---\n                                    Attributes allowed:\n                                    {\'Eating\': {\'food\': \'&lt;string&gt; # e.g., pancakes, porridge, etc.\', \'amount\': \'&lt;string&gt; # e.g., 1, 2 bowls, etc.\', \'method\': \'&lt;string&gt;  # e.g., oral, tube, etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, after shower, etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}, \'Excretion\': {\'type\': \'&lt;string&gt; # e.g., urine, stool, etc.\', \'frequency\': \'&lt;string&gt; # e.g., 2x, once, etc.\', \'quality\': \'&lt;string&gt; # e.g., loose, hard, etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, after shower, etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}, \'Family\': {\'interaction\': \'&lt;string&gt; # e.g., visit, call, communication, etc.\', \'relation\': \'&lt;string&gt; # e.g., mother, son, etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, after shower, etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}, \'Pain\': {\'severity\': \'&lt;string&gt; # e.g., mild, moderate, severe, numeric scale if present, etc.\', \'location\': \'&lt;string&gt; # e.g., right knee, head, etc.\', \'duration\': \'&lt;string&gt; # e.g., all night, 3 hours, etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, after shower, etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}, \'Sleep\': {\'quality\': \'&lt;string&gt; # e.g., good, poor, restless, etc.\', \'duration\': \'&lt;string&gt; # e.g., 6 hours, phrases like "all night", etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, after shower, etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}}\n                                    If no relevant attribute exists for an event, return an empty object {}.\n                                    \n                        \n                        ---\n                                    Keyword evidence (Ki):\n                                    Additional facts: A keyword matching algorithm without context detected keyword(s) [\'urine\', \'eaten\', \'brother\', \'sleeping\', \'mother\', \'sleep\', \'family\', \'sisters\', \'husband\'].\n                                    Use this only as a pointer. If context contradicts, ignore.\n                        ---\n                        Output Schema (strict):\n                        {\n                                    "events": [\n                                        {\n                                        "event_type": "&lt;Pain | Sleep | Excretion | Eating | Family&gt;",\n                                        "text_quote": "&lt;fragement from the text indicating &gt;",\n                "attributes": {\n                    "&lt;attribute_name&gt;": "&lt;attribute_value&gt;"\n                }\n                                        }\n                                    ]\n                                    }\n                        \n                            Rules:\n                                - Ensure the output is valid JSON (parseable).\n                                - "eventS" must always be an array (can be empty).\n                                - Multiple instances of the same event type appear as individual elements in the event array.\n                                - Events appear in the array in the same order in which they appear in the text.\n                                - Do not include extra keys, comments, or text.\n                                - Each object in "events" must contain "event_type", "text_quote", and "attributes".\n                                -If an event attribute type has no value mentioned, return "attributes": {"&lt; attribute name &gt;:Unknown"} for each attribute type defined for the event type \n                        \n                        \n                        \n                ---\n                Examples:\n                \n                text: "Patient ate breakfast this morning. He seems less anxious."\n                output: {\n                "events": [\n                    {\n                    "event_type": "Eating",\n                    "text_quote":"Patient ate breakfast this morning",\n                    "attributes": {"food": "breakfast", \n                                   "amount": "Unknown",\n                                   "method": "Unknown",\n                                   "time":"morning",\n                                   "caused_by":"Unknown"}\n                    }\n                ]\n                }\n                \n                text: "Patient reported severe abdominal pain."\n                output: {\n                "events": [\n                    {\n                    "event_type": "Pain",\n                    "text_quote": "severe abdominal Pain",\n                    "attributes": {"severity": "severe", \n                                   "location": "abdominal",\n                                   "duration": "Unknown",\n                                   "time":"Unknown",\n                                   "caused_by":"Unknown"}\n                    }\n                ]\n                }\n                \n                text: "Patient called his son around 3 pm."\n                output: {\n                "events": [\n                    {\n                    "event_type": "Family",\n                    "text_quote": "called his son around 3 pm",\n                    "attributes": {"interaction": "call", \n                                    "relation": "son",\n                                    "time":"3 pm",\n                                    "caused_by":"Unknown"}\n                    }\n                ]\n                }\n                \n                text: "Patient had a loose stool overnight."\n                output: {\n                "events": [\n                    {\n                    "event_type": "Excretion",\n                    "text_quote": "loose stool overnight",\n                    "attributes": {"type": "stool", \n                                   "quality": "loose", \n                                   "frequency":"overnight", \n                                   "time":"night",\n                                   "caused_by":"Unknown"}\n                    }\n                ]\n                }\n                \n                text: "Patient was able to sleep well last night."\n                output: {\n                "events": [\n                    {\n                    "event_type": "Sleep",\n                    "text_quote": "sleep well last night",\n                    "attributes": {"quality": "well",\n                                    "duration": "Unknown", \n                                    "time":"night",\n                                    "caused_by":"Unknown"}\n                    }\n                ]\n                }\n                \n                text: "The patient couldn\'t sleep due to severe pain."\n                output: {\n                "events": [\n                    {\n                    "event_type": "Sleep",\n                    "text_quote": "couldn\'t sleep",\n                    "attributes": {"quality": "poor", \n                                    "duration": "Unknown",\n                                   "time":"Unknown",\n                                   "caused_by":"Pain"}\n                    },\n                    {\n                    "event_type": "Pain",\n                    "text_quote": "severe pain",\n                    "attributes": {"severity": "severe", \n                                    "location": "Unknown", \n                                    "duration": "Unknown", \n                                   "time":"before Sleep",\n                                   "caused_by":"Unknown"}\n                    }\n                ]\n                }\n                \n                text: "The patient complained of severe back pain, was given Tylenol, but the pain persisted and he was then prescribed stronger morphine."\n                output: {\n                "events": [\n                    {\n                    "event_type": "Pain",\n                    "text_quote": "complained of severe back pain",\n                    "attributes": {"severity": "severe", \n                                    "location": "back",\n                                    "duration": "Unknown", \n                                    "time":"Unknown",\n                                    "caused_by":"Unknown"}\n                    },\n                    {\n                    "event_type": "Pain",\n                    "text_quote": "pain persisted",\n                    "attributes": {"severity": "severe", \n                                   "location": "back",\n                                   "duration": "persistent", \n                                   "time":"after Tylenol",\n                                   "caused_by":"Unknown"}\n                    }\n                ]\n                }\n                \n                        ', 'event_detection_time': 16.370424310007365}</t>
+          <t>['eat', 'mother', 'sleep', 'husband', 'family', 'urine', 'sister', 'brother', 'sleeping']</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
         <is>
+          <t>{'text': 'ccu nsg note: alt in cv/cardiomyopathy\ns: "i think i do feel better".\no: for complete vs see ccu flow sheet\nthis 39y old woman comes to [**hospital1 2**] from osh with ~3mo history of sob and 3 week history of increasing sob, fever, lower extremity edema and severe exercise intolerance. echo shows ef of 10% with cardiomyopathy of unknown origen. she started captopril overnight with previous carvedolol dose d/c.\ncv: patient initially had bp in low 100s, but by 10pm dinamap and auscultated bp were unobtainable. doppler \rbps  weree  in the mid 80s with heart rate in the low 100s st with frequent pvcs. urine output also dropped and lungs were more congested with near constant coughing. it was decided to send here to the cath lab for swan placement. prior to going multiple radial aline attempts were made with no success. attempts in cath lab also failed and r 4f femoral aline was placed. in lab she had swan placed thru r ij. ra was 12, rv 45/16, pa 43/21 with wedge 17. co was 3.2 with index 1.53. she was boluses with 50mic/kilo of milrinone and started on drip at .375mic/kilo. patient returned to ccu ~1430 with aline in r groin, rij swan and milrinone running. co/ci have improved and at 1800 numbers were 6.0/2.83/853. paps have ranged 40s/14-20 with wedge 14 and ra [**6-2**]. heart rate has increased to  108-120s with frequent pvcs, runs of ventricular trigemininy and episodes of alternans from systole seen by aline tracing. at 1530 anesthesia was able to place a l radial aline and at 1600 femoral aline was removed. there is no ooze or hematoma and all pulses palpable. all extremities remain cool. extremities were dusky this am, but color has improved since milrinone added. she received lasix 20mg ivp at 1530. bp now low 100s to 1-teens /60-70s. cough has greatly improved. nimc transplant team has been notified and if patient needs immediate intervention she will be transfered there, if not she will stay here and see them as outpatient if cardiomyopathy does not adequately resolve.\nid: temp on return from lab was 101.7. tylenol given and bc x 2 and urine sent. wbc 16.1 (10.4 this am).\nresp: breath sounds in am were crackles primarily at bases but by 10am she has decreased breath sounds throughout with experitory squeeking noise. she was sating 98-100% but coughing very frequently despite anti-tussives. since returning from the lab her breathing has much improved with only decreased bs at bases. she is sating 97% on 3l np. and gas was 7.47/29/80/22.\ngi: apetite poor and she has eaten nothing today. no bm\nrenal: she has had fair response to lasix and is presently ~900cc neg for the day.\nms/comfort: patient was very anxious about going to lab and also have so many sticks for aline. she received ativan .5mg iv pre and post lab with good results. she also received morphine 2mg iv upon return from lab to help with discomfort.  she has finally been sleeping since line was pulled.\nsocial: her mother sisters and brother and [**name2 (ni) 10815**] were in to visit as well as her husband. [**name (ni) **] husband will sleep here tonight. family aware of severity of patient condition but\n', 'event': ['Eating', 'Excretion', 'Family', 'Sleep', 'Pain'], 'event_id': ['e1', 'e2', 'e3', 'e4', 'e5'], 'phrase': '', 'raw_output': '{\n  "events": [\n    {\n      "event_id": "e1",\n      "event_type": "Eating",\n      "text_quote": "she has eaten nothing today.",\n      "attributes": {\n        "food": "Unknown",\n        "amount": "0",\n        "method": "Unknown",\n        "negation": "true",\n        "time": "today",\n        "caused_by": "Unknown"\n      }\n    },\n    {\n      "event_id": "e2",\n      "event_type": "Excretion",\n      "text_quote": "she has had fair response to lasix and is presently ~900cc neg for the day.",\n      "attributes": {\n        "type": "urine",\n        "frequency": "~900cc",\n        "quality": "Unknown",\n        "negation": "false",\n        "time": "day",\n        "caused_by": "lasix"\n      }\n    },\n    {\n      "event_id": "e3",\n      "event_type": "Family",\n      "text_quote": "her mother sisters and brother and [**name2 (ni) 10815**] were in to visit as well as her husband.",\n      "attributes": {\n        "interaction": "visit",\n        "relation": "mother, sisters, brother, husband",\n        "negation": "false",\n        "time": "Unknown",\n        "caused_by": "Unknown"\n      }\n    },\n    {\n      "event_id": "e4",\n      "event_type": "Sleep",\n      "text_quote": "she has finally been sleeping since line was pulled.",\n      "attributes": {\n        "quality": "good",\n        "duration": "Unknown",\n        "negation": "false",\n        "time": "since line was pulled",\n        "caused_by": "line being pulled"\n      }\n    },\n    {\n      "event_id": "e5",\n      "event_type": "Pain",\n      "text_quote": "she received morphine 2mg iv upon return from lab to help with discomfort.",\n      "attributes": {\n        "severity": "Unknown",\n        "location": "Unknown",\n        "duration": "Unknown",\n        "negation": "false",\n        "time": "upon return from lab",\n        "caused_by": "discomfort"\n      }\n    }\n  ],\n  "order": []\n}', 'attributes': [{'Eating': {'food': 'Unknown', 'amount': '0', 'method': 'Unknown', 'negation': 'true', 'time': 'today', 'caused_by': 'Unknown'}}, {'Excretion': {'type': 'urine', 'frequency': '~900cc', 'quality': 'Unknown', 'negation': 'false', 'time': 'day', 'caused_by': 'lasix'}}, {'Family': {'interaction': 'visit', 'relation': 'mother, sisters, brother, husband', 'negation': 'false', 'time': 'Unknown', 'caused_by': 'Unknown'}}, {'Sleep': {'quality': 'good', 'duration': 'Unknown', 'negation': 'false', 'time': 'since line was pulled', 'caused_by': 'line being pulled'}}, {'Pain': {'severity': 'Unknown', 'location': 'Unknown', 'duration': 'Unknown', 'negation': 'false', 'time': 'upon return from lab', 'caused_by': 'discomfort'}}], 'orders': [[]], 'text_quotes': ['she has eaten nothing today.', 'she has had fair response to lasix and is presently ~900cc neg for the day.', 'her mother sisters and brother and [**name2 (ni) 10815**] were in to visit as well as her husband.', 'she has finally been sleeping since line was pulled.', 'she received morphine 2mg iv upon return from lab to help with discomfort.'], 'event_name_prompt': 'Given the text: ccu nsg note: alt in cv/cardiomyopathy\ns: "i think i do feel better".\no: for complete vs see ccu flow sheet\nthis 39y old woman comes to [**hospital1 2**] from osh with ~3mo history of sob and 3 week history of increasing sob, fever, lower extremity edema and severe exercise intolerance. echo shows ef of 10% with cardiomyopathy of unknown origen. she started captopril overnight with previous carvedolol dose d/c.\ncv: patient initially had bp in low 100s, but by 10pm dinamap and auscultated bp were unobtainable. doppler \rbps  weree  in the mid 80s with heart rate in the low 100s st with frequent pvcs. urine output also dropped and lungs were more congested with near constant coughing. it was decided to send here to the cath lab for swan placement. prior to going multiple radial aline attempts were made with no success. attempts in cath lab also failed and r 4f femoral aline was placed. in lab she had swan placed thru r ij. ra was 12, rv 45/16, pa 43/21 with wedge 17. co was 3.2 with index 1.53. she was boluses with 50mic/kilo of milrinone and started on drip at .375mic/kilo. patient returned to ccu ~1430 with aline in r groin, rij swan and milrinone running. co/ci have improved and at 1800 numbers were 6.0/2.83/853. paps have ranged 40s/14-20 with wedge 14 and ra [**6-2**]. heart rate has increased to  108-120s with frequent pvcs, runs of ventricular trigemininy and episodes of alternans from systole seen by aline tracing. at 1530 anesthesia was able to place a l radial aline and at 1600 femoral aline was removed. there is no ooze or hematoma and all pulses palpable. all extremities remain cool. extremities were dusky this am, but color has improved since milrinone added. she received lasix 20mg ivp at 1530. bp now low 100s to 1-teens /60-70s. cough has greatly improved. nimc transplant team has been notified and if patient needs immediate intervention she will be transfered there, if not she will stay here and see them as outpatient if cardiomyopathy does not adequately resolve.\nid: temp on return from lab was 101.7. tylenol given and bc x 2 and urine sent. wbc 16.1 (10.4 this am).\nresp: breath sounds in am were crackles primarily at bases but by 10am she has decreased breath sounds throughout with experitory squeeking noise. she was sating 98-100% but coughing very frequently despite anti-tussives. since returning from the lab her breathing has much improved with only decreased bs at bases. she is sating 97% on 3l np. and gas was 7.47/29/80/22.\ngi: apetite poor and she has eaten nothing today. no bm\nrenal: she has had fair response to lasix and is presently ~900cc neg for the day.\nms/comfort: patient was very anxious about going to lab and also have so many sticks for aline. she received ativan .5mg iv pre and post lab with good results. she also received morphine 2mg iv upon return from lab to help with discomfort.  she has finally been sleeping since line was pulled.\nsocial: her mother sisters and brother and [**name2 (ni) 10815**] were in to visit as well as her husband. [**name (ni) **] husband will sleep here tonight. family aware of severity of patient condition but\n, \n                        and the following event types with their definitions: Eating : The patient takes food into their body by mouth.\nExcretion : The patient discharges waste matter from their body.\nFamily : The patient has a visit, call, or communication with a family member.\nPain : The patient reports or shows signs of pain.\nSleep : The patient sleeps or the sleep’s quality or quantity is described.\nUnknown : choose "Unknown" if none of the other event type are applicable. \n                        ---\n                        Your task:\n                        0. Identify ALL events in the text (zero, one, or more).\n1. For each event, assign an event_type from the list above.\n2. If multiple event of same type is mentioned, assign the event_type multiple times\n3. Extract attributes for each event using ONLY the allowed attributes listed below.\n4. Use keyword evidence (Ki) ONLY if it is consistent with the text context.\n5. Output strictly valid JSON following the schema below.\n                        ---\n                        Classification Rules:\n                        - A text may contain multiple events of the same or different types.\n- Create a separate event object for each event mention.\n- If the text is explicitly a NEGATION (e.g., "denies pain"), do not extract that event.\n- If the text describes a FUTURE or HYPOTHETICAL event (e.g., "will eat tomorrow"), ignore it.\n- A valid event should have occurred in the recent past or is occurring during the time of writing of the text.\n- If no events are found or if unsure, return {"events": []}\n                        \n                        ---\n                                    Attributes allowed:\n                                    {\'Eating\': {\'food\': \'&lt;string&gt; # e.g., pancakes, porridge, etc.\', \'amount\': \'&lt;string&gt; # e.g., 1, 2 bowls, etc.\', \'method\': \'&lt;string&gt;  # e.g., oral, tube, etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, evening etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}, \'Excretion\': {\'type\': \'&lt;string&gt; # e.g., urine, stool, etc.\', \'frequency\': \'&lt;string&gt; # e.g., 2x, once, etc.\', \'quality\': \'&lt;string&gt; # e.g., loose, hard, etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, evening etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}, \'Family\': {\'interaction\': \'&lt;string&gt; # e.g., visit, call, communication, etc.\', \'relation\': \'&lt;string&gt; # e.g., mother, son, etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, evening etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}, \'Pain\': {\'severity\': \'&lt;string&gt; # e.g., mild, moderate, severe, numeric scale if present, etc.\', \'location\': \'&lt;string&gt; # e.g., right knee, head, etc.\', \'duration\': \'&lt;string&gt; # e.g., all night, 3 hours, etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, evening etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}, \'Sleep\': {\'quality\': \'&lt;string&gt; # e.g., good, poor, restless, etc.\', \'duration\': \'&lt;string&gt; # e.g., 6 hours, phrases like "all night", etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, evening etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}}\n                                    If no relevant attribute exists for an event, return an empty object {}.\n                                    \n                        \n                        ---\n                                    Keyword evidence (Ki):\n                                    Additional facts: A keyword matching algorithm without context detected keyword(s) (\'mother\', \'sleep\', \'husband\', \'family\', \'urine\', \'sisters\', \'eaten\', \'brother\', \'sleeping\').\n                                    Use this only as a pointer. If context contradicts, ignore.\n                        ---\n                        Output Schema (strict):\n                        {\n                                    "events": [\n                                        {\n                                        "event_id": "&lt; A unique id eg.: e1 | e2 |...&gt;"\n                                        "event_type": "&lt;Pain | Sleep | Excretion | Eating | Family&gt;",\n                                        "text_quote": "&lt;fragement from the text indicating the event_type&gt;",\n                "attributes": {\n                    "&lt;attribute_name&gt;": "&lt;attribute_value&gt;"\n                }\n                                        }\n                                    ],\n                                    "order": [\n                                        ["e1", "before" | "after" | "simultaneous", "e2" ]\n                                    ]\n                                    }\n                        \n                            Rules:\n                                - Ensure the output is valid JSON (parseable).\n                                - "eventS" must always be an array (can be empty).\n                                - Multiple instances of the same event type appear with different ids.\n                                - Events appear in the array in the same order in which they appear in the text.\n                                - Their partial orders can be expressed using the "order" section.\n                                - Do not include extra keys, comments, or text.\n                                - Each object in "events" must contain "event_type", "text_quote", and "attributes".\n                                - If an event attribute type has no value mentioned, return "attributes": {"&lt; attribute name &gt;:Unknown"} for each attribute type defined for the event type \n                        \n                        \n                        \n                ---\n                Examples:\n                \n                text: "Patient ate breakfast this morning. He seems less anxious."\n                output: {\n                "events": [\n                    {"event_id": "e1",\n                    "event_type": "Eating",\n                    "text_quote":"Patient ate breakfast this morning",\n                    "attributes": {"food": "breakfast", \n                                   "amount": "Unknown",\n                                   "method": "Unknown",\n                                   "negation": "false",\n                                   "time":"morning",\n                                   "caused_by":"Unknown"}\n                    }\n                ],\n                "order":[]\n                }\n                \n                text: "Patient reported severe abdominal pain."\n                output: {\n                "events": [\n                    {"event_id": "e1",\n                    "event_type": "Pain",\n                    "text_quote": "severe abdominal Pain",\n                    "attributes": {"severity": "severe", \n                                   "location": "abdominal",\n                                   "duration": "Unknown",\n                                   "negation": "false",\n                                   "time":"Unknown",\n                                   "caused_by":"Unknown"}\n                    }\n                ],\n                "order":[]\n                }\n                \n                text: "Patient called his son around 3 pm."\n                output: {\n                "events": [\n                    {"event_id": "e1",\n                    "event_type": "Family",\n                    "text_quote": "called his son around 3 pm",\n                    "attributes": {"interaction": "call", \n                                    "relation": "son",\n                                    "negation": "false",\n                                    "time":"3 pm",\n                                    "caused_by":"Unknown"}\n                    }\n                ],\n                "order":[]\n                }\n                \n                text: "Patient had a loose stool overnight."\n                output: {\n                "events": [\n                    {"event_id": "e1",\n                    "event_type": "Excretion",\n                    "text_quote": "loose stool overnight",\n                    "attributes": {"type": "stool", \n                                   "quality": "loose", \n                                   "frequency":"overnight", \n                                   "negation": "false",\n                                   "time":"night",\n                                   "caused_by":"Unknown"}\n                    }\n                ],\n                "order":[]\n                }\n                \n                text: "Patient was able to sleep well last night."\n                output: {\n                "events": [\n                    {"event_id": "e1",\n                    "event_type": "Sleep",\n                    "text_quote": "sleep well last night",\n                    "attributes": {"quality": "well",\n                                    "duration": "Unknown", \n                                    "negation": "false",\n                                    "time":"night",\n                                    "caused_by":"Unknown"}\n                    }\n                ],\n                "order":[]\n                }\n                \n                text: "The patient couldn\'t sleep due to severe pain."\n                output: {\n                "events": [\n                    {"event_id": "e1",\n                    "event_type": "Sleep",\n                    "text_quote": "couldn\'t sleep",\n                    "attributes": {"quality": "poor", \n                                    "duration": "Unknown",\n                                    "negation": "true",\n                                    "time":"Unknown",\n                                    "caused_by":"Pain"}\n                    },\n                    {"event_id": "e2",\n                    "event_type": "Pain",\n                    "text_quote": "severe pain",\n                    "attributes": {"severity": "severe", \n                                    "location": "Unknown", \n                                    "duration": "Unknown", \n                                    "time":"Unknown",\n                                    "caused_by":"Unknown"}\n                    }\n                ],\n                "order":["e1", "after", "e2"]\n                }\n                \n                text: "The patient complained of severe back pain, was given Tylenol, but the pain persisted and he was then prescribed stronger morphine."\n                output: {\n                "events": [\n                    {"event_id": "e1",\n                    "event_type": "Pain",\n                    "text_quote": "complained of severe back pain",\n                    "attributes": {"severity": "severe", \n                                    "location": "back",\n                                    "duration": "Unknown", \n                                    "time":"Unknown",\n                                    "caused_by":"Unknown"}\n                    },\n                    {"event_id": "e2",\n                    "event_type": "Pain",\n                    "text_quote": "pain persisted",\n                    "attributes": {"severity": "severe", \n                                   "location": "back",\n                                   "duration": "persistent", \n                                   "time":"after Tylenol",\n                                   "caused_by":"Unknown"}\n                    }\n                ],\n                "order":[["e1", "before", "e2"]]\n                }\n                \n                        ', 'event_detection_time': 18.101382217020728}</t>
+        </is>
+      </c>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t>['Eating', 'Excretion', 'Family', 'Sleep', 'Pain']</t>
+        </is>
+      </c>
+      <c r="H16" t="inlineStr">
+        <is>
+          <t>[{'Eating': {'food': 'Unknown', 'amount': '0', 'method': 'Unknown', 'negation': 'true', 'time': 'today', 'caused_by': 'Unknown'}}, {'Excretion': {'type': 'urine', 'frequency': '~900cc', 'quality': 'Unknown', 'negation': 'false', 'time': 'day', 'caused_by': 'lasix'}}, {'Family': {'interaction': 'visit', 'relation': 'mother, sisters, brother, husband', 'negation': 'false', 'time': 'Unknown', 'caused_by': 'Unknown'}}, {'Sleep': {'quality': 'good', 'duration': 'Unknown', 'negation': 'false', 'time': 'since line was pulled', 'caused_by': 'line being pulled'}}, {'Pain': {'severity': 'Unknown', 'location': 'Unknown', 'duration': 'Unknown', 'negation': 'false', 'time': 'upon return from lab', 'caused_by': 'discomfort'}}]</t>
+        </is>
+      </c>
+      <c r="I16" t="inlineStr">
+        <is>
+          <t>['she has eaten nothing today.', 'she has had fair response to lasix and is presently ~900cc neg for the day.', 'her mother sisters and brother and [**name2 (ni) 10815**] were in to visit as well as her husband.', 'she has finally been sleeping since line was pulled.', 'she received morphine 2mg iv upon return from lab to help with discomfort.']</t>
+        </is>
+      </c>
+      <c r="J16" t="inlineStr">
+        <is>
+          <t>[[]]</t>
+        </is>
+      </c>
+      <c r="K16" t="inlineStr">
+        <is>
+          <t>{'text': 'ccu nsg note: alt in cv/cardiomyopathy\ns: "i think i do feel better".\no: for complete vs see ccu flow sheet\nthis 39y old woman comes to [**hospital1 2**] from osh with ~3mo history of sob and 3 week history of increasing sob, fever, lower extremity edema and severe exercise intolerance. echo shows ef of 10% with cardiomyopathy of unknown origen. she started captopril overnight with previous carvedolol dose d/c.\ncv: patient initially had bp in low 100s, but by 10pm dinamap and auscultated bp were unobtainable. doppler \rbps  weree  in the mid 80s with heart rate in the low 100s st with frequent pvcs. urine output also dropped and lungs were more congested with near constant coughing. it was decided to send here to the cath lab for swan placement. prior to going multiple radial aline attempts were made with no success. attempts in cath lab also failed and r 4f femoral aline was placed. in lab she had swan placed thru r ij. ra was 12, rv 45/16, pa 43/21 with wedge 17. co was 3.2 with index 1.53. she was boluses with 50mic/kilo of milrinone and started on drip at .375mic/kilo. patient returned to ccu ~1430 with aline in r groin, rij swan and milrinone running. co/ci have improved and at 1800 numbers were 6.0/2.83/853. paps have ranged 40s/14-20 with wedge 14 and ra [**6-2**]. heart rate has increased to  108-120s with frequent pvcs, runs of ventricular trigemininy and episodes of alternans from systole seen by aline tracing. at 1530 anesthesia was able to place a l radial aline and at 1600 femoral aline was removed. there is no ooze or hematoma and all pulses palpable. all extremities remain cool. extremities were dusky this am, but color has improved since milrinone added. she received lasix 20mg ivp at 1530. bp now low 100s to 1-teens /60-70s. cough has greatly improved. nimc transplant team has been notified and if patient needs immediate intervention she will be transfered there, if not she will stay here and see them as outpatient if cardiomyopathy does not adequately resolve.\nid: temp on return from lab was 101.7. tylenol given and bc x 2 and urine sent. wbc 16.1 (10.4 this am).\nresp: breath sounds in am were crackles primarily at bases but by 10am she has decreased breath sounds throughout with experitory squeeking noise. she was sating 98-100% but coughing very frequently despite anti-tussives. since returning from the lab her breathing has much improved with only decreased bs at bases. she is sating 97% on 3l np. and gas was 7.47/29/80/22.\ngi: apetite poor and she has eaten nothing today. no bm\nrenal: she has had fair response to lasix and is presently ~900cc neg for the day.\nms/comfort: patient was very anxious about going to lab and also have so many sticks for aline. she received ativan .5mg iv pre and post lab with good results. she also received morphine 2mg iv upon return from lab to help with discomfort.  she has finally been sleeping since line was pulled.\nsocial: her mother sisters and brother and [**name2 (ni) 10815**] were in to visit as well as her husband. [**name (ni) **] husband will sleep here tonight. family aware of severity of patient condition but\n', 'event': ['Eating', 'Excretion', 'Family', 'Pain', 'Sleep'], 'event_id': ['e1', 'e2', 'e3', 'e4', 'e5'], 'phrase': '', 'raw_output': '{\n  "events": [\n    {\n      "event_id": "e1",\n      "event_type": "Eating",\n      "text_quote": "she has eaten nothing today.",\n      "attributes": {\n        "food": "Unknown",\n        "amount": "Unknown",\n        "method": "Unknown",\n        "negation": true,\n        "time": "today",\n        "caused_by": "Unknown"\n      }\n    },\n    {\n      "event_id": "e2",\n      "event_type": "Excretion",\n      "text_quote": "she has had fair response to lasix and is presently ~900cc neg for the day.",\n      "attributes": {\n        "type": "urine",\n        "frequency": "Unknown",\n        "quality": "Unknown",\n        "negation": false,\n        "time": "today",\n        "caused_by": "lasix"\n      }\n    },\n    {\n      "event_id": "e3",\n      "event_type": "Family",\n      "text_quote": "her mother sisters and brother and [**name2 (ni) 10815**] were in to visit as well as her husband.",\n      "attributes": {\n        "interaction": "visit",\n        "relation": "mother, sisters, brother, husband",\n        "negation": false,\n        "time": "Unknown",\n        "caused_by": "Unknown"\n      }\n    },\n    {\n      "event_id": "e4",\n      "event_type": "Pain",\n      "text_quote": "she received morphine 2mg iv upon return from lab to help with discomfort.",\n      "attributes": {\n        "severity": "Unknown",\n        "location": "Unknown",\n        "duration": "Unknown",\n        "negation": false,\n        "time": "upon return from lab",\n        "caused_by": "discomfort"\n      }\n    },\n    {\n      "event_id": "e5",\n      "event_type": "Sleep",\n      "text_quote": "she has finally been sleeping since line was pulled.",\n      "attributes": {\n        "quality": "Unknown",\n        "duration": "Unknown",\n        "negation": false,\n        "time": "since line was pulled",\n        "caused_by": "Unknown"\n      }\n    }\n  ],\n  "order": [\n    ["e1", "before", "e2"],\n    ["e2", "before", "e3"],\n    ["e3", "before", "e4"],\n    ["e4", "before", "e5"]\n  ]\n}', 'attributes': [{'Eating': {'food': 'Unknown', 'amount': 'Unknown', 'method': 'Unknown', 'negation': True, 'time': 'today', 'caused_by': 'Unknown'}}, {'Excretion': {'type': 'urine', 'frequency': 'Unknown', 'quality': 'Unknown', 'negation': False, 'time': 'today', 'caused_by': 'lasix'}}, {'Family': {'interaction': 'visit', 'relation': 'mother, sisters, brother, husband', 'negation': False, 'time': 'Unknown', 'caused_by': 'Unknown'}}, {'Pain': {'severity': 'Unknown', 'location': 'Unknown', 'duration': 'Unknown', 'negation': False, 'time': 'upon return from lab', 'caused_by': 'discomfort'}}, {'Sleep': {'quality': 'Unknown', 'duration': 'Unknown', 'negation': False, 'time': 'since line was pulled', 'caused_by': 'Unknown'}}], 'orders': [[['e1', 'before', 'e2'], ['e2', 'before', 'e3'], ['e3', 'before', 'e4'], ['e4', 'before', 'e5']]], 'text_quotes': ['she has eaten nothing today.', 'she has had fair response to lasix and is presently ~900cc neg for the day.', 'her mother sisters and brother and [**name2 (ni) 10815**] were in to visit as well as her husband.', 'she received morphine 2mg iv upon return from lab to help with discomfort.', 'she has finally been sleeping since line was pulled.'], 'event_name_prompt': 'Given the text: ccu nsg note: alt in cv/cardiomyopathy\ns: "i think i do feel better".\no: for complete vs see ccu flow sheet\nthis 39y old woman comes to [**hospital1 2**] from osh with ~3mo history of sob and 3 week history of increasing sob, fever, lower extremity edema and severe exercise intolerance. echo shows ef of 10% with cardiomyopathy of unknown origen. she started captopril overnight with previous carvedolol dose d/c.\ncv: patient initially had bp in low 100s, but by 10pm dinamap and auscultated bp were unobtainable. doppler \rbps  weree  in the mid 80s with heart rate in the low 100s st with frequent pvcs. urine output also dropped and lungs were more congested with near constant coughing. it was decided to send here to the cath lab for swan placement. prior to going multiple radial aline attempts were made with no success. attempts in cath lab also failed and r 4f femoral aline was placed. in lab she had swan placed thru r ij. ra was 12, rv 45/16, pa 43/21 with wedge 17. co was 3.2 with index 1.53. she was boluses with 50mic/kilo of milrinone and started on drip at .375mic/kilo. patient returned to ccu ~1430 with aline in r groin, rij swan and milrinone running. co/ci have improved and at 1800 numbers were 6.0/2.83/853. paps have ranged 40s/14-20 with wedge 14 and ra [**6-2**]. heart rate has increased to  108-120s with frequent pvcs, runs of ventricular trigemininy and episodes of alternans from systole seen by aline tracing. at 1530 anesthesia was able to place a l radial aline and at 1600 femoral aline was removed. there is no ooze or hematoma and all pulses palpable. all extremities remain cool. extremities were dusky this am, but color has improved since milrinone added. she received lasix 20mg ivp at 1530. bp now low 100s to 1-teens /60-70s. cough has greatly improved. nimc transplant team has been notified and if patient needs immediate intervention she will be transfered there, if not she will stay here and see them as outpatient if cardiomyopathy does not adequately resolve.\nid: temp on return from lab was 101.7. tylenol given and bc x 2 and urine sent. wbc 16.1 (10.4 this am).\nresp: breath sounds in am were crackles primarily at bases but by 10am she has decreased breath sounds throughout with experitory squeeking noise. she was sating 98-100% but coughing very frequently despite anti-tussives. since returning from the lab her breathing has much improved with only decreased bs at bases. she is sating 97% on 3l np. and gas was 7.47/29/80/22.\ngi: apetite poor and she has eaten nothing today. no bm\nrenal: she has had fair response to lasix and is presently ~900cc neg for the day.\nms/comfort: patient was very anxious about going to lab and also have so many sticks for aline. she received ativan .5mg iv pre and post lab with good results. she also received morphine 2mg iv upon return from lab to help with discomfort.  she has finally been sleeping since line was pulled.\nsocial: her mother sisters and brother and [**name2 (ni) 10815**] were in to visit as well as her husband. [**name (ni) **] husband will sleep here tonight. family aware of severity of patient condition but\n, \n                        and the following event types with their definitions: Eating : The patient takes food into their body by mouth.\nExcretion : The patient discharges waste matter from their body.\nFamily : The patient has a visit, call, or communication with a family member.\nPain : The patient reports or shows signs of pain.\nSleep : The patient sleeps or the sleep’s quality or quantity is described.\nUnknown : choose "Unknown" if none of the other event type are applicable. \n                        ---\n                        Your task:\n                        0. Identify ALL events in the text (zero, one, or more).\n1. For each event, assign an event_type from the list above.\n2. If multiple event of same type is mentioned, assign the event_type multiple times\n3. Extract attributes for each event using ONLY the allowed attributes listed below.\n4. Use keyword evidence (Ki) ONLY if it is consistent with the text context.\n5. Output strictly valid JSON following the schema below.\n                        ---\n                        Classification Rules:\n                        - A text may contain multiple events of the same or different types.\n- Create a separate event object for each event mention.\n- If the text is explicitly a NEGATION (e.g., "denies pain"), do not extract that event.\n- If the text describes a FUTURE or HYPOTHETICAL event (e.g., "will eat tomorrow"), ignore it.\n- A valid event should have occurred in the recent past or is occurring during the time of writing of the text.\n- If no events are found or if unsure, return {"events": []}\n                        \n                        ---\n                                    Attributes allowed:\n                                    {\'Eating\': {\'food\': \'&lt;string&gt; # e.g., pancakes, porridge, etc.\', \'amount\': \'&lt;string&gt; # e.g., 1, 2 bowls, etc.\', \'method\': \'&lt;string&gt;  # e.g., oral, tube, etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, evening etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}, \'Excretion\': {\'type\': \'&lt;string&gt; # e.g., urine, stool, etc.\', \'frequency\': \'&lt;string&gt; # e.g., 2x, once, etc.\', \'quality\': \'&lt;string&gt; # e.g., loose, hard, etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, evening etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}, \'Family\': {\'interaction\': \'&lt;string&gt; # e.g., visit, call, communication, etc.\', \'relation\': \'&lt;string&gt; # e.g., mother, son, etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, evening etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}, \'Pain\': {\'severity\': \'&lt;string&gt; # e.g., mild, moderate, severe, numeric scale if present, etc.\', \'location\': \'&lt;string&gt; # e.g., right knee, head, etc.\', \'duration\': \'&lt;string&gt; # e.g., all night, 3 hours, etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, evening etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}, \'Sleep\': {\'quality\': \'&lt;string&gt; # e.g., good, poor, restless, etc.\', \'duration\': \'&lt;string&gt; # e.g., 6 hours, phrases like "all night", etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, evening etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}}\n                                    If no relevant attribute exists for an event, return an empty object {}.\n                                    \n                        \n                        ---\n                                    Keyword evidence (Ki):\n                                    Additional facts: A keyword matching algorithm without context detected keyword(s) (\'mother\', \'sleep\', \'husband\', \'family\', \'urine\', \'sisters\', \'eaten\', \'brother\', \'sleeping\').\n                                    Use this only as a pointer. If context contradicts, ignore.\n                        ---\n                        Output Schema (strict):\n                        {\n                                    "events": [\n                                        {\n                                        "event_id": "&lt; A unique id eg.: e1 | e2 |...&gt;"\n                                        "event_type": "&lt;Pain | Sleep | Excretion | Eating | Family&gt;",\n                                        "text_quote": "&lt;fragement from the text indicating the event_type&gt;",\n                "attributes": {\n                    "&lt;attribute_name&gt;": "&lt;attribute_value&gt;"\n                }\n                                        }\n                                    ],\n                                    "order": [\n                                        ["e1", "before" | "after" | "simultaneous", "e2" ]\n                                    ]\n                                    }\n                        \n                            Rules:\n                                - Ensure the output is valid JSON (parseable).\n                                - "eventS" must always be an array (can be empty).\n                                - Multiple instances of the same event type appear with different ids.\n                                - Events appear in the array in the same order in which they appear in the text.\n                                - Their partial orders can be expressed using the "order" section.\n                                - Do not include extra keys, comments, or text.\n                                - Each object in "events" must contain "event_type", "text_quote", and "attributes".\n                                - If an event attribute type has no value mentioned, return "attributes": {"&lt; attribute name &gt;:Unknown"} for each attribute type defined for the event type \n                        \n                        \n                        \n                        ', 'event_detection_time': 18.14297115500085}</t>
+        </is>
+      </c>
+      <c r="L16" t="inlineStr">
+        <is>
           <t>['Eating', 'Excretion', 'Family', 'Pain', 'Sleep']</t>
         </is>
       </c>
-      <c r="G16" t="inlineStr">
-        <is>
-          <t>[{'Eating': {'food': 'Unknown', 'amount': '0', 'method': 'Unknown', 'negation': True, 'time': 'today', 'caused_by': 'Unknown'}}, {'Excretion': {'type': 'urine', 'frequency': '~900cc', 'quality': 'Unknown', 'negation': False, 'time': 'today', 'caused_by': 'lasix'}}, {'Family': {'interaction': 'visit', 'relation': 'mother, sisters, brother, husband', 'negation': False, 'time': 'Unknown', 'caused_by': 'Unknown'}}, {'Pain': {'severity': 'Unknown', 'location': 'Unknown', 'duration': 'Unknown', 'negation': False, 'time': 'upon return from lab', 'caused_by': 'discomfort'}}, {'Sleep': {'quality': 'Unknown', 'duration': 'since line was pulled', 'negation': False, 'time': 'since line was pulled', 'caused_by': 'line was pulled'}}]</t>
-        </is>
-      </c>
-      <c r="H16" t="inlineStr">
+      <c r="M16" t="inlineStr">
+        <is>
+          <t>[{'Eating': {'food': 'Unknown', 'amount': 'Unknown', 'method': 'Unknown', 'negation': True, 'time': 'today', 'caused_by': 'Unknown'}}, {'Excretion': {'type': 'urine', 'frequency': 'Unknown', 'quality': 'Unknown', 'negation': False, 'time': 'today', 'caused_by': 'lasix'}}, {'Family': {'interaction': 'visit', 'relation': 'mother, sisters, brother, husband', 'negation': False, 'time': 'Unknown', 'caused_by': 'Unknown'}}, {'Pain': {'severity': 'Unknown', 'location': 'Unknown', 'duration': 'Unknown', 'negation': False, 'time': 'upon return from lab', 'caused_by': 'discomfort'}}, {'Sleep': {'quality': 'Unknown', 'duration': 'Unknown', 'negation': False, 'time': 'since line was pulled', 'caused_by': 'Unknown'}}]</t>
+        </is>
+      </c>
+      <c r="N16" t="inlineStr">
         <is>
           <t>['she has eaten nothing today.', 'she has had fair response to lasix and is presently ~900cc neg for the day.', 'her mother sisters and brother and [**name2 (ni) 10815**] were in to visit as well as her husband.', 'she received morphine 2mg iv upon return from lab to help with discomfort.', 'she has finally been sleeping since line was pulled.']</t>
         </is>
       </c>
-      <c r="I16" t="inlineStr">
-        <is>
-          <t>{'text': 'ccu nsg note: alt in cv/cardiomyopathy\ns: "i think i do feel better".\no: for complete vs see ccu flow sheet\nthis 39y old woman comes to [**hospital1 2**] from osh with ~3mo history of sob and 3 week history of increasing sob, fever, lower extremity edema and severe exercise intolerance. echo shows ef of 10% with cardiomyopathy of unknown origen. she started captopril overnight with previous carvedolol dose d/c.\ncv: patient initially had bp in low 100s, but by 10pm dinamap and auscultated bp were unobtainable. doppler \rbps  weree  in the mid 80s with heart rate in the low 100s st with frequent pvcs. urine output also dropped and lungs were more congested with near constant coughing. it was decided to send here to the cath lab for swan placement. prior to going multiple radial aline attempts were made with no success. attempts in cath lab also failed and r 4f femoral aline was placed. in lab she had swan placed thru r ij. ra was 12, rv 45/16, pa 43/21 with wedge 17. co was 3.2 with index 1.53. she was boluses with 50mic/kilo of milrinone and started on drip at .375mic/kilo. patient returned to ccu ~1430 with aline in r groin, rij swan and milrinone running. co/ci have improved and at 1800 numbers were 6.0/2.83/853. paps have ranged 40s/14-20 with wedge 14 and ra [**6-2**]. heart rate has increased to  108-120s with frequent pvcs, runs of ventricular trigemininy and episodes of alternans from systole seen by aline tracing. at 1530 anesthesia was able to place a l radial aline and at 1600 femoral aline was removed. there is no ooze or hematoma and all pulses palpable. all extremities remain cool. extremities were dusky this am, but color has improved since milrinone added. she received lasix 20mg ivp at 1530. bp now low 100s to 1-teens /60-70s. cough has greatly improved. nimc transplant team has been notified and if patient needs immediate intervention she will be transfered there, if not she will stay here and see them as outpatient if cardiomyopathy does not adequately resolve.\nid: temp on return from lab was 101.7. tylenol given and bc x 2 and urine sent. wbc 16.1 (10.4 this am).\nresp: breath sounds in am were crackles primarily at bases but by 10am she has decreased breath sounds throughout with experitory squeeking noise. she was sating 98-100% but coughing very frequently despite anti-tussives. since returning from the lab her breathing has much improved with only decreased bs at bases. she is sating 97% on 3l np. and gas was 7.47/29/80/22.\ngi: apetite poor and she has eaten nothing today. no bm\nrenal: she has had fair response to lasix and is presently ~900cc neg for the day.\nms/comfort: patient was very anxious about going to lab and also have so many sticks for aline. she received ativan .5mg iv pre and post lab with good results. she also received morphine 2mg iv upon return from lab to help with discomfort.  she has finally been sleeping since line was pulled.\nsocial: her mother sisters and brother and [**name2 (ni) 10815**] were in to visit as well as her husband. [**name (ni) **] husband will sleep here tonight. family aware of severity of patient condition but\n', 'event': ['Eating', 'Excretion', 'Excretion', 'Family', 'Pain', 'Sleep'], 'phrase': '', 'raw_output': '{\n  "events": [\n    {\n      "event_type": "Eating",\n      "text_quote": "apetite poor and she has eaten nothing today.",\n      "attributes": {\n        "food": "Unknown",\n        "amount": "Unknown",\n        "method": "Unknown",\n        "negation": true,\n        "time": "today",\n        "caused_by": "Unknown"\n      }\n    },\n    {\n      "event_type": "Excretion",\n      "text_quote": "renal: she has had fair response to lasix and is presently ~900cc neg for the day.",\n      "attributes": {\n        "type": "urine",\n        "frequency": "Unknown",\n        "quality": "Unknown",\n        "negation": false,\n        "time": "today",\n        "caused_by": "lasix"\n      }\n    },\n    {\n      "event_type": "Excretion",\n      "text_quote": "no bm",\n      "attributes": {\n        "type": "stool",\n        "frequency": "Unknown",\n        "quality": "Unknown",\n        "negation": true,\n        "time": "today",\n        "caused_by": "Unknown"\n      }\n    },\n    {\n      "event_type": "Family",\n      "text_quote": "her mother sisters and brother and [**name2 (ni) 10815**] were in to visit as well as her husband.",\n      "attributes": {\n        "interaction": "visit",\n        "relation": "mother, sisters, brother, husband",\n        "negation": false,\n        "time": "Unknown",\n        "caused_by": "Unknown"\n      }\n    },\n    {\n      "event_type": "Pain",\n      "text_quote": "she received morphine 2mg iv upon return from lab to help with discomfort.",\n      "attributes": {\n        "severity": "Unknown",\n        "location": "Unknown",\n        "duration": "Unknown",\n        "negation": false,\n        "time": "upon return from lab",\n        "caused_by": "discomfort"\n      }\n    },\n    {\n      "event_type": "Sleep",\n      "text_quote": "she has finally been sleeping since line was pulled.",\n      "attributes": {\n        "quality": "Unknown",\n        "duration": "Unknown",\n        "negation": false,\n        "time": "since line was pulled",\n        "caused_by": "line was pulled"\n      }\n    }\n  ]\n}', 'attributes': [{'Eating': {'food': 'Unknown', 'amount': 'Unknown', 'method': 'Unknown', 'negation': True, 'time': 'today', 'caused_by': 'Unknown'}}, {'Excretion': {'type': 'urine', 'frequency': 'Unknown', 'quality': 'Unknown', 'negation': False, 'time': 'today', 'caused_by': 'lasix'}}, {'Excretion': {'type': 'stool', 'frequency': 'Unknown', 'quality': 'Unknown', 'negation': True, 'time': 'today', 'caused_by': 'Unknown'}}, {'Family': {'interaction': 'visit', 'relation': 'mother, sisters, brother, husband', 'negation': False, 'time': 'Unknown', 'caused_by': 'Unknown'}}, {'Pain': {'severity': 'Unknown', 'location': 'Unknown', 'duration': 'Unknown', 'negation': False, 'time': 'upon return from lab', 'caused_by': 'discomfort'}}, {'Sleep': {'quality': 'Unknown', 'duration': 'Unknown', 'negation': False, 'time': 'since line was pulled', 'caused_by': 'line was pulled'}}], 'text_quotes': ['apetite poor and she has eaten nothing today.', 'renal: she has had fair response to lasix and is presently ~900cc neg for the day.', 'no bm', 'her mother sisters and brother and [**name2 (ni) 10815**] were in to visit as well as her husband.', 'she received morphine 2mg iv upon return from lab to help with discomfort.', 'she has finally been sleeping since line was pulled.'], 'event_name_prompt': 'Given the text: ccu nsg note: alt in cv/cardiomyopathy\ns: "i think i do feel better".\no: for complete vs see ccu flow sheet\nthis 39y old woman comes to [**hospital1 2**] from osh with ~3mo history of sob and 3 week history of increasing sob, fever, lower extremity edema and severe exercise intolerance. echo shows ef of 10% with cardiomyopathy of unknown origen. she started captopril overnight with previous carvedolol dose d/c.\ncv: patient initially had bp in low 100s, but by 10pm dinamap and auscultated bp were unobtainable. doppler \rbps  weree  in the mid 80s with heart rate in the low 100s st with frequent pvcs. urine output also dropped and lungs were more congested with near constant coughing. it was decided to send here to the cath lab for swan placement. prior to going multiple radial aline attempts were made with no success. attempts in cath lab also failed and r 4f femoral aline was placed. in lab she had swan placed thru r ij. ra was 12, rv 45/16, pa 43/21 with wedge 17. co was 3.2 with index 1.53. she was boluses with 50mic/kilo of milrinone and started on drip at .375mic/kilo. patient returned to ccu ~1430 with aline in r groin, rij swan and milrinone running. co/ci have improved and at 1800 numbers were 6.0/2.83/853. paps have ranged 40s/14-20 with wedge 14 and ra [**6-2**]. heart rate has increased to  108-120s with frequent pvcs, runs of ventricular trigemininy and episodes of alternans from systole seen by aline tracing. at 1530 anesthesia was able to place a l radial aline and at 1600 femoral aline was removed. there is no ooze or hematoma and all pulses palpable. all extremities remain cool. extremities were dusky this am, but color has improved since milrinone added. she received lasix 20mg ivp at 1530. bp now low 100s to 1-teens /60-70s. cough has greatly improved. nimc transplant team has been notified and if patient needs immediate intervention she will be transfered there, if not she will stay here and see them as outpatient if cardiomyopathy does not adequately resolve.\nid: temp on return from lab was 101.7. tylenol given and bc x 2 and urine sent. wbc 16.1 (10.4 this am).\nresp: breath sounds in am were crackles primarily at bases but by 10am she has decreased breath sounds throughout with experitory squeeking noise. she was sating 98-100% but coughing very frequently despite anti-tussives. since returning from the lab her breathing has much improved with only decreased bs at bases. she is sating 97% on 3l np. and gas was 7.47/29/80/22.\ngi: apetite poor and she has eaten nothing today. no bm\nrenal: she has had fair response to lasix and is presently ~900cc neg for the day.\nms/comfort: patient was very anxious about going to lab and also have so many sticks for aline. she received ativan .5mg iv pre and post lab with good results. she also received morphine 2mg iv upon return from lab to help with discomfort.  she has finally been sleeping since line was pulled.\nsocial: her mother sisters and brother and [**name2 (ni) 10815**] were in to visit as well as her husband. [**name (ni) **] husband will sleep here tonight. family aware of severity of patient condition but\n, \n                        and the following event types with their definitions: Eating : The patient takes food into their body by mouth.\nExcretion : The patient discharges waste matter from their body.\nFamily : The patient has a visit, call, or communication with a family member.\nPain : The patient reports or shows signs of pain.\nSleep : The patient sleeps or the sleep’s quality or quantity is described.\nUnknown : choose "Unknown" if none of the other event type are applicable. \n                        ---\n                        Your task:\n                        0. Identify ALL events in the text (zero, one, or more).\n1. For each event, assign an event_type from the list above.\n2. If multiple event of same type is mentioned, assign the event_type multiple times\n3. Extract attributes for each event using ONLY the allowed attributes listed below.\n4. Use keyword evidence (Ki) ONLY if it is consistent with the text context.\n5. Output strictly valid JSON following the schema below.\n                        ---\n                        Classification Rules:\n                        - A text may contain multiple events of the same or different types.\n- Create a separate event object for each event mention.\n- If the text is explicitly a NEGATION (e.g., "denies pain"), do not extract that event.\n- If the text describes a FUTURE or HYPOTHETICAL event (e.g., "will eat tomorrow"), ignore it.\n- A valid event should have occurred in the recent past or is occurring during the time of writing of the text.\n- If no events are found or if unsure, return {"events": []}\n                        \n                        ---\n                                    Attributes allowed:\n                                    {\'Eating\': {\'food\': \'&lt;string&gt; # e.g., pancakes, porridge, etc.\', \'amount\': \'&lt;string&gt; # e.g., 1, 2 bowls, etc.\', \'method\': \'&lt;string&gt;  # e.g., oral, tube, etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, after shower, etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}, \'Excretion\': {\'type\': \'&lt;string&gt; # e.g., urine, stool, etc.\', \'frequency\': \'&lt;string&gt; # e.g., 2x, once, etc.\', \'quality\': \'&lt;string&gt; # e.g., loose, hard, etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, after shower, etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}, \'Family\': {\'interaction\': \'&lt;string&gt; # e.g., visit, call, communication, etc.\', \'relation\': \'&lt;string&gt; # e.g., mother, son, etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, after shower, etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}, \'Pain\': {\'severity\': \'&lt;string&gt; # e.g., mild, moderate, severe, numeric scale if present, etc.\', \'location\': \'&lt;string&gt; # e.g., right knee, head, etc.\', \'duration\': \'&lt;string&gt; # e.g., all night, 3 hours, etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, after shower, etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}, \'Sleep\': {\'quality\': \'&lt;string&gt; # e.g., good, poor, restless, etc.\', \'duration\': \'&lt;string&gt; # e.g., 6 hours, phrases like "all night", etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, after shower, etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}}\n                                    If no relevant attribute exists for an event, return an empty object {}.\n                                    \n                        \n                        ---\n                                    Keyword evidence (Ki):\n                                    Additional facts: A keyword matching algorithm without context detected keyword(s) [\'urine\', \'eaten\', \'brother\', \'sleeping\', \'mother\', \'sleep\', \'family\', \'sisters\', \'husband\'].\n                                    Use this only as a pointer. If context contradicts, ignore.\n                        ---\n                        Output Schema (strict):\n                        {\n                                    "events": [\n                                        {\n                                        "event_type": "&lt;Pain | Sleep | Excretion | Eating | Family&gt;",\n                                        "text_quote": "&lt;fragement from the text indicating &gt;",\n                "attributes": {\n                    "&lt;attribute_name&gt;": "&lt;attribute_value&gt;"\n                }\n                                        }\n                                    ]\n                                    }\n                        \n                            Rules:\n                                - Ensure the output is valid JSON (parseable).\n                                - "eventS" must always be an array (can be empty).\n                                - Multiple instances of the same event type appear as individual elements in the event array.\n                                - Events appear in the array in the same order in which they appear in the text.\n                                - Do not include extra keys, comments, or text.\n                                - Each object in "events" must contain "event_type", "text_quote", and "attributes".\n                                -If an event attribute type has no value mentioned, return "attributes": {"&lt; attribute name &gt;:Unknown"} for each attribute type defined for the event type \n                        \n                        \n                        \n                        ', 'event_detection_time': 17.519396514006075}</t>
-        </is>
-      </c>
-      <c r="J16" t="inlineStr">
-        <is>
-          <t>['Eating', 'Excretion', 'Excretion', 'Family', 'Pain', 'Sleep']</t>
-        </is>
-      </c>
-      <c r="K16" t="inlineStr">
-        <is>
-          <t>[{'Eating': {'food': 'Unknown', 'amount': 'Unknown', 'method': 'Unknown', 'negation': True, 'time': 'today', 'caused_by': 'Unknown'}}, {'Excretion': {'type': 'urine', 'frequency': 'Unknown', 'quality': 'Unknown', 'negation': False, 'time': 'today', 'caused_by': 'lasix'}}, {'Excretion': {'type': 'stool', 'frequency': 'Unknown', 'quality': 'Unknown', 'negation': True, 'time': 'today', 'caused_by': 'Unknown'}}, {'Family': {'interaction': 'visit', 'relation': 'mother, sisters, brother, husband', 'negation': False, 'time': 'Unknown', 'caused_by': 'Unknown'}}, {'Pain': {'severity': 'Unknown', 'location': 'Unknown', 'duration': 'Unknown', 'negation': False, 'time': 'upon return from lab', 'caused_by': 'discomfort'}}, {'Sleep': {'quality': 'Unknown', 'duration': 'Unknown', 'negation': False, 'time': 'since line was pulled', 'caused_by': 'line was pulled'}}]</t>
-        </is>
-      </c>
-      <c r="L16" t="inlineStr">
-        <is>
-          <t>['apetite poor and she has eaten nothing today.', 'renal: she has had fair response to lasix and is presently ~900cc neg for the day.', 'no bm', 'her mother sisters and brother and [**name2 (ni) 10815**] were in to visit as well as her husband.', 'she received morphine 2mg iv upon return from lab to help with discomfort.', 'she has finally been sleeping since line was pulled.']</t>
-        </is>
-      </c>
-      <c r="M16" t="inlineStr">
-        <is>
-          <t>{'text': 'ccu nsg note: alt in cv/cardiomyopathy\ns: "i think i do feel better".\no: for complete vs see ccu flow sheet\nthis 39y old woman comes to [**hospital1 2**] from osh with ~3mo history of sob and 3 week history of increasing sob, fever, lower extremity edema and severe exercise intolerance. echo shows ef of 10% with cardiomyopathy of unknown origen. she started captopril overnight with previous carvedolol dose d/c.\ncv: patient initially had bp in low 100s, but by 10pm dinamap and auscultated bp were unobtainable. doppler \rbps  weree  in the mid 80s with heart rate in the low 100s st with frequent pvcs. urine output also dropped and lungs were more congested with near constant coughing. it was decided to send here to the cath lab for swan placement. prior to going multiple radial aline attempts were made with no success. attempts in cath lab also failed and r 4f femoral aline was placed. in lab she had swan placed thru r ij. ra was 12, rv 45/16, pa 43/21 with wedge 17. co was 3.2 with index 1.53. she was boluses with 50mic/kilo of milrinone and started on drip at .375mic/kilo. patient returned to ccu ~1430 with aline in r groin, rij swan and milrinone running. co/ci have improved and at 1800 numbers were 6.0/2.83/853. paps have ranged 40s/14-20 with wedge 14 and ra [**6-2**]. heart rate has increased to  108-120s with frequent pvcs, runs of ventricular trigemininy and episodes of alternans from systole seen by aline tracing. at 1530 anesthesia was able to place a l radial aline and at 1600 femoral aline was removed. there is no ooze or hematoma and all pulses palpable. all extremities remain cool. extremities were dusky this am, but color has improved since milrinone added. she received lasix 20mg ivp at 1530. bp now low 100s to 1-teens /60-70s. cough has greatly improved. nimc transplant team has been notified and if patient needs immediate intervention she will be transfered there, if not she will stay here and see them as outpatient if cardiomyopathy does not adequately resolve.\nid: temp on return from lab was 101.7. tylenol given and bc x 2 and urine sent. wbc 16.1 (10.4 this am).\nresp: breath sounds in am were crackles primarily at bases but by 10am she has decreased breath sounds throughout with experitory squeeking noise. she was sating 98-100% but coughing very frequently despite anti-tussives. since returning from the lab her breathing has much improved with only decreased bs at bases. she is sating 97% on 3l np. and gas was 7.47/29/80/22.\ngi: apetite poor and she has eaten nothing today. no bm\nrenal: she has had fair response to lasix and is presently ~900cc neg for the day.\nms/comfort: patient was very anxious about going to lab and also have so many sticks for aline. she received ativan .5mg iv pre and post lab with good results. she also received morphine 2mg iv upon return from lab to help with discomfort.  she has finally been sleeping since line was pulled.\nsocial: her mother sisters and brother and [**name2 (ni) 10815**] were in to visit as well as her husband. [**name (ni) **] husband will sleep here tonight. family aware of severity of patient condition but\n', 'event': ['Sleep', 'Pain', 'Family', 'Eating', 'Excretion'], 'phrase': '', 'raw_output': '{\n  "events": [\n    {\n      "event_type": "Sleep",\n      "text_quote": "she has finally been sleeping since line was pulled.",\n      "attributes": {\n        "quality": "good",\n        "duration": "Unknown",\n        "time": "after line was pulled",\n        "caused_by": "line being pulled"\n      }\n    },\n    {\n      "event_type": "Pain",\n      "text_quote": "she received morphine 2mg iv upon return from lab to help with discomfort.",\n      "attributes": {\n        "severity": "Unknown",\n        "location": "Unknown",\n        "duration": "Unknown",\n        "time": "upon return from lab",\n        "caused_by": "discomfort"\n      }\n    },\n    {\n      "event_type": "Family",\n      "text_quote": "her mother sisters and brother and [**name2 (ni) 10815**] were in to visit as well as her husband.",\n      "attributes": {\n        "interaction": "visit",\n        "relation": "mother, sisters, brother, husband",\n        "time": "Unknown",\n        "caused_by": "Unknown"\n      }\n    },\n    {\n      "event_type": "Eating",\n      "text_quote": "apetite poor and she has eaten nothing today.",\n      "attributes": {\n        "food": "nothing",\n        "amount": "0",\n        "method": "Unknown",\n        "time": "today",\n        "caused_by": "poor appetite"\n      }\n    },\n    {\n      "event_type": "Excretion",\n      "text_quote": "she has had fair response to lasix and is presently ~900cc neg for the day.",\n      "attributes": {\n        "type": "urine",\n        "frequency": "~900cc",\n        "quality": "Unknown",\n        "time": "today",\n        "caused_by": "lasix"\n      }\n    }\n  ]\n}', 'attributes': [{'Sleep': {'quality': 'good', 'duration': 'Unknown', 'time': 'after line was pulled', 'caused_by': 'line being pulled'}}, {'Pain': {'severity': 'Unknown', 'location': 'Unknown', 'duration': 'Unknown', 'time': 'upon return from lab', 'caused_by': 'discomfort'}}, {'Family': {'interaction': 'visit', 'relation': 'mother, sisters, brother, husband', 'time': 'Unknown', 'caused_by': 'Unknown'}}, {'Eating': {'food': 'nothing', 'amount': '0', 'method': 'Unknown', 'time': 'today', 'caused_by': 'poor appetite'}}, {'Excretion': {'type': 'urine', 'frequency': '~900cc', 'quality': 'Unknown', 'time': 'today', 'caused_by': 'lasix'}}], 'text_quotes': ['she has finally been sleeping since line was pulled.', 'she received morphine 2mg iv upon return from lab to help with discomfort.', 'her mother sisters and brother and [**name2 (ni) 10815**] were in to visit as well as her husband.', 'apetite poor and she has eaten nothing today.', 'she has had fair response to lasix and is presently ~900cc neg for the day.'], 'event_name_prompt': 'Given the text: ccu nsg note: alt in cv/cardiomyopathy\ns: "i think i do feel better".\no: for complete vs see ccu flow sheet\nthis 39y old woman comes to [**hospital1 2**] from osh with ~3mo history of sob and 3 week history of increasing sob, fever, lower extremity edema and severe exercise intolerance. echo shows ef of 10% with cardiomyopathy of unknown origen. she started captopril overnight with previous carvedolol dose d/c.\ncv: patient initially had bp in low 100s, but by 10pm dinamap and auscultated bp were unobtainable. doppler \rbps  weree  in the mid 80s with heart rate in the low 100s st with frequent pvcs. urine output also dropped and lungs were more congested with near constant coughing. it was decided to send here to the cath lab for swan placement. prior to going multiple radial aline attempts were made with no success. attempts in cath lab also failed and r 4f femoral aline was placed. in lab she had swan placed thru r ij. ra was 12, rv 45/16, pa 43/21 with wedge 17. co was 3.2 with index 1.53. she was boluses with 50mic/kilo of milrinone and started on drip at .375mic/kilo. patient returned to ccu ~1430 with aline in r groin, rij swan and milrinone running. co/ci have improved and at 1800 numbers were 6.0/2.83/853. paps have ranged 40s/14-20 with wedge 14 and ra [**6-2**]. heart rate has increased to  108-120s with frequent pvcs, runs of ventricular trigemininy and episodes of alternans from systole seen by aline tracing. at 1530 anesthesia was able to place a l radial aline and at 1600 femoral aline was removed. there is no ooze or hematoma and all pulses palpable. all extremities remain cool. extremities were dusky this am, but color has improved since milrinone added. she received lasix 20mg ivp at 1530. bp now low 100s to 1-teens /60-70s. cough has greatly improved. nimc transplant team has been notified and if patient needs immediate intervention she will be transfered there, if not she will stay here and see them as outpatient if cardiomyopathy does not adequately resolve.\nid: temp on return from lab was 101.7. tylenol given and bc x 2 and urine sent. wbc 16.1 (10.4 this am).\nresp: breath sounds in am were crackles primarily at bases but by 10am she has decreased breath sounds throughout with experitory squeeking noise. she was sating 98-100% but coughing very frequently despite anti-tussives. since returning from the lab her breathing has much improved with only decreased bs at bases. she is sating 97% on 3l np. and gas was 7.47/29/80/22.\ngi: apetite poor and she has eaten nothing today. no bm\nrenal: she has had fair response to lasix and is presently ~900cc neg for the day.\nms/comfort: patient was very anxious about going to lab and also have so many sticks for aline. she received ativan .5mg iv pre and post lab with good results. she also received morphine 2mg iv upon return from lab to help with discomfort.  she has finally been sleeping since line was pulled.\nsocial: her mother sisters and brother and [**name2 (ni) 10815**] were in to visit as well as her husband. [**name (ni) **] husband will sleep here tonight. family aware of severity of patient condition but\n, \n                        and the following event types with their definitions: Eating : The patient takes food into their body by mouth.\nExcretion : The patient discharges waste matter from their body.\nFamily : The patient has a visit, call, or communication with a family member.\nPain : The patient reports or shows signs of pain.\nSleep : The patient sleeps or the sleep’s quality or quantity is described.\nUnknown : choose "Unknown" if none of the other event type are applicable. \n                        ---\n                        Your task:\n                        0. Identify ALL events in the text (zero, one, or more).\n1. For each event, assign an event_type from the list above.\n2. If multiple event of same type is mentioned, assign the event_type multiple times\n3. Extract attributes for each event using ONLY the allowed attributes listed below.\n4. Output strictly valid JSON following the schema below.\n                        ---\n                        Classification Rules:\n                        - A text may contain multiple events of the same or different types.\n- Create a separate event object for each event mention.\n- If the text is explicitly a NEGATION (e.g., "denies pain"), do not extract that event.\n- If the text describes a FUTURE or HYPOTHETICAL event (e.g., "will eat tomorrow"), ignore it.\n- A valid event should have occurred in the recent past or is occurring during the time of writing of the text.\n- If no events are found or if unsure, return {"events": []}\n                        \n                        ---\n                                    Attributes allowed:\n                                    {\'Eating\': {\'food\': \'&lt;string&gt; # e.g., pancakes, porridge, etc.\', \'amount\': \'&lt;string&gt; # e.g., 1, 2 bowls, etc.\', \'method\': \'&lt;string&gt;  # e.g., oral, tube, etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, after shower, etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}, \'Excretion\': {\'type\': \'&lt;string&gt; # e.g., urine, stool, etc.\', \'frequency\': \'&lt;string&gt; # e.g., 2x, once, etc.\', \'quality\': \'&lt;string&gt; # e.g., loose, hard, etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, after shower, etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}, \'Family\': {\'interaction\': \'&lt;string&gt; # e.g., visit, call, communication, etc.\', \'relation\': \'&lt;string&gt; # e.g., mother, son, etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, after shower, etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}, \'Pain\': {\'severity\': \'&lt;string&gt; # e.g., mild, moderate, severe, numeric scale if present, etc.\', \'location\': \'&lt;string&gt; # e.g., right knee, head, etc.\', \'duration\': \'&lt;string&gt; # e.g., all night, 3 hours, etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, after shower, etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}, \'Sleep\': {\'quality\': \'&lt;string&gt; # e.g., good, poor, restless, etc.\', \'duration\': \'&lt;string&gt; # e.g., 6 hours, phrases like "all night", etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, after shower, etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}}\n                                    If no relevant attribute exists for an event, return an empty object {}.\n                                    \n                        \n                        \n                        ---\n                        Output Schema (strict):\n                        {\n                                    "events": [\n                                        {\n                                        "event_type": "&lt;Pain | Sleep | Excretion | Eating | Family&gt;",\n                                        "text_quote": "&lt;fragement from the text indicating &gt;",\n                "attributes": {\n                    "&lt;attribute_name&gt;": "&lt;attribute_value&gt;"\n                }\n                                        }\n                                    ]\n                                    }\n                        \n                            Rules:\n                                - Ensure the output is valid JSON (parseable).\n                                - "eventS" must always be an array (can be empty).\n                                - Multiple instances of the same event type appear as individual elements in the event array.\n                                - Events appear in the array in the same order in which they appear in the text.\n                                - Do not include extra keys, comments, or text.\n                                - Each object in "events" must contain "event_type", "text_quote", and "attributes".\n                                -If an event attribute type has no value mentioned, return "attributes": {"&lt; attribute name &gt;:Unknown"} for each attribute type defined for the event type \n                        \n                        \n                        \n                ---\n                Examples:\n                \n                text: "Patient ate breakfast this morning. He seems less anxious."\n                output: {\n                "events": [\n                    {\n                    "event_type": "Eating",\n                    "text_quote":"Patient ate breakfast this morning",\n                    "attributes": {"food": "breakfast", \n                                   "amount": "Unknown",\n                                   "method": "Unknown",\n                                   "time":"morning",\n                                   "caused_by":"Unknown"}\n                    }\n                ]\n                }\n                \n                text: "Patient reported severe abdominal pain."\n                output: {\n                "events": [\n                    {\n                    "event_type": "Pain",\n                    "text_quote": "severe abdominal Pain",\n                    "attributes": {"severity": "severe", \n                                   "location": "abdominal",\n                                   "duration": "Unknown",\n                                   "time":"Unknown",\n                                   "caused_by":"Unknown"}\n                    }\n                ]\n                }\n                \n                text: "Patient called his son around 3 pm."\n                output: {\n                "events": [\n                    {\n                    "event_type": "Family",\n                    "text_quote": "called his son around 3 pm",\n                    "attributes": {"interaction": "call", \n                                    "relation": "son",\n                                    "time":"3 pm",\n                                    "caused_by":"Unknown"}\n                    }\n                ]\n                }\n                \n                text: "Patient had a loose stool overnight."\n                output: {\n                "events": [\n                    {\n                    "event_type": "Excretion",\n                    "text_quote": "loose stool overnight",\n                    "attributes": {"type": "stool", \n                                   "quality": "loose", \n                                   "frequency":"overnight", \n                                   "time":"night",\n                                   "caused_by":"Unknown"}\n                    }\n                ]\n                }\n                \n                text: "Patient was able to sleep well last night."\n                output: {\n                "events": [\n                    {\n                    "event_type": "Sleep",\n                    "text_quote": "sleep well last night",\n                    "attributes": {"quality": "well",\n                                    "duration": "Unknown", \n                                    "time":"night",\n                                    "caused_by":"Unknown"}\n                    }\n                ]\n                }\n                \n                text: "The patient couldn\'t sleep due to severe pain."\n                output: {\n                "events": [\n                    {\n                    "event_type": "Sleep",\n                    "text_quote": "couldn\'t sleep",\n                    "attributes": {"quality": "poor", \n                                    "duration": "Unknown",\n                                   "time":"Unknown",\n                                   "caused_by":"Pain"}\n                    },\n                    {\n                    "event_type": "Pain",\n                    "text_quote": "severe pain",\n                    "attributes": {"severity": "severe", \n                                    "location": "Unknown", \n                                    "duration": "Unknown", \n                                   "time":"before Sleep",\n                                   "caused_by":"Unknown"}\n                    }\n                ]\n                }\n                \n                text: "The patient complained of severe back pain, was given Tylenol, but the pain persisted and he was then prescribed stronger morphine."\n                output: {\n                "events": [\n                    {\n                    "event_type": "Pain",\n                    "text_quote": "complained of severe back pain",\n                    "attributes": {"severity": "severe", \n                                    "location": "back",\n                                    "duration": "Unknown", \n                                    "time":"Unknown",\n                                    "caused_by":"Unknown"}\n                    },\n                    {\n                    "event_type": "Pain",\n                    "text_quote": "pain persisted",\n                    "attributes": {"severity": "severe", \n                                   "location": "back",\n                                   "duration": "persistent", \n                                   "time":"after Tylenol",\n                                   "caused_by":"Unknown"}\n                    }\n                ]\n                }\n                \n                        ', 'event_detection_time': 15.239436780000688}</t>
-        </is>
-      </c>
-      <c r="N16" t="inlineStr">
-        <is>
-          <t>['Sleep', 'Pain', 'Family', 'Eating', 'Excretion']</t>
-        </is>
-      </c>
       <c r="O16" t="inlineStr">
         <is>
-          <t>[{'Sleep': {'quality': 'good', 'duration': 'Unknown', 'time': 'after line was pulled', 'caused_by': 'line being pulled'}}, {'Pain': {'severity': 'Unknown', 'location': 'Unknown', 'duration': 'Unknown', 'time': 'upon return from lab', 'caused_by': 'discomfort'}}, {'Family': {'interaction': 'visit', 'relation': 'mother, sisters, brother, husband', 'time': 'Unknown', 'caused_by': 'Unknown'}}, {'Eating': {'food': 'nothing', 'amount': '0', 'method': 'Unknown', 'time': 'today', 'caused_by': 'poor appetite'}}, {'Excretion': {'type': 'urine', 'frequency': '~900cc', 'quality': 'Unknown', 'time': 'today', 'caused_by': 'lasix'}}]</t>
-        </is>
-      </c>
-      <c r="P16" t="inlineStr">
-        <is>
-          <t>['she has finally been sleeping since line was pulled.', 'she received morphine 2mg iv upon return from lab to help with discomfort.', 'her mother sisters and brother and [**name2 (ni) 10815**] were in to visit as well as her husband.', 'apetite poor and she has eaten nothing today.', 'she has had fair response to lasix and is presently ~900cc neg for the day.']</t>
-        </is>
-      </c>
-      <c r="Q16" t="n">
-        <v>0.003081118000409333</v>
-      </c>
-      <c r="R16" t="inlineStr">
+          <t>[[['e1', 'before', 'e2'], ['e2', 'before', 'e3'], ['e3', 'before', 'e4'], ['e4', 'before', 'e5']]]</t>
+        </is>
+      </c>
+      <c r="P16" t="n">
+        <v>0.002449888001137879</v>
+      </c>
+      <c r="Q16" t="inlineStr">
         <is>
           <t>Sleep</t>
         </is>
       </c>
-      <c r="S16" t="b">
-        <v>0</v>
+      <c r="R16" t="b">
+        <v>0</v>
+      </c>
+      <c r="S16" t="n">
+        <v>1</v>
       </c>
       <c r="T16" t="n">
         <v>1</v>
       </c>
-      <c r="U16" t="n">
-        <v>1</v>
-      </c>
-      <c r="V16" t="inlineStr">
+      <c r="U16" t="inlineStr">
         <is>
           <t>('eat', 'mother', 'sleep', 'husband', 'family', 'urine', 'sister', 'brother', 'sleeping')</t>
         </is>
       </c>
+      <c r="V16" t="n">
+        <v>18.10138221702073</v>
+      </c>
       <c r="W16" t="n">
-        <v>16.37042431000737</v>
+        <v>18.14297115500085</v>
       </c>
       <c r="X16" t="n">
-        <v>17.51939651400608</v>
+        <v>1</v>
       </c>
       <c r="Y16" t="n">
-        <v>15.23943678000069</v>
+        <v>1</v>
       </c>
       <c r="Z16" t="n">
-        <v>1</v>
-      </c>
-      <c r="AA16" t="n">
-        <v>1</v>
-      </c>
-      <c r="AB16" t="n">
-        <v>1</v>
-      </c>
-      <c r="AC16" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="17">
-      <c r="A17" t="n">
-        <v>1325551</v>
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>1325551</t>
+        </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>['Eating', 'Unknown', 'Sleep', 'Pain', 'Excretion', 'Family']</t>
+          <t>('Pain', 'Eating', 'Unknown', 'Excretion', 'Family', 'Sleep')</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>['ate', 'daughter', 'urine', 'slept', 'pain', 'sleeping', 'family', 'husband']</t>
+          <t>('daughter', 'husband', 'ate', 'family', 'pain', 'urine', 'slept', 'sleeping')</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
@@ -2632,120 +2488,111 @@
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>{'text': 'nursing progress note 1900-0700\ns: "i feel so hot"\n\no: please see carevue for complete objective data\n\ncv: st/nsr, 90-110\'s, freq pvc\'s. on amio tid. diastolic blood pressure 90-120\'s, gave captopril 6.25mg @ [**2155**], diastolic blood pressure dropped to 79/low 80\'s @ 2100. co/ci numbers unchanged from earlier in day and patient felt no side effects. milrinone remains @ 0.375mcg/kg/min. co/ci/svr-4.9/2.3/1159. cvp 6-10, w-16. r fem angio site cd&amp;i, no hematoma. pulses palp. extremities warm and pale.\n\nresp: lungs clr c dim bases. last abg-7.48/33/87/25/1, on 4l nc. mvo2-64. persistant productive cough. no c/o sob although tachypneic at times. cxr done, gave benzonatate for cough relief.\n\ngi/gu: bs present, no bm. ate very small amount for dinner. uo decreased to nothing for 2 hours. gave 250cc ivfb x 2, and uo improved slightly. +400cc for day and -700 for los. urine becoming more concentrated.\n\nneuro: lethargic/sleeping @ change of shift. a&amp;o x 3, mae. becoming more interactive as night went on, but slept well through night. c/o pain in r ear (reports having chronic ear infections), md aware.\n\nid/access: wbc down to 13.1 from 16. slightly febrile to 100.6 at start of shift, gave tylenol 650mg, and temp down to 98.9 this am. bc x2, urine cx pending. needs sputum cx. has rij pa cath, 2 piv\'s.\n\nsocial: husband stayed in room overnoc, supportive with care. patient has 20yo and 9yo daughter, should be into visit today. social work consulted.\n\na/p: 39yo female c severe cardiomyopathy and hf, unknown etiology. requiring milrinone and being worked up for heart transplant. continue to monitor hemodynamics and response to meds. obtain sputum cx, monitor temp. watch uo and fluid status. follow up with labs and cxr. emotionally support patient and family and keep updated on plan.\n', 'event': ['Eating', 'Excretion', 'Excretion', 'Pain', 'Sleep', 'Sleep', 'Family', 'Family'], 'phrase': '', 'raw_output': '{\n  "events": [\n    {\n      "event_type": "Eating",\n      "text_quote": "ate very small amount for dinner",\n      "attributes": {\n        "food": "dinner",\n        "amount": "small",\n        "method": "Unknown",\n        "negation": false,\n        "time": "night",\n        "caused_by": "Unknown"\n      }\n    },\n    {\n      "event_type": "Excretion",\n      "text_quote": "uo decreased to nothing for 2 hours",\n      "attributes": {\n        "type": "urine",\n        "frequency": "decreased",\n        "quality": "Unknown",\n        "negation": false,\n        "time": "night",\n        "caused_by": "Unknown"\n      }\n    },\n    {\n      "event_type": "Excretion",\n      "text_quote": "+400cc for day and -700 for los",\n      "attributes": {\n        "type": "urine",\n        "frequency": "increased",\n        "quality": "Unknown",\n        "negation": false,\n        "time": "day",\n        "caused_by": "Unknown"\n      }\n    },\n    {\n      "event_type": "Pain",\n      "text_quote": "c/o pain in r ear (reports having chronic ear infections)",\n      "attributes": {\n        "severity": "Unknown",\n        "location": "r ear",\n        "duration": "chronic",\n        "negation": false,\n        "time": "Unknown",\n        "caused_by": "ear infections"\n      }\n    },\n    {\n      "event_type": "Sleep",\n      "text_quote": "lethargic/sleeping @ change of shift",\n      "attributes": {\n        "quality": "poor",\n        "duration": "Unknown",\n        "negation": false,\n        "time": "night",\n        "caused_by": "Unknown"\n      }\n    },\n    {\n      "event_type": "Sleep",\n      "text_quote": "slept well through night",\n      "attributes": {\n        "quality": "well",\n        "duration": "all night",\n        "negation": false,\n        "time": "night",\n        "caused_by": "Unknown"\n      }\n    },\n    {\n      "event_type": "Family",\n      "text_quote": "husband stayed in room overnoc, supportive with care",\n      "attributes": {\n        "interaction": "visit",\n        "relation": "husband",\n        "negation": false,\n        "time": "night",\n        "caused_by": "Unknown"\n      }\n    },\n    {\n      "event_type": "Family",\n      "text_quote": "patient has 20yo and 9yo daughter, should be into visit today",\n      "attributes": {\n        "interaction": "visit",\n        "relation": "daughter",\n        "negation": false,\n        "time": "today",\n        "caused_by": "Unknown"\n      }\n    }\n  ]\n}', 'attributes': [{'Eating': {'food': 'dinner', 'amount': 'small', 'method': 'Unknown', 'negation': False, 'time': 'night', 'caused_by': 'Unknown'}}, {'Excretion': {'type': 'urine', 'frequency': 'decreased', 'quality': 'Unknown', 'negation': False, 'time': 'night', 'caused_by': 'Unknown'}}, {'Excretion': {'type': 'urine', 'frequency': 'increased', 'quality': 'Unknown', 'negation': False, 'time': 'day', 'caused_by': 'Unknown'}}, {'Pain': {'severity': 'Unknown', 'location': 'r ear', 'duration': 'chronic', 'negation': False, 'time': 'Unknown', 'caused_by': 'ear infections'}}, {'Sleep': {'quality': 'poor', 'duration': 'Unknown', 'negation': False, 'time': 'night', 'caused_by': 'Unknown'}}, {'Sleep': {'quality': 'well', 'duration': 'all night', 'negation': False, 'time': 'night', 'caused_by': 'Unknown'}}, {'Family': {'interaction': 'visit', 'relation': 'husband', 'negation': False, 'time': 'night', 'caused_by': 'Unknown'}}, {'Family': {'interaction': 'visit', 'relation': 'daughter', 'negation': False, 'time': 'today', 'caused_by': 'Unknown'}}], 'text_quotes': ['ate very small amount for dinner', 'uo decreased to nothing for 2 hours', '+400cc for day and -700 for los', 'c/o pain in r ear (reports having chronic ear infections)', 'lethargic/sleeping @ change of shift', 'slept well through night', 'husband stayed in room overnoc, supportive with care', 'patient has 20yo and 9yo daughter, should be into visit today'], 'event_name_prompt': 'Given the text: nursing progress note 1900-0700\ns: "i feel so hot"\n\no: please see carevue for complete objective data\n\ncv: st/nsr, 90-110\'s, freq pvc\'s. on amio tid. diastolic blood pressure 90-120\'s, gave captopril 6.25mg @ [**2155**], diastolic blood pressure dropped to 79/low 80\'s @ 2100. co/ci numbers unchanged from earlier in day and patient felt no side effects. milrinone remains @ 0.375mcg/kg/min. co/ci/svr-4.9/2.3/1159. cvp 6-10, w-16. r fem angio site cd&amp;i, no hematoma. pulses palp. extremities warm and pale.\n\nresp: lungs clr c dim bases. last abg-7.48/33/87/25/1, on 4l nc. mvo2-64. persistant productive cough. no c/o sob although tachypneic at times. cxr done, gave benzonatate for cough relief.\n\ngi/gu: bs present, no bm. ate very small amount for dinner. uo decreased to nothing for 2 hours. gave 250cc ivfb x 2, and uo improved slightly. +400cc for day and -700 for los. urine becoming more concentrated.\n\nneuro: lethargic/sleeping @ change of shift. a&amp;o x 3, mae. becoming more interactive as night went on, but slept well through night. c/o pain in r ear (reports having chronic ear infections), md aware.\n\nid/access: wbc down to 13.1 from 16. slightly febrile to 100.6 at start of shift, gave tylenol 650mg, and temp down to 98.9 this am. bc x2, urine cx pending. needs sputum cx. has rij pa cath, 2 piv\'s.\n\nsocial: husband stayed in room overnoc, supportive with care. patient has 20yo and 9yo daughter, should be into visit today. social work consulted.\n\na/p: 39yo female c severe cardiomyopathy and hf, unknown etiology. requiring milrinone and being worked up for heart transplant. continue to monitor hemodynamics and response to meds. obtain sputum cx, monitor temp. watch uo and fluid status. follow up with labs and cxr. emotionally support patient and family and keep updated on plan.\n, \n                        and the following event types with their definitions: Eating : The patient takes food into their body by mouth.\nExcretion : The patient discharges waste matter from their body.\nFamily : The patient has a visit, call, or communication with a family member.\nPain : The patient reports or shows signs of pain.\nSleep : The patient sleeps or the sleep’s quality or quantity is described.\nUnknown : choose "Unknown" if none of the other event type are applicable. \n                        ---\n                        Your task:\n                        0. Identify ALL events in the text (zero, one, or more).\n1. For each event, assign an event_type from the list above.\n2. If multiple event of same type is mentioned, assign the event_type multiple times\n3. Extract attributes for each event using ONLY the allowed attributes listed below.\n4. Use keyword evidence (Ki) ONLY if it is consistent with the text context.\n5. Output strictly valid JSON following the schema below.\n                        ---\n                        Classification Rules:\n                        - A text may contain multiple events of the same or different types.\n- Create a separate event object for each event mention.\n- If the text is explicitly a NEGATION (e.g., "denies pain"), do not extract that event.\n- If the text describes a FUTURE or HYPOTHETICAL event (e.g., "will eat tomorrow"), ignore it.\n- A valid event should have occurred in the recent past or is occurring during the time of writing of the text.\n- If no events are found or if unsure, return {"events": []}\n                        \n                        ---\n                                    Attributes allowed:\n                                    {\'Eating\': {\'food\': \'&lt;string&gt; # e.g., pancakes, porridge, etc.\', \'amount\': \'&lt;string&gt; # e.g., 1, 2 bowls, etc.\', \'method\': \'&lt;string&gt;  # e.g., oral, tube, etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, after shower, etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}, \'Excretion\': {\'type\': \'&lt;string&gt; # e.g., urine, stool, etc.\', \'frequency\': \'&lt;string&gt; # e.g., 2x, once, etc.\', \'quality\': \'&lt;string&gt; # e.g., loose, hard, etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, after shower, etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}, \'Family\': {\'interaction\': \'&lt;string&gt; # e.g., visit, call, communication, etc.\', \'relation\': \'&lt;string&gt; # e.g., mother, son, etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, after shower, etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}, \'Pain\': {\'severity\': \'&lt;string&gt; # e.g., mild, moderate, severe, numeric scale if present, etc.\', \'location\': \'&lt;string&gt; # e.g., right knee, head, etc.\', \'duration\': \'&lt;string&gt; # e.g., all night, 3 hours, etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, after shower, etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}, \'Sleep\': {\'quality\': \'&lt;string&gt; # e.g., good, poor, restless, etc.\', \'duration\': \'&lt;string&gt; # e.g., 6 hours, phrases like "all night", etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, after shower, etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}}\n                                    If no relevant attribute exists for an event, return an empty object {}.\n                                    \n                        \n                        ---\n                                    Keyword evidence (Ki):\n                                    Additional facts: A keyword matching algorithm without context detected keyword(s) [\'ate\', \'daughter\', \'urine\', \'slept\', \'pain\', \'sleeping\', \'family\', \'husband\'].\n                                    Use this only as a pointer. If context contradicts, ignore.\n                        ---\n                        Output Schema (strict):\n                        {\n                                    "events": [\n                                        {\n                                        "event_type": "&lt;Pain | Sleep | Excretion | Eating | Family&gt;",\n                                        "text_quote": "&lt;fragement from the text indicating &gt;",\n                "attributes": {\n                    "&lt;attribute_name&gt;": "&lt;attribute_value&gt;"\n                }\n                                        }\n                                    ]\n                                    }\n                        \n                            Rules:\n                                - Ensure the output is valid JSON (parseable).\n                                - "eventS" must always be an array (can be empty).\n                                - Multiple instances of the same event type appear as individual elements in the event array.\n                                - Events appear in the array in the same order in which they appear in the text.\n                                - Do not include extra keys, comments, or text.\n                                - Each object in "events" must contain "event_type", "text_quote", and "attributes".\n                                -If an event attribute type has no value mentioned, return "attributes": {"&lt; attribute name &gt;:Unknown"} for each attribute type defined for the event type \n                        \n                        \n                        \n                ---\n                Examples:\n                \n                text: "Patient ate breakfast this morning. He seems less anxious."\n                output: {\n                "events": [\n                    {\n                    "event_type": "Eating",\n                    "text_quote":"Patient ate breakfast this morning",\n                    "attributes": {"food": "breakfast", \n                                   "amount": "Unknown",\n                                   "method": "Unknown",\n                                   "time":"morning",\n                                   "caused_by":"Unknown"}\n                    }\n                ]\n                }\n                \n                text: "Patient reported severe abdominal pain."\n                output: {\n                "events": [\n                    {\n                    "event_type": "Pain",\n                    "text_quote": "severe abdominal Pain",\n                    "attributes": {"severity": "severe", \n                                   "location": "abdominal",\n                                   "duration": "Unknown",\n                                   "time":"Unknown",\n                                   "caused_by":"Unknown"}\n                    }\n                ]\n                }\n                \n                text: "Patient called his son around 3 pm."\n                output: {\n                "events": [\n                    {\n                    "event_type": "Family",\n                    "text_quote": "called his son around 3 pm",\n                    "attributes": {"interaction": "call", \n                                    "relation": "son",\n                                    "time":"3 pm",\n                                    "caused_by":"Unknown"}\n                    }\n                ]\n                }\n                \n                text: "Patient had a loose stool overnight."\n                output: {\n                "events": [\n                    {\n                    "event_type": "Excretion",\n                    "text_quote": "loose stool overnight",\n                    "attributes": {"type": "stool", \n                                   "quality": "loose", \n                                   "frequency":"overnight", \n                                   "time":"night",\n                                   "caused_by":"Unknown"}\n                    }\n                ]\n                }\n                \n                text: "Patient was able to sleep well last night."\n                output: {\n                "events": [\n                    {\n                    "event_type": "Sleep",\n                    "text_quote": "sleep well last night",\n                    "attributes": {"quality": "well",\n                                    "duration": "Unknown", \n                                    "time":"night",\n                                    "caused_by":"Unknown"}\n                    }\n                ]\n                }\n                \n                text: "The patient couldn\'t sleep due to severe pain."\n                output: {\n                "events": [\n                    {\n                    "event_type": "Sleep",\n                    "text_quote": "couldn\'t sleep",\n                    "attributes": {"quality": "poor", \n                                    "duration": "Unknown",\n                                   "time":"Unknown",\n                                   "caused_by":"Pain"}\n                    },\n                    {\n                    "event_type": "Pain",\n                    "text_quote": "severe pain",\n                    "attributes": {"severity": "severe", \n                                    "location": "Unknown", \n                                    "duration": "Unknown", \n                                   "time":"before Sleep",\n                                   "caused_by":"Unknown"}\n                    }\n                ]\n                }\n                \n                text: "The patient complained of severe back pain, was given Tylenol, but the pain persisted and he was then prescribed stronger morphine."\n                output: {\n                "events": [\n                    {\n                    "event_type": "Pain",\n                    "text_quote": "complained of severe back pain",\n                    "attributes": {"severity": "severe", \n                                    "location": "back",\n                                    "duration": "Unknown", \n                                    "time":"Unknown",\n                                    "caused_by":"Unknown"}\n                    },\n                    {\n                    "event_type": "Pain",\n                    "text_quote": "pain persisted",\n                    "attributes": {"severity": "severe", \n                                   "location": "back",\n                                   "duration": "persistent", \n                                   "time":"after Tylenol",\n                                   "caused_by":"Unknown"}\n                    }\n                ]\n                }\n                \n                        ', 'event_detection_time': 21.682898761006072}</t>
+          <t>['eat', 'sleep', 'daughter', 'husband', 'family', 'pain', 'urine', 'sleeping']</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
         <is>
+          <t>{'text': 'nursing progress note 1900-0700\ns: "i feel so hot"\n\no: please see carevue for complete objective data\n\ncv: st/nsr, 90-110\'s, freq pvc\'s. on amio tid. diastolic blood pressure 90-120\'s, gave captopril 6.25mg @ [**2155**], diastolic blood pressure dropped to 79/low 80\'s @ 2100. co/ci numbers unchanged from earlier in day and patient felt no side effects. milrinone remains @ 0.375mcg/kg/min. co/ci/svr-4.9/2.3/1159. cvp 6-10, w-16. r fem angio site cd&amp;i, no hematoma. pulses palp. extremities warm and pale.\n\nresp: lungs clr c dim bases. last abg-7.48/33/87/25/1, on 4l nc. mvo2-64. persistant productive cough. no c/o sob although tachypneic at times. cxr done, gave benzonatate for cough relief.\n\ngi/gu: bs present, no bm. ate very small amount for dinner. uo decreased to nothing for 2 hours. gave 250cc ivfb x 2, and uo improved slightly. +400cc for day and -700 for los. urine becoming more concentrated.\n\nneuro: lethargic/sleeping @ change of shift. a&amp;o x 3, mae. becoming more interactive as night went on, but slept well through night. c/o pain in r ear (reports having chronic ear infections), md aware.\n\nid/access: wbc down to 13.1 from 16. slightly febrile to 100.6 at start of shift, gave tylenol 650mg, and temp down to 98.9 this am. bc x2, urine cx pending. needs sputum cx. has rij pa cath, 2 piv\'s.\n\nsocial: husband stayed in room overnoc, supportive with care. patient has 20yo and 9yo daughter, should be into visit today. social work consulted.\n\na/p: 39yo female c severe cardiomyopathy and hf, unknown etiology. requiring milrinone and being worked up for heart transplant. continue to monitor hemodynamics and response to meds. obtain sputum cx, monitor temp. watch uo and fluid status. follow up with labs and cxr. emotionally support patient and family and keep updated on plan.\n', 'event': ['Eating', 'Excretion', 'Excretion', 'Pain', 'Sleep', 'Sleep', 'Family', 'Family'], 'event_id': ['e1', 'e2', 'e3', 'e4', 'e5', 'e6', 'e7', 'e8'], 'phrase': '', 'raw_output': '{\n  "events": [\n    {\n      "event_id": "e1",\n      "event_type": "Eating",\n      "text_quote": "ate very small amount for dinner",\n      "attributes": {\n        "food": "dinner",\n        "amount": "small",\n        "method": "Unknown",\n        "negation": "false",\n        "time": "evening",\n        "caused_by": "Unknown"\n      }\n    },\n    {\n      "event_id": "e2",\n      "event_type": "Excretion",\n      "text_quote": "uo decreased to nothing for 2 hours",\n      "attributes": {\n        "type": "urine",\n        "frequency": "decreased",\n        "quality": "Unknown",\n        "negation": "false",\n        "time": "evening",\n        "caused_by": "Unknown"\n      }\n    },\n    {\n      "event_id": "e3",\n      "event_type": "Excretion",\n      "text_quote": "+400cc for day and -700 for los",\n      "attributes": {\n        "type": "urine",\n        "frequency": "increased",\n        "quality": "Unknown",\n        "negation": "false",\n        "time": "day",\n        "caused_by": "Unknown"\n      }\n    },\n    {\n      "event_id": "e4",\n      "event_type": "Pain",\n      "text_quote": "c/o pain in r ear",\n      "attributes": {\n        "severity": "Unknown",\n        "location": "right ear",\n        "duration": "Unknown",\n        "negation": "false",\n        "time": "evening",\n        "caused_by": "Unknown"\n      }\n    },\n    {\n      "event_id": "e5",\n      "event_type": "Sleep",\n      "text_quote": "lethargic/sleeping @ change of shift",\n      "attributes": {\n        "quality": "poor",\n        "duration": "Unknown",\n        "negation": "false",\n        "time": "evening",\n        "caused_by": "Unknown"\n      }\n    },\n    {\n      "event_id": "e6",\n      "event_type": "Sleep",\n      "text_quote": "slept well through night",\n      "attributes": {\n        "quality": "well",\n        "duration": "all night",\n        "negation": "false",\n        "time": "night",\n        "caused_by": "Unknown"\n      }\n    },\n    {\n      "event_id": "e7",\n      "event_type": "Family",\n      "text_quote": "husband stayed in room overnoc, supportive with care",\n      "attributes": {\n        "interaction": "visit",\n        "relation": "husband",\n        "negation": "false",\n        "time": "overnight",\n        "caused_by": "Unknown"\n      }\n    },\n    {\n      "event_id": "e8",\n      "event_type": "Family",\n      "text_quote": "patient has 20yo and 9yo daughter, should be into visit today",\n      "attributes": {\n        "interaction": "visit",\n        "relation": "daughter",\n        "negation": "false",\n        "time": "today",\n        "caused_by": "Unknown"\n      }\n    }\n  ],\n  "order": [\n    ["e1", "before", "e2"],\n    ["e2", "before", "e3"],\n    ["e3", "before", "e4"],\n    ["e4", "before", "e5"],\n    ["e5", "before", "e6"],\n    ["e6", "after", "e7"],\n    ["e7", "before", "e8"]\n  ]\n}', 'attributes': [{'Eating': {'food': 'dinner', 'amount': 'small', 'method': 'Unknown', 'negation': 'false', 'time': 'evening', 'caused_by': 'Unknown'}}, {'Excretion': {'type': 'urine', 'frequency': 'decreased', 'quality': 'Unknown', 'negation': 'false', 'time': 'evening', 'caused_by': 'Unknown'}}, {'Excretion': {'type': 'urine', 'frequency': 'increased', 'quality': 'Unknown', 'negation': 'false', 'time': 'day', 'caused_by': 'Unknown'}}, {'Pain': {'severity': 'Unknown', 'location': 'right ear', 'duration': 'Unknown', 'negation': 'false', 'time': 'evening', 'caused_by': 'Unknown'}}, {'Sleep': {'quality': 'poor', 'duration': 'Unknown', 'negation': 'false', 'time': 'evening', 'caused_by': 'Unknown'}}, {'Sleep': {'quality': 'well', 'duration': 'all night', 'negation': 'false', 'time': 'night', 'caused_by': 'Unknown'}}, {'Family': {'interaction': 'visit', 'relation': 'husband', 'negation': 'false', 'time': 'overnight', 'caused_by': 'Unknown'}}, {'Family': {'interaction': 'visit', 'relation': 'daughter', 'negation': 'false', 'time': 'today', 'caused_by': 'Unknown'}}], 'orders': [[['e1', 'before', 'e2'], ['e2', 'before', 'e3'], ['e3', 'before', 'e4'], ['e4', 'before', 'e5'], ['e5', 'before', 'e6'], ['e6', 'after', 'e7'], ['e7', 'before', 'e8']]], 'text_quotes': ['ate very small amount for dinner', 'uo decreased to nothing for 2 hours', '+400cc for day and -700 for los', 'c/o pain in r ear', 'lethargic/sleeping @ change of shift', 'slept well through night', 'husband stayed in room overnoc, supportive with care', 'patient has 20yo and 9yo daughter, should be into visit today'], 'event_name_prompt': 'Given the text: nursing progress note 1900-0700\ns: "i feel so hot"\n\no: please see carevue for complete objective data\n\ncv: st/nsr, 90-110\'s, freq pvc\'s. on amio tid. diastolic blood pressure 90-120\'s, gave captopril 6.25mg @ [**2155**], diastolic blood pressure dropped to 79/low 80\'s @ 2100. co/ci numbers unchanged from earlier in day and patient felt no side effects. milrinone remains @ 0.375mcg/kg/min. co/ci/svr-4.9/2.3/1159. cvp 6-10, w-16. r fem angio site cd&amp;i, no hematoma. pulses palp. extremities warm and pale.\n\nresp: lungs clr c dim bases. last abg-7.48/33/87/25/1, on 4l nc. mvo2-64. persistant productive cough. no c/o sob although tachypneic at times. cxr done, gave benzonatate for cough relief.\n\ngi/gu: bs present, no bm. ate very small amount for dinner. uo decreased to nothing for 2 hours. gave 250cc ivfb x 2, and uo improved slightly. +400cc for day and -700 for los. urine becoming more concentrated.\n\nneuro: lethargic/sleeping @ change of shift. a&amp;o x 3, mae. becoming more interactive as night went on, but slept well through night. c/o pain in r ear (reports having chronic ear infections), md aware.\n\nid/access: wbc down to 13.1 from 16. slightly febrile to 100.6 at start of shift, gave tylenol 650mg, and temp down to 98.9 this am. bc x2, urine cx pending. needs sputum cx. has rij pa cath, 2 piv\'s.\n\nsocial: husband stayed in room overnoc, supportive with care. patient has 20yo and 9yo daughter, should be into visit today. social work consulted.\n\na/p: 39yo female c severe cardiomyopathy and hf, unknown etiology. requiring milrinone and being worked up for heart transplant. continue to monitor hemodynamics and response to meds. obtain sputum cx, monitor temp. watch uo and fluid status. follow up with labs and cxr. emotionally support patient and family and keep updated on plan.\n, \n                        and the following event types with their definitions: Eating : The patient takes food into their body by mouth.\nExcretion : The patient discharges waste matter from their body.\nFamily : The patient has a visit, call, or communication with a family member.\nPain : The patient reports or shows signs of pain.\nSleep : The patient sleeps or the sleep’s quality or quantity is described.\nUnknown : choose "Unknown" if none of the other event type are applicable. \n                        ---\n                        Your task:\n                        0. Identify ALL events in the text (zero, one, or more).\n1. For each event, assign an event_type from the list above.\n2. If multiple event of same type is mentioned, assign the event_type multiple times\n3. Extract attributes for each event using ONLY the allowed attributes listed below.\n4. Use keyword evidence (Ki) ONLY if it is consistent with the text context.\n5. Output strictly valid JSON following the schema below.\n                        ---\n                        Classification Rules:\n                        - A text may contain multiple events of the same or different types.\n- Create a separate event object for each event mention.\n- If the text is explicitly a NEGATION (e.g., "denies pain"), do not extract that event.\n- If the text describes a FUTURE or HYPOTHETICAL event (e.g., "will eat tomorrow"), ignore it.\n- A valid event should have occurred in the recent past or is occurring during the time of writing of the text.\n- If no events are found or if unsure, return {"events": []}\n                        \n                        ---\n                                    Attributes allowed:\n                                    {\'Eating\': {\'food\': \'&lt;string&gt; # e.g., pancakes, porridge, etc.\', \'amount\': \'&lt;string&gt; # e.g., 1, 2 bowls, etc.\', \'method\': \'&lt;string&gt;  # e.g., oral, tube, etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, evening etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}, \'Excretion\': {\'type\': \'&lt;string&gt; # e.g., urine, stool, etc.\', \'frequency\': \'&lt;string&gt; # e.g., 2x, once, etc.\', \'quality\': \'&lt;string&gt; # e.g., loose, hard, etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, evening etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}, \'Family\': {\'interaction\': \'&lt;string&gt; # e.g., visit, call, communication, etc.\', \'relation\': \'&lt;string&gt; # e.g., mother, son, etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, evening etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}, \'Pain\': {\'severity\': \'&lt;string&gt; # e.g., mild, moderate, severe, numeric scale if present, etc.\', \'location\': \'&lt;string&gt; # e.g., right knee, head, etc.\', \'duration\': \'&lt;string&gt; # e.g., all night, 3 hours, etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, evening etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}, \'Sleep\': {\'quality\': \'&lt;string&gt; # e.g., good, poor, restless, etc.\', \'duration\': \'&lt;string&gt; # e.g., 6 hours, phrases like "all night", etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, evening etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}}\n                                    If no relevant attribute exists for an event, return an empty object {}.\n                                    \n                        \n                        ---\n                                    Keyword evidence (Ki):\n                                    Additional facts: A keyword matching algorithm without context detected keyword(s) (\'daughter\', \'husband\', \'ate\', \'family\', \'pain\', \'urine\', \'slept\', \'sleeping\').\n                                    Use this only as a pointer. If context contradicts, ignore.\n                        ---\n                        Output Schema (strict):\n                        {\n                                    "events": [\n                                        {\n                                        "event_id": "&lt; A unique id eg.: e1 | e2 |...&gt;"\n                                        "event_type": "&lt;Pain | Sleep | Excretion | Eating | Family&gt;",\n                                        "text_quote": "&lt;fragement from the text indicating the event_type&gt;",\n                "attributes": {\n                    "&lt;attribute_name&gt;": "&lt;attribute_value&gt;"\n                }\n                                        }\n                                    ],\n                                    "order": [\n                                        ["e1", "before" | "after" | "simultaneous", "e2" ]\n                                    ]\n                                    }\n                        \n                            Rules:\n                                - Ensure the output is valid JSON (parseable).\n                                - "eventS" must always be an array (can be empty).\n                                - Multiple instances of the same event type appear with different ids.\n                                - Events appear in the array in the same order in which they appear in the text.\n                                - Their partial orders can be expressed using the "order" section.\n                                - Do not include extra keys, comments, or text.\n                                - Each object in "events" must contain "event_type", "text_quote", and "attributes".\n                                - If an event attribute type has no value mentioned, return "attributes": {"&lt; attribute name &gt;:Unknown"} for each attribute type defined for the event type \n                        \n                        \n                        \n                ---\n                Examples:\n                \n                text: "Patient ate breakfast this morning. He seems less anxious."\n                output: {\n                "events": [\n                    {"event_id": "e1",\n                    "event_type": "Eating",\n                    "text_quote":"Patient ate breakfast this morning",\n                    "attributes": {"food": "breakfast", \n                                   "amount": "Unknown",\n                                   "method": "Unknown",\n                                   "negation": "false",\n                                   "time":"morning",\n                                   "caused_by":"Unknown"}\n                    }\n                ],\n                "order":[]\n                }\n                \n                text: "Patient reported severe abdominal pain."\n                output: {\n                "events": [\n                    {"event_id": "e1",\n                    "event_type": "Pain",\n                    "text_quote": "severe abdominal Pain",\n                    "attributes": {"severity": "severe", \n                                   "location": "abdominal",\n                                   "duration": "Unknown",\n                                   "negation": "false",\n                                   "time":"Unknown",\n                                   "caused_by":"Unknown"}\n                    }\n                ],\n                "order":[]\n                }\n                \n                text: "Patient called his son around 3 pm."\n                output: {\n                "events": [\n                    {"event_id": "e1",\n                    "event_type": "Family",\n                    "text_quote": "called his son around 3 pm",\n                    "attributes": {"interaction": "call", \n                                    "relation": "son",\n                                    "negation": "false",\n                                    "time":"3 pm",\n                                    "caused_by":"Unknown"}\n                    }\n                ],\n                "order":[]\n                }\n                \n                text: "Patient had a loose stool overnight."\n                output: {\n                "events": [\n                    {"event_id": "e1",\n                    "event_type": "Excretion",\n                    "text_quote": "loose stool overnight",\n                    "attributes": {"type": "stool", \n                                   "quality": "loose", \n                                   "frequency":"overnight", \n                                   "negation": "false",\n                                   "time":"night",\n                                   "caused_by":"Unknown"}\n                    }\n                ],\n                "order":[]\n                }\n                \n                text: "Patient was able to sleep well last night."\n                output: {\n                "events": [\n                    {"event_id": "e1",\n                    "event_type": "Sleep",\n                    "text_quote": "sleep well last night",\n                    "attributes": {"quality": "well",\n                                    "duration": "Unknown", \n                                    "negation": "false",\n                                    "time":"night",\n                                    "caused_by":"Unknown"}\n                    }\n                ],\n                "order":[]\n                }\n                \n                text: "The patient couldn\'t sleep due to severe pain."\n                output: {\n                "events": [\n                    {"event_id": "e1",\n                    "event_type": "Sleep",\n                    "text_quote": "couldn\'t sleep",\n                    "attributes": {"quality": "poor", \n                                    "duration": "Unknown",\n                                    "negation": "true",\n                                    "time":"Unknown",\n                                    "caused_by":"Pain"}\n                    },\n                    {"event_id": "e2",\n                    "event_type": "Pain",\n                    "text_quote": "severe pain",\n                    "attributes": {"severity": "severe", \n                                    "location": "Unknown", \n                                    "duration": "Unknown", \n                                    "time":"Unknown",\n                                    "caused_by":"Unknown"}\n                    }\n                ],\n                "order":["e1", "after", "e2"]\n                }\n                \n                text: "The patient complained of severe back pain, was given Tylenol, but the pain persisted and he was then prescribed stronger morphine."\n                output: {\n                "events": [\n                    {"event_id": "e1",\n                    "event_type": "Pain",\n                    "text_quote": "complained of severe back pain",\n                    "attributes": {"severity": "severe", \n                                    "location": "back",\n                                    "duration": "Unknown", \n                                    "time":"Unknown",\n                                    "caused_by":"Unknown"}\n                    },\n                    {"event_id": "e2",\n                    "event_type": "Pain",\n                    "text_quote": "pain persisted",\n                    "attributes": {"severity": "severe", \n                                   "location": "back",\n                                   "duration": "persistent", \n                                   "time":"after Tylenol",\n                                   "caused_by":"Unknown"}\n                    }\n                ],\n                "order":[["e1", "before", "e2"]]\n                }\n                \n                        ', 'event_detection_time': 27.09508548397571}</t>
+        </is>
+      </c>
+      <c r="G17" t="inlineStr">
+        <is>
           <t>['Eating', 'Excretion', 'Excretion', 'Pain', 'Sleep', 'Sleep', 'Family', 'Family']</t>
         </is>
       </c>
-      <c r="G17" t="inlineStr">
-        <is>
-          <t>[{'Eating': {'food': 'dinner', 'amount': 'small', 'method': 'Unknown', 'negation': False, 'time': 'night', 'caused_by': 'Unknown'}}, {'Excretion': {'type': 'urine', 'frequency': 'decreased', 'quality': 'Unknown', 'negation': False, 'time': 'night', 'caused_by': 'Unknown'}}, {'Excretion': {'type': 'urine', 'frequency': 'increased', 'quality': 'Unknown', 'negation': False, 'time': 'day', 'caused_by': 'Unknown'}}, {'Pain': {'severity': 'Unknown', 'location': 'r ear', 'duration': 'chronic', 'negation': False, 'time': 'Unknown', 'caused_by': 'ear infections'}}, {'Sleep': {'quality': 'poor', 'duration': 'Unknown', 'negation': False, 'time': 'night', 'caused_by': 'Unknown'}}, {'Sleep': {'quality': 'well', 'duration': 'all night', 'negation': False, 'time': 'night', 'caused_by': 'Unknown'}}, {'Family': {'interaction': 'visit', 'relation': 'husband', 'negation': False, 'time': 'night', 'caused_by': 'Unknown'}}, {'Family': {'interaction': 'visit', 'relation': 'daughter', 'negation': False, 'time': 'today', 'caused_by': 'Unknown'}}]</t>
-        </is>
-      </c>
       <c r="H17" t="inlineStr">
         <is>
-          <t>['ate very small amount for dinner', 'uo decreased to nothing for 2 hours', '+400cc for day and -700 for los', 'c/o pain in r ear (reports having chronic ear infections)', 'lethargic/sleeping @ change of shift', 'slept well through night', 'husband stayed in room overnoc, supportive with care', 'patient has 20yo and 9yo daughter, should be into visit today']</t>
+          <t>[{'Eating': {'food': 'dinner', 'amount': 'small', 'method': 'Unknown', 'negation': 'false', 'time': 'evening', 'caused_by': 'Unknown'}}, {'Excretion': {'type': 'urine', 'frequency': 'decreased', 'quality': 'Unknown', 'negation': 'false', 'time': 'evening', 'caused_by': 'Unknown'}}, {'Excretion': {'type': 'urine', 'frequency': 'increased', 'quality': 'Unknown', 'negation': 'false', 'time': 'day', 'caused_by': 'Unknown'}}, {'Pain': {'severity': 'Unknown', 'location': 'right ear', 'duration': 'Unknown', 'negation': 'false', 'time': 'evening', 'caused_by': 'Unknown'}}, {'Sleep': {'quality': 'poor', 'duration': 'Unknown', 'negation': 'false', 'time': 'evening', 'caused_by': 'Unknown'}}, {'Sleep': {'quality': 'well', 'duration': 'all night', 'negation': 'false', 'time': 'night', 'caused_by': 'Unknown'}}, {'Family': {'interaction': 'visit', 'relation': 'husband', 'negation': 'false', 'time': 'overnight', 'caused_by': 'Unknown'}}, {'Family': {'interaction': 'visit', 'relation': 'daughter', 'negation': 'false', 'time': 'today', 'caused_by': 'Unknown'}}]</t>
         </is>
       </c>
       <c r="I17" t="inlineStr">
         <is>
-          <t>{'text': 'nursing progress note 1900-0700\ns: "i feel so hot"\n\no: please see carevue for complete objective data\n\ncv: st/nsr, 90-110\'s, freq pvc\'s. on amio tid. diastolic blood pressure 90-120\'s, gave captopril 6.25mg @ [**2155**], diastolic blood pressure dropped to 79/low 80\'s @ 2100. co/ci numbers unchanged from earlier in day and patient felt no side effects. milrinone remains @ 0.375mcg/kg/min. co/ci/svr-4.9/2.3/1159. cvp 6-10, w-16. r fem angio site cd&amp;i, no hematoma. pulses palp. extremities warm and pale.\n\nresp: lungs clr c dim bases. last abg-7.48/33/87/25/1, on 4l nc. mvo2-64. persistant productive cough. no c/o sob although tachypneic at times. cxr done, gave benzonatate for cough relief.\n\ngi/gu: bs present, no bm. ate very small amount for dinner. uo decreased to nothing for 2 hours. gave 250cc ivfb x 2, and uo improved slightly. +400cc for day and -700 for los. urine becoming more concentrated.\n\nneuro: lethargic/sleeping @ change of shift. a&amp;o x 3, mae. becoming more interactive as night went on, but slept well through night. c/o pain in r ear (reports having chronic ear infections), md aware.\n\nid/access: wbc down to 13.1 from 16. slightly febrile to 100.6 at start of shift, gave tylenol 650mg, and temp down to 98.9 this am. bc x2, urine cx pending. needs sputum cx. has rij pa cath, 2 piv\'s.\n\nsocial: husband stayed in room overnoc, supportive with care. patient has 20yo and 9yo daughter, should be into visit today. social work consulted.\n\na/p: 39yo female c severe cardiomyopathy and hf, unknown etiology. requiring milrinone and being worked up for heart transplant. continue to monitor hemodynamics and response to meds. obtain sputum cx, monitor temp. watch uo and fluid status. follow up with labs and cxr. emotionally support patient and family and keep updated on plan.\n', 'event': ['Eating', 'Excretion', 'Excretion', 'Family', 'Family', 'Pain', 'Sleep', 'Sleep'], 'phrase': '', 'raw_output': '{\n  "events": [\n    {\n      "event_type": "Eating",\n      "text_quote": "ate very small amount for dinner.",\n      "attributes": {\n        "food": "dinner",\n        "amount": "very small",\n        "method": "",\n        "negation": false,\n        "time": "",\n        "caused_by": ""\n      }\n    },\n    {\n      "event_type": "Excretion",\n      "text_quote": "uo decreased to nothing for 2 hours.",\n      "attributes": {\n        "type": "urine",\n        "frequency": "",\n        "quality": "",\n        "negation": false,\n        "time": "2 hours",\n        "caused_by": ""\n      }\n    },\n    {\n      "event_type": "Excretion",\n      "text_quote": "+400cc for day and -700 for los.",\n      "attributes": {\n        "type": "urine",\n        "frequency": "",\n        "quality": "",\n        "negation": false,\n        "time": "",\n        "caused_by": ""\n      }\n    },\n    {\n      "event_type": "Family",\n      "text_quote": "husband stayed in room overnoc, supportive with care.",\n      "attributes": {\n        "interaction": "visit",\n        "relation": "husband",\n        "negation": false,\n        "time": "",\n        "caused_by": ""\n      }\n    },\n    {\n      "event_type": "Family",\n      "text_quote": "patient has 20yo and 9yo daughter, should be into visit today.",\n      "attributes": {\n        "interaction": "visit",\n        "relation": "daughter",\n        "negation": false,\n        "time": "",\n        "caused_by": ""\n      }\n    },\n    {\n      "event_type": "Pain",\n      "text_quote": "c/o pain in r ear (reports having chronic ear infections)",\n      "attributes": {\n        "severity": "",\n        "location": "r ear",\n        "duration": "",\n        "negation": false,\n        "time": "",\n        "caused_by": ""\n      }\n    },\n    {\n      "event_type": "Sleep",\n      "text_quote": "lethargic/sleeping @ change of shift.",\n      "attributes": {\n        "quality": "",\n        "duration": "",\n        "negation": false,\n        "time": "@ change of shift",\n        "caused_by": ""\n      }\n    },\n    {\n      "event_type": "Sleep",\n      "text_quote": "slept well through night.",\n      "attributes": {\n        "quality": "well",\n        "duration": "",\n        "negation": false,\n        "time": "through night",\n        "caused_by": ""\n      }\n    }\n  ]\n}', 'attributes': [{'Eating': {'food': 'dinner', 'amount': 'very small', 'method': '', 'negation': False, 'time': '', 'caused_by': ''}}, {'Excretion': {'type': 'urine', 'frequency': '', 'quality': '', 'negation': False, 'time': '2 hours', 'caused_by': ''}}, {'Excretion': {'type': 'urine', 'frequency': '', 'quality': '', 'negation': False, 'time': '', 'caused_by': ''}}, {'Family': {'interaction': 'visit', 'relation': 'husband', 'negation': False, 'time': '', 'caused_by': ''}}, {'Family': {'interaction': 'visit', 'relation': 'daughter', 'negation': False, 'time': '', 'caused_by': ''}}, {'Pain': {'severity': '', 'location': 'r ear', 'duration': '', 'negation': False, 'time': '', 'caused_by': ''}}, {'Sleep': {'quality': '', 'duration': '', 'negation': False, 'time': '@ change of shift', 'caused_by': ''}}, {'Sleep': {'quality': 'well', 'duration': '', 'negation': False, 'time': 'through night', 'caused_by': ''}}], 'text_quotes': ['ate very small amount for dinner.', 'uo decreased to nothing for 2 hours.', '+400cc for day and -700 for los.', 'husband stayed in room overnoc, supportive with care.', 'patient has 20yo and 9yo daughter, should be into visit today.', 'c/o pain in r ear (reports having chronic ear infections)', 'lethargic/sleeping @ change of shift.', 'slept well through night.'], 'event_name_prompt': 'Given the text: nursing progress note 1900-0700\ns: "i feel so hot"\n\no: please see carevue for complete objective data\n\ncv: st/nsr, 90-110\'s, freq pvc\'s. on amio tid. diastolic blood pressure 90-120\'s, gave captopril 6.25mg @ [**2155**], diastolic blood pressure dropped to 79/low 80\'s @ 2100. co/ci numbers unchanged from earlier in day and patient felt no side effects. milrinone remains @ 0.375mcg/kg/min. co/ci/svr-4.9/2.3/1159. cvp 6-10, w-16. r fem angio site cd&amp;i, no hematoma. pulses palp. extremities warm and pale.\n\nresp: lungs clr c dim bases. last abg-7.48/33/87/25/1, on 4l nc. mvo2-64. persistant productive cough. no c/o sob although tachypneic at times. cxr done, gave benzonatate for cough relief.\n\ngi/gu: bs present, no bm. ate very small amount for dinner. uo decreased to nothing for 2 hours. gave 250cc ivfb x 2, and uo improved slightly. +400cc for day and -700 for los. urine becoming more concentrated.\n\nneuro: lethargic/sleeping @ change of shift. a&amp;o x 3, mae. becoming more interactive as night went on, but slept well through night. c/o pain in r ear (reports having chronic ear infections), md aware.\n\nid/access: wbc down to 13.1 from 16. slightly febrile to 100.6 at start of shift, gave tylenol 650mg, and temp down to 98.9 this am. bc x2, urine cx pending. needs sputum cx. has rij pa cath, 2 piv\'s.\n\nsocial: husband stayed in room overnoc, supportive with care. patient has 20yo and 9yo daughter, should be into visit today. social work consulted.\n\na/p: 39yo female c severe cardiomyopathy and hf, unknown etiology. requiring milrinone and being worked up for heart transplant. continue to monitor hemodynamics and response to meds. obtain sputum cx, monitor temp. watch uo and fluid status. follow up with labs and cxr. emotionally support patient and family and keep updated on plan.\n, \n                        and the following event types with their definitions: Eating : The patient takes food into their body by mouth.\nExcretion : The patient discharges waste matter from their body.\nFamily : The patient has a visit, call, or communication with a family member.\nPain : The patient reports or shows signs of pain.\nSleep : The patient sleeps or the sleep’s quality or quantity is described.\nUnknown : choose "Unknown" if none of the other event type are applicable. \n                        ---\n                        Your task:\n                        0. Identify ALL events in the text (zero, one, or more).\n1. For each event, assign an event_type from the list above.\n2. If multiple event of same type is mentioned, assign the event_type multiple times\n3. Extract attributes for each event using ONLY the allowed attributes listed below.\n4. Use keyword evidence (Ki) ONLY if it is consistent with the text context.\n5. Output strictly valid JSON following the schema below.\n                        ---\n                        Classification Rules:\n                        - A text may contain multiple events of the same or different types.\n- Create a separate event object for each event mention.\n- If the text is explicitly a NEGATION (e.g., "denies pain"), do not extract that event.\n- If the text describes a FUTURE or HYPOTHETICAL event (e.g., "will eat tomorrow"), ignore it.\n- A valid event should have occurred in the recent past or is occurring during the time of writing of the text.\n- If no events are found or if unsure, return {"events": []}\n                        \n                        ---\n                                    Attributes allowed:\n                                    {\'Eating\': {\'food\': \'&lt;string&gt; # e.g., pancakes, porridge, etc.\', \'amount\': \'&lt;string&gt; # e.g., 1, 2 bowls, etc.\', \'method\': \'&lt;string&gt;  # e.g., oral, tube, etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, after shower, etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}, \'Excretion\': {\'type\': \'&lt;string&gt; # e.g., urine, stool, etc.\', \'frequency\': \'&lt;string&gt; # e.g., 2x, once, etc.\', \'quality\': \'&lt;string&gt; # e.g., loose, hard, etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, after shower, etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}, \'Family\': {\'interaction\': \'&lt;string&gt; # e.g., visit, call, communication, etc.\', \'relation\': \'&lt;string&gt; # e.g., mother, son, etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, after shower, etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}, \'Pain\': {\'severity\': \'&lt;string&gt; # e.g., mild, moderate, severe, numeric scale if present, etc.\', \'location\': \'&lt;string&gt; # e.g., right knee, head, etc.\', \'duration\': \'&lt;string&gt; # e.g., all night, 3 hours, etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, after shower, etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}, \'Sleep\': {\'quality\': \'&lt;string&gt; # e.g., good, poor, restless, etc.\', \'duration\': \'&lt;string&gt; # e.g., 6 hours, phrases like "all night", etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, after shower, etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}}\n                                    If no relevant attribute exists for an event, return an empty object {}.\n                                    \n                        \n                        ---\n                                    Keyword evidence (Ki):\n                                    Additional facts: A keyword matching algorithm without context detected keyword(s) [\'ate\', \'daughter\', \'urine\', \'slept\', \'pain\', \'sleeping\', \'family\', \'husband\'].\n                                    Use this only as a pointer. If context contradicts, ignore.\n                        ---\n                        Output Schema (strict):\n                        {\n                                    "events": [\n                                        {\n                                        "event_type": "&lt;Pain | Sleep | Excretion | Eating | Family&gt;",\n                                        "text_quote": "&lt;fragement from the text indicating &gt;",\n                "attributes": {\n                    "&lt;attribute_name&gt;": "&lt;attribute_value&gt;"\n                }\n                                        }\n                                    ]\n                                    }\n                        \n                            Rules:\n                                - Ensure the output is valid JSON (parseable).\n                                - "eventS" must always be an array (can be empty).\n                                - Multiple instances of the same event type appear as individual elements in the event array.\n                                - Events appear in the array in the same order in which they appear in the text.\n                                - Do not include extra keys, comments, or text.\n                                - Each object in "events" must contain "event_type", "text_quote", and "attributes".\n                                -If an event attribute type has no value mentioned, return "attributes": {"&lt; attribute name &gt;:Unknown"} for each attribute type defined for the event type \n                        \n                        \n                        \n                        ', 'event_detection_time': 19.167489810992265}</t>
+          <t>['ate very small amount for dinner', 'uo decreased to nothing for 2 hours', '+400cc for day and -700 for los', 'c/o pain in r ear', 'lethargic/sleeping @ change of shift', 'slept well through night', 'husband stayed in room overnoc, supportive with care', 'patient has 20yo and 9yo daughter, should be into visit today']</t>
         </is>
       </c>
       <c r="J17" t="inlineStr">
         <is>
+          <t>[[['e1', 'before', 'e2'], ['e2', 'before', 'e3'], ['e3', 'before', 'e4'], ['e4', 'before', 'e5'], ['e5', 'before', 'e6'], ['e6', 'after', 'e7'], ['e7', 'before', 'e8']]]</t>
+        </is>
+      </c>
+      <c r="K17" t="inlineStr">
+        <is>
+          <t>{'text': 'nursing progress note 1900-0700\ns: "i feel so hot"\n\no: please see carevue for complete objective data\n\ncv: st/nsr, 90-110\'s, freq pvc\'s. on amio tid. diastolic blood pressure 90-120\'s, gave captopril 6.25mg @ [**2155**], diastolic blood pressure dropped to 79/low 80\'s @ 2100. co/ci numbers unchanged from earlier in day and patient felt no side effects. milrinone remains @ 0.375mcg/kg/min. co/ci/svr-4.9/2.3/1159. cvp 6-10, w-16. r fem angio site cd&amp;i, no hematoma. pulses palp. extremities warm and pale.\n\nresp: lungs clr c dim bases. last abg-7.48/33/87/25/1, on 4l nc. mvo2-64. persistant productive cough. no c/o sob although tachypneic at times. cxr done, gave benzonatate for cough relief.\n\ngi/gu: bs present, no bm. ate very small amount for dinner. uo decreased to nothing for 2 hours. gave 250cc ivfb x 2, and uo improved slightly. +400cc for day and -700 for los. urine becoming more concentrated.\n\nneuro: lethargic/sleeping @ change of shift. a&amp;o x 3, mae. becoming more interactive as night went on, but slept well through night. c/o pain in r ear (reports having chronic ear infections), md aware.\n\nid/access: wbc down to 13.1 from 16. slightly febrile to 100.6 at start of shift, gave tylenol 650mg, and temp down to 98.9 this am. bc x2, urine cx pending. needs sputum cx. has rij pa cath, 2 piv\'s.\n\nsocial: husband stayed in room overnoc, supportive with care. patient has 20yo and 9yo daughter, should be into visit today. social work consulted.\n\na/p: 39yo female c severe cardiomyopathy and hf, unknown etiology. requiring milrinone and being worked up for heart transplant. continue to monitor hemodynamics and response to meds. obtain sputum cx, monitor temp. watch uo and fluid status. follow up with labs and cxr. emotionally support patient and family and keep updated on plan.\n', 'event': ['Eating', 'Excretion', 'Excretion', 'Family', 'Family', 'Pain', 'Sleep', 'Sleep'], 'event_id': ['e1', 'e2', 'e3', 'e4', 'e5', 'e6', 'e7', 'e8'], 'phrase': '', 'raw_output': '{\n  "events": [\n    {\n      "event_id": "e1",\n      "event_type": "Eating",\n      "text_quote": "ate very small amount for dinner.",\n      "attributes": {\n        "food": "Unknown",\n        "amount": "small",\n        "method": "oral",\n        "negation": false,\n        "time": "dinner",\n        "caused_by": "Unknown"\n      }\n    },\n    {\n      "event_id": "e2",\n      "event_type": "Excretion",\n      "text_quote": "uo decreased to nothing for 2 hours.",\n      "attributes": {\n        "type": "urine",\n        "frequency": "decreased",\n        "quality": "Unknown",\n        "negation": false,\n        "time": "2 hours",\n        "caused_by": "Unknown"\n      }\n    },\n    {\n      "event_id": "e3",\n      "event_type": "Excretion",\n      "text_quote": "+400cc for day and -700 for los.",\n      "attributes": {\n        "type": "urine",\n        "frequency": "increased",\n        "quality": "Unknown",\n        "negation": false,\n        "time": "day",\n        "caused_by": "Unknown"\n      }\n    },\n    {\n      "event_id": "e4",\n      "event_type": "Family",\n      "text_quote": "husband stayed in room overnoc, supportive with care.",\n      "attributes": {\n        "interaction": "visit",\n        "relation": "husband",\n        "negation": false,\n        "time": "overnight",\n        "caused_by": "Unknown"\n      }\n    },\n    {\n      "event_id": "e5",\n      "event_type": "Family",\n      "text_quote": "patient has 20yo and 9yo daughter, should be into visit today.",\n      "attributes": {\n        "interaction": "visit",\n        "relation": "daughter",\n        "negation": false,\n        "time": "today",\n        "caused_by": "Unknown"\n      }\n    },\n    {\n      "event_id": "e6",\n      "event_type": "Pain",\n      "text_quote": "c/o pain in r ear (reports having chronic ear infections)",\n      "attributes": {\n        "severity": "Unknown",\n        "location": "right ear",\n        "duration": "chronic",\n        "negation": false,\n        "time": "Unknown",\n        "caused_by": "ear infections"\n      }\n    },\n    {\n      "event_id": "e7",\n      "event_type": "Sleep",\n      "text_quote": "lethargic/sleeping @ change of shift.",\n      "attributes": {\n        "quality": "poor",\n        "duration": "Unknown",\n        "negation": false,\n        "time": "change of shift",\n        "caused_by": "Unknown"\n      }\n    },\n    {\n      "event_id": "e8",\n      "event_type": "Sleep",\n      "text_quote": "slept well through night.",\n      "attributes": {\n        "quality": "good",\n        "duration": "all night",\n        "negation": false,\n        "time": "night",\n        "caused_by": "Unknown"\n      }\n    }\n  ],\n  "order": [\n    ["e1", "before", "e2"],\n    ["e2", "before", "e3"],\n    ["e3", "before", "e4"],\n    ["e4", "before", "e5"],\n    ["e5", "before", "e6"],\n    ["e6", "before", "e7"],\n    ["e7", "before", "e8"]\n  ]\n}', 'attributes': [{'Eating': {'food': 'Unknown', 'amount': 'small', 'method': 'oral', 'negation': False, 'time': 'dinner', 'caused_by': 'Unknown'}}, {'Excretion': {'type': 'urine', 'frequency': 'decreased', 'quality': 'Unknown', 'negation': False, 'time': '2 hours', 'caused_by': 'Unknown'}}, {'Excretion': {'type': 'urine', 'frequency': 'increased', 'quality': 'Unknown', 'negation': False, 'time': 'day', 'caused_by': 'Unknown'}}, {'Family': {'interaction': 'visit', 'relation': 'husband', 'negation': False, 'time': 'overnight', 'caused_by': 'Unknown'}}, {'Family': {'interaction': 'visit', 'relation': 'daughter', 'negation': False, 'time': 'today', 'caused_by': 'Unknown'}}, {'Pain': {'severity': 'Unknown', 'location': 'right ear', 'duration': 'chronic', 'negation': False, 'time': 'Unknown', 'caused_by': 'ear infections'}}, {'Sleep': {'quality': 'poor', 'duration': 'Unknown', 'negation': False, 'time': 'change of shift', 'caused_by': 'Unknown'}}, {'Sleep': {'quality': 'good', 'duration': 'all night', 'negation': False, 'time': 'night', 'caused_by': 'Unknown'}}], 'orders': [[['e1', 'before', 'e2'], ['e2', 'before', 'e3'], ['e3', 'before', 'e4'], ['e4', 'before', 'e5'], ['e5', 'before', 'e6'], ['e6', 'before', 'e7'], ['e7', 'before', 'e8']]], 'text_quotes': ['ate very small amount for dinner.', 'uo decreased to nothing for 2 hours.', '+400cc for day and -700 for los.', 'husband stayed in room overnoc, supportive with care.', 'patient has 20yo and 9yo daughter, should be into visit today.', 'c/o pain in r ear (reports having chronic ear infections)', 'lethargic/sleeping @ change of shift.', 'slept well through night.'], 'event_name_prompt': 'Given the text: nursing progress note 1900-0700\ns: "i feel so hot"\n\no: please see carevue for complete objective data\n\ncv: st/nsr, 90-110\'s, freq pvc\'s. on amio tid. diastolic blood pressure 90-120\'s, gave captopril 6.25mg @ [**2155**], diastolic blood pressure dropped to 79/low 80\'s @ 2100. co/ci numbers unchanged from earlier in day and patient felt no side effects. milrinone remains @ 0.375mcg/kg/min. co/ci/svr-4.9/2.3/1159. cvp 6-10, w-16. r fem angio site cd&amp;i, no hematoma. pulses palp. extremities warm and pale.\n\nresp: lungs clr c dim bases. last abg-7.48/33/87/25/1, on 4l nc. mvo2-64. persistant productive cough. no c/o sob although tachypneic at times. cxr done, gave benzonatate for cough relief.\n\ngi/gu: bs present, no bm. ate very small amount for dinner. uo decreased to nothing for 2 hours. gave 250cc ivfb x 2, and uo improved slightly. +400cc for day and -700 for los. urine becoming more concentrated.\n\nneuro: lethargic/sleeping @ change of shift. a&amp;o x 3, mae. becoming more interactive as night went on, but slept well through night. c/o pain in r ear (reports having chronic ear infections), md aware.\n\nid/access: wbc down to 13.1 from 16. slightly febrile to 100.6 at start of shift, gave tylenol 650mg, and temp down to 98.9 this am. bc x2, urine cx pending. needs sputum cx. has rij pa cath, 2 piv\'s.\n\nsocial: husband stayed in room overnoc, supportive with care. patient has 20yo and 9yo daughter, should be into visit today. social work consulted.\n\na/p: 39yo female c severe cardiomyopathy and hf, unknown etiology. requiring milrinone and being worked up for heart transplant. continue to monitor hemodynamics and response to meds. obtain sputum cx, monitor temp. watch uo and fluid status. follow up with labs and cxr. emotionally support patient and family and keep updated on plan.\n, \n                        and the following event types with their definitions: Eating : The patient takes food into their body by mouth.\nExcretion : The patient discharges waste matter from their body.\nFamily : The patient has a visit, call, or communication with a family member.\nPain : The patient reports or shows signs of pain.\nSleep : The patient sleeps or the sleep’s quality or quantity is described.\nUnknown : choose "Unknown" if none of the other event type are applicable. \n                        ---\n                        Your task:\n                        0. Identify ALL events in the text (zero, one, or more).\n1. For each event, assign an event_type from the list above.\n2. If multiple event of same type is mentioned, assign the event_type multiple times\n3. Extract attributes for each event using ONLY the allowed attributes listed below.\n4. Use keyword evidence (Ki) ONLY if it is consistent with the text context.\n5. Output strictly valid JSON following the schema below.\n                        ---\n                        Classification Rules:\n                        - A text may contain multiple events of the same or different types.\n- Create a separate event object for each event mention.\n- If the text is explicitly a NEGATION (e.g., "denies pain"), do not extract that event.\n- If the text describes a FUTURE or HYPOTHETICAL event (e.g., "will eat tomorrow"), ignore it.\n- A valid event should have occurred in the recent past or is occurring during the time of writing of the text.\n- If no events are found or if unsure, return {"events": []}\n                        \n                        ---\n                                    Attributes allowed:\n                                    {\'Eating\': {\'food\': \'&lt;string&gt; # e.g., pancakes, porridge, etc.\', \'amount\': \'&lt;string&gt; # e.g., 1, 2 bowls, etc.\', \'method\': \'&lt;string&gt;  # e.g., oral, tube, etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, evening etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}, \'Excretion\': {\'type\': \'&lt;string&gt; # e.g., urine, stool, etc.\', \'frequency\': \'&lt;string&gt; # e.g., 2x, once, etc.\', \'quality\': \'&lt;string&gt; # e.g., loose, hard, etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, evening etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}, \'Family\': {\'interaction\': \'&lt;string&gt; # e.g., visit, call, communication, etc.\', \'relation\': \'&lt;string&gt; # e.g., mother, son, etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, evening etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}, \'Pain\': {\'severity\': \'&lt;string&gt; # e.g., mild, moderate, severe, numeric scale if present, etc.\', \'location\': \'&lt;string&gt; # e.g., right knee, head, etc.\', \'duration\': \'&lt;string&gt; # e.g., all night, 3 hours, etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, evening etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}, \'Sleep\': {\'quality\': \'&lt;string&gt; # e.g., good, poor, restless, etc.\', \'duration\': \'&lt;string&gt; # e.g., 6 hours, phrases like "all night", etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, evening etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}}\n                                    If no relevant attribute exists for an event, return an empty object {}.\n                                    \n                        \n                        ---\n                                    Keyword evidence (Ki):\n                                    Additional facts: A keyword matching algorithm without context detected keyword(s) (\'daughter\', \'husband\', \'ate\', \'family\', \'pain\', \'urine\', \'slept\', \'sleeping\').\n                                    Use this only as a pointer. If context contradicts, ignore.\n                        ---\n                        Output Schema (strict):\n                        {\n                                    "events": [\n                                        {\n                                        "event_id": "&lt; A unique id eg.: e1 | e2 |...&gt;"\n                                        "event_type": "&lt;Pain | Sleep | Excretion | Eating | Family&gt;",\n                                        "text_quote": "&lt;fragement from the text indicating the event_type&gt;",\n                "attributes": {\n                    "&lt;attribute_name&gt;": "&lt;attribute_value&gt;"\n                }\n                                        }\n                                    ],\n                                    "order": [\n                                        ["e1", "before" | "after" | "simultaneous", "e2" ]\n                                    ]\n                                    }\n                        \n                            Rules:\n                                - Ensure the output is valid JSON (parseable).\n                                - "eventS" must always be an array (can be empty).\n                                - Multiple instances of the same event type appear with different ids.\n                                - Events appear in the array in the same order in which they appear in the text.\n                                - Their partial orders can be expressed using the "order" section.\n                                - Do not include extra keys, comments, or text.\n                                - Each object in "events" must contain "event_type", "text_quote", and "attributes".\n                                - If an event attribute type has no value mentioned, return "attributes": {"&lt; attribute name &gt;:Unknown"} for each attribute type defined for the event type \n                        \n                        \n                        \n                        ', 'event_detection_time': 25.57279084197944}</t>
+        </is>
+      </c>
+      <c r="L17" t="inlineStr">
+        <is>
           <t>['Eating', 'Excretion', 'Excretion', 'Family', 'Family', 'Pain', 'Sleep', 'Sleep']</t>
         </is>
       </c>
-      <c r="K17" t="inlineStr">
-        <is>
-          <t>[{'Eating': {'food': 'dinner', 'amount': 'very small', 'method': '', 'negation': False, 'time': '', 'caused_by': ''}}, {'Excretion': {'type': 'urine', 'frequency': '', 'quality': '', 'negation': False, 'time': '2 hours', 'caused_by': ''}}, {'Excretion': {'type': 'urine', 'frequency': '', 'quality': '', 'negation': False, 'time': '', 'caused_by': ''}}, {'Family': {'interaction': 'visit', 'relation': 'husband', 'negation': False, 'time': '', 'caused_by': ''}}, {'Family': {'interaction': 'visit', 'relation': 'daughter', 'negation': False, 'time': '', 'caused_by': ''}}, {'Pain': {'severity': '', 'location': 'r ear', 'duration': '', 'negation': False, 'time': '', 'caused_by': ''}}, {'Sleep': {'quality': '', 'duration': '', 'negation': False, 'time': '@ change of shift', 'caused_by': ''}}, {'Sleep': {'quality': 'well', 'duration': '', 'negation': False, 'time': 'through night', 'caused_by': ''}}]</t>
-        </is>
-      </c>
-      <c r="L17" t="inlineStr">
+      <c r="M17" t="inlineStr">
+        <is>
+          <t>[{'Eating': {'food': 'Unknown', 'amount': 'small', 'method': 'oral', 'negation': False, 'time': 'dinner', 'caused_by': 'Unknown'}}, {'Excretion': {'type': 'urine', 'frequency': 'decreased', 'quality': 'Unknown', 'negation': False, 'time': '2 hours', 'caused_by': 'Unknown'}}, {'Excretion': {'type': 'urine', 'frequency': 'increased', 'quality': 'Unknown', 'negation': False, 'time': 'day', 'caused_by': 'Unknown'}}, {'Family': {'interaction': 'visit', 'relation': 'husband', 'negation': False, 'time': 'overnight', 'caused_by': 'Unknown'}}, {'Family': {'interaction': 'visit', 'relation': 'daughter', 'negation': False, 'time': 'today', 'caused_by': 'Unknown'}}, {'Pain': {'severity': 'Unknown', 'location': 'right ear', 'duration': 'chronic', 'negation': False, 'time': 'Unknown', 'caused_by': 'ear infections'}}, {'Sleep': {'quality': 'poor', 'duration': 'Unknown', 'negation': False, 'time': 'change of shift', 'caused_by': 'Unknown'}}, {'Sleep': {'quality': 'good', 'duration': 'all night', 'negation': False, 'time': 'night', 'caused_by': 'Unknown'}}]</t>
+        </is>
+      </c>
+      <c r="N17" t="inlineStr">
         <is>
           <t>['ate very small amount for dinner.', 'uo decreased to nothing for 2 hours.', '+400cc for day and -700 for los.', 'husband stayed in room overnoc, supportive with care.', 'patient has 20yo and 9yo daughter, should be into visit today.', 'c/o pain in r ear (reports having chronic ear infections)', 'lethargic/sleeping @ change of shift.', 'slept well through night.']</t>
         </is>
       </c>
-      <c r="M17" t="inlineStr">
-        <is>
-          <t>{'text': 'nursing progress note 1900-0700\ns: "i feel so hot"\n\no: please see carevue for complete objective data\n\ncv: st/nsr, 90-110\'s, freq pvc\'s. on amio tid. diastolic blood pressure 90-120\'s, gave captopril 6.25mg @ [**2155**], diastolic blood pressure dropped to 79/low 80\'s @ 2100. co/ci numbers unchanged from earlier in day and patient felt no side effects. milrinone remains @ 0.375mcg/kg/min. co/ci/svr-4.9/2.3/1159. cvp 6-10, w-16. r fem angio site cd&amp;i, no hematoma. pulses palp. extremities warm and pale.\n\nresp: lungs clr c dim bases. last abg-7.48/33/87/25/1, on 4l nc. mvo2-64. persistant productive cough. no c/o sob although tachypneic at times. cxr done, gave benzonatate for cough relief.\n\ngi/gu: bs present, no bm. ate very small amount for dinner. uo decreased to nothing for 2 hours. gave 250cc ivfb x 2, and uo improved slightly. +400cc for day and -700 for los. urine becoming more concentrated.\n\nneuro: lethargic/sleeping @ change of shift. a&amp;o x 3, mae. becoming more interactive as night went on, but slept well through night. c/o pain in r ear (reports having chronic ear infections), md aware.\n\nid/access: wbc down to 13.1 from 16. slightly febrile to 100.6 at start of shift, gave tylenol 650mg, and temp down to 98.9 this am. bc x2, urine cx pending. needs sputum cx. has rij pa cath, 2 piv\'s.\n\nsocial: husband stayed in room overnoc, supportive with care. patient has 20yo and 9yo daughter, should be into visit today. social work consulted.\n\na/p: 39yo female c severe cardiomyopathy and hf, unknown etiology. requiring milrinone and being worked up for heart transplant. continue to monitor hemodynamics and response to meds. obtain sputum cx, monitor temp. watch uo and fluid status. follow up with labs and cxr. emotionally support patient and family and keep updated on plan.\n', 'event': ['Pain', 'Sleep', 'Eating', 'Excretion', 'Family', 'Family'], 'phrase': '', 'raw_output': '{\n  "events": [\n    {\n      "event_type": "Pain",\n      "text_quote": "c/o pain in r ear (reports having chronic ear infections)",\n      "attributes": {\n        "severity": "Unknown",\n        "location": "r ear",\n        "duration": "Unknown",\n        "time": "Unknown",\n        "caused_by": "chronic ear infections"\n      }\n    },\n    {\n      "event_type": "Sleep",\n      "text_quote": "lethargic/sleeping @ change of shift. a&amp;o x 3, mae. becoming more interactive as night went on, but slept well through night.",\n      "attributes": {\n        "quality": "well",\n        "duration": "through night",\n        "time": "night",\n        "caused_by": "Unknown"\n      }\n    },\n    {\n      "event_type": "Eating",\n      "text_quote": "ate very small amount for dinner.",\n      "attributes": {\n        "food": "dinner",\n        "amount": "small",\n        "method": "oral",\n        "time": "dinner time",\n        "caused_by": "Unknown"\n      }\n    },\n    {\n      "event_type": "Excretion",\n      "text_quote": "uo decreased to nothing for 2 hours. gave 250cc ivfb x 2, and uo improved slightly.",\n      "attributes": {\n        "type": "urine",\n        "frequency": "decreased",\n        "quality": "Unknown",\n        "time": "2 hours",\n        "caused_by": "ivfb"\n      }\n    },\n    {\n      "event_type": "Family",\n      "text_quote": "husband stayed in room overnoc, supportive with care. patient has 20yo and 9yo daughter, should be into visit today.",\n      "attributes": {\n        "interaction": "visit",\n        "relation": "husband",\n        "time": "overnight",\n        "caused_by": "Unknown"\n      }\n    },\n    {\n      "event_type": "Family",\n      "text_quote": "patient has 20yo and 9yo daughter, should be into visit today.",\n      "attributes": {\n        "interaction": "visit",\n        "relation": "daughter",\n        "time": "today",\n        "caused_by": "Unknown"\n      }\n    }\n  ]\n}', 'attributes': [{'Pain': {'severity': 'Unknown', 'location': 'r ear', 'duration': 'Unknown', 'time': 'Unknown', 'caused_by': 'chronic ear infections'}}, {'Sleep': {'quality': 'well', 'duration': 'through night', 'time': 'night', 'caused_by': 'Unknown'}}, {'Eating': {'food': 'dinner', 'amount': 'small', 'method': 'oral', 'time': 'dinner time', 'caused_by': 'Unknown'}}, {'Excretion': {'type': 'urine', 'frequency': 'decreased', 'quality': 'Unknown', 'time': '2 hours', 'caused_by': 'ivfb'}}, {'Family': {'interaction': 'visit', 'relation': 'husband', 'time': 'overnight', 'caused_by': 'Unknown'}}, {'Family': {'interaction': 'visit', 'relation': 'daughter', 'time': 'today', 'caused_by': 'Unknown'}}], 'text_quotes': ['c/o pain in r ear (reports having chronic ear infections)', 'lethargic/sleeping @ change of shift. a&amp;o x 3, mae. becoming more interactive as night went on, but slept well through night.', 'ate very small amount for dinner.', 'uo decreased to nothing for 2 hours. gave 250cc ivfb x 2, and uo improved slightly.', 'husband stayed in room overnoc, supportive with care. patient has 20yo and 9yo daughter, should be into visit today.', 'patient has 20yo and 9yo daughter, should be into visit today.'], 'event_name_prompt': 'Given the text: nursing progress note 1900-0700\ns: "i feel so hot"\n\no: please see carevue for complete objective data\n\ncv: st/nsr, 90-110\'s, freq pvc\'s. on amio tid. diastolic blood pressure 90-120\'s, gave captopril 6.25mg @ [**2155**], diastolic blood pressure dropped to 79/low 80\'s @ 2100. co/ci numbers unchanged from earlier in day and patient felt no side effects. milrinone remains @ 0.375mcg/kg/min. co/ci/svr-4.9/2.3/1159. cvp 6-10, w-16. r fem angio site cd&amp;i, no hematoma. pulses palp. extremities warm and pale.\n\nresp: lungs clr c dim bases. last abg-7.48/33/87/25/1, on 4l nc. mvo2-64. persistant productive cough. no c/o sob although tachypneic at times. cxr done, gave benzonatate for cough relief.\n\ngi/gu: bs present, no bm. ate very small amount for dinner. uo decreased to nothing for 2 hours. gave 250cc ivfb x 2, and uo improved slightly. +400cc for day and -700 for los. urine becoming more concentrated.\n\nneuro: lethargic/sleeping @ change of shift. a&amp;o x 3, mae. becoming more interactive as night went on, but slept well through night. c/o pain in r ear (reports having chronic ear infections), md aware.\n\nid/access: wbc down to 13.1 from 16. slightly febrile to 100.6 at start of shift, gave tylenol 650mg, and temp down to 98.9 this am. bc x2, urine cx pending. needs sputum cx. has rij pa cath, 2 piv\'s.\n\nsocial: husband stayed in room overnoc, supportive with care. patient has 20yo and 9yo daughter, should be into visit today. social work consulted.\n\na/p: 39yo female c severe cardiomyopathy and hf, unknown etiology. requiring milrinone and being worked up for heart transplant. continue to monitor hemodynamics and response to meds. obtain sputum cx, monitor temp. watch uo and fluid status. follow up with labs and cxr. emotionally support patient and family and keep updated on plan.\n, \n                        and the following event types with their definitions: Eating : The patient takes food into their body by mouth.\nExcretion : The patient discharges waste matter from their body.\nFamily : The patient has a visit, call, or communication with a family member.\nPain : The patient reports or shows signs of pain.\nSleep : The patient sleeps or the sleep’s quality or quantity is described.\nUnknown : choose "Unknown" if none of the other event type are applicable. \n                        ---\n                        Your task:\n                        0. Identify ALL events in the text (zero, one, or more).\n1. For each event, assign an event_type from the list above.\n2. If multiple event of same type is mentioned, assign the event_type multiple times\n3. Extract attributes for each event using ONLY the allowed attributes listed below.\n4. Output strictly valid JSON following the schema below.\n                        ---\n                        Classification Rules:\n                        - A text may contain multiple events of the same or different types.\n- Create a separate event object for each event mention.\n- If the text is explicitly a NEGATION (e.g., "denies pain"), do not extract that event.\n- If the text describes a FUTURE or HYPOTHETICAL event (e.g., "will eat tomorrow"), ignore it.\n- A valid event should have occurred in the recent past or is occurring during the time of writing of the text.\n- If no events are found or if unsure, return {"events": []}\n                        \n                        ---\n                                    Attributes allowed:\n                                    {\'Eating\': {\'food\': \'&lt;string&gt; # e.g., pancakes, porridge, etc.\', \'amount\': \'&lt;string&gt; # e.g., 1, 2 bowls, etc.\', \'method\': \'&lt;string&gt;  # e.g., oral, tube, etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, after shower, etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}, \'Excretion\': {\'type\': \'&lt;string&gt; # e.g., urine, stool, etc.\', \'frequency\': \'&lt;string&gt; # e.g., 2x, once, etc.\', \'quality\': \'&lt;string&gt; # e.g., loose, hard, etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, after shower, etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}, \'Family\': {\'interaction\': \'&lt;string&gt; # e.g., visit, call, communication, etc.\', \'relation\': \'&lt;string&gt; # e.g., mother, son, etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, after shower, etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}, \'Pain\': {\'severity\': \'&lt;string&gt; # e.g., mild, moderate, severe, numeric scale if present, etc.\', \'location\': \'&lt;string&gt; # e.g., right knee, head, etc.\', \'duration\': \'&lt;string&gt; # e.g., all night, 3 hours, etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, after shower, etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}, \'Sleep\': {\'quality\': \'&lt;string&gt; # e.g., good, poor, restless, etc.\', \'duration\': \'&lt;string&gt; # e.g., 6 hours, phrases like "all night", etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, after shower, etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}}\n                                    If no relevant attribute exists for an event, return an empty object {}.\n                                    \n                        \n                        \n                        ---\n                        Output Schema (strict):\n                        {\n                                    "events": [\n                                        {\n                                        "event_type": "&lt;Pain | Sleep | Excretion | Eating | Family&gt;",\n                                        "text_quote": "&lt;fragement from the text indicating &gt;",\n                "attributes": {\n                    "&lt;attribute_name&gt;": "&lt;attribute_value&gt;"\n                }\n                                        }\n                                    ]\n                                    }\n                        \n                            Rules:\n                                - Ensure the output is valid JSON (parseable).\n                                - "eventS" must always be an array (can be empty).\n                                - Multiple instances of the same event type appear as individual elements in the event array.\n                                - Events appear in the array in the same order in which they appear in the text.\n                                - Do not include extra keys, comments, or text.\n                                - Each object in "events" must contain "event_type", "text_quote", and "attributes".\n                                -If an event attribute type has no value mentioned, return "attributes": {"&lt; attribute name &gt;:Unknown"} for each attribute type defined for the event type \n                        \n                        \n                        \n                ---\n                Examples:\n                \n                text: "Patient ate breakfast this morning. He seems less anxious."\n                output: {\n                "events": [\n                    {\n                    "event_type": "Eating",\n                    "text_quote":"Patient ate breakfast this morning",\n                    "attributes": {"food": "breakfast", \n                                   "amount": "Unknown",\n                                   "method": "Unknown",\n                                   "time":"morning",\n                                   "caused_by":"Unknown"}\n                    }\n                ]\n                }\n                \n                text: "Patient reported severe abdominal pain."\n                output: {\n                "events": [\n                    {\n                    "event_type": "Pain",\n                    "text_quote": "severe abdominal Pain",\n                    "attributes": {"severity": "severe", \n                                   "location": "abdominal",\n                                   "duration": "Unknown",\n                                   "time":"Unknown",\n                                   "caused_by":"Unknown"}\n                    }\n                ]\n                }\n                \n                text: "Patient called his son around 3 pm."\n                output: {\n                "events": [\n                    {\n                    "event_type": "Family",\n                    "text_quote": "called his son around 3 pm",\n                    "attributes": {"interaction": "call", \n                                    "relation": "son",\n                                    "time":"3 pm",\n                                    "caused_by":"Unknown"}\n                    }\n                ]\n                }\n                \n                text: "Patient had a loose stool overnight."\n                output: {\n                "events": [\n                    {\n                    "event_type": "Excretion",\n                    "text_quote": "loose stool overnight",\n                    "attributes": {"type": "stool", \n                                   "quality": "loose", \n                                   "frequency":"overnight", \n                                   "time":"night",\n                                   "caused_by":"Unknown"}\n                    }\n                ]\n                }\n                \n                text: "Patient was able to sleep well last night."\n                output: {\n                "events": [\n                    {\n                    "event_type": "Sleep",\n                    "text_quote": "sleep well last night",\n                    "attributes": {"quality": "well",\n                                    "duration": "Unknown", \n                                    "time":"night",\n                                    "caused_by":"Unknown"}\n                    }\n                ]\n                }\n                \n                text: "The patient couldn\'t sleep due to severe pain."\n                output: {\n                "events": [\n                    {\n                    "event_type": "Sleep",\n                    "text_quote": "couldn\'t sleep",\n                    "attributes": {"quality": "poor", \n                                    "duration": "Unknown",\n                                   "time":"Unknown",\n                                   "caused_by":"Pain"}\n                    },\n                    {\n                    "event_type": "Pain",\n                    "text_quote": "severe pain",\n                    "attributes": {"severity": "severe", \n                                    "location": "Unknown", \n                                    "duration": "Unknown", \n                                   "time":"before Sleep",\n                                   "caused_by":"Unknown"}\n                    }\n                ]\n                }\n                \n                text: "The patient complained of severe back pain, was given Tylenol, but the pain persisted and he was then prescribed stronger morphine."\n                output: {\n                "events": [\n                    {\n                    "event_type": "Pain",\n                    "text_quote": "complained of severe back pain",\n                    "attributes": {"severity": "severe", \n                                    "location": "back",\n                                    "duration": "Unknown", \n                                    "time":"Unknown",\n                                    "caused_by":"Unknown"}\n                    },\n                    {\n                    "event_type": "Pain",\n                    "text_quote": "pain persisted",\n                    "attributes": {"severity": "severe", \n                                   "location": "back",\n                                   "duration": "persistent", \n                                   "time":"after Tylenol",\n                                   "caused_by":"Unknown"}\n                    }\n                ]\n                }\n                \n                        ', 'event_detection_time': 17.584409018003498}</t>
-        </is>
-      </c>
-      <c r="N17" t="inlineStr">
-        <is>
-          <t>['Pain', 'Sleep', 'Eating', 'Excretion', 'Family', 'Family']</t>
-        </is>
-      </c>
       <c r="O17" t="inlineStr">
         <is>
-          <t>[{'Pain': {'severity': 'Unknown', 'location': 'r ear', 'duration': 'Unknown', 'time': 'Unknown', 'caused_by': 'chronic ear infections'}}, {'Sleep': {'quality': 'well', 'duration': 'through night', 'time': 'night', 'caused_by': 'Unknown'}}, {'Eating': {'food': 'dinner', 'amount': 'small', 'method': 'oral', 'time': 'dinner time', 'caused_by': 'Unknown'}}, {'Excretion': {'type': 'urine', 'frequency': 'decreased', 'quality': 'Unknown', 'time': '2 hours', 'caused_by': 'ivfb'}}, {'Family': {'interaction': 'visit', 'relation': 'husband', 'time': 'overnight', 'caused_by': 'Unknown'}}, {'Family': {'interaction': 'visit', 'relation': 'daughter', 'time': 'today', 'caused_by': 'Unknown'}}]</t>
-        </is>
-      </c>
-      <c r="P17" t="inlineStr">
-        <is>
-          <t>['c/o pain in r ear (reports having chronic ear infections)', 'lethargic/sleeping @ change of shift. a&amp;o x 3, mae. becoming more interactive as night went on, but slept well through night.', 'ate very small amount for dinner.', 'uo decreased to nothing for 2 hours. gave 250cc ivfb x 2, and uo improved slightly.', 'husband stayed in room overnoc, supportive with care. patient has 20yo and 9yo daughter, should be into visit today.', 'patient has 20yo and 9yo daughter, should be into visit today.']</t>
-        </is>
-      </c>
-      <c r="Q17" t="n">
-        <v>0.002976354999191244</v>
-      </c>
-      <c r="R17" t="inlineStr">
+          <t>[[['e1', 'before', 'e2'], ['e2', 'before', 'e3'], ['e3', 'before', 'e4'], ['e4', 'before', 'e5'], ['e5', 'before', 'e6'], ['e6', 'before', 'e7'], ['e7', 'before', 'e8']]]</t>
+        </is>
+      </c>
+      <c r="P17" t="n">
+        <v>0.002413090998743428</v>
+      </c>
+      <c r="Q17" t="inlineStr">
         <is>
           <t>Sleep</t>
         </is>
       </c>
-      <c r="S17" t="b">
-        <v>0</v>
+      <c r="R17" t="b">
+        <v>0</v>
+      </c>
+      <c r="S17" t="n">
+        <v>1</v>
       </c>
       <c r="T17" t="n">
         <v>1</v>
       </c>
-      <c r="U17" t="n">
-        <v>1</v>
-      </c>
-      <c r="V17" t="inlineStr">
+      <c r="U17" t="inlineStr">
         <is>
           <t>('eat', 'sleep', 'daughter', 'husband', 'family', 'pain', 'urine', 'sleeping')</t>
         </is>
       </c>
+      <c r="V17" t="n">
+        <v>27.09508548397571</v>
+      </c>
       <c r="W17" t="n">
-        <v>21.68289876100607</v>
+        <v>25.57279084197944</v>
       </c>
       <c r="X17" t="n">
-        <v>19.16748981099227</v>
+        <v>1</v>
       </c>
       <c r="Y17" t="n">
-        <v>17.5844090180035</v>
+        <v>1</v>
       </c>
       <c r="Z17" t="n">
-        <v>1</v>
-      </c>
-      <c r="AA17" t="n">
-        <v>1</v>
-      </c>
-      <c r="AB17" t="n">
-        <v>1</v>
-      </c>
-      <c r="AC17" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="18">
-      <c r="A18" t="n">
-        <v>1325552</v>
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>1325552</t>
+        </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>['Pain', 'Sleep', 'Family', 'Unknown']</t>
+          <t>('Family', 'Sleep', 'Pain', 'Unknown')</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>['sleeping', 'naps', 'husband', 'pain']</t>
+          <t>('pain', 'husband', 'sleeping', 'naps')</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
@@ -2765,120 +2612,111 @@
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>{'text': '39 yr old c cardiomyopathy\n\nst c pvcs. 3 mg captopril given p weaning milrinone to .200 .hemodynamics unchanged .ci 2.6/svr 1185.w 13 .cvp 11.bp transiently to 80 but patient asymptomatic .map &gt;60.to be started on coreg .\n\nsats 93 to 98,bs diminished .coughing continuously,med pro re nata c some relief.sputum had some blood in it .\n\nappetite fair.pos bs no stool.\n\nhuo responding to fluid 250 cc x1,then 100cc.heart rate for 1 liter.\n\npatient sleeping in naps p med for pain.husband at bedside all day .\n\nt to 100.9,tylenol given .ppd planted .\n\nmonitor fluid status\ntitrate meds as tol\nsupportive care\n', 'event': ['Eating', 'Excretion', 'Family', 'Pain', 'Sleep', 'Pain', 'Sleep'], 'phrase': '', 'raw_output': '{\n  "events": [\n    {\n      "event_type": "Eating",\n      "text_quote": "appetite fair",\n      "attributes": {\n        "food": "Unknown",\n        "amount": "Unknown",\n        "method": "Unknown",\n        "negation": "false",\n        "time": "Unknown",\n        "caused_by": "Unknown"\n      }\n    },\n    {\n      "event_type": "Excretion",\n      "text_quote": "pos bs no stool",\n      "attributes": {\n        "type": "stool",\n        "frequency": "no",\n        "quality": "Unknown",\n        "negation": "false",\n        "time": "Unknown",\n        "caused_by": "Unknown"\n      }\n    },\n    {\n      "event_type": "Family",\n      "text_quote": "husband at bedside all day",\n      "attributes": {\n        "interaction": "visit",\n        "relation": "husband",\n        "negation": "false",\n        "time": "all day",\n        "caused_by": "Unknown"\n      }\n    },\n    {\n      "event_type": "Pain",\n      "text_quote": "patient sleeping in naps p med for pain",\n      "attributes": {\n        "severity": "Unknown",\n        "location": "Unknown",\n        "duration": "Unknown",\n        "negation": "false",\n        "time": "after medication",\n        "caused_by": "medication"\n      }\n    },\n    {\n      "event_type": "Sleep",\n      "text_quote": "patient sleeping in naps p med for pain",\n      "attributes": {\n        "quality": "Unknown",\n        "duration": "naps",\n        "negation": "false",\n        "time": "after medication",\n        "caused_by": "medication"\n      }\n    },\n    {\n      "event_type": "Pain",\n      "text_quote": "coughing continuously, med pro re nata c some relief",\n      "attributes": {\n        "severity": "Unknown",\n        "location": "Unknown",\n        "duration": "continuous",\n        "negation": "false",\n        "time": "Unknown",\n        "caused_by": "Unknown"\n      }\n    },\n    {\n      "event_type": "Sleep",\n      "text_quote": "patient sleeping in naps p med for pain",\n      "attributes": {\n        "quality": "Unknown",\n        "duration": "naps",\n        "negation": "false",\n        "time": "after medication",\n        "caused_by": "medication"\n      }\n    }\n  ]\n}', 'attributes': [{'Eating': {'food': 'Unknown', 'amount': 'Unknown', 'method': 'Unknown', 'negation': 'false', 'time': 'Unknown', 'caused_by': 'Unknown'}}, {'Excretion': {'type': 'stool', 'frequency': 'no', 'quality': 'Unknown', 'negation': 'false', 'time': 'Unknown', 'caused_by': 'Unknown'}}, {'Family': {'interaction': 'visit', 'relation': 'husband', 'negation': 'false', 'time': 'all day', 'caused_by': 'Unknown'}}, {'Pain': {'severity': 'Unknown', 'location': 'Unknown', 'duration': 'Unknown', 'negation': 'false', 'time': 'after medication', 'caused_by': 'medication'}}, {'Sleep': {'quality': 'Unknown', 'duration': 'naps', 'negation': 'false', 'time': 'after medication', 'caused_by': 'medication'}}, {'Pain': {'severity': 'Unknown', 'location': 'Unknown', 'duration': 'continuous', 'negation': 'false', 'time': 'Unknown', 'caused_by': 'Unknown'}}, {'Sleep': {'quality': 'Unknown', 'duration': 'naps', 'negation': 'false', 'time': 'after medication', 'caused_by': 'medication'}}], 'text_quotes': ['appetite fair', 'pos bs no stool', 'husband at bedside all day', 'patient sleeping in naps p med for pain', 'patient sleeping in naps p med for pain', 'coughing continuously, med pro re nata c some relief', 'patient sleeping in naps p med for pain'], 'event_name_prompt': 'Given the text: 39 yr old c cardiomyopathy\n\nst c pvcs. 3 mg captopril given p weaning milrinone to .200 .hemodynamics unchanged .ci 2.6/svr 1185.w 13 .cvp 11.bp transiently to 80 but patient asymptomatic .map &gt;60.to be started on coreg .\n\nsats 93 to 98,bs diminished .coughing continuously,med pro re nata c some relief.sputum had some blood in it .\n\nappetite fair.pos bs no stool.\n\nhuo responding to fluid 250 cc x1,then 100cc.heart rate for 1 liter.\n\npatient sleeping in naps p med for pain.husband at bedside all day .\n\nt to 100.9,tylenol given .ppd planted .\n\nmonitor fluid status\ntitrate meds as tol\nsupportive care\n, \n                        and the following event types with their definitions: Eating : The patient takes food into their body by mouth.\nExcretion : The patient discharges waste matter from their body.\nFamily : The patient has a visit, call, or communication with a family member.\nPain : The patient reports or shows signs of pain.\nSleep : The patient sleeps or the sleep’s quality or quantity is described.\nUnknown : choose "Unknown" if none of the other event type are applicable. \n                        ---\n                        Your task:\n                        0. Identify ALL events in the text (zero, one, or more).\n1. For each event, assign an event_type from the list above.\n2. If multiple event of same type is mentioned, assign the event_type multiple times\n3. Extract attributes for each event using ONLY the allowed attributes listed below.\n4. Use keyword evidence (Ki) ONLY if it is consistent with the text context.\n5. Output strictly valid JSON following the schema below.\n                        ---\n                        Classification Rules:\n                        - A text may contain multiple events of the same or different types.\n- Create a separate event object for each event mention.\n- If the text is explicitly a NEGATION (e.g., "denies pain"), do not extract that event.\n- If the text describes a FUTURE or HYPOTHETICAL event (e.g., "will eat tomorrow"), ignore it.\n- A valid event should have occurred in the recent past or is occurring during the time of writing of the text.\n- If no events are found or if unsure, return {"events": []}\n                        \n                        ---\n                                    Attributes allowed:\n                                    {\'Eating\': {\'food\': \'&lt;string&gt; # e.g., pancakes, porridge, etc.\', \'amount\': \'&lt;string&gt; # e.g., 1, 2 bowls, etc.\', \'method\': \'&lt;string&gt;  # e.g., oral, tube, etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, after shower, etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}, \'Excretion\': {\'type\': \'&lt;string&gt; # e.g., urine, stool, etc.\', \'frequency\': \'&lt;string&gt; # e.g., 2x, once, etc.\', \'quality\': \'&lt;string&gt; # e.g., loose, hard, etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, after shower, etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}, \'Family\': {\'interaction\': \'&lt;string&gt; # e.g., visit, call, communication, etc.\', \'relation\': \'&lt;string&gt; # e.g., mother, son, etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, after shower, etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}, \'Pain\': {\'severity\': \'&lt;string&gt; # e.g., mild, moderate, severe, numeric scale if present, etc.\', \'location\': \'&lt;string&gt; # e.g., right knee, head, etc.\', \'duration\': \'&lt;string&gt; # e.g., all night, 3 hours, etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, after shower, etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}, \'Sleep\': {\'quality\': \'&lt;string&gt; # e.g., good, poor, restless, etc.\', \'duration\': \'&lt;string&gt; # e.g., 6 hours, phrases like "all night", etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, after shower, etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}}\n                                    If no relevant attribute exists for an event, return an empty object {}.\n                                    \n                        \n                        ---\n                                    Keyword evidence (Ki):\n                                    Additional facts: A keyword matching algorithm without context detected keyword(s) [\'sleeping\', \'naps\', \'husband\', \'pain\'].\n                                    Use this only as a pointer. If context contradicts, ignore.\n                        ---\n                        Output Schema (strict):\n                        {\n                                    "events": [\n                                        {\n                                        "event_type": "&lt;Pain | Sleep | Excretion | Eating | Family&gt;",\n                                        "text_quote": "&lt;fragement from the text indicating &gt;",\n                "attributes": {\n                    "&lt;attribute_name&gt;": "&lt;attribute_value&gt;"\n                }\n                                        }\n                                    ]\n                                    }\n                        \n                            Rules:\n                                - Ensure the output is valid JSON (parseable).\n                                - "eventS" must always be an array (can be empty).\n                                - Multiple instances of the same event type appear as individual elements in the event array.\n                                - Events appear in the array in the same order in which they appear in the text.\n                                - Do not include extra keys, comments, or text.\n                                - Each object in "events" must contain "event_type", "text_quote", and "attributes".\n                                -If an event attribute type has no value mentioned, return "attributes": {"&lt; attribute name &gt;:Unknown"} for each attribute type defined for the event type \n                        \n                        \n                        \n                ---\n                Examples:\n                \n                text: "Patient ate breakfast this morning. He seems less anxious."\n                output: {\n                "events": [\n                    {\n                    "event_type": "Eating",\n                    "text_quote":"Patient ate breakfast this morning",\n                    "attributes": {"food": "breakfast", \n                                   "amount": "Unknown",\n                                   "method": "Unknown",\n                                   "time":"morning",\n                                   "caused_by":"Unknown"}\n                    }\n                ]\n                }\n                \n                text: "Patient reported severe abdominal pain."\n                output: {\n                "events": [\n                    {\n                    "event_type": "Pain",\n                    "text_quote": "severe abdominal Pain",\n                    "attributes": {"severity": "severe", \n                                   "location": "abdominal",\n                                   "duration": "Unknown",\n                                   "time":"Unknown",\n                                   "caused_by":"Unknown"}\n                    }\n                ]\n                }\n                \n                text: "Patient called his son around 3 pm."\n                output: {\n                "events": [\n                    {\n                    "event_type": "Family",\n                    "text_quote": "called his son around 3 pm",\n                    "attributes": {"interaction": "call", \n                                    "relation": "son",\n                                    "time":"3 pm",\n                                    "caused_by":"Unknown"}\n                    }\n                ]\n                }\n                \n                text: "Patient had a loose stool overnight."\n                output: {\n                "events": [\n                    {\n                    "event_type": "Excretion",\n                    "text_quote": "loose stool overnight",\n                    "attributes": {"type": "stool", \n                                   "quality": "loose", \n                                   "frequency":"overnight", \n                                   "time":"night",\n                                   "caused_by":"Unknown"}\n                    }\n                ]\n                }\n                \n                text: "Patient was able to sleep well last night."\n                output: {\n                "events": [\n                    {\n                    "event_type": "Sleep",\n                    "text_quote": "sleep well last night",\n                    "attributes": {"quality": "well",\n                                    "duration": "Unknown", \n                                    "time":"night",\n                                    "caused_by":"Unknown"}\n                    }\n                ]\n                }\n                \n                text: "The patient couldn\'t sleep due to severe pain."\n                output: {\n                "events": [\n                    {\n                    "event_type": "Sleep",\n                    "text_quote": "couldn\'t sleep",\n                    "attributes": {"quality": "poor", \n                                    "duration": "Unknown",\n                                   "time":"Unknown",\n                                   "caused_by":"Pain"}\n                    },\n                    {\n                    "event_type": "Pain",\n                    "text_quote": "severe pain",\n                    "attributes": {"severity": "severe", \n                                    "location": "Unknown", \n                                    "duration": "Unknown", \n                                   "time":"before Sleep",\n                                   "caused_by":"Unknown"}\n                    }\n                ]\n                }\n                \n                text: "The patient complained of severe back pain, was given Tylenol, but the pain persisted and he was then prescribed stronger morphine."\n                output: {\n                "events": [\n                    {\n                    "event_type": "Pain",\n                    "text_quote": "complained of severe back pain",\n                    "attributes": {"severity": "severe", \n                                    "location": "back",\n                                    "duration": "Unknown", \n                                    "time":"Unknown",\n                                    "caused_by":"Unknown"}\n                    },\n                    {\n                    "event_type": "Pain",\n                    "text_quote": "pain persisted",\n                    "attributes": {"severity": "severe", \n                                   "location": "back",\n                                   "duration": "persistent", \n                                   "time":"after Tylenol",\n                                   "caused_by":"Unknown"}\n                    }\n                ]\n                }\n                \n                        ', 'event_detection_time': 18.573997673011036}</t>
+          <t>['pain', 'husband', 'nap', 'sleeping']</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>['Eating', 'Excretion', 'Family', 'Pain', 'Sleep', 'Pain', 'Sleep']</t>
+          <t>{'text': '39 yr old c cardiomyopathy\n\nst c pvcs. 3 mg captopril given p weaning milrinone to .200 .hemodynamics unchanged .ci 2.6/svr 1185.w 13 .cvp 11.bp transiently to 80 but patient asymptomatic .map &gt;60.to be started on coreg .\n\nsats 93 to 98,bs diminished .coughing continuously,med pro re nata c some relief.sputum had some blood in it .\n\nappetite fair.pos bs no stool.\n\nhuo responding to fluid 250 cc x1,then 100cc.heart rate for 1 liter.\n\npatient sleeping in naps p med for pain.husband at bedside all day .\n\nt to 100.9,tylenol given .ppd planted .\n\nmonitor fluid status\ntitrate meds as tol\nsupportive care\n', 'event': ['Eating', 'Excretion', 'Pain', 'Sleep', 'Family'], 'event_id': ['e1', 'e2', 'e3', 'e4', 'e5'], 'phrase': '', 'raw_output': '{\n  "events": [\n    {\n      "event_id": "e1",\n      "event_type": "Eating",\n      "text_quote": "appetite fair",\n      "attributes": {\n        "food": "Unknown",\n        "amount": "Unknown",\n        "method": "Unknown",\n        "negation": "false",\n        "time": "Unknown",\n        "caused_by": "Unknown"\n      }\n    },\n    {\n      "event_id": "e2",\n      "event_type": "Excretion",\n      "text_quote": "pos bs no stool",\n      "attributes": {\n        "type": "stool",\n        "frequency": "none",\n        "quality": "Unknown",\n        "negation": "true",\n        "time": "Unknown",\n        "caused_by": "Unknown"\n      }\n    },\n    {\n      "event_id": "e3",\n      "event_type": "Pain",\n      "text_quote": "patient sleeping in naps p med for pain",\n      "attributes": {\n        "severity": "Unknown",\n        "location": "Unknown",\n        "duration": "Unknown",\n        "negation": "false",\n        "time": "after medication",\n        "caused_by": "medication"\n      }\n    },\n    {\n      "event_id": "e4",\n      "event_type": "Sleep",\n      "text_quote": "patient sleeping in naps p med for pain",\n      "attributes": {\n        "quality": "Unknown",\n        "duration": "naps",\n        "negation": "false",\n        "time": "after medication",\n        "caused_by": "medication"\n      }\n    },\n    {\n      "event_id": "e5",\n      "event_type": "Family",\n      "text_quote": "husband at bedside all day",\n      "attributes": {\n        "interaction": "visit",\n        "relation": "husband",\n        "negation": "false",\n        "time": "all day",\n        "caused_by": "Unknown"\n      }\n    }\n  ],\n  "order": []\n}', 'attributes': [{'Eating': {'food': 'Unknown', 'amount': 'Unknown', 'method': 'Unknown', 'negation': 'false', 'time': 'Unknown', 'caused_by': 'Unknown'}}, {'Excretion': {'type': 'stool', 'frequency': 'none', 'quality': 'Unknown', 'negation': 'true', 'time': 'Unknown', 'caused_by': 'Unknown'}}, {'Pain': {'severity': 'Unknown', 'location': 'Unknown', 'duration': 'Unknown', 'negation': 'false', 'time': 'after medication', 'caused_by': 'medication'}}, {'Sleep': {'quality': 'Unknown', 'duration': 'naps', 'negation': 'false', 'time': 'after medication', 'caused_by': 'medication'}}, {'Family': {'interaction': 'visit', 'relation': 'husband', 'negation': 'false', 'time': 'all day', 'caused_by': 'Unknown'}}], 'orders': [[]], 'text_quotes': ['appetite fair', 'pos bs no stool', 'patient sleeping in naps p med for pain', 'patient sleeping in naps p med for pain', 'husband at bedside all day'], 'event_name_prompt': 'Given the text: 39 yr old c cardiomyopathy\n\nst c pvcs. 3 mg captopril given p weaning milrinone to .200 .hemodynamics unchanged .ci 2.6/svr 1185.w 13 .cvp 11.bp transiently to 80 but patient asymptomatic .map &gt;60.to be started on coreg .\n\nsats 93 to 98,bs diminished .coughing continuously,med pro re nata c some relief.sputum had some blood in it .\n\nappetite fair.pos bs no stool.\n\nhuo responding to fluid 250 cc x1,then 100cc.heart rate for 1 liter.\n\npatient sleeping in naps p med for pain.husband at bedside all day .\n\nt to 100.9,tylenol given .ppd planted .\n\nmonitor fluid status\ntitrate meds as tol\nsupportive care\n, \n                        and the following event types with their definitions: Eating : The patient takes food into their body by mouth.\nExcretion : The patient discharges waste matter from their body.\nFamily : The patient has a visit, call, or communication with a family member.\nPain : The patient reports or shows signs of pain.\nSleep : The patient sleeps or the sleep’s quality or quantity is described.\nUnknown : choose "Unknown" if none of the other event type are applicable. \n                        ---\n                        Your task:\n                        0. Identify ALL events in the text (zero, one, or more).\n1. For each event, assign an event_type from the list above.\n2. If multiple event of same type is mentioned, assign the event_type multiple times\n3. Extract attributes for each event using ONLY the allowed attributes listed below.\n4. Use keyword evidence (Ki) ONLY if it is consistent with the text context.\n5. Output strictly valid JSON following the schema below.\n                        ---\n                        Classification Rules:\n                        - A text may contain multiple events of the same or different types.\n- Create a separate event object for each event mention.\n- If the text is explicitly a NEGATION (e.g., "denies pain"), do not extract that event.\n- If the text describes a FUTURE or HYPOTHETICAL event (e.g., "will eat tomorrow"), ignore it.\n- A valid event should have occurred in the recent past or is occurring during the time of writing of the text.\n- If no events are found or if unsure, return {"events": []}\n                        \n                        ---\n                                    Attributes allowed:\n                                    {\'Eating\': {\'food\': \'&lt;string&gt; # e.g., pancakes, porridge, etc.\', \'amount\': \'&lt;string&gt; # e.g., 1, 2 bowls, etc.\', \'method\': \'&lt;string&gt;  # e.g., oral, tube, etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, evening etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}, \'Excretion\': {\'type\': \'&lt;string&gt; # e.g., urine, stool, etc.\', \'frequency\': \'&lt;string&gt; # e.g., 2x, once, etc.\', \'quality\': \'&lt;string&gt; # e.g., loose, hard, etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, evening etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}, \'Family\': {\'interaction\': \'&lt;string&gt; # e.g., visit, call, communication, etc.\', \'relation\': \'&lt;string&gt; # e.g., mother, son, etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, evening etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}, \'Pain\': {\'severity\': \'&lt;string&gt; # e.g., mild, moderate, severe, numeric scale if present, etc.\', \'location\': \'&lt;string&gt; # e.g., right knee, head, etc.\', \'duration\': \'&lt;string&gt; # e.g., all night, 3 hours, etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, evening etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}, \'Sleep\': {\'quality\': \'&lt;string&gt; # e.g., good, poor, restless, etc.\', \'duration\': \'&lt;string&gt; # e.g., 6 hours, phrases like "all night", etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, evening etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}}\n                                    If no relevant attribute exists for an event, return an empty object {}.\n                                    \n                        \n                        ---\n                                    Keyword evidence (Ki):\n                                    Additional facts: A keyword matching algorithm without context detected keyword(s) (\'pain\', \'husband\', \'sleeping\', \'naps\').\n                                    Use this only as a pointer. If context contradicts, ignore.\n                        ---\n                        Output Schema (strict):\n                        {\n                                    "events": [\n                                        {\n                                        "event_id": "&lt; A unique id eg.: e1 | e2 |...&gt;"\n                                        "event_type": "&lt;Pain | Sleep | Excretion | Eating | Family&gt;",\n                                        "text_quote": "&lt;fragement from the text indicating the event_type&gt;",\n                "attributes": {\n                    "&lt;attribute_name&gt;": "&lt;attribute_value&gt;"\n                }\n                                        }\n                                    ],\n                                    "order": [\n                                        ["e1", "before" | "after" | "simultaneous", "e2" ]\n                                    ]\n                                    }\n                        \n                            Rules:\n                                - Ensure the output is valid JSON (parseable).\n                                - "eventS" must always be an array (can be empty).\n                                - Multiple instances of the same event type appear with different ids.\n                                - Events appear in the array in the same order in which they appear in the text.\n                                - Their partial orders can be expressed using the "order" section.\n                                - Do not include extra keys, comments, or text.\n                                - Each object in "events" must contain "event_type", "text_quote", and "attributes".\n                                - If an event attribute type has no value mentioned, return "attributes": {"&lt; attribute name &gt;:Unknown"} for each attribute type defined for the event type \n                        \n                        \n                        \n                ---\n                Examples:\n                \n                text: "Patient ate breakfast this morning. He seems less anxious."\n                output: {\n                "events": [\n                    {"event_id": "e1",\n                    "event_type": "Eating",\n                    "text_quote":"Patient ate breakfast this morning",\n                    "attributes": {"food": "breakfast", \n                                   "amount": "Unknown",\n                                   "method": "Unknown",\n                                   "negation": "false",\n                                   "time":"morning",\n                                   "caused_by":"Unknown"}\n                    }\n                ],\n                "order":[]\n                }\n                \n                text: "Patient reported severe abdominal pain."\n                output: {\n                "events": [\n                    {"event_id": "e1",\n                    "event_type": "Pain",\n                    "text_quote": "severe abdominal Pain",\n                    "attributes": {"severity": "severe", \n                                   "location": "abdominal",\n                                   "duration": "Unknown",\n                                   "negation": "false",\n                                   "time":"Unknown",\n                                   "caused_by":"Unknown"}\n                    }\n                ],\n                "order":[]\n                }\n                \n                text: "Patient called his son around 3 pm."\n                output: {\n                "events": [\n                    {"event_id": "e1",\n                    "event_type": "Family",\n                    "text_quote": "called his son around 3 pm",\n                    "attributes": {"interaction": "call", \n                                    "relation": "son",\n                                    "negation": "false",\n                                    "time":"3 pm",\n                                    "caused_by":"Unknown"}\n                    }\n                ],\n                "order":[]\n                }\n                \n                text: "Patient had a loose stool overnight."\n                output: {\n                "events": [\n                    {"event_id": "e1",\n                    "event_type": "Excretion",\n                    "text_quote": "loose stool overnight",\n                    "attributes": {"type": "stool", \n                                   "quality": "loose", \n                                   "frequency":"overnight", \n                                   "negation": "false",\n                                   "time":"night",\n                                   "caused_by":"Unknown"}\n                    }\n                ],\n                "order":[]\n                }\n                \n                text: "Patient was able to sleep well last night."\n                output: {\n                "events": [\n                    {"event_id": "e1",\n                    "event_type": "Sleep",\n                    "text_quote": "sleep well last night",\n                    "attributes": {"quality": "well",\n                                    "duration": "Unknown", \n                                    "negation": "false",\n                                    "time":"night",\n                                    "caused_by":"Unknown"}\n                    }\n                ],\n                "order":[]\n                }\n                \n                text: "The patient couldn\'t sleep due to severe pain."\n                output: {\n                "events": [\n                    {"event_id": "e1",\n                    "event_type": "Sleep",\n                    "text_quote": "couldn\'t sleep",\n                    "attributes": {"quality": "poor", \n                                    "duration": "Unknown",\n                                    "negation": "true",\n                                    "time":"Unknown",\n                                    "caused_by":"Pain"}\n                    },\n                    {"event_id": "e2",\n                    "event_type": "Pain",\n                    "text_quote": "severe pain",\n                    "attributes": {"severity": "severe", \n                                    "location": "Unknown", \n                                    "duration": "Unknown", \n                                    "time":"Unknown",\n                                    "caused_by":"Unknown"}\n                    }\n                ],\n                "order":["e1", "after", "e2"]\n                }\n                \n                text: "The patient complained of severe back pain, was given Tylenol, but the pain persisted and he was then prescribed stronger morphine."\n                output: {\n                "events": [\n                    {"event_id": "e1",\n                    "event_type": "Pain",\n                    "text_quote": "complained of severe back pain",\n                    "attributes": {"severity": "severe", \n                                    "location": "back",\n                                    "duration": "Unknown", \n                                    "time":"Unknown",\n                                    "caused_by":"Unknown"}\n                    },\n                    {"event_id": "e2",\n                    "event_type": "Pain",\n                    "text_quote": "pain persisted",\n                    "attributes": {"severity": "severe", \n                                   "location": "back",\n                                   "duration": "persistent", \n                                   "time":"after Tylenol",\n                                   "caused_by":"Unknown"}\n                    }\n                ],\n                "order":[["e1", "before", "e2"]]\n                }\n                \n                        ', 'event_detection_time': 15.619935891008936}</t>
         </is>
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>[{'Eating': {'food': 'Unknown', 'amount': 'Unknown', 'method': 'Unknown', 'negation': 'false', 'time': 'Unknown', 'caused_by': 'Unknown'}}, {'Excretion': {'type': 'stool', 'frequency': 'no', 'quality': 'Unknown', 'negation': 'false', 'time': 'Unknown', 'caused_by': 'Unknown'}}, {'Family': {'interaction': 'visit', 'relation': 'husband', 'negation': 'false', 'time': 'all day', 'caused_by': 'Unknown'}}, {'Pain': {'severity': 'Unknown', 'location': 'Unknown', 'duration': 'Unknown', 'negation': 'false', 'time': 'after medication', 'caused_by': 'medication'}}, {'Sleep': {'quality': 'Unknown', 'duration': 'naps', 'negation': 'false', 'time': 'after medication', 'caused_by': 'medication'}}, {'Pain': {'severity': 'Unknown', 'location': 'Unknown', 'duration': 'continuous', 'negation': 'false', 'time': 'Unknown', 'caused_by': 'Unknown'}}, {'Sleep': {'quality': 'Unknown', 'duration': 'naps', 'negation': 'false', 'time': 'after medication', 'caused_by': 'medication'}}]</t>
+          <t>['Eating', 'Excretion', 'Pain', 'Sleep', 'Family']</t>
         </is>
       </c>
       <c r="H18" t="inlineStr">
         <is>
-          <t>['appetite fair', 'pos bs no stool', 'husband at bedside all day', 'patient sleeping in naps p med for pain', 'patient sleeping in naps p med for pain', 'coughing continuously, med pro re nata c some relief', 'patient sleeping in naps p med for pain']</t>
+          <t>[{'Eating': {'food': 'Unknown', 'amount': 'Unknown', 'method': 'Unknown', 'negation': 'false', 'time': 'Unknown', 'caused_by': 'Unknown'}}, {'Excretion': {'type': 'stool', 'frequency': 'none', 'quality': 'Unknown', 'negation': 'true', 'time': 'Unknown', 'caused_by': 'Unknown'}}, {'Pain': {'severity': 'Unknown', 'location': 'Unknown', 'duration': 'Unknown', 'negation': 'false', 'time': 'after medication', 'caused_by': 'medication'}}, {'Sleep': {'quality': 'Unknown', 'duration': 'naps', 'negation': 'false', 'time': 'after medication', 'caused_by': 'medication'}}, {'Family': {'interaction': 'visit', 'relation': 'husband', 'negation': 'false', 'time': 'all day', 'caused_by': 'Unknown'}}]</t>
         </is>
       </c>
       <c r="I18" t="inlineStr">
         <is>
-          <t>{'text': '39 yr old c cardiomyopathy\n\nst c pvcs. 3 mg captopril given p weaning milrinone to .200 .hemodynamics unchanged .ci 2.6/svr 1185.w 13 .cvp 11.bp transiently to 80 but patient asymptomatic .map &gt;60.to be started on coreg .\n\nsats 93 to 98,bs diminished .coughing continuously,med pro re nata c some relief.sputum had some blood in it .\n\nappetite fair.pos bs no stool.\n\nhuo responding to fluid 250 cc x1,then 100cc.heart rate for 1 liter.\n\npatient sleeping in naps p med for pain.husband at bedside all day .\n\nt to 100.9,tylenol given .ppd planted .\n\nmonitor fluid status\ntitrate meds as tol\nsupportive care\n', 'event': ['Sleep', 'Pain', 'Family', 'Excretion', 'Eating'], 'phrase': '', 'raw_output': '{\n  "events": [\n    {\n      "event_type": "Sleep",\n      "text_quote": "patient sleeping in naps p med for pain.",\n      "attributes": {\n        "quality": "Unknown",\n        "duration": "naps",\n        "negation": false,\n        "time": "Unknown",\n        "caused_by": "med"\n      }\n    },\n    {\n      "event_type": "Pain",\n      "text_quote": "patient sleeping in naps p med for pain.",\n      "attributes": {\n        "severity": "Unknown",\n        "location": "Unknown",\n        "duration": "Unknown",\n        "negation": false,\n        "time": "Unknown",\n        "caused_by": "Unknown"\n      }\n    },\n    {\n      "event_type": "Family",\n      "text_quote": "husband at bedside all day .",\n      "attributes": {\n        "interaction": "visit",\n        "relation": "husband",\n        "negation": false,\n        "time": "all day",\n        "caused_by": "Unknown"\n      }\n    },\n    {\n      "event_type": "Excretion",\n      "text_quote": "pos bs no stool.",\n      "attributes": {\n        "type": "stool",\n        "frequency": "no",\n        "quality": "Unknown",\n        "negation": false,\n        "time": "Unknown",\n        "caused_by": "Unknown"\n      }\n    },\n    {\n      "event_type": "Eating",\n      "text_quote": "appetite fair.",\n      "attributes": {\n        "food": "Unknown",\n        "amount": "Unknown",\n        "method": "Unknown",\n        "negation": false,\n        "time": "Unknown",\n        "caused_by": "Unknown"\n      }\n    }\n  ]\n}', 'attributes': [{'Sleep': {'quality': 'Unknown', 'duration': 'naps', 'negation': False, 'time': 'Unknown', 'caused_by': 'med'}}, {'Pain': {'severity': 'Unknown', 'location': 'Unknown', 'duration': 'Unknown', 'negation': False, 'time': 'Unknown', 'caused_by': 'Unknown'}}, {'Family': {'interaction': 'visit', 'relation': 'husband', 'negation': False, 'time': 'all day', 'caused_by': 'Unknown'}}, {'Excretion': {'type': 'stool', 'frequency': 'no', 'quality': 'Unknown', 'negation': False, 'time': 'Unknown', 'caused_by': 'Unknown'}}, {'Eating': {'food': 'Unknown', 'amount': 'Unknown', 'method': 'Unknown', 'negation': False, 'time': 'Unknown', 'caused_by': 'Unknown'}}], 'text_quotes': ['patient sleeping in naps p med for pain.', 'patient sleeping in naps p med for pain.', 'husband at bedside all day .', 'pos bs no stool.', 'appetite fair.'], 'event_name_prompt': 'Given the text: 39 yr old c cardiomyopathy\n\nst c pvcs. 3 mg captopril given p weaning milrinone to .200 .hemodynamics unchanged .ci 2.6/svr 1185.w 13 .cvp 11.bp transiently to 80 but patient asymptomatic .map &gt;60.to be started on coreg .\n\nsats 93 to 98,bs diminished .coughing continuously,med pro re nata c some relief.sputum had some blood in it .\n\nappetite fair.pos bs no stool.\n\nhuo responding to fluid 250 cc x1,then 100cc.heart rate for 1 liter.\n\npatient sleeping in naps p med for pain.husband at bedside all day .\n\nt to 100.9,tylenol given .ppd planted .\n\nmonitor fluid status\ntitrate meds as tol\nsupportive care\n, \n                        and the following event types with their definitions: Eating : The patient takes food into their body by mouth.\nExcretion : The patient discharges waste matter from their body.\nFamily : The patient has a visit, call, or communication with a family member.\nPain : The patient reports or shows signs of pain.\nSleep : The patient sleeps or the sleep’s quality or quantity is described.\nUnknown : choose "Unknown" if none of the other event type are applicable. \n                        ---\n                        Your task:\n                        0. Identify ALL events in the text (zero, one, or more).\n1. For each event, assign an event_type from the list above.\n2. If multiple event of same type is mentioned, assign the event_type multiple times\n3. Extract attributes for each event using ONLY the allowed attributes listed below.\n4. Use keyword evidence (Ki) ONLY if it is consistent with the text context.\n5. Output strictly valid JSON following the schema below.\n                        ---\n                        Classification Rules:\n                        - A text may contain multiple events of the same or different types.\n- Create a separate event object for each event mention.\n- If the text is explicitly a NEGATION (e.g., "denies pain"), do not extract that event.\n- If the text describes a FUTURE or HYPOTHETICAL event (e.g., "will eat tomorrow"), ignore it.\n- A valid event should have occurred in the recent past or is occurring during the time of writing of the text.\n- If no events are found or if unsure, return {"events": []}\n                        \n                        ---\n                                    Attributes allowed:\n                                    {\'Eating\': {\'food\': \'&lt;string&gt; # e.g., pancakes, porridge, etc.\', \'amount\': \'&lt;string&gt; # e.g., 1, 2 bowls, etc.\', \'method\': \'&lt;string&gt;  # e.g., oral, tube, etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, after shower, etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}, \'Excretion\': {\'type\': \'&lt;string&gt; # e.g., urine, stool, etc.\', \'frequency\': \'&lt;string&gt; # e.g., 2x, once, etc.\', \'quality\': \'&lt;string&gt; # e.g., loose, hard, etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, after shower, etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}, \'Family\': {\'interaction\': \'&lt;string&gt; # e.g., visit, call, communication, etc.\', \'relation\': \'&lt;string&gt; # e.g., mother, son, etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, after shower, etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}, \'Pain\': {\'severity\': \'&lt;string&gt; # e.g., mild, moderate, severe, numeric scale if present, etc.\', \'location\': \'&lt;string&gt; # e.g., right knee, head, etc.\', \'duration\': \'&lt;string&gt; # e.g., all night, 3 hours, etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, after shower, etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}, \'Sleep\': {\'quality\': \'&lt;string&gt; # e.g., good, poor, restless, etc.\', \'duration\': \'&lt;string&gt; # e.g., 6 hours, phrases like "all night", etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, after shower, etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}}\n                                    If no relevant attribute exists for an event, return an empty object {}.\n                                    \n                        \n                        ---\n                                    Keyword evidence (Ki):\n                                    Additional facts: A keyword matching algorithm without context detected keyword(s) [\'sleeping\', \'naps\', \'husband\', \'pain\'].\n                                    Use this only as a pointer. If context contradicts, ignore.\n                        ---\n                        Output Schema (strict):\n                        {\n                                    "events": [\n                                        {\n                                        "event_type": "&lt;Pain | Sleep | Excretion | Eating | Family&gt;",\n                                        "text_quote": "&lt;fragement from the text indicating &gt;",\n                "attributes": {\n                    "&lt;attribute_name&gt;": "&lt;attribute_value&gt;"\n                }\n                                        }\n                                    ]\n                                    }\n                        \n                            Rules:\n                                - Ensure the output is valid JSON (parseable).\n                                - "eventS" must always be an array (can be empty).\n                                - Multiple instances of the same event type appear as individual elements in the event array.\n                                - Events appear in the array in the same order in which they appear in the text.\n                                - Do not include extra keys, comments, or text.\n                                - Each object in "events" must contain "event_type", "text_quote", and "attributes".\n                                -If an event attribute type has no value mentioned, return "attributes": {"&lt; attribute name &gt;:Unknown"} for each attribute type defined for the event type \n                        \n                        \n                        \n                        ', 'event_detection_time': 12.768016572998022}</t>
+          <t>['appetite fair', 'pos bs no stool', 'patient sleeping in naps p med for pain', 'patient sleeping in naps p med for pain', 'husband at bedside all day']</t>
         </is>
       </c>
       <c r="J18" t="inlineStr">
         <is>
-          <t>['Sleep', 'Pain', 'Family', 'Excretion', 'Eating']</t>
+          <t>[[]]</t>
         </is>
       </c>
       <c r="K18" t="inlineStr">
         <is>
-          <t>[{'Sleep': {'quality': 'Unknown', 'duration': 'naps', 'negation': False, 'time': 'Unknown', 'caused_by': 'med'}}, {'Pain': {'severity': 'Unknown', 'location': 'Unknown', 'duration': 'Unknown', 'negation': False, 'time': 'Unknown', 'caused_by': 'Unknown'}}, {'Family': {'interaction': 'visit', 'relation': 'husband', 'negation': False, 'time': 'all day', 'caused_by': 'Unknown'}}, {'Excretion': {'type': 'stool', 'frequency': 'no', 'quality': 'Unknown', 'negation': False, 'time': 'Unknown', 'caused_by': 'Unknown'}}, {'Eating': {'food': 'Unknown', 'amount': 'Unknown', 'method': 'Unknown', 'negation': False, 'time': 'Unknown', 'caused_by': 'Unknown'}}]</t>
+          <t>{'text': '39 yr old c cardiomyopathy\n\nst c pvcs. 3 mg captopril given p weaning milrinone to .200 .hemodynamics unchanged .ci 2.6/svr 1185.w 13 .cvp 11.bp transiently to 80 but patient asymptomatic .map &gt;60.to be started on coreg .\n\nsats 93 to 98,bs diminished .coughing continuously,med pro re nata c some relief.sputum had some blood in it .\n\nappetite fair.pos bs no stool.\n\nhuo responding to fluid 250 cc x1,then 100cc.heart rate for 1 liter.\n\npatient sleeping in naps p med for pain.husband at bedside all day .\n\nt to 100.9,tylenol given .ppd planted .\n\nmonitor fluid status\ntitrate meds as tol\nsupportive care\n', 'event': ['Pain', 'Sleep', 'Family', 'Eating', 'Excretion'], 'event_id': ['e1', 'e2', 'e3', 'e4', 'e5'], 'phrase': '', 'raw_output': '{\n  "events": [\n    {\n      "event_id": "e1",\n      "event_type": "Pain",\n      "text_quote": "patient sleeping in naps p med for pain",\n      "attributes": {\n        "severity": "Unknown",\n        "location": "Unknown",\n        "duration": "Unknown",\n        "negation": false,\n        "time": "Unknown",\n        "caused_by": "medication"\n      }\n    },\n    {\n      "event_id": "e2",\n      "event_type": "Sleep",\n      "text_quote": "patient sleeping in naps p med for pain",\n      "attributes": {\n        "quality": "Unknown",\n        "duration": "naps",\n        "negation": false,\n        "time": "Unknown",\n        "caused_by": "medication"\n      }\n    },\n    {\n      "event_id": "e3",\n      "event_type": "Family",\n      "text_quote": "husband at bedside all day",\n      "attributes": {\n        "interaction": "visit",\n        "relation": "husband",\n        "negation": false,\n        "time": "all day",\n        "caused_by": "Unknown"\n      }\n    },\n    {\n      "event_id": "e4",\n      "event_type": "Eating",\n      "text_quote": "appetite fair",\n      "attributes": {\n        "food": "Unknown",\n        "amount": "Unknown",\n        "method": "Unknown",\n        "negation": false,\n        "time": "Unknown",\n        "caused_by": "Unknown"\n      }\n    },\n    {\n      "event_id": "e5",\n      "event_type": "Excretion",\n      "text_quote": "pos bs no stool",\n      "attributes": {\n        "type": "stool",\n        "frequency": "no",\n        "quality": "Unknown",\n        "negation": false,\n        "time": "Unknown",\n        "caused_by": "Unknown"\n      }\n    }\n  ],\n  "order": [\n    ["e1", "simultaneous", "e2"],\n    ["e3", "after", "e1"],\n    ["e4", "before", "e5"]\n  ]\n}', 'attributes': [{'Pain': {'severity': 'Unknown', 'location': 'Unknown', 'duration': 'Unknown', 'negation': False, 'time': 'Unknown', 'caused_by': 'medication'}}, {'Sleep': {'quality': 'Unknown', 'duration': 'naps', 'negation': False, 'time': 'Unknown', 'caused_by': 'medication'}}, {'Family': {'interaction': 'visit', 'relation': 'husband', 'negation': False, 'time': 'all day', 'caused_by': 'Unknown'}}, {'Eating': {'food': 'Unknown', 'amount': 'Unknown', 'method': 'Unknown', 'negation': False, 'time': 'Unknown', 'caused_by': 'Unknown'}}, {'Excretion': {'type': 'stool', 'frequency': 'no', 'quality': 'Unknown', 'negation': False, 'time': 'Unknown', 'caused_by': 'Unknown'}}], 'orders': [[['e1', 'simultaneous', 'e2'], ['e3', 'after', 'e1'], ['e4', 'before', 'e5']]], 'text_quotes': ['patient sleeping in naps p med for pain', 'patient sleeping in naps p med for pain', 'husband at bedside all day', 'appetite fair', 'pos bs no stool'], 'event_name_prompt': 'Given the text: 39 yr old c cardiomyopathy\n\nst c pvcs. 3 mg captopril given p weaning milrinone to .200 .hemodynamics unchanged .ci 2.6/svr 1185.w 13 .cvp 11.bp transiently to 80 but patient asymptomatic .map &gt;60.to be started on coreg .\n\nsats 93 to 98,bs diminished .coughing continuously,med pro re nata c some relief.sputum had some blood in it .\n\nappetite fair.pos bs no stool.\n\nhuo responding to fluid 250 cc x1,then 100cc.heart rate for 1 liter.\n\npatient sleeping in naps p med for pain.husband at bedside all day .\n\nt to 100.9,tylenol given .ppd planted .\n\nmonitor fluid status\ntitrate meds as tol\nsupportive care\n, \n                        and the following event types with their definitions: Eating : The patient takes food into their body by mouth.\nExcretion : The patient discharges waste matter from their body.\nFamily : The patient has a visit, call, or communication with a family member.\nPain : The patient reports or shows signs of pain.\nSleep : The patient sleeps or the sleep’s quality or quantity is described.\nUnknown : choose "Unknown" if none of the other event type are applicable. \n                        ---\n                        Your task:\n                        0. Identify ALL events in the text (zero, one, or more).\n1. For each event, assign an event_type from the list above.\n2. If multiple event of same type is mentioned, assign the event_type multiple times\n3. Extract attributes for each event using ONLY the allowed attributes listed below.\n4. Use keyword evidence (Ki) ONLY if it is consistent with the text context.\n5. Output strictly valid JSON following the schema below.\n                        ---\n                        Classification Rules:\n                        - A text may contain multiple events of the same or different types.\n- Create a separate event object for each event mention.\n- If the text is explicitly a NEGATION (e.g., "denies pain"), do not extract that event.\n- If the text describes a FUTURE or HYPOTHETICAL event (e.g., "will eat tomorrow"), ignore it.\n- A valid event should have occurred in the recent past or is occurring during the time of writing of the text.\n- If no events are found or if unsure, return {"events": []}\n                        \n                        ---\n                                    Attributes allowed:\n                                    {\'Eating\': {\'food\': \'&lt;string&gt; # e.g., pancakes, porridge, etc.\', \'amount\': \'&lt;string&gt; # e.g., 1, 2 bowls, etc.\', \'method\': \'&lt;string&gt;  # e.g., oral, tube, etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, evening etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}, \'Excretion\': {\'type\': \'&lt;string&gt; # e.g., urine, stool, etc.\', \'frequency\': \'&lt;string&gt; # e.g., 2x, once, etc.\', \'quality\': \'&lt;string&gt; # e.g., loose, hard, etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, evening etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}, \'Family\': {\'interaction\': \'&lt;string&gt; # e.g., visit, call, communication, etc.\', \'relation\': \'&lt;string&gt; # e.g., mother, son, etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, evening etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}, \'Pain\': {\'severity\': \'&lt;string&gt; # e.g., mild, moderate, severe, numeric scale if present, etc.\', \'location\': \'&lt;string&gt; # e.g., right knee, head, etc.\', \'duration\': \'&lt;string&gt; # e.g., all night, 3 hours, etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, evening etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}, \'Sleep\': {\'quality\': \'&lt;string&gt; # e.g., good, poor, restless, etc.\', \'duration\': \'&lt;string&gt; # e.g., 6 hours, phrases like "all night", etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, evening etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}}\n                                    If no relevant attribute exists for an event, return an empty object {}.\n                                    \n                        \n                        ---\n                                    Keyword evidence (Ki):\n                                    Additional facts: A keyword matching algorithm without context detected keyword(s) (\'pain\', \'husband\', \'sleeping\', \'naps\').\n                                    Use this only as a pointer. If context contradicts, ignore.\n                        ---\n                        Output Schema (strict):\n                        {\n                                    "events": [\n                                        {\n                                        "event_id": "&lt; A unique id eg.: e1 | e2 |...&gt;"\n                                        "event_type": "&lt;Pain | Sleep | Excretion | Eating | Family&gt;",\n                                        "text_quote": "&lt;fragement from the text indicating the event_type&gt;",\n                "attributes": {\n                    "&lt;attribute_name&gt;": "&lt;attribute_value&gt;"\n                }\n                                        }\n                                    ],\n                                    "order": [\n                                        ["e1", "before" | "after" | "simultaneous", "e2" ]\n                                    ]\n                                    }\n                        \n                            Rules:\n                                - Ensure the output is valid JSON (parseable).\n                                - "eventS" must always be an array (can be empty).\n                                - Multiple instances of the same event type appear with different ids.\n                                - Events appear in the array in the same order in which they appear in the text.\n                                - Their partial orders can be expressed using the "order" section.\n                                - Do not include extra keys, comments, or text.\n                                - Each object in "events" must contain "event_type", "text_quote", and "attributes".\n                                - If an event attribute type has no value mentioned, return "attributes": {"&lt; attribute name &gt;:Unknown"} for each attribute type defined for the event type \n                        \n                        \n                        \n                        ', 'event_detection_time': 15.503746634989511}</t>
         </is>
       </c>
       <c r="L18" t="inlineStr">
         <is>
-          <t>['patient sleeping in naps p med for pain.', 'patient sleeping in naps p med for pain.', 'husband at bedside all day .', 'pos bs no stool.', 'appetite fair.']</t>
+          <t>['Pain', 'Sleep', 'Family', 'Eating', 'Excretion']</t>
         </is>
       </c>
       <c r="M18" t="inlineStr">
         <is>
-          <t>{'text': '39 yr old c cardiomyopathy\n\nst c pvcs. 3 mg captopril given p weaning milrinone to .200 .hemodynamics unchanged .ci 2.6/svr 1185.w 13 .cvp 11.bp transiently to 80 but patient asymptomatic .map &gt;60.to be started on coreg .\n\nsats 93 to 98,bs diminished .coughing continuously,med pro re nata c some relief.sputum had some blood in it .\n\nappetite fair.pos bs no stool.\n\nhuo responding to fluid 250 cc x1,then 100cc.heart rate for 1 liter.\n\npatient sleeping in naps p med for pain.husband at bedside all day .\n\nt to 100.9,tylenol given .ppd planted .\n\nmonitor fluid status\ntitrate meds as tol\nsupportive care\n', 'event': ['Eating', 'Excretion', 'Pain', 'Sleep', 'Family', 'Pain', 'Sleep'], 'phrase': '', 'raw_output': '{\n  "events": [\n    {\n      "event_type": "Eating",\n      "text_quote": "appetite fair",\n      "attributes": {\n        "food": "Unknown",\n        "amount": "Unknown",\n        "method": "Unknown",\n        "negation": "false",\n        "time": "Unknown",\n        "caused_by": "Unknown"\n      }\n    },\n    {\n      "event_type": "Excretion",\n      "text_quote": "pos bs no stool",\n      "attributes": {\n        "type": "stool",\n        "frequency": "none",\n        "quality": "Unknown",\n        "negation": "false",\n        "time": "Unknown",\n        "caused_by": "Unknown"\n      }\n    },\n    {\n      "event_type": "Pain",\n      "text_quote": "patient sleeping in naps p med for pain",\n      "attributes": {\n        "severity": "Unknown",\n        "location": "Unknown",\n        "duration": "Unknown",\n        "negation": "false",\n        "time": "after medication",\n        "caused_by": "medication"\n      }\n    },\n    {\n      "event_type": "Sleep",\n      "text_quote": "patient sleeping in naps p med for pain",\n      "attributes": {\n        "quality": "poor",\n        "duration": "naps",\n        "negation": "false",\n        "time": "after medication",\n        "caused_by": "medication"\n      }\n    },\n    {\n      "event_type": "Family",\n      "text_quote": "husband at bedside all day",\n      "attributes": {\n        "interaction": "visit",\n        "relation": "husband",\n        "negation": "false",\n        "time": "all day",\n        "caused_by": "Unknown"\n      }\n    },\n    {\n      "event_type": "Pain",\n      "text_quote": "coughing continuously,med pro re nata c some relief",\n      "attributes": {\n        "severity": "severe",\n        "location": "Unknown",\n        "duration": "continuous",\n        "negation": "false",\n        "time": "Unknown",\n        "caused_by": "Unknown"\n      }\n    },\n    {\n      "event_type": "Sleep",\n      "text_quote": "patient sleeping in naps p med for pain",\n      "attributes": {\n        "quality": "poor",\n        "duration": "naps",\n        "negation": "false",\n        "time": "after medication",\n        "caused_by": "medication"\n      }\n    }\n  ]\n}', 'attributes': [{'Eating': {'food': 'Unknown', 'amount': 'Unknown', 'method': 'Unknown', 'negation': 'false', 'time': 'Unknown', 'caused_by': 'Unknown'}}, {'Excretion': {'type': 'stool', 'frequency': 'none', 'quality': 'Unknown', 'negation': 'false', 'time': 'Unknown', 'caused_by': 'Unknown'}}, {'Pain': {'severity': 'Unknown', 'location': 'Unknown', 'duration': 'Unknown', 'negation': 'false', 'time': 'after medication', 'caused_by': 'medication'}}, {'Sleep': {'quality': 'poor', 'duration': 'naps', 'negation': 'false', 'time': 'after medication', 'caused_by': 'medication'}}, {'Family': {'interaction': 'visit', 'relation': 'husband', 'negation': 'false', 'time': 'all day', 'caused_by': 'Unknown'}}, {'Pain': {'severity': 'severe', 'location': 'Unknown', 'duration': 'continuous', 'negation': 'false', 'time': 'Unknown', 'caused_by': 'Unknown'}}, {'Sleep': {'quality': 'poor', 'duration': 'naps', 'negation': 'false', 'time': 'after medication', 'caused_by': 'medication'}}], 'text_quotes': ['appetite fair', 'pos bs no stool', 'patient sleeping in naps p med for pain', 'patient sleeping in naps p med for pain', 'husband at bedside all day', 'coughing continuously,med pro re nata c some relief', 'patient sleeping in naps p med for pain'], 'event_name_prompt': 'Given the text: 39 yr old c cardiomyopathy\n\nst c pvcs. 3 mg captopril given p weaning milrinone to .200 .hemodynamics unchanged .ci 2.6/svr 1185.w 13 .cvp 11.bp transiently to 80 but patient asymptomatic .map &gt;60.to be started on coreg .\n\nsats 93 to 98,bs diminished .coughing continuously,med pro re nata c some relief.sputum had some blood in it .\n\nappetite fair.pos bs no stool.\n\nhuo responding to fluid 250 cc x1,then 100cc.heart rate for 1 liter.\n\npatient sleeping in naps p med for pain.husband at bedside all day .\n\nt to 100.9,tylenol given .ppd planted .\n\nmonitor fluid status\ntitrate meds as tol\nsupportive care\n, \n                        and the following event types with their definitions: Eating : The patient takes food into their body by mouth.\nExcretion : The patient discharges waste matter from their body.\nFamily : The patient has a visit, call, or communication with a family member.\nPain : The patient reports or shows signs of pain.\nSleep : The patient sleeps or the sleep’s quality or quantity is described.\nUnknown : choose "Unknown" if none of the other event type are applicable. \n                        ---\n                        Your task:\n                        0. Identify ALL events in the text (zero, one, or more).\n1. For each event, assign an event_type from the list above.\n2. If multiple event of same type is mentioned, assign the event_type multiple times\n3. Extract attributes for each event using ONLY the allowed attributes listed below.\n4. Output strictly valid JSON following the schema below.\n                        ---\n                        Classification Rules:\n                        - A text may contain multiple events of the same or different types.\n- Create a separate event object for each event mention.\n- If the text is explicitly a NEGATION (e.g., "denies pain"), do not extract that event.\n- If the text describes a FUTURE or HYPOTHETICAL event (e.g., "will eat tomorrow"), ignore it.\n- A valid event should have occurred in the recent past or is occurring during the time of writing of the text.\n- If no events are found or if unsure, return {"events": []}\n                        \n                        ---\n                                    Attributes allowed:\n                                    {\'Eating\': {\'food\': \'&lt;string&gt; # e.g., pancakes, porridge, etc.\', \'amount\': \'&lt;string&gt; # e.g., 1, 2 bowls, etc.\', \'method\': \'&lt;string&gt;  # e.g., oral, tube, etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, after shower, etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}, \'Excretion\': {\'type\': \'&lt;string&gt; # e.g., urine, stool, etc.\', \'frequency\': \'&lt;string&gt; # e.g., 2x, once, etc.\', \'quality\': \'&lt;string&gt; # e.g., loose, hard, etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, after shower, etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}, \'Family\': {\'interaction\': \'&lt;string&gt; # e.g., visit, call, communication, etc.\', \'relation\': \'&lt;string&gt; # e.g., mother, son, etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, after shower, etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}, \'Pain\': {\'severity\': \'&lt;string&gt; # e.g., mild, moderate, severe, numeric scale if present, etc.\', \'location\': \'&lt;string&gt; # e.g., right knee, head, etc.\', \'duration\': \'&lt;string&gt; # e.g., all night, 3 hours, etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, after shower, etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}, \'Sleep\': {\'quality\': \'&lt;string&gt; # e.g., good, poor, restless, etc.\', \'duration\': \'&lt;string&gt; # e.g., 6 hours, phrases like "all night", etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, after shower, etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}}\n                                    If no relevant attribute exists for an event, return an empty object {}.\n                                    \n                        \n                        \n                        ---\n                        Output Schema (strict):\n                        {\n                                    "events": [\n                                        {\n                                        "event_type": "&lt;Pain | Sleep | Excretion | Eating | Family&gt;",\n                                        "text_quote": "&lt;fragement from the text indicating &gt;",\n                "attributes": {\n                    "&lt;attribute_name&gt;": "&lt;attribute_value&gt;"\n                }\n                                        }\n                                    ]\n                                    }\n                        \n                            Rules:\n                                - Ensure the output is valid JSON (parseable).\n                                - "eventS" must always be an array (can be empty).\n                                - Multiple instances of the same event type appear as individual elements in the event array.\n                                - Events appear in the array in the same order in which they appear in the text.\n                                - Do not include extra keys, comments, or text.\n                                - Each object in "events" must contain "event_type", "text_quote", and "attributes".\n                                -If an event attribute type has no value mentioned, return "attributes": {"&lt; attribute name &gt;:Unknown"} for each attribute type defined for the event type \n                        \n                        \n                        \n                ---\n                Examples:\n                \n                text: "Patient ate breakfast this morning. He seems less anxious."\n                output: {\n                "events": [\n                    {\n                    "event_type": "Eating",\n                    "text_quote":"Patient ate breakfast this morning",\n                    "attributes": {"food": "breakfast", \n                                   "amount": "Unknown",\n                                   "method": "Unknown",\n                                   "time":"morning",\n                                   "caused_by":"Unknown"}\n                    }\n                ]\n                }\n                \n                text: "Patient reported severe abdominal pain."\n                output: {\n                "events": [\n                    {\n                    "event_type": "Pain",\n                    "text_quote": "severe abdominal Pain",\n                    "attributes": {"severity": "severe", \n                                   "location": "abdominal",\n                                   "duration": "Unknown",\n                                   "time":"Unknown",\n                                   "caused_by":"Unknown"}\n                    }\n                ]\n                }\n                \n                text: "Patient called his son around 3 pm."\n                output: {\n                "events": [\n                    {\n                    "event_type": "Family",\n                    "text_quote": "called his son around 3 pm",\n                    "attributes": {"interaction": "call", \n                                    "relation": "son",\n                                    "time":"3 pm",\n                                    "caused_by":"Unknown"}\n                    }\n                ]\n                }\n                \n                text: "Patient had a loose stool overnight."\n                output: {\n                "events": [\n                    {\n                    "event_type": "Excretion",\n                    "text_quote": "loose stool overnight",\n                    "attributes": {"type": "stool", \n                                   "quality": "loose", \n                                   "frequency":"overnight", \n                                   "time":"night",\n                                   "caused_by":"Unknown"}\n                    }\n                ]\n                }\n                \n                text: "Patient was able to sleep well last night."\n                output: {\n                "events": [\n                    {\n                    "event_type": "Sleep",\n                    "text_quote": "sleep well last night",\n                    "attributes": {"quality": "well",\n                                    "duration": "Unknown", \n                                    "time":"night",\n                                    "caused_by":"Unknown"}\n                    }\n                ]\n                }\n                \n                text: "The patient couldn\'t sleep due to severe pain."\n                output: {\n                "events": [\n                    {\n                    "event_type": "Sleep",\n                    "text_quote": "couldn\'t sleep",\n                    "attributes": {"quality": "poor", \n                                    "duration": "Unknown",\n                                   "time":"Unknown",\n                                   "caused_by":"Pain"}\n                    },\n                    {\n                    "event_type": "Pain",\n                    "text_quote": "severe pain",\n                    "attributes": {"severity": "severe", \n                                    "location": "Unknown", \n                                    "duration": "Unknown", \n                                   "time":"before Sleep",\n                                   "caused_by":"Unknown"}\n                    }\n                ]\n                }\n                \n                text: "The patient complained of severe back pain, was given Tylenol, but the pain persisted and he was then prescribed stronger morphine."\n                output: {\n                "events": [\n                    {\n                    "event_type": "Pain",\n                    "text_quote": "complained of severe back pain",\n                    "attributes": {"severity": "severe", \n                                    "location": "back",\n                                    "duration": "Unknown", \n                                    "time":"Unknown",\n                                    "caused_by":"Unknown"}\n                    },\n                    {\n                    "event_type": "Pain",\n                    "text_quote": "pain persisted",\n                    "attributes": {"severity": "severe", \n                                   "location": "back",\n                                   "duration": "persistent", \n                                   "time":"after Tylenol",\n                                   "caused_by":"Unknown"}\n                    }\n                ]\n                }\n                \n                        ', 'event_detection_time': 18.58683973699226}</t>
+          <t>[{'Pain': {'severity': 'Unknown', 'location': 'Unknown', 'duration': 'Unknown', 'negation': False, 'time': 'Unknown', 'caused_by': 'medication'}}, {'Sleep': {'quality': 'Unknown', 'duration': 'naps', 'negation': False, 'time': 'Unknown', 'caused_by': 'medication'}}, {'Family': {'interaction': 'visit', 'relation': 'husband', 'negation': False, 'time': 'all day', 'caused_by': 'Unknown'}}, {'Eating': {'food': 'Unknown', 'amount': 'Unknown', 'method': 'Unknown', 'negation': False, 'time': 'Unknown', 'caused_by': 'Unknown'}}, {'Excretion': {'type': 'stool', 'frequency': 'no', 'quality': 'Unknown', 'negation': False, 'time': 'Unknown', 'caused_by': 'Unknown'}}]</t>
         </is>
       </c>
       <c r="N18" t="inlineStr">
         <is>
-          <t>['Eating', 'Excretion', 'Pain', 'Sleep', 'Family', 'Pain', 'Sleep']</t>
+          <t>['patient sleeping in naps p med for pain', 'patient sleeping in naps p med for pain', 'husband at bedside all day', 'appetite fair', 'pos bs no stool']</t>
         </is>
       </c>
       <c r="O18" t="inlineStr">
         <is>
-          <t>[{'Eating': {'food': 'Unknown', 'amount': 'Unknown', 'method': 'Unknown', 'negation': 'false', 'time': 'Unknown', 'caused_by': 'Unknown'}}, {'Excretion': {'type': 'stool', 'frequency': 'none', 'quality': 'Unknown', 'negation': 'false', 'time': 'Unknown', 'caused_by': 'Unknown'}}, {'Pain': {'severity': 'Unknown', 'location': 'Unknown', 'duration': 'Unknown', 'negation': 'false', 'time': 'after medication', 'caused_by': 'medication'}}, {'Sleep': {'quality': 'poor', 'duration': 'naps', 'negation': 'false', 'time': 'after medication', 'caused_by': 'medication'}}, {'Family': {'interaction': 'visit', 'relation': 'husband', 'negation': 'false', 'time': 'all day', 'caused_by': 'Unknown'}}, {'Pain': {'severity': 'severe', 'location': 'Unknown', 'duration': 'continuous', 'negation': 'false', 'time': 'Unknown', 'caused_by': 'Unknown'}}, {'Sleep': {'quality': 'poor', 'duration': 'naps', 'negation': 'false', 'time': 'after medication', 'caused_by': 'medication'}}]</t>
-        </is>
-      </c>
-      <c r="P18" t="inlineStr">
-        <is>
-          <t>['appetite fair', 'pos bs no stool', 'patient sleeping in naps p med for pain', 'patient sleeping in naps p med for pain', 'husband at bedside all day', 'coughing continuously,med pro re nata c some relief', 'patient sleeping in naps p med for pain']</t>
-        </is>
-      </c>
-      <c r="Q18" t="n">
-        <v>0.003061003000766505</v>
-      </c>
-      <c r="R18" t="inlineStr">
+          <t>[[['e1', 'simultaneous', 'e2'], ['e3', 'after', 'e1'], ['e4', 'before', 'e5']]]</t>
+        </is>
+      </c>
+      <c r="P18" t="n">
+        <v>0.002399173001322197</v>
+      </c>
+      <c r="Q18" t="inlineStr">
         <is>
           <t>Sleep</t>
         </is>
       </c>
-      <c r="S18" t="b">
-        <v>0</v>
+      <c r="R18" t="b">
+        <v>0</v>
+      </c>
+      <c r="S18" t="n">
+        <v>1</v>
       </c>
       <c r="T18" t="n">
         <v>1</v>
       </c>
-      <c r="U18" t="n">
-        <v>1</v>
-      </c>
-      <c r="V18" t="inlineStr">
+      <c r="U18" t="inlineStr">
         <is>
           <t>('pain', 'husband', 'nap', 'sleeping')</t>
         </is>
       </c>
+      <c r="V18" t="n">
+        <v>15.61993589100894</v>
+      </c>
       <c r="W18" t="n">
-        <v>18.57399767301104</v>
+        <v>15.50374663498951</v>
       </c>
       <c r="X18" t="n">
-        <v>12.76801657299802</v>
+        <v>1</v>
       </c>
       <c r="Y18" t="n">
-        <v>18.58683973699226</v>
+        <v>1</v>
       </c>
       <c r="Z18" t="n">
-        <v>1</v>
-      </c>
-      <c r="AA18" t="n">
-        <v>1</v>
-      </c>
-      <c r="AB18" t="n">
-        <v>1</v>
-      </c>
-      <c r="AC18" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="19">
-      <c r="A19" t="n">
-        <v>1325553</v>
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>1325553</t>
+        </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>['Family', 'Unknown']</t>
+          <t>('Family', 'Unknown')</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>['family', 'daughter']</t>
+          <t>('family', 'daughter')</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
@@ -2897,105 +2735,94 @@
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>{'text': 'nursing progress note 1900-0700\ns: "i feel pretty good right now"\n\no: please see flowsheet for complete objective data.\n\ncv: heart rate 90-110\'s, nsr/st, freq pvc\'s. had a few runs of asymptomatic vt ~6-8 beats long. diastolic blood pressure 80-110\'s, captopril and and coreg given last pm. cvp 7-10, pad\'s 19-20\'s. fellow pulled pa line back 1cm. co/ci/svr-5.4/2.54/963. milrinone remains @ 0.2mcg/kg/min.\n\nresp: productive cough, yellow/clr blood tinged sputum. sats 92-100 on 2lnc. ocassionally takes o2 off and maintains sats. lungs clr c dim bases.\n\ngi/gu: fair appetite, bs present, no bm. foley draining cyu. ivf d/c\'d and ~even for day, +1.1l for los.\n\naccess/id: rij pa line, l radial aline, 2 piv\'s. febrile to 101.0 @ [**2155**], gave tylenol 650mg with effect. tcurrent 99.8. to be started on ceftriaxone this am.\n\nneuro/social: a&amp;o x 3, pleasant and coopreative. became anxious and rec\'d ativan 0.5mg iv x 2 throughout the night. good effect. daughter stayed the night in the room.\n\np: cont to monitor hemodynamics and uo. follow up c labs. emotionally support patient and family. keep updated on plans.\n', 'event': ['Family', 'Sleep'], 'phrase': '', 'raw_output': '{\n  "events": [\n    {\n      "event_type": "Family",\n      "text_quote": "daughter stayed the night in the room.",\n      "attributes": {"interaction": "visit", \n                     "relation": "daughter",\n                     "time":"night",\n                     "caused_by":"Unknown"}\n    },\n    {\n      "event_type": "Sleep",\n      "text_quote": "daughter stayed the night in the room.",\n      "attributes": {"quality": "Unknown", \n                     "duration": "all night", \n                     "time":"night",\n                     "caused_by":"Unknown"}\n    }\n  ]\n}', 'attributes': [{'Family': {'interaction': 'visit', 'relation': 'daughter', 'time': 'night', 'caused_by': 'Unknown'}}, {'Sleep': {'quality': 'Unknown', 'duration': 'all night', 'time': 'night', 'caused_by': 'Unknown'}}], 'text_quotes': ['daughter stayed the night in the room.', 'daughter stayed the night in the room.'], 'event_name_prompt': 'Given the text: nursing progress note 1900-0700\ns: "i feel pretty good right now"\n\no: please see flowsheet for complete objective data.\n\ncv: heart rate 90-110\'s, nsr/st, freq pvc\'s. had a few runs of asymptomatic vt ~6-8 beats long. diastolic blood pressure 80-110\'s, captopril and and coreg given last pm. cvp 7-10, pad\'s 19-20\'s. fellow pulled pa line back 1cm. co/ci/svr-5.4/2.54/963. milrinone remains @ 0.2mcg/kg/min.\n\nresp: productive cough, yellow/clr blood tinged sputum. sats 92-100 on 2lnc. ocassionally takes o2 off and maintains sats. lungs clr c dim bases.\n\ngi/gu: fair appetite, bs present, no bm. foley draining cyu. ivf d/c\'d and ~even for day, +1.1l for los.\n\naccess/id: rij pa line, l radial aline, 2 piv\'s. febrile to 101.0 @ [**2155**], gave tylenol 650mg with effect. tcurrent 99.8. to be started on ceftriaxone this am.\n\nneuro/social: a&amp;o x 3, pleasant and coopreative. became anxious and rec\'d ativan 0.5mg iv x 2 throughout the night. good effect. daughter stayed the night in the room.\n\np: cont to monitor hemodynamics and uo. follow up c labs. emotionally support patient and family. keep updated on plans.\n, \n                        and the following event types with their definitions: Eating : The patient takes food into their body by mouth.\nExcretion : The patient discharges waste matter from their body.\nFamily : The patient has a visit, call, or communication with a family member.\nPain : The patient reports or shows signs of pain.\nSleep : The patient sleeps or the sleep’s quality or quantity is described.\nUnknown : choose "Unknown" if none of the other event type are applicable. \n                        ---\n                        Your task:\n                        0. Identify ALL events in the text (zero, one, or more).\n1. For each event, assign an event_type from the list above.\n2. If multiple event of same type is mentioned, assign the event_type multiple times\n3. Extract attributes for each event using ONLY the allowed attributes listed below.\n4. Use keyword evidence (Ki) ONLY if it is consistent with the text context.\n5. Output strictly valid JSON following the schema below.\n                        ---\n                        Classification Rules:\n                        - A text may contain multiple events of the same or different types.\n- Create a separate event object for each event mention.\n- If the text is explicitly a NEGATION (e.g., "denies pain"), do not extract that event.\n- If the text describes a FUTURE or HYPOTHETICAL event (e.g., "will eat tomorrow"), ignore it.\n- A valid event should have occurred in the recent past or is occurring during the time of writing of the text.\n- If no events are found or if unsure, return {"events": []}\n                        \n                        ---\n                                    Attributes allowed:\n                                    {\'Eating\': {\'food\': \'&lt;string&gt; # e.g., pancakes, porridge, etc.\', \'amount\': \'&lt;string&gt; # e.g., 1, 2 bowls, etc.\', \'method\': \'&lt;string&gt;  # e.g., oral, tube, etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, after shower, etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}, \'Excretion\': {\'type\': \'&lt;string&gt; # e.g., urine, stool, etc.\', \'frequency\': \'&lt;string&gt; # e.g., 2x, once, etc.\', \'quality\': \'&lt;string&gt; # e.g., loose, hard, etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, after shower, etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}, \'Family\': {\'interaction\': \'&lt;string&gt; # e.g., visit, call, communication, etc.\', \'relation\': \'&lt;string&gt; # e.g., mother, son, etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, after shower, etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}, \'Pain\': {\'severity\': \'&lt;string&gt; # e.g., mild, moderate, severe, numeric scale if present, etc.\', \'location\': \'&lt;string&gt; # e.g., right knee, head, etc.\', \'duration\': \'&lt;string&gt; # e.g., all night, 3 hours, etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, after shower, etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}, \'Sleep\': {\'quality\': \'&lt;string&gt; # e.g., good, poor, restless, etc.\', \'duration\': \'&lt;string&gt; # e.g., 6 hours, phrases like "all night", etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, after shower, etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}}\n                                    If no relevant attribute exists for an event, return an empty object {}.\n                                    \n                        \n                        ---\n                                    Keyword evidence (Ki):\n                                    Additional facts: A keyword matching algorithm without context detected keyword(s) [\'family\', \'daughter\'].\n                                    Use this only as a pointer. If context contradicts, ignore.\n                        ---\n                        Output Schema (strict):\n                        {\n                                    "events": [\n                                        {\n                                        "event_type": "&lt;Pain | Sleep | Excretion | Eating | Family&gt;",\n                                        "text_quote": "&lt;fragement from the text indicating &gt;",\n                "attributes": {\n                    "&lt;attribute_name&gt;": "&lt;attribute_value&gt;"\n                }\n                                        }\n                                    ]\n                                    }\n                        \n                            Rules:\n                                - Ensure the output is valid JSON (parseable).\n                                - "eventS" must always be an array (can be empty).\n                                - Multiple instances of the same event type appear as individual elements in the event array.\n                                - Events appear in the array in the same order in which they appear in the text.\n                                - Do not include extra keys, comments, or text.\n                                - Each object in "events" must contain "event_type", "text_quote", and "attributes".\n                                -If an event attribute type has no value mentioned, return "attributes": {"&lt; attribute name &gt;:Unknown"} for each attribute type defined for the event type \n                        \n                        \n                        \n                ---\n                Examples:\n                \n                text: "Patient ate breakfast this morning. He seems less anxious."\n                output: {\n                "events": [\n                    {\n                    "event_type": "Eating",\n                    "text_quote":"Patient ate breakfast this morning",\n                    "attributes": {"food": "breakfast", \n                                   "amount": "Unknown",\n                                   "method": "Unknown",\n                                   "time":"morning",\n                                   "caused_by":"Unknown"}\n                    }\n                ]\n                }\n                \n                text: "Patient reported severe abdominal pain."\n                output: {\n                "events": [\n                    {\n                    "event_type": "Pain",\n                    "text_quote": "severe abdominal Pain",\n                    "attributes": {"severity": "severe", \n                                   "location": "abdominal",\n                                   "duration": "Unknown",\n                                   "time":"Unknown",\n                                   "caused_by":"Unknown"}\n                    }\n                ]\n                }\n                \n                text: "Patient called his son around 3 pm."\n                output: {\n                "events": [\n                    {\n                    "event_type": "Family",\n                    "text_quote": "called his son around 3 pm",\n                    "attributes": {"interaction": "call", \n                                    "relation": "son",\n                                    "time":"3 pm",\n                                    "caused_by":"Unknown"}\n                    }\n                ]\n                }\n                \n                text: "Patient had a loose stool overnight."\n                output: {\n                "events": [\n                    {\n                    "event_type": "Excretion",\n                    "text_quote": "loose stool overnight",\n                    "attributes": {"type": "stool", \n                                   "quality": "loose", \n                                   "frequency":"overnight", \n                                   "time":"night",\n                                   "caused_by":"Unknown"}\n                    }\n                ]\n                }\n                \n                text: "Patient was able to sleep well last night."\n                output: {\n                "events": [\n                    {\n                    "event_type": "Sleep",\n                    "text_quote": "sleep well last night",\n                    "attributes": {"quality": "well",\n                                    "duration": "Unknown", \n                                    "time":"night",\n                                    "caused_by":"Unknown"}\n                    }\n                ]\n                }\n                \n                text: "The patient couldn\'t sleep due to severe pain."\n                output: {\n                "events": [\n                    {\n                    "event_type": "Sleep",\n                    "text_quote": "couldn\'t sleep",\n                    "attributes": {"quality": "poor", \n                                    "duration": "Unknown",\n                                   "time":"Unknown",\n                                   "caused_by":"Pain"}\n                    },\n                    {\n                    "event_type": "Pain",\n                    "text_quote": "severe pain",\n                    "attributes": {"severity": "severe", \n                                    "location": "Unknown", \n                                    "duration": "Unknown", \n                                   "time":"before Sleep",\n                                   "caused_by":"Unknown"}\n                    }\n                ]\n                }\n                \n                text: "The patient complained of severe back pain, was given Tylenol, but the pain persisted and he was then prescribed stronger morphine."\n                output: {\n                "events": [\n                    {\n                    "event_type": "Pain",\n                    "text_quote": "complained of severe back pain",\n                    "attributes": {"severity": "severe", \n                                    "location": "back",\n                                    "duration": "Unknown", \n                                    "time":"Unknown",\n                                    "caused_by":"Unknown"}\n                    },\n                    {\n                    "event_type": "Pain",\n                    "text_quote": "pain persisted",\n                    "attributes": {"severity": "severe", \n                                   "location": "back",\n                                   "duration": "persistent", \n                                   "time":"after Tylenol",\n                                   "caused_by":"Unknown"}\n                    }\n                ]\n                }\n                \n                        ', 'event_detection_time': 6.157393226996646}</t>
+          <t>['family', 'daughter']</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>['Family', 'Sleep']</t>
+          <t>{'text': 'nursing progress note 1900-0700\ns: "i feel pretty good right now"\n\no: please see flowsheet for complete objective data.\n\ncv: heart rate 90-110\'s, nsr/st, freq pvc\'s. had a few runs of asymptomatic vt ~6-8 beats long. diastolic blood pressure 80-110\'s, captopril and and coreg given last pm. cvp 7-10, pad\'s 19-20\'s. fellow pulled pa line back 1cm. co/ci/svr-5.4/2.54/963. milrinone remains @ 0.2mcg/kg/min.\n\nresp: productive cough, yellow/clr blood tinged sputum. sats 92-100 on 2lnc. ocassionally takes o2 off and maintains sats. lungs clr c dim bases.\n\ngi/gu: fair appetite, bs present, no bm. foley draining cyu. ivf d/c\'d and ~even for day, +1.1l for los.\n\naccess/id: rij pa line, l radial aline, 2 piv\'s. febrile to 101.0 @ [**2155**], gave tylenol 650mg with effect. tcurrent 99.8. to be started on ceftriaxone this am.\n\nneuro/social: a&amp;o x 3, pleasant and coopreative. became anxious and rec\'d ativan 0.5mg iv x 2 throughout the night. good effect. daughter stayed the night in the room.\n\np: cont to monitor hemodynamics and uo. follow up c labs. emotionally support patient and family. keep updated on plans.\n', 'event': ['Family', 'Sleep', 'Eating', 'Excretion', 'Excretion', 'Pain', 'Sleep'], 'event_id': ['e1', 'e2', 'e3', 'e4', 'e5', 'e6', 'e7'], 'phrase': '', 'raw_output': '{\n  "events": [\n    {\n      "event_id": "e1",\n      "event_type": "Family",\n      "text_quote": "daughter stayed the night in the room.",\n      "attributes": {\n        "interaction": "visit",\n        "relation": "daughter",\n        "negation": "false",\n        "time": "night",\n        "caused_by": "Unknown"\n      }\n    },\n    {\n      "event_id": "e2",\n      "event_type": "Sleep",\n      "text_quote": "daughter stayed the night in the room.",\n      "attributes": {\n        "quality": "Unknown",\n        "duration": "night",\n        "negation": "false",\n        "time": "night",\n        "caused_by": "Unknown"\n      }\n    },\n    {\n      "event_id": "e3",\n      "event_type": "Eating",\n      "text_quote": "fair appetite, bs present, no bm.",\n      "attributes": {\n        "food": "Unknown",\n        "amount": "Unknown",\n        "method": "Unknown",\n        "negation": "false",\n        "time": "Unknown",\n        "caused_by": "Unknown"\n      }\n    },\n    {\n      "event_id": "e4",\n      "event_type": "Excretion",\n      "text_quote": "no bm.",\n      "attributes": {\n        "type": "stool",\n        "frequency": "none",\n        "quality": "Unknown",\n        "negation": "true",\n        "time": "Unknown",\n        "caused_by": "Unknown"\n      }\n    },\n    {\n      "event_id": "e5",\n      "event_type": "Excretion",\n      "text_quote": "foley draining cyu.",\n      "attributes": {\n        "type": "urine",\n        "frequency": "Unknown",\n        "quality": "Unknown",\n        "negation": "false",\n        "time": "Unknown",\n        "caused_by": "Unknown"\n      }\n    },\n    {\n      "event_id": "e6",\n      "event_type": "Pain",\n      "text_quote": "became anxious and rec\'d ativan 0.5mg iv x 2 throughout the night.",\n      "attributes": {\n        "severity": "Unknown",\n        "location": "Unknown",\n        "duration": "night",\n        "negation": "false",\n        "time": "night",\n        "caused_by": "anxiety"\n      }\n    },\n    {\n      "event_id": "e7",\n      "event_type": "Sleep",\n      "text_quote": "became anxious and rec\'d ativan 0.5mg iv x 2 throughout the night.",\n      "attributes": {\n        "quality": "Unknown",\n        "duration": "night",\n        "negation": "false",\n        "time": "night",\n        "caused_by": "anxiety"\n      }\n    }\n  ],\n  "order": [\n    ["e1", "simultaneous", "e2"],\n    ["e3", "before", "e4"],\n    ["e5", "after", "e6"],\n    ["e6", "simultaneous", "e7"]\n  ]\n}', 'attributes': [{'Family': {'interaction': 'visit', 'relation': 'daughter', 'negation': 'false', 'time': 'night', 'caused_by': 'Unknown'}}, {'Sleep': {'quality': 'Unknown', 'duration': 'night', 'negation': 'false', 'time': 'night', 'caused_by': 'Unknown'}}, {'Eating': {'food': 'Unknown', 'amount': 'Unknown', 'method': 'Unknown', 'negation': 'false', 'time': 'Unknown', 'caused_by': 'Unknown'}}, {'Excretion': {'type': 'stool', 'frequency': 'none', 'quality': 'Unknown', 'negation': 'true', 'time': 'Unknown', 'caused_by': 'Unknown'}}, {'Excretion': {'type': 'urine', 'frequency': 'Unknown', 'quality': 'Unknown', 'negation': 'false', 'time': 'Unknown', 'caused_by': 'Unknown'}}, {'Pain': {'severity': 'Unknown', 'location': 'Unknown', 'duration': 'night', 'negation': 'false', 'time': 'night', 'caused_by': 'anxiety'}}, {'Sleep': {'quality': 'Unknown', 'duration': 'night', 'negation': 'false', 'time': 'night', 'caused_by': 'anxiety'}}], 'orders': [[['e1', 'simultaneous', 'e2'], ['e3', 'before', 'e4'], ['e5', 'after', 'e6'], ['e6', 'simultaneous', 'e7']]], 'text_quotes': ['daughter stayed the night in the room.', 'daughter stayed the night in the room.', 'fair appetite, bs present, no bm.', 'no bm.', 'foley draining cyu.', "became anxious and rec'd ativan 0.5mg iv x 2 throughout the night.", "became anxious and rec'd ativan 0.5mg iv x 2 throughout the night."], 'event_name_prompt': 'Given the text: nursing progress note 1900-0700\ns: "i feel pretty good right now"\n\no: please see flowsheet for complete objective data.\n\ncv: heart rate 90-110\'s, nsr/st, freq pvc\'s. had a few runs of asymptomatic vt ~6-8 beats long. diastolic blood pressure 80-110\'s, captopril and and coreg given last pm. cvp 7-10, pad\'s 19-20\'s. fellow pulled pa line back 1cm. co/ci/svr-5.4/2.54/963. milrinone remains @ 0.2mcg/kg/min.\n\nresp: productive cough, yellow/clr blood tinged sputum. sats 92-100 on 2lnc. ocassionally takes o2 off and maintains sats. lungs clr c dim bases.\n\ngi/gu: fair appetite, bs present, no bm. foley draining cyu. ivf d/c\'d and ~even for day, +1.1l for los.\n\naccess/id: rij pa line, l radial aline, 2 piv\'s. febrile to 101.0 @ [**2155**], gave tylenol 650mg with effect. tcurrent 99.8. to be started on ceftriaxone this am.\n\nneuro/social: a&amp;o x 3, pleasant and coopreative. became anxious and rec\'d ativan 0.5mg iv x 2 throughout the night. good effect. daughter stayed the night in the room.\n\np: cont to monitor hemodynamics and uo. follow up c labs. emotionally support patient and family. keep updated on plans.\n, \n                        and the following event types with their definitions: Eating : The patient takes food into their body by mouth.\nExcretion : The patient discharges waste matter from their body.\nFamily : The patient has a visit, call, or communication with a family member.\nPain : The patient reports or shows signs of pain.\nSleep : The patient sleeps or the sleep’s quality or quantity is described.\nUnknown : choose "Unknown" if none of the other event type are applicable. \n                        ---\n                        Your task:\n                        0. Identify ALL events in the text (zero, one, or more).\n1. For each event, assign an event_type from the list above.\n2. If multiple event of same type is mentioned, assign the event_type multiple times\n3. Extract attributes for each event using ONLY the allowed attributes listed below.\n4. Use keyword evidence (Ki) ONLY if it is consistent with the text context.\n5. Output strictly valid JSON following the schema below.\n                        ---\n                        Classification Rules:\n                        - A text may contain multiple events of the same or different types.\n- Create a separate event object for each event mention.\n- If the text is explicitly a NEGATION (e.g., "denies pain"), do not extract that event.\n- If the text describes a FUTURE or HYPOTHETICAL event (e.g., "will eat tomorrow"), ignore it.\n- A valid event should have occurred in the recent past or is occurring during the time of writing of the text.\n- If no events are found or if unsure, return {"events": []}\n                        \n                        ---\n                                    Attributes allowed:\n                                    {\'Eating\': {\'food\': \'&lt;string&gt; # e.g., pancakes, porridge, etc.\', \'amount\': \'&lt;string&gt; # e.g., 1, 2 bowls, etc.\', \'method\': \'&lt;string&gt;  # e.g., oral, tube, etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, evening etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}, \'Excretion\': {\'type\': \'&lt;string&gt; # e.g., urine, stool, etc.\', \'frequency\': \'&lt;string&gt; # e.g., 2x, once, etc.\', \'quality\': \'&lt;string&gt; # e.g., loose, hard, etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, evening etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}, \'Family\': {\'interaction\': \'&lt;string&gt; # e.g., visit, call, communication, etc.\', \'relation\': \'&lt;string&gt; # e.g., mother, son, etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, evening etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}, \'Pain\': {\'severity\': \'&lt;string&gt; # e.g., mild, moderate, severe, numeric scale if present, etc.\', \'location\': \'&lt;string&gt; # e.g., right knee, head, etc.\', \'duration\': \'&lt;string&gt; # e.g., all night, 3 hours, etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, evening etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}, \'Sleep\': {\'quality\': \'&lt;string&gt; # e.g., good, poor, restless, etc.\', \'duration\': \'&lt;string&gt; # e.g., 6 hours, phrases like "all night", etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, evening etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}}\n                                    If no relevant attribute exists for an event, return an empty object {}.\n                                    \n                        \n                        ---\n                                    Keyword evidence (Ki):\n                                    Additional facts: A keyword matching algorithm without context detected keyword(s) (\'family\', \'daughter\').\n                                    Use this only as a pointer. If context contradicts, ignore.\n                        ---\n                        Output Schema (strict):\n                        {\n                                    "events": [\n                                        {\n                                        "event_id": "&lt; A unique id eg.: e1 | e2 |...&gt;"\n                                        "event_type": "&lt;Pain | Sleep | Excretion | Eating | Family&gt;",\n                                        "text_quote": "&lt;fragement from the text indicating the event_type&gt;",\n                "attributes": {\n                    "&lt;attribute_name&gt;": "&lt;attribute_value&gt;"\n                }\n                                        }\n                                    ],\n                                    "order": [\n                                        ["e1", "before" | "after" | "simultaneous", "e2" ]\n                                    ]\n                                    }\n                        \n                            Rules:\n                                - Ensure the output is valid JSON (parseable).\n                                - "eventS" must always be an array (can be empty).\n                                - Multiple instances of the same event type appear with different ids.\n                                - Events appear in the array in the same order in which they appear in the text.\n                                - Their partial orders can be expressed using the "order" section.\n                                - Do not include extra keys, comments, or text.\n                                - Each object in "events" must contain "event_type", "text_quote", and "attributes".\n                                - If an event attribute type has no value mentioned, return "attributes": {"&lt; attribute name &gt;:Unknown"} for each attribute type defined for the event type \n                        \n                        \n                        \n                ---\n                Examples:\n                \n                text: "Patient ate breakfast this morning. He seems less anxious."\n                output: {\n                "events": [\n                    {"event_id": "e1",\n                    "event_type": "Eating",\n                    "text_quote":"Patient ate breakfast this morning",\n                    "attributes": {"food": "breakfast", \n                                   "amount": "Unknown",\n                                   "method": "Unknown",\n                                   "negation": "false",\n                                   "time":"morning",\n                                   "caused_by":"Unknown"}\n                    }\n                ],\n                "order":[]\n                }\n                \n                text: "Patient reported severe abdominal pain."\n                output: {\n                "events": [\n                    {"event_id": "e1",\n                    "event_type": "Pain",\n                    "text_quote": "severe abdominal Pain",\n                    "attributes": {"severity": "severe", \n                                   "location": "abdominal",\n                                   "duration": "Unknown",\n                                   "negation": "false",\n                                   "time":"Unknown",\n                                   "caused_by":"Unknown"}\n                    }\n                ],\n                "order":[]\n                }\n                \n                text: "Patient called his son around 3 pm."\n                output: {\n                "events": [\n                    {"event_id": "e1",\n                    "event_type": "Family",\n                    "text_quote": "called his son around 3 pm",\n                    "attributes": {"interaction": "call", \n                                    "relation": "son",\n                                    "negation": "false",\n                                    "time":"3 pm",\n                                    "caused_by":"Unknown"}\n                    }\n                ],\n                "order":[]\n                }\n                \n                text: "Patient had a loose stool overnight."\n                output: {\n                "events": [\n                    {"event_id": "e1",\n                    "event_type": "Excretion",\n                    "text_quote": "loose stool overnight",\n                    "attributes": {"type": "stool", \n                                   "quality": "loose", \n                                   "frequency":"overnight", \n                                   "negation": "false",\n                                   "time":"night",\n                                   "caused_by":"Unknown"}\n                    }\n                ],\n                "order":[]\n                }\n                \n                text: "Patient was able to sleep well last night."\n                output: {\n                "events": [\n                    {"event_id": "e1",\n                    "event_type": "Sleep",\n                    "text_quote": "sleep well last night",\n                    "attributes": {"quality": "well",\n                                    "duration": "Unknown", \n                                    "negation": "false",\n                                    "time":"night",\n                                    "caused_by":"Unknown"}\n                    }\n                ],\n                "order":[]\n                }\n                \n                text: "The patient couldn\'t sleep due to severe pain."\n                output: {\n                "events": [\n                    {"event_id": "e1",\n                    "event_type": "Sleep",\n                    "text_quote": "couldn\'t sleep",\n                    "attributes": {"quality": "poor", \n                                    "duration": "Unknown",\n                                    "negation": "true",\n                                    "time":"Unknown",\n                                    "caused_by":"Pain"}\n                    },\n                    {"event_id": "e2",\n                    "event_type": "Pain",\n                    "text_quote": "severe pain",\n                    "attributes": {"severity": "severe", \n                                    "location": "Unknown", \n                                    "duration": "Unknown", \n                                    "time":"Unknown",\n                                    "caused_by":"Unknown"}\n                    }\n                ],\n                "order":["e1", "after", "e2"]\n                }\n                \n                text: "The patient complained of severe back pain, was given Tylenol, but the pain persisted and he was then prescribed stronger morphine."\n                output: {\n                "events": [\n                    {"event_id": "e1",\n                    "event_type": "Pain",\n                    "text_quote": "complained of severe back pain",\n                    "attributes": {"severity": "severe", \n                                    "location": "back",\n                                    "duration": "Unknown", \n                                    "time":"Unknown",\n                                    "caused_by":"Unknown"}\n                    },\n                    {"event_id": "e2",\n                    "event_type": "Pain",\n                    "text_quote": "pain persisted",\n                    "attributes": {"severity": "severe", \n                                   "location": "back",\n                                   "duration": "persistent", \n                                   "time":"after Tylenol",\n                                   "caused_by":"Unknown"}\n                    }\n                ],\n                "order":[["e1", "before", "e2"]]\n                }\n                \n                        ', 'event_detection_time': 23.119513176032342}</t>
         </is>
       </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t>[{'Family': {'interaction': 'visit', 'relation': 'daughter', 'time': 'night', 'caused_by': 'Unknown'}}, {'Sleep': {'quality': 'Unknown', 'duration': 'all night', 'time': 'night', 'caused_by': 'Unknown'}}]</t>
+          <t>['Family', 'Sleep', 'Eating', 'Excretion', 'Excretion', 'Pain', 'Sleep']</t>
         </is>
       </c>
       <c r="H19" t="inlineStr">
         <is>
-          <t>['daughter stayed the night in the room.', 'daughter stayed the night in the room.']</t>
+          <t>[{'Family': {'interaction': 'visit', 'relation': 'daughter', 'negation': 'false', 'time': 'night', 'caused_by': 'Unknown'}}, {'Sleep': {'quality': 'Unknown', 'duration': 'night', 'negation': 'false', 'time': 'night', 'caused_by': 'Unknown'}}, {'Eating': {'food': 'Unknown', 'amount': 'Unknown', 'method': 'Unknown', 'negation': 'false', 'time': 'Unknown', 'caused_by': 'Unknown'}}, {'Excretion': {'type': 'stool', 'frequency': 'none', 'quality': 'Unknown', 'negation': 'true', 'time': 'Unknown', 'caused_by': 'Unknown'}}, {'Excretion': {'type': 'urine', 'frequency': 'Unknown', 'quality': 'Unknown', 'negation': 'false', 'time': 'Unknown', 'caused_by': 'Unknown'}}, {'Pain': {'severity': 'Unknown', 'location': 'Unknown', 'duration': 'night', 'negation': 'false', 'time': 'night', 'caused_by': 'anxiety'}}, {'Sleep': {'quality': 'Unknown', 'duration': 'night', 'negation': 'false', 'time': 'night', 'caused_by': 'anxiety'}}]</t>
         </is>
       </c>
       <c r="I19" t="inlineStr">
         <is>
-          <t>{'text': 'nursing progress note 1900-0700\ns: "i feel pretty good right now"\n\no: please see flowsheet for complete objective data.\n\ncv: heart rate 90-110\'s, nsr/st, freq pvc\'s. had a few runs of asymptomatic vt ~6-8 beats long. diastolic blood pressure 80-110\'s, captopril and and coreg given last pm. cvp 7-10, pad\'s 19-20\'s. fellow pulled pa line back 1cm. co/ci/svr-5.4/2.54/963. milrinone remains @ 0.2mcg/kg/min.\n\nresp: productive cough, yellow/clr blood tinged sputum. sats 92-100 on 2lnc. ocassionally takes o2 off and maintains sats. lungs clr c dim bases.\n\ngi/gu: fair appetite, bs present, no bm. foley draining cyu. ivf d/c\'d and ~even for day, +1.1l for los.\n\naccess/id: rij pa line, l radial aline, 2 piv\'s. febrile to 101.0 @ [**2155**], gave tylenol 650mg with effect. tcurrent 99.8. to be started on ceftriaxone this am.\n\nneuro/social: a&amp;o x 3, pleasant and coopreative. became anxious and rec\'d ativan 0.5mg iv x 2 throughout the night. good effect. daughter stayed the night in the room.\n\np: cont to monitor hemodynamics and uo. follow up c labs. emotionally support patient and family. keep updated on plans.\n', 'event': ['Family', 'Eating', 'Excretion', 'Excretion', 'Sleep'], 'phrase': '', 'raw_output': '{\n  "events": [\n    {\n      "event_type": "Family",\n      "text_quote": "daughter stayed the night in the room.",\n      "attributes": {\n        "interaction": "visit",\n        "relation": "daughter",\n        "negation": false,\n        "time": "night"\n      }\n    },\n    {\n      "event_type": "Eating",\n      "text_quote": "fair appetite, bs present, no bm.",\n      "attributes": {\n        "food": "Unknown",\n        "amount": "Unknown",\n        "method": "oral",\n        "negation": false,\n        "time": "Unknown"\n      }\n    },\n    {\n      "event_type": "Excretion",\n      "text_quote": "no bm.",\n      "attributes": {\n        "type": "stool",\n        "frequency": "none",\n        "quality": "Unknown",\n        "negation": false,\n        "time": "Unknown"\n      }\n    },\n    {\n      "event_type": "Excretion",\n      "text_quote": "foley draining cyu.",\n      "attributes": {\n        "type": "urine",\n        "frequency": "Unknown",\n        "quality": "Unknown",\n        "negation": false,\n        "time": "Unknown"\n      }\n    },\n    {\n      "event_type": "Sleep",\n      "text_quote": "daughter stayed the night in the room.",\n      "attributes": {\n        "quality": "Unknown",\n        "duration": "night",\n        "negation": false,\n        "time": "night"\n      }\n    }\n  ]\n}', 'attributes': [{'Family': {'interaction': 'visit', 'relation': 'daughter', 'negation': False, 'time': 'night'}}, {'Eating': {'food': 'Unknown', 'amount': 'Unknown', 'method': 'oral', 'negation': False, 'time': 'Unknown'}}, {'Excretion': {'type': 'stool', 'frequency': 'none', 'quality': 'Unknown', 'negation': False, 'time': 'Unknown'}}, {'Excretion': {'type': 'urine', 'frequency': 'Unknown', 'quality': 'Unknown', 'negation': False, 'time': 'Unknown'}}, {'Sleep': {'quality': 'Unknown', 'duration': 'night', 'negation': False, 'time': 'night'}}], 'text_quotes': ['daughter stayed the night in the room.', 'fair appetite, bs present, no bm.', 'no bm.', 'foley draining cyu.', 'daughter stayed the night in the room.'], 'event_name_prompt': 'Given the text: nursing progress note 1900-0700\ns: "i feel pretty good right now"\n\no: please see flowsheet for complete objective data.\n\ncv: heart rate 90-110\'s, nsr/st, freq pvc\'s. had a few runs of asymptomatic vt ~6-8 beats long. diastolic blood pressure 80-110\'s, captopril and and coreg given last pm. cvp 7-10, pad\'s 19-20\'s. fellow pulled pa line back 1cm. co/ci/svr-5.4/2.54/963. milrinone remains @ 0.2mcg/kg/min.\n\nresp: productive cough, yellow/clr blood tinged sputum. sats 92-100 on 2lnc. ocassionally takes o2 off and maintains sats. lungs clr c dim bases.\n\ngi/gu: fair appetite, bs present, no bm. foley draining cyu. ivf d/c\'d and ~even for day, +1.1l for los.\n\naccess/id: rij pa line, l radial aline, 2 piv\'s. febrile to 101.0 @ [**2155**], gave tylenol 650mg with effect. tcurrent 99.8. to be started on ceftriaxone this am.\n\nneuro/social: a&amp;o x 3, pleasant and coopreative. became anxious and rec\'d ativan 0.5mg iv x 2 throughout the night. good effect. daughter stayed the night in the room.\n\np: cont to monitor hemodynamics and uo. follow up c labs. emotionally support patient and family. keep updated on plans.\n, \n                        and the following event types with their definitions: Eating : The patient takes food into their body by mouth.\nExcretion : The patient discharges waste matter from their body.\nFamily : The patient has a visit, call, or communication with a family member.\nPain : The patient reports or shows signs of pain.\nSleep : The patient sleeps or the sleep’s quality or quantity is described.\nUnknown : choose "Unknown" if none of the other event type are applicable. \n                        ---\n                        Your task:\n                        0. Identify ALL events in the text (zero, one, or more).\n1. For each event, assign an event_type from the list above.\n2. If multiple event of same type is mentioned, assign the event_type multiple times\n3. Extract attributes for each event using ONLY the allowed attributes listed below.\n4. Use keyword evidence (Ki) ONLY if it is consistent with the text context.\n5. Output strictly valid JSON following the schema below.\n                        ---\n                        Classification Rules:\n                        - A text may contain multiple events of the same or different types.\n- Create a separate event object for each event mention.\n- If the text is explicitly a NEGATION (e.g., "denies pain"), do not extract that event.\n- If the text describes a FUTURE or HYPOTHETICAL event (e.g., "will eat tomorrow"), ignore it.\n- A valid event should have occurred in the recent past or is occurring during the time of writing of the text.\n- If no events are found or if unsure, return {"events": []}\n                        \n                        ---\n                                    Attributes allowed:\n                                    {\'Eating\': {\'food\': \'&lt;string&gt; # e.g., pancakes, porridge, etc.\', \'amount\': \'&lt;string&gt; # e.g., 1, 2 bowls, etc.\', \'method\': \'&lt;string&gt;  # e.g., oral, tube, etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, after shower, etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}, \'Excretion\': {\'type\': \'&lt;string&gt; # e.g., urine, stool, etc.\', \'frequency\': \'&lt;string&gt; # e.g., 2x, once, etc.\', \'quality\': \'&lt;string&gt; # e.g., loose, hard, etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, after shower, etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}, \'Family\': {\'interaction\': \'&lt;string&gt; # e.g., visit, call, communication, etc.\', \'relation\': \'&lt;string&gt; # e.g., mother, son, etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, after shower, etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}, \'Pain\': {\'severity\': \'&lt;string&gt; # e.g., mild, moderate, severe, numeric scale if present, etc.\', \'location\': \'&lt;string&gt; # e.g., right knee, head, etc.\', \'duration\': \'&lt;string&gt; # e.g., all night, 3 hours, etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, after shower, etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}, \'Sleep\': {\'quality\': \'&lt;string&gt; # e.g., good, poor, restless, etc.\', \'duration\': \'&lt;string&gt; # e.g., 6 hours, phrases like "all night", etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, after shower, etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}}\n                                    If no relevant attribute exists for an event, return an empty object {}.\n                                    \n                        \n                        ---\n                                    Keyword evidence (Ki):\n                                    Additional facts: A keyword matching algorithm without context detected keyword(s) [\'family\', \'daughter\'].\n                                    Use this only as a pointer. If context contradicts, ignore.\n                        ---\n                        Output Schema (strict):\n                        {\n                                    "events": [\n                                        {\n                                        "event_type": "&lt;Pain | Sleep | Excretion | Eating | Family&gt;",\n                                        "text_quote": "&lt;fragement from the text indicating &gt;",\n                "attributes": {\n                    "&lt;attribute_name&gt;": "&lt;attribute_value&gt;"\n                }\n                                        }\n                                    ]\n                                    }\n                        \n                            Rules:\n                                - Ensure the output is valid JSON (parseable).\n                                - "eventS" must always be an array (can be empty).\n                                - Multiple instances of the same event type appear as individual elements in the event array.\n                                - Events appear in the array in the same order in which they appear in the text.\n                                - Do not include extra keys, comments, or text.\n                                - Each object in "events" must contain "event_type", "text_quote", and "attributes".\n                                -If an event attribute type has no value mentioned, return "attributes": {"&lt; attribute name &gt;:Unknown"} for each attribute type defined for the event type \n                        \n                        \n                        \n                        ', 'event_detection_time': 11.43244439001137}</t>
+          <t>['daughter stayed the night in the room.', 'daughter stayed the night in the room.', 'fair appetite, bs present, no bm.', 'no bm.', 'foley draining cyu.', "became anxious and rec'd ativan 0.5mg iv x 2 throughout the night.", "became anxious and rec'd ativan 0.5mg iv x 2 throughout the night."]</t>
         </is>
       </c>
       <c r="J19" t="inlineStr">
         <is>
-          <t>['Family', 'Eating', 'Excretion', 'Excretion', 'Sleep']</t>
+          <t>[[['e1', 'simultaneous', 'e2'], ['e3', 'before', 'e4'], ['e5', 'after', 'e6'], ['e6', 'simultaneous', 'e7']]]</t>
         </is>
       </c>
       <c r="K19" t="inlineStr">
         <is>
-          <t>[{'Family': {'interaction': 'visit', 'relation': 'daughter', 'negation': False, 'time': 'night'}}, {'Eating': {'food': 'Unknown', 'amount': 'Unknown', 'method': 'oral', 'negation': False, 'time': 'Unknown'}}, {'Excretion': {'type': 'stool', 'frequency': 'none', 'quality': 'Unknown', 'negation': False, 'time': 'Unknown'}}, {'Excretion': {'type': 'urine', 'frequency': 'Unknown', 'quality': 'Unknown', 'negation': False, 'time': 'Unknown'}}, {'Sleep': {'quality': 'Unknown', 'duration': 'night', 'negation': False, 'time': 'night'}}]</t>
+          <t>{'text': 'nursing progress note 1900-0700\ns: "i feel pretty good right now"\n\no: please see flowsheet for complete objective data.\n\ncv: heart rate 90-110\'s, nsr/st, freq pvc\'s. had a few runs of asymptomatic vt ~6-8 beats long. diastolic blood pressure 80-110\'s, captopril and and coreg given last pm. cvp 7-10, pad\'s 19-20\'s. fellow pulled pa line back 1cm. co/ci/svr-5.4/2.54/963. milrinone remains @ 0.2mcg/kg/min.\n\nresp: productive cough, yellow/clr blood tinged sputum. sats 92-100 on 2lnc. ocassionally takes o2 off and maintains sats. lungs clr c dim bases.\n\ngi/gu: fair appetite, bs present, no bm. foley draining cyu. ivf d/c\'d and ~even for day, +1.1l for los.\n\naccess/id: rij pa line, l radial aline, 2 piv\'s. febrile to 101.0 @ [**2155**], gave tylenol 650mg with effect. tcurrent 99.8. to be started on ceftriaxone this am.\n\nneuro/social: a&amp;o x 3, pleasant and coopreative. became anxious and rec\'d ativan 0.5mg iv x 2 throughout the night. good effect. daughter stayed the night in the room.\n\np: cont to monitor hemodynamics and uo. follow up c labs. emotionally support patient and family. keep updated on plans.\n', 'event': ['Family', 'Excretion', 'Excretion', 'Eating', 'Sleep', 'Pain'], 'event_id': ['e1', 'e2', 'e3', 'e4', 'e5', 'e6'], 'phrase': '', 'raw_output': '{\n  "events": [\n    {\n      "event_id": "e1",\n      "event_type": "Family",\n      "text_quote": "daughter stayed the night in the room.",\n      "attributes": {\n        "interaction": "visit",\n        "relation": "daughter",\n        "negation": false,\n        "time": "night"\n      }\n    },\n    {\n      "event_id": "e2",\n      "event_type": "Excretion",\n      "text_quote": "foley draining cyu.",\n      "attributes": {\n        "type": "urine",\n        "frequency": "Unknown",\n        "quality": "Unknown",\n        "negation": false,\n        "time": "Unknown"\n      }\n    },\n    {\n      "event_id": "e3",\n      "event_type": "Excretion",\n      "text_quote": "bs present, no bm.",\n      "attributes": {\n        "type": "stool",\n        "frequency": "Unknown",\n        "quality": "Unknown",\n        "negation": false,\n        "time": "Unknown"\n      }\n    },\n    {\n      "event_id": "e4",\n      "event_type": "Eating",\n      "text_quote": "fair appetite",\n      "attributes": {\n        "food": "Unknown",\n        "amount": "Unknown",\n        "method": "oral",\n        "negation": false,\n        "time": "Unknown"\n      }\n    },\n    {\n      "event_id": "e5",\n      "event_type": "Sleep",\n      "text_quote": "daughter stayed the night in the room.",\n      "attributes": {\n        "quality": "Unknown",\n        "duration": "night",\n        "negation": false,\n        "time": "night"\n      }\n    },\n    {\n      "event_id": "e6",\n      "event_type": "Pain",\n      "text_quote": "became anxious and rec\'d ativan 0.5mg iv x 2 throughout the night.",\n      "attributes": {\n        "severity": "Unknown",\n        "location": "Unknown",\n        "duration": "night",\n        "negation": false,\n        "time": "night"\n      }\n    }\n  ],\n  "order": [\n    ["e1", "simultaneous", "e5"],\n    ["e2", "before", "e3"],\n    ["e4", "after", "e6"]\n  ]\n}', 'attributes': [{'Family': {'interaction': 'visit', 'relation': 'daughter', 'negation': False, 'time': 'night'}}, {'Excretion': {'type': 'urine', 'frequency': 'Unknown', 'quality': 'Unknown', 'negation': False, 'time': 'Unknown'}}, {'Excretion': {'type': 'stool', 'frequency': 'Unknown', 'quality': 'Unknown', 'negation': False, 'time': 'Unknown'}}, {'Eating': {'food': 'Unknown', 'amount': 'Unknown', 'method': 'oral', 'negation': False, 'time': 'Unknown'}}, {'Sleep': {'quality': 'Unknown', 'duration': 'night', 'negation': False, 'time': 'night'}}, {'Pain': {'severity': 'Unknown', 'location': 'Unknown', 'duration': 'night', 'negation': False, 'time': 'night'}}], 'orders': [[['e1', 'simultaneous', 'e5'], ['e2', 'before', 'e3'], ['e4', 'after', 'e6']]], 'text_quotes': ['daughter stayed the night in the room.', 'foley draining cyu.', 'bs present, no bm.', 'fair appetite', 'daughter stayed the night in the room.', "became anxious and rec'd ativan 0.5mg iv x 2 throughout the night."], 'event_name_prompt': 'Given the text: nursing progress note 1900-0700\ns: "i feel pretty good right now"\n\no: please see flowsheet for complete objective data.\n\ncv: heart rate 90-110\'s, nsr/st, freq pvc\'s. had a few runs of asymptomatic vt ~6-8 beats long. diastolic blood pressure 80-110\'s, captopril and and coreg given last pm. cvp 7-10, pad\'s 19-20\'s. fellow pulled pa line back 1cm. co/ci/svr-5.4/2.54/963. milrinone remains @ 0.2mcg/kg/min.\n\nresp: productive cough, yellow/clr blood tinged sputum. sats 92-100 on 2lnc. ocassionally takes o2 off and maintains sats. lungs clr c dim bases.\n\ngi/gu: fair appetite, bs present, no bm. foley draining cyu. ivf d/c\'d and ~even for day, +1.1l for los.\n\naccess/id: rij pa line, l radial aline, 2 piv\'s. febrile to 101.0 @ [**2155**], gave tylenol 650mg with effect. tcurrent 99.8. to be started on ceftriaxone this am.\n\nneuro/social: a&amp;o x 3, pleasant and coopreative. became anxious and rec\'d ativan 0.5mg iv x 2 throughout the night. good effect. daughter stayed the night in the room.\n\np: cont to monitor hemodynamics and uo. follow up c labs. emotionally support patient and family. keep updated on plans.\n, \n                        and the following event types with their definitions: Eating : The patient takes food into their body by mouth.\nExcretion : The patient discharges waste matter from their body.\nFamily : The patient has a visit, call, or communication with a family member.\nPain : The patient reports or shows signs of pain.\nSleep : The patient sleeps or the sleep’s quality or quantity is described.\nUnknown : choose "Unknown" if none of the other event type are applicable. \n                        ---\n                        Your task:\n                        0. Identify ALL events in the text (zero, one, or more).\n1. For each event, assign an event_type from the list above.\n2. If multiple event of same type is mentioned, assign the event_type multiple times\n3. Extract attributes for each event using ONLY the allowed attributes listed below.\n4. Use keyword evidence (Ki) ONLY if it is consistent with the text context.\n5. Output strictly valid JSON following the schema below.\n                        ---\n                        Classification Rules:\n                        - A text may contain multiple events of the same or different types.\n- Create a separate event object for each event mention.\n- If the text is explicitly a NEGATION (e.g., "denies pain"), do not extract that event.\n- If the text describes a FUTURE or HYPOTHETICAL event (e.g., "will eat tomorrow"), ignore it.\n- A valid event should have occurred in the recent past or is occurring during the time of writing of the text.\n- If no events are found or if unsure, return {"events": []}\n                        \n                        ---\n                                    Attributes allowed:\n                                    {\'Eating\': {\'food\': \'&lt;string&gt; # e.g., pancakes, porridge, etc.\', \'amount\': \'&lt;string&gt; # e.g., 1, 2 bowls, etc.\', \'method\': \'&lt;string&gt;  # e.g., oral, tube, etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, evening etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}, \'Excretion\': {\'type\': \'&lt;string&gt; # e.g., urine, stool, etc.\', \'frequency\': \'&lt;string&gt; # e.g., 2x, once, etc.\', \'quality\': \'&lt;string&gt; # e.g., loose, hard, etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, evening etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}, \'Family\': {\'interaction\': \'&lt;string&gt; # e.g., visit, call, communication, etc.\', \'relation\': \'&lt;string&gt; # e.g., mother, son, etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, evening etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}, \'Pain\': {\'severity\': \'&lt;string&gt; # e.g., mild, moderate, severe, numeric scale if present, etc.\', \'location\': \'&lt;string&gt; # e.g., right knee, head, etc.\', \'duration\': \'&lt;string&gt; # e.g., all night, 3 hours, etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, evening etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}, \'Sleep\': {\'quality\': \'&lt;string&gt; # e.g., good, poor, restless, etc.\', \'duration\': \'&lt;string&gt; # e.g., 6 hours, phrases like "all night", etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, evening etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}}\n                                    If no relevant attribute exists for an event, return an empty object {}.\n                                    \n                        \n                        ---\n                                    Keyword evidence (Ki):\n                                    Additional facts: A keyword matching algorithm without context detected keyword(s) (\'family\', \'daughter\').\n                                    Use this only as a pointer. If context contradicts, ignore.\n                        ---\n                        Output Schema (strict):\n                        {\n                                    "events": [\n                                        {\n                                        "event_id": "&lt; A unique id eg.: e1 | e2 |...&gt;"\n                                        "event_type": "&lt;Pain | Sleep | Excretion | Eating | Family&gt;",\n                                        "text_quote": "&lt;fragement from the text indicating the event_type&gt;",\n                "attributes": {\n                    "&lt;attribute_name&gt;": "&lt;attribute_value&gt;"\n                }\n                                        }\n                                    ],\n                                    "order": [\n                                        ["e1", "before" | "after" | "simultaneous", "e2" ]\n                                    ]\n                                    }\n                        \n                            Rules:\n                                - Ensure the output is valid JSON (parseable).\n                                - "eventS" must always be an array (can be empty).\n                                - Multiple instances of the same event type appear with different ids.\n                                - Events appear in the array in the same order in which they appear in the text.\n                                - Their partial orders can be expressed using the "order" section.\n                                - Do not include extra keys, comments, or text.\n                                - Each object in "events" must contain "event_type", "text_quote", and "attributes".\n                                - If an event attribute type has no value mentioned, return "attributes": {"&lt; attribute name &gt;:Unknown"} for each attribute type defined for the event type \n                        \n                        \n                        \n                        ', 'event_detection_time': 16.799395417969208}</t>
         </is>
       </c>
       <c r="L19" t="inlineStr">
         <is>
-          <t>['daughter stayed the night in the room.', 'fair appetite, bs present, no bm.', 'no bm.', 'foley draining cyu.', 'daughter stayed the night in the room.']</t>
+          <t>['Family', 'Excretion', 'Excretion', 'Eating', 'Sleep', 'Pain']</t>
         </is>
       </c>
       <c r="M19" t="inlineStr">
         <is>
-          <t>{'text': 'nursing progress note 1900-0700\ns: "i feel pretty good right now"\n\no: please see flowsheet for complete objective data.\n\ncv: heart rate 90-110\'s, nsr/st, freq pvc\'s. had a few runs of asymptomatic vt ~6-8 beats long. diastolic blood pressure 80-110\'s, captopril and and coreg given last pm. cvp 7-10, pad\'s 19-20\'s. fellow pulled pa line back 1cm. co/ci/svr-5.4/2.54/963. milrinone remains @ 0.2mcg/kg/min.\n\nresp: productive cough, yellow/clr blood tinged sputum. sats 92-100 on 2lnc. ocassionally takes o2 off and maintains sats. lungs clr c dim bases.\n\ngi/gu: fair appetite, bs present, no bm. foley draining cyu. ivf d/c\'d and ~even for day, +1.1l for los.\n\naccess/id: rij pa line, l radial aline, 2 piv\'s. febrile to 101.0 @ [**2155**], gave tylenol 650mg with effect. tcurrent 99.8. to be started on ceftriaxone this am.\n\nneuro/social: a&amp;o x 3, pleasant and coopreative. became anxious and rec\'d ativan 0.5mg iv x 2 throughout the night. good effect. daughter stayed the night in the room.\n\np: cont to monitor hemodynamics and uo. follow up c labs. emotionally support patient and family. keep updated on plans.\n', 'event': ['Eating', 'Excretion', 'Excretion', 'Family', 'Pain', 'Sleep', 'Pain', 'Sleep'], 'phrase': '', 'raw_output': '{\n  "events": [\n    {\n      "event_type": "Eating",\n      "text_quote": "fair appetite, bs present, no bm.",\n      "attributes": {\n        "food": "Unknown",\n        "amount": "Unknown",\n        "method": "Unknown",\n        "negation": "false",\n        "time": "Unknown",\n        "caused_by": "Unknown"\n      }\n    },\n    {\n      "event_type": "Excretion",\n      "text_quote": "no bm.",\n      "attributes": {\n        "type": "stool",\n        "frequency": "none",\n        "quality": "Unknown",\n        "negation": "false",\n        "time": "Unknown",\n        "caused_by": "Unknown"\n      }\n    },\n    {\n      "event_type": "Excretion",\n      "text_quote": "Foley draining cyu.",\n      "attributes": {\n        "type": "urine",\n        "frequency": "Unknown",\n        "quality": "Unknown",\n        "negation": "false",\n        "time": "Unknown",\n        "caused_by": "Unknown"\n      }\n    },\n    {\n      "event_type": "Family",\n      "text_quote": "daughter stayed the night in the room.",\n      "attributes": {\n        "interaction": "visit",\n        "relation": "daughter",\n        "negation": "false",\n        "time": "night",\n        "caused_by": "Unknown"\n      }\n    },\n    {\n      "event_type": "Pain",\n      "text_quote": "became anxious and rec\'d ativan 0.5mg iv x 2 throughout the night.",\n      "attributes": {\n        "severity": "Unknown",\n        "location": "Unknown",\n        "duration": "throughout the night",\n        "negation": "false",\n        "time": "night",\n        "caused_by": "Unknown"\n      }\n    },\n    {\n      "event_type": "Sleep",\n      "text_quote": "became anxious and rec\'d ativan 0.5mg iv x 2 throughout the night.",\n      "attributes": {\n        "quality": "poor",\n        "duration": "throughout the night",\n        "negation": "false",\n        "time": "night",\n        "caused_by": "anxiety"\n      }\n    },\n    {\n      "event_type": "Pain",\n      "text_quote": "febrile to 101.0 @ [**2155**], gave tylenol 650mg with effect.",\n      "attributes": {\n        "severity": "Unknown",\n        "location": "Unknown",\n        "duration": "Unknown",\n        "negation": "false",\n        "time": "[**2155**]",\n        "caused_by": "fever"\n      }\n    },\n    {\n      "event_type": "Sleep",\n      "text_quote": "daughter stayed the night in the room.",\n      "attributes": {\n        "quality": "Unknown",\n        "duration": "night",\n        "negation": "false",\n        "time": "night",\n        "caused_by": "Unknown"\n      }\n    }\n  ]\n}', 'attributes': [{'Eating': {'food': 'Unknown', 'amount': 'Unknown', 'method': 'Unknown', 'negation': 'false', 'time': 'Unknown', 'caused_by': 'Unknown'}}, {'Excretion': {'type': 'stool', 'frequency': 'none', 'quality': 'Unknown', 'negation': 'false', 'time': 'Unknown', 'caused_by': 'Unknown'}}, {'Excretion': {'type': 'urine', 'frequency': 'Unknown', 'quality': 'Unknown', 'negation': 'false', 'time': 'Unknown', 'caused_by': 'Unknown'}}, {'Family': {'interaction': 'visit', 'relation': 'daughter', 'negation': 'false', 'time': 'night', 'caused_by': 'Unknown'}}, {'Pain': {'severity': 'Unknown', 'location': 'Unknown', 'duration': 'throughout the night', 'negation': 'false', 'time': 'night', 'caused_by': 'Unknown'}}, {'Sleep': {'quality': 'poor', 'duration': 'throughout the night', 'negation': 'false', 'time': 'night', 'caused_by': 'anxiety'}}, {'Pain': {'severity': 'Unknown', 'location': 'Unknown', 'duration': 'Unknown', 'negation': 'false', 'time': '[**2155**]', 'caused_by': 'fever'}}, {'Sleep': {'quality': 'Unknown', 'duration': 'night', 'negation': 'false', 'time': 'night', 'caused_by': 'Unknown'}}], 'text_quotes': ['fair appetite, bs present, no bm.', 'no bm.', 'Foley draining cyu.', 'daughter stayed the night in the room.', "became anxious and rec'd ativan 0.5mg iv x 2 throughout the night.", "became anxious and rec'd ativan 0.5mg iv x 2 throughout the night.", 'febrile to 101.0 @ [**2155**], gave tylenol 650mg with effect.', 'daughter stayed the night in the room.'], 'event_name_prompt': 'Given the text: nursing progress note 1900-0700\ns: "i feel pretty good right now"\n\no: please see flowsheet for complete objective data.\n\ncv: heart rate 90-110\'s, nsr/st, freq pvc\'s. had a few runs of asymptomatic vt ~6-8 beats long. diastolic blood pressure 80-110\'s, captopril and and coreg given last pm. cvp 7-10, pad\'s 19-20\'s. fellow pulled pa line back 1cm. co/ci/svr-5.4/2.54/963. milrinone remains @ 0.2mcg/kg/min.\n\nresp: productive cough, yellow/clr blood tinged sputum. sats 92-100 on 2lnc. ocassionally takes o2 off and maintains sats. lungs clr c dim bases.\n\ngi/gu: fair appetite, bs present, no bm. foley draining cyu. ivf d/c\'d and ~even for day, +1.1l for los.\n\naccess/id: rij pa line, l radial aline, 2 piv\'s. febrile to 101.0 @ [**2155**], gave tylenol 650mg with effect. tcurrent 99.8. to be started on ceftriaxone this am.\n\nneuro/social: a&amp;o x 3, pleasant and coopreative. became anxious and rec\'d ativan 0.5mg iv x 2 throughout the night. good effect. daughter stayed the night in the room.\n\np: cont to monitor hemodynamics and uo. follow up c labs. emotionally support patient and family. keep updated on plans.\n, \n                        and the following event types with their definitions: Eating : The patient takes food into their body by mouth.\nExcretion : The patient discharges waste matter from their body.\nFamily : The patient has a visit, call, or communication with a family member.\nPain : The patient reports or shows signs of pain.\nSleep : The patient sleeps or the sleep’s quality or quantity is described.\nUnknown : choose "Unknown" if none of the other event type are applicable. \n                        ---\n                        Your task:\n                        0. Identify ALL events in the text (zero, one, or more).\n1. For each event, assign an event_type from the list above.\n2. If multiple event of same type is mentioned, assign the event_type multiple times\n3. Extract attributes for each event using ONLY the allowed attributes listed below.\n4. Output strictly valid JSON following the schema below.\n                        ---\n                        Classification Rules:\n                        - A text may contain multiple events of the same or different types.\n- Create a separate event object for each event mention.\n- If the text is explicitly a NEGATION (e.g., "denies pain"), do not extract that event.\n- If the text describes a FUTURE or HYPOTHETICAL event (e.g., "will eat tomorrow"), ignore it.\n- A valid event should have occurred in the recent past or is occurring during the time of writing of the text.\n- If no events are found or if unsure, return {"events": []}\n                        \n                        ---\n                                    Attributes allowed:\n                                    {\'Eating\': {\'food\': \'&lt;string&gt; # e.g., pancakes, porridge, etc.\', \'amount\': \'&lt;string&gt; # e.g., 1, 2 bowls, etc.\', \'method\': \'&lt;string&gt;  # e.g., oral, tube, etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, after shower, etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}, \'Excretion\': {\'type\': \'&lt;string&gt; # e.g., urine, stool, etc.\', \'frequency\': \'&lt;string&gt; # e.g., 2x, once, etc.\', \'quality\': \'&lt;string&gt; # e.g., loose, hard, etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, after shower, etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}, \'Family\': {\'interaction\': \'&lt;string&gt; # e.g., visit, call, communication, etc.\', \'relation\': \'&lt;string&gt; # e.g., mother, son, etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, after shower, etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}, \'Pain\': {\'severity\': \'&lt;string&gt; # e.g., mild, moderate, severe, numeric scale if present, etc.\', \'location\': \'&lt;string&gt; # e.g., right knee, head, etc.\', \'duration\': \'&lt;string&gt; # e.g., all night, 3 hours, etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, after shower, etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}, \'Sleep\': {\'quality\': \'&lt;string&gt; # e.g., good, poor, restless, etc.\', \'duration\': \'&lt;string&gt; # e.g., 6 hours, phrases like "all night", etc.\', \'negation\': \'&lt;boolean&gt; # true if the event is negated, false otherwise\', \'time\': \'&lt;string&gt; # e.g., 2 am, 5 pm, night, after shower, etc.\', \'caused_by\': \'&lt;string&gt; # e.g., medication, treatment, etc.\'}}\n                                    If no relevant attribute exists for an event, return an empty object {}.\n                                    \n                        \n                        \n                        ---\n                        Output Schema (strict):\n                        {\n                                    "events": [\n                                        {\n                                        "event_type": "&lt;Pain | Sleep | Excretion | Eating | Family&gt;",\n                                        "text_quote": "&lt;fragement from the text indicating &gt;",\n                "attributes": {\n                    "&lt;attribute_name&gt;": "&lt;attribute_value&gt;"\n                }\n                                        }\n                                    ]\n                                    }\n                        \n                            Rules:\n                                - Ensure the output is valid JSON (parseable).\n                                - "eventS" must always be an array (can be empty).\n                                - Multiple instances of the same event type appear as individual elements in the event array.\n                                - Events appear in the array in the same order in which they appear in the text.\n                                - Do not include extra keys, comments, or text.\n                                - Each object in "events" must contain "event_type", "text_quote", and "attributes".\n                                -If an event attribute type has no value mentioned, return "attributes": {"&lt; attribute name &gt;:Unknown"} for each attribute type defined for the event type \n                        \n                        \n                        \n                ---\n                Examples:\n                \n                text: "Patient ate breakfast this morning. He seems less anxious."\n                output: {\n                "events": [\n                    {\n                    "event_type": "Eating",\n                    "text_quote":"Patient ate breakfast this morning",\n                    "attributes": {"food": "breakfast", \n                                   "amount": "Unknown",\n                                   "method": "Unknown",\n                                   "time":"morning",\n                                   "caused_by":"Unknown"}\n                    }\n                ]\n                }\n                \n                text: "Patient reported severe abdominal pain."\n                output: {\n                "events": [\n                    {\n                    "event_type": "Pain",\n                    "text_quote": "severe abdominal Pain",\n                    "attributes": {"severity": "severe", \n                                   "location": "abdominal",\n                                   "duration": "Unknown",\n                                   "time":"Unknown",\n                                   "caused_by":"Unknown"}\n                    }\n                ]\n                }\n                \n                text: "Patient called his son around 3 pm."\n                output: {\n                "events": [\n                    {\n                    "event_type": "Family",\n                    "text_quote": "called his son around 3 pm",\n                    "attributes": {"interaction": "call", \n                                    "relation": "son",\n                                    "time":"3 pm",\n                                    "caused_by":"Unknown"}\n                    }\n                ]\n                }\n                \n                text: "Patient had a loose stool overnight."\n                output: {\n                "events": [\n                    {\n                    "event_type": "Excretion",\n                    "text_quote": "loose stool overnight",\n                    "attributes": {"type": "stool", \n                                   "quality": "loose", \n                                   "frequency":"overnight", \n                                   "time":"night",\n                                   "caused_by":"Unknown"}\n                    }\n                ]\n                }\n                \n                text: "Patient was able to sleep well last night."\n                output: {\n                "events": [\n                    {\n                    "event_type": "Sleep",\n                    "text_quote": "sleep well last night",\n                    "attributes": {"quality": "well",\n                                    "duration": "Unknown", \n                                    "time":"night",\n                                    "caused_by":"Unknown"}\n                    }\n                ]\n                }\n                \n                text: "The patient couldn\'t sleep due to severe pain."\n                output: {\n                "events": [\n                    {\n                    "event_type": "Sleep",\n                    "text_quote": "couldn\'t sleep",\n                    "attributes": {"quality": "poor", \n                                    "duration": "Unknown",\n                                   "time":"Unknown",\n                                   "caused_by":"Pain"}\n                    },\n                    {\n                    "event_type": "Pain",\n                    "text_quote": "severe pain",\n                    "attributes": {"severity": "severe", \n                                    "location": "Unknown", \n                                    "duration": "Unknown", \n                                   "time":"before Sleep",\n                                   "caused_by":"Unknown"}\n                    }\n                ]\n                }\n                \n                text: "The patient complained of severe back pain, was given Tylenol, but the pain persisted and he was then prescribed stronger morphine."\n                output: {\n                "events": [\n                    {\n                    "event_type": "Pain",\n                    "text_quote": "complained of severe back pain",\n                    "attributes": {"severity": "severe", \n                                    "location": "back",\n                                    "duration": "Unknown", \n                                    "time":"Unknown",\n                                    "caused_by":"Unknown"}\n                    },\n                    {\n                    "event_type": "Pain",\n                    "text_quote": "pain persisted",\n                    "attributes": {"severity": "severe", \n                                   "location": "back",\n                                   "duration": "persistent", \n                                   "time":"after Tylenol",\n                                   "caused_by":"Unknown"}\n                    }\n                ]\n                }\n                \n                        ', 'event_detection_time': 22.188900797002134}</t>
+          <t>[{'Family': {'interaction': 'visit', 'relation': 'daughter', 'negation': False, 'time': 'night'}}, {'Excretion': {'type': 'urine', 'frequency': 'Unknown', 'quality': 'Unknown', 'negation': False, 'time': 'Unknown'}}, {'Excretion': {'type': 'stool', 'frequency': 'Unknown', 'quality': 'Unknown', 'negation': False, 'time': 'Unknown'}}, {'Eating': {'food': 'Unknown', 'amount': 'Unknown', 'method': 'oral', 'negation': False, 'time': 'Unknown'}}, {'Sleep': {'quality': 'Unknown', 'duration': 'night', 'negation': False, 'time': 'night'}}, {'Pain': {'severity': 'Unknown', 'location': 'Unknown', 'duration': 'night', 'negation': False, 'time': 'night'}}]</t>
         </is>
       </c>
       <c r="N19" t="inlineStr">
         <is>
-          <t>['Eating', 'Excretion', 'Excretion', 'Family', 'Pain', 'Sleep', 'Pain', 'Sleep']</t>
+          <t>['daughter stayed the night in the room.', 'foley draining cyu.', 'bs present, no bm.', 'fair appetite', 'daughter stayed the night in the room.', "became anxious and rec'd ativan 0.5mg iv x 2 throughout the night."]</t>
         </is>
       </c>
       <c r="O19" t="inlineStr">
         <is>
-          <t>[{'Eating': {'food': 'Unknown', 'amount': 'Unknown', 'method': 'Unknown', 'negation': 'false', 'time': 'Unknown', 'caused_by': 'Unknown'}}, {'Excretion': {'type': 'stool', 'frequency': 'none', 'quality': 'Unknown', 'negation': 'false', 'time': 'Unknown', 'caused_by': 'Unknown'}}, {'Excretion': {'type': 'urine', 'frequency': 'Unknown', 'quality': 'Unknown', 'negation': 'false', 'time': 'Unknown', 'caused_by': 'Unknown'}}, {'Family': {'interaction': 'visit', 'relation': 'daughter', 'negation': 'false', 'time': 'night', 'caused_by': 'Unknown'}}, {'Pain': {'severity': 'Unknown', 'location': 'Unknown', 'duration': 'throughout the night', 'negation': 'false', 'time': 'night', 'caused_by': 'Unknown'}}, {'Sleep': {'quality': 'poor', 'duration': 'throughout the night', 'negation': 'false', 'time': 'night', 'caused_by': 'anxiety'}}, {'Pain': {'severity': 'Unknown', 'location': 'Unknown', 'duration': 'Unknown', 'negation': 'false', 'time': '[**2155**]', 'caused_by': 'fever'}}, {'Sleep': {'quality': 'Unknown', 'duration': 'night', 'negation': 'false', 'time': 'night', 'caused_by': 'Unknown'}}]</t>
-        </is>
-      </c>
-      <c r="P19" t="inlineStr">
-        <is>
-          <t>['fair appetite, bs present, no bm.', 'no bm.', 'Foley draining cyu.', 'daughter stayed the night in the room.', "became anxious and rec'd ativan 0.5mg iv x 2 throughout the night.", "became anxious and rec'd ativan 0.5mg iv x 2 throughout the night.", 'febrile to 101.0 @ [**2155**], gave tylenol 650mg with effect.', 'daughter stayed the night in the room.']</t>
-        </is>
-      </c>
-      <c r="Q19" t="n">
-        <v>0.002946742000858649</v>
-      </c>
-      <c r="R19" t="inlineStr">
+          <t>[[['e1', 'simultaneous', 'e5'], ['e2', 'before', 'e3'], ['e4', 'after', 'e6']]]</t>
+        </is>
+      </c>
+      <c r="P19" t="n">
+        <v>0.002362964001804357</v>
+      </c>
+      <c r="Q19" t="inlineStr">
         <is>
           <t>Sleep</t>
         </is>
       </c>
-      <c r="S19" t="b">
-        <v>0</v>
+      <c r="R19" t="b">
+        <v>0</v>
+      </c>
+      <c r="S19" t="n">
+        <v>1</v>
       </c>
       <c r="T19" t="n">
-        <v>1</v>
-      </c>
-      <c r="U19" t="n">
-        <v>0</v>
-      </c>
-      <c r="V19" t="inlineStr">
+        <v>0</v>
+      </c>
+      <c r="U19" t="inlineStr">
         <is>
           <t>('family', 'daughter')</t>
         </is>
       </c>
+      <c r="V19" t="n">
+        <v>23.11951317603234</v>
+      </c>
       <c r="W19" t="n">
-        <v>6.157393226996646</v>
+        <v>16.79939541796921</v>
       </c>
       <c r="X19" t="n">
-        <v>11.43244439001137</v>
+        <v>0</v>
       </c>
       <c r="Y19" t="n">
-        <v>22.18890079700213</v>
+        <v>1</v>
       </c>
       <c r="Z19" t="n">
-        <v>0</v>
-      </c>
-      <c r="AA19" t="n">
-        <v>1</v>
-      </c>
-      <c r="AB19" t="n">
-        <v>1</v>
-      </c>
-      <c r="AC19" t="n">
         <v>1</v>
       </c>
     </row>

</xml_diff>